<commit_message>
Deploying to gh-pages from @ rhmdnd/content@bce5e0ea2125a7539a7dad36cc5fd0c09b756d54 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -3945,7 +3945,7 @@
       </c>
       <c r="F50" s="2" t="inlineStr">
         <is>
-          <t>The operating system must require individuals to be authenticated with an individual authenticator prior to using a group authenticator.</t>
+          <t>Red Hat Enterprise Linux 9must require individuals to be authenticated with an individual authenticator prior to using a group authenticator.</t>
         </is>
       </c>
       <c r="G50" s="2" t="inlineStr">
@@ -4999,7 +4999,7 @@
       </c>
       <c r="F65" s="2" t="inlineStr">
         <is>
-          <t>The operating system must use multifactor authentication for network access to non-privileged accounts.</t>
+          <t>Red Hat Enterprise Linux 9 must use multifactor authentication for network access to non-privileged accounts.</t>
         </is>
       </c>
       <c r="G65" s="2" t="inlineStr">
@@ -6042,7 +6042,7 @@
       </c>
       <c r="F80" s="2" t="inlineStr">
         <is>
-          <t>The operating system must use multifactor authentication for local access to privileged accounts.</t>
+          <t>Red Hat Enterprise Linux 9 must use multifactor authentication for local access to privileged accounts.</t>
         </is>
       </c>
       <c r="G80" s="2" t="inlineStr">
@@ -6088,7 +6088,14 @@
         </is>
       </c>
       <c r="L80" s="2" t="n"/>
-      <c r="M80" s="2" t="inlineStr"/>
+      <c r="M80" s="2" t="inlineStr">
+        <is>
+          <t>To configure the system add or modify the following line in "/etc/ssh/sshd_config".
+PubkeyAuthentication yes
+Restart the SSH daemon for the settings to take effect:
+$ sudo systemctl restart sshd.service</t>
+        </is>
+      </c>
       <c r="N80" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -9410,7 +9417,7 @@
       </c>
       <c r="F129" s="2" t="inlineStr">
         <is>
-          <t>The operating system must use multifactor authentication for local access to non-privileged accounts.</t>
+          <t>Red Hat Enterprise Linux 9 must use multifactor authentication for local access to non-privileged accounts.</t>
         </is>
       </c>
       <c r="G129" s="2" t="inlineStr">
@@ -10979,7 +10986,7 @@
       </c>
       <c r="F151" s="2" t="inlineStr">
         <is>
-          <t>The operating system must use multifactor authentication for network access to privileged accounts.</t>
+          <t>Red Hat Enterprise Linux 9 must use multifactor authentication for network access to privileged accounts.</t>
         </is>
       </c>
       <c r="G151" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@08436ce586a70cfaaa22411167d9cdf80fdcb182 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -541,7 +541,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AU-4, AU-4 (1)</t>
+          <t>AU-4,AU-4 (1)</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -554,7 +554,11 @@
           <t>SRG-OS-000341-GPOS-00132,SRG-OS-000342-GPOS-00133</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr"/>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>CCE-88173-0</t>
+        </is>
+      </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
           <t>The operating system must allocate audit record storage capacity to store at least one weeks worth of audit records, when audit records are not immediately sent to a central audit record storage facility.</t>
@@ -562,7 +566,7 @@
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>The operating system must allocate audit record storage capacity to store at least one weeks worth of audit records, when audit records are not immediately sent to a central audit record storage facility.</t>
+          <t>Red Hat Enterprise Linux 9 must allocate audit record storage capacity to store at least one weeks worth of audit records, when audit records are not immediately sent to a central audit record storage facility.</t>
         </is>
       </c>
       <c r="G2" s="2" t="inlineStr">
@@ -621,7 +625,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b, SC-5, SC-5 (2)</t>
+          <t>SC-5 (2),CM-6 b,SC-5</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -634,7 +638,11 @@
           <t>SRG-OS-000480-GPOS-00227,SRG-OS-000420-GPOS-00186,SRG-OS-000142-GPOS-00071</t>
         </is>
       </c>
-      <c r="D3" s="2" t="inlineStr"/>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>CCE-84006-6</t>
+        </is>
+      </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
           <t>The operating system must manage excess capacity, bandwidth, or other redundancy to limit the effects of information flooding types of Denial of Service (DoS) attacks.</t>
@@ -642,7 +650,7 @@
       </c>
       <c r="F3" s="2" t="inlineStr">
         <is>
-          <t>The operating system must manage excess capacity, bandwidth, or other redundancy to limit the effects of information flooding types of Denial of Service (DoS) attacks.</t>
+          <t>Red Hat Enterprise Linux 9 must manage excess capacity, bandwidth, or other redundancy to limit the effects of information flooding types of Denial of Service (DoS) attacks.</t>
         </is>
       </c>
       <c r="G3" s="2" t="inlineStr">
@@ -695,7 +703,15 @@
         </is>
       </c>
       <c r="L3" s="2" t="n"/>
-      <c r="M3" s="2" t="inlineStr"/>
+      <c r="M3" s="2" t="inlineStr">
+        <is>
+          <t>Configure Red Hat Enterprise Linux 9 to use TCP syncookies.
+Add or edit the following line in a system configuration file in the "/etc/sysctl.d/" directory:
+ net.ipv4.tcp_syncookies = 1
+ Load settings from all system configuration files with the following command:
+ $ sudo sysctl --system</t>
+        </is>
+      </c>
       <c r="N3" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -708,7 +724,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (8), AC-6 (9), AU-12 (3), AU-7 a, AU-7 a, AU-7 a, AU-7 a, AU-7 a, AU-7 b, AU-7 b, AU-8 b, AU-8 b, CM-5 (1)</t>
+          <t>AC-6 (9),AU-12 (3),AU-8 b,AU-7 b,AU-7 a,AC-6 (8),CM-5 (1)</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -721,7 +737,11 @@
           <t>SRG-OS-000326-GPOS-00126,SRG-OS-000327-GPOS-00127,SRG-OS-000337-GPOS-00129,SRG-OS-000348-GPOS-00136,SRG-OS-000349-GPOS-00137,SRG-OS-000350-GPOS-00138,SRG-OS-000351-GPOS-00139,SRG-OS-000352-GPOS-00140,SRG-OS-000353-GPOS-00141,SRG-OS-000354-GPOS-00142,SRG-OS-000358-GPOS-00145,SRG-OS-000359-GPOS-00146,SRG-OS-000365-GPOS-00152</t>
         </is>
       </c>
-      <c r="D4" s="2" t="inlineStr"/>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>CCE-86402-5</t>
+        </is>
+      </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
           <t>The operating system must provide a report generation capability that supports on-demand audit review and analysis.</t>
@@ -729,7 +749,7 @@
       </c>
       <c r="F4" s="2" t="inlineStr">
         <is>
-          <t>The operating system must provide a report generation capability that supports on-demand audit review and analysis.</t>
+          <t>Red Hat Enterprise Linux 9 must provide a report generation capability that supports on-demand audit review and analysis.</t>
         </is>
       </c>
       <c r="G4" s="2" t="inlineStr">
@@ -784,7 +804,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b, AC-17 (1), AC-17 (9), CM-6 b, CM-6 b</t>
+          <t>AC-17 (9),CM-6 b,CM-7 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -797,7 +817,11 @@
           <t>SRG-OS-000096-GPOS-00050,SRG-OS-000297-GPOS-00115,SRG-OS-000298-GPOS-00116,SRG-OS-000480-GPOS-00227,SRG-OS-000480-GPOS-00232</t>
         </is>
       </c>
-      <c r="D5" s="2" t="inlineStr"/>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>CCE-84021-5</t>
+        </is>
+      </c>
       <c r="E5" s="2" t="inlineStr">
         <is>
           <t>The operating system must provide the capability to immediately disconnect or disable remote access to the operating system.</t>
@@ -805,7 +829,7 @@
       </c>
       <c r="F5" s="2" t="inlineStr">
         <is>
-          <t>The operating system must provide the capability to immediately disconnect or disable remote access to the operating system.</t>
+          <t>Red Hat Enterprise Linux 9 must provide the capability to immediately disconnect or disable remote access to the operating system.</t>
         </is>
       </c>
       <c r="G5" s="2" t="inlineStr">
@@ -965,7 +989,7 @@
       </c>
       <c r="F7" s="2" t="inlineStr">
         <is>
-          <t>The operating system must require devices to re-authenticate when changing authenticators.</t>
+          <t>Red Hat Enterprise Linux 9 must require devices to re-authenticate when changing authenticators.</t>
         </is>
       </c>
       <c r="G7" s="2" t="inlineStr">
@@ -1000,7 +1024,7 @@
     <row r="8" ht="130" customHeight="1">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11), IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
@@ -1013,7 +1037,11 @@
           <t>SRG-OS-000375-GPOS-00160,SRG-OS-000376-GPOS-00161</t>
         </is>
       </c>
-      <c r="D8" s="2" t="inlineStr"/>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83595-9</t>
+        </is>
+      </c>
       <c r="E8" s="2" t="inlineStr">
         <is>
           <t>The operating system must accept Personal Identity Verification (PIV) credentials.</t>
@@ -1021,7 +1049,7 @@
       </c>
       <c r="F8" s="2" t="inlineStr">
         <is>
-          <t>The operating system must accept Personal Identity Verification (PIV) credentials.</t>
+          <t>Red Hat Enterprise Linux 9 must accept Personal Identity Verification (PIV) credentials.</t>
         </is>
       </c>
       <c r="G8" s="2" t="inlineStr">
@@ -1147,7 +1175,7 @@
     <row r="10" ht="130" customHeight="1">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b), CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
@@ -1160,7 +1188,11 @@
           <t>SRG-OS-000370-GPOS-00155,SRG-OS-000368-GPOS-00154</t>
         </is>
       </c>
-      <c r="D10" s="2" t="inlineStr"/>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>CCE-84224-5</t>
+        </is>
+      </c>
       <c r="E10" s="2" t="inlineStr">
         <is>
           <t>The operating system must prevent program execution in accordance with local policies regarding software program usage and restrictions and/or rules authorizing the terms and conditions of software program usage.</t>
@@ -1168,7 +1200,7 @@
       </c>
       <c r="F10" s="2" t="inlineStr">
         <is>
-          <t>The operating system must prevent program execution in accordance with local policies regarding software program usage and restrictions and/or rules authorizing the terms and conditions of software program usage.</t>
+          <t>Red Hat Enterprise Linux 9 must prevent program execution in accordance with local policies regarding software program usage and restrictions and/or rules authorizing the terms and conditions of software program usage.</t>
         </is>
       </c>
       <c r="G10" s="2" t="inlineStr">
@@ -1232,7 +1264,11 @@
           <t>SRG-OS-000118-GPOS-00060</t>
         </is>
       </c>
-      <c r="D11" s="2" t="inlineStr"/>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83627-0</t>
+        </is>
+      </c>
       <c r="E11" s="2" t="inlineStr">
         <is>
           <t>The operating system must disable account identifiers (individuals, groups, roles, and devices) after 35 days of inactivity.</t>
@@ -1299,7 +1335,7 @@
     <row r="12" ht="130" customHeight="1">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b, AC-7 a</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
@@ -1312,7 +1348,11 @@
           <t>SRG-OS-000329-GPOS-00128,SRG-OS-000021-GPOS-00005</t>
         </is>
       </c>
-      <c r="D12" s="2" t="inlineStr"/>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83587-6</t>
+        </is>
+      </c>
       <c r="E12" s="2" t="inlineStr">
         <is>
           <t>The operating system must enforce the limit of three consecutive invalid logon attempts by a user during a 15-minute time period.</t>
@@ -1320,7 +1360,7 @@
       </c>
       <c r="F12" s="2" t="inlineStr">
         <is>
-          <t>The operating system must enforce the limit of three consecutive invalid logon attempts by a user during a 15-minute time period.</t>
+          <t>Red Hat Enterprise Linux 9 must enforce the limit of three consecutive invalid logon attempts by a user during a 15-minute time period.</t>
         </is>
       </c>
       <c r="G12" s="2" t="inlineStr">
@@ -1392,7 +1432,11 @@
           <t>SRG-OS-000076-GPOS-00044</t>
         </is>
       </c>
-      <c r="D13" s="2" t="inlineStr"/>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83606-4</t>
+        </is>
+      </c>
       <c r="E13" s="2" t="inlineStr">
         <is>
           <t>Operating systems must enforce a 60-day maximum password lifetime restriction.</t>
@@ -1479,7 +1523,7 @@
       </c>
       <c r="F14" s="2" t="inlineStr">
         <is>
-          <t>The operating system must allow operating system admins to pass information to any other operating system admin or user.</t>
+          <t>Red Hat Enterprise Linux 9 must allow operating system admins to pass information to any other operating system admin or user.</t>
         </is>
       </c>
       <c r="G14" s="2" t="inlineStr">
@@ -1514,7 +1558,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>IA-2, IA-8, AU-3 (1)</t>
+          <t>IA-2,IA-8,AU-3 (1)</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1527,7 +1571,11 @@
           <t>SRG-OS-000104-GPOS-00051,SRG-OS-000121-GPOS-00062,SRG-OS-000042-GPOS-00020</t>
         </is>
       </c>
-      <c r="D15" s="2" t="inlineStr"/>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>CCE-88493-2</t>
+        </is>
+      </c>
       <c r="E15" s="2" t="inlineStr">
         <is>
           <t>The operating system must generate audit records containing the full-text recording of privileged commands.</t>
@@ -1535,7 +1583,7 @@
       </c>
       <c r="F15" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records containing the full-text recording of privileged commands.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records containing the full-text recording of privileged commands.</t>
         </is>
       </c>
       <c r="G15" s="2" t="inlineStr">
@@ -1588,7 +1636,7 @@
     <row r="16" ht="130" customHeight="1">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10), CM-6 b</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
@@ -1601,7 +1649,11 @@
           <t>SRG-OS-000324-GPOS-00125,SRG-OS-000480-GPOS-00227</t>
         </is>
       </c>
-      <c r="D16" s="2" t="inlineStr"/>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90308-8</t>
+        </is>
+      </c>
       <c r="E16" s="2" t="inlineStr">
         <is>
           <t>The operating system must prevent non-privileged users from executing privileged functions to include disabling, circumventing, or altering implemented security safeguards/countermeasures.</t>
@@ -1609,7 +1661,7 @@
       </c>
       <c r="F16" s="2" t="inlineStr">
         <is>
-          <t>The operating system must prevent non-privileged users from executing privileged functions to include disabling, circumventing, or altering implemented security safeguards/countermeasures.</t>
+          <t>Red Hat Enterprise Linux 9 must prevent non-privileged users from executing privileged functions to include disabling, circumventing, or altering implemented security safeguards/countermeasures.</t>
         </is>
       </c>
       <c r="G16" s="2" t="inlineStr">
@@ -1660,7 +1712,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3 (1), AU-12 a, MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -1673,7 +1725,11 @@
           <t>SRG-OS-000037-GPOS-00015,SRG-OS-000042-GPOS-00020,SRG-OS-000062-GPOS-00031,SRG-OS-000392-GPOS-00172,SRG-OS-000462-GPOS-00206,SRG-OS-000471-GPOS-00215,SRG-OS-000064-GPOS-00033,SRG-OS-000466-GPOS-00210,SRG-OS-000458-GPOS-00203</t>
         </is>
       </c>
-      <c r="D17" s="2" t="inlineStr"/>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83830-0</t>
+        </is>
+      </c>
       <c r="E17" s="2" t="inlineStr">
         <is>
           <t>The operating system must generate audit records when successful/unsuccessful attempts to modify privileges occur.</t>
@@ -1681,7 +1737,7 @@
       </c>
       <c r="F17" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records when successful/unsuccessful attempts to modify privileges occur.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records when successful/unsuccessful attempts to modify privileges occur.</t>
         </is>
       </c>
       <c r="G17" s="2" t="inlineStr">
@@ -1752,7 +1808,7 @@
       </c>
       <c r="F18" s="2" t="inlineStr">
         <is>
-          <t>In the event of a system failure, the operating system must preserve any information necessary to determine cause of failure and any information necessary to return to operations with least disruption to mission processes.</t>
+          <t>In the event of a system failure, Red Hat Enterprise Linux 9 must preserve any information necessary to determine cause of failure and any information necessary to return to operations with least disruption to mission processes.</t>
         </is>
       </c>
       <c r="G18" s="2" t="inlineStr">
@@ -1787,7 +1843,7 @@
     <row r="19" ht="130" customHeight="1">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (b), IA-5 (1) (a), IA-5 (1) (a), IA-5 (1) (a), IA-5 (1) (a), CM-6 b, IA-5 (1) (a)</t>
+          <t>IA-5 (1) (b),CM-6 b,IA-5 (1) (a)</t>
         </is>
       </c>
       <c r="B19" s="2" t="inlineStr">
@@ -1800,7 +1856,11 @@
           <t>SRG-OS-000072-GPOS-00040,SRG-OS-000071-GPOS-00039,SRG-OS-000070-GPOS-00038,SRG-OS-000266-GPOS-00101,SRG-OS-000078-GPOS-00046,SRG-OS-000480-GPOS-00225,SRG-OS-000069-GPOS-00037</t>
         </is>
       </c>
-      <c r="D19" s="2" t="inlineStr"/>
+      <c r="D19" s="2" t="inlineStr">
+        <is>
+          <t>CCE-86356-3</t>
+        </is>
+      </c>
       <c r="E19" s="2" t="inlineStr">
         <is>
           <t>The operating system must enforce password complexity by requiring that at least one lower-case character be used.</t>
@@ -1878,7 +1938,11 @@
           <t>SRG-OS-000478-GPOS-00223</t>
         </is>
       </c>
-      <c r="D20" s="2" t="inlineStr"/>
+      <c r="D20" s="2" t="inlineStr">
+        <is>
+          <t>CCE-86547-7</t>
+        </is>
+      </c>
       <c r="E20" s="2" t="inlineStr">
         <is>
           <t>The operating system must implement NIST FIPS-validated cryptography for the following: to provision digital signatures, to generate cryptographic hashes, and to protect unclassified information requiring confidentiality and cryptographic protection in accordance with applicable federal laws, Executive Orders, directives, policies, regulations, and standards.</t>
@@ -1886,7 +1950,7 @@
       </c>
       <c r="F20" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement NIST FIPS-validated cryptography for the following: to provision digital signatures, to generate cryptographic hashes, and to protect unclassified information requiring confidentiality and cryptographic protection in accordance with applicable federal laws, Executive Orders, directives, policies, regulations, and standards.</t>
+          <t>Red Hat Enterprise Linux 9 must implement NIST FIPS-validated cryptography for the following: to provision digital signatures, to generate cryptographic hashes, and to protect unclassified information requiring confidentiality and cryptographic protection in accordance with applicable federal laws, Executive Orders, directives, policies, regulations, and standards.</t>
         </is>
       </c>
       <c r="G20" s="2" t="inlineStr">
@@ -1935,7 +1999,7 @@
     <row r="21" ht="130" customHeight="1">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>MA-4 e, SC-10, AC-12, MA-4 (7)</t>
+          <t>AC-12,MA-4 e,SC-10,MA-4 (7)</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
@@ -1948,7 +2012,11 @@
           <t>SRG-OS-000126-GPOS-00066,SRG-OS-000163-GPOS-00072,SRG-OS-000279-GPOS-00109,SRG-OS-000395-GPOS-00175</t>
         </is>
       </c>
-      <c r="D21" s="2" t="inlineStr"/>
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90811-1</t>
+        </is>
+      </c>
       <c r="E21" s="2" t="inlineStr">
         <is>
           <t>The operating system must terminate all network connections associated with a communications session at the end of the session, or as follows: for in-band management sessions (privileged sessions), the session must be terminated after 10 minutes of inactivity; and for user sessions (non-privileged session), the session must be terminated after 15 minutes of inactivity, except to fulfill documented and validated mission requirements.</t>
@@ -1956,7 +2024,7 @@
       </c>
       <c r="F21" s="2" t="inlineStr">
         <is>
-          <t>The operating system must terminate all network connections associated with a communications session at the end of the session, or as follows: for in-band management sessions (privileged sessions), the session must be terminated after 10 minutes of inacti</t>
+          <t>Red Hat Enterprise Linux 9 must terminate all network connections associated with a communications session at the end of the session, or as follows: for in-band management sessions (privileged sessions), the session must be terminated after 10 minutes of inacti</t>
         </is>
       </c>
       <c r="G21" s="2" t="inlineStr">
@@ -2006,7 +2074,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3, AU-3, AU-3, AU-3, AU-3 (1), AU-6 (4), AU-7 (1), AU-7 a, AU-14 (1), AU-3, CM-5 (1), MA-4 (1) (a), CM-6 b, AU-12 a, AU-7 a</t>
+          <t>AU-14 (1),MA-4 (1) (a),AU-12 a,AU-6 (4),CM-6 b,AU-3,AU-7 a,AU-3 (1),AU-7 (1),CM-5 (1)</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -2019,7 +2087,11 @@
           <t>SRG-OS-000037-GPOS-00015,SRG-OS-000038-GPOS-00016,SRG-OS-000039-GPOS-00017,SRG-OS-000040-GPOS-00018,SRG-OS-000041-GPOS-00019,SRG-OS-000042-GPOS-00021,SRG-OS-000051-GPOS-00024,SRG-OS-000054-GPOS-00025,SRG-OS-000122-GPOS-00063,SRG-OS-000254-GPOS-00095,SRG-OS-000255-GPOS-00096,SRG-OS-000365-GPOS-00152,SRG-OS-000392-GPOS-00172,SRG-OS-000480-GPOS-00227,SRG-OS-000062-GPOS-00031,SRG-OS-000349-GPOS-00137</t>
         </is>
       </c>
-      <c r="D22" s="2" t="inlineStr"/>
+      <c r="D22" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90829-3</t>
+        </is>
+      </c>
       <c r="E22" s="2" t="inlineStr">
         <is>
           <t>The operating system must produce audit records containing information to establish the outcome of the events.</t>
@@ -2107,7 +2179,7 @@
       </c>
       <c r="F23" s="2" t="inlineStr">
         <is>
-          <t>The operating system must allow operating system admins to change security attributes on users, the operating system, or the operating systems components.</t>
+          <t>Red Hat Enterprise Linux 9 must allow operating system admins to change security attributes on users, the operating system, or the operating systems components.</t>
         </is>
       </c>
       <c r="G23" s="2" t="inlineStr">
@@ -2155,7 +2227,11 @@
           <t>SRG-OS-000278-GPOS-00108</t>
         </is>
       </c>
-      <c r="D24" s="2" t="inlineStr"/>
+      <c r="D24" s="2" t="inlineStr">
+        <is>
+          <t>CCE-87757-1</t>
+        </is>
+      </c>
       <c r="E24" s="2" t="inlineStr">
         <is>
           <t>The operating system must use cryptographic mechanisms to protect the integrity of audit tools.</t>
@@ -2163,7 +2239,7 @@
       </c>
       <c r="F24" s="2" t="inlineStr">
         <is>
-          <t>The operating system must use cryptographic mechanisms to protect the integrity of audit tools.</t>
+          <t>Red Hat Enterprise Linux 9 must use cryptographic mechanisms to protect the integrity of audit tools.</t>
         </is>
       </c>
       <c r="G24" s="2" t="inlineStr">
@@ -2235,7 +2311,7 @@
     <row r="25" ht="130" customHeight="1">
       <c r="A25" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3 (1), AU-12 a, MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B25" s="2" t="inlineStr">
@@ -2248,7 +2324,11 @@
           <t>SRG-OS-000037-GPOS-00015,SRG-OS-000042-GPOS-00020,SRG-OS-000062-GPOS-00031,SRG-OS-000392-GPOS-00172,SRG-OS-000462-GPOS-00206,SRG-OS-000471-GPOS-00215,SRG-OS-000064-GPOS-00033,SRG-OS-000458-GPOS-00203,SRG-OS-000461-GPOS-00205</t>
         </is>
       </c>
-      <c r="D25" s="2" t="inlineStr"/>
+      <c r="D25" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83786-4</t>
+        </is>
+      </c>
       <c r="E25" s="2" t="inlineStr">
         <is>
           <t>The operating system must generate audit records when successful/unsuccessful attempts to access categories of information (e.g., classification levels) occur.</t>
@@ -2256,7 +2336,7 @@
       </c>
       <c r="F25" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records when successful/unsuccessful attempts to access categories of information (e.g., classification levels) occur.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records when successful/unsuccessful attempts to access categories of information (e.g., classification levels) occur.</t>
         </is>
       </c>
       <c r="G25" s="2" t="inlineStr">
@@ -2317,7 +2397,11 @@
           <t>SRG-OS-000068-GPOS-00036</t>
         </is>
       </c>
-      <c r="D26" s="2" t="inlineStr"/>
+      <c r="D26" s="2" t="inlineStr">
+        <is>
+          <t>CCE-89737-1</t>
+        </is>
+      </c>
       <c r="E26" s="2" t="inlineStr">
         <is>
           <t>The operating system must map the authenticated identity to the user or group account for PKI-based authentication.</t>
@@ -2464,7 +2548,7 @@
       </c>
       <c r="F28" s="2" t="inlineStr">
         <is>
-          <t>The operating system must automatically terminate a user session after inactivity time-outs have expired or at shutdown.</t>
+          <t>Red Hat Enterprise Linux 9 must automatically terminate a user session after inactivity time-outs have expired or at shutdown.</t>
         </is>
       </c>
       <c r="G28" s="2" t="inlineStr">
@@ -2501,7 +2585,7 @@
     <row r="29" ht="130" customHeight="1">
       <c r="A29" s="2" t="inlineStr">
         <is>
-          <t>SC-8, SC-8 (1), SC-8 (2), SC-8 (2)</t>
+          <t>SC-8,SC-8 (1),SC-8 (2)</t>
         </is>
       </c>
       <c r="B29" s="2" t="inlineStr">
@@ -2514,7 +2598,11 @@
           <t>SRG-OS-000423-GPOS-00187,SRG-OS-000424-GPOS-00188,SRG-OS-000425-GPOS-00189,SRG-OS-000426-GPOS-00190</t>
         </is>
       </c>
-      <c r="D29" s="2" t="inlineStr"/>
+      <c r="D29" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90823-6</t>
+        </is>
+      </c>
       <c r="E29" s="2" t="inlineStr">
         <is>
           <t>The operating system must protect the confidentiality and integrity of transmitted information.</t>
@@ -2522,7 +2610,7 @@
       </c>
       <c r="F29" s="2" t="inlineStr">
         <is>
-          <t>The operating system must protect the confidentiality and integrity of transmitted information.</t>
+          <t>Red Hat Enterprise Linux 9 must protect the confidentiality and integrity of transmitted information.</t>
         </is>
       </c>
       <c r="G29" s="2" t="inlineStr">
@@ -2626,7 +2714,7 @@
     <row r="31" ht="130" customHeight="1">
       <c r="A31" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4), AU-3, AU-3 (1), AU-12 a, AC-2 (4), MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AC-2 (4), AC-2 (4), AC-2 (4), AC-2 (4), AC-2 (4), AU-12 c, AU-12 c</t>
+          <t>MA-4 (1) (a),AC-2 (4),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B31" s="2" t="inlineStr">
@@ -2639,7 +2727,11 @@
           <t>SRG-OS-000004-GPOS-00004,SRG-OS-000037-GPOS-00015,SRG-OS-000042-GPOS-00020,SRG-OS-000062-GPOS-00031,SRG-OS-000304-GPOS-00121,SRG-OS-000392-GPOS-00172,SRG-OS-000462-GPOS-00206,SRG-OS-000470-GPOS-00214,SRG-OS-000471-GPOS-00215,SRG-OS-000239-GPOS-00089,SRG-OS-000240-GPOS-00090,SRG-OS-000241-GPOS-00091,SRG-OS-000303-GPOS-00120,SRG-OS-000304-GPOS-00121,SRG-OS-000466-GPOS-00210,SRG-OS-000476-GPOS-00221</t>
         </is>
       </c>
-      <c r="D31" s="2" t="inlineStr"/>
+      <c r="D31" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90176-9</t>
+        </is>
+      </c>
       <c r="E31" s="2" t="inlineStr">
         <is>
           <t>The operating system must audit all account removal actions.</t>
@@ -2647,7 +2739,7 @@
       </c>
       <c r="F31" s="2" t="inlineStr">
         <is>
-          <t>The operating system must audit all account removal actions.</t>
+          <t>Red Hat Enterprise Linux 9 must audit all account removal actions.</t>
         </is>
       </c>
       <c r="G31" s="2" t="inlineStr">
@@ -2724,7 +2816,7 @@
       </c>
       <c r="F32" s="2" t="inlineStr">
         <is>
-          <t>The operating system must produce audit records containing information to establish what type of events occurred.</t>
+          <t>Red Hat Enterprise Linux 9 must produce audit records containing information to establish what type of events occurred.</t>
         </is>
       </c>
       <c r="G32" s="2" t="inlineStr">
@@ -2773,7 +2865,11 @@
           <t>SRG-OS-000480-GPOS-00226</t>
         </is>
       </c>
-      <c r="D33" s="2" t="inlineStr"/>
+      <c r="D33" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83635-3</t>
+        </is>
+      </c>
       <c r="E33" s="2" t="inlineStr">
         <is>
           <t>The operating system must enforce a delay of at least 4 seconds between logon prompts following a failed logon attempt.</t>
@@ -2781,7 +2877,7 @@
       </c>
       <c r="F33" s="2" t="inlineStr">
         <is>
-          <t>The operating system must enforce a delay of at least 4 seconds between logon prompts following a failed logon attempt.</t>
+          <t>Red Hat Enterprise Linux 9 must enforce a delay of at least 4 seconds between logon prompts following a failed logon attempt.</t>
         </is>
       </c>
       <c r="G33" s="2" t="inlineStr">
@@ -2830,7 +2926,7 @@
     <row r="34" ht="130" customHeight="1">
       <c r="A34" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a, AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B34" s="2" t="inlineStr">
@@ -2843,7 +2939,11 @@
           <t>SRG-OS-000030-GPOS-00011,SRG-OS-000028-GPOS-00009</t>
         </is>
       </c>
-      <c r="D34" s="2" t="inlineStr"/>
+      <c r="D34" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83599-1</t>
+        </is>
+      </c>
       <c r="E34" s="2" t="inlineStr">
         <is>
           <t>The operating system must provide the capability for users to directly initiate a session lock for all connection types.</t>
@@ -2917,7 +3017,11 @@
           <t>SRG-OS-000077-GPOS-00045</t>
         </is>
       </c>
-      <c r="D35" s="2" t="inlineStr"/>
+      <c r="D35" s="2" t="inlineStr">
+        <is>
+          <t>CCE-86354-8</t>
+        </is>
+      </c>
       <c r="E35" s="2" t="inlineStr">
         <is>
           <t>The operating system must prohibit password reuse for a minimum of five generations.</t>
@@ -2925,7 +3029,7 @@
       </c>
       <c r="F35" s="2" t="inlineStr">
         <is>
-          <t>The operating system must prohibit password reuse for a minimum of five generations.</t>
+          <t>Red Hat Enterprise Linux 9 must prohibit password reuse for a minimum of five generations.</t>
         </is>
       </c>
       <c r="G35" s="2" t="inlineStr">
@@ -2988,7 +3092,11 @@
           <t>SRG-OS-000051-GPOS-00024</t>
         </is>
       </c>
-      <c r="D36" s="2" t="inlineStr"/>
+      <c r="D36" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83704-7</t>
+        </is>
+      </c>
       <c r="E36" s="2" t="inlineStr">
         <is>
           <t>The operating system must provide the capability to centrally review and analyze audit records from multiple components within the system.</t>
@@ -2996,7 +3104,7 @@
       </c>
       <c r="F36" s="2" t="inlineStr">
         <is>
-          <t>The operating system must provide the capability to centrally review and analyze audit records from multiple components within the system.</t>
+          <t>Red Hat Enterprise Linux 9 must provide the capability to centrally review and analyze audit records from multiple components within the system.</t>
         </is>
       </c>
       <c r="G36" s="2" t="inlineStr">
@@ -3102,7 +3210,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AU-9, AU-9, AU-9, SI-11 b</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3115,7 +3223,11 @@
           <t>SRG-OS-000057-GPOS-00027,SRG-OS-000058-GPOS-00028,SRG-OS-000059-GPOS-00029,SRG-OS-000206-GPOS-00084</t>
         </is>
       </c>
-      <c r="D38" s="2" t="inlineStr"/>
+      <c r="D38" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90516-6</t>
+        </is>
+      </c>
       <c r="E38" s="2" t="inlineStr">
         <is>
           <t>The operating system must reveal error messages only to authorized users.</t>
@@ -3123,7 +3235,7 @@
       </c>
       <c r="F38" s="2" t="inlineStr">
         <is>
-          <t>The operating system must reveal error messages only to authorized users.</t>
+          <t>Red Hat Enterprise Linux 9 must reveal error messages only to authorized users.</t>
         </is>
       </c>
       <c r="G38" s="2" t="inlineStr">
@@ -3170,7 +3282,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AU-3, CM-6 b</t>
+          <t>CM-6 b,AU-3</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3183,7 +3295,11 @@
           <t>SRG-OS-000255-GPOS-00096,SRG-OS-000480-GPOS-00227</t>
         </is>
       </c>
-      <c r="D39" s="2" t="inlineStr"/>
+      <c r="D39" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83696-5</t>
+        </is>
+      </c>
       <c r="E39" s="2" t="inlineStr">
         <is>
           <t>The operating system must produce audit records containing information to establish the identity of any individual or process associated with the event.</t>
@@ -3191,7 +3307,7 @@
       </c>
       <c r="F39" s="2" t="inlineStr">
         <is>
-          <t>The operating system must produce audit records containing information to establish the identity of any individual or process associated with the event.</t>
+          <t>Red Hat Enterprise Linux 9 must produce audit records containing information to establish the identity of any individual or process associated with the event.</t>
         </is>
       </c>
       <c r="G39" s="2" t="inlineStr">
@@ -3261,7 +3377,7 @@
       </c>
       <c r="F40" s="2" t="inlineStr">
         <is>
-          <t>The operating system must not alter original content or time ordering of audit records when it provides an audit reduction capability.</t>
+          <t>Red Hat Enterprise Linux 9 must not alter original content or time ordering of audit records when it provides an audit reduction capability.</t>
         </is>
       </c>
       <c r="G40" s="2" t="inlineStr">
@@ -3297,7 +3413,7 @@
     <row r="41" ht="130" customHeight="1">
       <c r="A41" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1), AU-4 (1)</t>
+          <t>AU-4 (1)</t>
         </is>
       </c>
       <c r="B41" s="2" t="inlineStr">
@@ -3318,7 +3434,7 @@
       </c>
       <c r="F41" s="2" t="inlineStr">
         <is>
-          <t>The operating system must off-load audit records onto a different system or media from the system being audited.</t>
+          <t>Red Hat Enterprise Linux 9 must off-load audit records onto a different system or media from the system being audited.</t>
         </is>
       </c>
       <c r="G41" s="2" t="inlineStr">
@@ -3369,7 +3485,7 @@
     <row r="42" ht="130" customHeight="1">
       <c r="A42" s="2" t="inlineStr">
         <is>
-          <t>SC-28 (1), SC-28, SC-28 (1)</t>
+          <t>SC-28 (1),SC-28</t>
         </is>
       </c>
       <c r="B42" s="2" t="inlineStr">
@@ -3382,7 +3498,11 @@
           <t>SRG-OS-000405-GPOS-00184,SRG-OS-000185-GPOS-00079,SRG-OS-000404-GPOS-00183</t>
         </is>
       </c>
-      <c r="D42" s="2" t="inlineStr"/>
+      <c r="D42" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90849-1</t>
+        </is>
+      </c>
       <c r="E42" s="2" t="inlineStr">
         <is>
           <t>The operating system must implement cryptographic mechanisms to prevent unauthorized modification of all information at rest on all operating system components.</t>
@@ -3390,7 +3510,7 @@
       </c>
       <c r="F42" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement cryptographic mechanisms to prevent unauthorized modification of all information at rest on all operating system components.</t>
+          <t>Red Hat Enterprise Linux 9 must implement cryptographic mechanisms to prevent unauthorized modification of all information at rest on all operating system components.</t>
         </is>
       </c>
       <c r="G42" s="2" t="inlineStr">
@@ -3431,7 +3551,13 @@
         </is>
       </c>
       <c r="L42" s="2" t="n"/>
-      <c r="M42" s="2" t="inlineStr"/>
+      <c r="M42" s="2" t="inlineStr">
+        <is>
+          <t>Configure Red Hat Enterprise Linux 9 to prevent unauthorized modification of all information at rest by using disk encryption.
+Encrypting a partition in an already installed system is more difficult, because existing partitions will need to be resized and changed.
+To encrypt an entire partition, dedicate a partition for encryption in the partition layout.</t>
+        </is>
+      </c>
       <c r="N42" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -3457,7 +3583,11 @@
           <t>SRG-OS-000027-GPOS-00008</t>
         </is>
       </c>
-      <c r="D43" s="2" t="inlineStr"/>
+      <c r="D43" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83641-1</t>
+        </is>
+      </c>
       <c r="E43" s="2" t="inlineStr">
         <is>
           <t>The operating system must limit the number of concurrent sessions to ten for all accounts and/or account types.</t>
@@ -3465,7 +3595,7 @@
       </c>
       <c r="F43" s="2" t="inlineStr">
         <is>
-          <t>The operating system must limit the number of concurrent sessions to ten for all accounts and/or account types.</t>
+          <t>Red Hat Enterprise Linux 9 must limit the number of concurrent sessions to ten for all accounts and/or account types.</t>
         </is>
       </c>
       <c r="G43" s="2" t="inlineStr">
@@ -3515,7 +3645,7 @@
     <row r="44" ht="130" customHeight="1">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>IA-11, IA-11, IA-11</t>
+          <t>IA-11</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
@@ -3528,7 +3658,11 @@
           <t>SRG-OS-000373-GPOS-00156,SRG-OS-000373-GPOS-00157,SRG-OS-000373-GPOS-00158</t>
         </is>
       </c>
-      <c r="D44" s="2" t="inlineStr"/>
+      <c r="D44" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83544-7</t>
+        </is>
+      </c>
       <c r="E44" s="2" t="inlineStr">
         <is>
           <t>The operating system must require users to re-authenticate when changing authenticators.</t>
@@ -3536,7 +3670,7 @@
       </c>
       <c r="F44" s="2" t="inlineStr">
         <is>
-          <t>The operating system must require users to re-authenticate when changing authenticators.</t>
+          <t>Red Hat Enterprise Linux 9 must require users to re-authenticate when changing authenticators.</t>
         </is>
       </c>
       <c r="G44" s="2" t="inlineStr">
@@ -3585,7 +3719,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a, AC-8 b, AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 b,AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3598,7 +3732,11 @@
           <t>SRG-OS-000023-GPOS-00006,SRG-OS-000024-GPOS-00007,SRG-OS-000228-GPOS-00088</t>
         </is>
       </c>
-      <c r="D45" s="2" t="inlineStr"/>
+      <c r="D45" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90807-9</t>
+        </is>
+      </c>
       <c r="E45" s="2" t="inlineStr">
         <is>
           <t>Any publically accessible connection to the operating system must display the Standard Mandatory DoD Notice and Consent Banner before granting access to the system.</t>
@@ -3606,7 +3744,7 @@
       </c>
       <c r="F45" s="2" t="inlineStr">
         <is>
-          <t>Any publically accessible connection to the operating system must display the Standard Mandatory DoD Notice and Consent Banner before granting access to the system.</t>
+          <t>Any publically accessible connection to Red Hat Enterprise Linux 9 must display the Standard Mandatory DoD Notice and Consent Banner before granting access to the system.</t>
         </is>
       </c>
       <c r="G45" s="2" t="inlineStr">
@@ -3704,7 +3842,7 @@
       </c>
       <c r="F46" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records when successful/unsuccessful attempts to access security objects occur.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records when successful/unsuccessful attempts to access security objects occur.</t>
         </is>
       </c>
       <c r="G46" s="2" t="inlineStr">
@@ -3760,7 +3898,7 @@
       </c>
       <c r="F47" s="2" t="inlineStr">
         <is>
-          <t>The operating system must notify system administrators and ISSOs of account enabling actions.</t>
+          <t>Red Hat Enterprise Linux 9 must notify system administrators and ISSOs of account enabling actions.</t>
         </is>
       </c>
       <c r="G47" s="2" t="inlineStr">
@@ -3796,7 +3934,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b, CM-6 b</t>
+          <t>CM-6 b</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -3809,7 +3947,11 @@
           <t>SRG-OS-000480-GPOS-00228,SRG-OS-000480-GPOS-00227</t>
         </is>
       </c>
-      <c r="D48" s="2" t="inlineStr"/>
+      <c r="D48" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83644-5</t>
+        </is>
+      </c>
       <c r="E48" s="2" t="inlineStr">
         <is>
           <t>The operating system must define default permissions for all authenticated users in such a way that the user can only read and modify their own files.</t>
@@ -3817,7 +3959,7 @@
       </c>
       <c r="F48" s="2" t="inlineStr">
         <is>
-          <t>The operating system must define default permissions for all authenticated users in such a way that the user can only read and modify their own files.</t>
+          <t>Red Hat Enterprise Linux 9 must define default permissions for all authenticated users in such a way that the user can only read and modify their own files.</t>
         </is>
       </c>
       <c r="G48" s="2" t="inlineStr">
@@ -3889,7 +4031,7 @@
       </c>
       <c r="F49" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement cryptographic mechanisms to prevent unauthorized disclosure of all information at rest on all operating system components.</t>
+          <t>Red Hat Enterprise Linux 9 must implement cryptographic mechanisms to prevent unauthorized disclosure of all information at rest on all operating system components.</t>
         </is>
       </c>
       <c r="G49" s="2" t="inlineStr">
@@ -3924,7 +4066,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5), CM-6 b</t>
+          <t>IA-2 (5),CM-6 b</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -3937,7 +4079,11 @@
           <t>SRG-OS-000109-GPOS-00056,SRG-OS-000480-GPOS-00227</t>
         </is>
       </c>
-      <c r="D50" s="2" t="inlineStr"/>
+      <c r="D50" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90800-4</t>
+        </is>
+      </c>
       <c r="E50" s="2" t="inlineStr">
         <is>
           <t>The operating system must require individuals to be authenticated with an individual authenticator prior to using a group authenticator.</t>
@@ -4019,7 +4165,7 @@
       </c>
       <c r="F51" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement cryptographic mechanisms to prevent unauthorized disclosure of information and/or detect changes to information during transmission unless otherwise protected by alternative physical safeguards, such as, at a minimum, a</t>
+          <t>Red Hat Enterprise Linux 9 must implement cryptographic mechanisms to prevent unauthorized disclosure of information and/or detect changes to information during transmission unless otherwise protected by alternative physical safeguards, such as, at a minimum, a</t>
         </is>
       </c>
       <c r="G51" s="2" t="inlineStr">
@@ -4069,7 +4215,11 @@
           <t>SRG-OS-000120-GPOS-00061</t>
         </is>
       </c>
-      <c r="D52" s="2" t="inlineStr"/>
+      <c r="D52" s="2" t="inlineStr">
+        <is>
+          <t>CCE-84221-1</t>
+        </is>
+      </c>
       <c r="E52" s="2" t="inlineStr">
         <is>
           <t>The operating system must use mechanisms meeting the requirements of applicable federal laws, Executive orders, directives, policies, regulations, standards, and guidance for authentication to a cryptographic module.</t>
@@ -4132,7 +4282,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>SC-13, MA-4 (6), MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4145,7 +4295,11 @@
           <t>SRG-OS-000396-GPOS-00176,SRG-OS-000393-GPOS-00173,SRG-OS-000394-GPOS-00174</t>
         </is>
       </c>
-      <c r="D53" s="2" t="inlineStr"/>
+      <c r="D53" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83450-7</t>
+        </is>
+      </c>
       <c r="E53" s="2" t="inlineStr">
         <is>
           <t>The operating system must implement cryptographic mechanisms to protect the integrity of nonlocal maintenance and diagnostic communications, when used for nonlocal maintenance sessions.</t>
@@ -4153,7 +4307,7 @@
       </c>
       <c r="F53" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement cryptographic mechanisms to protect the integrity of nonlocal maintenance and diagnostic communications, when used for nonlocal maintenance sessions.</t>
+          <t>Red Hat Enterprise Linux 9 must implement cryptographic mechanisms to protect the integrity of nonlocal maintenance and diagnostic communications, when used for nonlocal maintenance sessions.</t>
         </is>
       </c>
       <c r="G53" s="2" t="inlineStr">
@@ -4269,7 +4423,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2), SC-8</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4282,7 +4436,11 @@
           <t>SRG-OS-000250-GPOS-00093,SRG-OS-000423-GPOS-00187</t>
         </is>
       </c>
-      <c r="D55" s="2" t="inlineStr"/>
+      <c r="D55" s="2" t="inlineStr">
+        <is>
+          <t>CCE-86860-4</t>
+        </is>
+      </c>
       <c r="E55" s="2" t="inlineStr">
         <is>
           <t>The operating system must implement cryptography to protect the integrity of remote access sessions.</t>
@@ -4290,7 +4448,7 @@
       </c>
       <c r="F55" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement cryptography to protect the integrity of remote access sessions.</t>
+          <t>Red Hat Enterprise Linux 9 must implement cryptography to protect the integrity of remote access sessions.</t>
         </is>
       </c>
       <c r="G55" s="2" t="inlineStr">
@@ -4340,7 +4498,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a), AU-12 c, AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4353,7 +4511,11 @@
           <t>SRG-OS-000392-GPOS-00172,SRG-OS-000470-GPOS-00214,SRG-OS-000473-GPOS-00218</t>
         </is>
       </c>
-      <c r="D56" s="2" t="inlineStr"/>
+      <c r="D56" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83783-1</t>
+        </is>
+      </c>
       <c r="E56" s="2" t="inlineStr">
         <is>
           <t>The operating system must generate audit records when successful/unsuccessful logon attempts occur.</t>
@@ -4361,7 +4523,7 @@
       </c>
       <c r="F56" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records when successful/unsuccessful logon attempts occur.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records when successful/unsuccessful logon attempts occur.</t>
         </is>
       </c>
       <c r="G56" s="2" t="inlineStr">
@@ -4420,7 +4582,11 @@
           <t>SRG-OS-000433-GPOS-00192</t>
         </is>
       </c>
-      <c r="D57" s="2" t="inlineStr"/>
+      <c r="D57" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83970-4</t>
+        </is>
+      </c>
       <c r="E57" s="2" t="inlineStr">
         <is>
           <t>The operating system must implement non-executable data to protect its memory from unauthorized code execution.</t>
@@ -4428,7 +4594,7 @@
       </c>
       <c r="F57" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement non-executable data to protect its memory from unauthorized code execution.</t>
+          <t>Red Hat Enterprise Linux 9 must implement non-executable data to protect its memory from unauthorized code execution.</t>
         </is>
       </c>
       <c r="G57" s="2" t="inlineStr">
@@ -4507,7 +4673,11 @@
           <t>SRG-OS-000029-GPOS-00010</t>
         </is>
       </c>
-      <c r="D58" s="2" t="inlineStr"/>
+      <c r="D58" s="2" t="inlineStr">
+        <is>
+          <t>CCE-89876-7</t>
+        </is>
+      </c>
       <c r="E58" s="2" t="inlineStr">
         <is>
           <t>The operating system must initiate a session lock after a 15-minute period of inactivity for all connection types.</t>
@@ -4515,7 +4685,7 @@
       </c>
       <c r="F58" s="2" t="inlineStr">
         <is>
-          <t>The operating system must initiate a session lock after a 15-minute period of inactivity for all connection types.</t>
+          <t>Red Hat Enterprise Linux 9 must initiate a session lock after a 15-minute period of inactivity for all connection types.</t>
         </is>
       </c>
       <c r="G58" s="2" t="inlineStr">
@@ -4585,7 +4755,7 @@
       </c>
       <c r="F59" s="2" t="inlineStr">
         <is>
-          <t>The operating system must uniquely identify peripherals before establishing a connection.</t>
+          <t>Red Hat Enterprise Linux 9 must uniquely identify peripherals before establishing a connection.</t>
         </is>
       </c>
       <c r="G59" s="2" t="inlineStr">
@@ -4736,7 +4906,7 @@
       </c>
       <c r="F61" s="2" t="inlineStr">
         <is>
-          <t>The operating system must provide the capability for assigned IMOs/ISSOs or designated SAs to change the auditing to be performed on all operating system components, based on all selectable event criteria in near real time.</t>
+          <t>Red Hat Enterprise Linux 9 must provide the capability for assigned IMOs/ISSOs or designated SAs to change the auditing to be performed on all operating system components, based on all selectable event criteria in near real time.</t>
         </is>
       </c>
       <c r="G61" s="2" t="inlineStr">
@@ -4792,7 +4962,7 @@
       </c>
       <c r="F62" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records when successful/unsuccessful attempts to delete privileges occur.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records when successful/unsuccessful attempts to delete privileges occur.</t>
         </is>
       </c>
       <c r="G62" s="2" t="inlineStr">
@@ -4827,7 +4997,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a, AU-5 (1)</t>
+          <t>AU-5 a,AU-5 (1)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -4840,7 +5010,11 @@
           <t>SRG-OS-000046-GPOS-00022,SRG-OS-000343-GPOS-00134</t>
         </is>
       </c>
-      <c r="D63" s="2" t="inlineStr"/>
+      <c r="D63" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83698-1</t>
+        </is>
+      </c>
       <c r="E63" s="2" t="inlineStr">
         <is>
           <t>The operating system must immediately notify the SA and ISSO (at a minimum) when allocated audit record storage volume reaches 75% of the repository maximum audit record storage capacity.</t>
@@ -4848,7 +5022,7 @@
       </c>
       <c r="F63" s="2" t="inlineStr">
         <is>
-          <t>The operating system must immediately notify the SA and ISSO (at a minimum) when allocated audit record storage volume reaches 75% of the repository maximum audit record storage capacity.</t>
+          <t>Red Hat Enterprise Linux 9 must immediately notify the SA and ISSO (at a minimum) when allocated audit record storage volume reaches 75% of the repository maximum audit record storage capacity.</t>
         </is>
       </c>
       <c r="G63" s="2" t="inlineStr">
@@ -4928,7 +5102,7 @@
       </c>
       <c r="H64" s="2" t="inlineStr">
         <is>
-          <t>To prevent the compromise of authentication information, such as passwords during the authentication process, the feedback from the operating system must not provide any information allowing an unauthorized user to compromise the authentication mechanism.
+          <t>To prevent the compromise of authentication information, such as passwords during the authentication process, the feedback from Red Hat Enterprise Linux 9 must not provide any information allowing an unauthorized user to compromise the authentication mechanism.
 Obfuscation of user-provided information that is typed into the system is a method used when addressing this risk.
 For example, displaying asterisks when a user types in a password is an example of obscuring feedback of authentication information.</t>
         </is>
@@ -4978,7 +5152,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2), CM-6 b, CM-6 b</t>
+          <t>CM-6 b,IA-2 (2)</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -4991,7 +5165,11 @@
           <t>SRG-OS-000106-GPOS-00053,SRG-OS-000480-GPOS-00229,SRG-OS-000480-GPOS-00227</t>
         </is>
       </c>
-      <c r="D65" s="2" t="inlineStr"/>
+      <c r="D65" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90799-8</t>
+        </is>
+      </c>
       <c r="E65" s="2" t="inlineStr">
         <is>
           <t>The operating system must use multifactor authentication for network access to non-privileged accounts.</t>
@@ -5082,7 +5260,7 @@
       </c>
       <c r="F66" s="2" t="inlineStr">
         <is>
-          <t>The operating system must enforce password complexity by requiring that at least one special character be used.</t>
+          <t>Red Hat Enterprise Linux 9 must enforce password complexity by requiring that at least one special character be used.</t>
         </is>
       </c>
       <c r="G66" s="2" t="inlineStr">
@@ -5118,7 +5296,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3 (1), AU-12 a, MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5131,7 +5309,11 @@
           <t>SRG-OS-000037-GPOS-00015,SRG-OS-000042-GPOS-00020,SRG-OS-000062-GPOS-00031,SRG-OS-000392-GPOS-00172,SRG-OS-000458-GPOS-00203,SRG-OS-000462-GPOS-00206,SRG-OS-000463-GPOS-00207,SRG-OS-000471-GPOS-00215,SRG-OS-000474-GPOS-00219,SRG-OS-000466-GPOS-00210,SRG-OS-000064-GPOS-00033</t>
         </is>
       </c>
-      <c r="D67" s="2" t="inlineStr"/>
+      <c r="D67" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83821-9</t>
+        </is>
+      </c>
       <c r="E67" s="2" t="inlineStr">
         <is>
           <t>The operating system must generate audit records when successful/unsuccessful attempts to modify security objects occur.</t>
@@ -5139,7 +5321,7 @@
       </c>
       <c r="F67" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records when successful/unsuccessful attempts to modify security objects occur.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records when successful/unsuccessful attempts to modify security objects occur.</t>
         </is>
       </c>
       <c r="G67" s="2" t="inlineStr">
@@ -5210,7 +5392,7 @@
       </c>
       <c r="F68" s="2" t="inlineStr">
         <is>
-          <t>The operating system must limit the ability of non-privileged users to grant other users direct access to the contents of their home directories/folders.</t>
+          <t>Red Hat Enterprise Linux 9 must limit the ability of non-privileged users to grant other users direct access to the contents of their home directories/folders.</t>
         </is>
       </c>
       <c r="G68" s="2" t="inlineStr">
@@ -5244,7 +5426,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-7 a, AU-12 (3), AU-7 a, AU-7 a, AU-7 a, AU-7 a, AU-7 a, AU-7 b, AU-7 b, AU-8 b, AU-8 b, CM-5 (1), AU-12 c, AU-12 c, CM-6 b, AU-12 a</t>
+          <t>AU-12 c,AU-12 (3),AU-8 b,AU-12 a,AU-7 b,CM-6 b,AU-7 a,CM-5 (1)</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5257,7 +5439,11 @@
           <t>SRG-OS-000122-GPOS-00063,SRG-OS-000337-GPOS-00129,SRG-OS-000348-GPOS-00136,SRG-OS-000349-GPOS-00137,SRG-OS-000350-GPOS-00138,SRG-OS-000351-GPOS-00139,SRG-OS-000352-GPOS-00140,SRG-OS-000353-GPOS-00141,SRG-OS-000354-GPOS-00142,SRG-OS-000358-GPOS-00145,SRG-OS-000359-GPOS-00146,SRG-OS-000365-GPOS-00152,SRG-OS-000474-GPOS-00219,SRG-OS-000475-GPOS-00220,SRG-OS-000480-GPOS-00227,SRG-OS-000062-GPOS-00031</t>
         </is>
       </c>
-      <c r="D69" s="2" t="inlineStr"/>
+      <c r="D69" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83649-4</t>
+        </is>
+      </c>
       <c r="E69" s="2" t="inlineStr">
         <is>
           <t>The operating system must produce audit records containing information to establish when (date and time) the events occurred.</t>
@@ -5328,7 +5514,11 @@
           <t>SRG-OS-000138-GPOS-00069</t>
         </is>
       </c>
-      <c r="D70" s="2" t="inlineStr"/>
+      <c r="D70" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83895-3</t>
+        </is>
+      </c>
       <c r="E70" s="2" t="inlineStr">
         <is>
           <t>Operating systems must prevent unauthorized and unintended information transfer via shared system resources.</t>
@@ -5394,7 +5584,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-4 (1), AU-4 (1)</t>
+          <t>AU-3,AU-4 (1)</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5407,7 +5597,11 @@
           <t>SRG-OS-000039-GPOS-00017,SRG-OS-000342-GPOS-00133,SRG-OS-000479-GPOS-00224</t>
         </is>
       </c>
-      <c r="D71" s="2" t="inlineStr"/>
+      <c r="D71" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83686-6</t>
+        </is>
+      </c>
       <c r="E71" s="2" t="inlineStr">
         <is>
           <t>The operating system must produce audit records containing information to establish where the events occurred.</t>
@@ -5557,7 +5751,7 @@
       </c>
       <c r="F73" s="2" t="inlineStr">
         <is>
-          <t>The operating system must not alter original content or time ordering of audit records when it provides a report generation capability.</t>
+          <t>Red Hat Enterprise Linux 9 must not alter original content or time ordering of audit records when it provides a report generation capability.</t>
         </is>
       </c>
       <c r="G73" s="2" t="inlineStr">
@@ -5606,7 +5800,11 @@
           <t>SRG-OS-000062-GPOS-00031</t>
         </is>
       </c>
-      <c r="D74" s="2" t="inlineStr"/>
+      <c r="D74" s="2" t="inlineStr">
+        <is>
+          <t>CCE-84206-2</t>
+        </is>
+      </c>
       <c r="E74" s="2" t="inlineStr">
         <is>
           <t>The operating system must provide audit record generation capability for DoD-defined auditable events for all operating system components.</t>
@@ -5614,7 +5812,7 @@
       </c>
       <c r="F74" s="2" t="inlineStr">
         <is>
-          <t>The operating system must provide audit record generation capability for DoD-defined auditable events for all operating system components.</t>
+          <t>Red Hat Enterprise Linux 9 must provide audit record generation capability for DoD-defined auditable events for all operating system components.</t>
         </is>
       </c>
       <c r="G74" s="2" t="inlineStr">
@@ -5751,7 +5949,7 @@
       </c>
       <c r="F76" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement NSA-approved cryptography to protect classified information in accordance with applicable federal laws, Executive Orders, directives, policies, regulations, and standards.</t>
+          <t>Red Hat Enterprise Linux 9 must implement NSA-approved cryptography to protect classified information in accordance with applicable federal laws, Executive Orders, directives, policies, regulations, and standards.</t>
         </is>
       </c>
       <c r="G76" s="2" t="inlineStr">
@@ -5785,7 +5983,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4), AU-3, AU-3 (1), AU-12 a, AC-2 (4), MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AC-2 (4), AC-2 (4), AC-2 (4), AC-2 (4), AC-2 (4), AU-12 c, AU-12 c, AC-2 (4), AC-2 (4), AC-2 (4), AC-2 (4)</t>
+          <t>MA-4 (1) (a),AC-2 (4),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -5798,7 +5996,11 @@
           <t>SRG-OS-000004-GPOS-00004,SRG-OS-000037-GPOS-00015,SRG-OS-000042-GPOS-00020,SRG-OS-000062-GPOS-00031,SRG-OS-000304-GPOS-00121,SRG-OS-000392-GPOS-00172,SRG-OS-000462-GPOS-00206,SRG-OS-000470-GPOS-00214,SRG-OS-000471-GPOS-00215,SRG-OS-000239-GPOS-00089,SRG-OS-000240-GPOS-00090,SRG-OS-000241-GPOS-00091,SRG-OS-000303-GPOS-00120,SRG-OS-000304-GPOS-00121,SRG-OS-000466-GPOS-00210,SRG-OS-000476-GPOS-00221,SRG-OS-000274-GPOS-00104,SRG-OS-000275-GPOS-00105,SRG-OS-000276-GPOS-00106,SRG-OS-000277-GPOS-00107</t>
         </is>
       </c>
-      <c r="D77" s="2" t="inlineStr"/>
+      <c r="D77" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83714-6</t>
+        </is>
+      </c>
       <c r="E77" s="2" t="inlineStr">
         <is>
           <t>The operating system must notify system administrators and ISSOs when accounts are removed.</t>
@@ -5885,7 +6087,11 @@
           <t>SRG-OS-000125-GPOS-00065</t>
         </is>
       </c>
-      <c r="D78" s="2" t="inlineStr"/>
+      <c r="D78" s="2" t="inlineStr">
+        <is>
+          <t>CCE-86722-6</t>
+        </is>
+      </c>
       <c r="E78" s="2" t="inlineStr">
         <is>
           <t>The operating system must employ strong authenticators in the establishment of nonlocal maintenance and diagnostic sessions.</t>
@@ -5950,7 +6156,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-9, AU-9, AU-9, AU-9 (3)</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -5963,7 +6169,11 @@
           <t>SRG-OS-000256-GPOS-00097,SRG-OS-000257-GPOS-00098,SRG-OS-000258-GPOS-00099,SRG-OS-000278-GPOS-00108</t>
         </is>
       </c>
-      <c r="D79" s="2" t="inlineStr"/>
+      <c r="D79" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90840-0</t>
+        </is>
+      </c>
       <c r="E79" s="2" t="inlineStr">
         <is>
           <t>The operating system must protect audit tools from unauthorized deletion.</t>
@@ -5971,7 +6181,7 @@
       </c>
       <c r="F79" s="2" t="inlineStr">
         <is>
-          <t>The operating system must protect audit tools from unauthorized deletion.</t>
+          <t>Red Hat Enterprise Linux 9 must protect audit tools from unauthorized deletion.</t>
         </is>
       </c>
       <c r="G79" s="2" t="inlineStr">
@@ -6021,7 +6231,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1), IA-2 (2), IA-2 (3), IA-2 (4)</t>
+          <t>IA-2 (1),IA-2 (3),IA-2 (4),IA-2 (2)</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6108,7 +6318,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b, CM-5 (3)</t>
+          <t>CM-5 (3),CM-6 b</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6121,7 +6331,11 @@
           <t>SRG-OS-000480-GPOS-00227,SRG-OS-000366-GPOS-00153</t>
         </is>
       </c>
-      <c r="D81" s="2" t="inlineStr"/>
+      <c r="D81" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83954-8</t>
+        </is>
+      </c>
       <c r="E81" s="2" t="inlineStr">
         <is>
           <t>The operating system must prevent the installation of patches, service packs, device drivers, or operating system components without verification they have been digitally signed using a certificate that is recognized and approved by the organization.</t>
@@ -6129,7 +6343,7 @@
       </c>
       <c r="F81" s="2" t="inlineStr">
         <is>
-          <t>The operating system must prevent the installation of patches, service packs, device drivers, or operating system components without verification they have been digitally signed using a certificate that is recognized and approved by the organization.</t>
+          <t>Red Hat Enterprise Linux 9 must prevent the installation of patches, service packs, device drivers, or operating system components without verification they have been digitally signed using a certificate that is recognized and approved by the organization.</t>
         </is>
       </c>
       <c r="G81" s="2" t="inlineStr">
@@ -6214,7 +6428,7 @@
       </c>
       <c r="F82" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records when successful/unsuccessful attempts to access privileges occur.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records when successful/unsuccessful attempts to access privileges occur.</t>
         </is>
       </c>
       <c r="G82" s="2" t="inlineStr">
@@ -6327,7 +6541,7 @@
       </c>
       <c r="F84" s="2" t="inlineStr">
         <is>
-          <t>The operating system must protect against or limit the effects of Denial of Service (DoS) attacks by ensuring the operating system is implementing rate-limiting measures on impacted network interfaces.</t>
+          <t>Red Hat Enterprise Linux 9 must protect against or limit the effects of Denial of Service (DoS) attacks by ensuring the operating system is implementing rate-limiting measures on impacted network interfaces.</t>
         </is>
       </c>
       <c r="G84" s="2" t="inlineStr">
@@ -6406,7 +6620,7 @@
       </c>
       <c r="F85" s="2" t="inlineStr">
         <is>
-          <t>The operating system must prevent all software from executing at higher privilege levels than users executing the software.</t>
+          <t>Red Hat Enterprise Linux 9 must prevent all software from executing at higher privilege levels than users executing the software.</t>
         </is>
       </c>
       <c r="G85" s="2" t="inlineStr">
@@ -6441,7 +6655,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3 (1), AU-12 a, MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -6454,7 +6668,11 @@
           <t>SRG-OS-000037-GPOS-00015,SRG-OS-000042-GPOS-00020,SRG-OS-000062-GPOS-00031,SRG-OS-000392-GPOS-00172,SRG-OS-000462-GPOS-00206,SRG-OS-000471-GPOS-00215,SRG-OS-000064-GPOS-00033,SRG-OS-000466-GPOS-00210,SRG-OS-000458-GPOS-00203,SRG-OS-000474-GPOS-00219</t>
         </is>
       </c>
-      <c r="D86" s="2" t="inlineStr"/>
+      <c r="D86" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83812-8</t>
+        </is>
+      </c>
       <c r="E86" s="2" t="inlineStr">
         <is>
           <t>The operating system must generate audit records when successful/unsuccessful accesses to objects occur.</t>
@@ -6462,7 +6680,7 @@
       </c>
       <c r="F86" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records when successful/unsuccessful accesses to objects occur.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records when successful/unsuccessful accesses to objects occur.</t>
         </is>
       </c>
       <c r="G86" s="2" t="inlineStr">
@@ -6525,7 +6743,11 @@
           <t>SRG-OS-000073-GPOS-00041</t>
         </is>
       </c>
-      <c r="D87" s="2" t="inlineStr"/>
+      <c r="D87" s="2" t="inlineStr">
+        <is>
+          <t>CCE-88865-1</t>
+        </is>
+      </c>
       <c r="E87" s="2" t="inlineStr">
         <is>
           <t>The operating system must store only encrypted representations of passwords.</t>
@@ -6533,7 +6755,7 @@
       </c>
       <c r="F87" s="2" t="inlineStr">
         <is>
-          <t>The operating system must store only encrypted representations of passwords.</t>
+          <t>Red Hat Enterprise Linux 9 must store only encrypted representations of passwords.</t>
         </is>
       </c>
       <c r="G87" s="2" t="inlineStr">
@@ -6587,7 +6809,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4), AC-2 (4), AC-2 (4), AC-2 (4), AU-12 c, AC-6 (9), AU-12 c, CM-5 (1), AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c</t>
+          <t>AU-12 c,AC-2 (4),AC-6 (9),CM-5 (1)</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -6608,7 +6830,7 @@
       </c>
       <c r="F88" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records showing starting and ending time for user access to the system.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records showing starting and ending time for user access to the system.</t>
         </is>
       </c>
       <c r="G88" s="2" t="inlineStr">
@@ -6654,7 +6876,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>IA-2, IA-2 (2), IA-2 (3), IA-2 (5), IA-2 (4)</t>
+          <t>IA-2 (5),IA-2,IA-2 (3),IA-2 (4),IA-2 (2)</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -6667,7 +6889,11 @@
           <t>SRG-OS-000104-GPOS-00051,SRG-OS-000106-GPOS-00053,SRG-OS-000107-GPOS-00054,SRG-OS-000109-GPOS-00056,SRG-OS-000108-GPOS-00055,SRG-OS-000108-GPOS-00057,SRG-OS-000108-GPOS-00058</t>
         </is>
       </c>
-      <c r="D89" s="2" t="inlineStr"/>
+      <c r="D89" s="2" t="inlineStr">
+        <is>
+          <t>CCE-89122-6</t>
+        </is>
+      </c>
       <c r="E89" s="2" t="inlineStr">
         <is>
           <t>The operating system must uniquely identify and must authenticate organizational users (or processes acting on behalf of organizational users).</t>
@@ -6734,7 +6960,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11), IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -6747,7 +6973,11 @@
           <t>SRG-OS-000375-GPOS-00160,SRG-OS-000377-GPOS-00162</t>
         </is>
       </c>
-      <c r="D90" s="2" t="inlineStr"/>
+      <c r="D90" s="2" t="inlineStr">
+        <is>
+          <t>CCE-87088-1</t>
+        </is>
+      </c>
       <c r="E90" s="2" t="inlineStr">
         <is>
           <t>The operating system must implement multifactor authentication for remote access to privileged accounts in such a way that one of the factors is provided by a device separate from the system gaining access.</t>
@@ -6755,7 +6985,7 @@
       </c>
       <c r="F90" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement multifactor authentication for remote access to privileged accounts in such a way that one of the factors is provided by a device separate from the system gaining access.</t>
+          <t>Red Hat Enterprise Linux 9 must implement multifactor authentication for remote access to privileged accounts in such a way that one of the factors is provided by a device separate from the system gaining access.</t>
         </is>
       </c>
       <c r="G90" s="2" t="inlineStr">
@@ -6810,7 +7040,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>AU-9, AU-9, AU-9 (3)</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -6823,7 +7053,11 @@
           <t>SRG-OS-000256-GPOS-00097,SRG-OS-000257-GPOS-00098,SRG-OS-000278-GPOS-00108</t>
         </is>
       </c>
-      <c r="D91" s="2" t="inlineStr"/>
+      <c r="D91" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90842-6</t>
+        </is>
+      </c>
       <c r="E91" s="2" t="inlineStr">
         <is>
           <t>The operating system must protect audit tools from unauthorized modification.</t>
@@ -6831,7 +7065,7 @@
       </c>
       <c r="F91" s="2" t="inlineStr">
         <is>
-          <t>The operating system must protect audit tools from unauthorized modification.</t>
+          <t>Red Hat Enterprise Linux 9 must protect audit tools from unauthorized modification.</t>
         </is>
       </c>
       <c r="G91" s="2" t="inlineStr">
@@ -6994,7 +7228,7 @@
       </c>
       <c r="F93" s="2" t="inlineStr">
         <is>
-          <t>The operating system must, at a minimum, off-load audit data from interconnected systems in real time and off-load audit data from standalone systems weekly.</t>
+          <t>Red Hat Enterprise Linux 9 must, at a minimum, off-load audit data from interconnected systems in real time and off-load audit data from standalone systems weekly.</t>
         </is>
       </c>
       <c r="G93" s="2" t="inlineStr">
@@ -7042,7 +7276,11 @@
           <t>SRG-OS-000075-GPOS-00043</t>
         </is>
       </c>
-      <c r="D94" s="2" t="inlineStr"/>
+      <c r="D94" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83610-6</t>
+        </is>
+      </c>
       <c r="E94" s="2" t="inlineStr">
         <is>
           <t>Operating systems must enforce 24 hours/1 day as the minimum password lifetime.</t>
@@ -7119,7 +7357,11 @@
           <t>SRG-OS-000072-GPOS-00040</t>
         </is>
       </c>
-      <c r="D95" s="2" t="inlineStr"/>
+      <c r="D95" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83564-5</t>
+        </is>
+      </c>
       <c r="E95" s="2" t="inlineStr">
         <is>
           <t>The operating system must require the change of at least 50% of the total number of characters when passwords are changed.</t>
@@ -7127,7 +7369,7 @@
       </c>
       <c r="F95" s="2" t="inlineStr">
         <is>
-          <t>The operating system must require the change of at least 50% of the total number of characters when passwords are changed.</t>
+          <t>Red Hat Enterprise Linux 9 must require the change of at least 50% of the total number of characters when passwords are changed.</t>
         </is>
       </c>
       <c r="G95" s="2" t="inlineStr">
@@ -7184,7 +7426,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1), AC-18 (1), SC-8 (1), SC-8</t>
+          <t>AC-18 (1),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7197,7 +7439,11 @@
           <t>SRG-OS-000299-GPOS-00117,SRG-OS-000300-GPOS-00118,SRG-OS-000424-GPOS-00188,SRG-OS-000481-GPOS-000481</t>
         </is>
       </c>
-      <c r="D96" s="2" t="inlineStr"/>
+      <c r="D96" s="2" t="inlineStr">
+        <is>
+          <t>CCE-84066-0</t>
+        </is>
+      </c>
       <c r="E96" s="2" t="inlineStr">
         <is>
           <t>The operating system must protect wireless access to and from the system using encryption.</t>
@@ -7205,7 +7451,7 @@
       </c>
       <c r="F96" s="2" t="inlineStr">
         <is>
-          <t>The operating system must protect wireless access to and from the system using encryption.</t>
+          <t>Red Hat Enterprise Linux 9 must protect wireless access to and from the system using encryption.</t>
         </is>
       </c>
       <c r="G96" s="2" t="inlineStr">
@@ -7260,7 +7506,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (a), AU-8 (1) (b), AU-8 b</t>
+          <t>AU-8 b,AU-8 (1) (a),AU-8 (1) (b)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7273,7 +7519,11 @@
           <t>SRG-OS-000355-GPOS-00143,SRG-OS-000356-GPOS-00144,SRG-OS-000359-GPOS-00146</t>
         </is>
       </c>
-      <c r="D97" s="2" t="inlineStr"/>
+      <c r="D97" s="2" t="inlineStr">
+        <is>
+          <t>CCE-88648-1</t>
+        </is>
+      </c>
       <c r="E97" s="2" t="inlineStr">
         <is>
           <t>The operating system must synchronize internal information system clocks to the authoritative time source when the time difference is greater than one second.</t>
@@ -7281,7 +7531,7 @@
       </c>
       <c r="F97" s="2" t="inlineStr">
         <is>
-          <t>The operating system must synchronize internal information system clocks to the authoritative time source when the time difference is greater than one second.</t>
+          <t>Red Hat Enterprise Linux 9 must synchronize internal information system clocks to the authoritative time source when the time difference is greater than one second.</t>
         </is>
       </c>
       <c r="G97" s="2" t="inlineStr">
@@ -7346,7 +7596,11 @@
           <t>SRG-OS-000259-GPOS-00100</t>
         </is>
       </c>
-      <c r="D98" s="2" t="inlineStr"/>
+      <c r="D98" s="2" t="inlineStr">
+        <is>
+          <t>CCE-89858-5</t>
+        </is>
+      </c>
       <c r="E98" s="2" t="inlineStr">
         <is>
           <t>The operating system must limit privileges to change software resident within software libraries.</t>
@@ -7354,7 +7608,7 @@
       </c>
       <c r="F98" s="2" t="inlineStr">
         <is>
-          <t>The operating system must limit privileges to change software resident within software libraries.</t>
+          <t>Red Hat Enterprise Linux 9 must limit privileges to change software resident within software libraries.</t>
         </is>
       </c>
       <c r="G98" s="2" t="inlineStr">
@@ -7408,7 +7662,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-9, AU-9, AU-9</t>
+          <t>AU-9</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -7421,7 +7675,11 @@
           <t>SRG-OS-000057-GPOS-00027,SRG-OS-000058-GPOS-00028,SRG-OS-000059-GPOS-00029</t>
         </is>
       </c>
-      <c r="D99" s="2" t="inlineStr"/>
+      <c r="D99" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83716-1</t>
+        </is>
+      </c>
       <c r="E99" s="2" t="inlineStr">
         <is>
           <t>The operating system must protect audit information from unauthorized read access.</t>
@@ -7429,7 +7687,7 @@
       </c>
       <c r="F99" s="2" t="inlineStr">
         <is>
-          <t>The operating system must protect audit information from unauthorized read access.</t>
+          <t>Red Hat Enterprise Linux 9 must protect audit information from unauthorized read access.</t>
         </is>
       </c>
       <c r="G99" s="2" t="inlineStr">
@@ -7497,7 +7755,7 @@
       </c>
       <c r="F100" s="2" t="inlineStr">
         <is>
-          <t>The operating system must allow the use of a temporary password for system logons with an immediate change to a permanent password.</t>
+          <t>Red Hat Enterprise Linux 9 must allow the use of a temporary password for system logons with an immediate change to a permanent password.</t>
         </is>
       </c>
       <c r="G100" s="2" t="inlineStr">
@@ -7506,10 +7764,17 @@
 Temporary passwords are typically used to allow access when new accounts are created or passwords are changed. It is common practice for administrators to create temporary passwords for user accounts which allow the users to log on, yet force them to change the password once they have successfully authenticated.</t>
         </is>
       </c>
-      <c r="H100" s="2" t="inlineStr"/>
+      <c r="H100" s="2" t="inlineStr">
+        <is>
+          <t>Without providing this capability, an account may be created without a password.
+Non-repudiation cannot be guaranteed once an account is created if a user is not forced to change the temporary password upon initial logon.
+Temporary passwords are typically used to allow access when new accounts are created or passwords are changed.
+It is common practice for administrators to create temporary passwords for user accounts that allow the users to log on, yet force them to change the password once they have successfully authenticated.</t>
+        </is>
+      </c>
       <c r="I100" s="2" t="inlineStr">
         <is>
-          <t>Applicable - Configurable</t>
+          <t>Applicable - Inherently Met</t>
         </is>
       </c>
       <c r="J100" s="2" t="inlineStr">
@@ -7517,7 +7782,12 @@
           <t>Verify the operating system allows the use of a temporary password for system logons with an immediate change to a permanent password. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K100" s="2" t="n"/>
+      <c r="K100" s="2" t="inlineStr">
+        <is>
+          <t>Red Hat Enterprise Linux 9 supports this requirement and cannot be configured to be out of compliance.
+Red Hat Enterprise Linux 9 inherently meets this requirement.</t>
+        </is>
+      </c>
       <c r="L100" s="2" t="n"/>
       <c r="M100" s="2" t="n"/>
       <c r="N100" s="2" t="inlineStr">
@@ -7526,13 +7796,26 @@
         </is>
       </c>
       <c r="O100" s="2" t="n"/>
-      <c r="P100" s="2" t="n"/>
-      <c r="Q100" s="2" t="n"/>
+      <c r="P100" s="2" t="inlineStr">
+        <is>
+          <t>Red Hat Enterprise Linux 9 offers the following commands to facilitate the use of a temporary password.
+chage -d 0 [username]
+(forces the user to change their password at next logon)
+passwd -e [username]
+(expires the passwd for a given user forcing a change at next logon.)</t>
+        </is>
+      </c>
+      <c r="Q100" s="2" t="inlineStr">
+        <is>
+          <t>Red Hat Enterprise Linux 9 has the capability to perform temporary passwords based on organization policy.
+Configuration is not appropriate to define at an enterprise level.</t>
+        </is>
+      </c>
     </row>
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>IA-11, AC-3 (4)</t>
+          <t>AC-3 (4),IA-11</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -7545,7 +7828,11 @@
           <t>SRG-OS-000373-GPOS-00156,SRG-OS-000312-GPOS-00123</t>
         </is>
       </c>
-      <c r="D101" s="2" t="inlineStr"/>
+      <c r="D101" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90085-2</t>
+        </is>
+      </c>
       <c r="E101" s="2" t="inlineStr">
         <is>
           <t>The operating system must require users to re-authenticate for privilege escalation.</t>
@@ -7553,7 +7840,7 @@
       </c>
       <c r="F101" s="2" t="inlineStr">
         <is>
-          <t>The operating system must require users to re-authenticate for privilege escalation.</t>
+          <t>Red Hat Enterprise Linux 9 must require users to re-authenticate for privilege escalation.</t>
         </is>
       </c>
       <c r="G101" s="2" t="inlineStr">
@@ -7602,7 +7889,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3 (1), AU-12 a, MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -7615,7 +7902,11 @@
           <t>SRG-OS-000037-GPOS-00015,SRG-OS-000042-GPOS-00020,SRG-OS-000062-GPOS-00031,SRG-OS-000392-GPOS-00172,SRG-OS-000462-GPOS-00206,SRG-OS-000471-GPOS-00215,SRG-OS-000471-GPOS-00216,SRG-OS-000477-GPOS-00222</t>
         </is>
       </c>
-      <c r="D102" s="2" t="inlineStr"/>
+      <c r="D102" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83802-9</t>
+        </is>
+      </c>
       <c r="E102" s="2" t="inlineStr">
         <is>
           <t>The operating system must generate audit records for all kernel module load, unload, and restart actions, and also for all program initiations.</t>
@@ -7623,7 +7914,7 @@
       </c>
       <c r="F102" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records for all kernel module load, unload, and restart actions, and also for all program initiations.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records for all kernel module load, unload, and restart actions, and also for all program initiations.</t>
         </is>
       </c>
       <c r="G102" s="2" t="inlineStr">
@@ -7693,7 +7984,7 @@
       </c>
       <c r="F103" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement replay-resistant authentication mechanisms for network access to non-privileged accounts.</t>
+          <t>Red Hat Enterprise Linux 9 system must implement replay-resistant authentication mechanisms for network access to non-privileged accounts.</t>
         </is>
       </c>
       <c r="G103" s="2" t="inlineStr">
@@ -7707,7 +7998,7 @@
       <c r="H103" s="2" t="inlineStr"/>
       <c r="I103" s="2" t="inlineStr">
         <is>
-          <t>Applicable - Configurable</t>
+          <t>Applicable - Inherently Met</t>
         </is>
       </c>
       <c r="J103" s="2" t="inlineStr">
@@ -7715,17 +8006,36 @@
           <t>Verify the operating system implements replay-resistant authentication mechanisms for network access to non-privileged accounts. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K103" s="2" t="n"/>
+      <c r="K103" s="2" t="inlineStr">
+        <is>
+          <t>Red Hat Enterprise Linux 9 supports this requirement and cannot be configured to be out of compliance.
+Red Hat Enterprise Linux 9 inherently meets this requirement.</t>
+        </is>
+      </c>
       <c r="L103" s="2" t="n"/>
-      <c r="M103" s="2" t="n"/>
+      <c r="M103" s="2" t="inlineStr">
+        <is>
+          <t>Red Hat Enterprise Linux 9 inherently meets this requirement.
+No fix is required.</t>
+        </is>
+      </c>
       <c r="N103" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
         </is>
       </c>
       <c r="O103" s="2" t="n"/>
-      <c r="P103" s="2" t="n"/>
-      <c r="Q103" s="2" t="n"/>
+      <c r="P103" s="2" t="inlineStr">
+        <is>
+          <t>The release notes of OpenSSH 7.6 states "OpenSSH is a 100% complete SSH protocol 2.0 implementation and includes sftp client and server support."
+https://www.openssh.com/txt/release-7.6</t>
+        </is>
+      </c>
+      <c r="Q103" s="2" t="inlineStr">
+        <is>
+          <t>The OpenSSH package in Red Hat Enterprise Linux 9 is version 8.7, which is newer than 7.6 which only supports SSH protocol 2.0 which is restraint to replay attacks.</t>
+        </is>
+      </c>
     </row>
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
@@ -7751,7 +8061,7 @@
       </c>
       <c r="F104" s="2" t="inlineStr">
         <is>
-          <t>The operating system must audit all account enabling actions.</t>
+          <t>Red Hat Enterprise Linux 9 must audit all account enabling actions.</t>
         </is>
       </c>
       <c r="G104" s="2" t="inlineStr">
@@ -7799,7 +8109,11 @@
           <t>SRG-OS-000327-GPOS-00127</t>
         </is>
       </c>
-      <c r="D105" s="2" t="inlineStr"/>
+      <c r="D105" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83759-1</t>
+        </is>
+      </c>
       <c r="E105" s="2" t="inlineStr">
         <is>
           <t>The operating system must audit the execution of privileged functions.</t>
@@ -7807,7 +8121,7 @@
       </c>
       <c r="F105" s="2" t="inlineStr">
         <is>
-          <t>The operating system must audit the execution of privileged functions.</t>
+          <t>Red Hat Enterprise Linux 9 must audit the execution of privileged functions.</t>
         </is>
       </c>
       <c r="G105" s="2" t="inlineStr">
@@ -7887,7 +8201,7 @@
       </c>
       <c r="F106" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records for all direct access to the information system.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records for all direct access to the information system.</t>
         </is>
       </c>
       <c r="G106" s="2" t="inlineStr">
@@ -7943,7 +8257,7 @@
       </c>
       <c r="F107" s="2" t="inlineStr">
         <is>
-          <t>The operating system must provide a report generation capability that supports on-demand reporting requirements.</t>
+          <t>Red Hat Enterprise Linux 9 must provide a report generation capability that supports on-demand reporting requirements.</t>
         </is>
       </c>
       <c r="G107" s="2" t="inlineStr">
@@ -7999,7 +8313,7 @@
       </c>
       <c r="F108" s="2" t="inlineStr">
         <is>
-          <t>The operating system must protect audit information from unauthorized deletion.</t>
+          <t>Red Hat Enterprise Linux 9 must protect audit information from unauthorized deletion.</t>
         </is>
       </c>
       <c r="G108" s="2" t="inlineStr">
@@ -8133,7 +8447,7 @@
       </c>
       <c r="F110" s="2" t="inlineStr">
         <is>
-          <t>The operating system must maintain the confidentiality and integrity of information during reception.</t>
+          <t>Red Hat Enterprise Linux 9 must maintain the confidentiality and integrity of information during reception.</t>
         </is>
       </c>
       <c r="G110" s="2" t="inlineStr">
@@ -8169,7 +8483,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a, AU-5 b</t>
+          <t>AU-5 a,AU-5 b</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -8182,7 +8496,11 @@
           <t>SRG-OS-000046-GPOS-00022,SRG-OS-000047-GPOS-00023</t>
         </is>
       </c>
-      <c r="D111" s="2" t="inlineStr"/>
+      <c r="D111" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83709-6</t>
+        </is>
+      </c>
       <c r="E111" s="2" t="inlineStr">
         <is>
           <t>The operating system must shut down by default upon audit failure (unless availability is an overriding concern).</t>
@@ -8190,7 +8508,7 @@
       </c>
       <c r="F111" s="2" t="inlineStr">
         <is>
-          <t>The operating system must shut down by default upon audit failure (unless availability is an overriding concern).</t>
+          <t>Red Hat Enterprise Linux 9 must shut down by default upon audit failure (unless availability is an overriding concern).</t>
         </is>
       </c>
       <c r="G111" s="2" t="inlineStr">
@@ -8267,7 +8585,7 @@
       </c>
       <c r="F112" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records when concurrent logons to the same account occur from different sources.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records when concurrent logons to the same account occur from different sources.</t>
         </is>
       </c>
       <c r="G112" s="2" t="inlineStr">
@@ -8323,7 +8641,7 @@
       </c>
       <c r="F113" s="2" t="inlineStr">
         <is>
-          <t>The operating system must allow operating system admins to grant their privileges to other operating system admins.</t>
+          <t>Red Hat Enterprise Linux 9 must allow operating system admins to grant their privileges to other operating system admins.</t>
         </is>
       </c>
       <c r="G113" s="2" t="inlineStr">
@@ -8379,7 +8697,7 @@
       </c>
       <c r="F114" s="2" t="inlineStr">
         <is>
-          <t>The operating system must provide a report generation capability that supports after-the-fact investigations of security incidents.</t>
+          <t>Red Hat Enterprise Linux 9 must provide a report generation capability that supports after-the-fact investigations of security incidents.</t>
         </is>
       </c>
       <c r="G114" s="2" t="inlineStr">
@@ -8518,7 +8836,7 @@
       </c>
       <c r="F116" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">The operating system must notify system administrators and ISSOs when accounts are disabled. </t>
+          <t xml:space="preserve">Red Hat Enterprise Linux 9 must notify system administrators and ISSOs when accounts are disabled. </t>
         </is>
       </c>
       <c r="G116" s="2" t="inlineStr">
@@ -8571,7 +8889,11 @@
           <t>SRG-OS-000437-GPOS-00194</t>
         </is>
       </c>
-      <c r="D117" s="2" t="inlineStr"/>
+      <c r="D117" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83458-0</t>
+        </is>
+      </c>
       <c r="E117" s="2" t="inlineStr">
         <is>
           <t>The operating system must remove all software components after updated versions have been installed.</t>
@@ -8711,7 +9033,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3 (1), AU-12 a, MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -8724,7 +9046,11 @@
           <t>SRG-OS-000037-GPOS-00015,SRG-OS-000042-GPOS-00020,SRG-OS-000062-GPOS-00031,SRG-OS-000392-GPOS-00172,SRG-OS-000458-GPOS-00203,SRG-OS-000462-GPOS-00206,SRG-OS-000463-GPOS-00207,SRG-OS-000468-GPOS-00212,SRG-OS-000471-GPOS-00215,SRG-OS-000474-GPOS-00219,SRG-OS-000064-GPOS-00033</t>
         </is>
       </c>
-      <c r="D119" s="2" t="inlineStr"/>
+      <c r="D119" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83817-7</t>
+        </is>
+      </c>
       <c r="E119" s="2" t="inlineStr">
         <is>
           <t>The operating system must generate audit records when successful/unsuccessful attempts to delete security objects occur.</t>
@@ -8732,7 +9058,7 @@
       </c>
       <c r="F119" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records when successful/unsuccessful attempts to delete security objects occur.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records when successful/unsuccessful attempts to delete security objects occur.</t>
         </is>
       </c>
       <c r="G119" s="2" t="inlineStr">
@@ -8878,7 +9204,7 @@
       </c>
       <c r="F121" s="2" t="inlineStr">
         <is>
-          <t>The operating system must behave in a predictable and documented manner that reflects organizational and system objectives when invalid inputs are received.</t>
+          <t>Red Hat Enterprise Linux 9 must behave in a predictable and documented manner that reflects organizational and system objectives when invalid inputs are received.</t>
         </is>
       </c>
       <c r="G121" s="2" t="inlineStr">
@@ -8947,7 +9273,11 @@
           <t>SRG-OS-000378-GPOS-00163</t>
         </is>
       </c>
-      <c r="D122" s="2" t="inlineStr"/>
+      <c r="D122" s="2" t="inlineStr">
+        <is>
+          <t>CCE-84203-9</t>
+        </is>
+      </c>
       <c r="E122" s="2" t="inlineStr">
         <is>
           <t>The operating system must authenticate peripherals before establishing a connection.</t>
@@ -8955,7 +9285,7 @@
       </c>
       <c r="F122" s="2" t="inlineStr">
         <is>
-          <t>The operating system must authenticate peripherals before establishing a connection.</t>
+          <t>Red Hat Enterprise Linux 9 must authenticate peripherals before establishing a connection.</t>
         </is>
       </c>
       <c r="G122" s="2" t="inlineStr">
@@ -9001,7 +9331,7 @@
     <row r="123" ht="130" customHeight="1">
       <c r="A123" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b, CM-7 a</t>
+          <t>CM-7 a,CM-7 b</t>
         </is>
       </c>
       <c r="B123" s="2" t="inlineStr">
@@ -9014,7 +9344,11 @@
           <t>SRG-OS-000096-GPOS-00050,SRG-OS-000095-GPOS-00049</t>
         </is>
       </c>
-      <c r="D123" s="2" t="inlineStr"/>
+      <c r="D123" s="2" t="inlineStr">
+        <is>
+          <t>CCE-87543-5</t>
+        </is>
+      </c>
       <c r="E123" s="2" t="inlineStr">
         <is>
           <t>The operating system must be configured to prohibit or restrict the use of functions, ports, protocols, and/or services, as defined in the PPSM CAL and vulnerability assessments.</t>
@@ -9022,7 +9356,7 @@
       </c>
       <c r="F123" s="2" t="inlineStr">
         <is>
-          <t>The operating system must be configured to prohibit or restrict the use of functions, ports, protocols, and/or services, as defined in the PPSM CAL and vulnerability assessments.</t>
+          <t>Red Hat Enterprise Linux 9 must be configured to prohibit or restrict the use of functions, ports, protocols, and/or services, as defined in the PPSM CAL and vulnerability assessments.</t>
         </is>
       </c>
       <c r="G123" s="2" t="inlineStr">
@@ -9071,7 +9405,7 @@
     <row r="124" ht="130" customHeight="1">
       <c r="A124" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3 (1), AU-12 a, MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B124" s="2" t="inlineStr">
@@ -9084,7 +9418,11 @@
           <t>SRG-OS-000037-GPOS-00015,SRG-OS-000042-GPOS-00020,SRG-OS-000062-GPOS-00031,SRG-OS-000392-GPOS-00172,SRG-OS-000462-GPOS-00206,SRG-OS-000471-GPOS-00215,SRG-OS-000466-GPOS-00210,SRG-OS-000467-GPOS-00211,SRG-OS-000468-GPOS-00212</t>
         </is>
       </c>
-      <c r="D124" s="2" t="inlineStr"/>
+      <c r="D124" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83754-2</t>
+        </is>
+      </c>
       <c r="E124" s="2" t="inlineStr">
         <is>
           <t>The operating system must generate audit records when successful/unsuccessful attempts to delete security levels occur.</t>
@@ -9092,7 +9430,7 @@
       </c>
       <c r="F124" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records when successful/unsuccessful attempts to delete security levels occur.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records when successful/unsuccessful attempts to delete security levels occur.</t>
         </is>
       </c>
       <c r="G124" s="2" t="inlineStr">
@@ -9141,7 +9479,7 @@
     <row r="125" ht="130" customHeight="1">
       <c r="A125" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a, AC-18 (1)</t>
+          <t>CM-7 a,AC-18 (1)</t>
         </is>
       </c>
       <c r="B125" s="2" t="inlineStr">
@@ -9154,7 +9492,11 @@
           <t>SRG-OS-000095-GPOS-00049,SRG-OS-000300-GPOS-00118</t>
         </is>
       </c>
-      <c r="D125" s="2" t="inlineStr"/>
+      <c r="D125" s="2" t="inlineStr">
+        <is>
+          <t>CCE-84067-8</t>
+        </is>
+      </c>
       <c r="E125" s="2" t="inlineStr">
         <is>
           <t>The operating system must protect wireless access to the system using authentication of users and/or devices.</t>
@@ -9162,7 +9504,7 @@
       </c>
       <c r="F125" s="2" t="inlineStr">
         <is>
-          <t>The operating system must protect wireless access to the system using authentication of users and/or devices.</t>
+          <t>Red Hat Enterprise Linux 9 must protect wireless access to the system using authentication of users and/or devices.</t>
         </is>
       </c>
       <c r="G125" s="2" t="inlineStr">
@@ -9235,7 +9577,7 @@
       </c>
       <c r="F126" s="2" t="inlineStr">
         <is>
-          <t>The operating system must audit all account disabling actions.</t>
+          <t>Red Hat Enterprise Linux 9 must audit all account disabling actions.</t>
         </is>
       </c>
       <c r="G126" s="2" t="inlineStr">
@@ -9291,7 +9633,7 @@
       </c>
       <c r="F127" s="2" t="inlineStr">
         <is>
-          <t>The operating system must record time stamps for audit records that meet a minimum granularity of one second for a minimum degree of precision.</t>
+          <t>Red Hat Enterprise Linux 9 must record time stamps for audit records that meet a minimum granularity of one second for a minimum degree of precision.</t>
         </is>
       </c>
       <c r="G127" s="2" t="inlineStr">
@@ -9326,7 +9668,7 @@
     <row r="128" ht="130" customHeight="1">
       <c r="A128" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c), CM-7 a, CM-6 b</t>
+          <t>IA-5 (1) (c),CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B128" s="2" t="inlineStr">
@@ -9339,7 +9681,11 @@
           <t>SRG-OS-000074-GPOS-00042,SRG-OS-000095-GPOS-00049,SRG-OS-000480-GPOS-00227</t>
         </is>
       </c>
-      <c r="D128" s="2" t="inlineStr"/>
+      <c r="D128" s="2" t="inlineStr">
+        <is>
+          <t>CCE-84159-3</t>
+        </is>
+      </c>
       <c r="E128" s="2" t="inlineStr">
         <is>
           <t>The operating system must transmit only encrypted representations of passwords.</t>
@@ -9553,7 +9899,11 @@
           <t>SRG-OS-000071-GPOS-00039</t>
         </is>
       </c>
-      <c r="D131" s="2" t="inlineStr"/>
+      <c r="D131" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83566-0</t>
+        </is>
+      </c>
       <c r="E131" s="2" t="inlineStr">
         <is>
           <t>The operating system must enforce password complexity by requiring that at least one numeric character be used.</t>
@@ -9643,7 +9993,7 @@
       </c>
       <c r="F132" s="2" t="inlineStr">
         <is>
-          <t>The operating system must authenticate all endpoint devices before establishing a local, remote, and/or network connection using bidirectional authentication that is cryptographically based.</t>
+          <t>Red Hat Enterprise Linux 9 must authenticate all endpoint devices before establishing a local, remote, and/or network connection using bidirectional authentication that is cryptographically based.</t>
         </is>
       </c>
       <c r="G132" s="2" t="inlineStr">
@@ -9758,7 +10108,11 @@
           <t>SRG-OS-000046-GPOS-00022</t>
         </is>
       </c>
-      <c r="D134" s="2" t="inlineStr"/>
+      <c r="D134" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90826-9</t>
+        </is>
+      </c>
       <c r="E134" s="2" t="inlineStr">
         <is>
           <t>The operating system must alert the ISSO and SA (at a minimum) in the event of an audit processing failure.</t>
@@ -9766,7 +10120,7 @@
       </c>
       <c r="F134" s="2" t="inlineStr">
         <is>
-          <t>The operating system must alert the ISSO and SA (at a minimum) in the event of an audit processing failure.</t>
+          <t>Red Hat Enterprise Linux 9 must alert the ISSO and SA (at a minimum) in the event of an audit processing failure.</t>
         </is>
       </c>
       <c r="G134" s="2" t="inlineStr">
@@ -9830,7 +10184,11 @@
           <t>SRG-OS-000080-GPOS-00048</t>
         </is>
       </c>
-      <c r="D135" s="2" t="inlineStr"/>
+      <c r="D135" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83592-6</t>
+        </is>
+      </c>
       <c r="E135" s="2" t="inlineStr">
         <is>
           <t>The operating system must enforce approved authorizations for logical access to information and system resources in accordance with applicable access control policies.</t>
@@ -9838,7 +10196,7 @@
       </c>
       <c r="F135" s="2" t="inlineStr">
         <is>
-          <t>The operating system must enforce approved authorizations for logical access to information and system resources in accordance with applicable access control policies.</t>
+          <t>Red Hat Enterprise Linux 9 must enforce approved authorizations for logical access to information and system resources in accordance with applicable access control policies.</t>
         </is>
       </c>
       <c r="G135" s="2" t="inlineStr">
@@ -9888,7 +10246,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>AC-11 (1), AC-11 b</t>
+          <t>AC-11 b,AC-11 (1)</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -9901,7 +10259,11 @@
           <t>SRG-OS-000031-GPOS-00012,SRG-OS-000028-GPOS-00009</t>
         </is>
       </c>
-      <c r="D136" s="2" t="inlineStr"/>
+      <c r="D136" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90586-9</t>
+        </is>
+      </c>
       <c r="E136" s="2" t="inlineStr">
         <is>
           <t>The operating system must retain a users session lock until that user reestablishes access using established identification and authentication procedures.</t>
@@ -9996,7 +10358,7 @@
       </c>
       <c r="F137" s="2" t="inlineStr">
         <is>
-          <t>The operating system must notify system administrators and ISSOs when accounts are created.</t>
+          <t>Red Hat Enterprise Linux 9 must notify system administrators and ISSOs when accounts are created.</t>
         </is>
       </c>
       <c r="G137" s="2" t="inlineStr">
@@ -10109,7 +10471,7 @@
     <row r="139" ht="130" customHeight="1">
       <c r="A139" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5), SI-6 b, SI-6 d</t>
+          <t>SI-6 d,SI-6 b,CM-3 (5)</t>
         </is>
       </c>
       <c r="B139" s="2" t="inlineStr">
@@ -10122,7 +10484,11 @@
           <t>SRG-OS-000363-GPOS-00150,SRG-OS-000446-GPOS-00200,SRG-OS-000447-GPOS-00201</t>
         </is>
       </c>
-      <c r="D139" s="2" t="inlineStr"/>
+      <c r="D139" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83437-4</t>
+        </is>
+      </c>
       <c r="E139" s="2" t="inlineStr">
         <is>
           <t>The operating system must perform verification of the correct operation of security functions: upon system start-up and/or restart; upon command by a user with privileged access; and/or every 30 days.</t>
@@ -10130,7 +10496,7 @@
       </c>
       <c r="F139" s="2" t="inlineStr">
         <is>
-          <t>The operating system must perform verification of the correct operation of security functions: upon system start-up and/or restart; upon command by a user with privileged access; and/or every 30 days.</t>
+          <t>Red Hat Enterprise Linux 9 must perform verification of the correct operation of security functions: upon system start-up and/or restart; upon command by a user with privileged access; and/or every 30 days.</t>
         </is>
       </c>
       <c r="G139" s="2" t="inlineStr">
@@ -10210,7 +10576,7 @@
       </c>
       <c r="F140" s="2" t="inlineStr">
         <is>
-          <t>The operating system must be configured to disable non-essential capabilities.</t>
+          <t>Red Hat Enterprise Linux 9 must be configured to disable non-essential capabilities.</t>
         </is>
       </c>
       <c r="G140" s="2" t="inlineStr">
@@ -10267,7 +10633,7 @@
       </c>
       <c r="F141" s="2" t="inlineStr">
         <is>
-          <t>The operating system must provide an audit reduction capability that supports on-demand audit review and analysis.</t>
+          <t>Red Hat Enterprise Linux 9 must provide an audit reduction capability that supports on-demand audit review and analysis.</t>
         </is>
       </c>
       <c r="G141" s="2" t="inlineStr">
@@ -10302,7 +10668,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (2), AC-2 (2)</t>
+          <t>AC-2 (2)</t>
         </is>
       </c>
       <c r="B142" s="2" t="inlineStr">
@@ -10315,7 +10681,11 @@
           <t>SRG-OS-000123-GPOS-00064,SRG-OS-000002-GPOS-00002</t>
         </is>
       </c>
-      <c r="D142" s="2" t="inlineStr"/>
+      <c r="D142" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90560-4</t>
+        </is>
+      </c>
       <c r="E142" s="2" t="inlineStr">
         <is>
           <t>The operating system must automatically remove or disable temporary user accounts after 72 hours.</t>
@@ -10634,7 +11004,7 @@
       </c>
       <c r="F146" s="2" t="inlineStr">
         <is>
-          <t>The operating system must control remote access methods.</t>
+          <t>Red Hat Enterprise Linux 9 must control remote access methods.</t>
         </is>
       </c>
       <c r="G146" s="2" t="inlineStr">
@@ -10683,7 +11053,11 @@
           <t>SRG-OS-000032-GPOS-00013</t>
         </is>
       </c>
-      <c r="D147" s="2" t="inlineStr"/>
+      <c r="D147" s="2" t="inlineStr">
+        <is>
+          <t>CCE-86923-0</t>
+        </is>
+      </c>
       <c r="E147" s="2" t="inlineStr">
         <is>
           <t>The operating system must monitor remote access methods.</t>
@@ -10751,7 +11125,7 @@
     <row r="148" ht="130" customHeight="1">
       <c r="A148" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3 (1), AU-12 a, MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AU-14 (1)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-14 (1),AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B148" s="2" t="inlineStr">
@@ -10764,7 +11138,11 @@
           <t>SRG-OS-000037-GPOS-00015,SRG-OS-000042-GPOS-00020,SRG-OS-000062-GPOS-00031,SRG-OS-000392-GPOS-00172,SRG-OS-000462-GPOS-00206,SRG-OS-000471-GPOS-00215,SRG-OS-000473-GPOS-00218,SRG-OS-000254-GPOS-00095</t>
         </is>
       </c>
-      <c r="D148" s="2" t="inlineStr"/>
+      <c r="D148" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83651-0</t>
+        </is>
+      </c>
       <c r="E148" s="2" t="inlineStr">
         <is>
           <t>The operating system must initiate session audits at system start-up.</t>
@@ -10772,7 +11150,7 @@
       </c>
       <c r="F148" s="2" t="inlineStr">
         <is>
-          <t>The operating system must initiate session audits at system start-up.</t>
+          <t>Red Hat Enterprise Linux 9 must initiate session audits at system start-up.</t>
         </is>
       </c>
       <c r="G148" s="2" t="inlineStr">
@@ -10899,7 +11277,11 @@
           <t>SRG-OS-000063-GPOS-00032</t>
         </is>
       </c>
-      <c r="D150" s="2" t="inlineStr"/>
+      <c r="D150" s="2" t="inlineStr">
+        <is>
+          <t>CCE-89284-4</t>
+        </is>
+      </c>
       <c r="E150" s="2" t="inlineStr">
         <is>
           <t>The operating system must allow only the ISSM (or individuals or roles appointed by the ISSM) to select which auditable events are to be audited.</t>
@@ -11162,7 +11544,7 @@
       </c>
       <c r="F154" s="2" t="inlineStr">
         <is>
-          <t>The operating system must require users to re-authenticate when changing roles.</t>
+          <t>Red Hat Enterprise Linux 9 must require users to re-authenticate when changing roles.</t>
         </is>
       </c>
       <c r="G154" s="2" t="inlineStr">
@@ -11218,7 +11600,7 @@
       </c>
       <c r="F155" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement cryptographic mechanisms to protect the confidentiality of nonlocal maintenance and diagnostic communications, when used for nonlocal maintenance sessions.</t>
+          <t>Red Hat Enterprise Linux 9 must implement cryptographic mechanisms to protect the confidentiality of nonlocal maintenance and diagnostic communications, when used for nonlocal maintenance sessions.</t>
         </is>
       </c>
       <c r="G155" s="2" t="inlineStr">
@@ -11276,7 +11658,7 @@
       </c>
       <c r="F156" s="2" t="inlineStr">
         <is>
-          <t>The operating system must protect audit information from unauthorized modification.</t>
+          <t>Red Hat Enterprise Linux 9 must protect audit information from unauthorized modification.</t>
         </is>
       </c>
       <c r="G156" s="2" t="inlineStr">
@@ -11312,7 +11694,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3 (1), AU-12 a, MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B157" s="2" t="inlineStr">
@@ -11325,7 +11707,11 @@
           <t>SRG-OS-000037-GPOS-00015,SRG-OS-000042-GPOS-00020,SRG-OS-000062-GPOS-00031,SRG-OS-000392-GPOS-00172,SRG-OS-000462-GPOS-00206,SRG-OS-000468-GPOS-00212,SRG-OS-000471-GPOS-00215,SRG-OS-000463-GPOS-00207,SRG-OS-000465-GPOS-00209</t>
         </is>
       </c>
-      <c r="D157" s="2" t="inlineStr"/>
+      <c r="D157" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83748-4</t>
+        </is>
+      </c>
       <c r="E157" s="2" t="inlineStr">
         <is>
           <t>The operating system must generate audit records when successful/unsuccessful attempts to modify categories of information (e.g., classification levels) occur.</t>
@@ -11333,7 +11719,7 @@
       </c>
       <c r="F157" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records when successful/unsuccessful attempts to modify categories of information (e.g., classification levels) occur.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records when successful/unsuccessful attempts to modify categories of information (e.g., classification levels) occur.</t>
         </is>
       </c>
       <c r="G157" s="2" t="inlineStr">
@@ -11409,7 +11795,7 @@
       </c>
       <c r="F158" s="2" t="inlineStr">
         <is>
-          <t>The operating system must electronically verify Personal Identity Verification (PIV) credentials.</t>
+          <t>Red Hat Enterprise Linux 9 must electronically verify Personal Identity Verification (PIV) credentials.</t>
         </is>
       </c>
       <c r="G158" s="2" t="inlineStr">
@@ -11444,7 +11830,7 @@
     <row r="159" ht="130" customHeight="1">
       <c r="A159" s="2" t="inlineStr">
         <is>
-          <t>SC-8, AC-17 (2)</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B159" s="2" t="inlineStr">
@@ -11457,7 +11843,11 @@
           <t>SRG-OS-000423-GPOS-00187,SRG-OS-000033-GPOS-00014</t>
         </is>
       </c>
-      <c r="D159" s="2" t="inlineStr"/>
+      <c r="D159" s="2" t="inlineStr">
+        <is>
+          <t>CCE-87522-9</t>
+        </is>
+      </c>
       <c r="E159" s="2" t="inlineStr">
         <is>
           <t>The operating system must implement DoD-approved encryption to protect the confidentiality of remote access sessions.</t>
@@ -11465,7 +11855,7 @@
       </c>
       <c r="F159" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement DoD-approved encryption to protect the confidentiality of remote access sessions.</t>
+          <t>Red Hat Enterprise Linux 9 must implement DoD-approved encryption to protect the confidentiality of remote access sessions.</t>
         </is>
       </c>
       <c r="G159" s="2" t="inlineStr">
@@ -11605,7 +11995,11 @@
           <t>SRG-OS-000445-GPOS-00199</t>
         </is>
       </c>
-      <c r="D161" s="2" t="inlineStr"/>
+      <c r="D161" s="2" t="inlineStr">
+        <is>
+          <t>CCE-84074-4</t>
+        </is>
+      </c>
       <c r="E161" s="2" t="inlineStr">
         <is>
           <t>The operating system must verify correct operation of all security functions.</t>
@@ -11694,7 +12088,7 @@
       </c>
       <c r="F162" s="2" t="inlineStr">
         <is>
-          <t>The operating system must protect the confidentiality and integrity of communications with wireless peripherals.</t>
+          <t>Red Hat Enterprise Linux 9 must protect the confidentiality and integrity of communications with wireless peripherals.</t>
         </is>
       </c>
       <c r="G162" s="2" t="inlineStr">
@@ -11751,7 +12145,7 @@
       </c>
       <c r="F163" s="2" t="inlineStr">
         <is>
-          <t>The operating system must audit all activities performed during nonlocal maintenance and diagnostic sessions.</t>
+          <t>Red Hat Enterprise Linux 9 must audit all activities performed during nonlocal maintenance and diagnostic sessions.</t>
         </is>
       </c>
       <c r="G163" s="2" t="inlineStr">
@@ -11809,7 +12203,7 @@
       </c>
       <c r="F164" s="2" t="inlineStr">
         <is>
-          <t>The operating system must terminate all sessions and network connections related to nonlocal maintenance when nonlocal maintenance is completed.</t>
+          <t>Red Hat Enterprise Linux 9 must terminate all sessions and network connections related to nonlocal maintenance when nonlocal maintenance is completed.</t>
         </is>
       </c>
       <c r="G164" s="2" t="inlineStr">
@@ -11922,7 +12316,7 @@
       </c>
       <c r="F166" s="2" t="inlineStr">
         <is>
-          <t>The operating system must maintain the confidentiality and integrity of information during preparation for transmission.</t>
+          <t>Red Hat Enterprise Linux 9 must maintain the confidentiality and integrity of information during preparation for transmission.</t>
         </is>
       </c>
       <c r="G166" s="2" t="inlineStr">
@@ -11979,7 +12373,7 @@
       </c>
       <c r="F167" s="2" t="inlineStr">
         <is>
-          <t>The operating system must enforce password complexity by requiring that at least one upper-case character be used.</t>
+          <t>Red Hat Enterprise Linux 9 must enforce password complexity by requiring that at least one upper-case character be used.</t>
         </is>
       </c>
       <c r="G167" s="2" t="inlineStr">
@@ -12035,7 +12429,7 @@
       </c>
       <c r="F168" s="2" t="inlineStr">
         <is>
-          <t>The operating system must automatically lock an account until the locked account is released by an administrator when three unsuccessful logon attempts in 15 minutes occur.</t>
+          <t>Red Hat Enterprise Linux 9 must automatically lock an account until the locked account is released by an administrator when three unsuccessful logon attempts in 15 minutes occur.</t>
         </is>
       </c>
       <c r="G168" s="2" t="inlineStr">
@@ -12090,7 +12484,7 @@
       </c>
       <c r="F169" s="2" t="inlineStr">
         <is>
-          <t>The operating system must record time stamps for audit records that can be mapped to Coordinated Universal Time (UTC) or Greenwich Mean Time (GMT).</t>
+          <t>Red Hat Enterprise Linux 9 must record time stamps for audit records that can be mapped to Coordinated Universal Time (UTC) or Greenwich Mean Time (GMT).</t>
         </is>
       </c>
       <c r="G169" s="2" t="inlineStr">
@@ -12138,7 +12532,11 @@
           <t>SRG-OS-000480-GPOS-00225</t>
         </is>
       </c>
-      <c r="D170" s="2" t="inlineStr"/>
+      <c r="D170" s="2" t="inlineStr">
+        <is>
+          <t>CCE-88413-0</t>
+        </is>
+      </c>
       <c r="E170" s="2" t="inlineStr">
         <is>
           <t>The operating system must prevent the use of dictionary words for passwords.</t>
@@ -12146,7 +12544,7 @@
       </c>
       <c r="F170" s="2" t="inlineStr">
         <is>
-          <t>The operating system must prevent the use of dictionary words for passwords.</t>
+          <t>Red Hat Enterprise Linux 9 must prevent the use of dictionary words for passwords.</t>
         </is>
       </c>
       <c r="G170" s="2" t="inlineStr">
@@ -12219,7 +12617,7 @@
       </c>
       <c r="F171" s="2" t="inlineStr">
         <is>
-          <t>The operating system must protect audit tools from unauthorized access.</t>
+          <t>Red Hat Enterprise Linux 9 must protect audit tools from unauthorized access.</t>
         </is>
       </c>
       <c r="G171" s="2" t="inlineStr">
@@ -12334,7 +12732,7 @@
       </c>
       <c r="F173" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records for privileged activities or other system-level access.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records for privileged activities or other system-level access.</t>
         </is>
       </c>
       <c r="G173" s="2" t="inlineStr">
@@ -12390,7 +12788,7 @@
       </c>
       <c r="F174" s="2" t="inlineStr">
         <is>
-          <t>The operating system must shut down the information system, restart the information system, and/or notify the system administrator when anomalies in the operation of any security functions are discovered.</t>
+          <t>Red Hat Enterprise Linux 9 must shut down the information system, restart the information system, and/or notify the system administrator when anomalies in the operation of any security functions are discovered.</t>
         </is>
       </c>
       <c r="G174" s="2" t="inlineStr">
@@ -12427,7 +12825,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="2" t="inlineStr">
         <is>
-          <t>SI-16, CM-7 a</t>
+          <t>SI-16,CM-7 a</t>
         </is>
       </c>
       <c r="B175" s="2" t="inlineStr">
@@ -12440,7 +12838,11 @@
           <t>SRG-OS-000433-GPOS-00193,SRG-OS-000095-GPOS-00049</t>
         </is>
       </c>
-      <c r="D175" s="2" t="inlineStr"/>
+      <c r="D175" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83843-3</t>
+        </is>
+      </c>
       <c r="E175" s="2" t="inlineStr">
         <is>
           <t>The operating system must implement address space layout randomization to protect its memory from unauthorized code execution.</t>
@@ -12448,7 +12850,7 @@
       </c>
       <c r="F175" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement address space layout randomization to protect its memory from unauthorized code execution.</t>
+          <t>Red Hat Enterprise Linux 9 must implement address space layout randomization to protect its memory from unauthorized code execution.</t>
         </is>
       </c>
       <c r="G175" s="2" t="inlineStr">
@@ -12527,7 +12929,7 @@
       </c>
       <c r="F176" s="2" t="inlineStr">
         <is>
-          <t>The operating system must, for networked systems, compare internal information system clocks at least every 24 hours with a server which is synchronized to one of the redundant United States Naval Observatory (USNO) time servers, or a time server designat</t>
+          <t>Red Hat Enterprise Linux 9 must, for networked systems, compare internal information system clocks at least every 24 hours with a server which is synchronized to one of the redundant United States Naval Observatory (USNO) time servers, or a time server designat</t>
         </is>
       </c>
       <c r="G176" s="2" t="inlineStr">
@@ -12576,7 +12978,11 @@
           <t>SRG-OS-000383-GPOS-00166</t>
         </is>
       </c>
-      <c r="D177" s="2" t="inlineStr"/>
+      <c r="D177" s="2" t="inlineStr">
+        <is>
+          <t>CCE-87996-5</t>
+        </is>
+      </c>
       <c r="E177" s="2" t="inlineStr">
         <is>
           <t>The operating system must prohibit the use of cached authenticators after one day.</t>
@@ -12584,7 +12990,7 @@
       </c>
       <c r="F177" s="2" t="inlineStr">
         <is>
-          <t>The operating system must prohibit the use of cached authenticators after one day.</t>
+          <t>Red Hat Enterprise Linux 9 must prohibit the use of cached authenticators after one day.</t>
         </is>
       </c>
       <c r="G177" s="2" t="inlineStr">
@@ -12652,7 +13058,7 @@
       </c>
       <c r="F178" s="2" t="inlineStr">
         <is>
-          <t>The operating system must audit all account modifications.</t>
+          <t>Red Hat Enterprise Linux 9 must audit all account modifications.</t>
         </is>
       </c>
       <c r="G178" s="2" t="inlineStr">
@@ -12764,7 +13170,7 @@
       </c>
       <c r="F180" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records for all account creations, modifications, disabling, and termination events.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records for all account creations, modifications, disabling, and termination events.</t>
         </is>
       </c>
       <c r="G180" s="2" t="inlineStr">
@@ -12799,7 +13205,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b, SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">
@@ -12812,7 +13218,11 @@
           <t>SRG-OS-000480-GPOS-00227,SRG-OS-000134-GPOS-00068</t>
         </is>
       </c>
-      <c r="D181" s="2" t="inlineStr"/>
+      <c r="D181" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83842-5</t>
+        </is>
+      </c>
       <c r="E181" s="2" t="inlineStr">
         <is>
           <t>The operating system must isolate security functions from nonsecurity functions.</t>
@@ -12820,7 +13230,7 @@
       </c>
       <c r="F181" s="2" t="inlineStr">
         <is>
-          <t>The operating system must isolate security functions from nonsecurity functions.</t>
+          <t>Red Hat Enterprise Linux 9 must isolate security functions from nonsecurity functions.</t>
         </is>
       </c>
       <c r="G181" s="2" t="inlineStr">
@@ -12864,7 +13274,16 @@
         </is>
       </c>
       <c r="L181" s="2" t="n"/>
-      <c r="M181" s="2" t="inlineStr"/>
+      <c r="M181" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">To ensure that "vsyscall=none" is added as a kernel command line
+argument to newly installed kernels, add "vsyscall=none" to the
+default Grub2 command line for Linux operating systems.  Modify the line within
+"/etc/default/grub" as shown below:
+ GRUB_CMDLINE_LINUX="... vsyscall=none ..." 
+Run the following command to update command line for already installed kernels: # grubby --update-kernel=ALL --args="vsyscall=none" </t>
+        </is>
+      </c>
       <c r="N181" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -13046,7 +13465,11 @@
           <t>SRG-OS-000480-GPOS-00229</t>
         </is>
       </c>
-      <c r="D184" s="2" t="inlineStr"/>
+      <c r="D184" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90816-0</t>
+        </is>
+      </c>
       <c r="E184" s="2" t="inlineStr">
         <is>
           <t>The operating system must not allow an unattended or automatic logon to the system.</t>
@@ -13120,7 +13543,11 @@
           <t>SRG-OS-000480-GPOS-00227</t>
         </is>
       </c>
-      <c r="D185" s="2" t="inlineStr"/>
+      <c r="D185" s="2" t="inlineStr">
+        <is>
+          <t>CCE-84232-8</t>
+        </is>
+      </c>
       <c r="E185" s="2" t="inlineStr">
         <is>
           <t>The operating system must be configured in accordance with the security configuration settings based on DoD security configuration or implementation guidance, including STIGs, NSA configuration guides, CTOs, and DTMs.</t>
@@ -13128,7 +13555,7 @@
       </c>
       <c r="F185" s="2" t="inlineStr">
         <is>
-          <t>The operating system must be configured in accordance with the security configuration settings based on DoD security configuration or implementation guidance, including STIGs, NSA configuration guides, CTOs, and DTMs.</t>
+          <t>Red Hat Enterprise Linux 9 must be configured in accordance with the security configuration settings based on DoD security configuration or implementation guidance, including STIGs, NSA configuration guides, CTOs, and DTMs.</t>
         </is>
       </c>
       <c r="G185" s="2" t="inlineStr">
@@ -13293,7 +13720,7 @@
       </c>
       <c r="F187" s="2" t="inlineStr">
         <is>
-          <t>The operating system must enforce a minimum 15-character password length.</t>
+          <t>Red Hat Enterprise Linux 9 must enforce a minimum 15-character password length.</t>
         </is>
       </c>
       <c r="G187" s="2" t="inlineStr">
@@ -13420,7 +13847,7 @@
       </c>
       <c r="F189" s="2" t="inlineStr">
         <is>
-          <t>The operating system must audit the enforcement actions used to restrict access associated with changes to the system.</t>
+          <t>Red Hat Enterprise Linux 9 must audit the enforcement actions used to restrict access associated with changes to the system.</t>
         </is>
       </c>
       <c r="G189" s="2" t="inlineStr">
@@ -13476,7 +13903,7 @@
       </c>
       <c r="F190" s="2" t="inlineStr">
         <is>
-          <t>The operating system must notify designated personnel if baseline configurations are changed in an unauthorized manner.</t>
+          <t>Red Hat Enterprise Linux 9 must notify designated personnel if baseline configurations are changed in an unauthorized manner.</t>
         </is>
       </c>
       <c r="G190" s="2" t="inlineStr">
@@ -13612,7 +14039,7 @@
       </c>
       <c r="F192" s="2" t="inlineStr">
         <is>
-          <t>The operating system must protect the confidentiality and integrity of all information at rest.</t>
+          <t>Red Hat Enterprise Linux 9 must protect the confidentiality and integrity of all information at rest.</t>
         </is>
       </c>
       <c r="G192" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@28b8916bcf3dcf6146b687f891d01093e193fe9a 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -784,7 +784,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-5 (2),SC-5</t>
+          <t>SC-5,CM-6 b,SC-5 (2)</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -883,7 +883,7 @@
     <row r="6" ht="130" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (9),AU-7 b,AU-12 (3),CM-5 (1),AU-7 a,AC-6 (8),AU-8 b</t>
+          <t>AC-6 (9),AU-7 b,CM-5 (1),AU-7 a,AC-6 (8),AU-12 (3),AU-8 b</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -963,7 +963,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-7 b,AU-12 c,AU-12 (3),AU-12 a,CM-5 (1),AU-7 a,CM-6 b,AU-8 b</t>
+          <t>AU-12 a,AU-7 b,CM-6 b,CM-5 (1),AU-7 a,AU-12 c,AU-12 (3),AU-8 b</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1037,7 +1037,7 @@
     <row r="8" ht="130" customHeight="1">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (9),CM-6 b,CM-7 b,AC-17 (1)</t>
+          <t>AC-17 (9),AC-17 (1),CM-7 b,CM-6 b</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
@@ -1257,7 +1257,7 @@
     <row r="11" ht="130" customHeight="1">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B11" s="2" t="inlineStr">
@@ -1334,7 +1334,7 @@
     <row r="12" ht="130" customHeight="1">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
@@ -1484,7 +1484,7 @@
     <row r="14" ht="130" customHeight="1">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -1560,7 +1560,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -3832,7 +3832,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>IA-2,IA-8,AU-3 (1)</t>
+          <t>AU-3 (1),IA-2,IA-8</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3910,7 +3910,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -3985,7 +3985,7 @@
     <row r="47" ht="130" customHeight="1">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
@@ -4060,7 +4060,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4135,7 +4135,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4210,7 +4210,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4285,7 +4285,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4360,7 +4360,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
@@ -4435,7 +4435,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4510,7 +4510,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4585,7 +4585,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4660,7 +4660,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4735,7 +4735,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4810,7 +4810,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4885,7 +4885,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -4965,7 +4965,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5048,7 +5048,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5128,7 +5128,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5208,7 +5208,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5288,7 +5288,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5368,7 +5368,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5442,7 +5442,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5516,7 +5516,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5590,7 +5590,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5664,7 +5664,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5738,7 +5738,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5811,7 +5811,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5884,7 +5884,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -5957,7 +5957,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6030,7 +6030,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6103,7 +6103,7 @@
     <row r="75" ht="130" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
@@ -6176,7 +6176,7 @@
     <row r="76" ht="130" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
@@ -6250,7 +6250,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6324,7 +6324,7 @@
     <row r="78" ht="130" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
@@ -6398,7 +6398,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6469,7 +6469,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6549,7 +6549,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6629,7 +6629,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B82" s="2" t="inlineStr">
@@ -6709,7 +6709,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B83" s="2" t="inlineStr">
@@ -6789,7 +6789,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B84" s="2" t="inlineStr">
@@ -6949,7 +6949,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -7029,7 +7029,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7109,7 +7109,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7189,7 +7189,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7269,7 +7269,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7349,7 +7349,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7425,7 +7425,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
@@ -7502,7 +7502,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
@@ -7582,7 +7582,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B94" s="2" t="inlineStr">
@@ -7662,7 +7662,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
@@ -7742,7 +7742,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7822,7 +7822,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7902,7 +7902,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -7982,7 +7982,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8062,7 +8062,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8142,7 +8142,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8222,7 +8222,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8295,7 +8295,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3,AU-12 a</t>
+          <t>AC-2 (4),AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8376,7 +8376,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3,AU-12 a</t>
+          <t>AC-2 (4),AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8457,7 +8457,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3,AU-12 a</t>
+          <t>AC-2 (4),AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8528,7 +8528,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3</t>
+          <t>AC-2 (4),AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8603,7 +8603,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3,AU-12 a</t>
+          <t>AC-2 (4),AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8685,7 +8685,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3,AU-12 a</t>
+          <t>AC-2 (4),AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -8767,7 +8767,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3,AU-12 a</t>
+          <t>AC-2 (4),AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -8849,7 +8849,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3,AU-12 a</t>
+          <t>AC-2 (4),AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B110" s="2" t="inlineStr">
@@ -8931,7 +8931,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3,AU-12 a</t>
+          <t>AC-2 (4),AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9013,7 +9013,7 @@
     <row r="112" ht="130" customHeight="1">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-14 (1),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-3,AU-14 (1),AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
@@ -9707,7 +9707,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-12 c,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -9778,7 +9778,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-12 c,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -9849,7 +9849,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-12 c</t>
+          <t>AU-12 c,AU-9</t>
         </is>
       </c>
       <c r="B122" s="2" t="inlineStr">
@@ -10222,7 +10222,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (9),AC-2 (4),AU-12 c,CM-5 (1)</t>
+          <t>AC-2 (4),AU-12 c,AC-6 (9),CM-5 (1)</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -10345,7 +10345,7 @@
     <row r="129" ht="130" customHeight="1">
       <c r="A129" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (b),CM-6 b,IA-5 (1) (a)</t>
+          <t>IA-5 (1) (a),CM-6 b,IA-5 (1) (b)</t>
         </is>
       </c>
       <c r="B129" s="2" t="inlineStr">
@@ -10665,7 +10665,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>MA-4 c,SC-13,SC-8,AC-17 (2)</t>
+          <t>MA-4 c,SC-8,AC-17 (2),SC-13</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10747,7 +10747,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>MA-4 e,AC-12,MA-4 (7),SC-10</t>
+          <t>AC-12,SC-10,MA-4 (7),MA-4 e</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -10822,7 +10822,7 @@
     <row r="135" ht="130" customHeight="1">
       <c r="A135" s="2" t="inlineStr">
         <is>
-          <t>SC-10,AC-12</t>
+          <t>AC-12,SC-10</t>
         </is>
       </c>
       <c r="B135" s="2" t="inlineStr">
@@ -10901,7 +10901,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>SC-10,AC-12</t>
+          <t>AC-12,SC-10</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -11054,7 +11054,7 @@
     <row r="138" ht="130" customHeight="1">
       <c r="A138" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-14 (1),AU-7 (1),AU-3,AU-12 a,CM-5 (1),AU-6 (4),AU-7 a,CM-6 b</t>
+          <t>AU-12 a,AU-3,AU-14 (1),AU-3 (1),AU-7 (1),CM-6 b,AU-6 (4),MA-4 (1) (a),CM-5 (1),AU-7 a</t>
         </is>
       </c>
       <c r="B138" s="2" t="inlineStr">
@@ -13112,7 +13112,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8 (2),SC-8</t>
+          <t>SC-8 (2),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B166" s="2" t="inlineStr">
@@ -13265,7 +13265,7 @@
     <row r="168" ht="130" customHeight="1">
       <c r="A168" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2)</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B168" s="2" t="inlineStr">
@@ -13419,7 +13419,7 @@
     <row r="170" ht="130" customHeight="1">
       <c r="A170" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2)</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B170" s="2" t="inlineStr">
@@ -13494,7 +13494,7 @@
     <row r="171" ht="130" customHeight="1">
       <c r="A171" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (9),AC-2 (4),AU-12 c</t>
+          <t>AC-2 (4),AU-12 c,AC-6 (9)</t>
         </is>
       </c>
       <c r="B171" s="2" t="inlineStr">
@@ -13708,7 +13708,7 @@
     <row r="173" ht="130" customHeight="1">
       <c r="A173" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B173" s="2" t="inlineStr">
@@ -13786,7 +13786,7 @@
     <row r="174" ht="130" customHeight="1">
       <c r="A174" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B174" s="2" t="inlineStr">
@@ -13869,7 +13869,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B175" s="2" t="inlineStr">
@@ -14249,7 +14249,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="2" t="inlineStr">
         <is>
-          <t>AU-6 (4),CM-6 b,AU-4 (1)</t>
+          <t>CM-6 b,AU-6 (4),AU-4 (1)</t>
         </is>
       </c>
       <c r="B180" s="2" t="inlineStr">
@@ -14320,7 +14320,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 b,AC-17 (1)</t>
+          <t>CM-6 b,AC-17 (1),CM-7 b</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">
@@ -14399,7 +14399,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B182" s="2" t="inlineStr">
@@ -14471,7 +14471,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B183" s="2" t="inlineStr">
@@ -14543,7 +14543,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B184" s="2" t="inlineStr">
@@ -14617,7 +14617,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B185" s="2" t="inlineStr">
@@ -14691,7 +14691,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B186" s="2" t="inlineStr">
@@ -14765,7 +14765,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B187" s="2" t="inlineStr">
@@ -16315,7 +16315,7 @@
     <row r="208" ht="130" customHeight="1">
       <c r="A208" s="2" t="inlineStr">
         <is>
-          <t>SC-28 (1),SC-28</t>
+          <t>SC-28,SC-28 (1)</t>
         </is>
       </c>
       <c r="B208" s="2" t="inlineStr">
@@ -16629,7 +16629,7 @@
     <row r="212" ht="130" customHeight="1">
       <c r="A212" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B212" s="2" t="inlineStr">
@@ -16731,7 +16731,7 @@
     <row r="213" ht="130" customHeight="1">
       <c r="A213" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B213" s="2" t="inlineStr">
@@ -16841,7 +16841,7 @@
     <row r="214" ht="130" customHeight="1">
       <c r="A214" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B214" s="2" t="inlineStr">
@@ -16952,7 +16952,7 @@
     <row r="215" ht="130" customHeight="1">
       <c r="A215" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B215" s="2" t="inlineStr">
@@ -17440,7 +17440,7 @@
     <row r="221" ht="130" customHeight="1">
       <c r="A221" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2,IA-2 (2),IA-2 (3),IA-2 (5)</t>
+          <t>IA-2 (3),IA-2 (5),IA-2 (2),IA-2 (4),IA-2</t>
         </is>
       </c>
       <c r="B221" s="2" t="inlineStr">
@@ -17525,7 +17525,7 @@
     <row r="222" ht="130" customHeight="1">
       <c r="A222" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2,IA-2 (2),IA-2 (3),IA-2 (5)</t>
+          <t>IA-2 (3),IA-2 (5),IA-2 (2),IA-2 (4),IA-2</t>
         </is>
       </c>
       <c r="B222" s="2" t="inlineStr">
@@ -17610,7 +17610,7 @@
     <row r="223" ht="130" customHeight="1">
       <c r="A223" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),SC-8 (1),SC-8</t>
+          <t>SC-8,SC-8 (1),AC-18 (1)</t>
         </is>
       </c>
       <c r="B223" s="2" t="inlineStr">
@@ -17771,7 +17771,7 @@
     <row r="225" ht="130" customHeight="1">
       <c r="A225" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),IA-7</t>
+          <t>IA-7,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B225" s="2" t="inlineStr">
@@ -18172,7 +18172,7 @@
     <row r="230" ht="130" customHeight="1">
       <c r="A230" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-7 a</t>
+          <t>CM-7 a,IA-7</t>
         </is>
       </c>
       <c r="B230" s="2" t="inlineStr">
@@ -18251,7 +18251,7 @@
     <row r="231" ht="130" customHeight="1">
       <c r="A231" s="2" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B231" s="2" t="inlineStr">
@@ -18410,7 +18410,7 @@
     <row r="233" ht="130" customHeight="1">
       <c r="A233" s="2" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B233" s="2" t="inlineStr">
@@ -19240,7 +19240,7 @@
     <row r="244" ht="130" customHeight="1">
       <c r="A244" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-2,SI-16</t>
+          <t>CM-6 b,SI-16,SC-2</t>
         </is>
       </c>
       <c r="B244" s="2" t="inlineStr">
@@ -19400,7 +19400,7 @@
     <row r="246" ht="130" customHeight="1">
       <c r="A246" s="2" t="inlineStr">
         <is>
-          <t>SI-16,SC-3</t>
+          <t>SC-3,SI-16</t>
         </is>
       </c>
       <c r="B246" s="2" t="inlineStr">
@@ -20314,7 +20314,7 @@
     <row r="258" ht="130" customHeight="1">
       <c r="A258" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B258" s="2" t="inlineStr">
@@ -20389,7 +20389,7 @@
     <row r="259" ht="130" customHeight="1">
       <c r="A259" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B259" s="2" t="inlineStr">
@@ -20477,7 +20477,7 @@
     <row r="260" ht="130" customHeight="1">
       <c r="A260" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B260" s="2" t="inlineStr">
@@ -20554,7 +20554,7 @@
     <row r="261" ht="130" customHeight="1">
       <c r="A261" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B261" s="2" t="inlineStr">
@@ -20712,7 +20712,7 @@
     <row r="263" ht="130" customHeight="1">
       <c r="A263" s="2" t="inlineStr">
         <is>
-          <t>AU-5 (1),AU-5 a</t>
+          <t>AU-5 a,AU-5 (1)</t>
         </is>
       </c>
       <c r="B263" s="2" t="inlineStr">
@@ -21152,7 +21152,7 @@
     <row r="269" ht="130" customHeight="1">
       <c r="A269" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (2)</t>
+          <t>IA-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B269" s="2" t="inlineStr">
@@ -21239,7 +21239,7 @@
     <row r="270" ht="130" customHeight="1">
       <c r="A270" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (1),IA-2 (4),IA-2 (2)</t>
+          <t>IA-2 (2),IA-2 (4),IA-2 (3),IA-2 (1)</t>
         </is>
       </c>
       <c r="B270" s="2" t="inlineStr">
@@ -21626,7 +21626,7 @@
     <row r="275" ht="130" customHeight="1">
       <c r="A275" s="2" t="inlineStr">
         <is>
-          <t>SC-4,CM-6 b</t>
+          <t>CM-6 b,SC-4</t>
         </is>
       </c>
       <c r="B275" s="2" t="inlineStr">
@@ -22256,7 +22256,7 @@
     <row r="283" ht="130" customHeight="1">
       <c r="A283" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (3),CM-6 b</t>
+          <t>CM-6 b,CM-5 (3)</t>
         </is>
       </c>
       <c r="B283" s="2" t="inlineStr">
@@ -23356,7 +23356,7 @@
     <row r="297" ht="130" customHeight="1">
       <c r="A297" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B297" s="2" t="inlineStr">
@@ -23525,7 +23525,7 @@
     <row r="299" ht="130" customHeight="1">
       <c r="A299" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12),IA-2 (1)</t>
+          <t>IA-2 (12),IA-2 (11),IA-2 (1)</t>
         </is>
       </c>
       <c r="B299" s="2" t="inlineStr">
@@ -24347,7 +24347,7 @@
     <row r="309" ht="130" customHeight="1">
       <c r="A309" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (b),AU-8 b,AU-8 (1) (a)</t>
+          <t>AU-8 (1) (a),AU-8 (1) (b),AU-8 b</t>
         </is>
       </c>
       <c r="B309" s="2" t="inlineStr">
@@ -25300,7 +25300,7 @@
     <row r="321" ht="130" customHeight="1">
       <c r="A321" s="2" t="inlineStr">
         <is>
-          <t>AC-3 (4),IA-11</t>
+          <t>IA-11,AC-3 (4)</t>
         </is>
       </c>
       <c r="B321" s="2" t="inlineStr">
@@ -25764,7 +25764,7 @@
     <row r="327" ht="130" customHeight="1">
       <c r="A327" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,CM-5 (1)</t>
+          <t>CM-5 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B327" s="2" t="inlineStr">
@@ -25921,7 +25921,7 @@
     <row r="329" ht="130" customHeight="1">
       <c r="A329" s="2" t="inlineStr">
         <is>
-          <t>AU-5 b,AU-5 a</t>
+          <t>AU-5 a,AU-5 b</t>
         </is>
       </c>
       <c r="B329" s="2" t="inlineStr">
@@ -26915,7 +26915,7 @@
     <row r="342" ht="130" customHeight="1">
       <c r="A342" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-7 a</t>
+          <t>CM-7 a,CM-7 b</t>
         </is>
       </c>
       <c r="B342" s="2" t="inlineStr">
@@ -26989,7 +26989,7 @@
     <row r="343" ht="130" customHeight="1">
       <c r="A343" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-7 a</t>
+          <t>CM-7 a,CM-7 b</t>
         </is>
       </c>
       <c r="B343" s="2" t="inlineStr">
@@ -27063,7 +27063,7 @@
     <row r="344" ht="130" customHeight="1">
       <c r="A344" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (1)</t>
+          <t>AC-17 (1),CM-7 b</t>
         </is>
       </c>
       <c r="B344" s="2" t="inlineStr">
@@ -27149,7 +27149,7 @@
     <row r="345" ht="130" customHeight="1">
       <c r="A345" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),CM-7 a</t>
+          <t>CM-7 a,AC-18 (1)</t>
         </is>
       </c>
       <c r="B345" s="2" t="inlineStr">
@@ -27226,7 +27226,7 @@
     <row r="346" ht="130" customHeight="1">
       <c r="A346" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (c),CM-7 a</t>
+          <t>CM-7 a,CM-6 b,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B346" s="2" t="inlineStr">
@@ -28071,7 +28071,7 @@
     <row r="357" ht="130" customHeight="1">
       <c r="A357" s="2" t="inlineStr">
         <is>
-          <t>AC-11 (1),AC-11 b</t>
+          <t>AC-11 b,AC-11 (1)</t>
         </is>
       </c>
       <c r="B357" s="2" t="inlineStr">
@@ -28320,7 +28320,7 @@
     <row r="360" ht="130" customHeight="1">
       <c r="A360" s="2" t="inlineStr">
         <is>
-          <t>SI-6 b,SI-6 d,CM-3 (5)</t>
+          <t>SI-6 d,SI-6 b,CM-3 (5)</t>
         </is>
       </c>
       <c r="B360" s="2" t="inlineStr">
@@ -28404,7 +28404,7 @@
     <row r="361" ht="130" customHeight="1">
       <c r="A361" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B361" s="2" t="inlineStr">
@@ -29324,7 +29324,7 @@
     <row r="373" ht="130" customHeight="1">
       <c r="A373" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B373" s="2" t="inlineStr">
@@ -29395,7 +29395,7 @@
     <row r="374" ht="130" customHeight="1">
       <c r="A374" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B374" s="2" t="inlineStr">
@@ -29467,7 +29467,7 @@
     <row r="375" ht="130" customHeight="1">
       <c r="A375" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B375" s="2" t="inlineStr">
@@ -30536,7 +30536,7 @@
     <row r="388" ht="130" customHeight="1">
       <c r="A388" s="2" t="inlineStr">
         <is>
-          <t>SI-6 a,SC-3</t>
+          <t>SC-3,SI-6 a</t>
         </is>
       </c>
       <c r="B388" s="2" t="inlineStr">
@@ -30675,7 +30675,7 @@
     <row r="390" ht="130" customHeight="1">
       <c r="A390" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (a)</t>
+          <t>IA-5 (1) (a),CM-6 b</t>
         </is>
       </c>
       <c r="B390" s="2" t="inlineStr">
@@ -31231,7 +31231,7 @@
     <row r="397" ht="130" customHeight="1">
       <c r="A397" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B397" s="2" t="inlineStr">
@@ -31322,7 +31322,7 @@
     <row r="398" ht="130" customHeight="1">
       <c r="A398" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B398" s="2" t="inlineStr">
@@ -31416,7 +31416,7 @@
     <row r="399" ht="130" customHeight="1">
       <c r="A399" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B399" s="2" t="inlineStr">
@@ -34976,7 +34976,7 @@
     <row r="446" ht="130" customHeight="1">
       <c r="A446" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (1)</t>
+          <t>CM-5 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B446" s="2" t="inlineStr">
@@ -35049,7 +35049,7 @@
     <row r="447" ht="130" customHeight="1">
       <c r="A447" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (1)</t>
+          <t>CM-5 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B447" s="2" t="inlineStr">
@@ -42826,7 +42826,7 @@
     <row r="546" ht="130" customHeight="1">
       <c r="A546" s="2" t="inlineStr">
         <is>
-          <t>SI-2 (2),CM-6 b</t>
+          <t>CM-6 b,SI-2 (2)</t>
         </is>
       </c>
       <c r="B546" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@6a6af5544f2d7c0f7ec8379a871579a05ea4907e 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -541,7 +541,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-4 (1)</t>
+          <t>AU-4 (1),AU-4</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -625,7 +625,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-14 (1)</t>
+          <t>AU-14 (1),AU-4</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -708,7 +708,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>AU-4,CM-6 b</t>
+          <t>CM-6 b,AU-4</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -784,7 +784,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>SC-5,CM-6 b,SC-5 (2)</t>
+          <t>SC-5 (2),CM-6 b,SC-5</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -883,7 +883,7 @@
     <row r="6" ht="130" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (9),AU-7 b,CM-5 (1),AU-7 a,AC-6 (8),AU-12 (3),AU-8 b</t>
+          <t>AU-7 a,AU-12 (3),AC-6 (9),CM-5 (1),AC-6 (8),AU-7 b,AU-8 b</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -963,7 +963,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-7 b,CM-6 b,CM-5 (1),AU-7 a,AU-12 c,AU-12 (3),AU-8 b</t>
+          <t>AU-12 a,AU-7 a,AU-12 (3),CM-6 b,CM-5 (1),AU-12 c,AU-7 b,AU-8 b</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1037,7 +1037,7 @@
     <row r="8" ht="130" customHeight="1">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (9),AC-17 (1),CM-7 b,CM-6 b</t>
+          <t>AC-17 (9),AC-17 (1),CM-6 b,CM-7 b</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
@@ -1257,7 +1257,7 @@
     <row r="11" ht="130" customHeight="1">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B11" s="2" t="inlineStr">
@@ -1334,7 +1334,7 @@
     <row r="12" ht="130" customHeight="1">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
@@ -3910,7 +3910,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -3985,7 +3985,7 @@
     <row r="47" ht="130" customHeight="1">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
@@ -4060,7 +4060,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4135,7 +4135,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4210,7 +4210,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4285,7 +4285,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4360,7 +4360,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
@@ -4435,7 +4435,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4510,7 +4510,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4585,7 +4585,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4660,7 +4660,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4735,7 +4735,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4810,7 +4810,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4885,7 +4885,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -4965,7 +4965,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5048,7 +5048,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5128,7 +5128,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5208,7 +5208,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5288,7 +5288,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5368,7 +5368,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5442,7 +5442,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5516,7 +5516,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5590,7 +5590,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5664,7 +5664,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5738,7 +5738,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5811,7 +5811,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5884,7 +5884,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -5957,7 +5957,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6030,7 +6030,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6103,7 +6103,7 @@
     <row r="75" ht="130" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
@@ -6176,7 +6176,7 @@
     <row r="76" ht="130" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
@@ -6250,7 +6250,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6324,7 +6324,7 @@
     <row r="78" ht="130" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
@@ -6398,7 +6398,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6469,7 +6469,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6549,7 +6549,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6629,7 +6629,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B82" s="2" t="inlineStr">
@@ -6709,7 +6709,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B83" s="2" t="inlineStr">
@@ -6789,7 +6789,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B84" s="2" t="inlineStr">
@@ -6869,7 +6869,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B85" s="2" t="inlineStr">
@@ -6949,7 +6949,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -7029,7 +7029,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7109,7 +7109,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7189,7 +7189,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7269,7 +7269,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7425,7 +7425,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
@@ -7502,7 +7502,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
@@ -7582,7 +7582,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B94" s="2" t="inlineStr">
@@ -7662,7 +7662,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
@@ -7742,7 +7742,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7822,7 +7822,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7902,7 +7902,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -7982,7 +7982,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8062,7 +8062,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8142,7 +8142,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8222,7 +8222,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8295,7 +8295,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),AC-2 (4),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8376,7 +8376,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),AC-2 (4),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8457,7 +8457,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),AC-2 (4),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8528,7 +8528,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AC-2 (4),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8603,7 +8603,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),AC-2 (4),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8685,7 +8685,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),AC-2 (4),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -8767,7 +8767,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),AC-2 (4),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -8849,7 +8849,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),AC-2 (4),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B110" s="2" t="inlineStr">
@@ -8931,7 +8931,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 a,AU-3,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,AU-12 c,AU-3 (1),AC-2 (4),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9013,7 +9013,7 @@
     <row r="112" ht="130" customHeight="1">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-14 (1),AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-14 (1),AU-12 a,AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
@@ -9096,7 +9096,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9177,7 +9177,7 @@
     <row r="114" ht="130" customHeight="1">
       <c r="A114" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B114" s="2" t="inlineStr">
@@ -9263,7 +9263,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),AC-11 b</t>
+          <t>AC-11 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9341,7 +9341,7 @@
     <row r="116" ht="130" customHeight="1">
       <c r="A116" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B116" s="2" t="inlineStr">
@@ -9707,7 +9707,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -9778,7 +9778,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -10222,7 +10222,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 c,AC-6 (9),CM-5 (1)</t>
+          <t>AC-6 (9),AU-12 c,CM-5 (1),AC-2 (4)</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -10665,7 +10665,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>MA-4 c,SC-8,AC-17 (2),SC-13</t>
+          <t>MA-4 c,SC-13,AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10747,7 +10747,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>AC-12,SC-10,MA-4 (7),MA-4 e</t>
+          <t>SC-10,MA-4 (7),AC-12,MA-4 e</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -10822,7 +10822,7 @@
     <row r="135" ht="130" customHeight="1">
       <c r="A135" s="2" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B135" s="2" t="inlineStr">
@@ -10901,7 +10901,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -11054,7 +11054,7 @@
     <row r="138" ht="130" customHeight="1">
       <c r="A138" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-14 (1),AU-3 (1),AU-7 (1),CM-6 b,AU-6 (4),MA-4 (1) (a),CM-5 (1),AU-7 a</t>
+          <t>AU-14 (1),AU-7 (1),AU-12 a,AU-7 a,AU-3,AU-6 (4),CM-6 b,CM-5 (1),AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B138" s="2" t="inlineStr">
@@ -11291,7 +11291,7 @@
     <row r="141" ht="130" customHeight="1">
       <c r="A141" s="2" t="inlineStr">
         <is>
-          <t>AU-9 (3),AU-9</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B141" s="2" t="inlineStr">
@@ -11367,7 +11367,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="2" t="inlineStr">
         <is>
-          <t>AU-9 (3),AU-9</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B142" s="2" t="inlineStr">
@@ -11443,7 +11443,7 @@
     <row r="143" ht="130" customHeight="1">
       <c r="A143" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B143" s="2" t="inlineStr">
@@ -11512,7 +11512,7 @@
     <row r="144" ht="130" customHeight="1">
       <c r="A144" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B144" s="2" t="inlineStr">
@@ -11581,7 +11581,7 @@
     <row r="145" ht="130" customHeight="1">
       <c r="A145" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B145" s="2" t="inlineStr">
@@ -11651,7 +11651,7 @@
     <row r="146" ht="130" customHeight="1">
       <c r="A146" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B146" s="2" t="inlineStr">
@@ -11720,7 +11720,7 @@
     <row r="147" ht="130" customHeight="1">
       <c r="A147" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B147" s="2" t="inlineStr">
@@ -11789,7 +11789,7 @@
     <row r="148" ht="130" customHeight="1">
       <c r="A148" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B148" s="2" t="inlineStr">
@@ -11859,7 +11859,7 @@
     <row r="149" ht="130" customHeight="1">
       <c r="A149" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B149" s="2" t="inlineStr">
@@ -11928,7 +11928,7 @@
     <row r="150" ht="130" customHeight="1">
       <c r="A150" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B150" s="2" t="inlineStr">
@@ -11997,7 +11997,7 @@
     <row r="151" ht="130" customHeight="1">
       <c r="A151" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B151" s="2" t="inlineStr">
@@ -12067,7 +12067,7 @@
     <row r="152" ht="130" customHeight="1">
       <c r="A152" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B152" s="2" t="inlineStr">
@@ -12136,7 +12136,7 @@
     <row r="153" ht="130" customHeight="1">
       <c r="A153" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B153" s="2" t="inlineStr">
@@ -12205,7 +12205,7 @@
     <row r="154" ht="130" customHeight="1">
       <c r="A154" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B154" s="2" t="inlineStr">
@@ -12274,7 +12274,7 @@
     <row r="155" ht="130" customHeight="1">
       <c r="A155" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B155" s="2" t="inlineStr">
@@ -13112,7 +13112,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8 (1),SC-8</t>
+          <t>SC-8 (1),SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B166" s="2" t="inlineStr">
@@ -13494,7 +13494,7 @@
     <row r="171" ht="130" customHeight="1">
       <c r="A171" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 c,AC-6 (9)</t>
+          <t>AC-6 (9),AU-12 c,AC-2 (4)</t>
         </is>
       </c>
       <c r="B171" s="2" t="inlineStr">
@@ -13708,7 +13708,7 @@
     <row r="173" ht="130" customHeight="1">
       <c r="A173" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B173" s="2" t="inlineStr">
@@ -13786,7 +13786,7 @@
     <row r="174" ht="130" customHeight="1">
       <c r="A174" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B174" s="2" t="inlineStr">
@@ -13869,7 +13869,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B175" s="2" t="inlineStr">
@@ -14249,7 +14249,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-6 (4),AU-4 (1)</t>
+          <t>AU-6 (4),AU-4 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B180" s="2" t="inlineStr">
@@ -14320,7 +14320,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-17 (1),CM-7 b</t>
+          <t>AC-17 (1),CM-6 b,CM-7 b</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">
@@ -15286,7 +15286,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-3</t>
+          <t>AU-3,CM-6 b</t>
         </is>
       </c>
       <c r="B194" s="2" t="inlineStr">
@@ -16235,7 +16235,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-4 (1)</t>
+          <t>AU-4 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -16629,7 +16629,7 @@
     <row r="212" ht="130" customHeight="1">
       <c r="A212" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B212" s="2" t="inlineStr">
@@ -16731,7 +16731,7 @@
     <row r="213" ht="130" customHeight="1">
       <c r="A213" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B213" s="2" t="inlineStr">
@@ -16841,7 +16841,7 @@
     <row r="214" ht="130" customHeight="1">
       <c r="A214" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B214" s="2" t="inlineStr">
@@ -16952,7 +16952,7 @@
     <row r="215" ht="130" customHeight="1">
       <c r="A215" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B215" s="2" t="inlineStr">
@@ -17440,7 +17440,7 @@
     <row r="221" ht="130" customHeight="1">
       <c r="A221" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (5),IA-2 (2),IA-2 (4),IA-2</t>
+          <t>IA-2 (4),IA-2 (3),IA-2,IA-2 (5),IA-2 (2)</t>
         </is>
       </c>
       <c r="B221" s="2" t="inlineStr">
@@ -17525,7 +17525,7 @@
     <row r="222" ht="130" customHeight="1">
       <c r="A222" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (5),IA-2 (2),IA-2 (4),IA-2</t>
+          <t>IA-2 (4),IA-2 (3),IA-2,IA-2 (5),IA-2 (2)</t>
         </is>
       </c>
       <c r="B222" s="2" t="inlineStr">
@@ -17672,13 +17672,19 @@
           <t>Verify that there are no wireless interfaces configured on the system
 with the following command:
  $ sudo nmcli device 
-The output should contain the following:
- wifi disconnected 
-If it is not then this is a finding.</t>
+The output should only contain wireless devices in unavailable state, like in the
+following example:
+ wlp0s20f3          wifi      unavailable             --  
+If wireless interfaces are not active then this is a finding.</t>
         </is>
       </c>
       <c r="L223" s="2" t="n"/>
-      <c r="M223" s="2" t="inlineStr"/>
+      <c r="M223" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">To disable all wireless devices use the following command:
+ nmcli radio all off </t>
+        </is>
+      </c>
       <c r="N223" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -17771,7 +17777,7 @@
     <row r="225" ht="130" customHeight="1">
       <c r="A225" s="2" t="inlineStr">
         <is>
-          <t>IA-7,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),IA-7</t>
         </is>
       </c>
       <c r="B225" s="2" t="inlineStr">
@@ -18172,7 +18178,7 @@
     <row r="230" ht="130" customHeight="1">
       <c r="A230" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,IA-7</t>
+          <t>IA-7,CM-7 a</t>
         </is>
       </c>
       <c r="B230" s="2" t="inlineStr">
@@ -19007,7 +19013,7 @@
     <row r="241" ht="130" customHeight="1">
       <c r="A241" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B241" s="2" t="inlineStr">
@@ -19078,7 +19084,7 @@
     <row r="242" ht="130" customHeight="1">
       <c r="A242" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B242" s="2" t="inlineStr">
@@ -19240,7 +19246,7 @@
     <row r="244" ht="130" customHeight="1">
       <c r="A244" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-16,SC-2</t>
+          <t>SI-16,CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B244" s="2" t="inlineStr">
@@ -21152,7 +21158,7 @@
     <row r="269" ht="130" customHeight="1">
       <c r="A269" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),CM-6 b</t>
+          <t>CM-6 b,IA-2 (2)</t>
         </is>
       </c>
       <c r="B269" s="2" t="inlineStr">
@@ -21239,7 +21245,7 @@
     <row r="270" ht="130" customHeight="1">
       <c r="A270" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (4),IA-2 (3),IA-2 (1)</t>
+          <t>IA-2 (4),IA-2 (1),IA-2 (3),IA-2 (2)</t>
         </is>
       </c>
       <c r="B270" s="2" t="inlineStr">
@@ -21408,7 +21414,7 @@
     <row r="272" ht="130" customHeight="1">
       <c r="A272" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B272" s="2" t="inlineStr">
@@ -21626,7 +21632,7 @@
     <row r="275" ht="130" customHeight="1">
       <c r="A275" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-4</t>
+          <t>SC-4,CM-6 b</t>
         </is>
       </c>
       <c r="B275" s="2" t="inlineStr">
@@ -22033,7 +22039,7 @@
     <row r="280" ht="130" customHeight="1">
       <c r="A280" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,CM-6 b</t>
+          <t>CM-6 b,AU-12 a</t>
         </is>
       </c>
       <c r="B280" s="2" t="inlineStr">
@@ -23356,7 +23362,7 @@
     <row r="297" ht="130" customHeight="1">
       <c r="A297" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B297" s="2" t="inlineStr">
@@ -23525,7 +23531,7 @@
     <row r="299" ht="130" customHeight="1">
       <c r="A299" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11),IA-2 (1)</t>
+          <t>IA-2 (11),IA-2 (1),IA-2 (12)</t>
         </is>
       </c>
       <c r="B299" s="2" t="inlineStr">
@@ -24347,7 +24353,7 @@
     <row r="309" ht="130" customHeight="1">
       <c r="A309" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (a),AU-8 (1) (b),AU-8 b</t>
+          <t>AU-8 (1) (a),AU-8 b,AU-8 (1) (b)</t>
         </is>
       </c>
       <c r="B309" s="2" t="inlineStr">
@@ -25300,7 +25306,7 @@
     <row r="321" ht="130" customHeight="1">
       <c r="A321" s="2" t="inlineStr">
         <is>
-          <t>IA-11,AC-3 (4)</t>
+          <t>AC-3 (4),IA-11</t>
         </is>
       </c>
       <c r="B321" s="2" t="inlineStr">
@@ -27226,7 +27232,7 @@
     <row r="346" ht="130" customHeight="1">
       <c r="A346" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B346" s="2" t="inlineStr">
@@ -28071,7 +28077,7 @@
     <row r="357" ht="130" customHeight="1">
       <c r="A357" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 (1)</t>
+          <t>AC-11 (1),AC-11 b</t>
         </is>
       </c>
       <c r="B357" s="2" t="inlineStr">
@@ -28320,7 +28326,7 @@
     <row r="360" ht="130" customHeight="1">
       <c r="A360" s="2" t="inlineStr">
         <is>
-          <t>SI-6 d,SI-6 b,CM-3 (5)</t>
+          <t>SI-6 d,CM-3 (5),SI-6 b</t>
         </is>
       </c>
       <c r="B360" s="2" t="inlineStr">
@@ -28404,7 +28410,7 @@
     <row r="361" ht="130" customHeight="1">
       <c r="A361" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B361" s="2" t="inlineStr">
@@ -28784,7 +28790,7 @@
     <row r="366" ht="130" customHeight="1">
       <c r="A366" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,SI-16</t>
+          <t>SI-16,CM-7 a</t>
         </is>
       </c>
       <c r="B366" s="2" t="inlineStr">
@@ -29324,7 +29330,7 @@
     <row r="373" ht="130" customHeight="1">
       <c r="A373" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B373" s="2" t="inlineStr">
@@ -29395,7 +29401,7 @@
     <row r="374" ht="130" customHeight="1">
       <c r="A374" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B374" s="2" t="inlineStr">
@@ -29467,7 +29473,7 @@
     <row r="375" ht="130" customHeight="1">
       <c r="A375" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B375" s="2" t="inlineStr">
@@ -30990,7 +30996,7 @@
     <row r="394" ht="130" customHeight="1">
       <c r="A394" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-16</t>
+          <t>SI-16,CM-6 b</t>
         </is>
       </c>
       <c r="B394" s="2" t="inlineStr">
@@ -34826,7 +34832,7 @@
     <row r="444" ht="130" customHeight="1">
       <c r="A444" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),CM-6 b</t>
         </is>
       </c>
       <c r="B444" s="2" t="inlineStr">
@@ -34976,7 +34982,7 @@
     <row r="446" ht="130" customHeight="1">
       <c r="A446" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),CM-6 b</t>
+          <t>CM-6 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B446" s="2" t="inlineStr">
@@ -35049,7 +35055,7 @@
     <row r="447" ht="130" customHeight="1">
       <c r="A447" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),CM-6 b</t>
+          <t>CM-6 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B447" s="2" t="inlineStr">
@@ -42179,7 +42185,7 @@
     <row r="537" ht="130" customHeight="1">
       <c r="A537" s="2" t="inlineStr">
         <is>
-          <t>SI-2 (2),CM-6 b</t>
+          <t>CM-6 b,SI-2 (2)</t>
         </is>
       </c>
       <c r="B537" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@d584dbfa36a12c71e89dc73fd2aaa5ab3e6bf4f9 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -541,7 +541,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-4</t>
+          <t>AU-4,AU-4 (1)</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -625,7 +625,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),AU-4</t>
+          <t>AU-4,AU-14 (1)</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -708,7 +708,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-4</t>
+          <t>AU-4,CM-6 b</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -784,7 +784,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-5 (2),SC-5</t>
+          <t>SC-5,CM-6 b,SC-5 (2)</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -883,7 +883,7 @@
     <row r="6" ht="130" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>AU-12 (3),AC-6 (8),CM-5 (1),AU-7 b,AU-8 b,AU-7 a,AC-6 (9)</t>
+          <t>AU-12 (3),AU-8 b,CM-5 (1),AC-6 (9),AC-6 (8),AU-7 a,AU-7 b</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -963,7 +963,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-12 (3),CM-6 b,CM-5 (1),AU-7 b,AU-8 b,AU-7 a,AU-12 c,AU-12 a</t>
+          <t>AU-12 (3),AU-12 c,AU-8 b,AU-12 a,CM-5 (1),AU-7 a,CM-6 b,AU-7 b</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1037,7 +1037,7 @@
     <row r="8" ht="130" customHeight="1">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),AC-17 (9),CM-6 b,CM-7 b</t>
+          <t>CM-6 b,AC-17 (1),CM-7 b,AC-17 (9)</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
@@ -1484,7 +1484,7 @@
     <row r="14" ht="130" customHeight="1">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -1560,7 +1560,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1714,7 +1714,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -2084,7 +2084,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -2158,7 +2158,7 @@
     <row r="23" ht="130" customHeight="1">
       <c r="A23" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B23" s="2" t="inlineStr">
@@ -3286,7 +3286,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3370,7 +3370,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3455,7 +3455,7 @@
     <row r="40" ht="130" customHeight="1">
       <c r="A40" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B40" s="2" t="inlineStr">
@@ -3527,7 +3527,7 @@
     <row r="41" ht="130" customHeight="1">
       <c r="A41" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B41" s="2" t="inlineStr">
@@ -3832,7 +3832,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>IA-2,AU-3 (1),IA-8</t>
+          <t>AU-3 (1),IA-8,IA-2</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3910,7 +3910,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -3985,7 +3985,7 @@
     <row r="47" ht="130" customHeight="1">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
@@ -4060,7 +4060,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4135,7 +4135,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4210,7 +4210,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4285,7 +4285,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4360,7 +4360,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
@@ -4435,7 +4435,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4510,7 +4510,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4585,7 +4585,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4660,7 +4660,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4735,7 +4735,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4810,7 +4810,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4885,7 +4885,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -4965,7 +4965,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5048,7 +5048,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5128,7 +5128,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5208,7 +5208,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5288,7 +5288,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5368,7 +5368,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5442,7 +5442,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5516,7 +5516,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5590,7 +5590,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5664,7 +5664,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5738,7 +5738,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5811,7 +5811,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5884,7 +5884,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -5957,7 +5957,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6030,7 +6030,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6103,7 +6103,7 @@
     <row r="75" ht="130" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
@@ -6176,7 +6176,7 @@
     <row r="76" ht="130" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
@@ -6250,7 +6250,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6324,7 +6324,7 @@
     <row r="78" ht="130" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
@@ -6398,7 +6398,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6469,7 +6469,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6549,7 +6549,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6629,7 +6629,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B82" s="2" t="inlineStr">
@@ -6709,7 +6709,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B83" s="2" t="inlineStr">
@@ -6789,7 +6789,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B84" s="2" t="inlineStr">
@@ -6869,7 +6869,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3</t>
+          <t>AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B85" s="2" t="inlineStr">
@@ -6949,7 +6949,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -7029,7 +7029,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7109,7 +7109,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7189,7 +7189,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7269,7 +7269,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7349,7 +7349,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7425,7 +7425,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
@@ -7502,7 +7502,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
@@ -7582,7 +7582,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B94" s="2" t="inlineStr">
@@ -7662,7 +7662,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
@@ -7742,7 +7742,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7822,7 +7822,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7902,7 +7902,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -7982,7 +7982,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8062,7 +8062,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8142,7 +8142,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8222,7 +8222,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8295,7 +8295,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-12 a</t>
+          <t>AC-2 (4),AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8376,7 +8376,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-12 a</t>
+          <t>AC-2 (4),AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8457,7 +8457,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-12 a</t>
+          <t>AC-2 (4),AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8528,7 +8528,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c</t>
+          <t>AC-2 (4),AU-12 c,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8603,7 +8603,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-12 a</t>
+          <t>AC-2 (4),AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8685,7 +8685,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-12 a</t>
+          <t>AC-2 (4),AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -8767,7 +8767,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-12 a</t>
+          <t>AC-2 (4),AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -8849,7 +8849,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-12 a</t>
+          <t>AC-2 (4),AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B110" s="2" t="inlineStr">
@@ -8931,7 +8931,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-12 a</t>
+          <t>AC-2 (4),AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9013,7 +9013,7 @@
     <row r="112" ht="130" customHeight="1">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-14 (1),AU-3</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
@@ -9263,7 +9263,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),AC-11 b</t>
+          <t>AC-11 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9707,7 +9707,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -9778,7 +9778,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -9849,7 +9849,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-9</t>
+          <t>AU-9,AU-12 c</t>
         </is>
       </c>
       <c r="B122" s="2" t="inlineStr">
@@ -10222,7 +10222,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AC-6 (9),AU-12 c,AC-2 (4)</t>
+          <t>AC-6 (9),AC-2 (4),CM-5 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -10345,7 +10345,7 @@
     <row r="129" ht="130" customHeight="1">
       <c r="A129" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (a),IA-5 (1) (b)</t>
+          <t>IA-5 (1) (a),CM-6 b,IA-5 (1) (b)</t>
         </is>
       </c>
       <c r="B129" s="2" t="inlineStr">
@@ -10665,7 +10665,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8,MA-4 c,SC-13</t>
+          <t>SC-8,AC-17 (2),SC-13,MA-4 c</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10822,7 +10822,7 @@
     <row r="135" ht="130" customHeight="1">
       <c r="A135" s="2" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B135" s="2" t="inlineStr">
@@ -10901,7 +10901,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -10977,7 +10977,7 @@
     <row r="137" ht="130" customHeight="1">
       <c r="A137" s="2" t="inlineStr">
         <is>
-          <t>SC-10,AC-11 a</t>
+          <t>AC-11 a,SC-10</t>
         </is>
       </c>
       <c r="B137" s="2" t="inlineStr">
@@ -11054,7 +11054,7 @@
     <row r="138" ht="130" customHeight="1">
       <c r="A138" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-14 (1),AU-3 (1),CM-5 (1),AU-6 (4),AU-7 (1),AU-3,MA-4 (1) (a),AU-7 a,AU-12 a</t>
+          <t>AU-12 a,AU-6 (4),AU-3 (1),CM-5 (1),AU-7 (1),AU-7 a,CM-6 b,MA-4 (1) (a),AU-14 (1),AU-3</t>
         </is>
       </c>
       <c r="B138" s="2" t="inlineStr">
@@ -11304,7 +11304,7 @@
     <row r="141" ht="130" customHeight="1">
       <c r="A141" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B141" s="2" t="inlineStr">
@@ -11380,7 +11380,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B142" s="2" t="inlineStr">
@@ -11456,7 +11456,7 @@
     <row r="143" ht="130" customHeight="1">
       <c r="A143" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B143" s="2" t="inlineStr">
@@ -11525,7 +11525,7 @@
     <row r="144" ht="130" customHeight="1">
       <c r="A144" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B144" s="2" t="inlineStr">
@@ -11594,7 +11594,7 @@
     <row r="145" ht="130" customHeight="1">
       <c r="A145" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B145" s="2" t="inlineStr">
@@ -11664,7 +11664,7 @@
     <row r="146" ht="130" customHeight="1">
       <c r="A146" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B146" s="2" t="inlineStr">
@@ -11733,7 +11733,7 @@
     <row r="147" ht="130" customHeight="1">
       <c r="A147" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B147" s="2" t="inlineStr">
@@ -11802,7 +11802,7 @@
     <row r="148" ht="130" customHeight="1">
       <c r="A148" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B148" s="2" t="inlineStr">
@@ -11872,7 +11872,7 @@
     <row r="149" ht="130" customHeight="1">
       <c r="A149" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B149" s="2" t="inlineStr">
@@ -11941,7 +11941,7 @@
     <row r="150" ht="130" customHeight="1">
       <c r="A150" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B150" s="2" t="inlineStr">
@@ -12010,7 +12010,7 @@
     <row r="151" ht="130" customHeight="1">
       <c r="A151" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B151" s="2" t="inlineStr">
@@ -12080,7 +12080,7 @@
     <row r="152" ht="130" customHeight="1">
       <c r="A152" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B152" s="2" t="inlineStr">
@@ -12149,7 +12149,7 @@
     <row r="153" ht="130" customHeight="1">
       <c r="A153" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B153" s="2" t="inlineStr">
@@ -12218,7 +12218,7 @@
     <row r="154" ht="130" customHeight="1">
       <c r="A154" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B154" s="2" t="inlineStr">
@@ -12287,7 +12287,7 @@
     <row r="155" ht="130" customHeight="1">
       <c r="A155" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B155" s="2" t="inlineStr">
@@ -13125,7 +13125,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8,SC-8 (2)</t>
+          <t>SC-8 (2),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B166" s="2" t="inlineStr">
@@ -13278,7 +13278,7 @@
     <row r="168" ht="130" customHeight="1">
       <c r="A168" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8</t>
+          <t>SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B168" s="2" t="inlineStr">
@@ -13507,7 +13507,7 @@
     <row r="171" ht="130" customHeight="1">
       <c r="A171" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (9),AU-12 c,AC-2 (4)</t>
+          <t>AC-6 (9),AC-2 (4),AU-12 c</t>
         </is>
       </c>
       <c r="B171" s="2" t="inlineStr">
@@ -13721,7 +13721,7 @@
     <row r="173" ht="130" customHeight="1">
       <c r="A173" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B173" s="2" t="inlineStr">
@@ -14262,7 +14262,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-6 (4),AU-4 (1)</t>
+          <t>AU-4 (1),CM-6 b,AU-6 (4)</t>
         </is>
       </c>
       <c r="B180" s="2" t="inlineStr">
@@ -14333,7 +14333,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),CM-6 b,CM-7 b</t>
+          <t>CM-6 b,AC-17 (1),CM-7 b</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">
@@ -15299,7 +15299,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-3</t>
+          <t>AU-3,CM-6 b</t>
         </is>
       </c>
       <c r="B194" s="2" t="inlineStr">
@@ -15733,7 +15733,7 @@
     <row r="200" ht="130" customHeight="1">
       <c r="A200" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-3</t>
+          <t>AU-3,AU-4 (1)</t>
         </is>
       </c>
       <c r="B200" s="2" t="inlineStr">
@@ -16248,7 +16248,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-4 (1)</t>
+          <t>AU-4 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -16328,7 +16328,7 @@
     <row r="208" ht="130" customHeight="1">
       <c r="A208" s="2" t="inlineStr">
         <is>
-          <t>SC-28,SC-28 (1)</t>
+          <t>SC-28 (1),SC-28</t>
         </is>
       </c>
       <c r="B208" s="2" t="inlineStr">
@@ -17375,7 +17375,7 @@
     <row r="220" ht="130" customHeight="1">
       <c r="A220" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (5)</t>
+          <t>IA-2 (5),CM-6 b</t>
         </is>
       </c>
       <c r="B220" s="2" t="inlineStr">
@@ -17453,7 +17453,7 @@
     <row r="221" ht="130" customHeight="1">
       <c r="A221" s="2" t="inlineStr">
         <is>
-          <t>IA-2,IA-2 (4),IA-2 (3),IA-2 (2),IA-2 (5)</t>
+          <t>IA-2 (4),IA-2,IA-2 (2),IA-2 (5),IA-2 (3)</t>
         </is>
       </c>
       <c r="B221" s="2" t="inlineStr">
@@ -17538,7 +17538,7 @@
     <row r="222" ht="130" customHeight="1">
       <c r="A222" s="2" t="inlineStr">
         <is>
-          <t>IA-2,IA-2 (4),IA-2 (3),IA-2 (2),IA-2 (5)</t>
+          <t>IA-2 (4),IA-2,IA-2 (2),IA-2 (5),IA-2 (3)</t>
         </is>
       </c>
       <c r="B222" s="2" t="inlineStr">
@@ -17623,7 +17623,7 @@
     <row r="223" ht="130" customHeight="1">
       <c r="A223" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),AC-18 (1),SC-8</t>
+          <t>AC-18 (1),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B223" s="2" t="inlineStr">
@@ -17790,7 +17790,7 @@
     <row r="225" ht="130" customHeight="1">
       <c r="A225" s="2" t="inlineStr">
         <is>
-          <t>IA-7,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),IA-7</t>
         </is>
       </c>
       <c r="B225" s="2" t="inlineStr">
@@ -18191,7 +18191,7 @@
     <row r="230" ht="130" customHeight="1">
       <c r="A230" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,IA-7</t>
+          <t>IA-7,CM-7 a</t>
         </is>
       </c>
       <c r="B230" s="2" t="inlineStr">
@@ -19259,7 +19259,7 @@
     <row r="244" ht="130" customHeight="1">
       <c r="A244" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-16,SC-2</t>
+          <t>SI-16,CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B244" s="2" t="inlineStr">
@@ -21171,7 +21171,7 @@
     <row r="269" ht="130" customHeight="1">
       <c r="A269" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (2)</t>
+          <t>IA-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B269" s="2" t="inlineStr">
@@ -21726,7 +21726,7 @@
     <row r="276" ht="130" customHeight="1">
       <c r="A276" s="2" t="inlineStr">
         <is>
-          <t>SC-4,SC-2</t>
+          <t>SC-2,SC-4</t>
         </is>
       </c>
       <c r="B276" s="2" t="inlineStr">
@@ -21814,7 +21814,7 @@
     <row r="277" ht="130" customHeight="1">
       <c r="A277" s="2" t="inlineStr">
         <is>
-          <t>SC-4,SC-2</t>
+          <t>SC-2,SC-4</t>
         </is>
       </c>
       <c r="B277" s="2" t="inlineStr">
@@ -23544,7 +23544,7 @@
     <row r="299" ht="130" customHeight="1">
       <c r="A299" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12),IA-2 (1)</t>
+          <t>IA-2 (11),IA-2 (1),IA-2 (12)</t>
         </is>
       </c>
       <c r="B299" s="2" t="inlineStr">
@@ -24366,7 +24366,7 @@
     <row r="309" ht="130" customHeight="1">
       <c r="A309" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-8 (1) (b),AU-8 (1) (a)</t>
+          <t>AU-8 (1) (b),AU-8 b,AU-8 (1) (a)</t>
         </is>
       </c>
       <c r="B309" s="2" t="inlineStr">
@@ -25940,7 +25940,7 @@
     <row r="329" ht="130" customHeight="1">
       <c r="A329" s="2" t="inlineStr">
         <is>
-          <t>AU-5 b,AU-5 a</t>
+          <t>AU-5 a,AU-5 b</t>
         </is>
       </c>
       <c r="B329" s="2" t="inlineStr">
@@ -26859,7 +26859,7 @@
     <row r="341" ht="130" customHeight="1">
       <c r="A341" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-7 b</t>
+          <t>CM-7 b,IA-3</t>
         </is>
       </c>
       <c r="B341" s="2" t="inlineStr">
@@ -26934,7 +26934,7 @@
     <row r="342" ht="130" customHeight="1">
       <c r="A342" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-7 b</t>
+          <t>CM-7 b,CM-7 a</t>
         </is>
       </c>
       <c r="B342" s="2" t="inlineStr">
@@ -27008,7 +27008,7 @@
     <row r="343" ht="130" customHeight="1">
       <c r="A343" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-7 b</t>
+          <t>CM-7 b,CM-7 a</t>
         </is>
       </c>
       <c r="B343" s="2" t="inlineStr">
@@ -27168,7 +27168,7 @@
     <row r="345" ht="130" customHeight="1">
       <c r="A345" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,AC-18 (1)</t>
+          <t>AC-18 (1),CM-7 a</t>
         </is>
       </c>
       <c r="B345" s="2" t="inlineStr">
@@ -27245,7 +27245,7 @@
     <row r="346" ht="130" customHeight="1">
       <c r="A346" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B346" s="2" t="inlineStr">
@@ -28090,7 +28090,7 @@
     <row r="357" ht="130" customHeight="1">
       <c r="A357" s="2" t="inlineStr">
         <is>
-          <t>AC-11 (1),AC-11 b</t>
+          <t>AC-11 b,AC-11 (1)</t>
         </is>
       </c>
       <c r="B357" s="2" t="inlineStr">
@@ -28339,7 +28339,7 @@
     <row r="360" ht="130" customHeight="1">
       <c r="A360" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 b,SI-6 d</t>
+          <t>SI-6 b,SI-6 d,CM-3 (5)</t>
         </is>
       </c>
       <c r="B360" s="2" t="inlineStr">
@@ -28810,7 +28810,7 @@
     <row r="366" ht="130" customHeight="1">
       <c r="A366" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,SI-16</t>
+          <t>SI-16,CM-7 a</t>
         </is>
       </c>
       <c r="B366" s="2" t="inlineStr">
@@ -29350,7 +29350,7 @@
     <row r="373" ht="130" customHeight="1">
       <c r="A373" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B373" s="2" t="inlineStr">
@@ -29421,7 +29421,7 @@
     <row r="374" ht="130" customHeight="1">
       <c r="A374" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B374" s="2" t="inlineStr">
@@ -29493,7 +29493,7 @@
     <row r="375" ht="130" customHeight="1">
       <c r="A375" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B375" s="2" t="inlineStr">
@@ -30562,7 +30562,7 @@
     <row r="388" ht="130" customHeight="1">
       <c r="A388" s="2" t="inlineStr">
         <is>
-          <t>SC-3,SI-6 a</t>
+          <t>SI-6 a,SC-3</t>
         </is>
       </c>
       <c r="B388" s="2" t="inlineStr">
@@ -30701,7 +30701,7 @@
     <row r="390" ht="130" customHeight="1">
       <c r="A390" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (a)</t>
+          <t>IA-5 (1) (a),CM-6 b</t>
         </is>
       </c>
       <c r="B390" s="2" t="inlineStr">
@@ -31183,7 +31183,7 @@
     <row r="396" ht="130" customHeight="1">
       <c r="A396" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 d</t>
+          <t>SI-6 d,CM-3 (5)</t>
         </is>
       </c>
       <c r="B396" s="2" t="inlineStr">
@@ -31267,7 +31267,7 @@
     <row r="397" ht="130" customHeight="1">
       <c r="A397" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-16</t>
+          <t>SI-16,CM-6 b</t>
         </is>
       </c>
       <c r="B397" s="2" t="inlineStr">
@@ -35103,7 +35103,7 @@
     <row r="447" ht="130" customHeight="1">
       <c r="A447" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),CM-6 b</t>
         </is>
       </c>
       <c r="B447" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@f51f214bcb5daa09384e0c47b17c32fb0b021447 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -541,7 +541,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-4 (1)</t>
+          <t>AU-4 (1),AU-4</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -625,7 +625,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-14 (1)</t>
+          <t>AU-14 (1),AU-4</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -708,7 +708,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>AU-4,CM-6 b</t>
+          <t>CM-6 b,AU-4</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -883,7 +883,7 @@
     <row r="6" ht="130" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>AU-12 (3),AU-8 b,CM-5 (1),AC-6 (9),AC-6 (8),AU-7 a,AU-7 b</t>
+          <t>CM-5 (1),AU-7 b,AU-7 a,AC-6 (9),AU-8 b,AU-12 (3),AC-6 (8)</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -963,7 +963,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-12 (3),AU-12 c,AU-8 b,AU-12 a,CM-5 (1),AU-7 a,CM-6 b,AU-7 b</t>
+          <t>CM-5 (1),AU-12 c,AU-7 b,AU-12 a,AU-7 a,AU-8 b,CM-6 b,AU-12 (3)</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1037,7 +1037,7 @@
     <row r="8" ht="130" customHeight="1">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-17 (1),CM-7 b,AC-17 (9)</t>
+          <t>AC-17 (1),CM-6 b,CM-7 b,AC-17 (9)</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
@@ -3832,7 +3832,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),IA-8,IA-2</t>
+          <t>IA-2,IA-8,AU-3 (1)</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3910,7 +3910,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -3985,7 +3985,7 @@
     <row r="47" ht="130" customHeight="1">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
@@ -4060,7 +4060,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4135,7 +4135,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4210,7 +4210,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4285,7 +4285,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4360,7 +4360,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
@@ -4435,7 +4435,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4510,7 +4510,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4585,7 +4585,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4660,7 +4660,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4735,7 +4735,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4810,7 +4810,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4885,7 +4885,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -4965,7 +4965,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5048,7 +5048,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5128,7 +5128,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5208,7 +5208,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5288,7 +5288,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5368,7 +5368,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5442,7 +5442,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5516,7 +5516,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5590,7 +5590,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5664,7 +5664,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5738,7 +5738,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5811,7 +5811,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5884,7 +5884,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -5957,7 +5957,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6030,7 +6030,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6103,7 +6103,7 @@
     <row r="75" ht="130" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
@@ -6176,7 +6176,7 @@
     <row r="76" ht="130" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
@@ -6250,7 +6250,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6324,7 +6324,7 @@
     <row r="78" ht="130" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
@@ -6398,7 +6398,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6469,7 +6469,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6549,7 +6549,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6629,7 +6629,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B82" s="2" t="inlineStr">
@@ -6709,7 +6709,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B83" s="2" t="inlineStr">
@@ -6789,7 +6789,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B84" s="2" t="inlineStr">
@@ -6869,7 +6869,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B85" s="2" t="inlineStr">
@@ -6949,7 +6949,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -7029,7 +7029,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7109,7 +7109,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7189,7 +7189,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7269,7 +7269,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7349,7 +7349,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7425,7 +7425,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
@@ -7502,7 +7502,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
@@ -7582,7 +7582,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B94" s="2" t="inlineStr">
@@ -7662,7 +7662,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
@@ -7742,7 +7742,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7822,7 +7822,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7902,7 +7902,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -7982,7 +7982,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8062,7 +8062,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8142,7 +8142,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8222,7 +8222,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8295,7 +8295,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,AC-2 (4),MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8376,7 +8376,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,AC-2 (4),MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8457,7 +8457,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,AC-2 (4),MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8528,7 +8528,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 c,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-3,AC-2 (4),MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8603,7 +8603,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,AC-2 (4),MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8685,7 +8685,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,AC-2 (4),MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -8767,7 +8767,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,AC-2 (4),MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -8849,7 +8849,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,AC-2 (4),MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B110" s="2" t="inlineStr">
@@ -8931,7 +8931,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,AC-2 (4),MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9013,7 +9013,7 @@
     <row r="112" ht="130" customHeight="1">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-14 (1),AU-3</t>
+          <t>AU-12 c,AU-12 a,AU-3,AU-14 (1),MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
@@ -9096,7 +9096,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9177,7 +9177,7 @@
     <row r="114" ht="130" customHeight="1">
       <c r="A114" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B114" s="2" t="inlineStr">
@@ -9263,7 +9263,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-6 (10)</t>
+          <t>AC-6 (10),AC-11 b</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9341,7 +9341,7 @@
     <row r="116" ht="130" customHeight="1">
       <c r="A116" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B116" s="2" t="inlineStr">
@@ -9707,7 +9707,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -9778,7 +9778,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -9849,7 +9849,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-12 c</t>
+          <t>AU-12 c,AU-9</t>
         </is>
       </c>
       <c r="B122" s="2" t="inlineStr">
@@ -10222,7 +10222,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (9),AC-2 (4),CM-5 (1),AU-12 c</t>
+          <t>CM-5 (1),AC-2 (4),AU-12 c,AC-6 (9)</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -10345,7 +10345,7 @@
     <row r="129" ht="130" customHeight="1">
       <c r="A129" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (a),CM-6 b,IA-5 (1) (b)</t>
+          <t>IA-5 (1) (b),IA-5 (1) (a),CM-6 b</t>
         </is>
       </c>
       <c r="B129" s="2" t="inlineStr">
@@ -10665,7 +10665,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2),SC-13,MA-4 c</t>
+          <t>MA-4 c,AC-17 (2),SC-13,SC-8</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10747,7 +10747,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>MA-4 e,MA-4 (7),SC-10,AC-12</t>
+          <t>MA-4 e,AC-12,MA-4 (7),SC-10</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -10977,7 +10977,7 @@
     <row r="137" ht="130" customHeight="1">
       <c r="A137" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,SC-10</t>
+          <t>SC-10,AC-11 a</t>
         </is>
       </c>
       <c r="B137" s="2" t="inlineStr">
@@ -11054,7 +11054,7 @@
     <row r="138" ht="130" customHeight="1">
       <c r="A138" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-6 (4),AU-3 (1),CM-5 (1),AU-7 (1),AU-7 a,CM-6 b,MA-4 (1) (a),AU-14 (1),AU-3</t>
+          <t>CM-5 (1),AU-12 a,AU-3,AU-14 (1),AU-7 a,AU-7 (1),AU-6 (4),CM-6 b,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B138" s="2" t="inlineStr">
@@ -11456,7 +11456,7 @@
     <row r="143" ht="130" customHeight="1">
       <c r="A143" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B143" s="2" t="inlineStr">
@@ -11525,7 +11525,7 @@
     <row r="144" ht="130" customHeight="1">
       <c r="A144" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B144" s="2" t="inlineStr">
@@ -11594,7 +11594,7 @@
     <row r="145" ht="130" customHeight="1">
       <c r="A145" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B145" s="2" t="inlineStr">
@@ -11664,7 +11664,7 @@
     <row r="146" ht="130" customHeight="1">
       <c r="A146" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B146" s="2" t="inlineStr">
@@ -11733,7 +11733,7 @@
     <row r="147" ht="130" customHeight="1">
       <c r="A147" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B147" s="2" t="inlineStr">
@@ -11802,7 +11802,7 @@
     <row r="148" ht="130" customHeight="1">
       <c r="A148" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B148" s="2" t="inlineStr">
@@ -11872,7 +11872,7 @@
     <row r="149" ht="130" customHeight="1">
       <c r="A149" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B149" s="2" t="inlineStr">
@@ -11941,7 +11941,7 @@
     <row r="150" ht="130" customHeight="1">
       <c r="A150" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B150" s="2" t="inlineStr">
@@ -12010,7 +12010,7 @@
     <row r="151" ht="130" customHeight="1">
       <c r="A151" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B151" s="2" t="inlineStr">
@@ -12080,7 +12080,7 @@
     <row r="152" ht="130" customHeight="1">
       <c r="A152" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B152" s="2" t="inlineStr">
@@ -12149,7 +12149,7 @@
     <row r="153" ht="130" customHeight="1">
       <c r="A153" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B153" s="2" t="inlineStr">
@@ -12218,7 +12218,7 @@
     <row r="154" ht="130" customHeight="1">
       <c r="A154" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B154" s="2" t="inlineStr">
@@ -12287,7 +12287,7 @@
     <row r="155" ht="130" customHeight="1">
       <c r="A155" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B155" s="2" t="inlineStr">
@@ -13125,7 +13125,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8,SC-8 (1)</t>
+          <t>SC-8 (2),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B166" s="2" t="inlineStr">
@@ -13278,7 +13278,7 @@
     <row r="168" ht="130" customHeight="1">
       <c r="A168" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2)</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B168" s="2" t="inlineStr">
@@ -13507,7 +13507,7 @@
     <row r="171" ht="130" customHeight="1">
       <c r="A171" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (9),AC-2 (4),AU-12 c</t>
+          <t>AC-2 (4),AU-12 c,AC-6 (9)</t>
         </is>
       </c>
       <c r="B171" s="2" t="inlineStr">
@@ -13721,7 +13721,7 @@
     <row r="173" ht="130" customHeight="1">
       <c r="A173" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B173" s="2" t="inlineStr">
@@ -14262,7 +14262,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),CM-6 b,AU-6 (4)</t>
+          <t>AU-4 (1),AU-6 (4),CM-6 b</t>
         </is>
       </c>
       <c r="B180" s="2" t="inlineStr">
@@ -14333,7 +14333,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-17 (1),CM-7 b</t>
+          <t>AC-17 (1),CM-7 b,CM-6 b</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">
@@ -16642,7 +16642,7 @@
     <row r="212" ht="130" customHeight="1">
       <c r="A212" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B212" s="2" t="inlineStr">
@@ -16744,7 +16744,7 @@
     <row r="213" ht="130" customHeight="1">
       <c r="A213" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B213" s="2" t="inlineStr">
@@ -16854,7 +16854,7 @@
     <row r="214" ht="130" customHeight="1">
       <c r="A214" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B214" s="2" t="inlineStr">
@@ -16965,7 +16965,7 @@
     <row r="215" ht="130" customHeight="1">
       <c r="A215" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B215" s="2" t="inlineStr">
@@ -17623,7 +17623,7 @@
     <row r="223" ht="130" customHeight="1">
       <c r="A223" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),SC-8,SC-8 (1)</t>
+          <t>SC-8 (1),AC-18 (1),SC-8</t>
         </is>
       </c>
       <c r="B223" s="2" t="inlineStr">
@@ -17873,7 +17873,7 @@
     <row r="226" ht="130" customHeight="1">
       <c r="A226" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B226" s="2" t="inlineStr">
@@ -17949,7 +17949,7 @@
     <row r="227" ht="130" customHeight="1">
       <c r="A227" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B227" s="2" t="inlineStr">
@@ -18034,7 +18034,7 @@
     <row r="228" ht="130" customHeight="1">
       <c r="A228" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B228" s="2" t="inlineStr">
@@ -18191,7 +18191,7 @@
     <row r="230" ht="130" customHeight="1">
       <c r="A230" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-7 a</t>
+          <t>CM-7 a,IA-7</t>
         </is>
       </c>
       <c r="B230" s="2" t="inlineStr">
@@ -18270,7 +18270,7 @@
     <row r="231" ht="130" customHeight="1">
       <c r="A231" s="2" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B231" s="2" t="inlineStr">
@@ -18354,7 +18354,7 @@
     <row r="232" ht="130" customHeight="1">
       <c r="A232" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),MA-4 (6)</t>
+          <t>MA-4 (6),AC-17 (2)</t>
         </is>
       </c>
       <c r="B232" s="2" t="inlineStr">
@@ -18429,7 +18429,7 @@
     <row r="233" ht="130" customHeight="1">
       <c r="A233" s="2" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B233" s="2" t="inlineStr">
@@ -19026,7 +19026,7 @@
     <row r="241" ht="130" customHeight="1">
       <c r="A241" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B241" s="2" t="inlineStr">
@@ -19097,7 +19097,7 @@
     <row r="242" ht="130" customHeight="1">
       <c r="A242" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B242" s="2" t="inlineStr">
@@ -19259,7 +19259,7 @@
     <row r="244" ht="130" customHeight="1">
       <c r="A244" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-6 b,SC-2</t>
+          <t>SI-16,SC-2,CM-6 b</t>
         </is>
       </c>
       <c r="B244" s="2" t="inlineStr">
@@ -20333,7 +20333,7 @@
     <row r="258" ht="130" customHeight="1">
       <c r="A258" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B258" s="2" t="inlineStr">
@@ -20408,7 +20408,7 @@
     <row r="259" ht="130" customHeight="1">
       <c r="A259" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B259" s="2" t="inlineStr">
@@ -20496,7 +20496,7 @@
     <row r="260" ht="130" customHeight="1">
       <c r="A260" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B260" s="2" t="inlineStr">
@@ -20573,7 +20573,7 @@
     <row r="261" ht="130" customHeight="1">
       <c r="A261" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B261" s="2" t="inlineStr">
@@ -20731,7 +20731,7 @@
     <row r="263" ht="130" customHeight="1">
       <c r="A263" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 (1)</t>
+          <t>AU-5 (1),AU-5 a</t>
         </is>
       </c>
       <c r="B263" s="2" t="inlineStr">
@@ -21258,7 +21258,7 @@
     <row r="270" ht="130" customHeight="1">
       <c r="A270" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2 (2),IA-2 (1),IA-2 (3)</t>
+          <t>IA-2 (2),IA-2 (4),IA-2 (3),IA-2 (1)</t>
         </is>
       </c>
       <c r="B270" s="2" t="inlineStr">
@@ -21427,7 +21427,7 @@
     <row r="272" ht="130" customHeight="1">
       <c r="A272" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B272" s="2" t="inlineStr">
@@ -22052,7 +22052,7 @@
     <row r="280" ht="130" customHeight="1">
       <c r="A280" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-12 a</t>
+          <t>AU-12 a,CM-6 b</t>
         </is>
       </c>
       <c r="B280" s="2" t="inlineStr">
@@ -22275,7 +22275,7 @@
     <row r="283" ht="130" customHeight="1">
       <c r="A283" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (3)</t>
+          <t>CM-5 (3),CM-6 b</t>
         </is>
       </c>
       <c r="B283" s="2" t="inlineStr">
@@ -23544,7 +23544,7 @@
     <row r="299" ht="130" customHeight="1">
       <c r="A299" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (1),IA-2 (12)</t>
+          <t>IA-2 (11),IA-2 (12),IA-2 (1)</t>
         </is>
       </c>
       <c r="B299" s="2" t="inlineStr">
@@ -24366,7 +24366,7 @@
     <row r="309" ht="130" customHeight="1">
       <c r="A309" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (b),AU-8 b,AU-8 (1) (a)</t>
+          <t>AU-8 (1) (a),AU-8 (1) (b),AU-8 b</t>
         </is>
       </c>
       <c r="B309" s="2" t="inlineStr">
@@ -26859,7 +26859,7 @@
     <row r="341" ht="130" customHeight="1">
       <c r="A341" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,IA-3</t>
+          <t>IA-3,CM-7 b</t>
         </is>
       </c>
       <c r="B341" s="2" t="inlineStr">
@@ -26934,7 +26934,7 @@
     <row r="342" ht="130" customHeight="1">
       <c r="A342" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-7 a</t>
+          <t>CM-7 a,CM-7 b</t>
         </is>
       </c>
       <c r="B342" s="2" t="inlineStr">
@@ -27008,7 +27008,7 @@
     <row r="343" ht="130" customHeight="1">
       <c r="A343" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-7 a</t>
+          <t>CM-7 a,CM-7 b</t>
         </is>
       </c>
       <c r="B343" s="2" t="inlineStr">
@@ -27168,7 +27168,7 @@
     <row r="345" ht="130" customHeight="1">
       <c r="A345" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),CM-7 a</t>
+          <t>CM-7 a,AC-18 (1)</t>
         </is>
       </c>
       <c r="B345" s="2" t="inlineStr">
@@ -27245,7 +27245,7 @@
     <row r="346" ht="130" customHeight="1">
       <c r="A346" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-6 b,CM-7 a</t>
+          <t>CM-7 a,IA-5 (1) (c),CM-6 b</t>
         </is>
       </c>
       <c r="B346" s="2" t="inlineStr">
@@ -28090,7 +28090,7 @@
     <row r="357" ht="130" customHeight="1">
       <c r="A357" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 (1)</t>
+          <t>AC-11 (1),AC-11 b</t>
         </is>
       </c>
       <c r="B357" s="2" t="inlineStr">
@@ -28339,7 +28339,7 @@
     <row r="360" ht="130" customHeight="1">
       <c r="A360" s="2" t="inlineStr">
         <is>
-          <t>SI-6 b,SI-6 d,CM-3 (5)</t>
+          <t>SI-6 d,CM-3 (5),SI-6 b</t>
         </is>
       </c>
       <c r="B360" s="2" t="inlineStr">
@@ -28430,7 +28430,7 @@
     <row r="361" ht="130" customHeight="1">
       <c r="A361" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B361" s="2" t="inlineStr">
@@ -28810,7 +28810,7 @@
     <row r="366" ht="130" customHeight="1">
       <c r="A366" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-7 a</t>
+          <t>CM-7 a,SI-16</t>
         </is>
       </c>
       <c r="B366" s="2" t="inlineStr">
@@ -29350,7 +29350,7 @@
     <row r="373" ht="130" customHeight="1">
       <c r="A373" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B373" s="2" t="inlineStr">
@@ -29421,7 +29421,7 @@
     <row r="374" ht="130" customHeight="1">
       <c r="A374" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B374" s="2" t="inlineStr">
@@ -29493,7 +29493,7 @@
     <row r="375" ht="130" customHeight="1">
       <c r="A375" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B375" s="2" t="inlineStr">
@@ -30253,7 +30253,7 @@
     <row r="384" ht="130" customHeight="1">
       <c r="A384" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-17 (2)</t>
+          <t>AC-17 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B384" s="2" t="inlineStr">
@@ -31508,7 +31508,7 @@
     <row r="400" ht="130" customHeight="1">
       <c r="A400" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B400" s="2" t="inlineStr">
@@ -31599,7 +31599,7 @@
     <row r="401" ht="130" customHeight="1">
       <c r="A401" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B401" s="2" t="inlineStr">
@@ -31693,7 +31693,7 @@
     <row r="402" ht="130" customHeight="1">
       <c r="A402" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B402" s="2" t="inlineStr">
@@ -41137,7 +41137,7 @@
     <row r="523" ht="130" customHeight="1">
       <c r="A523" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-2</t>
+          <t>SC-2,CM-6 b</t>
         </is>
       </c>
       <c r="B523" s="2" t="inlineStr">
@@ -41224,7 +41224,7 @@
     <row r="524" ht="130" customHeight="1">
       <c r="A524" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-2</t>
+          <t>SC-2,CM-6 b</t>
         </is>
       </c>
       <c r="B524" s="2" t="inlineStr">
@@ -43535,12 +43535,18 @@
         <is>
           <t>To check how many characters are required in a password, run the following command:
  $ grep minlen /etc/security/pwquality.conf 
-Your output should contain  minlen =  
+Your output should contain  minlen = 15 
 If minlen is not found, or not equal to or greater than the required value then this is a finding.</t>
         </is>
       </c>
       <c r="L554" s="2" t="n"/>
-      <c r="M554" s="2" t="inlineStr"/>
+      <c r="M554" s="2" t="inlineStr">
+        <is>
+          <t>Configure Red Hat Enterprise Linux 9 to enforce a minimum 15-character password length.
+Add the following line to "/etc/security/pwquality.conf" (or modify the line to have the required value):
+minlen = 15</t>
+        </is>
+      </c>
       <c r="N554" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -43615,7 +43621,13 @@
         </is>
       </c>
       <c r="L555" s="2" t="n"/>
-      <c r="M555" s="2" t="inlineStr"/>
+      <c r="M555" s="2" t="inlineStr">
+        <is>
+          <t>Configure Red Hat Enterprise Linux 9 to enforce a minimum 15-character password length for new user accounts.
+Add, or modify the following line in the "/etc/login.defs" file:
+PASS_MIN_LEN 15</t>
+        </is>
+      </c>
       <c r="N555" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -43699,7 +43711,7 @@
     <row r="557" ht="130" customHeight="1">
       <c r="A557" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 a</t>
+          <t>SI-6 a,CM-3 (5)</t>
         </is>
       </c>
       <c r="B557" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@e8b288228919370eb9b8224cbb8a18b24b11ae6e 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -784,7 +784,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>SC-5,CM-6 b,SC-5 (2)</t>
+          <t>CM-6 b,SC-5 (2),SC-5</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -883,7 +883,7 @@
     <row r="6" ht="130" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (9),CM-5 (1),AU-7 b,AU-8 b,AC-6 (8),AU-12 (3),AU-7 a</t>
+          <t>AU-7 b,CM-5 (1),AU-12 (3),AC-6 (8),AC-6 (9),AU-7 a,AU-8 b</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -963,7 +963,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-12 c,CM-5 (1),AU-7 b,AU-12 a,AU-8 b,AU-12 (3),AU-7 a</t>
+          <t>AU-7 b,AU-12 c,CM-5 (1),AU-12 (3),CM-6 b,AU-7 a,AU-8 b,AU-12 a</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1037,7 +1037,7 @@
     <row r="8" ht="130" customHeight="1">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-6 b,AC-17 (1),AC-17 (9)</t>
+          <t>CM-6 b,AC-17 (9),CM-7 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
@@ -1484,7 +1484,7 @@
     <row r="14" ht="130" customHeight="1">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -1560,7 +1560,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -3286,7 +3286,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3370,7 +3370,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3455,7 +3455,7 @@
     <row r="40" ht="130" customHeight="1">
       <c r="A40" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B40" s="2" t="inlineStr">
@@ -3527,7 +3527,7 @@
     <row r="41" ht="130" customHeight="1">
       <c r="A41" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B41" s="2" t="inlineStr">
@@ -3832,7 +3832,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>IA-8,AU-3 (1),IA-2</t>
+          <t>AU-3 (1),IA-8,IA-2</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3910,7 +3910,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -3985,7 +3985,7 @@
     <row r="47" ht="130" customHeight="1">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
@@ -4060,7 +4060,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4135,7 +4135,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4210,7 +4210,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4285,7 +4285,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4360,7 +4360,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
@@ -4435,7 +4435,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4510,7 +4510,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4585,7 +4585,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4660,7 +4660,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4735,7 +4735,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4810,7 +4810,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4885,7 +4885,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -4965,7 +4965,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5048,7 +5048,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5128,7 +5128,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5208,7 +5208,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5288,7 +5288,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5368,7 +5368,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5442,7 +5442,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5516,7 +5516,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5590,7 +5590,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5664,7 +5664,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5738,7 +5738,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5811,7 +5811,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5884,7 +5884,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -5957,7 +5957,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6030,7 +6030,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6103,7 +6103,7 @@
     <row r="75" ht="130" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
@@ -6176,7 +6176,7 @@
     <row r="76" ht="130" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
@@ -6250,7 +6250,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6324,7 +6324,7 @@
     <row r="78" ht="130" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
@@ -6398,7 +6398,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6469,7 +6469,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6549,7 +6549,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6629,7 +6629,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B82" s="2" t="inlineStr">
@@ -6709,7 +6709,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B83" s="2" t="inlineStr">
@@ -6789,7 +6789,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B84" s="2" t="inlineStr">
@@ -6869,7 +6869,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B85" s="2" t="inlineStr">
@@ -6949,7 +6949,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -7029,7 +7029,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7109,7 +7109,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7189,7 +7189,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7269,7 +7269,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7425,7 +7425,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
@@ -7502,7 +7502,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
@@ -7582,7 +7582,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B94" s="2" t="inlineStr">
@@ -7662,7 +7662,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
@@ -7742,7 +7742,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7822,7 +7822,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7902,7 +7902,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -7982,7 +7982,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8062,7 +8062,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8142,7 +8142,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8222,7 +8222,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8295,7 +8295,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AC-2 (4),AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8376,7 +8376,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AC-2 (4),AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8457,7 +8457,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AC-2 (4),AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8528,7 +8528,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8603,7 +8603,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AC-2 (4),AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8685,7 +8685,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AC-2 (4),AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -8767,7 +8767,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AC-2 (4),AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -8849,7 +8849,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AC-2 (4),AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B110" s="2" t="inlineStr">
@@ -8931,7 +8931,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AC-2 (4),AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9013,7 +9013,7 @@
     <row r="112" ht="130" customHeight="1">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-14 (1),MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-14 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
@@ -9096,7 +9096,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9177,7 +9177,7 @@
     <row r="114" ht="130" customHeight="1">
       <c r="A114" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B114" s="2" t="inlineStr">
@@ -9263,7 +9263,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-6 (10)</t>
+          <t>AC-6 (10),AC-11 b</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9341,7 +9341,7 @@
     <row r="116" ht="130" customHeight="1">
       <c r="A116" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B116" s="2" t="inlineStr">
@@ -9707,7 +9707,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -9778,7 +9778,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -9849,7 +9849,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-12 c</t>
+          <t>AU-12 c,AU-9</t>
         </is>
       </c>
       <c r="B122" s="2" t="inlineStr">
@@ -10222,7 +10222,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AC-6 (9),AU-12 c,AC-2 (4)</t>
+          <t>AC-6 (9),AU-12 c,CM-5 (1),AC-2 (4)</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -10345,7 +10345,7 @@
     <row r="129" ht="130" customHeight="1">
       <c r="A129" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (b),IA-5 (1) (a),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (b),IA-5 (1) (a)</t>
         </is>
       </c>
       <c r="B129" s="2" t="inlineStr">
@@ -10665,7 +10665,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>SC-8,MA-4 c,AC-17 (2),SC-13</t>
+          <t>AC-17 (2),SC-8,MA-4 c,SC-13</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10747,7 +10747,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>AC-12,MA-4 e,SC-10,MA-4 (7)</t>
+          <t>SC-10,AC-12,MA-4 e,MA-4 (7)</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -10822,7 +10822,7 @@
     <row r="135" ht="130" customHeight="1">
       <c r="A135" s="2" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B135" s="2" t="inlineStr">
@@ -10901,7 +10901,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -11054,7 +11054,7 @@
     <row r="138" ht="130" customHeight="1">
       <c r="A138" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),CM-6 b,AU-14 (1),CM-5 (1),MA-4 (1) (a),AU-7 (1),AU-12 a,AU-3,AU-7 a,AU-6 (4)</t>
+          <t>AU-3,AU-3 (1),AU-7 (1),CM-5 (1),AU-12 a,CM-6 b,AU-14 (1),AU-7 a,MA-4 (1) (a),AU-6 (4)</t>
         </is>
       </c>
       <c r="B138" s="2" t="inlineStr">
@@ -11304,7 +11304,7 @@
     <row r="141" ht="130" customHeight="1">
       <c r="A141" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B141" s="2" t="inlineStr">
@@ -11380,7 +11380,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B142" s="2" t="inlineStr">
@@ -13125,7 +13125,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (1),SC-8 (2)</t>
+          <t>SC-8 (1),SC-8,SC-8 (2)</t>
         </is>
       </c>
       <c r="B166" s="2" t="inlineStr">
@@ -13278,7 +13278,7 @@
     <row r="168" ht="130" customHeight="1">
       <c r="A168" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2)</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B168" s="2" t="inlineStr">
@@ -13432,7 +13432,7 @@
     <row r="170" ht="130" customHeight="1">
       <c r="A170" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2)</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B170" s="2" t="inlineStr">
@@ -13581,7 +13581,7 @@
     <row r="172" ht="130" customHeight="1">
       <c r="A172" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B172" s="2" t="inlineStr">
@@ -13659,7 +13659,7 @@
     <row r="173" ht="130" customHeight="1">
       <c r="A173" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B173" s="2" t="inlineStr">
@@ -13742,7 +13742,7 @@
     <row r="174" ht="130" customHeight="1">
       <c r="A174" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B174" s="2" t="inlineStr">
@@ -14122,7 +14122,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-4 (1),AU-6 (4)</t>
+          <t>AU-4 (1),CM-6 b,AU-6 (4)</t>
         </is>
       </c>
       <c r="B179" s="2" t="inlineStr">
@@ -14193,7 +14193,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-6 b,AC-17 (1)</t>
+          <t>CM-6 b,CM-7 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B180" s="2" t="inlineStr">
@@ -16108,7 +16108,7 @@
     <row r="206" ht="130" customHeight="1">
       <c r="A206" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-4 (1)</t>
+          <t>AU-4 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B206" s="2" t="inlineStr">
@@ -17376,7 +17376,7 @@
     <row r="220" ht="130" customHeight="1">
       <c r="A220" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (5)</t>
+          <t>IA-2 (5),CM-6 b</t>
         </is>
       </c>
       <c r="B220" s="2" t="inlineStr">
@@ -17454,7 +17454,7 @@
     <row r="221" ht="130" customHeight="1">
       <c r="A221" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),IA-2 (3),IA-2 (2),IA-2,IA-2 (4)</t>
+          <t>IA-2 (4),IA-2,IA-2 (5),IA-2 (2),IA-2 (3)</t>
         </is>
       </c>
       <c r="B221" s="2" t="inlineStr">
@@ -17539,7 +17539,7 @@
     <row r="222" ht="130" customHeight="1">
       <c r="A222" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),IA-2 (3),IA-2 (2),IA-2,IA-2 (4)</t>
+          <t>IA-2 (4),IA-2,IA-2 (5),IA-2 (2),IA-2 (3)</t>
         </is>
       </c>
       <c r="B222" s="2" t="inlineStr">
@@ -17624,7 +17624,7 @@
     <row r="223" ht="130" customHeight="1">
       <c r="A223" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-18 (1),SC-8 (1)</t>
+          <t>SC-8 (1),SC-8,AC-18 (1)</t>
         </is>
       </c>
       <c r="B223" s="2" t="inlineStr">
@@ -18192,7 +18192,7 @@
     <row r="230" ht="130" customHeight="1">
       <c r="A230" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,IA-7</t>
+          <t>IA-7,CM-7 a</t>
         </is>
       </c>
       <c r="B230" s="2" t="inlineStr">
@@ -19260,7 +19260,7 @@
     <row r="244" ht="130" customHeight="1">
       <c r="A244" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-6 b,SC-2</t>
+          <t>SC-2,CM-6 b,SI-16</t>
         </is>
       </c>
       <c r="B244" s="2" t="inlineStr">
@@ -20334,7 +20334,7 @@
     <row r="258" ht="130" customHeight="1">
       <c r="A258" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B258" s="2" t="inlineStr">
@@ -20409,7 +20409,7 @@
     <row r="259" ht="130" customHeight="1">
       <c r="A259" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B259" s="2" t="inlineStr">
@@ -20497,7 +20497,7 @@
     <row r="260" ht="130" customHeight="1">
       <c r="A260" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B260" s="2" t="inlineStr">
@@ -20574,7 +20574,7 @@
     <row r="261" ht="130" customHeight="1">
       <c r="A261" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B261" s="2" t="inlineStr">
@@ -20732,7 +20732,7 @@
     <row r="263" ht="130" customHeight="1">
       <c r="A263" s="2" t="inlineStr">
         <is>
-          <t>AU-5 (1),AU-5 a</t>
+          <t>AU-5 a,AU-5 (1)</t>
         </is>
       </c>
       <c r="B263" s="2" t="inlineStr">
@@ -21259,7 +21259,7 @@
     <row r="270" ht="130" customHeight="1">
       <c r="A270" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (2),IA-2 (4),IA-2 (3)</t>
+          <t>IA-2 (4),IA-2 (2),IA-2 (3),IA-2 (1)</t>
         </is>
       </c>
       <c r="B270" s="2" t="inlineStr">
@@ -21727,7 +21727,7 @@
     <row r="276" ht="130" customHeight="1">
       <c r="A276" s="2" t="inlineStr">
         <is>
-          <t>SC-4,SC-2</t>
+          <t>SC-2,SC-4</t>
         </is>
       </c>
       <c r="B276" s="2" t="inlineStr">
@@ -21815,7 +21815,7 @@
     <row r="277" ht="130" customHeight="1">
       <c r="A277" s="2" t="inlineStr">
         <is>
-          <t>SC-4,SC-2</t>
+          <t>SC-2,SC-4</t>
         </is>
       </c>
       <c r="B277" s="2" t="inlineStr">
@@ -23545,7 +23545,7 @@
     <row r="299" ht="130" customHeight="1">
       <c r="A299" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (12),IA-2 (11),IA-2 (1)</t>
         </is>
       </c>
       <c r="B299" s="2" t="inlineStr">
@@ -24367,7 +24367,7 @@
     <row r="309" ht="130" customHeight="1">
       <c r="A309" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-8 (1) (a),AU-8 (1) (b)</t>
+          <t>AU-8 (1) (b),AU-8 b,AU-8 (1) (a)</t>
         </is>
       </c>
       <c r="B309" s="2" t="inlineStr">
@@ -25320,7 +25320,7 @@
     <row r="321" ht="130" customHeight="1">
       <c r="A321" s="2" t="inlineStr">
         <is>
-          <t>AC-3 (4),IA-11</t>
+          <t>IA-11,AC-3 (4)</t>
         </is>
       </c>
       <c r="B321" s="2" t="inlineStr">
@@ -25784,7 +25784,7 @@
     <row r="327" ht="130" customHeight="1">
       <c r="A327" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AU-12 c</t>
+          <t>AU-12 c,CM-5 (1)</t>
         </is>
       </c>
       <c r="B327" s="2" t="inlineStr">
@@ -26860,7 +26860,7 @@
     <row r="341" ht="130" customHeight="1">
       <c r="A341" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,IA-3</t>
+          <t>IA-3,CM-7 b</t>
         </is>
       </c>
       <c r="B341" s="2" t="inlineStr">
@@ -27169,7 +27169,7 @@
     <row r="345" ht="130" customHeight="1">
       <c r="A345" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,AC-18 (1)</t>
+          <t>AC-18 (1),CM-7 a</t>
         </is>
       </c>
       <c r="B345" s="2" t="inlineStr">
@@ -27246,7 +27246,7 @@
     <row r="346" ht="130" customHeight="1">
       <c r="A346" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B346" s="2" t="inlineStr">
@@ -28340,7 +28340,7 @@
     <row r="360" ht="130" customHeight="1">
       <c r="A360" s="2" t="inlineStr">
         <is>
-          <t>SI-6 d,SI-6 b,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 d,SI-6 b</t>
         </is>
       </c>
       <c r="B360" s="2" t="inlineStr">
@@ -28431,7 +28431,7 @@
     <row r="361" ht="130" customHeight="1">
       <c r="A361" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B361" s="2" t="inlineStr">
@@ -29351,7 +29351,7 @@
     <row r="373" ht="130" customHeight="1">
       <c r="A373" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B373" s="2" t="inlineStr">
@@ -29422,7 +29422,7 @@
     <row r="374" ht="130" customHeight="1">
       <c r="A374" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B374" s="2" t="inlineStr">
@@ -29494,7 +29494,7 @@
     <row r="375" ht="130" customHeight="1">
       <c r="A375" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B375" s="2" t="inlineStr">
@@ -30254,7 +30254,7 @@
     <row r="384" ht="130" customHeight="1">
       <c r="A384" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-17 (2)</t>
+          <t>AC-17 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B384" s="2" t="inlineStr">
@@ -30702,7 +30702,7 @@
     <row r="390" ht="130" customHeight="1">
       <c r="A390" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (a),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (a)</t>
         </is>
       </c>
       <c r="B390" s="2" t="inlineStr">
@@ -31184,7 +31184,7 @@
     <row r="396" ht="130" customHeight="1">
       <c r="A396" s="2" t="inlineStr">
         <is>
-          <t>SI-6 d,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 d</t>
         </is>
       </c>
       <c r="B396" s="2" t="inlineStr">
@@ -31268,7 +31268,7 @@
     <row r="397" ht="130" customHeight="1">
       <c r="A397" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-6 b</t>
+          <t>CM-6 b,SI-16</t>
         </is>
       </c>
       <c r="B397" s="2" t="inlineStr">
@@ -35104,7 +35104,7 @@
     <row r="447" ht="130" customHeight="1">
       <c r="A447" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),CM-6 b</t>
         </is>
       </c>
       <c r="B447" s="2" t="inlineStr">
@@ -35254,7 +35254,7 @@
     <row r="449" ht="130" customHeight="1">
       <c r="A449" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),CM-6 b</t>
+          <t>CM-6 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B449" s="2" t="inlineStr">
@@ -35327,7 +35327,7 @@
     <row r="450" ht="130" customHeight="1">
       <c r="A450" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),CM-6 b</t>
+          <t>CM-6 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B450" s="2" t="inlineStr">
@@ -41138,7 +41138,7 @@
     <row r="523" ht="130" customHeight="1">
       <c r="A523" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-2</t>
+          <t>SC-2,CM-6 b</t>
         </is>
       </c>
       <c r="B523" s="2" t="inlineStr">
@@ -41225,7 +41225,7 @@
     <row r="524" ht="130" customHeight="1">
       <c r="A524" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-2</t>
+          <t>SC-2,CM-6 b</t>
         </is>
       </c>
       <c r="B524" s="2" t="inlineStr">
@@ -43712,7 +43712,7 @@
     <row r="557" ht="130" customHeight="1">
       <c r="A557" s="2" t="inlineStr">
         <is>
-          <t>SI-6 a,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 a</t>
         </is>
       </c>
       <c r="B557" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@8e3f9b14c7fb366fb7b45878ba15b4606c5b8fea 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -541,7 +541,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-4</t>
+          <t>AU-4,AU-4 (1)</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -625,7 +625,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-14 (1)</t>
+          <t>AU-14 (1),AU-4</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -708,7 +708,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-4</t>
+          <t>AU-4,CM-6 b</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -784,7 +784,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-5 (2),SC-5</t>
+          <t>SC-5,CM-6 b,SC-5 (2)</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -883,7 +883,7 @@
     <row r="6" ht="130" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>AU-7 b,CM-5 (1),AU-12 (3),AC-6 (8),AC-6 (9),AU-7 a,AU-8 b</t>
+          <t>AU-8 b,AU-7 a,AC-6 (9),CM-5 (1),AC-6 (8),AU-7 b,AU-12 (3)</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -963,7 +963,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-7 b,AU-12 c,CM-5 (1),AU-12 (3),CM-6 b,AU-7 a,AU-8 b,AU-12 a</t>
+          <t>AU-8 b,CM-6 b,AU-7 a,AU-12 c,CM-5 (1),AU-7 b,AU-12 (3),AU-12 a</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1037,7 +1037,7 @@
     <row r="8" ht="130" customHeight="1">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-17 (9),CM-7 b,AC-17 (1)</t>
+          <t>AC-17 (9),CM-7 b,AC-17 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
@@ -1257,7 +1257,7 @@
     <row r="11" ht="130" customHeight="1">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B11" s="2" t="inlineStr">
@@ -1334,7 +1334,7 @@
     <row r="12" ht="130" customHeight="1">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
@@ -1714,7 +1714,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -2084,7 +2084,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -2158,7 +2158,7 @@
     <row r="23" ht="130" customHeight="1">
       <c r="A23" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B23" s="2" t="inlineStr">
@@ -3286,7 +3286,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3370,7 +3370,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3455,7 +3455,7 @@
     <row r="40" ht="130" customHeight="1">
       <c r="A40" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B40" s="2" t="inlineStr">
@@ -3527,7 +3527,7 @@
     <row r="41" ht="130" customHeight="1">
       <c r="A41" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B41" s="2" t="inlineStr">
@@ -3832,7 +3832,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),IA-8,IA-2</t>
+          <t>IA-8,AU-3 (1),IA-2</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3910,7 +3910,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -3985,7 +3985,7 @@
     <row r="47" ht="130" customHeight="1">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
@@ -4060,7 +4060,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4135,7 +4135,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4210,7 +4210,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4285,7 +4285,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4360,7 +4360,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
@@ -4435,7 +4435,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4510,7 +4510,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4585,7 +4585,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4660,7 +4660,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4735,7 +4735,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4810,7 +4810,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4885,7 +4885,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -4965,7 +4965,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5048,7 +5048,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5128,7 +5128,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5208,7 +5208,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5288,7 +5288,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5368,7 +5368,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5442,7 +5442,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5516,7 +5516,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5590,7 +5590,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5664,7 +5664,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5738,7 +5738,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5811,7 +5811,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5884,7 +5884,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -5957,7 +5957,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6030,7 +6030,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6103,7 +6103,7 @@
     <row r="75" ht="130" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
@@ -6176,7 +6176,7 @@
     <row r="76" ht="130" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
@@ -6250,7 +6250,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6324,7 +6324,7 @@
     <row r="78" ht="130" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
@@ -6398,7 +6398,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6469,7 +6469,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6549,7 +6549,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6629,7 +6629,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B82" s="2" t="inlineStr">
@@ -6709,7 +6709,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B83" s="2" t="inlineStr">
@@ -6789,7 +6789,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B84" s="2" t="inlineStr">
@@ -6869,7 +6869,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B85" s="2" t="inlineStr">
@@ -6949,7 +6949,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -7029,7 +7029,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7109,7 +7109,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7189,7 +7189,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7269,7 +7269,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7349,7 +7349,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7425,7 +7425,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
@@ -7502,7 +7502,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
@@ -7582,7 +7582,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B94" s="2" t="inlineStr">
@@ -7662,7 +7662,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
@@ -7742,7 +7742,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7822,7 +7822,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7902,7 +7902,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -7982,7 +7982,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8062,7 +8062,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8142,7 +8142,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8222,7 +8222,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8295,7 +8295,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AC-2 (4),AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8376,7 +8376,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AC-2 (4),AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8457,7 +8457,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AC-2 (4),AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8528,7 +8528,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AC-2 (4),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8603,7 +8603,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AC-2 (4),AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8685,7 +8685,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AC-2 (4),AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -8767,7 +8767,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AC-2 (4),AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -8849,7 +8849,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AC-2 (4),AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B110" s="2" t="inlineStr">
@@ -8931,7 +8931,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AC-2 (4),AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9013,7 +9013,7 @@
     <row r="112" ht="130" customHeight="1">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-14 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-14 (1),AU-3,AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
@@ -9096,7 +9096,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9177,7 +9177,7 @@
     <row r="114" ht="130" customHeight="1">
       <c r="A114" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B114" s="2" t="inlineStr">
@@ -9263,7 +9263,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),AC-11 b</t>
+          <t>AC-11 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9341,7 +9341,7 @@
     <row r="116" ht="130" customHeight="1">
       <c r="A116" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B116" s="2" t="inlineStr">
@@ -9707,7 +9707,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -9778,7 +9778,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -10222,7 +10222,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (9),AU-12 c,CM-5 (1),AC-2 (4)</t>
+          <t>AU-12 c,AC-2 (4),AC-6 (9),CM-5 (1)</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -10345,7 +10345,7 @@
     <row r="129" ht="130" customHeight="1">
       <c r="A129" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (b),IA-5 (1) (a)</t>
+          <t>IA-5 (1) (a),CM-6 b,IA-5 (1) (b)</t>
         </is>
       </c>
       <c r="B129" s="2" t="inlineStr">
@@ -10747,7 +10747,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>SC-10,AC-12,MA-4 e,MA-4 (7)</t>
+          <t>AC-12,MA-4 (7),MA-4 e,SC-10</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -10822,7 +10822,7 @@
     <row r="135" ht="130" customHeight="1">
       <c r="A135" s="2" t="inlineStr">
         <is>
-          <t>SC-10,AC-12</t>
+          <t>AC-12,SC-10</t>
         </is>
       </c>
       <c r="B135" s="2" t="inlineStr">
@@ -10901,7 +10901,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>SC-10,AC-12</t>
+          <t>AC-12,SC-10</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -10977,7 +10977,7 @@
     <row r="137" ht="130" customHeight="1">
       <c r="A137" s="2" t="inlineStr">
         <is>
-          <t>SC-10,AC-11 a</t>
+          <t>AC-11 a,SC-10</t>
         </is>
       </c>
       <c r="B137" s="2" t="inlineStr">
@@ -11054,7 +11054,7 @@
     <row r="138" ht="130" customHeight="1">
       <c r="A138" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-7 (1),CM-5 (1),AU-12 a,CM-6 b,AU-14 (1),AU-7 a,MA-4 (1) (a),AU-6 (4)</t>
+          <t>CM-6 b,AU-7 a,MA-4 (1) (a),AU-14 (1),AU-3,CM-5 (1),AU-6 (4),AU-3 (1),AU-7 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B138" s="2" t="inlineStr">
@@ -11456,7 +11456,7 @@
     <row r="143" ht="130" customHeight="1">
       <c r="A143" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B143" s="2" t="inlineStr">
@@ -11525,7 +11525,7 @@
     <row r="144" ht="130" customHeight="1">
       <c r="A144" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B144" s="2" t="inlineStr">
@@ -11594,7 +11594,7 @@
     <row r="145" ht="130" customHeight="1">
       <c r="A145" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B145" s="2" t="inlineStr">
@@ -11664,7 +11664,7 @@
     <row r="146" ht="130" customHeight="1">
       <c r="A146" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B146" s="2" t="inlineStr">
@@ -11733,7 +11733,7 @@
     <row r="147" ht="130" customHeight="1">
       <c r="A147" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B147" s="2" t="inlineStr">
@@ -11802,7 +11802,7 @@
     <row r="148" ht="130" customHeight="1">
       <c r="A148" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B148" s="2" t="inlineStr">
@@ -11872,7 +11872,7 @@
     <row r="149" ht="130" customHeight="1">
       <c r="A149" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B149" s="2" t="inlineStr">
@@ -11941,7 +11941,7 @@
     <row r="150" ht="130" customHeight="1">
       <c r="A150" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B150" s="2" t="inlineStr">
@@ -12010,7 +12010,7 @@
     <row r="151" ht="130" customHeight="1">
       <c r="A151" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B151" s="2" t="inlineStr">
@@ -12080,7 +12080,7 @@
     <row r="152" ht="130" customHeight="1">
       <c r="A152" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B152" s="2" t="inlineStr">
@@ -12149,7 +12149,7 @@
     <row r="153" ht="130" customHeight="1">
       <c r="A153" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B153" s="2" t="inlineStr">
@@ -12218,7 +12218,7 @@
     <row r="154" ht="130" customHeight="1">
       <c r="A154" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B154" s="2" t="inlineStr">
@@ -12287,7 +12287,7 @@
     <row r="155" ht="130" customHeight="1">
       <c r="A155" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B155" s="2" t="inlineStr">
@@ -13125,7 +13125,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8,SC-8 (2)</t>
+          <t>SC-8,SC-8 (2),SC-8 (1)</t>
         </is>
       </c>
       <c r="B166" s="2" t="inlineStr">
@@ -13278,7 +13278,7 @@
     <row r="168" ht="130" customHeight="1">
       <c r="A168" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8</t>
+          <t>SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B168" s="2" t="inlineStr">
@@ -13581,7 +13581,7 @@
     <row r="172" ht="130" customHeight="1">
       <c r="A172" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B172" s="2" t="inlineStr">
@@ -13659,7 +13659,7 @@
     <row r="173" ht="130" customHeight="1">
       <c r="A173" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B173" s="2" t="inlineStr">
@@ -13742,7 +13742,7 @@
     <row r="174" ht="130" customHeight="1">
       <c r="A174" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B174" s="2" t="inlineStr">
@@ -14122,7 +14122,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),CM-6 b,AU-6 (4)</t>
+          <t>AU-6 (4),CM-6 b,AU-4 (1)</t>
         </is>
       </c>
       <c r="B179" s="2" t="inlineStr">
@@ -16108,7 +16108,7 @@
     <row r="206" ht="130" customHeight="1">
       <c r="A206" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),CM-6 b</t>
+          <t>CM-6 b,AU-4 (1)</t>
         </is>
       </c>
       <c r="B206" s="2" t="inlineStr">
@@ -16934,7 +16934,7 @@
     <row r="215" ht="130" customHeight="1">
       <c r="A215" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (9),AU-12 c,AC-2 (4)</t>
+          <t>AU-12 c,AC-2 (4),AC-6 (9)</t>
         </is>
       </c>
       <c r="B215" s="2" t="inlineStr">
@@ -17376,7 +17376,7 @@
     <row r="220" ht="130" customHeight="1">
       <c r="A220" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),CM-6 b</t>
+          <t>CM-6 b,IA-2 (5)</t>
         </is>
       </c>
       <c r="B220" s="2" t="inlineStr">
@@ -17454,7 +17454,7 @@
     <row r="221" ht="130" customHeight="1">
       <c r="A221" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2,IA-2 (5),IA-2 (2),IA-2 (3)</t>
+          <t>IA-2,IA-2 (2),IA-2 (4),IA-2 (5),IA-2 (3)</t>
         </is>
       </c>
       <c r="B221" s="2" t="inlineStr">
@@ -17539,7 +17539,7 @@
     <row r="222" ht="130" customHeight="1">
       <c r="A222" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2,IA-2 (5),IA-2 (2),IA-2 (3)</t>
+          <t>IA-2,IA-2 (2),IA-2 (4),IA-2 (5),IA-2 (3)</t>
         </is>
       </c>
       <c r="B222" s="2" t="inlineStr">
@@ -18192,7 +18192,7 @@
     <row r="230" ht="130" customHeight="1">
       <c r="A230" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-7 a</t>
+          <t>CM-7 a,IA-7</t>
         </is>
       </c>
       <c r="B230" s="2" t="inlineStr">
@@ -18271,7 +18271,7 @@
     <row r="231" ht="130" customHeight="1">
       <c r="A231" s="2" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B231" s="2" t="inlineStr">
@@ -18430,7 +18430,7 @@
     <row r="233" ht="130" customHeight="1">
       <c r="A233" s="2" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B233" s="2" t="inlineStr">
@@ -19027,7 +19027,7 @@
     <row r="241" ht="130" customHeight="1">
       <c r="A241" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B241" s="2" t="inlineStr">
@@ -19098,7 +19098,7 @@
     <row r="242" ht="130" customHeight="1">
       <c r="A242" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B242" s="2" t="inlineStr">
@@ -19260,7 +19260,7 @@
     <row r="244" ht="130" customHeight="1">
       <c r="A244" s="2" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b,SI-16</t>
+          <t>SI-16,CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B244" s="2" t="inlineStr">
@@ -19420,7 +19420,7 @@
     <row r="246" ht="130" customHeight="1">
       <c r="A246" s="2" t="inlineStr">
         <is>
-          <t>SI-16,SC-3</t>
+          <t>SC-3,SI-16</t>
         </is>
       </c>
       <c r="B246" s="2" t="inlineStr">
@@ -20334,7 +20334,7 @@
     <row r="258" ht="130" customHeight="1">
       <c r="A258" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B258" s="2" t="inlineStr">
@@ -20409,7 +20409,7 @@
     <row r="259" ht="130" customHeight="1">
       <c r="A259" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B259" s="2" t="inlineStr">
@@ -20497,7 +20497,7 @@
     <row r="260" ht="130" customHeight="1">
       <c r="A260" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B260" s="2" t="inlineStr">
@@ -20574,7 +20574,7 @@
     <row r="261" ht="130" customHeight="1">
       <c r="A261" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B261" s="2" t="inlineStr">
@@ -21172,7 +21172,7 @@
     <row r="269" ht="130" customHeight="1">
       <c r="A269" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (2)</t>
+          <t>IA-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B269" s="2" t="inlineStr">
@@ -21259,7 +21259,7 @@
     <row r="270" ht="130" customHeight="1">
       <c r="A270" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2 (2),IA-2 (3),IA-2 (1)</t>
+          <t>IA-2 (2),IA-2 (1),IA-2 (4),IA-2 (3)</t>
         </is>
       </c>
       <c r="B270" s="2" t="inlineStr">
@@ -21428,7 +21428,7 @@
     <row r="272" ht="130" customHeight="1">
       <c r="A272" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B272" s="2" t="inlineStr">
@@ -21646,7 +21646,7 @@
     <row r="275" ht="130" customHeight="1">
       <c r="A275" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-4</t>
+          <t>SC-4,CM-6 b</t>
         </is>
       </c>
       <c r="B275" s="2" t="inlineStr">
@@ -21727,7 +21727,7 @@
     <row r="276" ht="130" customHeight="1">
       <c r="A276" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SC-4</t>
+          <t>SC-4,SC-2</t>
         </is>
       </c>
       <c r="B276" s="2" t="inlineStr">
@@ -21815,7 +21815,7 @@
     <row r="277" ht="130" customHeight="1">
       <c r="A277" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SC-4</t>
+          <t>SC-4,SC-2</t>
         </is>
       </c>
       <c r="B277" s="2" t="inlineStr">
@@ -22276,7 +22276,7 @@
     <row r="283" ht="130" customHeight="1">
       <c r="A283" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (3)</t>
+          <t>CM-5 (3),CM-6 b</t>
         </is>
       </c>
       <c r="B283" s="2" t="inlineStr">
@@ -23376,7 +23376,7 @@
     <row r="297" ht="130" customHeight="1">
       <c r="A297" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B297" s="2" t="inlineStr">
@@ -23545,7 +23545,7 @@
     <row r="299" ht="130" customHeight="1">
       <c r="A299" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11),IA-2 (1)</t>
+          <t>IA-2 (1),IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B299" s="2" t="inlineStr">
@@ -24367,7 +24367,7 @@
     <row r="309" ht="130" customHeight="1">
       <c r="A309" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (b),AU-8 b,AU-8 (1) (a)</t>
+          <t>AU-8 (1) (b),AU-8 (1) (a),AU-8 b</t>
         </is>
       </c>
       <c r="B309" s="2" t="inlineStr">
@@ -25784,7 +25784,7 @@
     <row r="327" ht="130" customHeight="1">
       <c r="A327" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,CM-5 (1)</t>
+          <t>CM-5 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B327" s="2" t="inlineStr">
@@ -26860,7 +26860,7 @@
     <row r="341" ht="130" customHeight="1">
       <c r="A341" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-7 b</t>
+          <t>CM-7 b,IA-3</t>
         </is>
       </c>
       <c r="B341" s="2" t="inlineStr">
@@ -26935,7 +26935,7 @@
     <row r="342" ht="130" customHeight="1">
       <c r="A342" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-7 b</t>
+          <t>CM-7 b,CM-7 a</t>
         </is>
       </c>
       <c r="B342" s="2" t="inlineStr">
@@ -27009,7 +27009,7 @@
     <row r="343" ht="130" customHeight="1">
       <c r="A343" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-7 b</t>
+          <t>CM-7 b,CM-7 a</t>
         </is>
       </c>
       <c r="B343" s="2" t="inlineStr">
@@ -27169,7 +27169,7 @@
     <row r="345" ht="130" customHeight="1">
       <c r="A345" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),CM-7 a</t>
+          <t>CM-7 a,AC-18 (1)</t>
         </is>
       </c>
       <c r="B345" s="2" t="inlineStr">
@@ -27246,7 +27246,7 @@
     <row r="346" ht="130" customHeight="1">
       <c r="A346" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-7 a,CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (c),CM-7 a</t>
         </is>
       </c>
       <c r="B346" s="2" t="inlineStr">
@@ -30702,7 +30702,7 @@
     <row r="390" ht="130" customHeight="1">
       <c r="A390" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (a)</t>
+          <t>IA-5 (1) (a),CM-6 b</t>
         </is>
       </c>
       <c r="B390" s="2" t="inlineStr">
@@ -31268,7 +31268,7 @@
     <row r="397" ht="130" customHeight="1">
       <c r="A397" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-16</t>
+          <t>SI-16,CM-6 b</t>
         </is>
       </c>
       <c r="B397" s="2" t="inlineStr">
@@ -31509,7 +31509,7 @@
     <row r="400" ht="130" customHeight="1">
       <c r="A400" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B400" s="2" t="inlineStr">
@@ -31600,7 +31600,7 @@
     <row r="401" ht="130" customHeight="1">
       <c r="A401" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B401" s="2" t="inlineStr">
@@ -31694,7 +31694,7 @@
     <row r="402" ht="130" customHeight="1">
       <c r="A402" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B402" s="2" t="inlineStr">
@@ -35254,7 +35254,7 @@
     <row r="449" ht="130" customHeight="1">
       <c r="A449" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (1)</t>
+          <t>CM-5 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B449" s="2" t="inlineStr">
@@ -35327,7 +35327,7 @@
     <row r="450" ht="130" customHeight="1">
       <c r="A450" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (1)</t>
+          <t>CM-5 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B450" s="2" t="inlineStr">
@@ -41138,7 +41138,7 @@
     <row r="523" ht="130" customHeight="1">
       <c r="A523" s="2" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b</t>
+          <t>CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B523" s="2" t="inlineStr">
@@ -41225,7 +41225,7 @@
     <row r="524" ht="130" customHeight="1">
       <c r="A524" s="2" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b</t>
+          <t>CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B524" s="2" t="inlineStr">
@@ -42457,7 +42457,7 @@
     <row r="540" ht="130" customHeight="1">
       <c r="A540" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-2 (2)</t>
+          <t>SI-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B540" s="2" t="inlineStr">
@@ -43104,7 +43104,7 @@
     <row r="549" ht="130" customHeight="1">
       <c r="A549" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-2 (2)</t>
+          <t>SI-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B549" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@05d38fec65ef1e7118a8b709216adf9d059cb830 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -625,7 +625,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),AU-4</t>
+          <t>AU-4,AU-14 (1)</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -784,7 +784,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>SC-5,CM-6 b,SC-5 (2)</t>
+          <t>SC-5,SC-5 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -883,7 +883,7 @@
     <row r="6" ht="130" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-7 a,AC-6 (9),CM-5 (1),AC-6 (8),AU-7 b,AU-12 (3)</t>
+          <t>AU-7 a,AC-6 (9),AU-7 b,CM-5 (1),AU-12 (3),AC-6 (8),AU-8 b</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -963,7 +963,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,CM-6 b,AU-7 a,AU-12 c,CM-5 (1),AU-7 b,AU-12 (3),AU-12 a</t>
+          <t>AU-7 a,CM-6 b,AU-7 b,AU-12 c,CM-5 (1),AU-12 (3),AU-12 a,AU-8 b</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -3286,7 +3286,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3370,7 +3370,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3455,7 +3455,7 @@
     <row r="40" ht="130" customHeight="1">
       <c r="A40" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B40" s="2" t="inlineStr">
@@ -3527,7 +3527,7 @@
     <row r="41" ht="130" customHeight="1">
       <c r="A41" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B41" s="2" t="inlineStr">
@@ -3832,7 +3832,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>IA-8,AU-3 (1),IA-2</t>
+          <t>AU-3 (1),IA-2,IA-8</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3910,7 +3910,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -3985,7 +3985,7 @@
     <row r="47" ht="130" customHeight="1">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
@@ -4060,7 +4060,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4135,7 +4135,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4210,7 +4210,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4285,7 +4285,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4360,7 +4360,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
@@ -4435,7 +4435,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4510,7 +4510,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4585,7 +4585,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4660,7 +4660,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4735,7 +4735,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4810,7 +4810,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4885,7 +4885,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -4965,7 +4965,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5048,7 +5048,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5128,7 +5128,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5208,7 +5208,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5288,7 +5288,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5368,7 +5368,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5442,7 +5442,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5516,7 +5516,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5590,7 +5590,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5664,7 +5664,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5738,7 +5738,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5811,7 +5811,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5884,7 +5884,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -5957,7 +5957,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6030,7 +6030,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6103,7 +6103,7 @@
     <row r="75" ht="130" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
@@ -6176,7 +6176,7 @@
     <row r="76" ht="130" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
@@ -6250,7 +6250,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6324,7 +6324,7 @@
     <row r="78" ht="130" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
@@ -6398,7 +6398,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6469,7 +6469,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6549,7 +6549,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6629,7 +6629,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B82" s="2" t="inlineStr">
@@ -6709,7 +6709,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B83" s="2" t="inlineStr">
@@ -6789,7 +6789,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B84" s="2" t="inlineStr">
@@ -6949,7 +6949,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -7029,7 +7029,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7109,7 +7109,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7189,7 +7189,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7269,7 +7269,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7349,7 +7349,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7425,7 +7425,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
@@ -7502,7 +7502,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
@@ -7582,7 +7582,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B94" s="2" t="inlineStr">
@@ -7662,7 +7662,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
@@ -7742,7 +7742,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7822,7 +7822,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7902,7 +7902,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -7982,7 +7982,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8062,7 +8062,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8142,7 +8142,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8222,7 +8222,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8295,7 +8295,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AC-2 (4),AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8376,7 +8376,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AC-2 (4),AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8457,7 +8457,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AC-2 (4),AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8528,7 +8528,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AC-2 (4),AU-3,AU-3 (1)</t>
+          <t>AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8603,7 +8603,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AC-2 (4),AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8685,7 +8685,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AC-2 (4),AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -8767,7 +8767,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AC-2 (4),AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -8849,7 +8849,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AC-2 (4),AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B110" s="2" t="inlineStr">
@@ -8931,7 +8931,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AC-2 (4),AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9013,7 +9013,7 @@
     <row r="112" ht="130" customHeight="1">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-14 (1),AU-3,AU-3 (1),AU-12 a</t>
+          <t>AU-14 (1),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
@@ -9707,7 +9707,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -9778,7 +9778,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -10222,7 +10222,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-2 (4),AC-6 (9),CM-5 (1)</t>
+          <t>CM-5 (1),AC-6 (9),AU-12 c,AC-2 (4)</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -10345,7 +10345,7 @@
     <row r="129" ht="130" customHeight="1">
       <c r="A129" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (a),CM-6 b,IA-5 (1) (b)</t>
+          <t>CM-6 b,IA-5 (1) (a),IA-5 (1) (b)</t>
         </is>
       </c>
       <c r="B129" s="2" t="inlineStr">
@@ -10665,7 +10665,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8,MA-4 c,SC-13</t>
+          <t>SC-8,MA-4 c,AC-17 (2),SC-13</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10747,7 +10747,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>AC-12,MA-4 (7),MA-4 e,SC-10</t>
+          <t>MA-4 e,MA-4 (7),AC-12,SC-10</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -11054,7 +11054,7 @@
     <row r="138" ht="130" customHeight="1">
       <c r="A138" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-7 a,MA-4 (1) (a),AU-14 (1),AU-3,CM-5 (1),AU-6 (4),AU-3 (1),AU-7 (1),AU-12 a</t>
+          <t>AU-7 a,AU-6 (4),AU-14 (1),CM-6 b,AU-3 (1),CM-5 (1),AU-7 (1),MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B138" s="2" t="inlineStr">
@@ -11456,7 +11456,7 @@
     <row r="143" ht="130" customHeight="1">
       <c r="A143" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B143" s="2" t="inlineStr">
@@ -11525,7 +11525,7 @@
     <row r="144" ht="130" customHeight="1">
       <c r="A144" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B144" s="2" t="inlineStr">
@@ -11594,7 +11594,7 @@
     <row r="145" ht="130" customHeight="1">
       <c r="A145" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B145" s="2" t="inlineStr">
@@ -11664,7 +11664,7 @@
     <row r="146" ht="130" customHeight="1">
       <c r="A146" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B146" s="2" t="inlineStr">
@@ -11733,7 +11733,7 @@
     <row r="147" ht="130" customHeight="1">
       <c r="A147" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B147" s="2" t="inlineStr">
@@ -11802,7 +11802,7 @@
     <row r="148" ht="130" customHeight="1">
       <c r="A148" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B148" s="2" t="inlineStr">
@@ -11872,7 +11872,7 @@
     <row r="149" ht="130" customHeight="1">
       <c r="A149" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B149" s="2" t="inlineStr">
@@ -11941,7 +11941,7 @@
     <row r="150" ht="130" customHeight="1">
       <c r="A150" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B150" s="2" t="inlineStr">
@@ -12010,7 +12010,7 @@
     <row r="151" ht="130" customHeight="1">
       <c r="A151" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B151" s="2" t="inlineStr">
@@ -12080,7 +12080,7 @@
     <row r="152" ht="130" customHeight="1">
       <c r="A152" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B152" s="2" t="inlineStr">
@@ -12149,7 +12149,7 @@
     <row r="153" ht="130" customHeight="1">
       <c r="A153" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B153" s="2" t="inlineStr">
@@ -12218,7 +12218,7 @@
     <row r="154" ht="130" customHeight="1">
       <c r="A154" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B154" s="2" t="inlineStr">
@@ -12287,7 +12287,7 @@
     <row r="155" ht="130" customHeight="1">
       <c r="A155" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B155" s="2" t="inlineStr">
@@ -13125,7 +13125,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (2),SC-8 (1)</t>
+          <t>SC-8,SC-8 (1),SC-8 (2)</t>
         </is>
       </c>
       <c r="B166" s="2" t="inlineStr">
@@ -13432,7 +13432,7 @@
     <row r="170" ht="130" customHeight="1">
       <c r="A170" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8</t>
+          <t>SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B170" s="2" t="inlineStr">
@@ -13581,7 +13581,7 @@
     <row r="172" ht="130" customHeight="1">
       <c r="A172" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B172" s="2" t="inlineStr">
@@ -13659,7 +13659,7 @@
     <row r="173" ht="130" customHeight="1">
       <c r="A173" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B173" s="2" t="inlineStr">
@@ -13742,7 +13742,7 @@
     <row r="174" ht="130" customHeight="1">
       <c r="A174" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B174" s="2" t="inlineStr">
@@ -14122,7 +14122,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="2" t="inlineStr">
         <is>
-          <t>AU-6 (4),CM-6 b,AU-4 (1)</t>
+          <t>AU-4 (1),AU-6 (4),CM-6 b</t>
         </is>
       </c>
       <c r="B179" s="2" t="inlineStr">
@@ -14193,7 +14193,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 b,AC-17 (1)</t>
+          <t>CM-7 b,AC-17 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B180" s="2" t="inlineStr">
@@ -14272,7 +14272,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">
@@ -14344,7 +14344,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B182" s="2" t="inlineStr">
@@ -14416,7 +14416,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B183" s="2" t="inlineStr">
@@ -14490,7 +14490,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B184" s="2" t="inlineStr">
@@ -14564,7 +14564,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B185" s="2" t="inlineStr">
@@ -14638,7 +14638,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B186" s="2" t="inlineStr">
@@ -15593,7 +15593,7 @@
     <row r="199" ht="130" customHeight="1">
       <c r="A199" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-4 (1)</t>
+          <t>AU-4 (1),AU-3</t>
         </is>
       </c>
       <c r="B199" s="2" t="inlineStr">
@@ -16108,7 +16108,7 @@
     <row r="206" ht="130" customHeight="1">
       <c r="A206" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-4 (1)</t>
+          <t>AU-4 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B206" s="2" t="inlineStr">
@@ -16188,7 +16188,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>SC-28 (1),SC-28</t>
+          <t>SC-28,SC-28 (1)</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -16934,7 +16934,7 @@
     <row r="215" ht="130" customHeight="1">
       <c r="A215" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-2 (4),AC-6 (9)</t>
+          <t>AC-6 (9),AU-12 c,AC-2 (4)</t>
         </is>
       </c>
       <c r="B215" s="2" t="inlineStr">
@@ -17376,7 +17376,7 @@
     <row r="220" ht="130" customHeight="1">
       <c r="A220" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (5)</t>
+          <t>IA-2 (5),CM-6 b</t>
         </is>
       </c>
       <c r="B220" s="2" t="inlineStr">
@@ -17454,7 +17454,7 @@
     <row r="221" ht="130" customHeight="1">
       <c r="A221" s="2" t="inlineStr">
         <is>
-          <t>IA-2,IA-2 (2),IA-2 (4),IA-2 (5),IA-2 (3)</t>
+          <t>IA-2 (3),IA-2 (5),IA-2 (2),IA-2,IA-2 (4)</t>
         </is>
       </c>
       <c r="B221" s="2" t="inlineStr">
@@ -17539,7 +17539,7 @@
     <row r="222" ht="130" customHeight="1">
       <c r="A222" s="2" t="inlineStr">
         <is>
-          <t>IA-2,IA-2 (2),IA-2 (4),IA-2 (5),IA-2 (3)</t>
+          <t>IA-2 (3),IA-2 (5),IA-2 (2),IA-2,IA-2 (4)</t>
         </is>
       </c>
       <c r="B222" s="2" t="inlineStr">
@@ -17624,7 +17624,7 @@
     <row r="223" ht="130" customHeight="1">
       <c r="A223" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8,AC-18 (1)</t>
+          <t>SC-8,SC-8 (1),AC-18 (1)</t>
         </is>
       </c>
       <c r="B223" s="2" t="inlineStr">
@@ -17791,7 +17791,7 @@
     <row r="225" ht="130" customHeight="1">
       <c r="A225" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),IA-7</t>
+          <t>IA-7,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B225" s="2" t="inlineStr">
@@ -17874,7 +17874,7 @@
     <row r="226" ht="130" customHeight="1">
       <c r="A226" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B226" s="2" t="inlineStr">
@@ -17950,7 +17950,7 @@
     <row r="227" ht="130" customHeight="1">
       <c r="A227" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B227" s="2" t="inlineStr">
@@ -18035,7 +18035,7 @@
     <row r="228" ht="130" customHeight="1">
       <c r="A228" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B228" s="2" t="inlineStr">
@@ -18355,7 +18355,7 @@
     <row r="232" ht="130" customHeight="1">
       <c r="A232" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),MA-4 (6)</t>
+          <t>MA-4 (6),AC-17 (2)</t>
         </is>
       </c>
       <c r="B232" s="2" t="inlineStr">
@@ -19027,7 +19027,7 @@
     <row r="241" ht="130" customHeight="1">
       <c r="A241" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B241" s="2" t="inlineStr">
@@ -19098,7 +19098,7 @@
     <row r="242" ht="130" customHeight="1">
       <c r="A242" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B242" s="2" t="inlineStr">
@@ -19260,7 +19260,7 @@
     <row r="244" ht="130" customHeight="1">
       <c r="A244" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-6 b,SC-2</t>
+          <t>SC-2,SI-16,CM-6 b</t>
         </is>
       </c>
       <c r="B244" s="2" t="inlineStr">
@@ -19420,7 +19420,7 @@
     <row r="246" ht="130" customHeight="1">
       <c r="A246" s="2" t="inlineStr">
         <is>
-          <t>SC-3,SI-16</t>
+          <t>SI-16,SC-3</t>
         </is>
       </c>
       <c r="B246" s="2" t="inlineStr">
@@ -20732,7 +20732,7 @@
     <row r="263" ht="130" customHeight="1">
       <c r="A263" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 (1)</t>
+          <t>AU-5 (1),AU-5 a</t>
         </is>
       </c>
       <c r="B263" s="2" t="inlineStr">
@@ -21259,7 +21259,7 @@
     <row r="270" ht="130" customHeight="1">
       <c r="A270" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (1),IA-2 (4),IA-2 (3)</t>
+          <t>IA-2 (1),IA-2 (2),IA-2 (3),IA-2 (4)</t>
         </is>
       </c>
       <c r="B270" s="2" t="inlineStr">
@@ -21428,7 +21428,7 @@
     <row r="272" ht="130" customHeight="1">
       <c r="A272" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B272" s="2" t="inlineStr">
@@ -21646,7 +21646,7 @@
     <row r="275" ht="130" customHeight="1">
       <c r="A275" s="2" t="inlineStr">
         <is>
-          <t>SC-4,CM-6 b</t>
+          <t>CM-6 b,SC-4</t>
         </is>
       </c>
       <c r="B275" s="2" t="inlineStr">
@@ -21727,7 +21727,7 @@
     <row r="276" ht="130" customHeight="1">
       <c r="A276" s="2" t="inlineStr">
         <is>
-          <t>SC-4,SC-2</t>
+          <t>SC-2,SC-4</t>
         </is>
       </c>
       <c r="B276" s="2" t="inlineStr">
@@ -21815,7 +21815,7 @@
     <row r="277" ht="130" customHeight="1">
       <c r="A277" s="2" t="inlineStr">
         <is>
-          <t>SC-4,SC-2</t>
+          <t>SC-2,SC-4</t>
         </is>
       </c>
       <c r="B277" s="2" t="inlineStr">
@@ -22053,7 +22053,7 @@
     <row r="280" ht="130" customHeight="1">
       <c r="A280" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-12 a</t>
+          <t>AU-12 a,CM-6 b</t>
         </is>
       </c>
       <c r="B280" s="2" t="inlineStr">
@@ -22276,7 +22276,7 @@
     <row r="283" ht="130" customHeight="1">
       <c r="A283" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (3),CM-6 b</t>
+          <t>CM-6 b,CM-5 (3)</t>
         </is>
       </c>
       <c r="B283" s="2" t="inlineStr">
@@ -24367,7 +24367,7 @@
     <row r="309" ht="130" customHeight="1">
       <c r="A309" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (b),AU-8 (1) (a),AU-8 b</t>
+          <t>AU-8 (1) (a),AU-8 (1) (b),AU-8 b</t>
         </is>
       </c>
       <c r="B309" s="2" t="inlineStr">
@@ -25320,7 +25320,7 @@
     <row r="321" ht="130" customHeight="1">
       <c r="A321" s="2" t="inlineStr">
         <is>
-          <t>IA-11,AC-3 (4)</t>
+          <t>AC-3 (4),IA-11</t>
         </is>
       </c>
       <c r="B321" s="2" t="inlineStr">
@@ -25941,7 +25941,7 @@
     <row r="329" ht="130" customHeight="1">
       <c r="A329" s="2" t="inlineStr">
         <is>
-          <t>AU-5 b,AU-5 a</t>
+          <t>AU-5 a,AU-5 b</t>
         </is>
       </c>
       <c r="B329" s="2" t="inlineStr">
@@ -26935,7 +26935,7 @@
     <row r="342" ht="130" customHeight="1">
       <c r="A342" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-7 a</t>
+          <t>CM-7 a,CM-7 b</t>
         </is>
       </c>
       <c r="B342" s="2" t="inlineStr">
@@ -27009,7 +27009,7 @@
     <row r="343" ht="130" customHeight="1">
       <c r="A343" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-7 a</t>
+          <t>CM-7 a,CM-7 b</t>
         </is>
       </c>
       <c r="B343" s="2" t="inlineStr">
@@ -27246,7 +27246,7 @@
     <row r="346" ht="130" customHeight="1">
       <c r="A346" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (c),CM-7 a</t>
+          <t>CM-7 a,CM-6 b,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B346" s="2" t="inlineStr">
@@ -28340,7 +28340,7 @@
     <row r="360" ht="130" customHeight="1">
       <c r="A360" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 d,SI-6 b</t>
+          <t>SI-6 d,CM-3 (5),SI-6 b</t>
         </is>
       </c>
       <c r="B360" s="2" t="inlineStr">
@@ -28431,7 +28431,7 @@
     <row r="361" ht="130" customHeight="1">
       <c r="A361" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B361" s="2" t="inlineStr">
@@ -28811,7 +28811,7 @@
     <row r="366" ht="130" customHeight="1">
       <c r="A366" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-7 a</t>
+          <t>CM-7 a,SI-16</t>
         </is>
       </c>
       <c r="B366" s="2" t="inlineStr">
@@ -29351,7 +29351,7 @@
     <row r="373" ht="130" customHeight="1">
       <c r="A373" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B373" s="2" t="inlineStr">
@@ -29422,7 +29422,7 @@
     <row r="374" ht="130" customHeight="1">
       <c r="A374" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B374" s="2" t="inlineStr">
@@ -29494,7 +29494,7 @@
     <row r="375" ht="130" customHeight="1">
       <c r="A375" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B375" s="2" t="inlineStr">
@@ -30254,7 +30254,7 @@
     <row r="384" ht="130" customHeight="1">
       <c r="A384" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),CM-6 b</t>
+          <t>CM-6 b,AC-17 (2)</t>
         </is>
       </c>
       <c r="B384" s="2" t="inlineStr">
@@ -35104,7 +35104,7 @@
     <row r="447" ht="130" customHeight="1">
       <c r="A447" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B447" s="2" t="inlineStr">
@@ -41138,7 +41138,7 @@
     <row r="523" ht="130" customHeight="1">
       <c r="A523" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-2</t>
+          <t>SC-2,CM-6 b</t>
         </is>
       </c>
       <c r="B523" s="2" t="inlineStr">
@@ -41225,7 +41225,7 @@
     <row r="524" ht="130" customHeight="1">
       <c r="A524" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-2</t>
+          <t>SC-2,CM-6 b</t>
         </is>
       </c>
       <c r="B524" s="2" t="inlineStr">
@@ -42457,7 +42457,7 @@
     <row r="540" ht="130" customHeight="1">
       <c r="A540" s="2" t="inlineStr">
         <is>
-          <t>SI-2 (2),CM-6 b</t>
+          <t>CM-6 b,SI-2 (2)</t>
         </is>
       </c>
       <c r="B540" s="2" t="inlineStr">
@@ -43104,7 +43104,7 @@
     <row r="549" ht="130" customHeight="1">
       <c r="A549" s="2" t="inlineStr">
         <is>
-          <t>SI-2 (2),CM-6 b</t>
+          <t>CM-6 b,SI-2 (2)</t>
         </is>
       </c>
       <c r="B549" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@650c1d99b8f637f5bb3cc79d4c2db8650c75bb46 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -625,7 +625,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-14 (1)</t>
+          <t>AU-14 (1),AU-4</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -784,7 +784,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>SC-5,SC-5 (2),CM-6 b</t>
+          <t>SC-5 (2),CM-6 b,SC-5</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -883,7 +883,7 @@
     <row r="6" ht="130" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>AU-7 a,AC-6 (9),AU-7 b,CM-5 (1),AU-12 (3),AC-6 (8),AU-8 b</t>
+          <t>AU-7 b,AC-6 (9),AU-7 a,AC-6 (8),CM-5 (1),AU-12 (3),AU-8 b</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -963,7 +963,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-7 a,CM-6 b,AU-7 b,AU-12 c,CM-5 (1),AU-12 (3),AU-12 a,AU-8 b</t>
+          <t>AU-7 b,AU-7 a,CM-5 (1),AU-12 (3),AU-8 b,AU-12 a,CM-6 b,AU-12 c</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1037,7 +1037,7 @@
     <row r="8" ht="130" customHeight="1">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (9),CM-7 b,AC-17 (1),CM-6 b</t>
+          <t>CM-6 b,CM-7 b,AC-17 (1),AC-17 (9)</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
@@ -1231,7 +1231,12 @@
 When operating systems provide the capability to change device authenticators, it is critical the device re-authenticate.</t>
         </is>
       </c>
-      <c r="H10" s="2" t="inlineStr"/>
+      <c r="H10" s="2" t="inlineStr">
+        <is>
+          <t>Without re-authentication, devices may access resources or perform tasks for which they do not have authorization. 
+When Red Hat Enterprise Linux 9 provide the capability to change device authenticators, it is critical the device re-authenticate.</t>
+        </is>
+      </c>
       <c r="I10" s="2" t="inlineStr">
         <is>
           <t>Applicable - Configurable</t>
@@ -1242,7 +1247,11 @@
           <t>Verify the operating system requires devices to re-authenticate when changing authenticators. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K10" s="2" t="n"/>
+      <c r="K10" s="2" t="inlineStr">
+        <is>
+          <t>This requirement is NA for Red Hat Enterprise Linux 9.</t>
+        </is>
+      </c>
       <c r="L10" s="2" t="n"/>
       <c r="M10" s="2" t="n"/>
       <c r="N10" s="2" t="inlineStr">
@@ -1252,7 +1261,11 @@
       </c>
       <c r="O10" s="2" t="n"/>
       <c r="P10" s="2" t="n"/>
-      <c r="Q10" s="2" t="n"/>
+      <c r="Q10" s="2" t="inlineStr">
+        <is>
+          <t>Devices are not assigned authenticators in Red Hat Enterprise Linux 9.</t>
+        </is>
+      </c>
     </row>
     <row r="11" ht="130" customHeight="1">
       <c r="A11" s="2" t="inlineStr">
@@ -1484,7 +1497,7 @@
     <row r="14" ht="130" customHeight="1">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -1560,7 +1573,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1714,7 +1727,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -2084,7 +2097,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -2158,7 +2171,7 @@
     <row r="23" ht="130" customHeight="1">
       <c r="A23" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B23" s="2" t="inlineStr">
@@ -3832,7 +3845,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),IA-2,IA-8</t>
+          <t>IA-2,AU-3 (1),IA-8</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3910,7 +3923,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -3985,7 +3998,7 @@
     <row r="47" ht="130" customHeight="1">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
@@ -4060,7 +4073,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4135,7 +4148,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4210,7 +4223,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4285,7 +4298,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4360,7 +4373,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
@@ -4435,7 +4448,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4510,7 +4523,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4585,7 +4598,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4660,7 +4673,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4735,7 +4748,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4810,7 +4823,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4885,7 +4898,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -4965,7 +4978,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5048,7 +5061,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5128,7 +5141,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5208,7 +5221,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5288,7 +5301,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5368,7 +5381,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5442,7 +5455,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5516,7 +5529,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5590,7 +5603,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5664,7 +5677,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5738,7 +5751,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5811,7 +5824,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5884,7 +5897,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -5957,7 +5970,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6030,7 +6043,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6103,7 +6116,7 @@
     <row r="75" ht="130" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
@@ -6176,7 +6189,7 @@
     <row r="76" ht="130" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
@@ -6250,7 +6263,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6324,7 +6337,7 @@
     <row r="78" ht="130" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
@@ -6398,7 +6411,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6469,7 +6482,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6549,7 +6562,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6629,7 +6642,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B82" s="2" t="inlineStr">
@@ -6709,7 +6722,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B83" s="2" t="inlineStr">
@@ -6789,7 +6802,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B84" s="2" t="inlineStr">
@@ -6869,7 +6882,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B85" s="2" t="inlineStr">
@@ -6949,7 +6962,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -7029,7 +7042,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7109,7 +7122,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7189,7 +7202,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7269,7 +7282,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7349,7 +7362,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7425,7 +7438,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
@@ -7502,7 +7515,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
@@ -7582,7 +7595,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B94" s="2" t="inlineStr">
@@ -7662,7 +7675,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
@@ -7742,7 +7755,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7822,7 +7835,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7902,7 +7915,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -7982,7 +7995,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8062,7 +8075,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8142,7 +8155,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8222,7 +8235,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8295,7 +8308,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AC-2 (4),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8376,7 +8389,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AC-2 (4),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8457,7 +8470,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AC-2 (4),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8528,7 +8541,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-3</t>
+          <t>MA-4 (1) (a),AC-2 (4),AU-3,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8603,7 +8616,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AC-2 (4),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8685,7 +8698,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AC-2 (4),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -8767,7 +8780,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AC-2 (4),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -8849,7 +8862,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AC-2 (4),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B110" s="2" t="inlineStr">
@@ -8931,7 +8944,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AC-2 (4),AU-3,AU-12 a,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9013,7 +9026,7 @@
     <row r="112" ht="130" customHeight="1">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-14 (1),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
@@ -9096,7 +9109,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9177,7 +9190,7 @@
     <row r="114" ht="130" customHeight="1">
       <c r="A114" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B114" s="2" t="inlineStr">
@@ -9263,7 +9276,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-6 (10)</t>
+          <t>AC-6 (10),AC-11 b</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9341,7 +9354,7 @@
     <row r="116" ht="130" customHeight="1">
       <c r="A116" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B116" s="2" t="inlineStr">
@@ -9707,7 +9720,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 a,AU-3,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -9778,7 +9791,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 a,AU-3,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -9849,7 +9862,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-9</t>
+          <t>AU-9,AU-12 c</t>
         </is>
       </c>
       <c r="B122" s="2" t="inlineStr">
@@ -10222,7 +10235,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AC-6 (9),AU-12 c,AC-2 (4)</t>
+          <t>AU-12 c,AC-6 (9),AC-2 (4),CM-5 (1)</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -10345,7 +10358,7 @@
     <row r="129" ht="130" customHeight="1">
       <c r="A129" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (a),IA-5 (1) (b)</t>
+          <t>IA-5 (1) (b),IA-5 (1) (a),CM-6 b</t>
         </is>
       </c>
       <c r="B129" s="2" t="inlineStr">
@@ -10665,7 +10678,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>SC-8,MA-4 c,AC-17 (2),SC-13</t>
+          <t>SC-13,SC-8,AC-17 (2),MA-4 c</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10747,7 +10760,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>MA-4 e,MA-4 (7),AC-12,SC-10</t>
+          <t>SC-10,AC-12,MA-4 (7),MA-4 e</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -10822,7 +10835,7 @@
     <row r="135" ht="130" customHeight="1">
       <c r="A135" s="2" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B135" s="2" t="inlineStr">
@@ -10901,7 +10914,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -10977,7 +10990,7 @@
     <row r="137" ht="130" customHeight="1">
       <c r="A137" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,SC-10</t>
+          <t>SC-10,AC-11 a</t>
         </is>
       </c>
       <c r="B137" s="2" t="inlineStr">
@@ -11054,7 +11067,7 @@
     <row r="138" ht="130" customHeight="1">
       <c r="A138" s="2" t="inlineStr">
         <is>
-          <t>AU-7 a,AU-6 (4),AU-14 (1),CM-6 b,AU-3 (1),CM-5 (1),AU-7 (1),MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-7 a,AU-7 (1),CM-5 (1),AU-6 (4),AU-3,AU-12 a,AU-14 (1),CM-6 b,AU-3 (1)</t>
         </is>
       </c>
       <c r="B138" s="2" t="inlineStr">
@@ -14122,7 +14135,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-6 (4),CM-6 b</t>
+          <t>AU-6 (4),CM-6 b,AU-4 (1)</t>
         </is>
       </c>
       <c r="B179" s="2" t="inlineStr">
@@ -14193,7 +14206,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (1),CM-6 b</t>
+          <t>CM-6 b,CM-7 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B180" s="2" t="inlineStr">
@@ -14272,7 +14285,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">
@@ -14344,7 +14357,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B182" s="2" t="inlineStr">
@@ -14416,7 +14429,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B183" s="2" t="inlineStr">
@@ -14490,7 +14503,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B184" s="2" t="inlineStr">
@@ -14564,7 +14577,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B185" s="2" t="inlineStr">
@@ -14638,7 +14651,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B186" s="2" t="inlineStr">
@@ -15159,7 +15172,7 @@
     <row r="193" ht="130" customHeight="1">
       <c r="A193" s="2" t="inlineStr">
         <is>
-          <t>AU-3,CM-6 b</t>
+          <t>CM-6 b,AU-3</t>
         </is>
       </c>
       <c r="B193" s="2" t="inlineStr">
@@ -15593,7 +15606,7 @@
     <row r="199" ht="130" customHeight="1">
       <c r="A199" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-3</t>
+          <t>AU-3,AU-4 (1)</t>
         </is>
       </c>
       <c r="B199" s="2" t="inlineStr">
@@ -16108,7 +16121,7 @@
     <row r="206" ht="130" customHeight="1">
       <c r="A206" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),CM-6 b</t>
+          <t>CM-6 b,AU-4 (1)</t>
         </is>
       </c>
       <c r="B206" s="2" t="inlineStr">
@@ -16188,7 +16201,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>SC-28,SC-28 (1)</t>
+          <t>SC-28 (1),SC-28</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -16934,7 +16947,7 @@
     <row r="215" ht="130" customHeight="1">
       <c r="A215" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (9),AU-12 c,AC-2 (4)</t>
+          <t>AU-12 c,AC-6 (9),AC-2 (4)</t>
         </is>
       </c>
       <c r="B215" s="2" t="inlineStr">
@@ -17376,7 +17389,7 @@
     <row r="220" ht="130" customHeight="1">
       <c r="A220" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),CM-6 b</t>
+          <t>CM-6 b,IA-2 (5)</t>
         </is>
       </c>
       <c r="B220" s="2" t="inlineStr">
@@ -17454,7 +17467,7 @@
     <row r="221" ht="130" customHeight="1">
       <c r="A221" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (5),IA-2 (2),IA-2,IA-2 (4)</t>
+          <t>IA-2 (2),IA-2 (4),IA-2,IA-2 (3),IA-2 (5)</t>
         </is>
       </c>
       <c r="B221" s="2" t="inlineStr">
@@ -17539,7 +17552,7 @@
     <row r="222" ht="130" customHeight="1">
       <c r="A222" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (5),IA-2 (2),IA-2,IA-2 (4)</t>
+          <t>IA-2 (2),IA-2 (4),IA-2,IA-2 (3),IA-2 (5)</t>
         </is>
       </c>
       <c r="B222" s="2" t="inlineStr">
@@ -17624,7 +17637,7 @@
     <row r="223" ht="130" customHeight="1">
       <c r="A223" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (1),AC-18 (1)</t>
+          <t>SC-8 (1),SC-8,AC-18 (1)</t>
         </is>
       </c>
       <c r="B223" s="2" t="inlineStr">
@@ -17791,7 +17804,7 @@
     <row r="225" ht="130" customHeight="1">
       <c r="A225" s="2" t="inlineStr">
         <is>
-          <t>IA-7,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),IA-7</t>
         </is>
       </c>
       <c r="B225" s="2" t="inlineStr">
@@ -17874,7 +17887,7 @@
     <row r="226" ht="130" customHeight="1">
       <c r="A226" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B226" s="2" t="inlineStr">
@@ -17950,7 +17963,7 @@
     <row r="227" ht="130" customHeight="1">
       <c r="A227" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B227" s="2" t="inlineStr">
@@ -18035,7 +18048,7 @@
     <row r="228" ht="130" customHeight="1">
       <c r="A228" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B228" s="2" t="inlineStr">
@@ -18192,7 +18205,7 @@
     <row r="230" ht="130" customHeight="1">
       <c r="A230" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,IA-7</t>
+          <t>IA-7,CM-7 a</t>
         </is>
       </c>
       <c r="B230" s="2" t="inlineStr">
@@ -18271,7 +18284,7 @@
     <row r="231" ht="130" customHeight="1">
       <c r="A231" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B231" s="2" t="inlineStr">
@@ -18355,7 +18368,7 @@
     <row r="232" ht="130" customHeight="1">
       <c r="A232" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),AC-17 (2)</t>
+          <t>AC-17 (2),MA-4 (6)</t>
         </is>
       </c>
       <c r="B232" s="2" t="inlineStr">
@@ -18430,7 +18443,7 @@
     <row r="233" ht="130" customHeight="1">
       <c r="A233" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B233" s="2" t="inlineStr">
@@ -19260,7 +19273,7 @@
     <row r="244" ht="130" customHeight="1">
       <c r="A244" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SI-16,CM-6 b</t>
+          <t>SC-2,CM-6 b,SI-16</t>
         </is>
       </c>
       <c r="B244" s="2" t="inlineStr">
@@ -20334,7 +20347,7 @@
     <row r="258" ht="130" customHeight="1">
       <c r="A258" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B258" s="2" t="inlineStr">
@@ -20409,7 +20422,7 @@
     <row r="259" ht="130" customHeight="1">
       <c r="A259" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B259" s="2" t="inlineStr">
@@ -20497,7 +20510,7 @@
     <row r="260" ht="130" customHeight="1">
       <c r="A260" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B260" s="2" t="inlineStr">
@@ -20574,7 +20587,7 @@
     <row r="261" ht="130" customHeight="1">
       <c r="A261" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B261" s="2" t="inlineStr">
@@ -21172,7 +21185,7 @@
     <row r="269" ht="130" customHeight="1">
       <c r="A269" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),CM-6 b</t>
+          <t>CM-6 b,IA-2 (2)</t>
         </is>
       </c>
       <c r="B269" s="2" t="inlineStr">
@@ -21259,7 +21272,7 @@
     <row r="270" ht="130" customHeight="1">
       <c r="A270" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (2),IA-2 (3),IA-2 (4)</t>
+          <t>IA-2 (3),IA-2 (2),IA-2 (4),IA-2 (1)</t>
         </is>
       </c>
       <c r="B270" s="2" t="inlineStr">
@@ -22053,7 +22066,7 @@
     <row r="280" ht="130" customHeight="1">
       <c r="A280" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,CM-6 b</t>
+          <t>CM-6 b,AU-12 a</t>
         </is>
       </c>
       <c r="B280" s="2" t="inlineStr">
@@ -22276,7 +22289,7 @@
     <row r="283" ht="130" customHeight="1">
       <c r="A283" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (3)</t>
+          <t>CM-5 (3),CM-6 b</t>
         </is>
       </c>
       <c r="B283" s="2" t="inlineStr">
@@ -23456,7 +23469,7 @@
     <row r="298" ht="130" customHeight="1">
       <c r="A298" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (1)</t>
         </is>
       </c>
       <c r="B298" s="2" t="inlineStr">
@@ -23545,7 +23558,7 @@
     <row r="299" ht="130" customHeight="1">
       <c r="A299" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (11),IA-2 (1),IA-2 (12)</t>
         </is>
       </c>
       <c r="B299" s="2" t="inlineStr">
@@ -24367,7 +24380,7 @@
     <row r="309" ht="130" customHeight="1">
       <c r="A309" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (a),AU-8 (1) (b),AU-8 b</t>
+          <t>AU-8 (1) (a),AU-8 b,AU-8 (1) (b)</t>
         </is>
       </c>
       <c r="B309" s="2" t="inlineStr">
@@ -25784,7 +25797,7 @@
     <row r="327" ht="130" customHeight="1">
       <c r="A327" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AU-12 c</t>
+          <t>AU-12 c,CM-5 (1)</t>
         </is>
       </c>
       <c r="B327" s="2" t="inlineStr">
@@ -26935,7 +26948,7 @@
     <row r="342" ht="130" customHeight="1">
       <c r="A342" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-7 b</t>
+          <t>CM-7 b,CM-7 a</t>
         </is>
       </c>
       <c r="B342" s="2" t="inlineStr">
@@ -27009,7 +27022,7 @@
     <row r="343" ht="130" customHeight="1">
       <c r="A343" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-7 b</t>
+          <t>CM-7 b,CM-7 a</t>
         </is>
       </c>
       <c r="B343" s="2" t="inlineStr">
@@ -27246,7 +27259,7 @@
     <row r="346" ht="130" customHeight="1">
       <c r="A346" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B346" s="2" t="inlineStr">
@@ -28340,7 +28353,7 @@
     <row r="360" ht="130" customHeight="1">
       <c r="A360" s="2" t="inlineStr">
         <is>
-          <t>SI-6 d,CM-3 (5),SI-6 b</t>
+          <t>CM-3 (5),SI-6 d,SI-6 b</t>
         </is>
       </c>
       <c r="B360" s="2" t="inlineStr">
@@ -28431,7 +28444,7 @@
     <row r="361" ht="130" customHeight="1">
       <c r="A361" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B361" s="2" t="inlineStr">
@@ -28811,7 +28824,7 @@
     <row r="366" ht="130" customHeight="1">
       <c r="A366" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,SI-16</t>
+          <t>SI-16,CM-7 a</t>
         </is>
       </c>
       <c r="B366" s="2" t="inlineStr">
@@ -29351,7 +29364,7 @@
     <row r="373" ht="130" customHeight="1">
       <c r="A373" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B373" s="2" t="inlineStr">
@@ -29422,7 +29435,7 @@
     <row r="374" ht="130" customHeight="1">
       <c r="A374" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B374" s="2" t="inlineStr">
@@ -29494,7 +29507,7 @@
     <row r="375" ht="130" customHeight="1">
       <c r="A375" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B375" s="2" t="inlineStr">
@@ -31268,7 +31281,7 @@
     <row r="397" ht="130" customHeight="1">
       <c r="A397" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-6 b</t>
+          <t>CM-6 b,SI-16</t>
         </is>
       </c>
       <c r="B397" s="2" t="inlineStr">
@@ -31509,7 +31522,7 @@
     <row r="400" ht="130" customHeight="1">
       <c r="A400" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B400" s="2" t="inlineStr">
@@ -31600,7 +31613,7 @@
     <row r="401" ht="130" customHeight="1">
       <c r="A401" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B401" s="2" t="inlineStr">
@@ -31694,7 +31707,7 @@
     <row r="402" ht="130" customHeight="1">
       <c r="A402" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B402" s="2" t="inlineStr">
@@ -35104,7 +35117,7 @@
     <row r="447" ht="130" customHeight="1">
       <c r="A447" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),CM-6 b</t>
         </is>
       </c>
       <c r="B447" s="2" t="inlineStr">
@@ -35254,7 +35267,7 @@
     <row r="449" ht="130" customHeight="1">
       <c r="A449" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),CM-6 b</t>
+          <t>CM-6 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B449" s="2" t="inlineStr">
@@ -35327,7 +35340,7 @@
     <row r="450" ht="130" customHeight="1">
       <c r="A450" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),CM-6 b</t>
+          <t>CM-6 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B450" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@5283c0baed996e97326890b8fc55822a76bbd8ce 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -625,7 +625,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-14 (1)</t>
+          <t>AU-14 (1),AU-4</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -708,7 +708,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>AU-4,CM-6 b</t>
+          <t>CM-6 b,AU-4</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -784,7 +784,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>SC-5 (2),SC-5,CM-6 b</t>
+          <t>SC-5,CM-6 b,SC-5 (2)</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -883,7 +883,7 @@
     <row r="6" ht="130" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (9),AU-7 b,AU-12 (3),AU-7 a,AU-8 b,AC-6 (8),CM-5 (1)</t>
+          <t>AC-6 (9),AU-8 b,AU-7 a,AU-12 (3),CM-5 (1),AC-6 (8),AU-7 b</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -893,7 +893,7 @@
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>SRG-OS-000326-GPOS-00126,SRG-OS-000327-GPOS-00127,SRG-OS-000337-GPOS-00129,SRG-OS-000348-GPOS-00136,SRG-OS-000349-GPOS-00137,SRG-OS-000350-GPOS-00138,SRG-OS-000351-GPOS-00139,SRG-OS-000352-GPOS-00140,SRG-OS-000353-GPOS-00141,SRG-OS-000354-GPOS-00142,SRG-OS-000358-GPOS-00145,SRG-OS-000359-GPOS-00146,SRG-OS-000365-GPOS-00152</t>
+          <t>SRG-OS-000326-GPOS-00126,SRG-OS-000327-GPOS-00127,SRG-OS-000337-GPOS-00129,SRG-OS-000348-GPOS-00136,SRG-OS-000349-GPOS-00137,SRG-OS-000350-GPOS-00138,SRG-OS-000351-GPOS-00139,SRG-OS-000352-GPOS-00140,SRG-OS-000353-GPOS-00141,SRG-OS-000354-GPOS-00142,SRG-OS-000358-GPOS-00145,SRG-OS-000365-GPOS-00152</t>
         </is>
       </c>
       <c r="D6" s="2" t="inlineStr">
@@ -963,7 +963,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-7 a,AU-7 b,AU-12 (3),AU-8 b,AU-12 c,CM-6 b,CM-5 (1)</t>
+          <t>AU-12 c,AU-8 b,AU-12 (3),AU-7 a,CM-5 (1),CM-6 b,AU-12 a,AU-7 b</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1015,7 +1015,7 @@
       <c r="K7" s="2" t="inlineStr">
         <is>
           <t>Run the following command to determine if the  audit  package is installed:  $ rpm -q audit 
-If the package is not installed then this is a finding.</t>
+If the audit package is not installed then this is a finding.</t>
         </is>
       </c>
       <c r="L7" s="2" t="n"/>
@@ -1269,7 +1269,7 @@
     <row r="11" ht="130" customHeight="1">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B11" s="2" t="inlineStr">
@@ -1346,7 +1346,7 @@
     <row r="12" ht="130" customHeight="1">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
@@ -3298,7 +3298,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3382,7 +3382,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3467,7 +3467,7 @@
     <row r="40" ht="130" customHeight="1">
       <c r="A40" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B40" s="2" t="inlineStr">
@@ -3539,7 +3539,7 @@
     <row r="41" ht="130" customHeight="1">
       <c r="A41" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B41" s="2" t="inlineStr">
@@ -3844,7 +3844,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>IA-8,IA-2,AU-3 (1)</t>
+          <t>AU-3 (1),IA-8,IA-2</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3922,7 +3922,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -3997,7 +3997,7 @@
     <row r="47" ht="130" customHeight="1">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
@@ -4072,7 +4072,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4147,7 +4147,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4222,7 +4222,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4297,7 +4297,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4372,7 +4372,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
@@ -4447,7 +4447,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4522,7 +4522,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4597,7 +4597,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4672,7 +4672,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4747,7 +4747,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4822,7 +4822,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4897,7 +4897,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -4977,7 +4977,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5060,7 +5060,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5140,7 +5140,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5220,7 +5220,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5300,7 +5300,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5380,7 +5380,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5454,7 +5454,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5528,7 +5528,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5602,7 +5602,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5676,7 +5676,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5750,7 +5750,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5823,7 +5823,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5896,7 +5896,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -5969,7 +5969,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6042,7 +6042,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6115,7 +6115,7 @@
     <row r="75" ht="130" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
@@ -6188,7 +6188,7 @@
     <row r="76" ht="130" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
@@ -6262,7 +6262,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6336,7 +6336,7 @@
     <row r="78" ht="130" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
@@ -6410,7 +6410,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6481,7 +6481,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6561,7 +6561,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6641,7 +6641,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B82" s="2" t="inlineStr">
@@ -6721,7 +6721,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B83" s="2" t="inlineStr">
@@ -6801,7 +6801,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B84" s="2" t="inlineStr">
@@ -6881,7 +6881,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B85" s="2" t="inlineStr">
@@ -6961,7 +6961,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -7041,7 +7041,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7121,7 +7121,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7201,7 +7201,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7281,7 +7281,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7361,7 +7361,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7437,7 +7437,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
@@ -7514,7 +7514,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
@@ -7594,7 +7594,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B94" s="2" t="inlineStr">
@@ -7674,7 +7674,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
@@ -7754,7 +7754,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7834,7 +7834,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7914,7 +7914,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -7994,7 +7994,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8074,7 +8074,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8154,7 +8154,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8234,7 +8234,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8307,7 +8307,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c,AC-2 (4)</t>
+          <t>AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8388,7 +8388,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c,AC-2 (4)</t>
+          <t>AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8469,7 +8469,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c,AC-2 (4)</t>
+          <t>AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8540,7 +8540,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c,AC-2 (4)</t>
+          <t>AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8615,7 +8615,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c,AC-2 (4)</t>
+          <t>AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8697,7 +8697,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c,AC-2 (4)</t>
+          <t>AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -8779,7 +8779,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c,AC-2 (4)</t>
+          <t>AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -8861,7 +8861,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c,AC-2 (4)</t>
+          <t>AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B110" s="2" t="inlineStr">
@@ -8943,7 +8943,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-12 c,AC-2 (4)</t>
+          <t>AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9025,7 +9025,7 @@
     <row r="112" ht="130" customHeight="1">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-14 (1),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-14 (1),AU-3 (1),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
@@ -9108,7 +9108,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9189,7 +9189,7 @@
     <row r="114" ht="130" customHeight="1">
       <c r="A114" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B114" s="2" t="inlineStr">
@@ -9353,7 +9353,7 @@
     <row r="116" ht="130" customHeight="1">
       <c r="A116" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B116" s="2" t="inlineStr">
@@ -9719,7 +9719,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -9790,7 +9790,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -9861,7 +9861,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-12 c</t>
+          <t>AU-12 c,AU-9</t>
         </is>
       </c>
       <c r="B122" s="2" t="inlineStr">
@@ -10234,7 +10234,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (9),AU-12 c,AC-2 (4),CM-5 (1)</t>
+          <t>CM-5 (1),AU-12 c,AC-6 (9),AC-2 (4)</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -10357,7 +10357,7 @@
     <row r="129" ht="130" customHeight="1">
       <c r="A129" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (b),IA-5 (1) (a),CM-6 b</t>
+          <t>IA-5 (1) (b),CM-6 b,IA-5 (1) (a)</t>
         </is>
       </c>
       <c r="B129" s="2" t="inlineStr">
@@ -10677,7 +10677,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-13,SC-8,MA-4 c</t>
+          <t>AC-17 (2),SC-13,MA-4 c,SC-8</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10759,7 +10759,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (7),AC-12,MA-4 e,SC-10</t>
+          <t>AC-12,MA-4 e,MA-4 (7),SC-10</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -10834,7 +10834,7 @@
     <row r="135" ht="130" customHeight="1">
       <c r="A135" s="2" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B135" s="2" t="inlineStr">
@@ -10913,7 +10913,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -11066,7 +11066,7 @@
     <row r="138" ht="130" customHeight="1">
       <c r="A138" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-6 (4),MA-4 (1) (a),AU-14 (1),AU-7 a,AU-7 (1),AU-3 (1),CM-6 b,CM-5 (1)</t>
+          <t>AU-7 a,AU-14 (1),MA-4 (1) (a),CM-5 (1),AU-7 (1),CM-6 b,AU-12 a,AU-3 (1),AU-6 (4),AU-3</t>
         </is>
       </c>
       <c r="B138" s="2" t="inlineStr">
@@ -13137,7 +13137,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8,SC-8 (2)</t>
+          <t>SC-8 (2),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B166" s="2" t="inlineStr">
@@ -13369,7 +13369,7 @@
     <row r="169" ht="130" customHeight="1">
       <c r="A169" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (2)</t>
+          <t>SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B169" s="2" t="inlineStr">
@@ -13593,7 +13593,7 @@
     <row r="172" ht="130" customHeight="1">
       <c r="A172" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B172" s="2" t="inlineStr">
@@ -13671,7 +13671,7 @@
     <row r="173" ht="130" customHeight="1">
       <c r="A173" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B173" s="2" t="inlineStr">
@@ -13754,7 +13754,7 @@
     <row r="174" ht="130" customHeight="1">
       <c r="A174" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B174" s="2" t="inlineStr">
@@ -14134,7 +14134,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-6 (4),CM-6 b</t>
+          <t>AU-6 (4),CM-6 b,AU-4 (1)</t>
         </is>
       </c>
       <c r="B179" s="2" t="inlineStr">
@@ -14205,7 +14205,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (9),AC-17 (1),CM-7 b,CM-6 b</t>
+          <t>AC-17 (9),AC-17 (1),CM-6 b,CM-7 b</t>
         </is>
       </c>
       <c r="B180" s="2" t="inlineStr">
@@ -14282,7 +14282,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),CM-7 b,CM-6 b</t>
+          <t>AC-17 (1),CM-6 b,CM-7 b</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">
@@ -15248,7 +15248,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="2" t="inlineStr">
         <is>
-          <t>AU-3,CM-6 b</t>
+          <t>CM-6 b,AU-3</t>
         </is>
       </c>
       <c r="B194" s="2" t="inlineStr">
@@ -16197,7 +16197,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),CM-6 b</t>
+          <t>CM-6 b,AU-4 (1)</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -16277,7 +16277,7 @@
     <row r="208" ht="130" customHeight="1">
       <c r="A208" s="2" t="inlineStr">
         <is>
-          <t>SC-28,SC-28 (1)</t>
+          <t>SC-28 (1),SC-28</t>
         </is>
       </c>
       <c r="B208" s="2" t="inlineStr">
@@ -17023,7 +17023,7 @@
     <row r="216" ht="130" customHeight="1">
       <c r="A216" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (9),AU-12 c,AC-2 (4)</t>
+          <t>AU-12 c,AC-6 (9),AC-2 (4)</t>
         </is>
       </c>
       <c r="B216" s="2" t="inlineStr">
@@ -17543,7 +17543,7 @@
     <row r="222" ht="130" customHeight="1">
       <c r="A222" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),IA-2,IA-2 (2),IA-2 (3),IA-2 (4)</t>
+          <t>IA-2 (2),IA-2 (4),IA-2 (3),IA-2 (5),IA-2</t>
         </is>
       </c>
       <c r="B222" s="2" t="inlineStr">
@@ -17628,7 +17628,7 @@
     <row r="223" ht="130" customHeight="1">
       <c r="A223" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),IA-2,IA-2 (2),IA-2 (3),IA-2 (4)</t>
+          <t>IA-2 (2),IA-2 (4),IA-2 (3),IA-2 (5),IA-2</t>
         </is>
       </c>
       <c r="B223" s="2" t="inlineStr">
@@ -17713,7 +17713,7 @@
     <row r="224" ht="130" customHeight="1">
       <c r="A224" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (1),AC-18 (1)</t>
+          <t>AC-18 (1),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B224" s="2" t="inlineStr">
@@ -18281,7 +18281,7 @@
     <row r="231" ht="130" customHeight="1">
       <c r="A231" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,IA-7</t>
+          <t>IA-7,CM-7 a</t>
         </is>
       </c>
       <c r="B231" s="2" t="inlineStr">
@@ -19116,7 +19116,7 @@
     <row r="242" ht="130" customHeight="1">
       <c r="A242" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B242" s="2" t="inlineStr">
@@ -19187,7 +19187,7 @@
     <row r="243" ht="130" customHeight="1">
       <c r="A243" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B243" s="2" t="inlineStr">
@@ -19349,7 +19349,7 @@
     <row r="245" ht="130" customHeight="1">
       <c r="A245" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SI-16,CM-6 b</t>
+          <t>SI-16,CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B245" s="2" t="inlineStr">
@@ -19509,7 +19509,7 @@
     <row r="247" ht="130" customHeight="1">
       <c r="A247" s="2" t="inlineStr">
         <is>
-          <t>SC-3,SI-16</t>
+          <t>SI-16,SC-3</t>
         </is>
       </c>
       <c r="B247" s="2" t="inlineStr">
@@ -20821,7 +20821,7 @@
     <row r="264" ht="130" customHeight="1">
       <c r="A264" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 (1)</t>
+          <t>AU-5 (1),AU-5 a</t>
         </is>
       </c>
       <c r="B264" s="2" t="inlineStr">
@@ -21348,7 +21348,7 @@
     <row r="271" ht="130" customHeight="1">
       <c r="A271" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (1),IA-2 (4),IA-2 (3)</t>
+          <t>IA-2 (3),IA-2 (2),IA-2 (4),IA-2 (1)</t>
         </is>
       </c>
       <c r="B271" s="2" t="inlineStr">
@@ -21517,7 +21517,7 @@
     <row r="273" ht="130" customHeight="1">
       <c r="A273" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B273" s="2" t="inlineStr">
@@ -21816,7 +21816,7 @@
     <row r="277" ht="130" customHeight="1">
       <c r="A277" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SC-4</t>
+          <t>SC-4,SC-2</t>
         </is>
       </c>
       <c r="B277" s="2" t="inlineStr">
@@ -21904,7 +21904,7 @@
     <row r="278" ht="130" customHeight="1">
       <c r="A278" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SC-4</t>
+          <t>SC-4,SC-2</t>
         </is>
       </c>
       <c r="B278" s="2" t="inlineStr">
@@ -22142,7 +22142,7 @@
     <row r="281" ht="130" customHeight="1">
       <c r="A281" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,CM-6 b</t>
+          <t>CM-6 b,AU-12 a</t>
         </is>
       </c>
       <c r="B281" s="2" t="inlineStr">
@@ -23465,7 +23465,7 @@
     <row r="298" ht="130" customHeight="1">
       <c r="A298" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B298" s="2" t="inlineStr">
@@ -23545,7 +23545,7 @@
     <row r="299" ht="130" customHeight="1">
       <c r="A299" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (1)</t>
         </is>
       </c>
       <c r="B299" s="2" t="inlineStr">
@@ -23634,7 +23634,7 @@
     <row r="300" ht="130" customHeight="1">
       <c r="A300" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (1),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12),IA-2 (1)</t>
         </is>
       </c>
       <c r="B300" s="2" t="inlineStr">
@@ -24456,7 +24456,7 @@
     <row r="310" ht="130" customHeight="1">
       <c r="A310" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-8 (1) (a),AU-8 (1) (b)</t>
+          <t>AU-8 (1) (a),AU-8 b,AU-8 (1) (b)</t>
         </is>
       </c>
       <c r="B310" s="2" t="inlineStr">
@@ -25873,7 +25873,7 @@
     <row r="328" ht="130" customHeight="1">
       <c r="A328" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,CM-5 (1)</t>
+          <t>CM-5 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B328" s="2" t="inlineStr">
@@ -27335,7 +27335,7 @@
     <row r="347" ht="130" customHeight="1">
       <c r="A347" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b,IA-5 (1) (c)</t>
+          <t>CM-6 b,IA-5 (1) (c),CM-7 a</t>
         </is>
       </c>
       <c r="B347" s="2" t="inlineStr">
@@ -28520,7 +28520,7 @@
     <row r="362" ht="130" customHeight="1">
       <c r="A362" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B362" s="2" t="inlineStr">
@@ -28900,7 +28900,7 @@
     <row r="367" ht="130" customHeight="1">
       <c r="A367" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,SI-16</t>
+          <t>SI-16,CM-7 a</t>
         </is>
       </c>
       <c r="B367" s="2" t="inlineStr">
@@ -29440,7 +29440,7 @@
     <row r="374" ht="130" customHeight="1">
       <c r="A374" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B374" s="2" t="inlineStr">
@@ -29511,7 +29511,7 @@
     <row r="375" ht="130" customHeight="1">
       <c r="A375" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B375" s="2" t="inlineStr">
@@ -29583,7 +29583,7 @@
     <row r="376" ht="130" customHeight="1">
       <c r="A376" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B376" s="2" t="inlineStr">
@@ -30652,7 +30652,7 @@
     <row r="389" ht="130" customHeight="1">
       <c r="A389" s="2" t="inlineStr">
         <is>
-          <t>SI-6 a,SC-3</t>
+          <t>SC-3,SI-6 a</t>
         </is>
       </c>
       <c r="B389" s="2" t="inlineStr">
@@ -30791,7 +30791,7 @@
     <row r="391" ht="130" customHeight="1">
       <c r="A391" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (a),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (a)</t>
         </is>
       </c>
       <c r="B391" s="2" t="inlineStr">
@@ -35343,7 +35343,7 @@
     <row r="450" ht="130" customHeight="1">
       <c r="A450" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (1)</t>
+          <t>CM-5 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B450" s="2" t="inlineStr">
@@ -35416,7 +35416,7 @@
     <row r="451" ht="130" customHeight="1">
       <c r="A451" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (1)</t>
+          <t>CM-5 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B451" s="2" t="inlineStr">
@@ -41227,7 +41227,7 @@
     <row r="524" ht="130" customHeight="1">
       <c r="A524" s="2" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b</t>
+          <t>CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B524" s="2" t="inlineStr">
@@ -41314,7 +41314,7 @@
     <row r="525" ht="130" customHeight="1">
       <c r="A525" s="2" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b</t>
+          <t>CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B525" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@9254d38f20190ee497263c3029308067ea3a0246 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -541,7 +541,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-4</t>
+          <t>AU-4,AU-4 (1)</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -625,7 +625,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),AU-4</t>
+          <t>AU-4,AU-14 (1)</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -784,7 +784,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>SC-5,CM-6 b,SC-5 (2)</t>
+          <t>CM-6 b,SC-5 (2),SC-5</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -883,7 +883,7 @@
     <row r="6" ht="130" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (9),AU-8 b,AU-7 a,AU-12 (3),CM-5 (1),AC-6 (8),AU-7 b</t>
+          <t>CM-5 (1),AC-6 (8),AU-7 b,AC-6 (9),AU-12 (3),AU-8 b,AU-7 a</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -963,7 +963,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-8 b,AU-12 (3),AU-7 a,CM-5 (1),CM-6 b,AU-12 a,AU-7 b</t>
+          <t>CM-5 (1),AU-7 b,AU-12 (3),AU-12 c,AU-8 b,AU-12 a,CM-6 b,AU-7 a</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1269,7 +1269,7 @@
     <row r="11" ht="130" customHeight="1">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B11" s="2" t="inlineStr">
@@ -1346,7 +1346,7 @@
     <row r="12" ht="130" customHeight="1">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
@@ -1496,7 +1496,7 @@
     <row r="14" ht="130" customHeight="1">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -1572,7 +1572,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1726,7 +1726,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -2096,7 +2096,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -2170,7 +2170,7 @@
     <row r="23" ht="130" customHeight="1">
       <c r="A23" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B23" s="2" t="inlineStr">
@@ -3298,7 +3298,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3382,7 +3382,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3467,7 +3467,7 @@
     <row r="40" ht="130" customHeight="1">
       <c r="A40" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B40" s="2" t="inlineStr">
@@ -3539,7 +3539,7 @@
     <row r="41" ht="130" customHeight="1">
       <c r="A41" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B41" s="2" t="inlineStr">
@@ -3844,7 +3844,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),IA-8,IA-2</t>
+          <t>IA-8,IA-2,AU-3 (1)</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3922,7 +3922,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -3997,7 +3997,7 @@
     <row r="47" ht="130" customHeight="1">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
@@ -4072,7 +4072,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4147,7 +4147,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4222,7 +4222,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4297,7 +4297,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4372,7 +4372,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
@@ -4447,7 +4447,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4522,7 +4522,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4597,7 +4597,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4672,7 +4672,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4747,7 +4747,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4822,7 +4822,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4897,7 +4897,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -4977,7 +4977,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5060,7 +5060,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5140,7 +5140,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5220,7 +5220,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5300,7 +5300,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5380,7 +5380,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5454,7 +5454,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5528,7 +5528,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5602,7 +5602,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5676,7 +5676,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5750,7 +5750,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5823,7 +5823,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5896,7 +5896,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -5969,7 +5969,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6042,7 +6042,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6115,7 +6115,7 @@
     <row r="75" ht="130" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
@@ -6188,7 +6188,7 @@
     <row r="76" ht="130" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
@@ -6262,7 +6262,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6336,7 +6336,7 @@
     <row r="78" ht="130" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
@@ -6410,7 +6410,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6481,7 +6481,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6561,7 +6561,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6641,7 +6641,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B82" s="2" t="inlineStr">
@@ -6721,7 +6721,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B83" s="2" t="inlineStr">
@@ -6801,7 +6801,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B84" s="2" t="inlineStr">
@@ -6881,7 +6881,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B85" s="2" t="inlineStr">
@@ -6961,7 +6961,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -7041,7 +7041,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7121,7 +7121,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7201,7 +7201,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7281,7 +7281,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7361,7 +7361,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7437,7 +7437,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
@@ -7514,7 +7514,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
@@ -7594,7 +7594,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B94" s="2" t="inlineStr">
@@ -7674,7 +7674,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
@@ -7754,7 +7754,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7834,7 +7834,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7914,7 +7914,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -7994,7 +7994,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8074,7 +8074,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8154,7 +8154,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8234,7 +8234,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8307,7 +8307,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AC-2 (4),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8388,7 +8388,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AC-2 (4),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8469,7 +8469,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AC-2 (4),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8540,7 +8540,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3 (1),AU-3</t>
+          <t>AU-3 (1),AC-2 (4),AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8615,7 +8615,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AC-2 (4),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8697,7 +8697,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AC-2 (4),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -8779,7 +8779,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AC-2 (4),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -8861,7 +8861,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AC-2 (4),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B110" s="2" t="inlineStr">
@@ -8943,7 +8943,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AC-2 (4),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-3 (1),AC-2 (4),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9025,7 +9025,7 @@
     <row r="112" ht="130" customHeight="1">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-14 (1),AU-3 (1),AU-12 a,AU-3</t>
+          <t>AU-14 (1),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
@@ -9275,7 +9275,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-6 (10)</t>
+          <t>AC-6 (10),AC-11 b</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9719,7 +9719,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -9790,7 +9790,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -10234,7 +10234,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AU-12 c,AC-6 (9),AC-2 (4)</t>
+          <t>AU-12 c,AC-2 (4),AC-6 (9),CM-5 (1)</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -10357,7 +10357,7 @@
     <row r="129" ht="130" customHeight="1">
       <c r="A129" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (b),CM-6 b,IA-5 (1) (a)</t>
+          <t>CM-6 b,IA-5 (1) (b),IA-5 (1) (a)</t>
         </is>
       </c>
       <c r="B129" s="2" t="inlineStr">
@@ -10677,7 +10677,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-13,MA-4 c,SC-8</t>
+          <t>SC-13,AC-17 (2),MA-4 c,SC-8</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10759,7 +10759,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>AC-12,MA-4 e,MA-4 (7),SC-10</t>
+          <t>MA-4 (7),SC-10,MA-4 e,AC-12</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -10989,7 +10989,7 @@
     <row r="137" ht="130" customHeight="1">
       <c r="A137" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,SC-10</t>
+          <t>SC-10,AC-11 a</t>
         </is>
       </c>
       <c r="B137" s="2" t="inlineStr">
@@ -11066,7 +11066,7 @@
     <row r="138" ht="130" customHeight="1">
       <c r="A138" s="2" t="inlineStr">
         <is>
-          <t>AU-7 a,AU-14 (1),MA-4 (1) (a),CM-5 (1),AU-7 (1),CM-6 b,AU-12 a,AU-3 (1),AU-6 (4),AU-3</t>
+          <t>AU-14 (1),CM-5 (1),AU-3 (1),MA-4 (1) (a),AU-6 (4),AU-3,AU-12 a,CM-6 b,AU-7 a,AU-7 (1)</t>
         </is>
       </c>
       <c r="B138" s="2" t="inlineStr">
@@ -13137,7 +13137,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8,SC-8 (1)</t>
+          <t>SC-8 (2),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B166" s="2" t="inlineStr">
@@ -13593,7 +13593,7 @@
     <row r="172" ht="130" customHeight="1">
       <c r="A172" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B172" s="2" t="inlineStr">
@@ -13671,7 +13671,7 @@
     <row r="173" ht="130" customHeight="1">
       <c r="A173" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B173" s="2" t="inlineStr">
@@ -13754,7 +13754,7 @@
     <row r="174" ht="130" customHeight="1">
       <c r="A174" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B174" s="2" t="inlineStr">
@@ -14134,7 +14134,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="2" t="inlineStr">
         <is>
-          <t>AU-6 (4),CM-6 b,AU-4 (1)</t>
+          <t>CM-6 b,AU-6 (4),AU-4 (1)</t>
         </is>
       </c>
       <c r="B179" s="2" t="inlineStr">
@@ -14205,7 +14205,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (9),AC-17 (1),CM-6 b,CM-7 b</t>
+          <t>CM-6 b,CM-7 b,AC-17 (9),AC-17 (1)</t>
         </is>
       </c>
       <c r="B180" s="2" t="inlineStr">
@@ -14282,7 +14282,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),CM-6 b,CM-7 b</t>
+          <t>CM-6 b,CM-7 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">
@@ -17023,7 +17023,7 @@
     <row r="216" ht="130" customHeight="1">
       <c r="A216" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-6 (9),AC-2 (4)</t>
+          <t>AU-12 c,AC-2 (4),AC-6 (9)</t>
         </is>
       </c>
       <c r="B216" s="2" t="inlineStr">
@@ -17543,7 +17543,7 @@
     <row r="222" ht="130" customHeight="1">
       <c r="A222" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (4),IA-2 (3),IA-2 (5),IA-2</t>
+          <t>IA-2 (3),IA-2,IA-2 (2),IA-2 (4),IA-2 (5)</t>
         </is>
       </c>
       <c r="B222" s="2" t="inlineStr">
@@ -17628,7 +17628,7 @@
     <row r="223" ht="130" customHeight="1">
       <c r="A223" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (4),IA-2 (3),IA-2 (5),IA-2</t>
+          <t>IA-2 (3),IA-2,IA-2 (2),IA-2 (4),IA-2 (5)</t>
         </is>
       </c>
       <c r="B223" s="2" t="inlineStr">
@@ -17713,7 +17713,7 @@
     <row r="224" ht="130" customHeight="1">
       <c r="A224" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),SC-8 (1),SC-8</t>
+          <t>SC-8,SC-8 (1),AC-18 (1)</t>
         </is>
       </c>
       <c r="B224" s="2" t="inlineStr">
@@ -17880,7 +17880,7 @@
     <row r="226" ht="130" customHeight="1">
       <c r="A226" s="2" t="inlineStr">
         <is>
-          <t>IA-7,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),IA-7</t>
         </is>
       </c>
       <c r="B226" s="2" t="inlineStr">
@@ -17963,7 +17963,7 @@
     <row r="227" ht="130" customHeight="1">
       <c r="A227" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B227" s="2" t="inlineStr">
@@ -18039,7 +18039,7 @@
     <row r="228" ht="130" customHeight="1">
       <c r="A228" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B228" s="2" t="inlineStr">
@@ -18124,7 +18124,7 @@
     <row r="229" ht="130" customHeight="1">
       <c r="A229" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B229" s="2" t="inlineStr">
@@ -18360,7 +18360,7 @@
     <row r="232" ht="130" customHeight="1">
       <c r="A232" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B232" s="2" t="inlineStr">
@@ -18519,7 +18519,7 @@
     <row r="234" ht="130" customHeight="1">
       <c r="A234" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B234" s="2" t="inlineStr">
@@ -19349,7 +19349,7 @@
     <row r="245" ht="130" customHeight="1">
       <c r="A245" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-6 b,SC-2</t>
+          <t>CM-6 b,SC-2,SI-16</t>
         </is>
       </c>
       <c r="B245" s="2" t="inlineStr">
@@ -20423,7 +20423,7 @@
     <row r="259" ht="130" customHeight="1">
       <c r="A259" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B259" s="2" t="inlineStr">
@@ -20498,7 +20498,7 @@
     <row r="260" ht="130" customHeight="1">
       <c r="A260" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B260" s="2" t="inlineStr">
@@ -20586,7 +20586,7 @@
     <row r="261" ht="130" customHeight="1">
       <c r="A261" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B261" s="2" t="inlineStr">
@@ -20663,7 +20663,7 @@
     <row r="262" ht="130" customHeight="1">
       <c r="A262" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B262" s="2" t="inlineStr">
@@ -20821,7 +20821,7 @@
     <row r="264" ht="130" customHeight="1">
       <c r="A264" s="2" t="inlineStr">
         <is>
-          <t>AU-5 (1),AU-5 a</t>
+          <t>AU-5 a,AU-5 (1)</t>
         </is>
       </c>
       <c r="B264" s="2" t="inlineStr">
@@ -21261,7 +21261,7 @@
     <row r="270" ht="130" customHeight="1">
       <c r="A270" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),CM-6 b</t>
+          <t>CM-6 b,IA-2 (2)</t>
         </is>
       </c>
       <c r="B270" s="2" t="inlineStr">
@@ -21348,7 +21348,7 @@
     <row r="271" ht="130" customHeight="1">
       <c r="A271" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (2),IA-2 (4),IA-2 (1)</t>
+          <t>IA-2 (2),IA-2 (4),IA-2 (3),IA-2 (1)</t>
         </is>
       </c>
       <c r="B271" s="2" t="inlineStr">
@@ -21735,7 +21735,7 @@
     <row r="276" ht="130" customHeight="1">
       <c r="A276" s="2" t="inlineStr">
         <is>
-          <t>SC-4,CM-6 b</t>
+          <t>CM-6 b,SC-4</t>
         </is>
       </c>
       <c r="B276" s="2" t="inlineStr">
@@ -21816,7 +21816,7 @@
     <row r="277" ht="130" customHeight="1">
       <c r="A277" s="2" t="inlineStr">
         <is>
-          <t>SC-4,SC-2</t>
+          <t>SC-2,SC-4</t>
         </is>
       </c>
       <c r="B277" s="2" t="inlineStr">
@@ -21904,7 +21904,7 @@
     <row r="278" ht="130" customHeight="1">
       <c r="A278" s="2" t="inlineStr">
         <is>
-          <t>SC-4,SC-2</t>
+          <t>SC-2,SC-4</t>
         </is>
       </c>
       <c r="B278" s="2" t="inlineStr">
@@ -22365,7 +22365,7 @@
     <row r="284" ht="130" customHeight="1">
       <c r="A284" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (3),CM-6 b</t>
+          <t>CM-6 b,CM-5 (3)</t>
         </is>
       </c>
       <c r="B284" s="2" t="inlineStr">
@@ -23465,7 +23465,7 @@
     <row r="298" ht="130" customHeight="1">
       <c r="A298" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B298" s="2" t="inlineStr">
@@ -23545,7 +23545,7 @@
     <row r="299" ht="130" customHeight="1">
       <c r="A299" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (1)</t>
+          <t>IA-2 (1),IA-2 (11)</t>
         </is>
       </c>
       <c r="B299" s="2" t="inlineStr">
@@ -25873,7 +25873,7 @@
     <row r="328" ht="130" customHeight="1">
       <c r="A328" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AU-12 c</t>
+          <t>AU-12 c,CM-5 (1)</t>
         </is>
       </c>
       <c r="B328" s="2" t="inlineStr">
@@ -26030,7 +26030,7 @@
     <row r="330" ht="130" customHeight="1">
       <c r="A330" s="2" t="inlineStr">
         <is>
-          <t>AU-5 b,AU-5 a</t>
+          <t>AU-5 a,AU-5 b</t>
         </is>
       </c>
       <c r="B330" s="2" t="inlineStr">
@@ -26949,7 +26949,7 @@
     <row r="342" ht="130" customHeight="1">
       <c r="A342" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-7 b</t>
+          <t>CM-7 b,IA-3</t>
         </is>
       </c>
       <c r="B342" s="2" t="inlineStr">
@@ -27024,7 +27024,7 @@
     <row r="343" ht="130" customHeight="1">
       <c r="A343" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-7 b</t>
+          <t>CM-7 b,CM-7 a</t>
         </is>
       </c>
       <c r="B343" s="2" t="inlineStr">
@@ -27098,7 +27098,7 @@
     <row r="344" ht="130" customHeight="1">
       <c r="A344" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-7 b</t>
+          <t>CM-7 b,CM-7 a</t>
         </is>
       </c>
       <c r="B344" s="2" t="inlineStr">
@@ -27172,7 +27172,7 @@
     <row r="345" ht="130" customHeight="1">
       <c r="A345" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),CM-7 b</t>
+          <t>CM-7 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B345" s="2" t="inlineStr">
@@ -28429,7 +28429,7 @@
     <row r="361" ht="130" customHeight="1">
       <c r="A361" s="2" t="inlineStr">
         <is>
-          <t>SI-6 d,SI-6 b,CM-3 (5)</t>
+          <t>SI-6 b,CM-3 (5),SI-6 d</t>
         </is>
       </c>
       <c r="B361" s="2" t="inlineStr">
@@ -30343,7 +30343,7 @@
     <row r="385" ht="130" customHeight="1">
       <c r="A385" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),CM-6 b</t>
+          <t>CM-6 b,AC-17 (2)</t>
         </is>
       </c>
       <c r="B385" s="2" t="inlineStr">
@@ -30652,7 +30652,7 @@
     <row r="389" ht="130" customHeight="1">
       <c r="A389" s="2" t="inlineStr">
         <is>
-          <t>SC-3,SI-6 a</t>
+          <t>SI-6 a,SC-3</t>
         </is>
       </c>
       <c r="B389" s="2" t="inlineStr">
@@ -31357,7 +31357,7 @@
     <row r="398" ht="130" customHeight="1">
       <c r="A398" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-6 b</t>
+          <t>CM-6 b,SI-16</t>
         </is>
       </c>
       <c r="B398" s="2" t="inlineStr">
@@ -31473,7 +31473,7 @@
       </c>
       <c r="F399" s="2" t="inlineStr">
         <is>
-          <t>Red Hat Enterprise Linux 9 must, for networked systems, compare internal information system clocks at least every 24 hours with a server which is synchronized to one of the redundant United States Naval Observatory (USNO) time servers, or a time server designat</t>
+          <t>Red Hat Enterprise Linux 9 must, for networked systems, compare internal information system clocks at least every 24 hours with a server which is synchronized to one of the redundant United States Naval Observatory (USNO) time servers, or a time server designated for the appropriate DoD network (NIPRNet/SIPRNet), and/or the Global Positioning System (GPS).</t>
         </is>
       </c>
       <c r="G399" s="2" t="inlineStr">
@@ -31598,7 +31598,7 @@
     <row r="401" ht="130" customHeight="1">
       <c r="A401" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B401" s="2" t="inlineStr">
@@ -31689,7 +31689,7 @@
     <row r="402" ht="130" customHeight="1">
       <c r="A402" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B402" s="2" t="inlineStr">
@@ -31783,7 +31783,7 @@
     <row r="403" ht="130" customHeight="1">
       <c r="A403" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B403" s="2" t="inlineStr">
@@ -35343,7 +35343,7 @@
     <row r="450" ht="130" customHeight="1">
       <c r="A450" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),CM-6 b</t>
+          <t>CM-6 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B450" s="2" t="inlineStr">
@@ -35416,7 +35416,7 @@
     <row r="451" ht="130" customHeight="1">
       <c r="A451" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),CM-6 b</t>
+          <t>CM-6 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B451" s="2" t="inlineStr">
@@ -42546,7 +42546,7 @@
     <row r="541" ht="130" customHeight="1">
       <c r="A541" s="2" t="inlineStr">
         <is>
-          <t>SI-2 (2),CM-6 b</t>
+          <t>CM-6 b,SI-2 (2)</t>
         </is>
       </c>
       <c r="B541" s="2" t="inlineStr">
@@ -43193,7 +43193,7 @@
     <row r="550" ht="130" customHeight="1">
       <c r="A550" s="2" t="inlineStr">
         <is>
-          <t>SI-2 (2),CM-6 b</t>
+          <t>CM-6 b,SI-2 (2)</t>
         </is>
       </c>
       <c r="B550" s="2" t="inlineStr">
@@ -43801,7 +43801,7 @@
     <row r="558" ht="130" customHeight="1">
       <c r="A558" s="2" t="inlineStr">
         <is>
-          <t>SI-6 a,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 a</t>
         </is>
       </c>
       <c r="B558" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@1b19a1e287060b7868036af7762529f5f9cf947a 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -708,7 +708,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-4</t>
+          <t>AU-4,CM-6 b</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -784,7 +784,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-5 (2),SC-5</t>
+          <t>SC-5,CM-6 b,SC-5 (2)</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -883,7 +883,7 @@
     <row r="6" ht="130" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AC-6 (8),AU-7 b,AC-6 (9),AU-12 (3),AU-8 b,AU-7 a</t>
+          <t>AC-6 (8),AU-8 b,AU-7 b,AU-7 a,CM-5 (1),AC-6 (9),AU-12 (3)</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -963,7 +963,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AU-7 b,AU-12 (3),AU-12 c,AU-8 b,AU-12 a,CM-6 b,AU-7 a</t>
+          <t>AU-8 b,AU-12 c,AU-7 b,AU-7 a,CM-5 (1),CM-6 b,AU-12 a,AU-12 (3)</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1269,7 +1269,7 @@
     <row r="11" ht="130" customHeight="1">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B11" s="2" t="inlineStr">
@@ -1346,7 +1346,7 @@
     <row r="12" ht="130" customHeight="1">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
@@ -1496,7 +1496,7 @@
     <row r="14" ht="130" customHeight="1">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -1572,7 +1572,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1726,7 +1726,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -2096,7 +2096,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -2170,7 +2170,7 @@
     <row r="23" ht="130" customHeight="1">
       <c r="A23" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B23" s="2" t="inlineStr">
@@ -3844,7 +3844,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>IA-8,IA-2,AU-3 (1)</t>
+          <t>AU-3 (1),IA-2,IA-8</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3922,7 +3922,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -3997,7 +3997,7 @@
     <row r="47" ht="130" customHeight="1">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
@@ -4072,7 +4072,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4147,7 +4147,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4222,7 +4222,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4297,7 +4297,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4372,7 +4372,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
@@ -4447,7 +4447,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4522,7 +4522,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4597,7 +4597,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4672,7 +4672,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4747,7 +4747,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4822,7 +4822,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4897,7 +4897,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -4977,7 +4977,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5060,7 +5060,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5140,7 +5140,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5220,7 +5220,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5300,7 +5300,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5380,7 +5380,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5454,7 +5454,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5528,7 +5528,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5602,7 +5602,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5676,7 +5676,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5750,7 +5750,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5823,7 +5823,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5896,7 +5896,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -5969,7 +5969,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6042,7 +6042,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6115,7 +6115,7 @@
     <row r="75" ht="130" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
@@ -6188,7 +6188,7 @@
     <row r="76" ht="130" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
@@ -6262,7 +6262,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6336,7 +6336,7 @@
     <row r="78" ht="130" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
@@ -6410,7 +6410,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6481,7 +6481,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6561,7 +6561,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6641,7 +6641,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B82" s="2" t="inlineStr">
@@ -6721,7 +6721,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B83" s="2" t="inlineStr">
@@ -6801,7 +6801,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B84" s="2" t="inlineStr">
@@ -6961,7 +6961,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -7041,7 +7041,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7121,7 +7121,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7201,7 +7201,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7281,7 +7281,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7361,7 +7361,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7437,7 +7437,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
@@ -7514,7 +7514,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
@@ -7594,7 +7594,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B94" s="2" t="inlineStr">
@@ -7674,7 +7674,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
@@ -7754,7 +7754,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7834,7 +7834,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7914,7 +7914,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -7994,7 +7994,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8074,7 +8074,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8154,7 +8154,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8234,7 +8234,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8307,7 +8307,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AC-2 (4),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AC-2 (4),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8388,7 +8388,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AC-2 (4),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AC-2 (4),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8469,7 +8469,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AC-2 (4),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AC-2 (4),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8540,7 +8540,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AC-2 (4),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AC-2 (4),MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8615,7 +8615,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AC-2 (4),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AC-2 (4),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8697,7 +8697,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AC-2 (4),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AC-2 (4),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -8779,7 +8779,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AC-2 (4),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AC-2 (4),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -8861,7 +8861,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AC-2 (4),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AC-2 (4),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B110" s="2" t="inlineStr">
@@ -8943,7 +8943,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AC-2 (4),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AC-2 (4),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9025,7 +9025,7 @@
     <row r="112" ht="130" customHeight="1">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-14 (1),AU-3,AU-12 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
@@ -9719,7 +9719,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 a,AU-3,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -9790,7 +9790,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 a,AU-3,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -10357,7 +10357,7 @@
     <row r="129" ht="130" customHeight="1">
       <c r="A129" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (b),IA-5 (1) (a)</t>
+          <t>CM-6 b,IA-5 (1) (a),IA-5 (1) (b)</t>
         </is>
       </c>
       <c r="B129" s="2" t="inlineStr">
@@ -10677,7 +10677,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>SC-13,AC-17 (2),MA-4 c,SC-8</t>
+          <t>AC-17 (2),SC-13,SC-8,MA-4 c</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10759,7 +10759,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (7),SC-10,MA-4 e,AC-12</t>
+          <t>MA-4 (7),SC-10,AC-12,MA-4 e</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -11066,7 +11066,7 @@
     <row r="138" ht="130" customHeight="1">
       <c r="A138" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),CM-5 (1),AU-3 (1),MA-4 (1) (a),AU-6 (4),AU-3,AU-12 a,CM-6 b,AU-7 a,AU-7 (1)</t>
+          <t>AU-6 (4),MA-4 (1) (a),AU-14 (1),AU-7 a,CM-5 (1),CM-6 b,AU-3,AU-12 a,AU-7 (1),AU-3 (1)</t>
         </is>
       </c>
       <c r="B138" s="2" t="inlineStr">
@@ -13593,7 +13593,7 @@
     <row r="172" ht="130" customHeight="1">
       <c r="A172" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B172" s="2" t="inlineStr">
@@ -13671,7 +13671,7 @@
     <row r="173" ht="130" customHeight="1">
       <c r="A173" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B173" s="2" t="inlineStr">
@@ -13754,7 +13754,7 @@
     <row r="174" ht="130" customHeight="1">
       <c r="A174" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B174" s="2" t="inlineStr">
@@ -14134,7 +14134,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-6 (4),AU-4 (1)</t>
+          <t>AU-4 (1),AU-6 (4),CM-6 b</t>
         </is>
       </c>
       <c r="B179" s="2" t="inlineStr">
@@ -14205,7 +14205,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 b,AC-17 (9),AC-17 (1)</t>
+          <t>AC-17 (1),CM-6 b,CM-7 b,AC-17 (9)</t>
         </is>
       </c>
       <c r="B180" s="2" t="inlineStr">
@@ -14282,7 +14282,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 b,AC-17 (1)</t>
+          <t>AC-17 (1),CM-6 b,CM-7 b</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">
@@ -14361,7 +14361,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B182" s="2" t="inlineStr">
@@ -14433,7 +14433,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B183" s="2" t="inlineStr">
@@ -14505,7 +14505,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B184" s="2" t="inlineStr">
@@ -14579,7 +14579,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B185" s="2" t="inlineStr">
@@ -14653,7 +14653,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B186" s="2" t="inlineStr">
@@ -14727,7 +14727,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B187" s="2" t="inlineStr">
@@ -16197,7 +16197,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-4 (1)</t>
+          <t>AU-4 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -16277,7 +16277,7 @@
     <row r="208" ht="130" customHeight="1">
       <c r="A208" s="2" t="inlineStr">
         <is>
-          <t>SC-28 (1),SC-28</t>
+          <t>SC-28,SC-28 (1)</t>
         </is>
       </c>
       <c r="B208" s="2" t="inlineStr">
@@ -17543,7 +17543,7 @@
     <row r="222" ht="130" customHeight="1">
       <c r="A222" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2,IA-2 (2),IA-2 (4),IA-2 (5)</t>
+          <t>IA-2 (2),IA-2 (4),IA-2 (5),IA-2,IA-2 (3)</t>
         </is>
       </c>
       <c r="B222" s="2" t="inlineStr">
@@ -17628,7 +17628,7 @@
     <row r="223" ht="130" customHeight="1">
       <c r="A223" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2,IA-2 (2),IA-2 (4),IA-2 (5)</t>
+          <t>IA-2 (2),IA-2 (4),IA-2 (5),IA-2,IA-2 (3)</t>
         </is>
       </c>
       <c r="B223" s="2" t="inlineStr">
@@ -17713,7 +17713,7 @@
     <row r="224" ht="130" customHeight="1">
       <c r="A224" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (1),AC-18 (1)</t>
+          <t>AC-18 (1),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B224" s="2" t="inlineStr">
@@ -17880,7 +17880,7 @@
     <row r="226" ht="130" customHeight="1">
       <c r="A226" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),IA-7</t>
+          <t>IA-7,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B226" s="2" t="inlineStr">
@@ -18360,7 +18360,7 @@
     <row r="232" ht="130" customHeight="1">
       <c r="A232" s="2" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B232" s="2" t="inlineStr">
@@ -18519,7 +18519,7 @@
     <row r="234" ht="130" customHeight="1">
       <c r="A234" s="2" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B234" s="2" t="inlineStr">
@@ -19116,7 +19116,7 @@
     <row r="242" ht="130" customHeight="1">
       <c r="A242" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B242" s="2" t="inlineStr">
@@ -19187,7 +19187,7 @@
     <row r="243" ht="130" customHeight="1">
       <c r="A243" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B243" s="2" t="inlineStr">
@@ -19349,7 +19349,7 @@
     <row r="245" ht="130" customHeight="1">
       <c r="A245" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-2,SI-16</t>
+          <t>SC-2,CM-6 b,SI-16</t>
         </is>
       </c>
       <c r="B245" s="2" t="inlineStr">
@@ -20821,7 +20821,7 @@
     <row r="264" ht="130" customHeight="1">
       <c r="A264" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 (1)</t>
+          <t>AU-5 (1),AU-5 a</t>
         </is>
       </c>
       <c r="B264" s="2" t="inlineStr">
@@ -21261,7 +21261,7 @@
     <row r="270" ht="130" customHeight="1">
       <c r="A270" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (2)</t>
+          <t>IA-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B270" s="2" t="inlineStr">
@@ -21348,7 +21348,7 @@
     <row r="271" ht="130" customHeight="1">
       <c r="A271" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (4),IA-2 (3),IA-2 (1)</t>
+          <t>IA-2 (2),IA-2 (3),IA-2 (4),IA-2 (1)</t>
         </is>
       </c>
       <c r="B271" s="2" t="inlineStr">
@@ -21517,7 +21517,7 @@
     <row r="273" ht="130" customHeight="1">
       <c r="A273" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B273" s="2" t="inlineStr">
@@ -23465,7 +23465,7 @@
     <row r="298" ht="130" customHeight="1">
       <c r="A298" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B298" s="2" t="inlineStr">
@@ -23545,7 +23545,7 @@
     <row r="299" ht="130" customHeight="1">
       <c r="A299" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (1)</t>
         </is>
       </c>
       <c r="B299" s="2" t="inlineStr">
@@ -24456,7 +24456,7 @@
     <row r="310" ht="130" customHeight="1">
       <c r="A310" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (a),AU-8 b,AU-8 (1) (b)</t>
+          <t>AU-8 (1) (a),AU-8 (1) (b),AU-8 b</t>
         </is>
       </c>
       <c r="B310" s="2" t="inlineStr">
@@ -25409,7 +25409,7 @@
     <row r="322" ht="130" customHeight="1">
       <c r="A322" s="2" t="inlineStr">
         <is>
-          <t>AC-3 (4),IA-11</t>
+          <t>IA-11,AC-3 (4)</t>
         </is>
       </c>
       <c r="B322" s="2" t="inlineStr">
@@ -26949,7 +26949,7 @@
     <row r="342" ht="130" customHeight="1">
       <c r="A342" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,IA-3</t>
+          <t>IA-3,CM-7 b</t>
         </is>
       </c>
       <c r="B342" s="2" t="inlineStr">
@@ -27024,7 +27024,7 @@
     <row r="343" ht="130" customHeight="1">
       <c r="A343" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-7 a</t>
+          <t>CM-7 a,CM-7 b</t>
         </is>
       </c>
       <c r="B343" s="2" t="inlineStr">
@@ -27098,7 +27098,7 @@
     <row r="344" ht="130" customHeight="1">
       <c r="A344" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-7 a</t>
+          <t>CM-7 a,CM-7 b</t>
         </is>
       </c>
       <c r="B344" s="2" t="inlineStr">
@@ -27172,7 +27172,7 @@
     <row r="345" ht="130" customHeight="1">
       <c r="A345" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (1)</t>
+          <t>AC-17 (1),CM-7 b</t>
         </is>
       </c>
       <c r="B345" s="2" t="inlineStr">
@@ -27335,7 +27335,7 @@
     <row r="347" ht="130" customHeight="1">
       <c r="A347" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (c),CM-7 a</t>
+          <t>CM-6 b,CM-7 a,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B347" s="2" t="inlineStr">
@@ -28180,7 +28180,7 @@
     <row r="358" ht="130" customHeight="1">
       <c r="A358" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 (1)</t>
+          <t>AC-11 (1),AC-11 b</t>
         </is>
       </c>
       <c r="B358" s="2" t="inlineStr">
@@ -28429,7 +28429,7 @@
     <row r="361" ht="130" customHeight="1">
       <c r="A361" s="2" t="inlineStr">
         <is>
-          <t>SI-6 b,CM-3 (5),SI-6 d</t>
+          <t>SI-6 b,SI-6 d,CM-3 (5)</t>
         </is>
       </c>
       <c r="B361" s="2" t="inlineStr">
@@ -28971,7 +28971,16 @@
         </is>
       </c>
       <c r="L367" s="2" t="n"/>
-      <c r="M367" s="2" t="inlineStr"/>
+      <c r="M367" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">To ensure that  pti=on  is added as a kernel command line
+argument to newly installed kernels, add  pti=on  to the
+default Grub2 command line for Linux operating systems.  Modify the line within
+ /etc/default/grub  as shown below:
+ GRUB_CMDLINE_LINUX="... pti=on ..." 
+Run the following command to update command line for already installed kernels: # grubby --update-kernel=ALL --args="pti=on" </t>
+        </is>
+      </c>
       <c r="N367" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -30343,7 +30352,7 @@
     <row r="385" ht="130" customHeight="1">
       <c r="A385" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-17 (2)</t>
+          <t>AC-17 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B385" s="2" t="inlineStr">
@@ -31357,7 +31366,7 @@
     <row r="398" ht="130" customHeight="1">
       <c r="A398" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-16</t>
+          <t>SI-16,CM-6 b</t>
         </is>
       </c>
       <c r="B398" s="2" t="inlineStr">
@@ -31435,7 +31444,14 @@
         </is>
       </c>
       <c r="L398" s="2" t="n"/>
-      <c r="M398" s="2" t="inlineStr"/>
+      <c r="M398" s="2" t="inlineStr">
+        <is>
+          <t>Add or edit the following line in a system configuration file in the "/etc/sysctl.d/" directory:
+kernel.randomize_va_space = 2
+Load settings from all system configuration files with the following command:
+$ sudo sysctl --system</t>
+        </is>
+      </c>
       <c r="N398" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -41227,7 +41243,7 @@
     <row r="524" ht="130" customHeight="1">
       <c r="A524" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-2</t>
+          <t>SC-2,CM-6 b</t>
         </is>
       </c>
       <c r="B524" s="2" t="inlineStr">
@@ -41314,7 +41330,7 @@
     <row r="525" ht="130" customHeight="1">
       <c r="A525" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-2</t>
+          <t>SC-2,CM-6 b</t>
         </is>
       </c>
       <c r="B525" s="2" t="inlineStr">
@@ -42546,7 +42562,7 @@
     <row r="541" ht="130" customHeight="1">
       <c r="A541" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-2 (2)</t>
+          <t>SI-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B541" s="2" t="inlineStr">
@@ -43193,7 +43209,7 @@
     <row r="550" ht="130" customHeight="1">
       <c r="A550" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-2 (2)</t>
+          <t>SI-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B550" s="2" t="inlineStr">
@@ -43801,7 +43817,7 @@
     <row r="558" ht="130" customHeight="1">
       <c r="A558" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 a</t>
+          <t>SI-6 a,CM-3 (5)</t>
         </is>
       </c>
       <c r="B558" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@862a6cb8c7dcbc47bcdd560f6738a413b2fa93e3 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -541,7 +541,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-4 (1)</t>
+          <t>AU-4 (1),AU-4</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -625,7 +625,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-14 (1)</t>
+          <t>AU-14 (1),AU-4</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -784,7 +784,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>SC-5,CM-6 b,SC-5 (2)</t>
+          <t>SC-5 (2),SC-5,CM-6 b</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -883,7 +883,7 @@
     <row r="6" ht="130" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (8),AU-8 b,AU-7 b,AU-7 a,CM-5 (1),AC-6 (9),AU-12 (3)</t>
+          <t>AC-6 (8),CM-5 (1),AU-7 b,AU-12 (3),AU-7 a,AU-8 b,AC-6 (9)</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -963,7 +963,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-12 c,AU-7 b,AU-7 a,CM-5 (1),CM-6 b,AU-12 a,AU-12 (3)</t>
+          <t>CM-5 (1),AU-7 b,AU-12 (3),AU-12 c,AU-7 a,AU-8 b,AU-12 a,CM-6 b</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -3844,7 +3844,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),IA-2,IA-8</t>
+          <t>IA-8,IA-2,AU-3 (1)</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3922,7 +3922,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -3997,7 +3997,7 @@
     <row r="47" ht="130" customHeight="1">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
@@ -4072,7 +4072,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4147,7 +4147,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4222,7 +4222,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4297,7 +4297,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4372,7 +4372,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
@@ -4447,7 +4447,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4522,7 +4522,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4597,7 +4597,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4672,7 +4672,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4747,7 +4747,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4822,7 +4822,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4897,7 +4897,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -4977,7 +4977,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5060,7 +5060,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5140,7 +5140,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5220,7 +5220,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5300,7 +5300,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5380,7 +5380,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5454,7 +5454,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5528,7 +5528,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5602,7 +5602,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5676,7 +5676,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5750,7 +5750,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5823,7 +5823,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5896,7 +5896,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -5969,7 +5969,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6042,7 +6042,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6115,7 +6115,7 @@
     <row r="75" ht="130" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
@@ -6188,7 +6188,7 @@
     <row r="76" ht="130" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
@@ -6262,7 +6262,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6336,7 +6336,7 @@
     <row r="78" ht="130" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
@@ -6410,7 +6410,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6481,7 +6481,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6561,7 +6561,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6641,7 +6641,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B82" s="2" t="inlineStr">
@@ -6721,7 +6721,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B83" s="2" t="inlineStr">
@@ -6801,7 +6801,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B84" s="2" t="inlineStr">
@@ -6881,7 +6881,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B85" s="2" t="inlineStr">
@@ -6961,7 +6961,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -7041,7 +7041,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7121,7 +7121,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7201,7 +7201,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7281,7 +7281,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7361,7 +7361,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7437,7 +7437,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
@@ -7514,7 +7514,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
@@ -7594,7 +7594,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B94" s="2" t="inlineStr">
@@ -7674,7 +7674,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
@@ -7754,7 +7754,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7834,7 +7834,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7914,7 +7914,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -7994,7 +7994,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8074,7 +8074,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8154,7 +8154,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8234,7 +8234,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8307,7 +8307,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AC-2 (4)</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8388,7 +8388,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AC-2 (4)</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8469,7 +8469,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AC-2 (4)</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8540,7 +8540,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AC-2 (4)</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8615,7 +8615,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AC-2 (4)</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8697,7 +8697,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AC-2 (4)</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -8779,7 +8779,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AC-2 (4)</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -8861,7 +8861,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AC-2 (4)</t>
         </is>
       </c>
       <c r="B110" s="2" t="inlineStr">
@@ -8943,7 +8943,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AC-2 (4)</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9025,7 +9025,7 @@
     <row r="112" ht="130" customHeight="1">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-14 (1),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-12 c,AU-14 (1),AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
@@ -9108,7 +9108,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9189,7 +9189,7 @@
     <row r="114" ht="130" customHeight="1">
       <c r="A114" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B114" s="2" t="inlineStr">
@@ -9353,7 +9353,7 @@
     <row r="116" ht="130" customHeight="1">
       <c r="A116" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B116" s="2" t="inlineStr">
@@ -9719,7 +9719,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -9790,7 +9790,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -10234,7 +10234,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-2 (4),AC-6 (9),CM-5 (1)</t>
+          <t>CM-5 (1),AU-12 c,AC-2 (4),AC-6 (9)</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -10357,7 +10357,7 @@
     <row r="129" ht="130" customHeight="1">
       <c r="A129" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (a),IA-5 (1) (b)</t>
+          <t>IA-5 (1) (b),IA-5 (1) (a),CM-6 b</t>
         </is>
       </c>
       <c r="B129" s="2" t="inlineStr">
@@ -10677,7 +10677,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-13,SC-8,MA-4 c</t>
+          <t>SC-13,AC-17 (2),MA-4 c,SC-8</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10759,7 +10759,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (7),SC-10,AC-12,MA-4 e</t>
+          <t>MA-4 (7),AC-12,SC-10,MA-4 e</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -10834,7 +10834,7 @@
     <row r="135" ht="130" customHeight="1">
       <c r="A135" s="2" t="inlineStr">
         <is>
-          <t>SC-10,AC-12</t>
+          <t>AC-12,SC-10</t>
         </is>
       </c>
       <c r="B135" s="2" t="inlineStr">
@@ -10913,7 +10913,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>SC-10,AC-12</t>
+          <t>AC-12,SC-10</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -10989,7 +10989,7 @@
     <row r="137" ht="130" customHeight="1">
       <c r="A137" s="2" t="inlineStr">
         <is>
-          <t>SC-10,AC-11 a</t>
+          <t>AC-11 a,SC-10</t>
         </is>
       </c>
       <c r="B137" s="2" t="inlineStr">
@@ -11066,7 +11066,7 @@
     <row r="138" ht="130" customHeight="1">
       <c r="A138" s="2" t="inlineStr">
         <is>
-          <t>AU-6 (4),MA-4 (1) (a),AU-14 (1),AU-7 a,CM-5 (1),CM-6 b,AU-3,AU-12 a,AU-7 (1),AU-3 (1)</t>
+          <t>CM-5 (1),AU-7 (1),AU-14 (1),AU-7 a,AU-3,AU-12 a,AU-3 (1),CM-6 b,AU-6 (4),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B138" s="2" t="inlineStr">
@@ -11316,7 +11316,7 @@
     <row r="141" ht="130" customHeight="1">
       <c r="A141" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B141" s="2" t="inlineStr">
@@ -11392,7 +11392,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B142" s="2" t="inlineStr">
@@ -14205,7 +14205,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),CM-6 b,CM-7 b,AC-17 (9)</t>
+          <t>CM-7 b,AC-17 (1),AC-17 (9),CM-6 b</t>
         </is>
       </c>
       <c r="B180" s="2" t="inlineStr">
@@ -14282,7 +14282,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),CM-6 b,CM-7 b</t>
+          <t>CM-7 b,AC-17 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">
@@ -14361,7 +14361,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B182" s="2" t="inlineStr">
@@ -14433,7 +14433,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B183" s="2" t="inlineStr">
@@ -14505,7 +14505,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B184" s="2" t="inlineStr">
@@ -14579,7 +14579,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B185" s="2" t="inlineStr">
@@ -14653,7 +14653,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B186" s="2" t="inlineStr">
@@ -14727,7 +14727,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B187" s="2" t="inlineStr">
@@ -15248,7 +15248,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-3</t>
+          <t>AU-3,CM-6 b</t>
         </is>
       </c>
       <c r="B194" s="2" t="inlineStr">
@@ -16591,7 +16591,7 @@
     <row r="212" ht="130" customHeight="1">
       <c r="A212" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B212" s="2" t="inlineStr">
@@ -16693,7 +16693,7 @@
     <row r="213" ht="130" customHeight="1">
       <c r="A213" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B213" s="2" t="inlineStr">
@@ -16803,7 +16803,7 @@
     <row r="214" ht="130" customHeight="1">
       <c r="A214" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B214" s="2" t="inlineStr">
@@ -16914,7 +16914,7 @@
     <row r="215" ht="130" customHeight="1">
       <c r="A215" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B215" s="2" t="inlineStr">
@@ -17543,7 +17543,7 @@
     <row r="222" ht="130" customHeight="1">
       <c r="A222" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (4),IA-2 (5),IA-2,IA-2 (3)</t>
+          <t>IA-2 (3),IA-2 (4),IA-2,IA-2 (2),IA-2 (5)</t>
         </is>
       </c>
       <c r="B222" s="2" t="inlineStr">
@@ -17628,7 +17628,7 @@
     <row r="223" ht="130" customHeight="1">
       <c r="A223" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (4),IA-2 (5),IA-2,IA-2 (3)</t>
+          <t>IA-2 (3),IA-2 (4),IA-2,IA-2 (2),IA-2 (5)</t>
         </is>
       </c>
       <c r="B223" s="2" t="inlineStr">
@@ -17713,7 +17713,7 @@
     <row r="224" ht="130" customHeight="1">
       <c r="A224" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),SC-8 (1),SC-8</t>
+          <t>SC-8 (1),SC-8,AC-18 (1)</t>
         </is>
       </c>
       <c r="B224" s="2" t="inlineStr">
@@ -17880,7 +17880,7 @@
     <row r="226" ht="130" customHeight="1">
       <c r="A226" s="2" t="inlineStr">
         <is>
-          <t>IA-7,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),IA-7</t>
         </is>
       </c>
       <c r="B226" s="2" t="inlineStr">
@@ -17963,7 +17963,7 @@
     <row r="227" ht="130" customHeight="1">
       <c r="A227" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B227" s="2" t="inlineStr">
@@ -18039,7 +18039,7 @@
     <row r="228" ht="130" customHeight="1">
       <c r="A228" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B228" s="2" t="inlineStr">
@@ -18124,7 +18124,7 @@
     <row r="229" ht="130" customHeight="1">
       <c r="A229" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B229" s="2" t="inlineStr">
@@ -18281,7 +18281,7 @@
     <row r="231" ht="130" customHeight="1">
       <c r="A231" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-7 a</t>
+          <t>CM-7 a,IA-7</t>
         </is>
       </c>
       <c r="B231" s="2" t="inlineStr">
@@ -18360,7 +18360,7 @@
     <row r="232" ht="130" customHeight="1">
       <c r="A232" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B232" s="2" t="inlineStr">
@@ -18519,7 +18519,7 @@
     <row r="234" ht="130" customHeight="1">
       <c r="A234" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B234" s="2" t="inlineStr">
@@ -19116,7 +19116,7 @@
     <row r="242" ht="130" customHeight="1">
       <c r="A242" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B242" s="2" t="inlineStr">
@@ -19187,7 +19187,7 @@
     <row r="243" ht="130" customHeight="1">
       <c r="A243" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B243" s="2" t="inlineStr">
@@ -19349,7 +19349,7 @@
     <row r="245" ht="130" customHeight="1">
       <c r="A245" s="2" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b,SI-16</t>
+          <t>CM-6 b,SI-16,SC-2</t>
         </is>
       </c>
       <c r="B245" s="2" t="inlineStr">
@@ -19509,7 +19509,7 @@
     <row r="247" ht="130" customHeight="1">
       <c r="A247" s="2" t="inlineStr">
         <is>
-          <t>SI-16,SC-3</t>
+          <t>SC-3,SI-16</t>
         </is>
       </c>
       <c r="B247" s="2" t="inlineStr">
@@ -20423,7 +20423,7 @@
     <row r="259" ht="130" customHeight="1">
       <c r="A259" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B259" s="2" t="inlineStr">
@@ -20498,7 +20498,7 @@
     <row r="260" ht="130" customHeight="1">
       <c r="A260" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B260" s="2" t="inlineStr">
@@ -20586,7 +20586,7 @@
     <row r="261" ht="130" customHeight="1">
       <c r="A261" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B261" s="2" t="inlineStr">
@@ -20663,7 +20663,7 @@
     <row r="262" ht="130" customHeight="1">
       <c r="A262" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B262" s="2" t="inlineStr">
@@ -21348,7 +21348,7 @@
     <row r="271" ht="130" customHeight="1">
       <c r="A271" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (3),IA-2 (4),IA-2 (1)</t>
+          <t>IA-2 (4),IA-2 (2),IA-2 (1),IA-2 (3)</t>
         </is>
       </c>
       <c r="B271" s="2" t="inlineStr">
@@ -21517,7 +21517,7 @@
     <row r="273" ht="130" customHeight="1">
       <c r="A273" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B273" s="2" t="inlineStr">
@@ -21735,7 +21735,7 @@
     <row r="276" ht="130" customHeight="1">
       <c r="A276" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-4</t>
+          <t>SC-4,CM-6 b</t>
         </is>
       </c>
       <c r="B276" s="2" t="inlineStr">
@@ -21816,7 +21816,7 @@
     <row r="277" ht="130" customHeight="1">
       <c r="A277" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SC-4</t>
+          <t>SC-4,SC-2</t>
         </is>
       </c>
       <c r="B277" s="2" t="inlineStr">
@@ -21904,7 +21904,7 @@
     <row r="278" ht="130" customHeight="1">
       <c r="A278" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SC-4</t>
+          <t>SC-4,SC-2</t>
         </is>
       </c>
       <c r="B278" s="2" t="inlineStr">
@@ -22142,7 +22142,7 @@
     <row r="281" ht="130" customHeight="1">
       <c r="A281" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-12 a</t>
+          <t>AU-12 a,CM-6 b</t>
         </is>
       </c>
       <c r="B281" s="2" t="inlineStr">
@@ -22365,7 +22365,7 @@
     <row r="284" ht="130" customHeight="1">
       <c r="A284" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (3)</t>
+          <t>CM-5 (3),CM-6 b</t>
         </is>
       </c>
       <c r="B284" s="2" t="inlineStr">
@@ -23634,7 +23634,7 @@
     <row r="300" ht="130" customHeight="1">
       <c r="A300" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12),IA-2 (1)</t>
+          <t>IA-2 (11),IA-2 (1),IA-2 (12)</t>
         </is>
       </c>
       <c r="B300" s="2" t="inlineStr">
@@ -24456,7 +24456,7 @@
     <row r="310" ht="130" customHeight="1">
       <c r="A310" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (a),AU-8 (1) (b),AU-8 b</t>
+          <t>AU-8 (1) (b),AU-8 b,AU-8 (1) (a)</t>
         </is>
       </c>
       <c r="B310" s="2" t="inlineStr">
@@ -25873,7 +25873,7 @@
     <row r="328" ht="130" customHeight="1">
       <c r="A328" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,CM-5 (1)</t>
+          <t>CM-5 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B328" s="2" t="inlineStr">
@@ -26030,7 +26030,7 @@
     <row r="330" ht="130" customHeight="1">
       <c r="A330" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 b</t>
+          <t>AU-5 b,AU-5 a</t>
         </is>
       </c>
       <c r="B330" s="2" t="inlineStr">
@@ -26949,7 +26949,7 @@
     <row r="342" ht="130" customHeight="1">
       <c r="A342" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-7 b</t>
+          <t>CM-7 b,IA-3</t>
         </is>
       </c>
       <c r="B342" s="2" t="inlineStr">
@@ -27172,7 +27172,7 @@
     <row r="345" ht="130" customHeight="1">
       <c r="A345" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),CM-7 b</t>
+          <t>CM-7 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B345" s="2" t="inlineStr">
@@ -27258,7 +27258,7 @@
     <row r="346" ht="130" customHeight="1">
       <c r="A346" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),CM-7 a</t>
+          <t>CM-7 a,AC-18 (1)</t>
         </is>
       </c>
       <c r="B346" s="2" t="inlineStr">
@@ -27335,7 +27335,7 @@
     <row r="347" ht="130" customHeight="1">
       <c r="A347" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B347" s="2" t="inlineStr">
@@ -28429,7 +28429,7 @@
     <row r="361" ht="130" customHeight="1">
       <c r="A361" s="2" t="inlineStr">
         <is>
-          <t>SI-6 b,SI-6 d,CM-3 (5)</t>
+          <t>SI-6 d,SI-6 b,CM-3 (5)</t>
         </is>
       </c>
       <c r="B361" s="2" t="inlineStr">
@@ -28497,7 +28497,7 @@
 The output should return something similar to the following:
  05 4 * * * root  --check 
 NOTE: The usage of special cron times, such as @daily or @weekly, is acceptable.
-If AIDE is not configured to periodicly scan then this is a finding.</t>
+If AIDE is not configured to scan periodically then this is a finding.</t>
         </is>
       </c>
       <c r="L361" s="2" t="n"/>
@@ -28520,7 +28520,7 @@
     <row r="362" ht="130" customHeight="1">
       <c r="A362" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B362" s="2" t="inlineStr">
@@ -28900,7 +28900,7 @@
     <row r="367" ht="130" customHeight="1">
       <c r="A367" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-7 a</t>
+          <t>CM-7 a,SI-16</t>
         </is>
       </c>
       <c r="B367" s="2" t="inlineStr">
@@ -29449,7 +29449,7 @@
     <row r="374" ht="130" customHeight="1">
       <c r="A374" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B374" s="2" t="inlineStr">
@@ -29520,7 +29520,7 @@
     <row r="375" ht="130" customHeight="1">
       <c r="A375" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B375" s="2" t="inlineStr">
@@ -29592,7 +29592,7 @@
     <row r="376" ht="130" customHeight="1">
       <c r="A376" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B376" s="2" t="inlineStr">
@@ -30661,7 +30661,7 @@
     <row r="389" ht="130" customHeight="1">
       <c r="A389" s="2" t="inlineStr">
         <is>
-          <t>SI-6 a,SC-3</t>
+          <t>SC-3,SI-6 a</t>
         </is>
       </c>
       <c r="B389" s="2" t="inlineStr">
@@ -30800,7 +30800,7 @@
     <row r="391" ht="130" customHeight="1">
       <c r="A391" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (a)</t>
+          <t>IA-5 (1) (a),CM-6 b</t>
         </is>
       </c>
       <c r="B391" s="2" t="inlineStr">
@@ -31614,7 +31614,7 @@
     <row r="401" ht="130" customHeight="1">
       <c r="A401" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B401" s="2" t="inlineStr">
@@ -31705,7 +31705,7 @@
     <row r="402" ht="130" customHeight="1">
       <c r="A402" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B402" s="2" t="inlineStr">
@@ -31799,7 +31799,7 @@
     <row r="403" ht="130" customHeight="1">
       <c r="A403" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B403" s="2" t="inlineStr">
@@ -35209,7 +35209,7 @@
     <row r="448" ht="130" customHeight="1">
       <c r="A448" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),CM-6 b</t>
         </is>
       </c>
       <c r="B448" s="2" t="inlineStr">
@@ -35359,7 +35359,7 @@
     <row r="450" ht="130" customHeight="1">
       <c r="A450" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (1)</t>
+          <t>CM-5 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B450" s="2" t="inlineStr">
@@ -35432,7 +35432,7 @@
     <row r="451" ht="130" customHeight="1">
       <c r="A451" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (1)</t>
+          <t>CM-5 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B451" s="2" t="inlineStr">
@@ -41243,7 +41243,7 @@
     <row r="524" ht="130" customHeight="1">
       <c r="A524" s="2" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b</t>
+          <t>CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B524" s="2" t="inlineStr">
@@ -41330,7 +41330,7 @@
     <row r="525" ht="130" customHeight="1">
       <c r="A525" s="2" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b</t>
+          <t>CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B525" s="2" t="inlineStr">
@@ -43817,7 +43817,7 @@
     <row r="558" ht="130" customHeight="1">
       <c r="A558" s="2" t="inlineStr">
         <is>
-          <t>SI-6 a,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 a</t>
         </is>
       </c>
       <c r="B558" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@1d01eff049db2a521ba3212318c7863baac55e32 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -708,7 +708,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>AU-4,CM-6 b</t>
+          <t>CM-6 b,AU-4</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -784,7 +784,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>SC-5 (2),SC-5,CM-6 b</t>
+          <t>CM-6 b,SC-5,SC-5 (2)</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -883,7 +883,7 @@
     <row r="6" ht="130" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (8),CM-5 (1),AU-7 b,AU-12 (3),AU-7 a,AU-8 b,AC-6 (9)</t>
+          <t>AU-7 b,CM-5 (1),AU-12 (3),AU-8 b,AC-6 (8),AC-6 (9),AU-7 a</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -963,7 +963,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AU-7 b,AU-12 (3),AU-12 c,AU-7 a,AU-8 b,AU-12 a,CM-6 b</t>
+          <t>CM-6 b,AU-7 b,CM-5 (1),AU-12 a,AU-12 (3),AU-8 b,AU-12 c,AU-7 a</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1269,7 +1269,7 @@
     <row r="11" ht="130" customHeight="1">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B11" s="2" t="inlineStr">
@@ -1346,7 +1346,7 @@
     <row r="12" ht="130" customHeight="1">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
@@ -3298,7 +3298,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3382,7 +3382,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3467,7 +3467,7 @@
     <row r="40" ht="130" customHeight="1">
       <c r="A40" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B40" s="2" t="inlineStr">
@@ -3539,7 +3539,7 @@
     <row r="41" ht="130" customHeight="1">
       <c r="A41" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B41" s="2" t="inlineStr">
@@ -3922,7 +3922,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -3997,7 +3997,7 @@
     <row r="47" ht="130" customHeight="1">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
@@ -4072,7 +4072,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4147,7 +4147,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4222,7 +4222,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4297,7 +4297,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4372,7 +4372,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
@@ -4447,7 +4447,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4522,7 +4522,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4597,7 +4597,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4672,7 +4672,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4747,7 +4747,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4822,7 +4822,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4897,7 +4897,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -4977,7 +4977,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5060,7 +5060,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5140,7 +5140,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5220,7 +5220,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5300,7 +5300,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5380,7 +5380,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5454,7 +5454,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5528,7 +5528,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5602,7 +5602,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5676,7 +5676,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5750,7 +5750,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5823,7 +5823,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5896,7 +5896,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -5969,7 +5969,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6042,7 +6042,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6115,7 +6115,7 @@
     <row r="75" ht="130" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
@@ -6188,7 +6188,7 @@
     <row r="76" ht="130" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
@@ -6262,7 +6262,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6336,7 +6336,7 @@
     <row r="78" ht="130" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
@@ -6410,7 +6410,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6468,7 +6468,14 @@
         </is>
       </c>
       <c r="L79" s="2" t="n"/>
-      <c r="M79" s="2" t="inlineStr"/>
+      <c r="M79" s="2" t="inlineStr">
+        <is>
+          <t>Configure Red Hat Enterprise Linux 9 to generate audit records for all account creations, modifications, disabling, and termination events that affect  /var/log/lastlog .
+Add or update the following file system rule to  /etc/audit/rules.d/audit.rules :
+-w /var/log/lastlog -p wa -k logins
+The audit daemon must be restarted for the changes to take effect.</t>
+        </is>
+      </c>
       <c r="N79" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -6481,7 +6488,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6561,7 +6568,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6641,7 +6648,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B82" s="2" t="inlineStr">
@@ -6721,7 +6728,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B83" s="2" t="inlineStr">
@@ -6801,7 +6808,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B84" s="2" t="inlineStr">
@@ -6881,7 +6888,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B85" s="2" t="inlineStr">
@@ -6961,7 +6968,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -7041,7 +7048,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7121,7 +7128,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7201,7 +7208,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7281,7 +7288,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7361,7 +7368,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7437,7 +7444,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
@@ -7514,7 +7521,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
@@ -7594,7 +7601,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B94" s="2" t="inlineStr">
@@ -7674,7 +7681,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
@@ -7754,7 +7761,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7834,7 +7841,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7914,7 +7921,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -7994,7 +8001,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8074,7 +8081,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8154,7 +8161,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8234,7 +8241,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8307,7 +8314,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AC-2 (4)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a),AC-2 (4)</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8388,7 +8395,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AC-2 (4)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a),AC-2 (4)</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8469,7 +8476,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AC-2 (4)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a),AC-2 (4)</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8540,7 +8547,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a),AC-2 (4)</t>
+          <t>AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a),AC-2 (4)</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8615,7 +8622,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AC-2 (4)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a),AC-2 (4)</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8697,7 +8704,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AC-2 (4)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a),AC-2 (4)</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -8779,7 +8786,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AC-2 (4)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a),AC-2 (4)</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -8861,7 +8868,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AC-2 (4)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a),AC-2 (4)</t>
         </is>
       </c>
       <c r="B110" s="2" t="inlineStr">
@@ -8943,7 +8950,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AC-2 (4)</t>
+          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a),AC-2 (4)</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9025,7 +9032,7 @@
     <row r="112" ht="130" customHeight="1">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-14 (1),AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3 (1),AU-14 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
@@ -9095,7 +9102,16 @@
         </is>
       </c>
       <c r="L112" s="2" t="n"/>
-      <c r="M112" s="2" t="inlineStr"/>
+      <c r="M112" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">To ensure that  audit=1  is added as a kernel command line
+argument to newly installed kernels, add  audit=1  to the
+default Grub2 command line for Linux operating systems.  Modify the line within
+ /etc/default/grub  as shown below:
+ GRUB_CMDLINE_LINUX="... audit=1 ..." 
+Run the following command to update command line for already installed kernels: # grubby --update-kernel=ALL --args="audit=1" </t>
+        </is>
+      </c>
       <c r="N112" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -9108,7 +9124,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9189,7 +9205,7 @@
     <row r="114" ht="130" customHeight="1">
       <c r="A114" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B114" s="2" t="inlineStr">
@@ -9275,7 +9291,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),AC-11 b</t>
+          <t>AC-11 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9353,7 +9369,7 @@
     <row r="116" ht="130" customHeight="1">
       <c r="A116" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B116" s="2" t="inlineStr">
@@ -9719,7 +9735,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -9790,7 +9806,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,MA-4 (1) (a),AU-12 a</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -9861,7 +9877,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-9</t>
+          <t>AU-9,AU-12 c</t>
         </is>
       </c>
       <c r="B122" s="2" t="inlineStr">
@@ -10234,7 +10250,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AU-12 c,AC-2 (4),AC-6 (9)</t>
+          <t>AC-2 (4),AU-12 c,AC-6 (9),CM-5 (1)</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -10357,7 +10373,7 @@
     <row r="129" ht="130" customHeight="1">
       <c r="A129" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (b),IA-5 (1) (a),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (a),IA-5 (1) (b)</t>
         </is>
       </c>
       <c r="B129" s="2" t="inlineStr">
@@ -10677,7 +10693,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>SC-13,AC-17 (2),MA-4 c,SC-8</t>
+          <t>SC-8,AC-17 (2),SC-13,MA-4 c</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10759,7 +10775,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (7),AC-12,SC-10,MA-4 e</t>
+          <t>AC-12,SC-10,MA-4 (7),MA-4 e</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -10834,7 +10850,7 @@
     <row r="135" ht="130" customHeight="1">
       <c r="A135" s="2" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B135" s="2" t="inlineStr">
@@ -10913,7 +10929,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -10989,7 +11005,7 @@
     <row r="137" ht="130" customHeight="1">
       <c r="A137" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,SC-10</t>
+          <t>SC-10,AC-11 a</t>
         </is>
       </c>
       <c r="B137" s="2" t="inlineStr">
@@ -11066,7 +11082,7 @@
     <row r="138" ht="130" customHeight="1">
       <c r="A138" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AU-7 (1),AU-14 (1),AU-7 a,AU-3,AU-12 a,AU-3 (1),CM-6 b,AU-6 (4),MA-4 (1) (a)</t>
+          <t>CM-6 b,AU-7 (1),CM-5 (1),AU-12 a,AU-6 (4),AU-3 (1),AU-14 (1),AU-3,MA-4 (1) (a),AU-7 a</t>
         </is>
       </c>
       <c r="B138" s="2" t="inlineStr">
@@ -11316,7 +11332,7 @@
     <row r="141" ht="130" customHeight="1">
       <c r="A141" s="2" t="inlineStr">
         <is>
-          <t>AU-9 (3),AU-9</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B141" s="2" t="inlineStr">
@@ -11392,7 +11408,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="2" t="inlineStr">
         <is>
-          <t>AU-9 (3),AU-9</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B142" s="2" t="inlineStr">
@@ -13137,7 +13153,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8 (1),SC-8</t>
+          <t>SC-8,SC-8 (1),SC-8 (2)</t>
         </is>
       </c>
       <c r="B166" s="2" t="inlineStr">
@@ -13290,7 +13306,7 @@
     <row r="168" ht="130" customHeight="1">
       <c r="A168" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8</t>
+          <t>SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B168" s="2" t="inlineStr">
@@ -13369,7 +13385,7 @@
     <row r="169" ht="130" customHeight="1">
       <c r="A169" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8</t>
+          <t>SC-8,SC-8 (2)</t>
         </is>
       </c>
       <c r="B169" s="2" t="inlineStr">
@@ -13444,7 +13460,7 @@
     <row r="170" ht="130" customHeight="1">
       <c r="A170" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8</t>
+          <t>SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B170" s="2" t="inlineStr">
@@ -14134,7 +14150,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-6 (4),CM-6 b</t>
+          <t>CM-6 b,AU-4 (1),AU-6 (4)</t>
         </is>
       </c>
       <c r="B179" s="2" t="inlineStr">
@@ -14205,7 +14221,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (1),AC-17 (9),CM-6 b</t>
+          <t>CM-6 b,AC-17 (9),CM-7 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B180" s="2" t="inlineStr">
@@ -14282,7 +14298,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (1),CM-6 b</t>
+          <t>CM-6 b,CM-7 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">
@@ -15248,7 +15264,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="2" t="inlineStr">
         <is>
-          <t>AU-3,CM-6 b</t>
+          <t>CM-6 b,AU-3</t>
         </is>
       </c>
       <c r="B194" s="2" t="inlineStr">
@@ -16197,7 +16213,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),CM-6 b</t>
+          <t>CM-6 b,AU-4 (1)</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -16277,7 +16293,7 @@
     <row r="208" ht="130" customHeight="1">
       <c r="A208" s="2" t="inlineStr">
         <is>
-          <t>SC-28,SC-28 (1)</t>
+          <t>SC-28 (1),SC-28</t>
         </is>
       </c>
       <c r="B208" s="2" t="inlineStr">
@@ -17023,7 +17039,7 @@
     <row r="216" ht="130" customHeight="1">
       <c r="A216" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-2 (4),AC-6 (9)</t>
+          <t>AC-2 (4),AU-12 c,AC-6 (9)</t>
         </is>
       </c>
       <c r="B216" s="2" t="inlineStr">
@@ -17465,7 +17481,7 @@
     <row r="221" ht="130" customHeight="1">
       <c r="A221" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),CM-6 b</t>
+          <t>CM-6 b,IA-2 (5)</t>
         </is>
       </c>
       <c r="B221" s="2" t="inlineStr">
@@ -17543,7 +17559,7 @@
     <row r="222" ht="130" customHeight="1">
       <c r="A222" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (4),IA-2,IA-2 (2),IA-2 (5)</t>
+          <t>IA-2 (2),IA-2 (5),IA-2 (3),IA-2,IA-2 (4)</t>
         </is>
       </c>
       <c r="B222" s="2" t="inlineStr">
@@ -17628,7 +17644,7 @@
     <row r="223" ht="130" customHeight="1">
       <c r="A223" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (4),IA-2,IA-2 (2),IA-2 (5)</t>
+          <t>IA-2 (2),IA-2 (5),IA-2 (3),IA-2,IA-2 (4)</t>
         </is>
       </c>
       <c r="B223" s="2" t="inlineStr">
@@ -17713,7 +17729,7 @@
     <row r="224" ht="130" customHeight="1">
       <c r="A224" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8,AC-18 (1)</t>
+          <t>AC-18 (1),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B224" s="2" t="inlineStr">
@@ -17880,7 +17896,7 @@
     <row r="226" ht="130" customHeight="1">
       <c r="A226" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),IA-7</t>
+          <t>IA-7,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B226" s="2" t="inlineStr">
@@ -17963,7 +17979,7 @@
     <row r="227" ht="130" customHeight="1">
       <c r="A227" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B227" s="2" t="inlineStr">
@@ -18039,7 +18055,7 @@
     <row r="228" ht="130" customHeight="1">
       <c r="A228" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B228" s="2" t="inlineStr">
@@ -18124,7 +18140,7 @@
     <row r="229" ht="130" customHeight="1">
       <c r="A229" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B229" s="2" t="inlineStr">
@@ -18281,7 +18297,7 @@
     <row r="231" ht="130" customHeight="1">
       <c r="A231" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,IA-7</t>
+          <t>IA-7,CM-7 a</t>
         </is>
       </c>
       <c r="B231" s="2" t="inlineStr">
@@ -18360,7 +18376,7 @@
     <row r="232" ht="130" customHeight="1">
       <c r="A232" s="2" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B232" s="2" t="inlineStr">
@@ -18444,7 +18460,7 @@
     <row r="233" ht="130" customHeight="1">
       <c r="A233" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),MA-4 (6)</t>
+          <t>MA-4 (6),AC-17 (2)</t>
         </is>
       </c>
       <c r="B233" s="2" t="inlineStr">
@@ -18519,7 +18535,7 @@
     <row r="234" ht="130" customHeight="1">
       <c r="A234" s="2" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B234" s="2" t="inlineStr">
@@ -19170,11 +19186,18 @@
         <is>
           <t>To verify that auditing is configured for system administrator actions, run the following command:
  $ sudo auditctl -l | grep "watch=/var/run/faillock\|-w /var/run/faillock" 
-If there is not output then this is a finding.</t>
+If there is no output then this is a finding.</t>
         </is>
       </c>
       <c r="L242" s="2" t="n"/>
-      <c r="M242" s="2" t="inlineStr"/>
+      <c r="M242" s="2" t="inlineStr">
+        <is>
+          <t>Configure Red Hat Enterprise Linux 9 to generate audit records for all account creations, modifications, disabling, and termination events that affect  /var/run/faillock .
+Add or update the following file system rule to  /etc/audit/rules.d/audit.rules :
+-w /var/run/faillock -p wa -k logins
+The audit daemon must be restarted for the changes to take effect.</t>
+        </is>
+      </c>
       <c r="N242" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -19245,7 +19268,14 @@
         </is>
       </c>
       <c r="L243" s="2" t="n"/>
-      <c r="M243" s="2" t="inlineStr"/>
+      <c r="M243" s="2" t="inlineStr">
+        <is>
+          <t>Configure Red Hat Enterprise Linux 9 to generate audit records for all account creations, modifications, disabling, and termination events that affect  /var/log/tallylog .
+Add or update the following file system rule to  /etc/audit/rules.d/audit.rules :
+-w /var/log/tallylog -p wa -k logins
+The audit daemon must be restarted for the changes to take effect.</t>
+        </is>
+      </c>
       <c r="N243" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -19349,7 +19379,7 @@
     <row r="245" ht="130" customHeight="1">
       <c r="A245" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-16,SC-2</t>
+          <t>CM-6 b,SC-2,SI-16</t>
         </is>
       </c>
       <c r="B245" s="2" t="inlineStr">
@@ -20423,7 +20453,7 @@
     <row r="259" ht="130" customHeight="1">
       <c r="A259" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B259" s="2" t="inlineStr">
@@ -20498,7 +20528,7 @@
     <row r="260" ht="130" customHeight="1">
       <c r="A260" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B260" s="2" t="inlineStr">
@@ -20586,7 +20616,7 @@
     <row r="261" ht="130" customHeight="1">
       <c r="A261" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B261" s="2" t="inlineStr">
@@ -20663,7 +20693,7 @@
     <row r="262" ht="130" customHeight="1">
       <c r="A262" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B262" s="2" t="inlineStr">
@@ -21261,7 +21291,7 @@
     <row r="270" ht="130" customHeight="1">
       <c r="A270" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),CM-6 b</t>
+          <t>CM-6 b,IA-2 (2)</t>
         </is>
       </c>
       <c r="B270" s="2" t="inlineStr">
@@ -21348,7 +21378,7 @@
     <row r="271" ht="130" customHeight="1">
       <c r="A271" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2 (2),IA-2 (1),IA-2 (3)</t>
+          <t>IA-2 (2),IA-2 (4),IA-2 (3),IA-2 (1)</t>
         </is>
       </c>
       <c r="B271" s="2" t="inlineStr">
@@ -21735,7 +21765,7 @@
     <row r="276" ht="130" customHeight="1">
       <c r="A276" s="2" t="inlineStr">
         <is>
-          <t>SC-4,CM-6 b</t>
+          <t>CM-6 b,SC-4</t>
         </is>
       </c>
       <c r="B276" s="2" t="inlineStr">
@@ -21816,7 +21846,7 @@
     <row r="277" ht="130" customHeight="1">
       <c r="A277" s="2" t="inlineStr">
         <is>
-          <t>SC-4,SC-2</t>
+          <t>SC-2,SC-4</t>
         </is>
       </c>
       <c r="B277" s="2" t="inlineStr">
@@ -21904,7 +21934,7 @@
     <row r="278" ht="130" customHeight="1">
       <c r="A278" s="2" t="inlineStr">
         <is>
-          <t>SC-4,SC-2</t>
+          <t>SC-2,SC-4</t>
         </is>
       </c>
       <c r="B278" s="2" t="inlineStr">
@@ -22142,7 +22172,7 @@
     <row r="281" ht="130" customHeight="1">
       <c r="A281" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,CM-6 b</t>
+          <t>CM-6 b,AU-12 a</t>
         </is>
       </c>
       <c r="B281" s="2" t="inlineStr">
@@ -22365,7 +22395,7 @@
     <row r="284" ht="130" customHeight="1">
       <c r="A284" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (3),CM-6 b</t>
+          <t>CM-6 b,CM-5 (3)</t>
         </is>
       </c>
       <c r="B284" s="2" t="inlineStr">
@@ -23465,7 +23495,7 @@
     <row r="298" ht="130" customHeight="1">
       <c r="A298" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B298" s="2" t="inlineStr">
@@ -23634,7 +23664,7 @@
     <row r="300" ht="130" customHeight="1">
       <c r="A300" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (1),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11),IA-2 (1)</t>
         </is>
       </c>
       <c r="B300" s="2" t="inlineStr">
@@ -24456,7 +24486,7 @@
     <row r="310" ht="130" customHeight="1">
       <c r="A310" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (b),AU-8 b,AU-8 (1) (a)</t>
+          <t>AU-8 b,AU-8 (1) (b),AU-8 (1) (a)</t>
         </is>
       </c>
       <c r="B310" s="2" t="inlineStr">
@@ -25873,7 +25903,7 @@
     <row r="328" ht="130" customHeight="1">
       <c r="A328" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AU-12 c</t>
+          <t>AU-12 c,CM-5 (1)</t>
         </is>
       </c>
       <c r="B328" s="2" t="inlineStr">
@@ -26030,7 +26060,7 @@
     <row r="330" ht="130" customHeight="1">
       <c r="A330" s="2" t="inlineStr">
         <is>
-          <t>AU-5 b,AU-5 a</t>
+          <t>AU-5 a,AU-5 b</t>
         </is>
       </c>
       <c r="B330" s="2" t="inlineStr">
@@ -26949,7 +26979,7 @@
     <row r="342" ht="130" customHeight="1">
       <c r="A342" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,IA-3</t>
+          <t>IA-3,CM-7 b</t>
         </is>
       </c>
       <c r="B342" s="2" t="inlineStr">
@@ -27258,7 +27288,7 @@
     <row r="346" ht="130" customHeight="1">
       <c r="A346" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,AC-18 (1)</t>
+          <t>AC-18 (1),CM-7 a</t>
         </is>
       </c>
       <c r="B346" s="2" t="inlineStr">
@@ -27335,7 +27365,7 @@
     <row r="347" ht="130" customHeight="1">
       <c r="A347" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B347" s="2" t="inlineStr">
@@ -28520,7 +28550,7 @@
     <row r="362" ht="130" customHeight="1">
       <c r="A362" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B362" s="2" t="inlineStr">
@@ -29449,7 +29479,7 @@
     <row r="374" ht="130" customHeight="1">
       <c r="A374" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B374" s="2" t="inlineStr">
@@ -29520,7 +29550,7 @@
     <row r="375" ht="130" customHeight="1">
       <c r="A375" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B375" s="2" t="inlineStr">
@@ -29592,7 +29622,7 @@
     <row r="376" ht="130" customHeight="1">
       <c r="A376" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B376" s="2" t="inlineStr">
@@ -30352,7 +30382,7 @@
     <row r="385" ht="130" customHeight="1">
       <c r="A385" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),CM-6 b</t>
+          <t>CM-6 b,AC-17 (2)</t>
         </is>
       </c>
       <c r="B385" s="2" t="inlineStr">
@@ -30800,7 +30830,7 @@
     <row r="391" ht="130" customHeight="1">
       <c r="A391" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (a),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (a)</t>
         </is>
       </c>
       <c r="B391" s="2" t="inlineStr">
@@ -31366,7 +31396,7 @@
     <row r="398" ht="130" customHeight="1">
       <c r="A398" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-6 b</t>
+          <t>CM-6 b,SI-16</t>
         </is>
       </c>
       <c r="B398" s="2" t="inlineStr">
@@ -31614,7 +31644,7 @@
     <row r="401" ht="130" customHeight="1">
       <c r="A401" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B401" s="2" t="inlineStr">
@@ -31705,7 +31735,7 @@
     <row r="402" ht="130" customHeight="1">
       <c r="A402" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B402" s="2" t="inlineStr">
@@ -31799,7 +31829,7 @@
     <row r="403" ht="130" customHeight="1">
       <c r="A403" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B403" s="2" t="inlineStr">
@@ -35209,7 +35239,7 @@
     <row r="448" ht="130" customHeight="1">
       <c r="A448" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B448" s="2" t="inlineStr">
@@ -35359,7 +35389,7 @@
     <row r="450" ht="130" customHeight="1">
       <c r="A450" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),CM-6 b</t>
+          <t>CM-6 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B450" s="2" t="inlineStr">
@@ -35432,7 +35462,7 @@
     <row r="451" ht="130" customHeight="1">
       <c r="A451" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),CM-6 b</t>
+          <t>CM-6 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B451" s="2" t="inlineStr">
@@ -42562,7 +42592,7 @@
     <row r="541" ht="130" customHeight="1">
       <c r="A541" s="2" t="inlineStr">
         <is>
-          <t>SI-2 (2),CM-6 b</t>
+          <t>CM-6 b,SI-2 (2)</t>
         </is>
       </c>
       <c r="B541" s="2" t="inlineStr">
@@ -43209,7 +43239,7 @@
     <row r="550" ht="130" customHeight="1">
       <c r="A550" s="2" t="inlineStr">
         <is>
-          <t>SI-2 (2),CM-6 b</t>
+          <t>CM-6 b,SI-2 (2)</t>
         </is>
       </c>
       <c r="B550" s="2" t="inlineStr">
@@ -43817,7 +43847,7 @@
     <row r="558" ht="130" customHeight="1">
       <c r="A558" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 a</t>
+          <t>SI-6 a,CM-3 (5)</t>
         </is>
       </c>
       <c r="B558" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@1ce120b5203c36034ee6236a67033a9b117b9cc4 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -541,7 +541,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-4</t>
+          <t>AU-4,AU-4 (1)</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -625,7 +625,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),AU-4</t>
+          <t>AU-4,AU-14 (1)</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -883,7 +883,7 @@
     <row r="6" ht="130" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>AU-7 b,CM-5 (1),AU-12 (3),AU-8 b,AC-6 (8),AC-6 (9),AU-7 a</t>
+          <t>CM-5 (1),AU-8 b,AC-6 (9),AU-12 (3),AU-7 b,AU-7 a,AC-6 (8)</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -963,7 +963,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-7 b,CM-5 (1),AU-12 a,AU-12 (3),AU-8 b,AU-12 c,AU-7 a</t>
+          <t>AU-12 c,CM-5 (1),AU-8 b,CM-6 b,AU-12 (3),AU-7 b,AU-12 a,AU-7 a</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1726,7 +1726,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -2096,7 +2096,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -2170,7 +2170,7 @@
     <row r="23" ht="130" customHeight="1">
       <c r="A23" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B23" s="2" t="inlineStr">
@@ -3298,7 +3298,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3382,7 +3382,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3467,7 +3467,7 @@
     <row r="40" ht="130" customHeight="1">
       <c r="A40" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B40" s="2" t="inlineStr">
@@ -3539,7 +3539,7 @@
     <row r="41" ht="130" customHeight="1">
       <c r="A41" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B41" s="2" t="inlineStr">
@@ -3844,7 +3844,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>IA-8,IA-2,AU-3 (1)</t>
+          <t>AU-3 (1),IA-2,IA-8</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3922,7 +3922,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -3997,7 +3997,7 @@
     <row r="47" ht="130" customHeight="1">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
@@ -4072,7 +4072,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4147,7 +4147,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4222,7 +4222,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4297,7 +4297,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4372,7 +4372,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
@@ -4447,7 +4447,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4522,7 +4522,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4597,7 +4597,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4672,7 +4672,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4747,7 +4747,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4822,7 +4822,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4897,7 +4897,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -4977,7 +4977,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5060,7 +5060,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5140,7 +5140,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5220,7 +5220,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5300,7 +5300,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5380,7 +5380,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5454,7 +5454,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5528,7 +5528,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5602,7 +5602,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5676,7 +5676,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5750,7 +5750,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5823,7 +5823,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5896,7 +5896,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -5969,7 +5969,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6042,7 +6042,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6115,7 +6115,7 @@
     <row r="75" ht="130" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
@@ -6188,7 +6188,7 @@
     <row r="76" ht="130" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
@@ -6262,7 +6262,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6336,7 +6336,7 @@
     <row r="78" ht="130" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
@@ -6410,7 +6410,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6488,7 +6488,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6568,7 +6568,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6648,7 +6648,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B82" s="2" t="inlineStr">
@@ -6728,7 +6728,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B83" s="2" t="inlineStr">
@@ -6808,7 +6808,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B84" s="2" t="inlineStr">
@@ -6968,7 +6968,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -7048,7 +7048,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7128,7 +7128,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7208,7 +7208,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7288,7 +7288,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7444,7 +7444,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
@@ -7521,7 +7521,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
@@ -7601,7 +7601,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B94" s="2" t="inlineStr">
@@ -7681,7 +7681,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
@@ -7761,7 +7761,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7841,7 +7841,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7921,7 +7921,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8001,7 +8001,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8081,7 +8081,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8161,7 +8161,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8241,7 +8241,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8314,7 +8314,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a),AC-2 (4)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AC-2 (4),AU-3 (1)</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8395,7 +8395,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a),AC-2 (4)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AC-2 (4),AU-3 (1)</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8476,7 +8476,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a),AC-2 (4)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AC-2 (4),AU-3 (1)</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8547,7 +8547,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a),AC-2 (4)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AC-2 (4),AU-3 (1)</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8622,7 +8622,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a),AC-2 (4)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AC-2 (4),AU-3 (1)</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8704,7 +8704,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a),AC-2 (4)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AC-2 (4),AU-3 (1)</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -8786,7 +8786,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a),AC-2 (4)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AC-2 (4),AU-3 (1)</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -8868,7 +8868,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a),AC-2 (4)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AC-2 (4),AU-3 (1)</t>
         </is>
       </c>
       <c r="B110" s="2" t="inlineStr">
@@ -8950,7 +8950,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a),AC-2 (4)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3,AC-2 (4),AU-3 (1)</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9032,7 +9032,7 @@
     <row r="112" ht="130" customHeight="1">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-14 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-14 (1),AU-12 a,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
@@ -9735,7 +9735,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -9806,7 +9806,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -9877,7 +9877,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-12 c</t>
+          <t>AU-12 c,AU-9</t>
         </is>
       </c>
       <c r="B122" s="2" t="inlineStr">
@@ -10250,7 +10250,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 c,AC-6 (9),CM-5 (1)</t>
+          <t>AC-2 (4),AC-6 (9),AU-12 c,CM-5 (1)</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -10373,7 +10373,7 @@
     <row r="129" ht="130" customHeight="1">
       <c r="A129" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (a),IA-5 (1) (b)</t>
+          <t>CM-6 b,IA-5 (1) (b),IA-5 (1) (a)</t>
         </is>
       </c>
       <c r="B129" s="2" t="inlineStr">
@@ -10693,7 +10693,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2),SC-13,MA-4 c</t>
+          <t>MA-4 c,SC-8,SC-13,AC-17 (2)</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10775,7 +10775,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>AC-12,SC-10,MA-4 (7),MA-4 e</t>
+          <t>MA-4 (7),AC-12,SC-10,MA-4 e</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -10850,7 +10850,7 @@
     <row r="135" ht="130" customHeight="1">
       <c r="A135" s="2" t="inlineStr">
         <is>
-          <t>SC-10,AC-12</t>
+          <t>AC-12,SC-10</t>
         </is>
       </c>
       <c r="B135" s="2" t="inlineStr">
@@ -10929,7 +10929,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>SC-10,AC-12</t>
+          <t>AC-12,SC-10</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -11005,7 +11005,7 @@
     <row r="137" ht="130" customHeight="1">
       <c r="A137" s="2" t="inlineStr">
         <is>
-          <t>SC-10,AC-11 a</t>
+          <t>AC-11 a,SC-10</t>
         </is>
       </c>
       <c r="B137" s="2" t="inlineStr">
@@ -11082,7 +11082,7 @@
     <row r="138" ht="130" customHeight="1">
       <c r="A138" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-7 (1),CM-5 (1),AU-12 a,AU-6 (4),AU-3 (1),AU-14 (1),AU-3,MA-4 (1) (a),AU-7 a</t>
+          <t>MA-4 (1) (a),CM-5 (1),CM-6 b,AU-14 (1),AU-7 (1),AU-12 a,AU-3,AU-6 (4),AU-7 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B138" s="2" t="inlineStr">
@@ -11332,7 +11332,7 @@
     <row r="141" ht="130" customHeight="1">
       <c r="A141" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B141" s="2" t="inlineStr">
@@ -11408,7 +11408,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B142" s="2" t="inlineStr">
@@ -11484,7 +11484,7 @@
     <row r="143" ht="130" customHeight="1">
       <c r="A143" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B143" s="2" t="inlineStr">
@@ -11553,7 +11553,7 @@
     <row r="144" ht="130" customHeight="1">
       <c r="A144" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B144" s="2" t="inlineStr">
@@ -11622,7 +11622,7 @@
     <row r="145" ht="130" customHeight="1">
       <c r="A145" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B145" s="2" t="inlineStr">
@@ -11692,7 +11692,7 @@
     <row r="146" ht="130" customHeight="1">
       <c r="A146" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B146" s="2" t="inlineStr">
@@ -11761,7 +11761,7 @@
     <row r="147" ht="130" customHeight="1">
       <c r="A147" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B147" s="2" t="inlineStr">
@@ -11830,7 +11830,7 @@
     <row r="148" ht="130" customHeight="1">
       <c r="A148" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B148" s="2" t="inlineStr">
@@ -11900,7 +11900,7 @@
     <row r="149" ht="130" customHeight="1">
       <c r="A149" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B149" s="2" t="inlineStr">
@@ -11969,7 +11969,7 @@
     <row r="150" ht="130" customHeight="1">
       <c r="A150" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B150" s="2" t="inlineStr">
@@ -12038,7 +12038,7 @@
     <row r="151" ht="130" customHeight="1">
       <c r="A151" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B151" s="2" t="inlineStr">
@@ -12108,7 +12108,7 @@
     <row r="152" ht="130" customHeight="1">
       <c r="A152" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B152" s="2" t="inlineStr">
@@ -12177,7 +12177,7 @@
     <row r="153" ht="130" customHeight="1">
       <c r="A153" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B153" s="2" t="inlineStr">
@@ -12246,7 +12246,7 @@
     <row r="154" ht="130" customHeight="1">
       <c r="A154" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B154" s="2" t="inlineStr">
@@ -12315,7 +12315,7 @@
     <row r="155" ht="130" customHeight="1">
       <c r="A155" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B155" s="2" t="inlineStr">
@@ -13609,7 +13609,7 @@
     <row r="172" ht="130" customHeight="1">
       <c r="A172" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B172" s="2" t="inlineStr">
@@ -13687,7 +13687,7 @@
     <row r="173" ht="130" customHeight="1">
       <c r="A173" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B173" s="2" t="inlineStr">
@@ -13770,7 +13770,7 @@
     <row r="174" ht="130" customHeight="1">
       <c r="A174" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B174" s="2" t="inlineStr">
@@ -14150,7 +14150,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-4 (1),AU-6 (4)</t>
+          <t>AU-6 (4),AU-4 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B179" s="2" t="inlineStr">
@@ -14221,7 +14221,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-17 (9),CM-7 b,AC-17 (1)</t>
+          <t>CM-7 b,AC-17 (1),CM-6 b,AC-17 (9)</t>
         </is>
       </c>
       <c r="B180" s="2" t="inlineStr">
@@ -14298,7 +14298,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 b,AC-17 (1)</t>
+          <t>CM-7 b,AC-17 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">
@@ -16293,7 +16293,7 @@
     <row r="208" ht="130" customHeight="1">
       <c r="A208" s="2" t="inlineStr">
         <is>
-          <t>SC-28 (1),SC-28</t>
+          <t>SC-28,SC-28 (1)</t>
         </is>
       </c>
       <c r="B208" s="2" t="inlineStr">
@@ -17039,7 +17039,7 @@
     <row r="216" ht="130" customHeight="1">
       <c r="A216" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 c,AC-6 (9)</t>
+          <t>AC-2 (4),AC-6 (9),AU-12 c</t>
         </is>
       </c>
       <c r="B216" s="2" t="inlineStr">
@@ -17481,7 +17481,7 @@
     <row r="221" ht="130" customHeight="1">
       <c r="A221" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (5)</t>
+          <t>IA-2 (5),CM-6 b</t>
         </is>
       </c>
       <c r="B221" s="2" t="inlineStr">
@@ -17559,7 +17559,7 @@
     <row r="222" ht="130" customHeight="1">
       <c r="A222" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (5),IA-2 (3),IA-2,IA-2 (4)</t>
+          <t>IA-2 (2),IA-2,IA-2 (4),IA-2 (5),IA-2 (3)</t>
         </is>
       </c>
       <c r="B222" s="2" t="inlineStr">
@@ -17644,7 +17644,7 @@
     <row r="223" ht="130" customHeight="1">
       <c r="A223" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (5),IA-2 (3),IA-2,IA-2 (4)</t>
+          <t>IA-2 (2),IA-2,IA-2 (4),IA-2 (5),IA-2 (3)</t>
         </is>
       </c>
       <c r="B223" s="2" t="inlineStr">
@@ -17729,7 +17729,7 @@
     <row r="224" ht="130" customHeight="1">
       <c r="A224" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),SC-8 (1),SC-8</t>
+          <t>AC-18 (1),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B224" s="2" t="inlineStr">
@@ -18297,7 +18297,7 @@
     <row r="231" ht="130" customHeight="1">
       <c r="A231" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-7 a</t>
+          <t>CM-7 a,IA-7</t>
         </is>
       </c>
       <c r="B231" s="2" t="inlineStr">
@@ -19132,7 +19132,7 @@
     <row r="242" ht="130" customHeight="1">
       <c r="A242" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B242" s="2" t="inlineStr">
@@ -19210,7 +19210,7 @@
     <row r="243" ht="130" customHeight="1">
       <c r="A243" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B243" s="2" t="inlineStr">
@@ -19379,7 +19379,7 @@
     <row r="245" ht="130" customHeight="1">
       <c r="A245" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-2,SI-16</t>
+          <t>CM-6 b,SI-16,SC-2</t>
         </is>
       </c>
       <c r="B245" s="2" t="inlineStr">
@@ -21378,7 +21378,7 @@
     <row r="271" ht="130" customHeight="1">
       <c r="A271" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (4),IA-2 (3),IA-2 (1)</t>
+          <t>IA-2 (3),IA-2 (1),IA-2 (2),IA-2 (4)</t>
         </is>
       </c>
       <c r="B271" s="2" t="inlineStr">
@@ -21547,7 +21547,7 @@
     <row r="273" ht="130" customHeight="1">
       <c r="A273" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B273" s="2" t="inlineStr">
@@ -21846,7 +21846,7 @@
     <row r="277" ht="130" customHeight="1">
       <c r="A277" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SC-4</t>
+          <t>SC-4,SC-2</t>
         </is>
       </c>
       <c r="B277" s="2" t="inlineStr">
@@ -21934,7 +21934,7 @@
     <row r="278" ht="130" customHeight="1">
       <c r="A278" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SC-4</t>
+          <t>SC-4,SC-2</t>
         </is>
       </c>
       <c r="B278" s="2" t="inlineStr">
@@ -24486,7 +24486,7 @@
     <row r="310" ht="130" customHeight="1">
       <c r="A310" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-8 (1) (b),AU-8 (1) (a)</t>
+          <t>AU-8 (1) (b),AU-8 (1) (a),AU-8 b</t>
         </is>
       </c>
       <c r="B310" s="2" t="inlineStr">
@@ -25439,7 +25439,7 @@
     <row r="322" ht="130" customHeight="1">
       <c r="A322" s="2" t="inlineStr">
         <is>
-          <t>IA-11,AC-3 (4)</t>
+          <t>AC-3 (4),IA-11</t>
         </is>
       </c>
       <c r="B322" s="2" t="inlineStr">
@@ -26979,7 +26979,7 @@
     <row r="342" ht="130" customHeight="1">
       <c r="A342" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-7 b</t>
+          <t>CM-7 b,IA-3</t>
         </is>
       </c>
       <c r="B342" s="2" t="inlineStr">
@@ -27054,7 +27054,7 @@
     <row r="343" ht="130" customHeight="1">
       <c r="A343" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-7 b</t>
+          <t>CM-7 b,CM-7 a</t>
         </is>
       </c>
       <c r="B343" s="2" t="inlineStr">
@@ -27128,7 +27128,7 @@
     <row r="344" ht="130" customHeight="1">
       <c r="A344" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-7 b</t>
+          <t>CM-7 b,CM-7 a</t>
         </is>
       </c>
       <c r="B344" s="2" t="inlineStr">
@@ -27288,7 +27288,7 @@
     <row r="346" ht="130" customHeight="1">
       <c r="A346" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),CM-7 a</t>
+          <t>CM-7 a,AC-18 (1)</t>
         </is>
       </c>
       <c r="B346" s="2" t="inlineStr">
@@ -27365,7 +27365,7 @@
     <row r="347" ht="130" customHeight="1">
       <c r="A347" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a,IA-5 (1) (c)</t>
+          <t>CM-7 a,CM-6 b,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B347" s="2" t="inlineStr">
@@ -28210,7 +28210,7 @@
     <row r="358" ht="130" customHeight="1">
       <c r="A358" s="2" t="inlineStr">
         <is>
-          <t>AC-11 (1),AC-11 b</t>
+          <t>AC-11 b,AC-11 (1)</t>
         </is>
       </c>
       <c r="B358" s="2" t="inlineStr">
@@ -29479,7 +29479,7 @@
     <row r="374" ht="130" customHeight="1">
       <c r="A374" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B374" s="2" t="inlineStr">
@@ -29550,7 +29550,7 @@
     <row r="375" ht="130" customHeight="1">
       <c r="A375" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B375" s="2" t="inlineStr">
@@ -29622,7 +29622,7 @@
     <row r="376" ht="130" customHeight="1">
       <c r="A376" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B376" s="2" t="inlineStr">
@@ -30691,7 +30691,7 @@
     <row r="389" ht="130" customHeight="1">
       <c r="A389" s="2" t="inlineStr">
         <is>
-          <t>SC-3,SI-6 a</t>
+          <t>SI-6 a,SC-3</t>
         </is>
       </c>
       <c r="B389" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@c8a33fe1784a5db5acd6db0768dbb63dee8668c3 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -541,7 +541,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-4 (1)</t>
+          <t>AU-4 (1),AU-4</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -625,7 +625,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-14 (1)</t>
+          <t>AU-14 (1),AU-4</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -883,7 +883,7 @@
     <row r="6" ht="130" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>AU-7 a,AC-6 (9),AC-6 (8),AU-7 b,AU-8 b,CM-5 (1),AU-12 (3)</t>
+          <t>AU-12 (3),AU-7 a,AC-6 (9),AU-8 b,CM-5 (1),AU-7 b,AC-6 (8)</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -963,7 +963,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-7 a,AU-7 b,AU-8 b,AU-12 a,CM-5 (1),AU-12 c,CM-6 b,AU-12 (3)</t>
+          <t>AU-12 (3),AU-12 c,CM-6 b,AU-7 a,AU-8 b,AU-12 a,CM-5 (1),AU-7 b</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1269,7 +1269,7 @@
     <row r="11" ht="130" customHeight="1">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B11" s="2" t="inlineStr">
@@ -1346,7 +1346,7 @@
     <row r="12" ht="130" customHeight="1">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
@@ -1496,7 +1496,7 @@
     <row r="14" ht="130" customHeight="1">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -1572,7 +1572,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1726,7 +1726,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -2096,7 +2096,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -2170,7 +2170,7 @@
     <row r="23" ht="130" customHeight="1">
       <c r="A23" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B23" s="2" t="inlineStr">
@@ -3298,7 +3298,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3382,7 +3382,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3467,7 +3467,7 @@
     <row r="40" ht="130" customHeight="1">
       <c r="A40" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B40" s="2" t="inlineStr">
@@ -3539,7 +3539,7 @@
     <row r="41" ht="130" customHeight="1">
       <c r="A41" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B41" s="2" t="inlineStr">
@@ -3844,7 +3844,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>IA-2,AU-3 (1),IA-8</t>
+          <t>AU-3 (1),IA-2,IA-8</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3922,7 +3922,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -3997,7 +3997,7 @@
     <row r="47" ht="130" customHeight="1">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
@@ -4072,7 +4072,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4147,7 +4147,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4222,7 +4222,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4297,7 +4297,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4372,7 +4372,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
@@ -4447,7 +4447,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4522,7 +4522,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4597,7 +4597,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4672,7 +4672,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4747,7 +4747,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4822,7 +4822,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4897,7 +4897,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -4977,7 +4977,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5060,7 +5060,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5140,7 +5140,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5220,7 +5220,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5300,7 +5300,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5380,7 +5380,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5454,7 +5454,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5528,7 +5528,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5602,7 +5602,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5676,7 +5676,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5750,7 +5750,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5823,7 +5823,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5896,7 +5896,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -5969,7 +5969,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6042,7 +6042,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6115,7 +6115,7 @@
     <row r="75" ht="130" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
@@ -6188,7 +6188,7 @@
     <row r="76" ht="130" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
@@ -6262,7 +6262,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6336,7 +6336,7 @@
     <row r="78" ht="130" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
@@ -6410,7 +6410,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6488,7 +6488,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6568,7 +6568,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6648,7 +6648,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B82" s="2" t="inlineStr">
@@ -6728,7 +6728,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B83" s="2" t="inlineStr">
@@ -6808,7 +6808,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B84" s="2" t="inlineStr">
@@ -6888,7 +6888,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B85" s="2" t="inlineStr">
@@ -6968,7 +6968,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -7048,7 +7048,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7128,7 +7128,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7208,7 +7208,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7288,7 +7288,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7368,7 +7368,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7444,7 +7444,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
@@ -7521,7 +7521,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
@@ -7601,7 +7601,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B94" s="2" t="inlineStr">
@@ -7681,7 +7681,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
@@ -7761,7 +7761,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7841,7 +7841,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7921,7 +7921,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8001,7 +8001,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8081,7 +8081,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8161,7 +8161,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8241,7 +8241,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8314,7 +8314,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AC-2 (4),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AC-2 (4),AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8395,7 +8395,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AC-2 (4),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AC-2 (4),AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8476,7 +8476,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AC-2 (4),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AC-2 (4),AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8547,7 +8547,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a)</t>
+          <t>AU-12 c,AC-2 (4),AU-3 (1),AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8622,7 +8622,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AC-2 (4),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AC-2 (4),AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8704,7 +8704,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AC-2 (4),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AC-2 (4),AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -8786,7 +8786,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AC-2 (4),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AC-2 (4),AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -8868,7 +8868,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AC-2 (4),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AC-2 (4),AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B110" s="2" t="inlineStr">
@@ -8950,7 +8950,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AC-2 (4),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AC-2 (4),AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9032,7 +9032,7 @@
     <row r="112" ht="130" customHeight="1">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-14 (1)</t>
+          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,AU-14 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
@@ -9124,7 +9124,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9205,7 +9205,7 @@
     <row r="114" ht="130" customHeight="1">
       <c r="A114" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B114" s="2" t="inlineStr">
@@ -9291,7 +9291,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-6 (10)</t>
+          <t>AC-6 (10),AC-11 b</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9369,7 +9369,7 @@
     <row r="116" ht="130" customHeight="1">
       <c r="A116" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B116" s="2" t="inlineStr">
@@ -9735,7 +9735,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -9806,7 +9806,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -9877,7 +9877,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-9</t>
+          <t>AU-9,AU-12 c</t>
         </is>
       </c>
       <c r="B122" s="2" t="inlineStr">
@@ -10250,7 +10250,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-6 (9),CM-5 (1),AC-2 (4)</t>
+          <t>CM-5 (1),AU-12 c,AC-2 (4),AC-6 (9)</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -10373,7 +10373,7 @@
     <row r="129" ht="130" customHeight="1">
       <c r="A129" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (b),CM-6 b,IA-5 (1) (a)</t>
+          <t>IA-5 (1) (a),IA-5 (1) (b),CM-6 b</t>
         </is>
       </c>
       <c r="B129" s="2" t="inlineStr">
@@ -10693,7 +10693,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),MA-4 c,SC-13,SC-8</t>
+          <t>SC-13,AC-17 (2),MA-4 c,SC-8</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10775,7 +10775,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>AC-12,MA-4 (7),SC-10,MA-4 e</t>
+          <t>SC-10,AC-12,MA-4 e,MA-4 (7)</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -10850,7 +10850,7 @@
     <row r="135" ht="130" customHeight="1">
       <c r="A135" s="2" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B135" s="2" t="inlineStr">
@@ -10929,7 +10929,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -11082,7 +11082,7 @@
     <row r="138" ht="130" customHeight="1">
       <c r="A138" s="2" t="inlineStr">
         <is>
-          <t>AU-6 (4),AU-7 a,AU-3,AU-7 (1),AU-12 a,CM-5 (1),AU-3 (1),MA-4 (1) (a),CM-6 b,AU-14 (1)</t>
+          <t>AU-7 (1),MA-4 (1) (a),CM-6 b,AU-7 a,AU-3 (1),AU-12 a,AU-3,CM-5 (1),AU-14 (1),AU-6 (4)</t>
         </is>
       </c>
       <c r="B138" s="2" t="inlineStr">
@@ -11484,7 +11484,7 @@
     <row r="143" ht="130" customHeight="1">
       <c r="A143" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B143" s="2" t="inlineStr">
@@ -11553,7 +11553,7 @@
     <row r="144" ht="130" customHeight="1">
       <c r="A144" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B144" s="2" t="inlineStr">
@@ -11622,7 +11622,7 @@
     <row r="145" ht="130" customHeight="1">
       <c r="A145" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B145" s="2" t="inlineStr">
@@ -11692,7 +11692,7 @@
     <row r="146" ht="130" customHeight="1">
       <c r="A146" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B146" s="2" t="inlineStr">
@@ -11761,7 +11761,7 @@
     <row r="147" ht="130" customHeight="1">
       <c r="A147" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B147" s="2" t="inlineStr">
@@ -11830,7 +11830,7 @@
     <row r="148" ht="130" customHeight="1">
       <c r="A148" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B148" s="2" t="inlineStr">
@@ -11900,7 +11900,7 @@
     <row r="149" ht="130" customHeight="1">
       <c r="A149" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B149" s="2" t="inlineStr">
@@ -11969,7 +11969,7 @@
     <row r="150" ht="130" customHeight="1">
       <c r="A150" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B150" s="2" t="inlineStr">
@@ -12038,7 +12038,7 @@
     <row r="151" ht="130" customHeight="1">
       <c r="A151" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B151" s="2" t="inlineStr">
@@ -12108,7 +12108,7 @@
     <row r="152" ht="130" customHeight="1">
       <c r="A152" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B152" s="2" t="inlineStr">
@@ -12177,7 +12177,7 @@
     <row r="153" ht="130" customHeight="1">
       <c r="A153" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B153" s="2" t="inlineStr">
@@ -12246,7 +12246,7 @@
     <row r="154" ht="130" customHeight="1">
       <c r="A154" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B154" s="2" t="inlineStr">
@@ -12315,7 +12315,7 @@
     <row r="155" ht="130" customHeight="1">
       <c r="A155" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B155" s="2" t="inlineStr">
@@ -13153,7 +13153,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (2),SC-8 (1)</t>
+          <t>SC-8 (2),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B166" s="2" t="inlineStr">
@@ -13306,7 +13306,7 @@
     <row r="168" ht="130" customHeight="1">
       <c r="A168" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2)</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B168" s="2" t="inlineStr">
@@ -13385,7 +13385,7 @@
     <row r="169" ht="130" customHeight="1">
       <c r="A169" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (2)</t>
+          <t>SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B169" s="2" t="inlineStr">
@@ -13609,7 +13609,7 @@
     <row r="172" ht="130" customHeight="1">
       <c r="A172" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B172" s="2" t="inlineStr">
@@ -13687,7 +13687,7 @@
     <row r="173" ht="130" customHeight="1">
       <c r="A173" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B173" s="2" t="inlineStr">
@@ -13770,7 +13770,7 @@
     <row r="174" ht="130" customHeight="1">
       <c r="A174" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B174" s="2" t="inlineStr">
@@ -14150,7 +14150,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="2" t="inlineStr">
         <is>
-          <t>AU-6 (4),CM-6 b,AU-4 (1)</t>
+          <t>AU-4 (1),AU-6 (4),CM-6 b</t>
         </is>
       </c>
       <c r="B179" s="2" t="inlineStr">
@@ -14221,7 +14221,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),CM-6 b,CM-7 b,AC-17 (9)</t>
+          <t>CM-7 b,AC-17 (9),AC-17 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B180" s="2" t="inlineStr">
@@ -14298,7 +14298,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),CM-6 b,CM-7 b</t>
+          <t>CM-7 b,AC-17 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">
@@ -15283,7 +15283,7 @@
     <row r="193" ht="130" customHeight="1">
       <c r="A193" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-3</t>
+          <t>AU-3,CM-6 b</t>
         </is>
       </c>
       <c r="B193" s="2" t="inlineStr">
@@ -15717,7 +15717,7 @@
     <row r="199" ht="130" customHeight="1">
       <c r="A199" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-4 (1)</t>
+          <t>AU-4 (1),AU-3</t>
         </is>
       </c>
       <c r="B199" s="2" t="inlineStr">
@@ -16232,7 +16232,7 @@
     <row r="206" ht="130" customHeight="1">
       <c r="A206" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-4 (1)</t>
+          <t>AU-4 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B206" s="2" t="inlineStr">
@@ -16312,7 +16312,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>SC-28,SC-28 (1)</t>
+          <t>SC-28 (1),SC-28</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -16626,7 +16626,7 @@
     <row r="211" ht="130" customHeight="1">
       <c r="A211" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B211" s="2" t="inlineStr">
@@ -16728,7 +16728,7 @@
     <row r="212" ht="130" customHeight="1">
       <c r="A212" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B212" s="2" t="inlineStr">
@@ -16838,7 +16838,7 @@
     <row r="213" ht="130" customHeight="1">
       <c r="A213" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B213" s="2" t="inlineStr">
@@ -16949,7 +16949,7 @@
     <row r="214" ht="130" customHeight="1">
       <c r="A214" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B214" s="2" t="inlineStr">
@@ -17058,7 +17058,7 @@
     <row r="215" ht="130" customHeight="1">
       <c r="A215" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-6 (9),AC-2 (4)</t>
+          <t>AU-12 c,AC-2 (4),AC-6 (9)</t>
         </is>
       </c>
       <c r="B215" s="2" t="inlineStr">
@@ -17500,7 +17500,7 @@
     <row r="220" ht="130" customHeight="1">
       <c r="A220" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (5)</t>
+          <t>IA-2 (5),CM-6 b</t>
         </is>
       </c>
       <c r="B220" s="2" t="inlineStr">
@@ -17578,7 +17578,7 @@
     <row r="221" ht="130" customHeight="1">
       <c r="A221" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (5),IA-2 (2),IA-2 (4),IA-2</t>
+          <t>IA-2 (5),IA-2 (2),IA-2,IA-2 (3),IA-2 (4)</t>
         </is>
       </c>
       <c r="B221" s="2" t="inlineStr">
@@ -17663,7 +17663,7 @@
     <row r="222" ht="130" customHeight="1">
       <c r="A222" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (5),IA-2 (2),IA-2 (4),IA-2</t>
+          <t>IA-2 (5),IA-2 (2),IA-2,IA-2 (3),IA-2 (4)</t>
         </is>
       </c>
       <c r="B222" s="2" t="inlineStr">
@@ -17748,7 +17748,7 @@
     <row r="223" ht="130" customHeight="1">
       <c r="A223" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-18 (1),SC-8 (1)</t>
+          <t>SC-8 (1),AC-18 (1),SC-8</t>
         </is>
       </c>
       <c r="B223" s="2" t="inlineStr">
@@ -17915,7 +17915,7 @@
     <row r="225" ht="130" customHeight="1">
       <c r="A225" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),IA-7</t>
+          <t>IA-7,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B225" s="2" t="inlineStr">
@@ -17998,7 +17998,7 @@
     <row r="226" ht="130" customHeight="1">
       <c r="A226" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B226" s="2" t="inlineStr">
@@ -18074,7 +18074,7 @@
     <row r="227" ht="130" customHeight="1">
       <c r="A227" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B227" s="2" t="inlineStr">
@@ -18159,7 +18159,7 @@
     <row r="228" ht="130" customHeight="1">
       <c r="A228" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B228" s="2" t="inlineStr">
@@ -18316,7 +18316,7 @@
     <row r="230" ht="130" customHeight="1">
       <c r="A230" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-7 a</t>
+          <t>CM-7 a,IA-7</t>
         </is>
       </c>
       <c r="B230" s="2" t="inlineStr">
@@ -19151,7 +19151,7 @@
     <row r="241" ht="130" customHeight="1">
       <c r="A241" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B241" s="2" t="inlineStr">
@@ -19229,7 +19229,7 @@
     <row r="242" ht="130" customHeight="1">
       <c r="A242" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B242" s="2" t="inlineStr">
@@ -19398,7 +19398,7 @@
     <row r="244" ht="130" customHeight="1">
       <c r="A244" s="2" t="inlineStr">
         <is>
-          <t>SI-16,SC-2,CM-6 b</t>
+          <t>SC-2,SI-16,CM-6 b</t>
         </is>
       </c>
       <c r="B244" s="2" t="inlineStr">
@@ -19558,7 +19558,7 @@
     <row r="246" ht="130" customHeight="1">
       <c r="A246" s="2" t="inlineStr">
         <is>
-          <t>SI-16,SC-3</t>
+          <t>SC-3,SI-16</t>
         </is>
       </c>
       <c r="B246" s="2" t="inlineStr">
@@ -21310,7 +21310,7 @@
     <row r="269" ht="130" customHeight="1">
       <c r="A269" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),CM-6 b</t>
+          <t>CM-6 b,IA-2 (2)</t>
         </is>
       </c>
       <c r="B269" s="2" t="inlineStr">
@@ -21397,7 +21397,7 @@
     <row r="270" ht="130" customHeight="1">
       <c r="A270" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (1),IA-2 (3),IA-2 (4)</t>
+          <t>IA-2 (3),IA-2 (4),IA-2 (1),IA-2 (2)</t>
         </is>
       </c>
       <c r="B270" s="2" t="inlineStr">
@@ -21566,7 +21566,7 @@
     <row r="272" ht="130" customHeight="1">
       <c r="A272" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B272" s="2" t="inlineStr">
@@ -21784,7 +21784,7 @@
     <row r="275" ht="130" customHeight="1">
       <c r="A275" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-4</t>
+          <t>SC-4,CM-6 b</t>
         </is>
       </c>
       <c r="B275" s="2" t="inlineStr">
@@ -21865,7 +21865,7 @@
     <row r="276" ht="130" customHeight="1">
       <c r="A276" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SC-4</t>
+          <t>SC-4,SC-2</t>
         </is>
       </c>
       <c r="B276" s="2" t="inlineStr">
@@ -21953,7 +21953,7 @@
     <row r="277" ht="130" customHeight="1">
       <c r="A277" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SC-4</t>
+          <t>SC-4,SC-2</t>
         </is>
       </c>
       <c r="B277" s="2" t="inlineStr">
@@ -23514,7 +23514,7 @@
     <row r="297" ht="130" customHeight="1">
       <c r="A297" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B297" s="2" t="inlineStr">
@@ -23683,7 +23683,7 @@
     <row r="299" ht="130" customHeight="1">
       <c r="A299" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (1),IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B299" s="2" t="inlineStr">
@@ -24505,7 +24505,7 @@
     <row r="309" ht="130" customHeight="1">
       <c r="A309" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (b),AU-8 (1) (a),AU-8 b</t>
+          <t>AU-8 b,AU-8 (1) (a),AU-8 (1) (b)</t>
         </is>
       </c>
       <c r="B309" s="2" t="inlineStr">
@@ -25996,7 +25996,7 @@
     <row r="328" ht="130" customHeight="1">
       <c r="A328" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,CM-5 (1)</t>
+          <t>CM-5 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B328" s="2" t="inlineStr">
@@ -27072,7 +27072,7 @@
     <row r="342" ht="130" customHeight="1">
       <c r="A342" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-7 b</t>
+          <t>CM-7 b,IA-3</t>
         </is>
       </c>
       <c r="B342" s="2" t="inlineStr">
@@ -27147,7 +27147,7 @@
     <row r="343" ht="130" customHeight="1">
       <c r="A343" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-7 a</t>
+          <t>CM-7 a,CM-7 b</t>
         </is>
       </c>
       <c r="B343" s="2" t="inlineStr">
@@ -27221,7 +27221,7 @@
     <row r="344" ht="130" customHeight="1">
       <c r="A344" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-7 a</t>
+          <t>CM-7 a,CM-7 b</t>
         </is>
       </c>
       <c r="B344" s="2" t="inlineStr">
@@ -27295,7 +27295,7 @@
     <row r="345" ht="130" customHeight="1">
       <c r="A345" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),CM-7 b</t>
+          <t>CM-7 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B345" s="2" t="inlineStr">
@@ -27381,7 +27381,7 @@
     <row r="346" ht="130" customHeight="1">
       <c r="A346" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),CM-7 a</t>
+          <t>CM-7 a,AC-18 (1)</t>
         </is>
       </c>
       <c r="B346" s="2" t="inlineStr">
@@ -27458,7 +27458,7 @@
     <row r="347" ht="130" customHeight="1">
       <c r="A347" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-6 b,CM-7 a</t>
+          <t>CM-7 a,IA-5 (1) (c),CM-6 b</t>
         </is>
       </c>
       <c r="B347" s="2" t="inlineStr">
@@ -28552,7 +28552,7 @@
     <row r="361" ht="130" customHeight="1">
       <c r="A361" s="2" t="inlineStr">
         <is>
-          <t>SI-6 d,SI-6 b,CM-3 (5)</t>
+          <t>SI-6 b,CM-3 (5),SI-6 d</t>
         </is>
       </c>
       <c r="B361" s="2" t="inlineStr">
@@ -28643,7 +28643,7 @@
     <row r="362" ht="130" customHeight="1">
       <c r="A362" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B362" s="2" t="inlineStr">
@@ -29023,7 +29023,7 @@
     <row r="367" ht="130" customHeight="1">
       <c r="A367" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-7 a</t>
+          <t>CM-7 a,SI-16</t>
         </is>
       </c>
       <c r="B367" s="2" t="inlineStr">
@@ -29572,7 +29572,7 @@
     <row r="374" ht="130" customHeight="1">
       <c r="A374" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B374" s="2" t="inlineStr">
@@ -29643,7 +29643,7 @@
     <row r="375" ht="130" customHeight="1">
       <c r="A375" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B375" s="2" t="inlineStr">
@@ -29715,7 +29715,7 @@
     <row r="376" ht="130" customHeight="1">
       <c r="A376" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B376" s="2" t="inlineStr">
@@ -30923,7 +30923,7 @@
     <row r="391" ht="130" customHeight="1">
       <c r="A391" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (a)</t>
+          <t>IA-5 (1) (a),CM-6 b</t>
         </is>
       </c>
       <c r="B391" s="2" t="inlineStr">
@@ -31405,7 +31405,7 @@
     <row r="397" ht="130" customHeight="1">
       <c r="A397" s="2" t="inlineStr">
         <is>
-          <t>SI-6 d,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 d</t>
         </is>
       </c>
       <c r="B397" s="2" t="inlineStr">
@@ -31737,7 +31737,7 @@
     <row r="401" ht="130" customHeight="1">
       <c r="A401" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B401" s="2" t="inlineStr">
@@ -31828,7 +31828,7 @@
     <row r="402" ht="130" customHeight="1">
       <c r="A402" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B402" s="2" t="inlineStr">
@@ -31922,7 +31922,7 @@
     <row r="403" ht="130" customHeight="1">
       <c r="A403" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B403" s="2" t="inlineStr">
@@ -35482,7 +35482,7 @@
     <row r="450" ht="130" customHeight="1">
       <c r="A450" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (1)</t>
+          <t>CM-5 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B450" s="2" t="inlineStr">
@@ -35555,7 +35555,7 @@
     <row r="451" ht="130" customHeight="1">
       <c r="A451" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (1)</t>
+          <t>CM-5 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B451" s="2" t="inlineStr">
@@ -36690,7 +36690,7 @@
       </c>
       <c r="H466" s="2" t="inlineStr">
         <is>
-          <t>Using interactive boot, the console user could disable auditing, firewalls,
+          <t>Using interactive or recovery boot, the console user could disable auditing, firewalls,
 or other services, weakening system security.</t>
         </is>
       </c>
@@ -36709,7 +36709,8 @@
           <t>Inspect  /etc/default/grub  for any instances of
  systemd.confirm_spawn=(1|yes|true|on)  in the kernel boot arguments.
 Presence of a  systemd.confirm_spawn=(1|yes|true|on)  indicates
-that interactive boot is enabled at boot time.
+that interactive boot is enabled at boot time and verify that
+ GRUB_DISABLE_RECOVERY=true  to disable recovery boot.
 If Interactive boot is enabled at boot time then this is a finding.</t>
         </is>
       </c>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@51bde53b768a42fb6bb80f58b72ea0ce12ef0dbb 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -708,7 +708,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>AU-4,CM-6 b</t>
+          <t>CM-6 b,AU-4</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -784,7 +784,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>SC-5 (2),SC-5,CM-6 b</t>
+          <t>CM-6 b,SC-5 (2),SC-5</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -883,7 +883,7 @@
     <row r="6" ht="130" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>AU-12 (3),AU-7 a,AC-6 (9),AU-8 b,CM-5 (1),AU-7 b,AC-6 (8)</t>
+          <t>AU-7 a,AC-6 (9),CM-5 (1),AC-6 (8),AU-8 b,AU-12 (3),AU-7 b</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -963,7 +963,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-12 (3),AU-12 c,CM-6 b,AU-7 a,AU-8 b,AU-12 a,CM-5 (1),AU-7 b</t>
+          <t>AU-7 a,CM-5 (1),AU-12 c,AU-12 a,AU-8 b,CM-6 b,AU-12 (3),AU-7 b</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1269,7 +1269,7 @@
     <row r="11" ht="130" customHeight="1">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B11" s="2" t="inlineStr">
@@ -1346,7 +1346,7 @@
     <row r="12" ht="130" customHeight="1">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
@@ -1496,7 +1496,7 @@
     <row r="14" ht="130" customHeight="1">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -1572,7 +1572,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1726,7 +1726,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -2096,7 +2096,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -2170,7 +2170,7 @@
     <row r="23" ht="130" customHeight="1">
       <c r="A23" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B23" s="2" t="inlineStr">
@@ -3922,7 +3922,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -3997,7 +3997,7 @@
     <row r="47" ht="130" customHeight="1">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
@@ -4072,7 +4072,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4147,7 +4147,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4222,7 +4222,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4297,7 +4297,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4372,7 +4372,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
@@ -4447,7 +4447,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4522,7 +4522,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4597,7 +4597,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4672,7 +4672,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4747,7 +4747,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4822,7 +4822,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4897,7 +4897,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -4977,7 +4977,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5060,7 +5060,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5140,7 +5140,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5220,7 +5220,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5300,7 +5300,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5380,7 +5380,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5454,7 +5454,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5528,7 +5528,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5602,7 +5602,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5676,7 +5676,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5750,7 +5750,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5823,7 +5823,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5896,7 +5896,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -5969,7 +5969,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6042,7 +6042,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6115,7 +6115,7 @@
     <row r="75" ht="130" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
@@ -6188,7 +6188,7 @@
     <row r="76" ht="130" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
@@ -6262,7 +6262,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6336,7 +6336,7 @@
     <row r="78" ht="130" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
@@ -6410,7 +6410,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6488,7 +6488,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6568,7 +6568,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6648,7 +6648,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B82" s="2" t="inlineStr">
@@ -6728,7 +6728,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B83" s="2" t="inlineStr">
@@ -6808,7 +6808,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B84" s="2" t="inlineStr">
@@ -6888,7 +6888,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B85" s="2" t="inlineStr">
@@ -6968,7 +6968,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -7048,7 +7048,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7128,7 +7128,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7208,7 +7208,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7288,7 +7288,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7368,7 +7368,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7444,7 +7444,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
@@ -7521,7 +7521,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
@@ -7601,7 +7601,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B94" s="2" t="inlineStr">
@@ -7681,7 +7681,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
@@ -7761,7 +7761,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7841,7 +7841,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7921,7 +7921,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8001,7 +8001,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8081,7 +8081,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8161,7 +8161,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8241,7 +8241,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8314,7 +8314,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-2 (4),AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AC-2 (4),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8395,7 +8395,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-2 (4),AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AC-2 (4),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8476,7 +8476,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-2 (4),AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AC-2 (4),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8547,7 +8547,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-2 (4),AU-3 (1),AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8622,7 +8622,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-2 (4),AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AC-2 (4),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8704,7 +8704,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-2 (4),AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AC-2 (4),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -8786,7 +8786,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-2 (4),AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AC-2 (4),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -8868,7 +8868,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-2 (4),AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AC-2 (4),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B110" s="2" t="inlineStr">
@@ -8950,7 +8950,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-2 (4),AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AC-2 (4),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9032,7 +9032,7 @@
     <row r="112" ht="130" customHeight="1">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,AU-14 (1),MA-4 (1) (a)</t>
+          <t>AU-14 (1),MA-4 (1) (a),AU-12 c,AU-12 a,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
@@ -9124,7 +9124,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9205,7 +9205,7 @@
     <row r="114" ht="130" customHeight="1">
       <c r="A114" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B114" s="2" t="inlineStr">
@@ -9369,7 +9369,7 @@
     <row r="116" ht="130" customHeight="1">
       <c r="A116" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B116" s="2" t="inlineStr">
@@ -9735,7 +9735,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -9806,7 +9806,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -10250,7 +10250,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AU-12 c,AC-2 (4),AC-6 (9)</t>
+          <t>CM-5 (1),AC-6 (9),AU-12 c,AC-2 (4)</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -10373,7 +10373,7 @@
     <row r="129" ht="130" customHeight="1">
       <c r="A129" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (a),IA-5 (1) (b),CM-6 b</t>
+          <t>IA-5 (1) (b),CM-6 b,IA-5 (1) (a)</t>
         </is>
       </c>
       <c r="B129" s="2" t="inlineStr">
@@ -10693,7 +10693,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>SC-13,AC-17 (2),MA-4 c,SC-8</t>
+          <t>AC-17 (2),MA-4 c,SC-13,SC-8</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10775,7 +10775,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>SC-10,AC-12,MA-4 e,MA-4 (7)</t>
+          <t>SC-10,MA-4 e,MA-4 (7),AC-12</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -11082,7 +11082,7 @@
     <row r="138" ht="130" customHeight="1">
       <c r="A138" s="2" t="inlineStr">
         <is>
-          <t>AU-7 (1),MA-4 (1) (a),CM-6 b,AU-7 a,AU-3 (1),AU-12 a,AU-3,CM-5 (1),AU-14 (1),AU-6 (4)</t>
+          <t>AU-14 (1),AU-7 a,MA-4 (1) (a),CM-5 (1),AU-12 a,AU-3 (1),AU-3,AU-6 (4),AU-7 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B138" s="2" t="inlineStr">
@@ -11332,7 +11332,7 @@
     <row r="141" ht="130" customHeight="1">
       <c r="A141" s="2" t="inlineStr">
         <is>
-          <t>AU-9 (3),AU-9</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B141" s="2" t="inlineStr">
@@ -11408,7 +11408,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="2" t="inlineStr">
         <is>
-          <t>AU-9 (3),AU-9</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B142" s="2" t="inlineStr">
@@ -13153,7 +13153,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8 (1),SC-8</t>
+          <t>SC-8 (1),SC-8,SC-8 (2)</t>
         </is>
       </c>
       <c r="B166" s="2" t="inlineStr">
@@ -13385,7 +13385,7 @@
     <row r="169" ht="130" customHeight="1">
       <c r="A169" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8</t>
+          <t>SC-8,SC-8 (2)</t>
         </is>
       </c>
       <c r="B169" s="2" t="inlineStr">
@@ -13609,7 +13609,7 @@
     <row r="172" ht="130" customHeight="1">
       <c r="A172" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B172" s="2" t="inlineStr">
@@ -13687,7 +13687,7 @@
     <row r="173" ht="130" customHeight="1">
       <c r="A173" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B173" s="2" t="inlineStr">
@@ -13770,7 +13770,7 @@
     <row r="174" ht="130" customHeight="1">
       <c r="A174" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B174" s="2" t="inlineStr">
@@ -14150,7 +14150,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-6 (4),CM-6 b</t>
+          <t>CM-6 b,AU-6 (4),AU-4 (1)</t>
         </is>
       </c>
       <c r="B179" s="2" t="inlineStr">
@@ -14221,7 +14221,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (9),AC-17 (1),CM-6 b</t>
+          <t>AC-17 (9),CM-6 b,AC-17 (1),CM-7 b</t>
         </is>
       </c>
       <c r="B180" s="2" t="inlineStr">
@@ -14298,7 +14298,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (1),CM-6 b</t>
+          <t>CM-6 b,AC-17 (1),CM-7 b</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">
@@ -14377,7 +14377,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B182" s="2" t="inlineStr">
@@ -14460,7 +14460,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B183" s="2" t="inlineStr">
@@ -14538,7 +14538,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B184" s="2" t="inlineStr">
@@ -14629,7 +14629,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B185" s="2" t="inlineStr">
@@ -14711,7 +14711,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B186" s="2" t="inlineStr">
@@ -15283,7 +15283,7 @@
     <row r="193" ht="130" customHeight="1">
       <c r="A193" s="2" t="inlineStr">
         <is>
-          <t>AU-3,CM-6 b</t>
+          <t>CM-6 b,AU-3</t>
         </is>
       </c>
       <c r="B193" s="2" t="inlineStr">
@@ -15717,7 +15717,7 @@
     <row r="199" ht="130" customHeight="1">
       <c r="A199" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-3</t>
+          <t>AU-3,AU-4 (1)</t>
         </is>
       </c>
       <c r="B199" s="2" t="inlineStr">
@@ -16232,7 +16232,7 @@
     <row r="206" ht="130" customHeight="1">
       <c r="A206" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),CM-6 b</t>
+          <t>CM-6 b,AU-4 (1)</t>
         </is>
       </c>
       <c r="B206" s="2" t="inlineStr">
@@ -16312,7 +16312,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>SC-28 (1),SC-28</t>
+          <t>SC-28,SC-28 (1)</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -16626,7 +16626,7 @@
     <row r="211" ht="130" customHeight="1">
       <c r="A211" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B211" s="2" t="inlineStr">
@@ -16728,7 +16728,7 @@
     <row r="212" ht="130" customHeight="1">
       <c r="A212" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B212" s="2" t="inlineStr">
@@ -16838,7 +16838,7 @@
     <row r="213" ht="130" customHeight="1">
       <c r="A213" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B213" s="2" t="inlineStr">
@@ -16949,7 +16949,7 @@
     <row r="214" ht="130" customHeight="1">
       <c r="A214" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B214" s="2" t="inlineStr">
@@ -17058,7 +17058,7 @@
     <row r="215" ht="130" customHeight="1">
       <c r="A215" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-2 (4),AC-6 (9)</t>
+          <t>AC-6 (9),AU-12 c,AC-2 (4)</t>
         </is>
       </c>
       <c r="B215" s="2" t="inlineStr">
@@ -17578,7 +17578,7 @@
     <row r="221" ht="130" customHeight="1">
       <c r="A221" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),IA-2 (2),IA-2,IA-2 (3),IA-2 (4)</t>
+          <t>IA-2,IA-2 (5),IA-2 (3),IA-2 (4),IA-2 (2)</t>
         </is>
       </c>
       <c r="B221" s="2" t="inlineStr">
@@ -17663,7 +17663,7 @@
     <row r="222" ht="130" customHeight="1">
       <c r="A222" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),IA-2 (2),IA-2,IA-2 (3),IA-2 (4)</t>
+          <t>IA-2,IA-2 (5),IA-2 (3),IA-2 (4),IA-2 (2)</t>
         </is>
       </c>
       <c r="B222" s="2" t="inlineStr">
@@ -17748,7 +17748,7 @@
     <row r="223" ht="130" customHeight="1">
       <c r="A223" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),AC-18 (1),SC-8</t>
+          <t>AC-18 (1),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B223" s="2" t="inlineStr">
@@ -17915,7 +17915,7 @@
     <row r="225" ht="130" customHeight="1">
       <c r="A225" s="2" t="inlineStr">
         <is>
-          <t>IA-7,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),IA-7</t>
         </is>
       </c>
       <c r="B225" s="2" t="inlineStr">
@@ -17998,7 +17998,7 @@
     <row r="226" ht="130" customHeight="1">
       <c r="A226" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B226" s="2" t="inlineStr">
@@ -18074,7 +18074,7 @@
     <row r="227" ht="130" customHeight="1">
       <c r="A227" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B227" s="2" t="inlineStr">
@@ -18159,7 +18159,7 @@
     <row r="228" ht="130" customHeight="1">
       <c r="A228" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B228" s="2" t="inlineStr">
@@ -18316,7 +18316,7 @@
     <row r="230" ht="130" customHeight="1">
       <c r="A230" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,IA-7</t>
+          <t>IA-7,CM-7 a</t>
         </is>
       </c>
       <c r="B230" s="2" t="inlineStr">
@@ -19151,7 +19151,7 @@
     <row r="241" ht="130" customHeight="1">
       <c r="A241" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B241" s="2" t="inlineStr">
@@ -19229,7 +19229,7 @@
     <row r="242" ht="130" customHeight="1">
       <c r="A242" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B242" s="2" t="inlineStr">
@@ -19398,7 +19398,7 @@
     <row r="244" ht="130" customHeight="1">
       <c r="A244" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SI-16,CM-6 b</t>
+          <t>CM-6 b,SI-16,SC-2</t>
         </is>
       </c>
       <c r="B244" s="2" t="inlineStr">
@@ -19558,7 +19558,7 @@
     <row r="246" ht="130" customHeight="1">
       <c r="A246" s="2" t="inlineStr">
         <is>
-          <t>SC-3,SI-16</t>
+          <t>SI-16,SC-3</t>
         </is>
       </c>
       <c r="B246" s="2" t="inlineStr">
@@ -20472,7 +20472,7 @@
     <row r="258" ht="130" customHeight="1">
       <c r="A258" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B258" s="2" t="inlineStr">
@@ -20547,7 +20547,7 @@
     <row r="259" ht="130" customHeight="1">
       <c r="A259" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B259" s="2" t="inlineStr">
@@ -20635,7 +20635,7 @@
     <row r="260" ht="130" customHeight="1">
       <c r="A260" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B260" s="2" t="inlineStr">
@@ -20712,7 +20712,7 @@
     <row r="261" ht="130" customHeight="1">
       <c r="A261" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B261" s="2" t="inlineStr">
@@ -21397,7 +21397,7 @@
     <row r="270" ht="130" customHeight="1">
       <c r="A270" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (4),IA-2 (1),IA-2 (2)</t>
+          <t>IA-2 (2),IA-2 (1),IA-2 (4),IA-2 (3)</t>
         </is>
       </c>
       <c r="B270" s="2" t="inlineStr">
@@ -21566,7 +21566,7 @@
     <row r="272" ht="130" customHeight="1">
       <c r="A272" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B272" s="2" t="inlineStr">
@@ -21784,7 +21784,7 @@
     <row r="275" ht="130" customHeight="1">
       <c r="A275" s="2" t="inlineStr">
         <is>
-          <t>SC-4,CM-6 b</t>
+          <t>CM-6 b,SC-4</t>
         </is>
       </c>
       <c r="B275" s="2" t="inlineStr">
@@ -22191,7 +22191,7 @@
     <row r="280" ht="130" customHeight="1">
       <c r="A280" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,CM-6 b</t>
+          <t>CM-6 b,AU-12 a</t>
         </is>
       </c>
       <c r="B280" s="2" t="inlineStr">
@@ -22414,7 +22414,7 @@
     <row r="283" ht="130" customHeight="1">
       <c r="A283" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (3),CM-6 b</t>
+          <t>CM-6 b,CM-5 (3)</t>
         </is>
       </c>
       <c r="B283" s="2" t="inlineStr">
@@ -23514,7 +23514,7 @@
     <row r="297" ht="130" customHeight="1">
       <c r="A297" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B297" s="2" t="inlineStr">
@@ -23683,7 +23683,7 @@
     <row r="299" ht="130" customHeight="1">
       <c r="A299" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (1),IA-2 (11)</t>
         </is>
       </c>
       <c r="B299" s="2" t="inlineStr">
@@ -24505,7 +24505,7 @@
     <row r="309" ht="130" customHeight="1">
       <c r="A309" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-8 (1) (a),AU-8 (1) (b)</t>
+          <t>AU-8 (1) (a),AU-8 b,AU-8 (1) (b)</t>
         </is>
       </c>
       <c r="B309" s="2" t="inlineStr">
@@ -25532,7 +25532,7 @@
     <row r="322" ht="130" customHeight="1">
       <c r="A322" s="2" t="inlineStr">
         <is>
-          <t>IA-11,AC-3 (4)</t>
+          <t>AC-3 (4),IA-11</t>
         </is>
       </c>
       <c r="B322" s="2" t="inlineStr">
@@ -27072,7 +27072,7 @@
     <row r="342" ht="130" customHeight="1">
       <c r="A342" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,IA-3</t>
+          <t>IA-3,CM-7 b</t>
         </is>
       </c>
       <c r="B342" s="2" t="inlineStr">
@@ -27295,7 +27295,7 @@
     <row r="345" ht="130" customHeight="1">
       <c r="A345" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (1)</t>
+          <t>AC-17 (1),CM-7 b</t>
         </is>
       </c>
       <c r="B345" s="2" t="inlineStr">
@@ -27381,7 +27381,7 @@
     <row r="346" ht="130" customHeight="1">
       <c r="A346" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,AC-18 (1)</t>
+          <t>AC-18 (1),CM-7 a</t>
         </is>
       </c>
       <c r="B346" s="2" t="inlineStr">
@@ -27458,7 +27458,7 @@
     <row r="347" ht="130" customHeight="1">
       <c r="A347" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,IA-5 (1) (c),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (c),CM-7 a</t>
         </is>
       </c>
       <c r="B347" s="2" t="inlineStr">
@@ -28303,7 +28303,7 @@
     <row r="358" ht="130" customHeight="1">
       <c r="A358" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 (1)</t>
+          <t>AC-11 (1),AC-11 b</t>
         </is>
       </c>
       <c r="B358" s="2" t="inlineStr">
@@ -28552,7 +28552,7 @@
     <row r="361" ht="130" customHeight="1">
       <c r="A361" s="2" t="inlineStr">
         <is>
-          <t>SI-6 b,CM-3 (5),SI-6 d</t>
+          <t>CM-3 (5),SI-6 b,SI-6 d</t>
         </is>
       </c>
       <c r="B361" s="2" t="inlineStr">
@@ -28643,7 +28643,7 @@
     <row r="362" ht="130" customHeight="1">
       <c r="A362" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B362" s="2" t="inlineStr">
@@ -29023,7 +29023,7 @@
     <row r="367" ht="130" customHeight="1">
       <c r="A367" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,SI-16</t>
+          <t>SI-16,CM-7 a</t>
         </is>
       </c>
       <c r="B367" s="2" t="inlineStr">
@@ -29572,7 +29572,7 @@
     <row r="374" ht="130" customHeight="1">
       <c r="A374" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B374" s="2" t="inlineStr">
@@ -29643,7 +29643,7 @@
     <row r="375" ht="130" customHeight="1">
       <c r="A375" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B375" s="2" t="inlineStr">
@@ -29715,7 +29715,7 @@
     <row r="376" ht="130" customHeight="1">
       <c r="A376" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B376" s="2" t="inlineStr">
@@ -30475,7 +30475,7 @@
     <row r="385" ht="130" customHeight="1">
       <c r="A385" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),CM-6 b</t>
+          <t>CM-6 b,AC-17 (2)</t>
         </is>
       </c>
       <c r="B385" s="2" t="inlineStr">
@@ -30784,7 +30784,7 @@
     <row r="389" ht="130" customHeight="1">
       <c r="A389" s="2" t="inlineStr">
         <is>
-          <t>SC-3,SI-6 a</t>
+          <t>SI-6 a,SC-3</t>
         </is>
       </c>
       <c r="B389" s="2" t="inlineStr">
@@ -30923,7 +30923,7 @@
     <row r="391" ht="130" customHeight="1">
       <c r="A391" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (a),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (a)</t>
         </is>
       </c>
       <c r="B391" s="2" t="inlineStr">
@@ -31489,7 +31489,7 @@
     <row r="398" ht="130" customHeight="1">
       <c r="A398" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-6 b</t>
+          <t>CM-6 b,SI-16</t>
         </is>
       </c>
       <c r="B398" s="2" t="inlineStr">
@@ -31737,7 +31737,7 @@
     <row r="401" ht="130" customHeight="1">
       <c r="A401" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B401" s="2" t="inlineStr">
@@ -31828,7 +31828,7 @@
     <row r="402" ht="130" customHeight="1">
       <c r="A402" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B402" s="2" t="inlineStr">
@@ -31922,7 +31922,7 @@
     <row r="403" ht="130" customHeight="1">
       <c r="A403" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B403" s="2" t="inlineStr">
@@ -35332,7 +35332,7 @@
     <row r="448" ht="130" customHeight="1">
       <c r="A448" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B448" s="2" t="inlineStr">
@@ -35482,7 +35482,7 @@
     <row r="450" ht="130" customHeight="1">
       <c r="A450" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),CM-6 b</t>
+          <t>CM-6 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B450" s="2" t="inlineStr">
@@ -35555,7 +35555,7 @@
     <row r="451" ht="130" customHeight="1">
       <c r="A451" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),CM-6 b</t>
+          <t>CM-6 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B451" s="2" t="inlineStr">
@@ -41367,7 +41367,7 @@
     <row r="524" ht="130" customHeight="1">
       <c r="A524" s="2" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b</t>
+          <t>CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B524" s="2" t="inlineStr">
@@ -41454,7 +41454,7 @@
     <row r="525" ht="130" customHeight="1">
       <c r="A525" s="2" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b</t>
+          <t>CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B525" s="2" t="inlineStr">
@@ -42686,7 +42686,7 @@
     <row r="541" ht="130" customHeight="1">
       <c r="A541" s="2" t="inlineStr">
         <is>
-          <t>SI-2 (2),CM-6 b</t>
+          <t>CM-6 b,SI-2 (2)</t>
         </is>
       </c>
       <c r="B541" s="2" t="inlineStr">
@@ -43333,7 +43333,7 @@
     <row r="550" ht="130" customHeight="1">
       <c r="A550" s="2" t="inlineStr">
         <is>
-          <t>SI-2 (2),CM-6 b</t>
+          <t>CM-6 b,SI-2 (2)</t>
         </is>
       </c>
       <c r="B550" s="2" t="inlineStr">
@@ -43941,7 +43941,7 @@
     <row r="558" ht="130" customHeight="1">
       <c r="A558" s="2" t="inlineStr">
         <is>
-          <t>SI-6 a,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 a</t>
         </is>
       </c>
       <c r="B558" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@3be457d4e63a9f3a6f4980cd98861bc5cb46620e 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -541,7 +541,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-4 (1)</t>
+          <t>AU-4 (1),AU-4</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -625,7 +625,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),AU-4</t>
+          <t>AU-4,AU-14 (1)</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -708,7 +708,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>AU-4,CM-6 b</t>
+          <t>CM-6 b,AU-4</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -784,7 +784,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>SC-5 (2),CM-6 b,SC-5</t>
+          <t>CM-6 b,SC-5 (2),SC-5</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -883,7 +883,7 @@
     <row r="6" ht="130" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,CM-5 (1),AC-6 (9),AU-7 b,AU-7 a,AC-6 (8),AU-12 (3)</t>
+          <t>AU-8 b,AU-7 a,AC-6 (8),AU-7 b,AU-12 (3),CM-5 (1),AC-6 (9)</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -963,7 +963,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,CM-6 b,AU-7 b,AU-12 (3),AU-7 a,AU-12 c,AU-12 a,CM-5 (1)</t>
+          <t>AU-12 c,AU-8 b,AU-7 a,CM-6 b,AU-7 b,AU-12 (3),CM-5 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1269,7 +1269,7 @@
     <row r="11" ht="130" customHeight="1">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B11" s="2" t="inlineStr">
@@ -1650,7 +1650,7 @@
     <row r="16" ht="130" customHeight="1">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
@@ -2020,7 +2020,7 @@
     <row r="21" ht="130" customHeight="1">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
@@ -2094,7 +2094,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -3222,7 +3222,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3306,7 +3306,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3391,7 +3391,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3463,7 +3463,7 @@
     <row r="40" ht="130" customHeight="1">
       <c r="A40" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B40" s="2" t="inlineStr">
@@ -3846,7 +3846,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3921,7 +3921,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -3996,7 +3996,7 @@
     <row r="47" ht="130" customHeight="1">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
@@ -4071,7 +4071,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4146,7 +4146,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4221,7 +4221,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4296,7 +4296,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4371,7 +4371,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
@@ -4446,7 +4446,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4521,7 +4521,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4596,7 +4596,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4671,7 +4671,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4746,7 +4746,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4821,7 +4821,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4901,7 +4901,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -4984,7 +4984,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5064,7 +5064,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5144,7 +5144,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5224,7 +5224,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5304,7 +5304,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5378,7 +5378,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5452,7 +5452,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5526,7 +5526,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5600,7 +5600,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5674,7 +5674,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5747,7 +5747,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5820,7 +5820,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5893,7 +5893,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -5966,7 +5966,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6039,7 +6039,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6112,7 +6112,7 @@
     <row r="75" ht="130" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
@@ -6186,7 +6186,7 @@
     <row r="76" ht="130" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
@@ -6260,7 +6260,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6334,7 +6334,7 @@
     <row r="78" ht="130" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
@@ -6412,7 +6412,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6492,7 +6492,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6572,7 +6572,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6652,7 +6652,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B82" s="2" t="inlineStr">
@@ -6732,7 +6732,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B83" s="2" t="inlineStr">
@@ -6812,7 +6812,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B84" s="2" t="inlineStr">
@@ -6892,7 +6892,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B85" s="2" t="inlineStr">
@@ -6972,7 +6972,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -7052,7 +7052,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7132,7 +7132,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7212,7 +7212,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7292,7 +7292,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7368,7 +7368,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7445,7 +7445,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
@@ -7525,7 +7525,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
@@ -7605,7 +7605,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B94" s="2" t="inlineStr">
@@ -7685,7 +7685,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
@@ -7765,7 +7765,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7845,7 +7845,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7925,7 +7925,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8005,7 +8005,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8085,7 +8085,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8165,7 +8165,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8238,7 +8238,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AC-2 (4),AU-12 a</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8319,7 +8319,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AC-2 (4),AU-12 a</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8400,7 +8400,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AC-2 (4),AU-12 a</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8471,7 +8471,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AC-2 (4)</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8546,7 +8546,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AC-2 (4),AU-12 a</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8628,7 +8628,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AC-2 (4),AU-12 a</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8710,7 +8710,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AC-2 (4),AU-12 a</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -8792,7 +8792,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AC-2 (4),AU-12 a</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -8874,7 +8874,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a),AC-2 (4),AU-12 a</t>
         </is>
       </c>
       <c r="B110" s="2" t="inlineStr">
@@ -8956,7 +8956,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-14 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),AU-14 (1),AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9659,7 +9659,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9730,7 +9730,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -10174,7 +10174,7 @@
     <row r="126" ht="130" customHeight="1">
       <c r="A126" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 c,CM-5 (1),AC-6 (9)</t>
+          <t>AC-6 (9),AC-2 (4),CM-5 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B126" s="2" t="inlineStr">
@@ -10297,7 +10297,7 @@
     <row r="128" ht="130" customHeight="1">
       <c r="A128" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (b),IA-5 (1) (a),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (b),IA-5 (1) (a)</t>
         </is>
       </c>
       <c r="B128" s="2" t="inlineStr">
@@ -10617,7 +10617,7 @@
     <row r="132" ht="130" customHeight="1">
       <c r="A132" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8,SC-13,MA-4 c</t>
+          <t>AC-17 (2),SC-13,MA-4 c,SC-8</t>
         </is>
       </c>
       <c r="B132" s="2" t="inlineStr">
@@ -10699,7 +10699,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>MA-4 e,SC-10,AC-12,MA-4 (7)</t>
+          <t>MA-4 (7),AC-12,SC-10,MA-4 e</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10774,7 +10774,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>SC-10,AC-12</t>
+          <t>AC-12,SC-10</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -10853,7 +10853,7 @@
     <row r="135" ht="130" customHeight="1">
       <c r="A135" s="2" t="inlineStr">
         <is>
-          <t>SC-10,AC-12</t>
+          <t>AC-12,SC-10</t>
         </is>
       </c>
       <c r="B135" s="2" t="inlineStr">
@@ -11006,7 +11006,7 @@
     <row r="137" ht="130" customHeight="1">
       <c r="A137" s="2" t="inlineStr">
         <is>
-          <t>AU-6 (4),CM-6 b,AU-7 (1),AU-3,AU-7 a,AU-3 (1),AU-14 (1),AU-12 a,MA-4 (1) (a),CM-5 (1)</t>
+          <t>AU-7 a,AU-3 (1),AU-7 (1),AU-14 (1),CM-6 b,AU-3,MA-4 (1) (a),CM-5 (1),AU-12 a,AU-6 (4)</t>
         </is>
       </c>
       <c r="B137" s="2" t="inlineStr">
@@ -11256,7 +11256,7 @@
     <row r="140" ht="130" customHeight="1">
       <c r="A140" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B140" s="2" t="inlineStr">
@@ -11332,7 +11332,7 @@
     <row r="141" ht="130" customHeight="1">
       <c r="A141" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B141" s="2" t="inlineStr">
@@ -11408,7 +11408,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B142" s="2" t="inlineStr">
@@ -11477,7 +11477,7 @@
     <row r="143" ht="130" customHeight="1">
       <c r="A143" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B143" s="2" t="inlineStr">
@@ -11546,7 +11546,7 @@
     <row r="144" ht="130" customHeight="1">
       <c r="A144" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B144" s="2" t="inlineStr">
@@ -11616,7 +11616,7 @@
     <row r="145" ht="130" customHeight="1">
       <c r="A145" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B145" s="2" t="inlineStr">
@@ -11685,7 +11685,7 @@
     <row r="146" ht="130" customHeight="1">
       <c r="A146" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B146" s="2" t="inlineStr">
@@ -11754,7 +11754,7 @@
     <row r="147" ht="130" customHeight="1">
       <c r="A147" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B147" s="2" t="inlineStr">
@@ -11824,7 +11824,7 @@
     <row r="148" ht="130" customHeight="1">
       <c r="A148" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B148" s="2" t="inlineStr">
@@ -11893,7 +11893,7 @@
     <row r="149" ht="130" customHeight="1">
       <c r="A149" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B149" s="2" t="inlineStr">
@@ -11962,7 +11962,7 @@
     <row r="150" ht="130" customHeight="1">
       <c r="A150" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B150" s="2" t="inlineStr">
@@ -12032,7 +12032,7 @@
     <row r="151" ht="130" customHeight="1">
       <c r="A151" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B151" s="2" t="inlineStr">
@@ -12101,7 +12101,7 @@
     <row r="152" ht="130" customHeight="1">
       <c r="A152" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B152" s="2" t="inlineStr">
@@ -12170,7 +12170,7 @@
     <row r="153" ht="130" customHeight="1">
       <c r="A153" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B153" s="2" t="inlineStr">
@@ -12239,7 +12239,7 @@
     <row r="154" ht="130" customHeight="1">
       <c r="A154" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B154" s="2" t="inlineStr">
@@ -13077,7 +13077,7 @@
     <row r="165" ht="130" customHeight="1">
       <c r="A165" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8,SC-8 (1)</t>
+          <t>SC-8 (2),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B165" s="2" t="inlineStr">
@@ -13154,7 +13154,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8,SC-8 (1)</t>
+          <t>SC-8 (2),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B166" s="2" t="inlineStr">
@@ -13374,14 +13374,21 @@
         <is>
           <t>To verify that BIND uses the system crypto policy, check out that the BIND config file
  /etc/named.conf  contains the  include "/etc/crypto-policies/back-ends/bind.config"; 
-directive:  grep 'include "/etc/crypto-policies/back-ends/bind.config";' /etc/named.conf ,
-and verify that the directive is at the bottom of the  options  section of the config file.
+directive:
+ $ sudo grep 'include "/etc/crypto-policies/back-ends/bind.config";' /etc/named.conf 
+Verify that the directive is at the bottom of the  options  section of the config file.
 If BIND is installed and the BIND config file doesn't contain the
  include "/etc/crypto-policies/back-ends/bind.config";  directive then this is a finding.</t>
         </is>
       </c>
       <c r="L168" s="2" t="n"/>
-      <c r="M168" s="2" t="inlineStr"/>
+      <c r="M168" s="2" t="inlineStr">
+        <is>
+          <t>Configure BIND to use the system crypto policy.
+Add the following line to the "options" section in "/etc/named.conf":
+include "/etc/crypto-policies/back-ends/bind.config";</t>
+        </is>
+      </c>
       <c r="N168" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -13543,7 +13550,7 @@
     <row r="171" ht="130" customHeight="1">
       <c r="A171" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B171" s="2" t="inlineStr">
@@ -13621,7 +13628,7 @@
     <row r="172" ht="130" customHeight="1">
       <c r="A172" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B172" s="2" t="inlineStr">
@@ -13704,7 +13711,7 @@
     <row r="173" ht="130" customHeight="1">
       <c r="A173" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B173" s="2" t="inlineStr">
@@ -14084,7 +14091,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-6 (4),AU-4 (1)</t>
+          <t>AU-4 (1),AU-6 (4),CM-6 b</t>
         </is>
       </c>
       <c r="B178" s="2" t="inlineStr">
@@ -14155,7 +14162,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (9),CM-7 b,CM-6 b,AC-17 (1)</t>
+          <t>AC-17 (1),AC-17 (9),CM-6 b,CM-7 b</t>
         </is>
       </c>
       <c r="B179" s="2" t="inlineStr">
@@ -14232,7 +14239,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-6 b,AC-17 (1)</t>
+          <t>AC-17 (1),CM-6 b,CM-7 b</t>
         </is>
       </c>
       <c r="B180" s="2" t="inlineStr">
@@ -14311,7 +14318,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">
@@ -14394,7 +14401,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B182" s="2" t="inlineStr">
@@ -14472,7 +14479,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B183" s="2" t="inlineStr">
@@ -14563,7 +14570,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B184" s="2" t="inlineStr">
@@ -14645,7 +14652,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B185" s="2" t="inlineStr">
@@ -15217,7 +15224,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="2" t="inlineStr">
         <is>
-          <t>AU-3,CM-6 b</t>
+          <t>CM-6 b,AU-3</t>
         </is>
       </c>
       <c r="B192" s="2" t="inlineStr">
@@ -15651,7 +15658,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-4 (1)</t>
+          <t>AU-4 (1),AU-3</t>
         </is>
       </c>
       <c r="B198" s="2" t="inlineStr">
@@ -16166,7 +16173,7 @@
     <row r="205" ht="130" customHeight="1">
       <c r="A205" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-4 (1)</t>
+          <t>AU-4 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B205" s="2" t="inlineStr">
@@ -16560,7 +16567,7 @@
     <row r="210" ht="130" customHeight="1">
       <c r="A210" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B210" s="2" t="inlineStr">
@@ -16662,7 +16669,7 @@
     <row r="211" ht="130" customHeight="1">
       <c r="A211" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B211" s="2" t="inlineStr">
@@ -16772,7 +16779,7 @@
     <row r="212" ht="130" customHeight="1">
       <c r="A212" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B212" s="2" t="inlineStr">
@@ -16883,7 +16890,7 @@
     <row r="213" ht="130" customHeight="1">
       <c r="A213" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B213" s="2" t="inlineStr">
@@ -16992,7 +16999,7 @@
     <row r="214" ht="130" customHeight="1">
       <c r="A214" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-12 c,AC-6 (9)</t>
+          <t>AC-6 (9),AC-2 (4),AU-12 c</t>
         </is>
       </c>
       <c r="B214" s="2" t="inlineStr">
@@ -17434,7 +17441,7 @@
     <row r="219" ht="130" customHeight="1">
       <c r="A219" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (5)</t>
+          <t>IA-2 (5),CM-6 b</t>
         </is>
       </c>
       <c r="B219" s="2" t="inlineStr">
@@ -17512,7 +17519,7 @@
     <row r="220" ht="130" customHeight="1">
       <c r="A220" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),IA-2 (4),IA-2 (2),IA-2,IA-2 (3)</t>
+          <t>IA-2,IA-2 (4),IA-2 (3),IA-2 (5),IA-2 (2)</t>
         </is>
       </c>
       <c r="B220" s="2" t="inlineStr">
@@ -17597,7 +17604,7 @@
     <row r="221" ht="130" customHeight="1">
       <c r="A221" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),IA-2 (4),IA-2 (2),IA-2,IA-2 (3)</t>
+          <t>IA-2,IA-2 (4),IA-2 (3),IA-2 (5),IA-2 (2)</t>
         </is>
       </c>
       <c r="B221" s="2" t="inlineStr">
@@ -17682,7 +17689,7 @@
     <row r="222" ht="130" customHeight="1">
       <c r="A222" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8,AC-18 (1)</t>
+          <t>AC-18 (1),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B222" s="2" t="inlineStr">
@@ -18250,7 +18257,7 @@
     <row r="229" ht="130" customHeight="1">
       <c r="A229" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,IA-7</t>
+          <t>IA-7,CM-7 a</t>
         </is>
       </c>
       <c r="B229" s="2" t="inlineStr">
@@ -18329,7 +18336,7 @@
     <row r="230" ht="130" customHeight="1">
       <c r="A230" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B230" s="2" t="inlineStr">
@@ -18413,7 +18420,7 @@
     <row r="231" ht="130" customHeight="1">
       <c r="A231" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),AC-17 (2)</t>
+          <t>AC-17 (2),MA-4 (6)</t>
         </is>
       </c>
       <c r="B231" s="2" t="inlineStr">
@@ -18488,7 +18495,7 @@
     <row r="232" ht="130" customHeight="1">
       <c r="A232" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B232" s="2" t="inlineStr">
@@ -19085,7 +19092,7 @@
     <row r="240" ht="130" customHeight="1">
       <c r="A240" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B240" s="2" t="inlineStr">
@@ -19163,7 +19170,7 @@
     <row r="241" ht="130" customHeight="1">
       <c r="A241" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B241" s="2" t="inlineStr">
@@ -19332,7 +19339,7 @@
     <row r="243" ht="130" customHeight="1">
       <c r="A243" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SI-16,CM-6 b</t>
+          <t>CM-6 b,SI-16,SC-2</t>
         </is>
       </c>
       <c r="B243" s="2" t="inlineStr">
@@ -20804,7 +20811,7 @@
     <row r="262" ht="130" customHeight="1">
       <c r="A262" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 (1)</t>
+          <t>AU-5 (1),AU-5 a</t>
         </is>
       </c>
       <c r="B262" s="2" t="inlineStr">
@@ -21244,7 +21251,7 @@
     <row r="268" ht="130" customHeight="1">
       <c r="A268" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (2)</t>
+          <t>IA-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B268" s="2" t="inlineStr">
@@ -21331,7 +21338,7 @@
     <row r="269" ht="130" customHeight="1">
       <c r="A269" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2 (1),IA-2 (2),IA-2 (3)</t>
+          <t>IA-2 (1),IA-2 (2),IA-2 (3),IA-2 (4)</t>
         </is>
       </c>
       <c r="B269" s="2" t="inlineStr">
@@ -21500,7 +21507,7 @@
     <row r="271" ht="130" customHeight="1">
       <c r="A271" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B271" s="2" t="inlineStr">
@@ -21718,7 +21725,7 @@
     <row r="274" ht="130" customHeight="1">
       <c r="A274" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-4</t>
+          <t>SC-4,CM-6 b</t>
         </is>
       </c>
       <c r="B274" s="2" t="inlineStr">
@@ -21799,7 +21806,7 @@
     <row r="275" ht="130" customHeight="1">
       <c r="A275" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SC-4</t>
+          <t>SC-4,SC-2</t>
         </is>
       </c>
       <c r="B275" s="2" t="inlineStr">
@@ -21887,7 +21894,7 @@
     <row r="276" ht="130" customHeight="1">
       <c r="A276" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SC-4</t>
+          <t>SC-4,SC-2</t>
         </is>
       </c>
       <c r="B276" s="2" t="inlineStr">
@@ -22125,7 +22132,7 @@
     <row r="279" ht="130" customHeight="1">
       <c r="A279" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,CM-6 b</t>
+          <t>CM-6 b,AU-12 a</t>
         </is>
       </c>
       <c r="B279" s="2" t="inlineStr">
@@ -22348,7 +22355,7 @@
     <row r="282" ht="130" customHeight="1">
       <c r="A282" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (3),CM-6 b</t>
+          <t>CM-6 b,CM-5 (3)</t>
         </is>
       </c>
       <c r="B282" s="2" t="inlineStr">
@@ -23448,7 +23455,7 @@
     <row r="296" ht="130" customHeight="1">
       <c r="A296" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B296" s="2" t="inlineStr">
@@ -23627,7 +23634,7 @@
     <row r="298" ht="130" customHeight="1">
       <c r="A298" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (1),IA-2 (11)</t>
+          <t>IA-2 (1),IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B298" s="2" t="inlineStr">
@@ -24449,7 +24456,7 @@
     <row r="308" ht="130" customHeight="1">
       <c r="A308" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-8 (1) (b),AU-8 (1) (a)</t>
+          <t>AU-8 b,AU-8 (1) (a),AU-8 (1) (b)</t>
         </is>
       </c>
       <c r="B308" s="2" t="inlineStr">
@@ -25940,7 +25947,7 @@
     <row r="327" ht="130" customHeight="1">
       <c r="A327" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,CM-5 (1)</t>
+          <t>CM-5 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B327" s="2" t="inlineStr">
@@ -26097,7 +26104,7 @@
     <row r="329" ht="130" customHeight="1">
       <c r="A329" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 b</t>
+          <t>AU-5 b,AU-5 a</t>
         </is>
       </c>
       <c r="B329" s="2" t="inlineStr">
@@ -27239,7 +27246,7 @@
     <row r="344" ht="130" customHeight="1">
       <c r="A344" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (1)</t>
+          <t>AC-17 (1),CM-7 b</t>
         </is>
       </c>
       <c r="B344" s="2" t="inlineStr">
@@ -27325,7 +27332,7 @@
     <row r="345" ht="130" customHeight="1">
       <c r="A345" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,AC-18 (1)</t>
+          <t>AC-18 (1),CM-7 a</t>
         </is>
       </c>
       <c r="B345" s="2" t="inlineStr">
@@ -27402,7 +27409,7 @@
     <row r="346" ht="130" customHeight="1">
       <c r="A346" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,IA-5 (1) (c),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (c),CM-7 a</t>
         </is>
       </c>
       <c r="B346" s="2" t="inlineStr">
@@ -28587,7 +28594,7 @@
     <row r="361" ht="130" customHeight="1">
       <c r="A361" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B361" s="2" t="inlineStr">
@@ -28967,7 +28974,7 @@
     <row r="366" ht="130" customHeight="1">
       <c r="A366" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,SI-16</t>
+          <t>SI-16,CM-7 a</t>
         </is>
       </c>
       <c r="B366" s="2" t="inlineStr">
@@ -29516,7 +29523,7 @@
     <row r="373" ht="130" customHeight="1">
       <c r="A373" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B373" s="2" t="inlineStr">
@@ -29587,7 +29594,7 @@
     <row r="374" ht="130" customHeight="1">
       <c r="A374" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B374" s="2" t="inlineStr">
@@ -29659,7 +29666,7 @@
     <row r="375" ht="130" customHeight="1">
       <c r="A375" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B375" s="2" t="inlineStr">
@@ -30867,7 +30874,7 @@
     <row r="390" ht="130" customHeight="1">
       <c r="A390" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (a),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (a)</t>
         </is>
       </c>
       <c r="B390" s="2" t="inlineStr">
@@ -31433,7 +31440,7 @@
     <row r="397" ht="130" customHeight="1">
       <c r="A397" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-6 b</t>
+          <t>CM-6 b,SI-16</t>
         </is>
       </c>
       <c r="B397" s="2" t="inlineStr">
@@ -31681,7 +31688,7 @@
     <row r="400" ht="130" customHeight="1">
       <c r="A400" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B400" s="2" t="inlineStr">
@@ -31772,7 +31779,7 @@
     <row r="401" ht="130" customHeight="1">
       <c r="A401" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B401" s="2" t="inlineStr">
@@ -31866,7 +31873,7 @@
     <row r="402" ht="130" customHeight="1">
       <c r="A402" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B402" s="2" t="inlineStr">
@@ -35276,7 +35283,7 @@
     <row r="447" ht="130" customHeight="1">
       <c r="A447" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B447" s="2" t="inlineStr">
@@ -41311,7 +41318,7 @@
     <row r="523" ht="130" customHeight="1">
       <c r="A523" s="2" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b</t>
+          <t>CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B523" s="2" t="inlineStr">
@@ -41398,7 +41405,7 @@
     <row r="524" ht="130" customHeight="1">
       <c r="A524" s="2" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b</t>
+          <t>CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B524" s="2" t="inlineStr">
@@ -42630,7 +42637,7 @@
     <row r="540" ht="130" customHeight="1">
       <c r="A540" s="2" t="inlineStr">
         <is>
-          <t>SI-2 (2),CM-6 b</t>
+          <t>CM-6 b,SI-2 (2)</t>
         </is>
       </c>
       <c r="B540" s="2" t="inlineStr">
@@ -43277,7 +43284,7 @@
     <row r="549" ht="130" customHeight="1">
       <c r="A549" s="2" t="inlineStr">
         <is>
-          <t>SI-2 (2),CM-6 b</t>
+          <t>CM-6 b,SI-2 (2)</t>
         </is>
       </c>
       <c r="B549" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@b9f42ab5685c83d511744efd66aab17f46fd0541 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -625,7 +625,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),AU-4</t>
+          <t>AU-4,AU-14 (1)</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -708,7 +708,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>AU-4,CM-6 b</t>
+          <t>CM-6 b,AU-4</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -784,7 +784,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>SC-5,SC-5 (2),CM-6 b</t>
+          <t>CM-6 b,SC-5,SC-5 (2)</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -883,7 +883,7 @@
     <row r="6" ht="130" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (9),AU-12 (3),AU-7 a,AU-7 b,AC-6 (8),CM-5 (1),AU-8 b</t>
+          <t>AU-7 a,AC-6 (8),AU-12 (3),AU-7 b,AC-6 (9),AU-8 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -963,7 +963,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-12 (3),AU-7 a,AU-7 b,CM-6 b,CM-5 (1),AU-8 b,AU-12 c</t>
+          <t>AU-7 a,AU-12 (3),CM-6 b,AU-7 b,AU-8 b,AU-12 c,AU-12 a,CM-5 (1)</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1269,7 +1269,7 @@
     <row r="11" ht="130" customHeight="1">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B11" s="2" t="inlineStr">
@@ -1420,7 +1420,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -1496,7 +1496,7 @@
     <row r="14" ht="130" customHeight="1">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -1650,7 +1650,7 @@
     <row r="16" ht="130" customHeight="1">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
@@ -2020,7 +2020,7 @@
     <row r="21" ht="130" customHeight="1">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
@@ -2094,7 +2094,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -3222,7 +3222,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3306,7 +3306,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3391,7 +3391,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3463,7 +3463,7 @@
     <row r="40" ht="130" customHeight="1">
       <c r="A40" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B40" s="2" t="inlineStr">
@@ -3768,7 +3768,7 @@
     <row r="44" ht="130" customHeight="1">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>IA-2,IA-8,AU-3 (1)</t>
+          <t>AU-3 (1),IA-2,IA-8</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
@@ -3846,7 +3846,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3921,7 +3921,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -3996,7 +3996,7 @@
     <row r="47" ht="130" customHeight="1">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
@@ -4071,7 +4071,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4146,7 +4146,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4221,7 +4221,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4296,7 +4296,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4371,7 +4371,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
@@ -4446,7 +4446,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4521,7 +4521,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4596,7 +4596,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4671,7 +4671,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4746,7 +4746,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4821,7 +4821,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4901,7 +4901,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -4984,7 +4984,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5064,7 +5064,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5144,7 +5144,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5224,7 +5224,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5304,7 +5304,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5378,7 +5378,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5452,7 +5452,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5526,7 +5526,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5600,7 +5600,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5674,7 +5674,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5747,7 +5747,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5820,7 +5820,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5893,7 +5893,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -5966,7 +5966,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6039,7 +6039,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6112,7 +6112,7 @@
     <row r="75" ht="130" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
@@ -6186,7 +6186,7 @@
     <row r="76" ht="130" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
@@ -6260,7 +6260,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6334,7 +6334,7 @@
     <row r="78" ht="130" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
@@ -6412,7 +6412,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6492,7 +6492,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6572,7 +6572,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6652,7 +6652,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B82" s="2" t="inlineStr">
@@ -6732,7 +6732,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B83" s="2" t="inlineStr">
@@ -6812,7 +6812,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B84" s="2" t="inlineStr">
@@ -6892,7 +6892,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B85" s="2" t="inlineStr">
@@ -6972,7 +6972,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -7052,7 +7052,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7132,7 +7132,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7212,7 +7212,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7292,7 +7292,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7368,7 +7368,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7445,7 +7445,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
@@ -7525,7 +7525,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
@@ -7605,7 +7605,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B94" s="2" t="inlineStr">
@@ -7685,7 +7685,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
@@ -7765,7 +7765,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3</t>
+          <t>AU-12 c,AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7845,7 +7845,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7925,7 +7925,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8005,7 +8005,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8085,7 +8085,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8165,7 +8165,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8238,7 +8238,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,AC-2 (4),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8319,7 +8319,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,AC-2 (4),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8400,7 +8400,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,AC-2 (4),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8471,7 +8471,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AC-2 (4),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8546,7 +8546,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,AC-2 (4),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8628,7 +8628,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,AC-2 (4),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8710,7 +8710,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,AC-2 (4),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -8792,7 +8792,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,AC-2 (4),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -8874,7 +8874,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,AC-2 (4),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B110" s="2" t="inlineStr">
@@ -8956,7 +8956,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,AU-14 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-14 (1),AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9801,7 +9801,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-12 c</t>
+          <t>AU-12 c,AU-9</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -10174,7 +10174,7 @@
     <row r="126" ht="130" customHeight="1">
       <c r="A126" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AC-6 (9),CM-5 (1),AU-12 c</t>
+          <t>AU-12 c,AC-2 (4),CM-5 (1),AC-6 (9)</t>
         </is>
       </c>
       <c r="B126" s="2" t="inlineStr">
@@ -10312,7 +10312,7 @@
     <row r="128" ht="130" customHeight="1">
       <c r="A128" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (b),CM-6 b,IA-5 (1) (a)</t>
+          <t>CM-6 b,IA-5 (1) (a),IA-5 (1) (b)</t>
         </is>
       </c>
       <c r="B128" s="2" t="inlineStr">
@@ -10632,7 +10632,7 @@
     <row r="132" ht="130" customHeight="1">
       <c r="A132" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),MA-4 c,SC-8,SC-13</t>
+          <t>SC-8,SC-13,MA-4 c,AC-17 (2)</t>
         </is>
       </c>
       <c r="B132" s="2" t="inlineStr">
@@ -10714,7 +10714,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>MA-4 e,AC-12,MA-4 (7),SC-10</t>
+          <t>MA-4 (7),SC-10,AC-12,MA-4 e</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10789,7 +10789,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -10868,7 +10868,7 @@
     <row r="135" ht="130" customHeight="1">
       <c r="A135" s="2" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B135" s="2" t="inlineStr">
@@ -10944,7 +10944,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,SC-10</t>
+          <t>SC-10,AC-11 a</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -11021,7 +11021,7 @@
     <row r="137" ht="130" customHeight="1">
       <c r="A137" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-7 a,CM-6 b,AU-14 (1),CM-5 (1),AU-6 (4),AU-7 (1),AU-3</t>
+          <t>AU-7 a,AU-7 (1),AU-14 (1),AU-3 (1),AU-3,AU-6 (4),CM-6 b,AU-12 a,MA-4 (1) (a),CM-5 (1)</t>
         </is>
       </c>
       <c r="B137" s="2" t="inlineStr">
@@ -13255,7 +13255,7 @@
     <row r="167" ht="130" customHeight="1">
       <c r="A167" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8</t>
+          <t>SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B167" s="2" t="inlineStr">
@@ -13416,7 +13416,7 @@
     <row r="169" ht="130" customHeight="1">
       <c r="A169" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8</t>
+          <t>SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B169" s="2" t="inlineStr">
@@ -13565,7 +13565,7 @@
     <row r="171" ht="130" customHeight="1">
       <c r="A171" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B171" s="2" t="inlineStr">
@@ -14106,7 +14106,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-6 (4),CM-6 b</t>
+          <t>AU-4 (1),CM-6 b,AU-6 (4)</t>
         </is>
       </c>
       <c r="B178" s="2" t="inlineStr">
@@ -14177,7 +14177,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (1),CM-6 b,AC-17 (9)</t>
+          <t>AC-17 (9),AC-17 (1),CM-6 b,CM-7 b</t>
         </is>
       </c>
       <c r="B179" s="2" t="inlineStr">
@@ -14254,7 +14254,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (1),CM-6 b</t>
+          <t>CM-6 b,AC-17 (1),CM-7 b</t>
         </is>
       </c>
       <c r="B180" s="2" t="inlineStr">
@@ -16268,7 +16268,7 @@
     <row r="206" ht="130" customHeight="1">
       <c r="A206" s="2" t="inlineStr">
         <is>
-          <t>SC-28,SC-28 (1)</t>
+          <t>SC-28 (1),SC-28</t>
         </is>
       </c>
       <c r="B206" s="2" t="inlineStr">
@@ -16491,11 +16491,17 @@
           <t>To determine if  !authenticate  has not been configured for sudo, run the following command:
  $ sudo grep -r \!authenticate /etc/sudoers /etc/sudoers.d/ 
 The command should return no output.
-If !authenticate is enabled in sudo then this is a finding.</t>
+If !authenticate is specified in the sudo config files then this is a finding.</t>
         </is>
       </c>
       <c r="L208" s="2" t="n"/>
-      <c r="M208" s="2" t="inlineStr"/>
+      <c r="M208" s="2" t="inlineStr">
+        <is>
+          <t>Check that Red Hat Enterprise Linux 9 is not configured to allow users to execute privileged actions without authenticating.
+Remove any occurrence of "!authenticate" found in "/etc/sudoers" file or files in the "/etc/sudoers.d" directory.
+$ sed -i '/\!authenticate/ s/^/# /g' /etc/sudoers /etc/sudoers.d/*</t>
+        </is>
+      </c>
       <c r="N208" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -16565,11 +16571,17 @@
           <t>To determine if  NOPASSWD  has been configured for sudo, run the following command:
  $ sudo grep -ri nopasswd /etc/sudoers /etc/sudoers.d/ 
 The command should return no output.
-If nopasswd is enabled in sudo then this is a finding.</t>
+If nopasswd is specified in the sudo config files then this is a finding.</t>
         </is>
       </c>
       <c r="L209" s="2" t="n"/>
-      <c r="M209" s="2" t="inlineStr"/>
+      <c r="M209" s="2" t="inlineStr">
+        <is>
+          <t>Check that Red Hat Enterprise Linux 9 is not configured to allow users to execute privileged actions without authenticating.
+Remove any occurrence of "NOPASSWD" found in "/etc/sudoers" file or files in the "/etc/sudoers.d" directory.
+$ sed -i '/NOPASSWD/ s/^/# /g' /etc/sudoers /etc/sudoers.d/*</t>
+        </is>
+      </c>
       <c r="N209" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -17014,7 +17026,7 @@
     <row r="214" ht="130" customHeight="1">
       <c r="A214" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AC-6 (9),AU-12 c</t>
+          <t>AU-12 c,AC-2 (4),AC-6 (9)</t>
         </is>
       </c>
       <c r="B214" s="2" t="inlineStr">
@@ -17456,7 +17468,7 @@
     <row r="219" ht="130" customHeight="1">
       <c r="A219" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),CM-6 b</t>
+          <t>CM-6 b,IA-2 (5)</t>
         </is>
       </c>
       <c r="B219" s="2" t="inlineStr">
@@ -17534,7 +17546,7 @@
     <row r="220" ht="130" customHeight="1">
       <c r="A220" s="2" t="inlineStr">
         <is>
-          <t>IA-2,IA-2 (5),IA-2 (4),IA-2 (2),IA-2 (3)</t>
+          <t>IA-2 (2),IA-2 (4),IA-2,IA-2 (3),IA-2 (5)</t>
         </is>
       </c>
       <c r="B220" s="2" t="inlineStr">
@@ -17619,7 +17631,7 @@
     <row r="221" ht="130" customHeight="1">
       <c r="A221" s="2" t="inlineStr">
         <is>
-          <t>IA-2,IA-2 (5),IA-2 (4),IA-2 (2),IA-2 (3)</t>
+          <t>IA-2 (2),IA-2 (4),IA-2,IA-2 (3),IA-2 (5)</t>
         </is>
       </c>
       <c r="B221" s="2" t="inlineStr">
@@ -17704,7 +17716,7 @@
     <row r="222" ht="130" customHeight="1">
       <c r="A222" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),AC-18 (1),SC-8</t>
+          <t>SC-8,AC-18 (1),SC-8 (1)</t>
         </is>
       </c>
       <c r="B222" s="2" t="inlineStr">
@@ -17871,7 +17883,7 @@
     <row r="224" ht="130" customHeight="1">
       <c r="A224" s="2" t="inlineStr">
         <is>
-          <t>IA-7,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),IA-7</t>
         </is>
       </c>
       <c r="B224" s="2" t="inlineStr">
@@ -17954,7 +17966,7 @@
     <row r="225" ht="130" customHeight="1">
       <c r="A225" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B225" s="2" t="inlineStr">
@@ -18030,7 +18042,7 @@
     <row r="226" ht="130" customHeight="1">
       <c r="A226" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B226" s="2" t="inlineStr">
@@ -18115,7 +18127,7 @@
     <row r="227" ht="130" customHeight="1">
       <c r="A227" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B227" s="2" t="inlineStr">
@@ -18272,7 +18284,7 @@
     <row r="229" ht="130" customHeight="1">
       <c r="A229" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-7 a</t>
+          <t>CM-7 a,IA-7</t>
         </is>
       </c>
       <c r="B229" s="2" t="inlineStr">
@@ -18351,7 +18363,7 @@
     <row r="230" ht="130" customHeight="1">
       <c r="A230" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B230" s="2" t="inlineStr">
@@ -18435,7 +18447,7 @@
     <row r="231" ht="130" customHeight="1">
       <c r="A231" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),MA-4 (6)</t>
+          <t>MA-4 (6),AC-17 (2)</t>
         </is>
       </c>
       <c r="B231" s="2" t="inlineStr">
@@ -18510,7 +18522,7 @@
     <row r="232" ht="130" customHeight="1">
       <c r="A232" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B232" s="2" t="inlineStr">
@@ -19354,7 +19366,7 @@
     <row r="243" ht="130" customHeight="1">
       <c r="A243" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SI-16,CM-6 b</t>
+          <t>CM-6 b,SI-16,SC-2</t>
         </is>
       </c>
       <c r="B243" s="2" t="inlineStr">
@@ -20428,7 +20440,7 @@
     <row r="257" ht="130" customHeight="1">
       <c r="A257" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B257" s="2" t="inlineStr">
@@ -20503,7 +20515,7 @@
     <row r="258" ht="130" customHeight="1">
       <c r="A258" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B258" s="2" t="inlineStr">
@@ -20591,7 +20603,7 @@
     <row r="259" ht="130" customHeight="1">
       <c r="A259" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B259" s="2" t="inlineStr">
@@ -20668,7 +20680,7 @@
     <row r="260" ht="130" customHeight="1">
       <c r="A260" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B260" s="2" t="inlineStr">
@@ -20826,7 +20838,7 @@
     <row r="262" ht="130" customHeight="1">
       <c r="A262" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 (1)</t>
+          <t>AU-5 (1),AU-5 a</t>
         </is>
       </c>
       <c r="B262" s="2" t="inlineStr">
@@ -21266,7 +21278,7 @@
     <row r="268" ht="130" customHeight="1">
       <c r="A268" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),CM-6 b</t>
+          <t>CM-6 b,IA-2 (2)</t>
         </is>
       </c>
       <c r="B268" s="2" t="inlineStr">
@@ -21353,7 +21365,7 @@
     <row r="269" ht="130" customHeight="1">
       <c r="A269" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (2),IA-2 (1),IA-2 (4)</t>
+          <t>IA-2 (3),IA-2 (1),IA-2 (2),IA-2 (4)</t>
         </is>
       </c>
       <c r="B269" s="2" t="inlineStr">
@@ -21740,7 +21752,7 @@
     <row r="274" ht="130" customHeight="1">
       <c r="A274" s="2" t="inlineStr">
         <is>
-          <t>SC-4,CM-6 b</t>
+          <t>CM-6 b,SC-4</t>
         </is>
       </c>
       <c r="B274" s="2" t="inlineStr">
@@ -21821,7 +21833,7 @@
     <row r="275" ht="130" customHeight="1">
       <c r="A275" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SC-4</t>
+          <t>SC-4,SC-2</t>
         </is>
       </c>
       <c r="B275" s="2" t="inlineStr">
@@ -21909,7 +21921,7 @@
     <row r="276" ht="130" customHeight="1">
       <c r="A276" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SC-4</t>
+          <t>SC-4,SC-2</t>
         </is>
       </c>
       <c r="B276" s="2" t="inlineStr">
@@ -22370,7 +22382,7 @@
     <row r="282" ht="130" customHeight="1">
       <c r="A282" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (3),CM-6 b</t>
+          <t>CM-6 b,CM-5 (3)</t>
         </is>
       </c>
       <c r="B282" s="2" t="inlineStr">
@@ -23548,7 +23560,7 @@
     <row r="297" ht="130" customHeight="1">
       <c r="A297" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B297" s="2" t="inlineStr">
@@ -23638,7 +23650,7 @@
     <row r="298" ht="130" customHeight="1">
       <c r="A298" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (1)</t>
         </is>
       </c>
       <c r="B298" s="2" t="inlineStr">
@@ -23727,7 +23739,7 @@
     <row r="299" ht="130" customHeight="1">
       <c r="A299" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11),IA-2 (1)</t>
+          <t>IA-2 (11),IA-2 (12),IA-2 (1)</t>
         </is>
       </c>
       <c r="B299" s="2" t="inlineStr">
@@ -24549,7 +24561,7 @@
     <row r="309" ht="130" customHeight="1">
       <c r="A309" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-8 (1) (a),AU-8 (1) (b)</t>
+          <t>AU-8 (1) (a),AU-8 (1) (b),AU-8 b</t>
         </is>
       </c>
       <c r="B309" s="2" t="inlineStr">
@@ -26040,7 +26052,7 @@
     <row r="328" ht="130" customHeight="1">
       <c r="A328" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AU-12 c</t>
+          <t>AU-12 c,CM-5 (1)</t>
         </is>
       </c>
       <c r="B328" s="2" t="inlineStr">
@@ -27191,7 +27203,7 @@
     <row r="343" ht="130" customHeight="1">
       <c r="A343" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-7 a</t>
+          <t>CM-7 a,CM-7 b</t>
         </is>
       </c>
       <c r="B343" s="2" t="inlineStr">
@@ -27265,7 +27277,7 @@
     <row r="344" ht="130" customHeight="1">
       <c r="A344" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-7 a</t>
+          <t>CM-7 a,CM-7 b</t>
         </is>
       </c>
       <c r="B344" s="2" t="inlineStr">
@@ -27339,7 +27351,7 @@
     <row r="345" ht="130" customHeight="1">
       <c r="A345" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (1)</t>
+          <t>AC-17 (1),CM-7 b</t>
         </is>
       </c>
       <c r="B345" s="2" t="inlineStr">
@@ -27425,7 +27437,7 @@
     <row r="346" ht="130" customHeight="1">
       <c r="A346" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),CM-7 a</t>
+          <t>CM-7 a,AC-18 (1)</t>
         </is>
       </c>
       <c r="B346" s="2" t="inlineStr">
@@ -27502,7 +27514,7 @@
     <row r="347" ht="130" customHeight="1">
       <c r="A347" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (c),CM-7 a</t>
+          <t>CM-7 a,IA-5 (1) (c),CM-6 b</t>
         </is>
       </c>
       <c r="B347" s="2" t="inlineStr">
@@ -28347,7 +28359,7 @@
     <row r="358" ht="130" customHeight="1">
       <c r="A358" s="2" t="inlineStr">
         <is>
-          <t>AC-11 (1),AC-11 b</t>
+          <t>AC-11 b,AC-11 (1)</t>
         </is>
       </c>
       <c r="B358" s="2" t="inlineStr">
@@ -29067,7 +29079,7 @@
     <row r="367" ht="130" customHeight="1">
       <c r="A367" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-7 a</t>
+          <t>CM-7 a,SI-16</t>
         </is>
       </c>
       <c r="B367" s="2" t="inlineStr">
@@ -29616,7 +29628,7 @@
     <row r="374" ht="130" customHeight="1">
       <c r="A374" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B374" s="2" t="inlineStr">
@@ -29687,7 +29699,7 @@
     <row r="375" ht="130" customHeight="1">
       <c r="A375" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B375" s="2" t="inlineStr">
@@ -29759,7 +29771,7 @@
     <row r="376" ht="130" customHeight="1">
       <c r="A376" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B376" s="2" t="inlineStr">
@@ -30519,7 +30531,7 @@
     <row r="385" ht="130" customHeight="1">
       <c r="A385" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),CM-6 b</t>
+          <t>CM-6 b,AC-17 (2)</t>
         </is>
       </c>
       <c r="B385" s="2" t="inlineStr">
@@ -30828,7 +30840,7 @@
     <row r="389" ht="130" customHeight="1">
       <c r="A389" s="2" t="inlineStr">
         <is>
-          <t>SC-3,SI-6 a</t>
+          <t>SI-6 a,SC-3</t>
         </is>
       </c>
       <c r="B389" s="2" t="inlineStr">
@@ -31533,7 +31545,7 @@
     <row r="398" ht="130" customHeight="1">
       <c r="A398" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-6 b</t>
+          <t>CM-6 b,SI-16</t>
         </is>
       </c>
       <c r="B398" s="2" t="inlineStr">
@@ -31781,7 +31793,7 @@
     <row r="401" ht="130" customHeight="1">
       <c r="A401" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B401" s="2" t="inlineStr">
@@ -31872,7 +31884,7 @@
     <row r="402" ht="130" customHeight="1">
       <c r="A402" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B402" s="2" t="inlineStr">
@@ -31966,7 +31978,7 @@
     <row r="403" ht="130" customHeight="1">
       <c r="A403" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B403" s="2" t="inlineStr">
@@ -35526,7 +35538,7 @@
     <row r="450" ht="130" customHeight="1">
       <c r="A450" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),CM-6 b</t>
+          <t>CM-6 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B450" s="2" t="inlineStr">
@@ -35599,7 +35611,7 @@
     <row r="451" ht="130" customHeight="1">
       <c r="A451" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),CM-6 b</t>
+          <t>CM-6 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B451" s="2" t="inlineStr">
@@ -41411,7 +41423,7 @@
     <row r="524" ht="130" customHeight="1">
       <c r="A524" s="2" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b</t>
+          <t>CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B524" s="2" t="inlineStr">
@@ -41498,7 +41510,7 @@
     <row r="525" ht="130" customHeight="1">
       <c r="A525" s="2" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b</t>
+          <t>CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B525" s="2" t="inlineStr">
@@ -42730,7 +42742,7 @@
     <row r="541" ht="130" customHeight="1">
       <c r="A541" s="2" t="inlineStr">
         <is>
-          <t>SI-2 (2),CM-6 b</t>
+          <t>CM-6 b,SI-2 (2)</t>
         </is>
       </c>
       <c r="B541" s="2" t="inlineStr">
@@ -43377,7 +43389,7 @@
     <row r="550" ht="130" customHeight="1">
       <c r="A550" s="2" t="inlineStr">
         <is>
-          <t>SI-2 (2),CM-6 b</t>
+          <t>CM-6 b,SI-2 (2)</t>
         </is>
       </c>
       <c r="B550" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@10c8092a48d15416be7741d5beb3e75fb300130c 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -541,7 +541,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-4</t>
+          <t>AU-4,AU-4 (1)</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -625,7 +625,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-14 (1)</t>
+          <t>AU-14 (1),AU-4</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -708,7 +708,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-4</t>
+          <t>AU-4,CM-6 b</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -784,7 +784,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-5,SC-5 (2)</t>
+          <t>SC-5 (2),CM-6 b,SC-5</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -883,7 +883,7 @@
     <row r="6" ht="130" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>AU-7 a,AC-6 (8),AU-12 (3),AU-7 b,AC-6 (9),AU-8 b,CM-5 (1)</t>
+          <t>AU-12 (3),AU-7 b,AU-8 b,AC-6 (8),AC-6 (9),CM-5 (1),AU-7 a</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -963,7 +963,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-7 a,AU-12 (3),CM-6 b,AU-7 b,AU-8 b,AU-12 c,AU-12 a,CM-5 (1)</t>
+          <t>AU-12 (3),CM-6 b,AU-12 c,AU-7 b,AU-8 b,AU-12 a,CM-5 (1),AU-7 a</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1420,7 +1420,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -1496,7 +1496,7 @@
     <row r="14" ht="130" customHeight="1">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -1650,7 +1650,7 @@
     <row r="16" ht="130" customHeight="1">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
@@ -2020,7 +2020,7 @@
     <row r="21" ht="130" customHeight="1">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
@@ -2094,7 +2094,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -3222,7 +3222,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3306,7 +3306,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3391,7 +3391,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3463,7 +3463,7 @@
     <row r="40" ht="130" customHeight="1">
       <c r="A40" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B40" s="2" t="inlineStr">
@@ -3768,7 +3768,7 @@
     <row r="44" ht="130" customHeight="1">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),IA-2,IA-8</t>
+          <t>IA-8,IA-2,AU-3 (1)</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
@@ -3846,7 +3846,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3921,7 +3921,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -3996,7 +3996,7 @@
     <row r="47" ht="130" customHeight="1">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
@@ -4071,7 +4071,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4146,7 +4146,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4221,7 +4221,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4296,7 +4296,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4371,7 +4371,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
@@ -4446,7 +4446,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4521,7 +4521,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4596,7 +4596,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4671,7 +4671,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4746,7 +4746,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4821,7 +4821,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4901,7 +4901,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -4984,7 +4984,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5064,7 +5064,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5144,7 +5144,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5224,7 +5224,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5304,7 +5304,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5378,7 +5378,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5452,7 +5452,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5526,7 +5526,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5600,7 +5600,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5674,7 +5674,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5747,7 +5747,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5820,7 +5820,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5893,7 +5893,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -5966,7 +5966,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6039,7 +6039,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6112,7 +6112,7 @@
     <row r="75" ht="130" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
@@ -6186,7 +6186,7 @@
     <row r="76" ht="130" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
@@ -6260,7 +6260,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6334,7 +6334,7 @@
     <row r="78" ht="130" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
@@ -6412,7 +6412,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6492,7 +6492,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6572,7 +6572,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6652,7 +6652,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B82" s="2" t="inlineStr">
@@ -6732,7 +6732,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B83" s="2" t="inlineStr">
@@ -6812,7 +6812,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B84" s="2" t="inlineStr">
@@ -6892,7 +6892,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B85" s="2" t="inlineStr">
@@ -6972,7 +6972,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -7052,7 +7052,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7132,7 +7132,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7212,7 +7212,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7368,7 +7368,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7445,7 +7445,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
@@ -7525,7 +7525,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
@@ -7605,7 +7605,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B94" s="2" t="inlineStr">
@@ -7685,7 +7685,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
@@ -7765,7 +7765,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7845,7 +7845,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7925,7 +7925,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8005,7 +8005,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8085,7 +8085,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8165,7 +8165,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8238,7 +8238,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,AC-2 (4),MA-4 (1) (a)</t>
+          <t>AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8319,7 +8319,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,AC-2 (4),MA-4 (1) (a)</t>
+          <t>AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8400,7 +8400,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,AC-2 (4),MA-4 (1) (a)</t>
+          <t>AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8471,7 +8471,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AC-2 (4),MA-4 (1) (a)</t>
+          <t>AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8546,7 +8546,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,AC-2 (4),MA-4 (1) (a)</t>
+          <t>AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8628,7 +8628,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,AC-2 (4),MA-4 (1) (a)</t>
+          <t>AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8710,7 +8710,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,AC-2 (4),MA-4 (1) (a)</t>
+          <t>AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -8792,7 +8792,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,AC-2 (4),MA-4 (1) (a)</t>
+          <t>AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -8874,7 +8874,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,AU-12 a,AC-2 (4),MA-4 (1) (a)</t>
+          <t>AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B110" s="2" t="inlineStr">
@@ -8956,7 +8956,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),AU-3 (1),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,AU-14 (1),MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9659,7 +9659,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-12 c,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9730,7 +9730,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-12 c,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -9801,7 +9801,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-9</t>
+          <t>AU-9,AU-12 c</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -10174,7 +10174,7 @@
     <row r="126" ht="130" customHeight="1">
       <c r="A126" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-2 (4),CM-5 (1),AC-6 (9)</t>
+          <t>AC-2 (4),CM-5 (1),AC-6 (9),AU-12 c</t>
         </is>
       </c>
       <c r="B126" s="2" t="inlineStr">
@@ -10312,7 +10312,7 @@
     <row r="128" ht="130" customHeight="1">
       <c r="A128" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (a),IA-5 (1) (b)</t>
+          <t>IA-5 (1) (a),IA-5 (1) (b),CM-6 b</t>
         </is>
       </c>
       <c r="B128" s="2" t="inlineStr">
@@ -10619,7 +10619,15 @@
         </is>
       </c>
       <c r="L131" s="2" t="n"/>
-      <c r="M131" s="2" t="inlineStr"/>
+      <c r="M131" s="2" t="inlineStr">
+        <is>
+          <t>Configure Red Hat Enterprise Linux 9 to run in FIPS mode.
+Run the following commands:
+$ sudo fips-mode-setup --enable
+$ sudo update-crypto-policies --set 
+The system needs to be rebooted for these changes to take effect.</t>
+        </is>
+      </c>
       <c r="N131" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -10632,7 +10640,7 @@
     <row r="132" ht="130" customHeight="1">
       <c r="A132" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-13,MA-4 c,AC-17 (2)</t>
+          <t>SC-8,SC-13,AC-17 (2),MA-4 c</t>
         </is>
       </c>
       <c r="B132" s="2" t="inlineStr">
@@ -10714,7 +10722,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (7),SC-10,AC-12,MA-4 e</t>
+          <t>MA-4 e,MA-4 (7),SC-10,AC-12</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10944,7 +10952,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>SC-10,AC-11 a</t>
+          <t>AC-11 a,SC-10</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -11021,7 +11029,7 @@
     <row r="137" ht="130" customHeight="1">
       <c r="A137" s="2" t="inlineStr">
         <is>
-          <t>AU-7 a,AU-7 (1),AU-14 (1),AU-3 (1),AU-3,AU-6 (4),CM-6 b,AU-12 a,MA-4 (1) (a),CM-5 (1)</t>
+          <t>AU-3 (1),CM-6 b,AU-14 (1),MA-4 (1) (a),AU-12 a,AU-6 (4),CM-5 (1),AU-3,AU-7 (1),AU-7 a</t>
         </is>
       </c>
       <c r="B137" s="2" t="inlineStr">
@@ -11423,7 +11431,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B142" s="2" t="inlineStr">
@@ -11492,7 +11500,7 @@
     <row r="143" ht="130" customHeight="1">
       <c r="A143" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B143" s="2" t="inlineStr">
@@ -11561,7 +11569,7 @@
     <row r="144" ht="130" customHeight="1">
       <c r="A144" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B144" s="2" t="inlineStr">
@@ -11631,7 +11639,7 @@
     <row r="145" ht="130" customHeight="1">
       <c r="A145" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B145" s="2" t="inlineStr">
@@ -11700,7 +11708,7 @@
     <row r="146" ht="130" customHeight="1">
       <c r="A146" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B146" s="2" t="inlineStr">
@@ -11769,7 +11777,7 @@
     <row r="147" ht="130" customHeight="1">
       <c r="A147" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B147" s="2" t="inlineStr">
@@ -11839,7 +11847,7 @@
     <row r="148" ht="130" customHeight="1">
       <c r="A148" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B148" s="2" t="inlineStr">
@@ -11908,7 +11916,7 @@
     <row r="149" ht="130" customHeight="1">
       <c r="A149" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B149" s="2" t="inlineStr">
@@ -11977,7 +11985,7 @@
     <row r="150" ht="130" customHeight="1">
       <c r="A150" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B150" s="2" t="inlineStr">
@@ -12047,7 +12055,7 @@
     <row r="151" ht="130" customHeight="1">
       <c r="A151" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B151" s="2" t="inlineStr">
@@ -12116,7 +12124,7 @@
     <row r="152" ht="130" customHeight="1">
       <c r="A152" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B152" s="2" t="inlineStr">
@@ -12185,7 +12193,7 @@
     <row r="153" ht="130" customHeight="1">
       <c r="A153" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B153" s="2" t="inlineStr">
@@ -12254,7 +12262,7 @@
     <row r="154" ht="130" customHeight="1">
       <c r="A154" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B154" s="2" t="inlineStr">
@@ -13092,7 +13100,7 @@
     <row r="165" ht="130" customHeight="1">
       <c r="A165" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (2),SC-8 (1)</t>
+          <t>SC-8 (1),SC-8,SC-8 (2)</t>
         </is>
       </c>
       <c r="B165" s="2" t="inlineStr">
@@ -13169,7 +13177,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (2),SC-8 (1)</t>
+          <t>SC-8 (1),SC-8,SC-8 (2)</t>
         </is>
       </c>
       <c r="B166" s="2" t="inlineStr">
@@ -13255,7 +13263,7 @@
     <row r="167" ht="130" customHeight="1">
       <c r="A167" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2)</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B167" s="2" t="inlineStr">
@@ -13416,7 +13424,7 @@
     <row r="169" ht="130" customHeight="1">
       <c r="A169" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2)</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B169" s="2" t="inlineStr">
@@ -13565,7 +13573,7 @@
     <row r="171" ht="130" customHeight="1">
       <c r="A171" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B171" s="2" t="inlineStr">
@@ -14106,7 +14114,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),CM-6 b,AU-6 (4)</t>
+          <t>CM-6 b,AU-4 (1),AU-6 (4)</t>
         </is>
       </c>
       <c r="B178" s="2" t="inlineStr">
@@ -14254,7 +14262,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-17 (1),CM-7 b</t>
+          <t>AC-17 (1),CM-6 b,CM-7 b</t>
         </is>
       </c>
       <c r="B180" s="2" t="inlineStr">
@@ -14333,7 +14341,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">
@@ -14416,7 +14424,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B182" s="2" t="inlineStr">
@@ -14494,7 +14502,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B183" s="2" t="inlineStr">
@@ -14585,7 +14593,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B184" s="2" t="inlineStr">
@@ -14667,7 +14675,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B185" s="2" t="inlineStr">
@@ -15239,7 +15247,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-3</t>
+          <t>AU-3,CM-6 b</t>
         </is>
       </c>
       <c r="B192" s="2" t="inlineStr">
@@ -15673,7 +15681,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-3</t>
+          <t>AU-3,AU-4 (1)</t>
         </is>
       </c>
       <c r="B198" s="2" t="inlineStr">
@@ -17026,7 +17034,7 @@
     <row r="214" ht="130" customHeight="1">
       <c r="A214" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-2 (4),AC-6 (9)</t>
+          <t>AC-2 (4),AC-6 (9),AU-12 c</t>
         </is>
       </c>
       <c r="B214" s="2" t="inlineStr">
@@ -17546,7 +17554,7 @@
     <row r="220" ht="130" customHeight="1">
       <c r="A220" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (4),IA-2,IA-2 (3),IA-2 (5)</t>
+          <t>IA-2,IA-2 (5),IA-2 (3),IA-2 (2),IA-2 (4)</t>
         </is>
       </c>
       <c r="B220" s="2" t="inlineStr">
@@ -17631,7 +17639,7 @@
     <row r="221" ht="130" customHeight="1">
       <c r="A221" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (4),IA-2,IA-2 (3),IA-2 (5)</t>
+          <t>IA-2,IA-2 (5),IA-2 (3),IA-2 (2),IA-2 (4)</t>
         </is>
       </c>
       <c r="B221" s="2" t="inlineStr">
@@ -17716,7 +17724,7 @@
     <row r="222" ht="130" customHeight="1">
       <c r="A222" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-18 (1),SC-8 (1)</t>
+          <t>AC-18 (1),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B222" s="2" t="inlineStr">
@@ -17966,7 +17974,7 @@
     <row r="225" ht="130" customHeight="1">
       <c r="A225" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B225" s="2" t="inlineStr">
@@ -18042,7 +18050,7 @@
     <row r="226" ht="130" customHeight="1">
       <c r="A226" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B226" s="2" t="inlineStr">
@@ -18127,7 +18135,7 @@
     <row r="227" ht="130" customHeight="1">
       <c r="A227" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B227" s="2" t="inlineStr">
@@ -19366,7 +19374,7 @@
     <row r="243" ht="130" customHeight="1">
       <c r="A243" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-16,SC-2</t>
+          <t>CM-6 b,SC-2,SI-16</t>
         </is>
       </c>
       <c r="B243" s="2" t="inlineStr">
@@ -20440,7 +20448,7 @@
     <row r="257" ht="130" customHeight="1">
       <c r="A257" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B257" s="2" t="inlineStr">
@@ -20515,7 +20523,7 @@
     <row r="258" ht="130" customHeight="1">
       <c r="A258" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B258" s="2" t="inlineStr">
@@ -20603,7 +20611,7 @@
     <row r="259" ht="130" customHeight="1">
       <c r="A259" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B259" s="2" t="inlineStr">
@@ -20680,7 +20688,7 @@
     <row r="260" ht="130" customHeight="1">
       <c r="A260" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B260" s="2" t="inlineStr">
@@ -21365,7 +21373,7 @@
     <row r="269" ht="130" customHeight="1">
       <c r="A269" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (1),IA-2 (2),IA-2 (4)</t>
+          <t>IA-2 (1),IA-2 (3),IA-2 (2),IA-2 (4)</t>
         </is>
       </c>
       <c r="B269" s="2" t="inlineStr">
@@ -21752,7 +21760,7 @@
     <row r="274" ht="130" customHeight="1">
       <c r="A274" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-4</t>
+          <t>SC-4,CM-6 b</t>
         </is>
       </c>
       <c r="B274" s="2" t="inlineStr">
@@ -22159,7 +22167,7 @@
     <row r="279" ht="130" customHeight="1">
       <c r="A279" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-12 a</t>
+          <t>AU-12 a,CM-6 b</t>
         </is>
       </c>
       <c r="B279" s="2" t="inlineStr">
@@ -23739,7 +23747,7 @@
     <row r="299" ht="130" customHeight="1">
       <c r="A299" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12),IA-2 (1)</t>
+          <t>IA-2 (1),IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B299" s="2" t="inlineStr">
@@ -24561,7 +24569,7 @@
     <row r="309" ht="130" customHeight="1">
       <c r="A309" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (a),AU-8 (1) (b),AU-8 b</t>
+          <t>AU-8 b,AU-8 (1) (b),AU-8 (1) (a)</t>
         </is>
       </c>
       <c r="B309" s="2" t="inlineStr">
@@ -26052,7 +26060,7 @@
     <row r="328" ht="130" customHeight="1">
       <c r="A328" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,CM-5 (1)</t>
+          <t>CM-5 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B328" s="2" t="inlineStr">
@@ -27128,7 +27136,7 @@
     <row r="342" ht="130" customHeight="1">
       <c r="A342" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,IA-3</t>
+          <t>IA-3,CM-7 b</t>
         </is>
       </c>
       <c r="B342" s="2" t="inlineStr">
@@ -27514,7 +27522,7 @@
     <row r="347" ht="130" customHeight="1">
       <c r="A347" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,IA-5 (1) (c),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (c),CM-7 a</t>
         </is>
       </c>
       <c r="B347" s="2" t="inlineStr">
@@ -28359,7 +28367,7 @@
     <row r="358" ht="130" customHeight="1">
       <c r="A358" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 (1)</t>
+          <t>AC-11 (1),AC-11 b</t>
         </is>
       </c>
       <c r="B358" s="2" t="inlineStr">
@@ -28608,7 +28616,7 @@
     <row r="361" ht="130" customHeight="1">
       <c r="A361" s="2" t="inlineStr">
         <is>
-          <t>SI-6 b,CM-3 (5),SI-6 d</t>
+          <t>CM-3 (5),SI-6 d,SI-6 b</t>
         </is>
       </c>
       <c r="B361" s="2" t="inlineStr">
@@ -28699,7 +28707,7 @@
     <row r="362" ht="130" customHeight="1">
       <c r="A362" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B362" s="2" t="inlineStr">
@@ -30531,7 +30539,7 @@
     <row r="385" ht="130" customHeight="1">
       <c r="A385" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-17 (2)</t>
+          <t>AC-17 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B385" s="2" t="inlineStr">
@@ -30840,7 +30848,7 @@
     <row r="389" ht="130" customHeight="1">
       <c r="A389" s="2" t="inlineStr">
         <is>
-          <t>SI-6 a,SC-3</t>
+          <t>SC-3,SI-6 a</t>
         </is>
       </c>
       <c r="B389" s="2" t="inlineStr">
@@ -30979,7 +30987,7 @@
     <row r="391" ht="130" customHeight="1">
       <c r="A391" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (a)</t>
+          <t>IA-5 (1) (a),CM-6 b</t>
         </is>
       </c>
       <c r="B391" s="2" t="inlineStr">
@@ -31793,7 +31801,7 @@
     <row r="401" ht="130" customHeight="1">
       <c r="A401" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B401" s="2" t="inlineStr">
@@ -31884,7 +31892,7 @@
     <row r="402" ht="130" customHeight="1">
       <c r="A402" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B402" s="2" t="inlineStr">
@@ -31978,7 +31986,7 @@
     <row r="403" ht="130" customHeight="1">
       <c r="A403" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B403" s="2" t="inlineStr">
@@ -35388,7 +35396,7 @@
     <row r="448" ht="130" customHeight="1">
       <c r="A448" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),CM-6 b</t>
         </is>
       </c>
       <c r="B448" s="2" t="inlineStr">
@@ -42742,7 +42750,7 @@
     <row r="541" ht="130" customHeight="1">
       <c r="A541" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-2 (2)</t>
+          <t>SI-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B541" s="2" t="inlineStr">
@@ -43389,7 +43397,7 @@
     <row r="550" ht="130" customHeight="1">
       <c r="A550" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-2 (2)</t>
+          <t>SI-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B550" s="2" t="inlineStr">
@@ -43997,7 +44005,7 @@
     <row r="558" ht="130" customHeight="1">
       <c r="A558" s="2" t="inlineStr">
         <is>
-          <t>SI-6 a,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 a</t>
         </is>
       </c>
       <c r="B558" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@385eb47db2464176d23e3cb36c1855bfc97c5200 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -625,7 +625,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),AU-4</t>
+          <t>AU-4,AU-14 (1)</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -784,7 +784,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>SC-5 (2),CM-6 b,SC-5</t>
+          <t>CM-6 b,SC-5 (2),SC-5</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -883,7 +883,7 @@
     <row r="6" ht="130" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>AU-12 (3),AU-7 b,AU-8 b,AC-6 (8),AC-6 (9),CM-5 (1),AU-7 a</t>
+          <t>AU-7 b,AC-6 (9),CM-5 (1),AU-8 b,AC-6 (8),AU-7 a,AU-12 (3)</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -963,7 +963,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-12 (3),CM-6 b,AU-12 c,AU-7 b,AU-8 b,AU-12 a,CM-5 (1),AU-7 a</t>
+          <t>AU-12 (3),AU-7 b,AU-8 b,CM-6 b,AU-12 a,AU-7 a,AU-12 c,CM-5 (1)</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1269,7 +1269,7 @@
     <row r="11" ht="130" customHeight="1">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B11" s="2" t="inlineStr">
@@ -1650,7 +1650,7 @@
     <row r="16" ht="130" customHeight="1">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
@@ -2020,7 +2020,7 @@
     <row r="21" ht="130" customHeight="1">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
@@ -2094,7 +2094,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -3222,7 +3222,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3306,7 +3306,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3391,7 +3391,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3463,7 +3463,7 @@
     <row r="40" ht="130" customHeight="1">
       <c r="A40" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B40" s="2" t="inlineStr">
@@ -3768,7 +3768,7 @@
     <row r="44" ht="130" customHeight="1">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>IA-8,IA-2,AU-3 (1)</t>
+          <t>IA-2,AU-3 (1),IA-8</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
@@ -3846,7 +3846,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3921,7 +3921,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -3996,7 +3996,7 @@
     <row r="47" ht="130" customHeight="1">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
@@ -4071,7 +4071,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4146,7 +4146,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4221,7 +4221,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4296,7 +4296,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4371,7 +4371,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
@@ -4446,7 +4446,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4521,7 +4521,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4596,7 +4596,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4671,7 +4671,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4746,7 +4746,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4821,7 +4821,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4901,7 +4901,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -4984,7 +4984,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5064,7 +5064,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5144,7 +5144,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5224,7 +5224,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5304,7 +5304,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5378,7 +5378,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5452,7 +5452,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5526,7 +5526,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5600,7 +5600,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5674,7 +5674,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5747,7 +5747,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5820,7 +5820,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5893,7 +5893,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -5966,7 +5966,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6039,7 +6039,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6112,7 +6112,7 @@
     <row r="75" ht="130" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
@@ -6186,7 +6186,7 @@
     <row r="76" ht="130" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
@@ -6260,7 +6260,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6334,7 +6334,7 @@
     <row r="78" ht="130" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
@@ -6412,7 +6412,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6492,7 +6492,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6572,7 +6572,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6652,7 +6652,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B82" s="2" t="inlineStr">
@@ -6732,7 +6732,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B83" s="2" t="inlineStr">
@@ -6812,7 +6812,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B84" s="2" t="inlineStr">
@@ -6892,7 +6892,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B85" s="2" t="inlineStr">
@@ -6972,7 +6972,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -7052,7 +7052,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7132,7 +7132,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7212,7 +7212,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7292,7 +7292,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7368,7 +7368,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7445,7 +7445,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
@@ -7525,7 +7525,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
@@ -7605,7 +7605,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B94" s="2" t="inlineStr">
@@ -7685,7 +7685,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
@@ -7765,7 +7765,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7845,7 +7845,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7925,7 +7925,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8005,7 +8005,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8085,7 +8085,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8165,7 +8165,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8238,7 +8238,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AC-2 (4),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8319,7 +8319,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AC-2 (4),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8400,7 +8400,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AC-2 (4),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8471,7 +8471,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>MA-4 (1) (a),AC-2 (4),AU-3,AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8546,7 +8546,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AC-2 (4),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8628,7 +8628,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AC-2 (4),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8710,7 +8710,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AC-2 (4),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -8792,7 +8792,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AC-2 (4),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -8874,7 +8874,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>MA-4 (1) (a),AC-2 (4),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B110" s="2" t="inlineStr">
@@ -8956,7 +8956,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AU-14 (1),MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-14 (1),MA-4 (1) (a),AU-3,AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9048,7 +9048,7 @@
     <row r="112" ht="130" customHeight="1">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
@@ -9129,7 +9129,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9293,7 +9293,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9659,7 +9659,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9730,7 +9730,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -9801,7 +9801,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-12 c</t>
+          <t>AU-12 c,AU-9</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -10174,7 +10174,7 @@
     <row r="126" ht="130" customHeight="1">
       <c r="A126" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),CM-5 (1),AC-6 (9),AU-12 c</t>
+          <t>AU-12 c,AC-2 (4),AC-6 (9),CM-5 (1)</t>
         </is>
       </c>
       <c r="B126" s="2" t="inlineStr">
@@ -10312,7 +10312,7 @@
     <row r="128" ht="130" customHeight="1">
       <c r="A128" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (a),IA-5 (1) (b),CM-6 b</t>
+          <t>IA-5 (1) (a),CM-6 b,IA-5 (1) (b)</t>
         </is>
       </c>
       <c r="B128" s="2" t="inlineStr">
@@ -10640,7 +10640,7 @@
     <row r="132" ht="130" customHeight="1">
       <c r="A132" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-13,AC-17 (2),MA-4 c</t>
+          <t>SC-13,SC-8,MA-4 c,AC-17 (2)</t>
         </is>
       </c>
       <c r="B132" s="2" t="inlineStr">
@@ -10722,7 +10722,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>MA-4 e,MA-4 (7),SC-10,AC-12</t>
+          <t>AC-12,MA-4 e,MA-4 (7),SC-10</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10797,7 +10797,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>SC-10,AC-12</t>
+          <t>AC-12,SC-10</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -10876,7 +10876,7 @@
     <row r="135" ht="130" customHeight="1">
       <c r="A135" s="2" t="inlineStr">
         <is>
-          <t>SC-10,AC-12</t>
+          <t>AC-12,SC-10</t>
         </is>
       </c>
       <c r="B135" s="2" t="inlineStr">
@@ -11029,7 +11029,7 @@
     <row r="137" ht="130" customHeight="1">
       <c r="A137" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),CM-6 b,AU-14 (1),MA-4 (1) (a),AU-12 a,AU-6 (4),CM-5 (1),AU-3,AU-7 (1),AU-7 a</t>
+          <t>AU-14 (1),MA-4 (1) (a),AU-7 (1),AU-3,CM-6 b,AU-3 (1),AU-12 a,AU-6 (4),AU-7 a,CM-5 (1)</t>
         </is>
       </c>
       <c r="B137" s="2" t="inlineStr">
@@ -11279,7 +11279,7 @@
     <row r="140" ht="130" customHeight="1">
       <c r="A140" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B140" s="2" t="inlineStr">
@@ -11355,7 +11355,7 @@
     <row r="141" ht="130" customHeight="1">
       <c r="A141" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B141" s="2" t="inlineStr">
@@ -11431,7 +11431,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B142" s="2" t="inlineStr">
@@ -11500,7 +11500,7 @@
     <row r="143" ht="130" customHeight="1">
       <c r="A143" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B143" s="2" t="inlineStr">
@@ -11569,7 +11569,7 @@
     <row r="144" ht="130" customHeight="1">
       <c r="A144" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B144" s="2" t="inlineStr">
@@ -11639,7 +11639,7 @@
     <row r="145" ht="130" customHeight="1">
       <c r="A145" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B145" s="2" t="inlineStr">
@@ -11708,7 +11708,7 @@
     <row r="146" ht="130" customHeight="1">
       <c r="A146" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B146" s="2" t="inlineStr">
@@ -11777,7 +11777,7 @@
     <row r="147" ht="130" customHeight="1">
       <c r="A147" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B147" s="2" t="inlineStr">
@@ -11847,7 +11847,7 @@
     <row r="148" ht="130" customHeight="1">
       <c r="A148" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B148" s="2" t="inlineStr">
@@ -11916,7 +11916,7 @@
     <row r="149" ht="130" customHeight="1">
       <c r="A149" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B149" s="2" t="inlineStr">
@@ -11985,7 +11985,7 @@
     <row r="150" ht="130" customHeight="1">
       <c r="A150" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B150" s="2" t="inlineStr">
@@ -12055,7 +12055,7 @@
     <row r="151" ht="130" customHeight="1">
       <c r="A151" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B151" s="2" t="inlineStr">
@@ -12124,7 +12124,7 @@
     <row r="152" ht="130" customHeight="1">
       <c r="A152" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B152" s="2" t="inlineStr">
@@ -12193,7 +12193,7 @@
     <row r="153" ht="130" customHeight="1">
       <c r="A153" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B153" s="2" t="inlineStr">
@@ -12262,7 +12262,7 @@
     <row r="154" ht="130" customHeight="1">
       <c r="A154" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B154" s="2" t="inlineStr">
@@ -13100,7 +13100,7 @@
     <row r="165" ht="130" customHeight="1">
       <c r="A165" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8,SC-8 (2)</t>
+          <t>SC-8 (2),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B165" s="2" t="inlineStr">
@@ -13177,7 +13177,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8,SC-8 (2)</t>
+          <t>SC-8 (2),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B166" s="2" t="inlineStr">
@@ -13263,7 +13263,7 @@
     <row r="167" ht="130" customHeight="1">
       <c r="A167" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8</t>
+          <t>SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B167" s="2" t="inlineStr">
@@ -13424,7 +13424,7 @@
     <row r="169" ht="130" customHeight="1">
       <c r="A169" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8</t>
+          <t>SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B169" s="2" t="inlineStr">
@@ -14185,7 +14185,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (9),AC-17 (1),CM-6 b,CM-7 b</t>
+          <t>CM-7 b,AC-17 (9),CM-6 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B179" s="2" t="inlineStr">
@@ -14262,7 +14262,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),CM-6 b,CM-7 b</t>
+          <t>CM-7 b,CM-6 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B180" s="2" t="inlineStr">
@@ -15247,7 +15247,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="2" t="inlineStr">
         <is>
-          <t>AU-3,CM-6 b</t>
+          <t>CM-6 b,AU-3</t>
         </is>
       </c>
       <c r="B192" s="2" t="inlineStr">
@@ -16196,7 +16196,7 @@
     <row r="205" ht="130" customHeight="1">
       <c r="A205" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),CM-6 b</t>
+          <t>CM-6 b,AU-4 (1)</t>
         </is>
       </c>
       <c r="B205" s="2" t="inlineStr">
@@ -16276,7 +16276,7 @@
     <row r="206" ht="130" customHeight="1">
       <c r="A206" s="2" t="inlineStr">
         <is>
-          <t>SC-28 (1),SC-28</t>
+          <t>SC-28,SC-28 (1)</t>
         </is>
       </c>
       <c r="B206" s="2" t="inlineStr">
@@ -16602,7 +16602,7 @@
     <row r="210" ht="130" customHeight="1">
       <c r="A210" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B210" s="2" t="inlineStr">
@@ -16704,7 +16704,7 @@
     <row r="211" ht="130" customHeight="1">
       <c r="A211" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B211" s="2" t="inlineStr">
@@ -16814,7 +16814,7 @@
     <row r="212" ht="130" customHeight="1">
       <c r="A212" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B212" s="2" t="inlineStr">
@@ -16925,7 +16925,7 @@
     <row r="213" ht="130" customHeight="1">
       <c r="A213" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B213" s="2" t="inlineStr">
@@ -17034,7 +17034,7 @@
     <row r="214" ht="130" customHeight="1">
       <c r="A214" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AC-6 (9),AU-12 c</t>
+          <t>AU-12 c,AC-2 (4),AC-6 (9)</t>
         </is>
       </c>
       <c r="B214" s="2" t="inlineStr">
@@ -17554,7 +17554,7 @@
     <row r="220" ht="130" customHeight="1">
       <c r="A220" s="2" t="inlineStr">
         <is>
-          <t>IA-2,IA-2 (5),IA-2 (3),IA-2 (2),IA-2 (4)</t>
+          <t>IA-2 (5),IA-2 (2),IA-2,IA-2 (4),IA-2 (3)</t>
         </is>
       </c>
       <c r="B220" s="2" t="inlineStr">
@@ -17639,7 +17639,7 @@
     <row r="221" ht="130" customHeight="1">
       <c r="A221" s="2" t="inlineStr">
         <is>
-          <t>IA-2,IA-2 (5),IA-2 (3),IA-2 (2),IA-2 (4)</t>
+          <t>IA-2 (5),IA-2 (2),IA-2,IA-2 (4),IA-2 (3)</t>
         </is>
       </c>
       <c r="B221" s="2" t="inlineStr">
@@ -17724,7 +17724,7 @@
     <row r="222" ht="130" customHeight="1">
       <c r="A222" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),SC-8 (1),SC-8</t>
+          <t>SC-8,SC-8 (1),AC-18 (1)</t>
         </is>
       </c>
       <c r="B222" s="2" t="inlineStr">
@@ -17891,7 +17891,7 @@
     <row r="224" ht="130" customHeight="1">
       <c r="A224" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),IA-7</t>
+          <t>IA-7,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B224" s="2" t="inlineStr">
@@ -17974,7 +17974,7 @@
     <row r="225" ht="130" customHeight="1">
       <c r="A225" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B225" s="2" t="inlineStr">
@@ -18050,7 +18050,7 @@
     <row r="226" ht="130" customHeight="1">
       <c r="A226" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B226" s="2" t="inlineStr">
@@ -18135,7 +18135,7 @@
     <row r="227" ht="130" customHeight="1">
       <c r="A227" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B227" s="2" t="inlineStr">
@@ -18455,7 +18455,7 @@
     <row r="231" ht="130" customHeight="1">
       <c r="A231" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),AC-17 (2)</t>
+          <t>AC-17 (2),MA-4 (6)</t>
         </is>
       </c>
       <c r="B231" s="2" t="inlineStr">
@@ -21373,7 +21373,7 @@
     <row r="269" ht="130" customHeight="1">
       <c r="A269" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (3),IA-2 (2),IA-2 (4)</t>
+          <t>IA-2 (2),IA-2 (4),IA-2 (1),IA-2 (3)</t>
         </is>
       </c>
       <c r="B269" s="2" t="inlineStr">
@@ -21760,7 +21760,7 @@
     <row r="274" ht="130" customHeight="1">
       <c r="A274" s="2" t="inlineStr">
         <is>
-          <t>SC-4,CM-6 b</t>
+          <t>CM-6 b,SC-4</t>
         </is>
       </c>
       <c r="B274" s="2" t="inlineStr">
@@ -21841,7 +21841,7 @@
     <row r="275" ht="130" customHeight="1">
       <c r="A275" s="2" t="inlineStr">
         <is>
-          <t>SC-4,SC-2</t>
+          <t>SC-2,SC-4</t>
         </is>
       </c>
       <c r="B275" s="2" t="inlineStr">
@@ -21929,7 +21929,7 @@
     <row r="276" ht="130" customHeight="1">
       <c r="A276" s="2" t="inlineStr">
         <is>
-          <t>SC-4,SC-2</t>
+          <t>SC-2,SC-4</t>
         </is>
       </c>
       <c r="B276" s="2" t="inlineStr">
@@ -22167,7 +22167,7 @@
     <row r="279" ht="130" customHeight="1">
       <c r="A279" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,CM-6 b</t>
+          <t>CM-6 b,AU-12 a</t>
         </is>
       </c>
       <c r="B279" s="2" t="inlineStr">
@@ -23568,7 +23568,7 @@
     <row r="297" ht="130" customHeight="1">
       <c r="A297" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B297" s="2" t="inlineStr">
@@ -23747,7 +23747,7 @@
     <row r="299" ht="130" customHeight="1">
       <c r="A299" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11),IA-2 (1)</t>
         </is>
       </c>
       <c r="B299" s="2" t="inlineStr">
@@ -24569,7 +24569,7 @@
     <row r="309" ht="130" customHeight="1">
       <c r="A309" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-8 (1) (b),AU-8 (1) (a)</t>
+          <t>AU-8 (1) (a),AU-8 b,AU-8 (1) (b)</t>
         </is>
       </c>
       <c r="B309" s="2" t="inlineStr">
@@ -25596,7 +25596,7 @@
     <row r="322" ht="130" customHeight="1">
       <c r="A322" s="2" t="inlineStr">
         <is>
-          <t>IA-11,AC-3 (4)</t>
+          <t>AC-3 (4),IA-11</t>
         </is>
       </c>
       <c r="B322" s="2" t="inlineStr">
@@ -26060,7 +26060,7 @@
     <row r="328" ht="130" customHeight="1">
       <c r="A328" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AU-12 c</t>
+          <t>AU-12 c,CM-5 (1)</t>
         </is>
       </c>
       <c r="B328" s="2" t="inlineStr">
@@ -26217,7 +26217,7 @@
     <row r="330" ht="130" customHeight="1">
       <c r="A330" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 b</t>
+          <t>AU-5 b,AU-5 a</t>
         </is>
       </c>
       <c r="B330" s="2" t="inlineStr">
@@ -27211,7 +27211,7 @@
     <row r="343" ht="130" customHeight="1">
       <c r="A343" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-7 b</t>
+          <t>CM-7 b,CM-7 a</t>
         </is>
       </c>
       <c r="B343" s="2" t="inlineStr">
@@ -27285,7 +27285,7 @@
     <row r="344" ht="130" customHeight="1">
       <c r="A344" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-7 b</t>
+          <t>CM-7 b,CM-7 a</t>
         </is>
       </c>
       <c r="B344" s="2" t="inlineStr">
@@ -27359,7 +27359,7 @@
     <row r="345" ht="130" customHeight="1">
       <c r="A345" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),CM-7 b</t>
+          <t>CM-7 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B345" s="2" t="inlineStr">
@@ -27522,7 +27522,7 @@
     <row r="347" ht="130" customHeight="1">
       <c r="A347" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (c),CM-7 a</t>
+          <t>CM-6 b,CM-7 a,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B347" s="2" t="inlineStr">
@@ -28707,7 +28707,7 @@
     <row r="362" ht="130" customHeight="1">
       <c r="A362" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B362" s="2" t="inlineStr">
@@ -29636,7 +29636,7 @@
     <row r="374" ht="130" customHeight="1">
       <c r="A374" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B374" s="2" t="inlineStr">
@@ -29707,7 +29707,7 @@
     <row r="375" ht="130" customHeight="1">
       <c r="A375" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B375" s="2" t="inlineStr">
@@ -29779,7 +29779,7 @@
     <row r="376" ht="130" customHeight="1">
       <c r="A376" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B376" s="2" t="inlineStr">
@@ -30539,7 +30539,7 @@
     <row r="385" ht="130" customHeight="1">
       <c r="A385" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),CM-6 b</t>
+          <t>CM-6 b,AC-17 (2)</t>
         </is>
       </c>
       <c r="B385" s="2" t="inlineStr">
@@ -30848,7 +30848,7 @@
     <row r="389" ht="130" customHeight="1">
       <c r="A389" s="2" t="inlineStr">
         <is>
-          <t>SC-3,SI-6 a</t>
+          <t>SI-6 a,SC-3</t>
         </is>
       </c>
       <c r="B389" s="2" t="inlineStr">
@@ -30987,7 +30987,7 @@
     <row r="391" ht="130" customHeight="1">
       <c r="A391" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (a),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (a)</t>
         </is>
       </c>
       <c r="B391" s="2" t="inlineStr">
@@ -31801,7 +31801,7 @@
     <row r="401" ht="130" customHeight="1">
       <c r="A401" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B401" s="2" t="inlineStr">
@@ -31892,7 +31892,7 @@
     <row r="402" ht="130" customHeight="1">
       <c r="A402" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B402" s="2" t="inlineStr">
@@ -31986,7 +31986,7 @@
     <row r="403" ht="130" customHeight="1">
       <c r="A403" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B403" s="2" t="inlineStr">
@@ -35396,7 +35396,7 @@
     <row r="448" ht="130" customHeight="1">
       <c r="A448" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B448" s="2" t="inlineStr">
@@ -43397,7 +43397,7 @@
     <row r="550" ht="130" customHeight="1">
       <c r="A550" s="2" t="inlineStr">
         <is>
-          <t>SI-2 (2),CM-6 b</t>
+          <t>CM-6 b,SI-2 (2)</t>
         </is>
       </c>
       <c r="B550" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@192996d107c705938cf398c416cbef21c75050a8 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -541,7 +541,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-4</t>
+          <t>AU-4,AU-4 (1)</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -625,7 +625,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),AU-4</t>
+          <t>AU-4,AU-14 (1)</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -708,7 +708,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-4</t>
+          <t>AU-4,CM-6 b</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -883,7 +883,7 @@
     <row r="6" ht="130" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (1),AU-12 c,AU-12 a,AU-8 b,AU-7 b,AU-7 a,AU-12 (3)</t>
+          <t>AU-12 (3),AU-7 b,CM-6 b,CM-5 (1),AU-12 c,AU-7 a,AU-8 b,AU-12 a</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -957,7 +957,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-7 (1),CM-6 b,CM-5 (1),AU-14 (1),MA-4 (1) (a),AU-6 (4),AU-3,AU-12 a,AU-3 (1),AU-7 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-6 (4),CM-6 b,CM-5 (1),AU-7 a,AU-7 (1),MA-4 (1) (a),AU-14 (1)</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1654,7 +1654,7 @@
     <row r="16" ht="130" customHeight="1">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
@@ -2024,7 +2024,7 @@
     <row r="21" ht="130" customHeight="1">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
@@ -2098,7 +2098,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -3772,7 +3772,7 @@
     <row r="44" ht="130" customHeight="1">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),IA-2,IA-8</t>
+          <t>IA-8,IA-2,AU-3 (1)</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
@@ -3850,7 +3850,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3925,7 +3925,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -4000,7 +4000,7 @@
     <row r="47" ht="130" customHeight="1">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
@@ -4075,7 +4075,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4150,7 +4150,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4225,7 +4225,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4300,7 +4300,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4375,7 +4375,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
@@ -4450,7 +4450,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4525,7 +4525,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4600,7 +4600,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4675,7 +4675,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4750,7 +4750,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4825,7 +4825,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4905,7 +4905,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -4988,7 +4988,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5068,7 +5068,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5148,7 +5148,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5228,7 +5228,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5308,7 +5308,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5382,7 +5382,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5456,7 +5456,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5530,7 +5530,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5604,7 +5604,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5678,7 +5678,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5751,7 +5751,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5824,7 +5824,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5897,7 +5897,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -5970,7 +5970,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6043,7 +6043,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6116,7 +6116,7 @@
     <row r="75" ht="130" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
@@ -6190,7 +6190,7 @@
     <row r="76" ht="130" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
@@ -6264,7 +6264,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6338,7 +6338,7 @@
     <row r="78" ht="130" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
@@ -6416,7 +6416,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6496,7 +6496,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6576,7 +6576,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6656,7 +6656,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B82" s="2" t="inlineStr">
@@ -6736,7 +6736,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B83" s="2" t="inlineStr">
@@ -6816,7 +6816,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B84" s="2" t="inlineStr">
@@ -6896,7 +6896,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B85" s="2" t="inlineStr">
@@ -6976,7 +6976,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -7056,7 +7056,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7136,7 +7136,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7216,7 +7216,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7296,7 +7296,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7372,7 +7372,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7449,7 +7449,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
@@ -7529,7 +7529,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
@@ -7609,7 +7609,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B94" s="2" t="inlineStr">
@@ -7689,7 +7689,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
@@ -7769,7 +7769,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7849,7 +7849,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7929,7 +7929,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8009,7 +8009,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8089,7 +8089,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8169,7 +8169,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8242,7 +8242,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-2 (4),MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8323,7 +8323,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-2 (4),MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8404,7 +8404,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-2 (4),MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8475,7 +8475,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-2 (4),MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-3,AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8550,7 +8550,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-2 (4),MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8632,7 +8632,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-2 (4),MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8714,7 +8714,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-2 (4),MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -8796,7 +8796,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-2 (4),MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -8878,7 +8878,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-2 (4),MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B110" s="2" t="inlineStr">
@@ -8960,7 +8960,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3,AU-12 a,AU-3 (1),AU-14 (1)</t>
+          <t>AU-3,AU-3 (1),AU-12 c,AU-14 (1),MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9052,7 +9052,7 @@
     <row r="112" ht="130" customHeight="1">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
@@ -9133,7 +9133,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9297,7 +9297,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9663,7 +9663,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9734,7 +9734,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -9934,7 +9934,7 @@
     <row r="123" ht="130" customHeight="1">
       <c r="A123" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (b),IA-5 (1) (a)</t>
+          <t>IA-5 (1) (a),CM-6 b,IA-5 (1) (b)</t>
         </is>
       </c>
       <c r="B123" s="2" t="inlineStr">
@@ -10262,7 +10262,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-13,MA-4 c,SC-8</t>
+          <t>SC-8,SC-13,MA-4 c,AC-17 (2)</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -10344,7 +10344,7 @@
     <row r="128" ht="130" customHeight="1">
       <c r="A128" s="2" t="inlineStr">
         <is>
-          <t>MA-4 e,AC-12,MA-4 (7),SC-10</t>
+          <t>AC-12,MA-4 e,MA-4 (7),SC-10</t>
         </is>
       </c>
       <c r="B128" s="2" t="inlineStr">
@@ -10574,7 +10574,7 @@
     <row r="131" ht="130" customHeight="1">
       <c r="A131" s="2" t="inlineStr">
         <is>
-          <t>SC-10,AC-11 a</t>
+          <t>AC-11 a,SC-10</t>
         </is>
       </c>
       <c r="B131" s="2" t="inlineStr">
@@ -10817,7 +10817,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>AU-9 (3),AU-9</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -10893,7 +10893,7 @@
     <row r="135" ht="130" customHeight="1">
       <c r="A135" s="2" t="inlineStr">
         <is>
-          <t>AU-9 (3),AU-9</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B135" s="2" t="inlineStr">
@@ -12337,7 +12337,7 @@
     <row r="155" ht="130" customHeight="1">
       <c r="A155" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8</t>
+          <t>SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B155" s="2" t="inlineStr">
@@ -12486,7 +12486,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B157" s="2" t="inlineStr">
@@ -12564,7 +12564,7 @@
     <row r="158" ht="130" customHeight="1">
       <c r="A158" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B158" s="2" t="inlineStr">
@@ -12647,7 +12647,7 @@
     <row r="159" ht="130" customHeight="1">
       <c r="A159" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B159" s="2" t="inlineStr">
@@ -13098,7 +13098,7 @@
     <row r="165" ht="130" customHeight="1">
       <c r="A165" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 b,AC-17 (9),AC-17 (1)</t>
+          <t>AC-17 (9),CM-7 b,CM-6 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B165" s="2" t="inlineStr">
@@ -13175,7 +13175,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 b,AC-17 (1)</t>
+          <t>CM-7 b,CM-6 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B166" s="2" t="inlineStr">
@@ -13254,7 +13254,7 @@
     <row r="167" ht="130" customHeight="1">
       <c r="A167" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B167" s="2" t="inlineStr">
@@ -13337,7 +13337,7 @@
     <row r="168" ht="130" customHeight="1">
       <c r="A168" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B168" s="2" t="inlineStr">
@@ -13415,7 +13415,7 @@
     <row r="169" ht="130" customHeight="1">
       <c r="A169" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B169" s="2" t="inlineStr">
@@ -13506,7 +13506,7 @@
     <row r="170" ht="130" customHeight="1">
       <c r="A170" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B170" s="2" t="inlineStr">
@@ -13588,7 +13588,7 @@
     <row r="171" ht="130" customHeight="1">
       <c r="A171" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B171" s="2" t="inlineStr">
@@ -14160,7 +14160,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-3</t>
+          <t>AU-3,CM-6 b</t>
         </is>
       </c>
       <c r="B178" s="2" t="inlineStr">
@@ -15109,7 +15109,7 @@
     <row r="191" ht="130" customHeight="1">
       <c r="A191" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-4 (1)</t>
+          <t>AU-4 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B191" s="2" t="inlineStr">
@@ -16389,7 +16389,7 @@
     <row r="205" ht="130" customHeight="1">
       <c r="A205" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (5)</t>
+          <t>IA-2 (5),CM-6 b</t>
         </is>
       </c>
       <c r="B205" s="2" t="inlineStr">
@@ -16467,7 +16467,7 @@
     <row r="206" ht="130" customHeight="1">
       <c r="A206" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (5),IA-2 (4),IA-2,IA-2 (2)</t>
+          <t>IA-2,IA-2 (3),IA-2 (4),IA-2 (2),IA-2 (5)</t>
         </is>
       </c>
       <c r="B206" s="2" t="inlineStr">
@@ -16552,7 +16552,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (5),IA-2 (4),IA-2,IA-2 (2)</t>
+          <t>IA-2,IA-2 (3),IA-2 (4),IA-2 (2),IA-2 (5)</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -16804,7 +16804,7 @@
     <row r="210" ht="130" customHeight="1">
       <c r="A210" s="2" t="inlineStr">
         <is>
-          <t>IA-7,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),IA-7</t>
         </is>
       </c>
       <c r="B210" s="2" t="inlineStr">
@@ -17205,7 +17205,7 @@
     <row r="215" ht="130" customHeight="1">
       <c r="A215" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-7 a</t>
+          <t>CM-7 a,IA-7</t>
         </is>
       </c>
       <c r="B215" s="2" t="inlineStr">
@@ -17368,7 +17368,7 @@
     <row r="217" ht="130" customHeight="1">
       <c r="A217" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),MA-4 (6)</t>
+          <t>MA-4 (6),AC-17 (2)</t>
         </is>
       </c>
       <c r="B217" s="2" t="inlineStr">
@@ -19361,7 +19361,7 @@
     <row r="243" ht="130" customHeight="1">
       <c r="A243" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B243" s="2" t="inlineStr">
@@ -19436,7 +19436,7 @@
     <row r="244" ht="130" customHeight="1">
       <c r="A244" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B244" s="2" t="inlineStr">
@@ -19524,7 +19524,7 @@
     <row r="245" ht="130" customHeight="1">
       <c r="A245" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B245" s="2" t="inlineStr">
@@ -19601,7 +19601,7 @@
     <row r="246" ht="130" customHeight="1">
       <c r="A246" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B246" s="2" t="inlineStr">
@@ -20199,7 +20199,7 @@
     <row r="254" ht="130" customHeight="1">
       <c r="A254" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (2)</t>
+          <t>IA-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B254" s="2" t="inlineStr">
@@ -20286,7 +20286,7 @@
     <row r="255" ht="130" customHeight="1">
       <c r="A255" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (2),IA-2 (1),IA-2 (4)</t>
+          <t>IA-2 (4),IA-2 (1),IA-2 (3),IA-2 (2)</t>
         </is>
       </c>
       <c r="B255" s="2" t="inlineStr">
@@ -20673,7 +20673,7 @@
     <row r="260" ht="130" customHeight="1">
       <c r="A260" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-4</t>
+          <t>SC-4,CM-6 b</t>
         </is>
       </c>
       <c r="B260" s="2" t="inlineStr">
@@ -21080,7 +21080,7 @@
     <row r="265" ht="130" customHeight="1">
       <c r="A265" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,CM-6 b</t>
+          <t>CM-6 b,AU-12 a</t>
         </is>
       </c>
       <c r="B265" s="2" t="inlineStr">
@@ -21303,7 +21303,7 @@
     <row r="268" ht="130" customHeight="1">
       <c r="A268" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (3)</t>
+          <t>CM-5 (3),CM-6 b</t>
         </is>
       </c>
       <c r="B268" s="2" t="inlineStr">
@@ -21379,7 +21379,14 @@
         </is>
       </c>
       <c r="L268" s="2" t="n"/>
-      <c r="M268" s="2" t="inlineStr"/>
+      <c r="M268" s="2" t="inlineStr">
+        <is>
+          <t>Add or edit the following line in a system configuration file in the "/etc/sysctl.d/" directory:
+kernel.kexec_load_disabled = 1
+Load settings from all system configuration files with the following command:
+$ sudo sysctl --system</t>
+        </is>
+      </c>
       <c r="N268" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -21457,7 +21464,12 @@
         </is>
       </c>
       <c r="L269" s="2" t="n"/>
-      <c r="M269" s="2" t="inlineStr"/>
+      <c r="M269" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The  subscription-manager  package can be installed with the following command:
+$ sudo dnf install subscription-manager </t>
+        </is>
+      </c>
       <c r="N269" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -21545,7 +21557,13 @@
         </is>
       </c>
       <c r="L270" s="2" t="n"/>
-      <c r="M270" s="2" t="inlineStr"/>
+      <c r="M270" s="2" t="inlineStr">
+        <is>
+          <t>Configure Red Hat Enterprise Linux 9 to always check package signatures before installation.
+Add or update the following line in /etc/dnf/dnf.conf:
+gpgcheck=1</t>
+        </is>
+      </c>
       <c r="N270" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -21623,7 +21641,13 @@
         </is>
       </c>
       <c r="L271" s="2" t="n"/>
-      <c r="M271" s="2" t="inlineStr"/>
+      <c r="M271" s="2" t="inlineStr">
+        <is>
+          <t>Configure Red Hat Enterprise Linux 9 to always check package signatures before installation of local packages.
+Add or update the following line in /etc/dnf/dnf.conf:
+localpkg_gpgcheck=1</t>
+        </is>
+      </c>
       <c r="N271" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -21703,7 +21727,13 @@
         </is>
       </c>
       <c r="L272" s="2" t="n"/>
-      <c r="M272" s="2" t="inlineStr"/>
+      <c r="M272" s="2" t="inlineStr">
+        <is>
+          <t>Ensure signature checking is enabled for all package repositories.
+Run the following commnad:
+$ sudo sed -i 's/gpgcheck\s*=.*/gpgcheck=1/g' /etc/yum.repos.d/*</t>
+        </is>
+      </c>
       <c r="N272" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -21780,7 +21810,12 @@
         </is>
       </c>
       <c r="L273" s="2" t="n"/>
-      <c r="M273" s="2" t="inlineStr"/>
+      <c r="M273" s="2" t="inlineStr">
+        <is>
+          <t>Install Red Hat Enterprise Linux 9 GPG key. Run the following command:
+$ sudo rpm --import "/etc/pki/rpm-gpg/RPM-GPG-KEY-redhat-release"</t>
+        </is>
+      </c>
       <c r="N273" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -21872,7 +21907,7 @@
     <row r="275" ht="130" customHeight="1">
       <c r="A275" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AC-6 (9),AU-8 b,AU-7 b,AU-7 a,AC-6 (8),AU-12 (3)</t>
+          <t>AU-12 (3),AU-7 b,CM-5 (1),AC-6 (8),AU-7 a,AU-8 b,AC-6 (9)</t>
         </is>
       </c>
       <c r="B275" s="2" t="inlineStr">
@@ -22740,7 +22775,7 @@
     <row r="286" ht="130" customHeight="1">
       <c r="A286" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (1),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (1),IA-2 (12)</t>
         </is>
       </c>
       <c r="B286" s="2" t="inlineStr">
@@ -25888,7 +25923,7 @@
     <row r="326" ht="130" customHeight="1">
       <c r="A326" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-7 b</t>
+          <t>CM-7 b,IA-3</t>
         </is>
       </c>
       <c r="B326" s="2" t="inlineStr">
@@ -26274,7 +26309,7 @@
     <row r="331" ht="130" customHeight="1">
       <c r="A331" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B331" s="2" t="inlineStr">
@@ -27368,7 +27403,7 @@
     <row r="345" ht="130" customHeight="1">
       <c r="A345" s="2" t="inlineStr">
         <is>
-          <t>SI-6 b,CM-3 (5),SI-6 d</t>
+          <t>CM-3 (5),SI-6 b,SI-6 d</t>
         </is>
       </c>
       <c r="B345" s="2" t="inlineStr">
@@ -27459,7 +27494,7 @@
     <row r="346" ht="130" customHeight="1">
       <c r="A346" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B346" s="2" t="inlineStr">
@@ -28388,7 +28423,7 @@
     <row r="358" ht="130" customHeight="1">
       <c r="A358" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B358" s="2" t="inlineStr">
@@ -28459,7 +28494,7 @@
     <row r="359" ht="130" customHeight="1">
       <c r="A359" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B359" s="2" t="inlineStr">
@@ -28531,7 +28566,7 @@
     <row r="360" ht="130" customHeight="1">
       <c r="A360" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B360" s="2" t="inlineStr">
@@ -29291,7 +29326,7 @@
     <row r="369" ht="130" customHeight="1">
       <c r="A369" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),CM-6 b</t>
+          <t>CM-6 b,AC-17 (2)</t>
         </is>
       </c>
       <c r="B369" s="2" t="inlineStr">
@@ -29600,7 +29635,7 @@
     <row r="373" ht="130" customHeight="1">
       <c r="A373" s="2" t="inlineStr">
         <is>
-          <t>SI-6 a,SC-3</t>
+          <t>SC-3,SI-6 a</t>
         </is>
       </c>
       <c r="B373" s="2" t="inlineStr">
@@ -29739,7 +29774,7 @@
     <row r="375" ht="130" customHeight="1">
       <c r="A375" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (a)</t>
+          <t>IA-5 (1) (a),CM-6 b</t>
         </is>
       </c>
       <c r="B375" s="2" t="inlineStr">
@@ -30553,7 +30588,7 @@
     <row r="385" ht="130" customHeight="1">
       <c r="A385" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B385" s="2" t="inlineStr">
@@ -30644,7 +30679,7 @@
     <row r="386" ht="130" customHeight="1">
       <c r="A386" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B386" s="2" t="inlineStr">
@@ -30738,7 +30773,7 @@
     <row r="387" ht="130" customHeight="1">
       <c r="A387" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B387" s="2" t="inlineStr">
@@ -34148,7 +34183,7 @@
     <row r="432" ht="130" customHeight="1">
       <c r="A432" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),CM-6 b</t>
         </is>
       </c>
       <c r="B432" s="2" t="inlineStr">
@@ -41502,7 +41537,7 @@
     <row r="525" ht="130" customHeight="1">
       <c r="A525" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-2 (2)</t>
+          <t>SI-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B525" s="2" t="inlineStr">
@@ -42149,7 +42184,7 @@
     <row r="534" ht="130" customHeight="1">
       <c r="A534" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-2 (2)</t>
+          <t>SI-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B534" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@7f24a1fa47b530abbff386305928b6d685496d7e 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -625,7 +625,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-14 (1)</t>
+          <t>AU-14 (1),AU-4</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -883,7 +883,7 @@
     <row r="6" ht="130" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>AU-12 (3),AU-7 b,CM-6 b,CM-5 (1),AU-12 c,AU-7 a,AU-8 b,AU-12 a</t>
+          <t>AU-12 a,CM-5 (1),CM-6 b,AU-12 c,AU-12 (3),AU-8 b,AU-7 a,AU-7 b</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -957,7 +957,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-6 (4),CM-6 b,CM-5 (1),AU-7 a,AU-7 (1),MA-4 (1) (a),AU-14 (1)</t>
+          <t>AU-14 (1),AU-3 (1),AU-7 (1),MA-4 (1) (a),AU-12 a,CM-5 (1),CM-6 b,AU-7 a,AU-6 (4),AU-3</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1273,7 +1273,7 @@
     <row r="11" ht="130" customHeight="1">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B11" s="2" t="inlineStr">
@@ -1424,7 +1424,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -1500,7 +1500,7 @@
     <row r="14" ht="130" customHeight="1">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -3772,7 +3772,7 @@
     <row r="44" ht="130" customHeight="1">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>IA-8,IA-2,AU-3 (1)</t>
+          <t>AU-3 (1),IA-2,IA-8</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
@@ -3850,7 +3850,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3925,7 +3925,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -4000,7 +4000,7 @@
     <row r="47" ht="130" customHeight="1">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
@@ -4075,7 +4075,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4150,7 +4150,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4225,7 +4225,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4300,7 +4300,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4375,7 +4375,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
@@ -4450,7 +4450,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4525,7 +4525,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4600,7 +4600,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4675,7 +4675,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4750,7 +4750,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4825,7 +4825,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4905,7 +4905,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -4988,7 +4988,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5068,7 +5068,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5148,7 +5148,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5228,7 +5228,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5308,7 +5308,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5382,7 +5382,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5456,7 +5456,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5530,7 +5530,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5604,7 +5604,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5678,7 +5678,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5751,7 +5751,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5824,7 +5824,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5897,7 +5897,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -5970,7 +5970,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6043,7 +6043,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6116,7 +6116,7 @@
     <row r="75" ht="130" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
@@ -6190,7 +6190,7 @@
     <row r="76" ht="130" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
@@ -6264,7 +6264,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6338,7 +6338,7 @@
     <row r="78" ht="130" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
@@ -6416,7 +6416,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6496,7 +6496,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6576,7 +6576,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6656,7 +6656,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B82" s="2" t="inlineStr">
@@ -6736,7 +6736,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B83" s="2" t="inlineStr">
@@ -6816,7 +6816,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B84" s="2" t="inlineStr">
@@ -6896,7 +6896,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B85" s="2" t="inlineStr">
@@ -6976,7 +6976,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -7056,7 +7056,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7136,7 +7136,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7216,7 +7216,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7296,7 +7296,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7372,7 +7372,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7449,7 +7449,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
@@ -7529,7 +7529,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
@@ -7609,7 +7609,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B94" s="2" t="inlineStr">
@@ -7689,7 +7689,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
@@ -7769,7 +7769,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7849,7 +7849,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7929,7 +7929,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8009,7 +8009,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8089,7 +8089,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8169,7 +8169,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8242,7 +8242,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8323,7 +8323,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8404,7 +8404,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8475,7 +8475,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8550,7 +8550,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8632,7 +8632,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8714,7 +8714,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -8796,7 +8796,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -8878,7 +8878,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B110" s="2" t="inlineStr">
@@ -8960,7 +8960,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-14 (1),MA-4 (1) (a),AU-12 a</t>
+          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-14 (1),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9052,7 +9052,7 @@
     <row r="112" ht="130" customHeight="1">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
@@ -9133,7 +9133,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9297,7 +9297,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9663,7 +9663,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9734,7 +9734,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -9934,7 +9934,7 @@
     <row r="123" ht="130" customHeight="1">
       <c r="A123" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (a),CM-6 b,IA-5 (1) (b)</t>
+          <t>CM-6 b,IA-5 (1) (b),IA-5 (1) (a)</t>
         </is>
       </c>
       <c r="B123" s="2" t="inlineStr">
@@ -10262,7 +10262,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-13,MA-4 c,AC-17 (2)</t>
+          <t>MA-4 c,AC-17 (2),SC-8,SC-13</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -10344,7 +10344,7 @@
     <row r="128" ht="130" customHeight="1">
       <c r="A128" s="2" t="inlineStr">
         <is>
-          <t>AC-12,MA-4 e,MA-4 (7),SC-10</t>
+          <t>SC-10,MA-4 e,AC-12,MA-4 (7)</t>
         </is>
       </c>
       <c r="B128" s="2" t="inlineStr">
@@ -10419,7 +10419,7 @@
     <row r="129" ht="130" customHeight="1">
       <c r="A129" s="2" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B129" s="2" t="inlineStr">
@@ -10498,7 +10498,7 @@
     <row r="130" ht="130" customHeight="1">
       <c r="A130" s="2" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B130" s="2" t="inlineStr">
@@ -10574,7 +10574,7 @@
     <row r="131" ht="130" customHeight="1">
       <c r="A131" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,SC-10</t>
+          <t>SC-10,AC-11 a</t>
         </is>
       </c>
       <c r="B131" s="2" t="inlineStr">
@@ -12013,7 +12013,7 @@
     <row r="151" ht="130" customHeight="1">
       <c r="A151" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8 (2),SC-8</t>
+          <t>SC-8 (2),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B151" s="2" t="inlineStr">
@@ -12090,7 +12090,7 @@
     <row r="152" ht="130" customHeight="1">
       <c r="A152" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8 (2),SC-8</t>
+          <t>SC-8 (2),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B152" s="2" t="inlineStr">
@@ -12337,7 +12337,7 @@
     <row r="155" ht="130" customHeight="1">
       <c r="A155" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2)</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B155" s="2" t="inlineStr">
@@ -12486,7 +12486,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B157" s="2" t="inlineStr">
@@ -12564,7 +12564,7 @@
     <row r="158" ht="130" customHeight="1">
       <c r="A158" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B158" s="2" t="inlineStr">
@@ -12647,7 +12647,7 @@
     <row r="159" ht="130" customHeight="1">
       <c r="A159" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B159" s="2" t="inlineStr">
@@ -13027,7 +13027,7 @@
     <row r="164" ht="130" customHeight="1">
       <c r="A164" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-4 (1),AU-6 (4)</t>
+          <t>AU-6 (4),AU-4 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B164" s="2" t="inlineStr">
@@ -13098,7 +13098,7 @@
     <row r="165" ht="130" customHeight="1">
       <c r="A165" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (9),CM-7 b,CM-6 b,AC-17 (1)</t>
+          <t>CM-7 b,AC-17 (1),CM-6 b,AC-17 (9)</t>
         </is>
       </c>
       <c r="B165" s="2" t="inlineStr">
@@ -13175,7 +13175,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-6 b,AC-17 (1)</t>
+          <t>CM-7 b,AC-17 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B166" s="2" t="inlineStr">
@@ -14160,7 +14160,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="2" t="inlineStr">
         <is>
-          <t>AU-3,CM-6 b</t>
+          <t>CM-6 b,AU-3</t>
         </is>
       </c>
       <c r="B178" s="2" t="inlineStr">
@@ -16467,7 +16467,7 @@
     <row r="206" ht="130" customHeight="1">
       <c r="A206" s="2" t="inlineStr">
         <is>
-          <t>IA-2,IA-2 (3),IA-2 (4),IA-2 (2),IA-2 (5)</t>
+          <t>IA-2 (3),IA-2 (2),IA-2 (4),IA-2 (5),IA-2</t>
         </is>
       </c>
       <c r="B206" s="2" t="inlineStr">
@@ -16552,7 +16552,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>IA-2,IA-2 (3),IA-2 (4),IA-2 (2),IA-2 (5)</t>
+          <t>IA-2 (3),IA-2 (2),IA-2 (4),IA-2 (5),IA-2</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -16637,7 +16637,7 @@
     <row r="208" ht="130" customHeight="1">
       <c r="A208" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),AC-18 (1),SC-8</t>
+          <t>AC-18 (1),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B208" s="2" t="inlineStr">
@@ -16804,7 +16804,7 @@
     <row r="210" ht="130" customHeight="1">
       <c r="A210" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),IA-7</t>
+          <t>IA-7,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B210" s="2" t="inlineStr">
@@ -16887,7 +16887,7 @@
     <row r="211" ht="130" customHeight="1">
       <c r="A211" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B211" s="2" t="inlineStr">
@@ -16963,7 +16963,7 @@
     <row r="212" ht="130" customHeight="1">
       <c r="A212" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B212" s="2" t="inlineStr">
@@ -17048,7 +17048,7 @@
     <row r="213" ht="130" customHeight="1">
       <c r="A213" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B213" s="2" t="inlineStr">
@@ -17205,7 +17205,7 @@
     <row r="215" ht="130" customHeight="1">
       <c r="A215" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,IA-7</t>
+          <t>IA-7,CM-7 a</t>
         </is>
       </c>
       <c r="B215" s="2" t="inlineStr">
@@ -17284,7 +17284,7 @@
     <row r="216" ht="130" customHeight="1">
       <c r="A216" s="2" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B216" s="2" t="inlineStr">
@@ -17443,7 +17443,7 @@
     <row r="218" ht="130" customHeight="1">
       <c r="A218" s="2" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B218" s="2" t="inlineStr">
@@ -18287,7 +18287,7 @@
     <row r="229" ht="130" customHeight="1">
       <c r="A229" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-2,SI-16</t>
+          <t>SC-2,CM-6 b,SI-16</t>
         </is>
       </c>
       <c r="B229" s="2" t="inlineStr">
@@ -19361,7 +19361,7 @@
     <row r="243" ht="130" customHeight="1">
       <c r="A243" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B243" s="2" t="inlineStr">
@@ -19436,7 +19436,7 @@
     <row r="244" ht="130" customHeight="1">
       <c r="A244" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B244" s="2" t="inlineStr">
@@ -19524,7 +19524,7 @@
     <row r="245" ht="130" customHeight="1">
       <c r="A245" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B245" s="2" t="inlineStr">
@@ -19601,7 +19601,7 @@
     <row r="246" ht="130" customHeight="1">
       <c r="A246" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B246" s="2" t="inlineStr">
@@ -19759,7 +19759,7 @@
     <row r="248" ht="130" customHeight="1">
       <c r="A248" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 (1)</t>
+          <t>AU-5 (1),AU-5 a</t>
         </is>
       </c>
       <c r="B248" s="2" t="inlineStr">
@@ -20199,7 +20199,7 @@
     <row r="254" ht="130" customHeight="1">
       <c r="A254" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),CM-6 b</t>
+          <t>CM-6 b,IA-2 (2)</t>
         </is>
       </c>
       <c r="B254" s="2" t="inlineStr">
@@ -20286,7 +20286,7 @@
     <row r="255" ht="130" customHeight="1">
       <c r="A255" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2 (1),IA-2 (3),IA-2 (2)</t>
+          <t>IA-2 (3),IA-2 (1),IA-2 (2),IA-2 (4)</t>
         </is>
       </c>
       <c r="B255" s="2" t="inlineStr">
@@ -20673,7 +20673,7 @@
     <row r="260" ht="130" customHeight="1">
       <c r="A260" s="2" t="inlineStr">
         <is>
-          <t>SC-4,CM-6 b</t>
+          <t>CM-6 b,SC-4</t>
         </is>
       </c>
       <c r="B260" s="2" t="inlineStr">
@@ -20754,7 +20754,7 @@
     <row r="261" ht="130" customHeight="1">
       <c r="A261" s="2" t="inlineStr">
         <is>
-          <t>SC-4,SC-2</t>
+          <t>SC-2,SC-4</t>
         </is>
       </c>
       <c r="B261" s="2" t="inlineStr">
@@ -20842,7 +20842,7 @@
     <row r="262" ht="130" customHeight="1">
       <c r="A262" s="2" t="inlineStr">
         <is>
-          <t>SC-4,SC-2</t>
+          <t>SC-2,SC-4</t>
         </is>
       </c>
       <c r="B262" s="2" t="inlineStr">
@@ -21080,7 +21080,7 @@
     <row r="265" ht="130" customHeight="1">
       <c r="A265" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-12 a</t>
+          <t>AU-12 a,CM-6 b</t>
         </is>
       </c>
       <c r="B265" s="2" t="inlineStr">
@@ -21303,7 +21303,7 @@
     <row r="268" ht="130" customHeight="1">
       <c r="A268" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (3),CM-6 b</t>
+          <t>CM-6 b,CM-5 (3)</t>
         </is>
       </c>
       <c r="B268" s="2" t="inlineStr">
@@ -21907,7 +21907,7 @@
     <row r="275" ht="130" customHeight="1">
       <c r="A275" s="2" t="inlineStr">
         <is>
-          <t>AU-12 (3),AU-7 b,CM-5 (1),AC-6 (8),AU-7 a,AU-8 b,AC-6 (9)</t>
+          <t>CM-5 (1),AC-6 (9),AU-12 (3),AU-7 a,AU-8 b,AU-7 b,AC-6 (8)</t>
         </is>
       </c>
       <c r="B275" s="2" t="inlineStr">
@@ -22596,7 +22596,7 @@
     <row r="284" ht="130" customHeight="1">
       <c r="A284" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B284" s="2" t="inlineStr">
@@ -22686,7 +22686,7 @@
     <row r="285" ht="130" customHeight="1">
       <c r="A285" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (1)</t>
         </is>
       </c>
       <c r="B285" s="2" t="inlineStr">
@@ -24624,7 +24624,7 @@
     <row r="309" ht="130" customHeight="1">
       <c r="A309" s="2" t="inlineStr">
         <is>
-          <t>AC-3 (4),IA-11</t>
+          <t>IA-11,AC-3 (4)</t>
         </is>
       </c>
       <c r="B309" s="2" t="inlineStr">
@@ -26309,7 +26309,7 @@
     <row r="331" ht="130" customHeight="1">
       <c r="A331" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-7 a,CM-6 b</t>
+          <t>CM-7 a,IA-5 (1) (c),CM-6 b</t>
         </is>
       </c>
       <c r="B331" s="2" t="inlineStr">
@@ -27403,7 +27403,7 @@
     <row r="345" ht="130" customHeight="1">
       <c r="A345" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 b,SI-6 d</t>
+          <t>SI-6 b,CM-3 (5),SI-6 d</t>
         </is>
       </c>
       <c r="B345" s="2" t="inlineStr">
@@ -29326,7 +29326,7 @@
     <row r="369" ht="130" customHeight="1">
       <c r="A369" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-17 (2)</t>
+          <t>AC-17 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B369" s="2" t="inlineStr">
@@ -29635,7 +29635,7 @@
     <row r="373" ht="130" customHeight="1">
       <c r="A373" s="2" t="inlineStr">
         <is>
-          <t>SC-3,SI-6 a</t>
+          <t>SI-6 a,SC-3</t>
         </is>
       </c>
       <c r="B373" s="2" t="inlineStr">
@@ -29774,7 +29774,7 @@
     <row r="375" ht="130" customHeight="1">
       <c r="A375" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (a),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (a)</t>
         </is>
       </c>
       <c r="B375" s="2" t="inlineStr">
@@ -30256,7 +30256,7 @@
     <row r="381" ht="130" customHeight="1">
       <c r="A381" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 d</t>
+          <t>SI-6 d,CM-3 (5)</t>
         </is>
       </c>
       <c r="B381" s="2" t="inlineStr">
@@ -40218,7 +40218,7 @@
     <row r="508" ht="130" customHeight="1">
       <c r="A508" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-2</t>
+          <t>SC-2,CM-6 b</t>
         </is>
       </c>
       <c r="B508" s="2" t="inlineStr">
@@ -40305,7 +40305,7 @@
     <row r="509" ht="130" customHeight="1">
       <c r="A509" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-2</t>
+          <t>SC-2,CM-6 b</t>
         </is>
       </c>
       <c r="B509" s="2" t="inlineStr">
@@ -42792,7 +42792,7 @@
     <row r="542" ht="130" customHeight="1">
       <c r="A542" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 a</t>
+          <t>SI-6 a,CM-3 (5)</t>
         </is>
       </c>
       <c r="B542" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@9631ba0a461a015c3adc159bb9067ec946b6df1e 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -541,7 +541,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-4 (1)</t>
+          <t>AU-4 (1),AU-4</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -708,7 +708,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>AU-4,CM-6 b</t>
+          <t>CM-6 b,AU-4</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -883,7 +883,7 @@
     <row r="6" ht="130" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,CM-5 (1),CM-6 b,AU-12 c,AU-12 (3),AU-8 b,AU-7 a,AU-7 b</t>
+          <t>AU-12 a,CM-5 (1),AU-7 a,AU-12 (3),AU-12 c,AU-7 b,AU-8 b,CM-6 b</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -957,7 +957,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),AU-3 (1),AU-7 (1),MA-4 (1) (a),AU-12 a,CM-5 (1),CM-6 b,AU-7 a,AU-6 (4),AU-3</t>
+          <t>AU-6 (4),AU-3,AU-12 a,CM-5 (1),AU-7 a,AU-3 (1),AU-7 (1),AU-14 (1),CM-6 b,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1424,7 +1424,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -1500,7 +1500,7 @@
     <row r="14" ht="130" customHeight="1">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -1654,7 +1654,7 @@
     <row r="16" ht="130" customHeight="1">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
@@ -2024,7 +2024,7 @@
     <row r="21" ht="130" customHeight="1">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
@@ -2098,7 +2098,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -3226,7 +3226,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3310,7 +3310,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3395,7 +3395,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3467,7 +3467,7 @@
     <row r="40" ht="130" customHeight="1">
       <c r="A40" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B40" s="2" t="inlineStr">
@@ -3772,7 +3772,7 @@
     <row r="44" ht="130" customHeight="1">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),IA-2,IA-8</t>
+          <t>IA-8,AU-3 (1),IA-2</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
@@ -3850,7 +3850,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3925,7 +3925,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -4000,7 +4000,7 @@
     <row r="47" ht="130" customHeight="1">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
@@ -4075,7 +4075,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4150,7 +4150,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4225,7 +4225,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4300,7 +4300,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4375,7 +4375,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
@@ -4450,7 +4450,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4525,7 +4525,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4600,7 +4600,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4675,7 +4675,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4750,7 +4750,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4825,7 +4825,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4905,7 +4905,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -4988,7 +4988,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5068,7 +5068,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5148,7 +5148,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5228,7 +5228,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5308,7 +5308,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5382,7 +5382,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5456,7 +5456,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5530,7 +5530,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5604,7 +5604,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5678,7 +5678,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5751,7 +5751,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5824,7 +5824,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5897,7 +5897,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -5970,7 +5970,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6043,7 +6043,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6116,7 +6116,7 @@
     <row r="75" ht="130" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
@@ -6190,7 +6190,7 @@
     <row r="76" ht="130" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
@@ -6264,7 +6264,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6338,7 +6338,7 @@
     <row r="78" ht="130" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
@@ -6416,7 +6416,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6496,7 +6496,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6576,7 +6576,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6656,7 +6656,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B82" s="2" t="inlineStr">
@@ -6736,7 +6736,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B83" s="2" t="inlineStr">
@@ -6816,7 +6816,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3</t>
+          <t>AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B84" s="2" t="inlineStr">
@@ -6896,7 +6896,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B85" s="2" t="inlineStr">
@@ -6976,7 +6976,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -7056,7 +7056,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7136,7 +7136,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7216,7 +7216,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7296,7 +7296,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7372,7 +7372,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7449,7 +7449,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
@@ -7529,7 +7529,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
@@ -7609,7 +7609,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B94" s="2" t="inlineStr">
@@ -7689,7 +7689,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
@@ -7769,7 +7769,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c</t>
+          <t>AU-12 c,AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7849,7 +7849,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7929,7 +7929,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8009,7 +8009,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8089,7 +8089,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8169,7 +8169,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8242,7 +8242,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AC-2 (4)</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8323,7 +8323,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AC-2 (4)</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8404,7 +8404,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AC-2 (4)</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8475,7 +8475,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-12 c,AU-3</t>
+          <t>AU-3,AU-3 (1),AU-12 c,MA-4 (1) (a),AC-2 (4)</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8550,7 +8550,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AC-2 (4)</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8632,7 +8632,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AC-2 (4)</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8714,7 +8714,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AC-2 (4)</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -8796,7 +8796,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AC-2 (4)</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -8878,7 +8878,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AC-2 (4)</t>
         </is>
       </c>
       <c r="B110" s="2" t="inlineStr">
@@ -8960,7 +8960,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),MA-4 (1) (a),AU-14 (1),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AU-12 c,AU-14 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9052,7 +9052,7 @@
     <row r="112" ht="130" customHeight="1">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
@@ -9133,7 +9133,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9219,7 +9219,7 @@
     <row r="114" ht="130" customHeight="1">
       <c r="A114" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-6 (10)</t>
+          <t>AC-6 (10),AC-11 b</t>
         </is>
       </c>
       <c r="B114" s="2" t="inlineStr">
@@ -9297,7 +9297,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9663,7 +9663,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9734,7 +9734,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -9805,7 +9805,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-12 c</t>
+          <t>AU-12 c,AU-9</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -9934,7 +9934,7 @@
     <row r="123" ht="130" customHeight="1">
       <c r="A123" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (b),IA-5 (1) (a)</t>
+          <t>IA-5 (1) (b),CM-6 b,IA-5 (1) (a)</t>
         </is>
       </c>
       <c r="B123" s="2" t="inlineStr">
@@ -10262,7 +10262,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>MA-4 c,AC-17 (2),SC-8,SC-13</t>
+          <t>MA-4 c,SC-13,AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -10344,7 +10344,7 @@
     <row r="128" ht="130" customHeight="1">
       <c r="A128" s="2" t="inlineStr">
         <is>
-          <t>SC-10,MA-4 e,AC-12,MA-4 (7)</t>
+          <t>AC-12,MA-4 e,SC-10,MA-4 (7)</t>
         </is>
       </c>
       <c r="B128" s="2" t="inlineStr">
@@ -10419,7 +10419,7 @@
     <row r="129" ht="130" customHeight="1">
       <c r="A129" s="2" t="inlineStr">
         <is>
-          <t>SC-10,AC-12</t>
+          <t>AC-12,SC-10</t>
         </is>
       </c>
       <c r="B129" s="2" t="inlineStr">
@@ -10498,7 +10498,7 @@
     <row r="130" ht="130" customHeight="1">
       <c r="A130" s="2" t="inlineStr">
         <is>
-          <t>SC-10,AC-12</t>
+          <t>AC-12,SC-10</t>
         </is>
       </c>
       <c r="B130" s="2" t="inlineStr">
@@ -10969,7 +10969,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -11038,7 +11038,7 @@
     <row r="137" ht="130" customHeight="1">
       <c r="A137" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B137" s="2" t="inlineStr">
@@ -11107,7 +11107,7 @@
     <row r="138" ht="130" customHeight="1">
       <c r="A138" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B138" s="2" t="inlineStr">
@@ -11177,7 +11177,7 @@
     <row r="139" ht="130" customHeight="1">
       <c r="A139" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B139" s="2" t="inlineStr">
@@ -11246,7 +11246,7 @@
     <row r="140" ht="130" customHeight="1">
       <c r="A140" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B140" s="2" t="inlineStr">
@@ -11315,7 +11315,7 @@
     <row r="141" ht="130" customHeight="1">
       <c r="A141" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B141" s="2" t="inlineStr">
@@ -11385,7 +11385,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B142" s="2" t="inlineStr">
@@ -11454,7 +11454,7 @@
     <row r="143" ht="130" customHeight="1">
       <c r="A143" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B143" s="2" t="inlineStr">
@@ -11523,7 +11523,7 @@
     <row r="144" ht="130" customHeight="1">
       <c r="A144" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B144" s="2" t="inlineStr">
@@ -11593,7 +11593,7 @@
     <row r="145" ht="130" customHeight="1">
       <c r="A145" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B145" s="2" t="inlineStr">
@@ -11662,7 +11662,7 @@
     <row r="146" ht="130" customHeight="1">
       <c r="A146" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B146" s="2" t="inlineStr">
@@ -11731,7 +11731,7 @@
     <row r="147" ht="130" customHeight="1">
       <c r="A147" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B147" s="2" t="inlineStr">
@@ -11800,7 +11800,7 @@
     <row r="148" ht="130" customHeight="1">
       <c r="A148" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B148" s="2" t="inlineStr">
@@ -12013,7 +12013,7 @@
     <row r="151" ht="130" customHeight="1">
       <c r="A151" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8,SC-8 (1)</t>
+          <t>SC-8 (1),SC-8,SC-8 (2)</t>
         </is>
       </c>
       <c r="B151" s="2" t="inlineStr">
@@ -12090,7 +12090,7 @@
     <row r="152" ht="130" customHeight="1">
       <c r="A152" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8,SC-8 (1)</t>
+          <t>SC-8 (1),SC-8,SC-8 (2)</t>
         </is>
       </c>
       <c r="B152" s="2" t="inlineStr">
@@ -12176,7 +12176,7 @@
     <row r="153" ht="130" customHeight="1">
       <c r="A153" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8</t>
+          <t>SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B153" s="2" t="inlineStr">
@@ -12255,7 +12255,7 @@
     <row r="154" ht="130" customHeight="1">
       <c r="A154" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8</t>
+          <t>SC-8,SC-8 (2)</t>
         </is>
       </c>
       <c r="B154" s="2" t="inlineStr">
@@ -12486,7 +12486,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B157" s="2" t="inlineStr">
@@ -12564,7 +12564,7 @@
     <row r="158" ht="130" customHeight="1">
       <c r="A158" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B158" s="2" t="inlineStr">
@@ -12647,7 +12647,7 @@
     <row r="159" ht="130" customHeight="1">
       <c r="A159" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B159" s="2" t="inlineStr">
@@ -13098,7 +13098,7 @@
     <row r="165" ht="130" customHeight="1">
       <c r="A165" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (1),CM-6 b,AC-17 (9)</t>
+          <t>CM-6 b,AC-17 (9),CM-7 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B165" s="2" t="inlineStr">
@@ -13175,7 +13175,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (1),CM-6 b</t>
+          <t>CM-6 b,CM-7 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B166" s="2" t="inlineStr">
@@ -15189,7 +15189,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="2" t="inlineStr">
         <is>
-          <t>SC-28 (1),SC-28</t>
+          <t>SC-28,SC-28 (1)</t>
         </is>
       </c>
       <c r="B192" s="2" t="inlineStr">
@@ -15515,7 +15515,7 @@
     <row r="196" ht="130" customHeight="1">
       <c r="A196" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B196" s="2" t="inlineStr">
@@ -15617,7 +15617,7 @@
     <row r="197" ht="130" customHeight="1">
       <c r="A197" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B197" s="2" t="inlineStr">
@@ -15727,7 +15727,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B198" s="2" t="inlineStr">
@@ -15838,7 +15838,7 @@
     <row r="199" ht="130" customHeight="1">
       <c r="A199" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B199" s="2" t="inlineStr">
@@ -15947,7 +15947,7 @@
     <row r="200" ht="130" customHeight="1">
       <c r="A200" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (9),AC-2 (4),AU-12 c</t>
+          <t>AU-12 c,AC-6 (9),AC-2 (4)</t>
         </is>
       </c>
       <c r="B200" s="2" t="inlineStr">
@@ -16389,7 +16389,7 @@
     <row r="205" ht="130" customHeight="1">
       <c r="A205" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),CM-6 b</t>
+          <t>CM-6 b,IA-2 (5)</t>
         </is>
       </c>
       <c r="B205" s="2" t="inlineStr">
@@ -16467,7 +16467,7 @@
     <row r="206" ht="130" customHeight="1">
       <c r="A206" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (2),IA-2 (4),IA-2 (5),IA-2</t>
+          <t>IA-2 (4),IA-2 (3),IA-2,IA-2 (2),IA-2 (5)</t>
         </is>
       </c>
       <c r="B206" s="2" t="inlineStr">
@@ -16552,7 +16552,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (2),IA-2 (4),IA-2 (5),IA-2</t>
+          <t>IA-2 (4),IA-2 (3),IA-2,IA-2 (2),IA-2 (5)</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -16637,7 +16637,7 @@
     <row r="208" ht="130" customHeight="1">
       <c r="A208" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),SC-8,SC-8 (1)</t>
+          <t>SC-8 (1),AC-18 (1),SC-8</t>
         </is>
       </c>
       <c r="B208" s="2" t="inlineStr">
@@ -17205,7 +17205,7 @@
     <row r="215" ht="130" customHeight="1">
       <c r="A215" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-7 a</t>
+          <t>CM-7 a,IA-7</t>
         </is>
       </c>
       <c r="B215" s="2" t="inlineStr">
@@ -17284,7 +17284,7 @@
     <row r="216" ht="130" customHeight="1">
       <c r="A216" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B216" s="2" t="inlineStr">
@@ -17368,7 +17368,7 @@
     <row r="217" ht="130" customHeight="1">
       <c r="A217" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),AC-17 (2)</t>
+          <t>AC-17 (2),MA-4 (6)</t>
         </is>
       </c>
       <c r="B217" s="2" t="inlineStr">
@@ -17443,7 +17443,7 @@
     <row r="218" ht="130" customHeight="1">
       <c r="A218" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B218" s="2" t="inlineStr">
@@ -18040,7 +18040,7 @@
     <row r="226" ht="130" customHeight="1">
       <c r="A226" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B226" s="2" t="inlineStr">
@@ -18118,7 +18118,7 @@
     <row r="227" ht="130" customHeight="1">
       <c r="A227" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B227" s="2" t="inlineStr">
@@ -18287,7 +18287,7 @@
     <row r="229" ht="130" customHeight="1">
       <c r="A229" s="2" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b,SI-16</t>
+          <t>SI-16,SC-2,CM-6 b</t>
         </is>
       </c>
       <c r="B229" s="2" t="inlineStr">
@@ -18447,7 +18447,7 @@
     <row r="231" ht="130" customHeight="1">
       <c r="A231" s="2" t="inlineStr">
         <is>
-          <t>SC-3,SI-16</t>
+          <t>SI-16,SC-3</t>
         </is>
       </c>
       <c r="B231" s="2" t="inlineStr">
@@ -19361,7 +19361,7 @@
     <row r="243" ht="130" customHeight="1">
       <c r="A243" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B243" s="2" t="inlineStr">
@@ -19436,7 +19436,7 @@
     <row r="244" ht="130" customHeight="1">
       <c r="A244" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B244" s="2" t="inlineStr">
@@ -19524,7 +19524,7 @@
     <row r="245" ht="130" customHeight="1">
       <c r="A245" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B245" s="2" t="inlineStr">
@@ -19601,7 +19601,7 @@
     <row r="246" ht="130" customHeight="1">
       <c r="A246" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B246" s="2" t="inlineStr">
@@ -19759,7 +19759,7 @@
     <row r="248" ht="130" customHeight="1">
       <c r="A248" s="2" t="inlineStr">
         <is>
-          <t>AU-5 (1),AU-5 a</t>
+          <t>AU-5 a,AU-5 (1)</t>
         </is>
       </c>
       <c r="B248" s="2" t="inlineStr">
@@ -20199,7 +20199,7 @@
     <row r="254" ht="130" customHeight="1">
       <c r="A254" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (2)</t>
+          <t>IA-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B254" s="2" t="inlineStr">
@@ -20286,7 +20286,7 @@
     <row r="255" ht="130" customHeight="1">
       <c r="A255" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (1),IA-2 (2),IA-2 (4)</t>
+          <t>IA-2 (4),IA-2 (1),IA-2 (3),IA-2 (2)</t>
         </is>
       </c>
       <c r="B255" s="2" t="inlineStr">
@@ -20455,7 +20455,7 @@
     <row r="257" ht="130" customHeight="1">
       <c r="A257" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B257" s="2" t="inlineStr">
@@ -20673,7 +20673,7 @@
     <row r="260" ht="130" customHeight="1">
       <c r="A260" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-4</t>
+          <t>SC-4,CM-6 b</t>
         </is>
       </c>
       <c r="B260" s="2" t="inlineStr">
@@ -20754,7 +20754,7 @@
     <row r="261" ht="130" customHeight="1">
       <c r="A261" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SC-4</t>
+          <t>SC-4,SC-2</t>
         </is>
       </c>
       <c r="B261" s="2" t="inlineStr">
@@ -20842,7 +20842,7 @@
     <row r="262" ht="130" customHeight="1">
       <c r="A262" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SC-4</t>
+          <t>SC-4,SC-2</t>
         </is>
       </c>
       <c r="B262" s="2" t="inlineStr">
@@ -21080,7 +21080,7 @@
     <row r="265" ht="130" customHeight="1">
       <c r="A265" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,CM-6 b</t>
+          <t>CM-6 b,AU-12 a</t>
         </is>
       </c>
       <c r="B265" s="2" t="inlineStr">
@@ -21907,7 +21907,7 @@
     <row r="275" ht="130" customHeight="1">
       <c r="A275" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AC-6 (9),AU-12 (3),AU-7 a,AU-8 b,AU-7 b,AC-6 (8)</t>
+          <t>AC-6 (9),CM-5 (1),AU-7 a,AU-12 (3),AU-7 b,AU-8 b,AC-6 (8)</t>
         </is>
       </c>
       <c r="B275" s="2" t="inlineStr">
@@ -23597,7 +23597,7 @@
     <row r="296" ht="130" customHeight="1">
       <c r="A296" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (a),AU-8 b,AU-8 (1) (b)</t>
+          <t>AU-8 (1) (a),AU-8 (1) (b),AU-8 b</t>
         </is>
       </c>
       <c r="B296" s="2" t="inlineStr">
@@ -24624,7 +24624,7 @@
     <row r="309" ht="130" customHeight="1">
       <c r="A309" s="2" t="inlineStr">
         <is>
-          <t>IA-11,AC-3 (4)</t>
+          <t>AC-3 (4),IA-11</t>
         </is>
       </c>
       <c r="B309" s="2" t="inlineStr">
@@ -25004,7 +25004,7 @@
     <row r="314" ht="130" customHeight="1">
       <c r="A314" s="2" t="inlineStr">
         <is>
-          <t>AU-5 b,AU-5 a</t>
+          <t>AU-5 a,AU-5 b</t>
         </is>
       </c>
       <c r="B314" s="2" t="inlineStr">
@@ -25923,7 +25923,7 @@
     <row r="326" ht="130" customHeight="1">
       <c r="A326" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,IA-3</t>
+          <t>IA-3,CM-7 b</t>
         </is>
       </c>
       <c r="B326" s="2" t="inlineStr">
@@ -25998,7 +25998,7 @@
     <row r="327" ht="130" customHeight="1">
       <c r="A327" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-7 a</t>
+          <t>CM-7 a,CM-7 b</t>
         </is>
       </c>
       <c r="B327" s="2" t="inlineStr">
@@ -26072,7 +26072,7 @@
     <row r="328" ht="130" customHeight="1">
       <c r="A328" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-7 a</t>
+          <t>CM-7 a,CM-7 b</t>
         </is>
       </c>
       <c r="B328" s="2" t="inlineStr">
@@ -26309,7 +26309,7 @@
     <row r="331" ht="130" customHeight="1">
       <c r="A331" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,IA-5 (1) (c),CM-6 b</t>
+          <t>CM-7 a,CM-6 b,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B331" s="2" t="inlineStr">
@@ -27154,7 +27154,7 @@
     <row r="342" ht="130" customHeight="1">
       <c r="A342" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 (1)</t>
+          <t>AC-11 (1),AC-11 b</t>
         </is>
       </c>
       <c r="B342" s="2" t="inlineStr">
@@ -27403,7 +27403,7 @@
     <row r="345" ht="130" customHeight="1">
       <c r="A345" s="2" t="inlineStr">
         <is>
-          <t>SI-6 b,CM-3 (5),SI-6 d</t>
+          <t>SI-6 b,SI-6 d,CM-3 (5)</t>
         </is>
       </c>
       <c r="B345" s="2" t="inlineStr">
@@ -27874,7 +27874,7 @@
     <row r="351" ht="130" customHeight="1">
       <c r="A351" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,SI-16</t>
+          <t>SI-16,CM-7 a</t>
         </is>
       </c>
       <c r="B351" s="2" t="inlineStr">
@@ -29326,7 +29326,7 @@
     <row r="369" ht="130" customHeight="1">
       <c r="A369" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),CM-6 b</t>
+          <t>CM-6 b,AC-17 (2)</t>
         </is>
       </c>
       <c r="B369" s="2" t="inlineStr">
@@ -30340,7 +30340,7 @@
     <row r="382" ht="130" customHeight="1">
       <c r="A382" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-16</t>
+          <t>SI-16,CM-6 b</t>
         </is>
       </c>
       <c r="B382" s="2" t="inlineStr">
@@ -30588,7 +30588,7 @@
     <row r="385" ht="130" customHeight="1">
       <c r="A385" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B385" s="2" t="inlineStr">
@@ -30679,7 +30679,7 @@
     <row r="386" ht="130" customHeight="1">
       <c r="A386" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B386" s="2" t="inlineStr">
@@ -30773,7 +30773,7 @@
     <row r="387" ht="130" customHeight="1">
       <c r="A387" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B387" s="2" t="inlineStr">
@@ -34183,7 +34183,7 @@
     <row r="432" ht="130" customHeight="1">
       <c r="A432" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B432" s="2" t="inlineStr">
@@ -34333,7 +34333,7 @@
     <row r="434" ht="130" customHeight="1">
       <c r="A434" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (1)</t>
+          <t>CM-5 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B434" s="2" t="inlineStr">
@@ -34406,7 +34406,7 @@
     <row r="435" ht="130" customHeight="1">
       <c r="A435" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (1)</t>
+          <t>CM-5 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B435" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@ab9d414591a5c9323febcbc6859398fdebdb4188 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -1446,7 +1446,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>AU-7 (1),AU-6 (4),AU-14 (1),MA-4 (1) (a),AU-3,CM-5 (1),AU-7 a,CM-6 b,AU-12 a,AU-3 (1)</t>
+          <t>AU-6 (4),AU-7 (1),CM-6 b,AU-3,AU-14 (1),MA-4 (1) (a),AU-3 (1),AU-7 a,AU-12 a,CM-5 (1)</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -3249,7 +3249,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-14 (1),MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3340,7 +3340,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-14 (1)</t>
+          <t>AU-14 (1),AU-4</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -4161,7 +4161,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-6 (4),AU-4 (1)</t>
+          <t>AU-6 (4),AU-4 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4231,7 +4231,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-4 (1)</t>
+          <t>AU-4 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4311,7 +4311,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (a),AU-8 (1) (b),AU-8 b</t>
+          <t>AU-8 b,AU-8 (1) (b),AU-8 (1) (a)</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4466,7 +4466,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4552,7 +4552,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12),IA-2 (1)</t>
+          <t>IA-2 (1),IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4812,7 +4812,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4887,7 +4887,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4962,7 +4962,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -5037,7 +5037,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5112,7 +5112,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5187,7 +5187,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5262,7 +5262,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5337,7 +5337,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5412,7 +5412,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5487,7 +5487,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-7 b,AU-8 b,AU-12 c,AU-12 (3),CM-5 (1),AU-7 a,CM-6 b,AU-12 a</t>
+          <t>CM-6 b,AU-7 b,AU-12 c,AU-12 (3),AU-8 b,AU-7 a,AU-12 a,CM-5 (1)</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5561,7 +5561,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1),AC-2 (4)</t>
+          <t>AU-3,AC-2 (4),AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5642,7 +5642,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1),AC-2 (4)</t>
+          <t>AU-3,AC-2 (4),AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5723,7 +5723,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1),AC-2 (4)</t>
+          <t>AU-3,AC-2 (4),AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5805,7 +5805,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1),AC-2 (4)</t>
+          <t>AU-3,AC-2 (4),AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5887,7 +5887,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1),AC-2 (4)</t>
+          <t>AU-3,AC-2 (4),AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5969,7 +5969,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1),AC-2 (4)</t>
+          <t>AU-3,AC-2 (4),AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -6051,7 +6051,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1),AC-2 (4)</t>
+          <t>AU-3,AC-2 (4),AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6133,7 +6133,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 a</t>
+          <t>SI-6 a,CM-3 (5)</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -7171,7 +7171,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7245,7 +7245,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7319,7 +7319,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7393,7 +7393,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7558,7 +7558,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),AC-17 (2)</t>
+          <t>AC-17 (2),MA-4 (6)</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
@@ -7817,7 +7817,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>AU-9 (3),AU-9</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
@@ -7893,7 +7893,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-9 (3),AU-9</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7969,7 +7969,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -8044,7 +8044,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8119,7 +8119,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8194,7 +8194,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8274,7 +8274,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8348,7 +8348,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8422,7 +8422,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8496,7 +8496,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8570,7 +8570,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8644,7 +8644,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8724,7 +8724,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8804,7 +8804,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -9055,7 +9055,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-6 (10)</t>
+          <t>AC-6 (10),AC-11 b</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9553,7 +9553,7 @@
     <row r="117" ht="130" customHeight="1">
       <c r="A117" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-13,MA-4 c,AC-17 (2)</t>
+          <t>SC-8,AC-17 (2),MA-4 c,SC-13</t>
         </is>
       </c>
       <c r="B117" s="2" t="inlineStr">
@@ -9635,7 +9635,7 @@
     <row r="118" ht="130" customHeight="1">
       <c r="A118" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B118" s="2" t="inlineStr">
@@ -9713,7 +9713,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9791,7 +9791,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -9869,7 +9869,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -9949,7 +9949,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B122" s="2" t="inlineStr">
@@ -10018,7 +10018,7 @@
     <row r="123" ht="130" customHeight="1">
       <c r="A123" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B123" s="2" t="inlineStr">
@@ -10087,7 +10087,7 @@
     <row r="124" ht="130" customHeight="1">
       <c r="A124" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B124" s="2" t="inlineStr">
@@ -10156,7 +10156,7 @@
     <row r="125" ht="130" customHeight="1">
       <c r="A125" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B125" s="2" t="inlineStr">
@@ -10225,7 +10225,7 @@
     <row r="126" ht="130" customHeight="1">
       <c r="A126" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B126" s="2" t="inlineStr">
@@ -10305,7 +10305,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>SC-28 (1),SC-28</t>
+          <t>SC-28,SC-28 (1)</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -11072,7 +11072,7 @@
     <row r="137" ht="130" customHeight="1">
       <c r="A137" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B137" s="2" t="inlineStr">
@@ -11153,7 +11153,7 @@
     <row r="138" ht="130" customHeight="1">
       <c r="A138" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B138" s="2" t="inlineStr">
@@ -11239,7 +11239,7 @@
     <row r="139" ht="130" customHeight="1">
       <c r="A139" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B139" s="2" t="inlineStr">
@@ -11605,7 +11605,7 @@
     <row r="143" ht="130" customHeight="1">
       <c r="A143" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B143" s="2" t="inlineStr">
@@ -11685,7 +11685,7 @@
     <row r="144" ht="130" customHeight="1">
       <c r="A144" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B144" s="2" t="inlineStr">
@@ -11765,7 +11765,7 @@
     <row r="145" ht="130" customHeight="1">
       <c r="A145" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B145" s="2" t="inlineStr">
@@ -11845,7 +11845,7 @@
     <row r="146" ht="130" customHeight="1">
       <c r="A146" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B146" s="2" t="inlineStr">
@@ -12941,7 +12941,7 @@
     <row r="160" ht="130" customHeight="1">
       <c r="A160" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B160" s="2" t="inlineStr">
@@ -13018,7 +13018,7 @@
     <row r="161" ht="130" customHeight="1">
       <c r="A161" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B161" s="2" t="inlineStr">
@@ -13091,7 +13091,7 @@
     <row r="162" ht="130" customHeight="1">
       <c r="A162" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3</t>
+          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B162" s="2" t="inlineStr">
@@ -13164,7 +13164,7 @@
     <row r="163" ht="130" customHeight="1">
       <c r="A163" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B163" s="2" t="inlineStr">
@@ -13249,7 +13249,7 @@
     <row r="164" ht="130" customHeight="1">
       <c r="A164" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B164" s="2" t="inlineStr">
@@ -13324,7 +13324,7 @@
     <row r="165" ht="130" customHeight="1">
       <c r="A165" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B165" s="2" t="inlineStr">
@@ -13399,7 +13399,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B166" s="2" t="inlineStr">
@@ -13474,7 +13474,7 @@
     <row r="167" ht="130" customHeight="1">
       <c r="A167" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B167" s="2" t="inlineStr">
@@ -13549,7 +13549,7 @@
     <row r="168" ht="130" customHeight="1">
       <c r="A168" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B168" s="2" t="inlineStr">
@@ -13620,7 +13620,7 @@
     <row r="169" ht="130" customHeight="1">
       <c r="A169" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B169" s="2" t="inlineStr">
@@ -13691,7 +13691,7 @@
     <row r="170" ht="130" customHeight="1">
       <c r="A170" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B170" s="2" t="inlineStr">
@@ -13763,7 +13763,7 @@
     <row r="171" ht="130" customHeight="1">
       <c r="A171" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B171" s="2" t="inlineStr">
@@ -13834,7 +13834,7 @@
     <row r="172" ht="130" customHeight="1">
       <c r="A172" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B172" s="2" t="inlineStr">
@@ -13905,7 +13905,7 @@
     <row r="173" ht="130" customHeight="1">
       <c r="A173" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B173" s="2" t="inlineStr">
@@ -13977,7 +13977,7 @@
     <row r="174" ht="130" customHeight="1">
       <c r="A174" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B174" s="2" t="inlineStr">
@@ -14052,7 +14052,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B175" s="2" t="inlineStr">
@@ -14123,7 +14123,7 @@
     <row r="176" ht="130" customHeight="1">
       <c r="A176" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B176" s="2" t="inlineStr">
@@ -14194,7 +14194,7 @@
     <row r="177" ht="130" customHeight="1">
       <c r="A177" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B177" s="2" t="inlineStr">
@@ -14266,7 +14266,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B178" s="2" t="inlineStr">
@@ -14341,7 +14341,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B179" s="2" t="inlineStr">
@@ -14423,7 +14423,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B180" s="2" t="inlineStr">
@@ -14505,7 +14505,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">
@@ -14587,7 +14587,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B182" s="2" t="inlineStr">
@@ -14669,7 +14669,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B183" s="2" t="inlineStr">
@@ -14751,7 +14751,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B184" s="2" t="inlineStr">
@@ -14833,7 +14833,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B185" s="2" t="inlineStr">
@@ -14915,7 +14915,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B186" s="2" t="inlineStr">
@@ -14997,7 +14997,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B187" s="2" t="inlineStr">
@@ -15079,7 +15079,7 @@
     <row r="188" ht="130" customHeight="1">
       <c r="A188" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B188" s="2" t="inlineStr">
@@ -15157,7 +15157,7 @@
     <row r="189" ht="130" customHeight="1">
       <c r="A189" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B189" s="2" t="inlineStr">
@@ -15236,7 +15236,7 @@
     <row r="190" ht="130" customHeight="1">
       <c r="A190" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B190" s="2" t="inlineStr">
@@ -15318,7 +15318,7 @@
     <row r="191" ht="130" customHeight="1">
       <c r="A191" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B191" s="2" t="inlineStr">
@@ -15400,7 +15400,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B192" s="2" t="inlineStr">
@@ -15482,7 +15482,7 @@
     <row r="193" ht="130" customHeight="1">
       <c r="A193" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B193" s="2" t="inlineStr">
@@ -15564,7 +15564,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B194" s="2" t="inlineStr">
@@ -15646,7 +15646,7 @@
     <row r="195" ht="130" customHeight="1">
       <c r="A195" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B195" s="2" t="inlineStr">
@@ -15728,7 +15728,7 @@
     <row r="196" ht="130" customHeight="1">
       <c r="A196" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B196" s="2" t="inlineStr">
@@ -15803,7 +15803,7 @@
     <row r="197" ht="130" customHeight="1">
       <c r="A197" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a,AU-3 (1),AC-2 (4)</t>
+          <t>AU-3,AC-2 (4),AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B197" s="2" t="inlineStr">
@@ -15876,7 +15876,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-3 (1),AC-2 (4)</t>
+          <t>AU-3,AC-2 (4),AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B198" s="2" t="inlineStr">
@@ -15953,7 +15953,7 @@
     <row r="199" ht="130" customHeight="1">
       <c r="A199" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (4),IA-2 (3),IA-2 (1)</t>
+          <t>IA-2 (2),IA-2 (1),IA-2 (3),IA-2 (4)</t>
         </is>
       </c>
       <c r="B199" s="2" t="inlineStr">
@@ -16040,7 +16040,7 @@
     <row r="200" ht="130" customHeight="1">
       <c r="A200" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),IA-2 (2),IA-2 (4),IA-2,IA-2 (3)</t>
+          <t>IA-2,IA-2 (2),IA-2 (3),IA-2 (5),IA-2 (4)</t>
         </is>
       </c>
       <c r="B200" s="2" t="inlineStr">
@@ -16129,7 +16129,7 @@
     <row r="201" ht="130" customHeight="1">
       <c r="A201" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),IA-2 (2),IA-2 (4),IA-2,IA-2 (3)</t>
+          <t>IA-2,IA-2 (2),IA-2 (3),IA-2 (5),IA-2 (4)</t>
         </is>
       </c>
       <c r="B201" s="2" t="inlineStr">
@@ -16809,7 +16809,7 @@
     <row r="210" ht="130" customHeight="1">
       <c r="A210" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (1),SC-8 (2)</t>
+          <t>SC-8 (1),SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B210" s="2" t="inlineStr">
@@ -16886,7 +16886,7 @@
     <row r="211" ht="130" customHeight="1">
       <c r="A211" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (1),SC-8 (2)</t>
+          <t>SC-8 (1),SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B211" s="2" t="inlineStr">
@@ -17740,7 +17740,7 @@
     <row r="222" ht="130" customHeight="1">
       <c r="A222" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-6 b,CM-7 a</t>
+          <t>CM-7 a,IA-5 (1) (c),CM-6 b</t>
         </is>
       </c>
       <c r="B222" s="2" t="inlineStr">
@@ -17900,7 +17900,7 @@
     <row r="224" ht="130" customHeight="1">
       <c r="A224" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-12 a</t>
+          <t>AU-12 a,CM-6 b</t>
         </is>
       </c>
       <c r="B224" s="2" t="inlineStr">
@@ -17986,7 +17986,7 @@
     <row r="225" ht="130" customHeight="1">
       <c r="A225" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-5,SC-5 (2)</t>
+          <t>SC-5,SC-5 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B225" s="2" t="inlineStr">
@@ -18258,7 +18258,7 @@
     <row r="228" ht="130" customHeight="1">
       <c r="A228" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-16</t>
+          <t>SI-16,CM-6 b</t>
         </is>
       </c>
       <c r="B228" s="2" t="inlineStr">
@@ -18356,7 +18356,7 @@
     <row r="229" ht="130" customHeight="1">
       <c r="A229" s="2" t="inlineStr">
         <is>
-          <t>IA-8,AU-3 (1),IA-2</t>
+          <t>AU-3 (1),IA-2,IA-8</t>
         </is>
       </c>
       <c r="B229" s="2" t="inlineStr">
@@ -19490,7 +19490,7 @@
     <row r="243" ht="130" customHeight="1">
       <c r="A243" s="2" t="inlineStr">
         <is>
-          <t>SC-3,SI-16</t>
+          <t>SI-16,SC-3</t>
         </is>
       </c>
       <c r="B243" s="2" t="inlineStr">
@@ -20188,7 +20188,7 @@
     <row r="252" ht="130" customHeight="1">
       <c r="A252" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (b),CM-6 b,IA-5 (1) (a)</t>
+          <t>IA-5 (1) (a),CM-6 b,IA-5 (1) (b)</t>
         </is>
       </c>
       <c r="B252" s="2" t="inlineStr">
@@ -21012,7 +21012,7 @@
     <row r="262" ht="130" customHeight="1">
       <c r="A262" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (1)</t>
+          <t>IA-2 (1),IA-2 (11)</t>
         </is>
       </c>
       <c r="B262" s="2" t="inlineStr">
@@ -21101,7 +21101,7 @@
     <row r="263" ht="130" customHeight="1">
       <c r="A263" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B263" s="2" t="inlineStr">
@@ -21426,7 +21426,7 @@
     <row r="267" ht="130" customHeight="1">
       <c r="A267" s="2" t="inlineStr">
         <is>
-          <t>SC-3,SI-6 a</t>
+          <t>SI-6 a,SC-3</t>
         </is>
       </c>
       <c r="B267" s="2" t="inlineStr">
@@ -21508,7 +21508,7 @@
     <row r="268" ht="130" customHeight="1">
       <c r="A268" s="2" t="inlineStr">
         <is>
-          <t>AU-7 b,AU-8 b,AC-6 (9),AU-12 (3),AC-6 (8),CM-5 (1),AU-7 a</t>
+          <t>AU-7 b,AC-6 (9),AU-12 (3),AU-8 b,AU-7 a,AC-6 (8),CM-5 (1)</t>
         </is>
       </c>
       <c r="B268" s="2" t="inlineStr">
@@ -21588,7 +21588,7 @@
     <row r="269" ht="130" customHeight="1">
       <c r="A269" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (5)</t>
+          <t>IA-2 (5),CM-6 b</t>
         </is>
       </c>
       <c r="B269" s="2" t="inlineStr">
@@ -22102,7 +22102,7 @@
     <row r="276" ht="130" customHeight="1">
       <c r="A276" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-9</t>
+          <t>AU-9,AU-12 c</t>
         </is>
       </c>
       <c r="B276" s="2" t="inlineStr">
@@ -22700,7 +22700,7 @@
     <row r="283" ht="130" customHeight="1">
       <c r="A283" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (a)</t>
+          <t>IA-5 (1) (a),CM-6 b</t>
         </is>
       </c>
       <c r="B283" s="2" t="inlineStr">
@@ -24139,7 +24139,7 @@
     <row r="302" ht="130" customHeight="1">
       <c r="A302" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-2 (4),AC-6 (9)</t>
+          <t>AC-6 (9),AC-2 (4),AU-12 c</t>
         </is>
       </c>
       <c r="B302" s="2" t="inlineStr">
@@ -28601,7 +28601,7 @@
     <row r="361" ht="130" customHeight="1">
       <c r="A361" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-17 (2)</t>
+          <t>AC-17 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B361" s="2" t="inlineStr">
@@ -30329,7 +30329,7 @@
     <row r="384" ht="130" customHeight="1">
       <c r="A384" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-3</t>
+          <t>AU-3,CM-6 b</t>
         </is>
       </c>
       <c r="B384" s="2" t="inlineStr">
@@ -30967,7 +30967,7 @@
     <row r="392" ht="130" customHeight="1">
       <c r="A392" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-17 (1),CM-7 b,AC-17 (9)</t>
+          <t>AC-17 (1),CM-6 b,CM-7 b,AC-17 (9)</t>
         </is>
       </c>
       <c r="B392" s="2" t="inlineStr">
@@ -36120,7 +36120,7 @@
     <row r="455" ht="130" customHeight="1">
       <c r="A455" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-2 (2)</t>
+          <t>SI-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B455" s="2" t="inlineStr">
@@ -36767,7 +36767,7 @@
     <row r="464" ht="130" customHeight="1">
       <c r="A464" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-2 (2)</t>
+          <t>SI-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B464" s="2" t="inlineStr">
@@ -37058,7 +37058,7 @@
     <row r="468" ht="130" customHeight="1">
       <c r="A468" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (7),AC-12,MA-4 e,SC-10</t>
+          <t>MA-4 e,AC-12,MA-4 (7),SC-10</t>
         </is>
       </c>
       <c r="B468" s="2" t="inlineStr">
@@ -37288,7 +37288,7 @@
     <row r="471" ht="130" customHeight="1">
       <c r="A471" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2)</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B471" s="2" t="inlineStr">
@@ -41155,7 +41155,7 @@
     <row r="520" ht="130" customHeight="1">
       <c r="A520" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (2)</t>
+          <t>SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B520" s="2" t="inlineStr">
@@ -42268,7 +42268,7 @@
     <row r="534" ht="130" customHeight="1">
       <c r="A534" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2)</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B534" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@fb5c21ac140d0d5c69865596379825bc716106ea 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -964,7 +964,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 b</t>
+          <t>AU-5 b,AU-5 a</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1446,7 +1446,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>AU-6 (4),AU-7 (1),CM-6 b,AU-3,AU-14 (1),MA-4 (1) (a),AU-3 (1),AU-7 a,AU-12 a,CM-5 (1)</t>
+          <t>CM-5 (1),AU-7 (1),AU-6 (4),MA-4 (1) (a),CM-6 b,AU-7 a,AU-3 (1),AU-14 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -1531,7 +1531,7 @@
     <row r="14" ht="130" customHeight="1">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -1607,7 +1607,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1761,7 +1761,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -2131,7 +2131,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -2205,7 +2205,7 @@
     <row r="23" ht="130" customHeight="1">
       <c r="A23" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B23" s="2" t="inlineStr">
@@ -3249,7 +3249,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-14 (1),MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-14 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3340,7 +3340,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),AU-4</t>
+          <t>AU-4,AU-14 (1)</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -4161,7 +4161,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>AU-6 (4),AU-4 (1),CM-6 b</t>
+          <t>AU-4 (1),AU-6 (4),CM-6 b</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4466,7 +4466,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4552,7 +4552,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12),IA-2 (1)</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4636,7 +4636,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>SI-6 d,SI-6 b,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 d,SI-6 b</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4728,7 +4728,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>SI-6 d,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 d</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4812,7 +4812,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4887,7 +4887,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4962,7 +4962,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -5037,7 +5037,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5112,7 +5112,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5187,7 +5187,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5262,7 +5262,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5337,7 +5337,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5412,7 +5412,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5487,7 +5487,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-7 b,AU-12 c,AU-12 (3),AU-8 b,AU-7 a,AU-12 a,CM-5 (1)</t>
+          <t>CM-5 (1),AU-12 c,AU-7 b,CM-6 b,AU-7 a,AU-8 b,AU-12 a,AU-12 (3)</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5561,7 +5561,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AC-2 (4),AU-12 a</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5642,7 +5642,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AC-2 (4),AU-12 a</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5723,7 +5723,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AC-2 (4),AU-12 a</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5805,7 +5805,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AC-2 (4),AU-12 a</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5887,7 +5887,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AC-2 (4),AU-12 a</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5969,7 +5969,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AC-2 (4),AU-12 a</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -6051,7 +6051,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AC-2 (4),AU-12 a</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6133,7 +6133,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>SI-6 a,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 a</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -7171,7 +7171,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7245,7 +7245,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7319,7 +7319,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7393,7 +7393,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7473,7 +7473,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7558,7 +7558,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),MA-4 (6)</t>
+          <t>MA-4 (6),AC-17 (2)</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
@@ -7634,7 +7634,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
@@ -7969,7 +7969,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -8044,7 +8044,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8119,7 +8119,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8194,7 +8194,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8274,7 +8274,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8348,7 +8348,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8422,7 +8422,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8496,7 +8496,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8570,7 +8570,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8644,7 +8644,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8724,7 +8724,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8804,7 +8804,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -9055,7 +9055,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),AC-11 b</t>
+          <t>AC-11 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9553,7 +9553,7 @@
     <row r="117" ht="130" customHeight="1">
       <c r="A117" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2),MA-4 c,SC-13</t>
+          <t>MA-4 c,SC-13,SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B117" s="2" t="inlineStr">
@@ -9713,7 +9713,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9869,7 +9869,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -10225,7 +10225,7 @@
     <row r="126" ht="130" customHeight="1">
       <c r="A126" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B126" s="2" t="inlineStr">
@@ -10305,7 +10305,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>SC-28,SC-28 (1)</t>
+          <t>SC-28 (1),SC-28</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -11072,7 +11072,7 @@
     <row r="137" ht="130" customHeight="1">
       <c r="A137" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B137" s="2" t="inlineStr">
@@ -11153,7 +11153,7 @@
     <row r="138" ht="130" customHeight="1">
       <c r="A138" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B138" s="2" t="inlineStr">
@@ -11239,7 +11239,7 @@
     <row r="139" ht="130" customHeight="1">
       <c r="A139" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B139" s="2" t="inlineStr">
@@ -11685,7 +11685,7 @@
     <row r="144" ht="130" customHeight="1">
       <c r="A144" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B144" s="2" t="inlineStr">
@@ -11765,7 +11765,7 @@
     <row r="145" ht="130" customHeight="1">
       <c r="A145" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B145" s="2" t="inlineStr">
@@ -11845,7 +11845,7 @@
     <row r="146" ht="130" customHeight="1">
       <c r="A146" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B146" s="2" t="inlineStr">
@@ -12544,7 +12544,7 @@
     <row r="155" ht="130" customHeight="1">
       <c r="A155" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B155" s="2" t="inlineStr">
@@ -12620,7 +12620,7 @@
     <row r="156" ht="130" customHeight="1">
       <c r="A156" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B156" s="2" t="inlineStr">
@@ -12705,7 +12705,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B157" s="2" t="inlineStr">
@@ -12941,7 +12941,7 @@
     <row r="160" ht="130" customHeight="1">
       <c r="A160" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B160" s="2" t="inlineStr">
@@ -13018,7 +13018,7 @@
     <row r="161" ht="130" customHeight="1">
       <c r="A161" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B161" s="2" t="inlineStr">
@@ -13091,7 +13091,7 @@
     <row r="162" ht="130" customHeight="1">
       <c r="A162" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B162" s="2" t="inlineStr">
@@ -13164,7 +13164,7 @@
     <row r="163" ht="130" customHeight="1">
       <c r="A163" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B163" s="2" t="inlineStr">
@@ -13249,7 +13249,7 @@
     <row r="164" ht="130" customHeight="1">
       <c r="A164" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B164" s="2" t="inlineStr">
@@ -13324,7 +13324,7 @@
     <row r="165" ht="130" customHeight="1">
       <c r="A165" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B165" s="2" t="inlineStr">
@@ -13399,7 +13399,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B166" s="2" t="inlineStr">
@@ -13474,7 +13474,7 @@
     <row r="167" ht="130" customHeight="1">
       <c r="A167" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B167" s="2" t="inlineStr">
@@ -13977,7 +13977,7 @@
     <row r="174" ht="130" customHeight="1">
       <c r="A174" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B174" s="2" t="inlineStr">
@@ -14266,7 +14266,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B178" s="2" t="inlineStr">
@@ -14341,7 +14341,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B179" s="2" t="inlineStr">
@@ -14423,7 +14423,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B180" s="2" t="inlineStr">
@@ -14505,7 +14505,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">
@@ -14587,7 +14587,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B182" s="2" t="inlineStr">
@@ -14669,7 +14669,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B183" s="2" t="inlineStr">
@@ -14751,7 +14751,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B184" s="2" t="inlineStr">
@@ -14833,7 +14833,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B185" s="2" t="inlineStr">
@@ -14915,7 +14915,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B186" s="2" t="inlineStr">
@@ -14997,7 +14997,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B187" s="2" t="inlineStr">
@@ -15079,7 +15079,7 @@
     <row r="188" ht="130" customHeight="1">
       <c r="A188" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B188" s="2" t="inlineStr">
@@ -15157,7 +15157,7 @@
     <row r="189" ht="130" customHeight="1">
       <c r="A189" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B189" s="2" t="inlineStr">
@@ -15236,7 +15236,7 @@
     <row r="190" ht="130" customHeight="1">
       <c r="A190" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B190" s="2" t="inlineStr">
@@ -15318,7 +15318,7 @@
     <row r="191" ht="130" customHeight="1">
       <c r="A191" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B191" s="2" t="inlineStr">
@@ -15400,7 +15400,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B192" s="2" t="inlineStr">
@@ -15482,7 +15482,7 @@
     <row r="193" ht="130" customHeight="1">
       <c r="A193" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B193" s="2" t="inlineStr">
@@ -15564,7 +15564,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B194" s="2" t="inlineStr">
@@ -15646,7 +15646,7 @@
     <row r="195" ht="130" customHeight="1">
       <c r="A195" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B195" s="2" t="inlineStr">
@@ -15728,7 +15728,7 @@
     <row r="196" ht="130" customHeight="1">
       <c r="A196" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B196" s="2" t="inlineStr">
@@ -15803,7 +15803,7 @@
     <row r="197" ht="130" customHeight="1">
       <c r="A197" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-12 c,MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AC-2 (4),AU-12 a</t>
         </is>
       </c>
       <c r="B197" s="2" t="inlineStr">
@@ -15876,7 +15876,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AC-2 (4)</t>
         </is>
       </c>
       <c r="B198" s="2" t="inlineStr">
@@ -15953,7 +15953,7 @@
     <row r="199" ht="130" customHeight="1">
       <c r="A199" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (1),IA-2 (3),IA-2 (4)</t>
+          <t>IA-2 (3),IA-2 (4),IA-2 (2),IA-2 (1)</t>
         </is>
       </c>
       <c r="B199" s="2" t="inlineStr">
@@ -16040,7 +16040,7 @@
     <row r="200" ht="130" customHeight="1">
       <c r="A200" s="2" t="inlineStr">
         <is>
-          <t>IA-2,IA-2 (2),IA-2 (3),IA-2 (5),IA-2 (4)</t>
+          <t>IA-2 (3),IA-2 (4),IA-2 (2),IA-2,IA-2 (5)</t>
         </is>
       </c>
       <c r="B200" s="2" t="inlineStr">
@@ -16129,7 +16129,7 @@
     <row r="201" ht="130" customHeight="1">
       <c r="A201" s="2" t="inlineStr">
         <is>
-          <t>IA-2,IA-2 (2),IA-2 (3),IA-2 (5),IA-2 (4)</t>
+          <t>IA-2 (3),IA-2 (4),IA-2 (2),IA-2,IA-2 (5)</t>
         </is>
       </c>
       <c r="B201" s="2" t="inlineStr">
@@ -16274,12 +16274,18 @@
  $ sudo grep -i "FAIL_DELAY" /etc/login.defs 
 All output must show the value of "FAIL_DELAY" set as shown in the below:
  $ sudo grep -i "FAIL_DELAY" /etc/login.defs
-FAIL_DELAY  
+FAIL_DELAY 4 
 If the above command returns no output, or FAIL_DELAY is configured less than the expected value then this is a finding.</t>
         </is>
       </c>
       <c r="L202" s="2" t="n"/>
-      <c r="M202" s="2" t="inlineStr"/>
+      <c r="M202" s="2" t="inlineStr">
+        <is>
+          <t>Configure the Red Hat Enterprise Linux 9 to enforce a delay of at least 4 seconds between logon prompts following a failed console logon attempt.
+Modify the "/etc/login.defs" file to set the "FAIL_DELAY" parameter to 4 or greater:
+FAIL_DELAY 4</t>
+        </is>
+      </c>
       <c r="N202" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -16809,7 +16815,7 @@
     <row r="210" ht="130" customHeight="1">
       <c r="A210" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8 (2),SC-8</t>
+          <t>SC-8 (2),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B210" s="2" t="inlineStr">
@@ -16886,7 +16892,7 @@
     <row r="211" ht="130" customHeight="1">
       <c r="A211" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8 (2),SC-8</t>
+          <t>SC-8 (2),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B211" s="2" t="inlineStr">
@@ -16972,7 +16978,7 @@
     <row r="212" ht="130" customHeight="1">
       <c r="A212" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (1),AC-18 (1)</t>
+          <t>AC-18 (1),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B212" s="2" t="inlineStr">
@@ -17740,7 +17746,7 @@
     <row r="222" ht="130" customHeight="1">
       <c r="A222" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,IA-5 (1) (c),CM-6 b</t>
+          <t>IA-5 (1) (c),CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B222" s="2" t="inlineStr">
@@ -17900,7 +17906,7 @@
     <row r="224" ht="130" customHeight="1">
       <c r="A224" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,CM-6 b</t>
+          <t>CM-6 b,AU-12 a</t>
         </is>
       </c>
       <c r="B224" s="2" t="inlineStr">
@@ -17986,7 +17992,7 @@
     <row r="225" ht="130" customHeight="1">
       <c r="A225" s="2" t="inlineStr">
         <is>
-          <t>SC-5,SC-5 (2),CM-6 b</t>
+          <t>CM-6 b,SC-5 (2),SC-5</t>
         </is>
       </c>
       <c r="B225" s="2" t="inlineStr">
@@ -18258,7 +18264,7 @@
     <row r="228" ht="130" customHeight="1">
       <c r="A228" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-6 b</t>
+          <t>CM-6 b,SI-16</t>
         </is>
       </c>
       <c r="B228" s="2" t="inlineStr">
@@ -18356,7 +18362,7 @@
     <row r="229" ht="130" customHeight="1">
       <c r="A229" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),IA-2,IA-8</t>
+          <t>IA-8,AU-3 (1),IA-2</t>
         </is>
       </c>
       <c r="B229" s="2" t="inlineStr">
@@ -19490,7 +19496,7 @@
     <row r="243" ht="130" customHeight="1">
       <c r="A243" s="2" t="inlineStr">
         <is>
-          <t>SI-16,SC-3</t>
+          <t>SC-3,SI-16</t>
         </is>
       </c>
       <c r="B243" s="2" t="inlineStr">
@@ -20188,7 +20194,7 @@
     <row r="252" ht="130" customHeight="1">
       <c r="A252" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (a),CM-6 b,IA-5 (1) (b)</t>
+          <t>CM-6 b,IA-5 (1) (b),IA-5 (1) (a)</t>
         </is>
       </c>
       <c r="B252" s="2" t="inlineStr">
@@ -20756,7 +20762,7 @@
     <row r="259" ht="130" customHeight="1">
       <c r="A259" s="2" t="inlineStr">
         <is>
-          <t>SC-4,CM-6 b</t>
+          <t>CM-6 b,SC-4</t>
         </is>
       </c>
       <c r="B259" s="2" t="inlineStr">
@@ -20837,7 +20843,7 @@
     <row r="260" ht="130" customHeight="1">
       <c r="A260" s="2" t="inlineStr">
         <is>
-          <t>SC-4,SC-2</t>
+          <t>SC-2,SC-4</t>
         </is>
       </c>
       <c r="B260" s="2" t="inlineStr">
@@ -20925,7 +20931,7 @@
     <row r="261" ht="130" customHeight="1">
       <c r="A261" s="2" t="inlineStr">
         <is>
-          <t>SC-4,SC-2</t>
+          <t>SC-2,SC-4</t>
         </is>
       </c>
       <c r="B261" s="2" t="inlineStr">
@@ -21012,7 +21018,7 @@
     <row r="262" ht="130" customHeight="1">
       <c r="A262" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (1)</t>
         </is>
       </c>
       <c r="B262" s="2" t="inlineStr">
@@ -21101,7 +21107,7 @@
     <row r="263" ht="130" customHeight="1">
       <c r="A263" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B263" s="2" t="inlineStr">
@@ -21426,7 +21432,7 @@
     <row r="267" ht="130" customHeight="1">
       <c r="A267" s="2" t="inlineStr">
         <is>
-          <t>SI-6 a,SC-3</t>
+          <t>SC-3,SI-6 a</t>
         </is>
       </c>
       <c r="B267" s="2" t="inlineStr">
@@ -21508,7 +21514,7 @@
     <row r="268" ht="130" customHeight="1">
       <c r="A268" s="2" t="inlineStr">
         <is>
-          <t>AU-7 b,AC-6 (9),AU-12 (3),AU-8 b,AU-7 a,AC-6 (8),CM-5 (1)</t>
+          <t>AC-6 (8),CM-5 (1),AU-7 b,AU-7 a,AU-8 b,AC-6 (9),AU-12 (3)</t>
         </is>
       </c>
       <c r="B268" s="2" t="inlineStr">
@@ -21588,7 +21594,7 @@
     <row r="269" ht="130" customHeight="1">
       <c r="A269" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),CM-6 b</t>
+          <t>CM-6 b,IA-2 (5)</t>
         </is>
       </c>
       <c r="B269" s="2" t="inlineStr">
@@ -22175,7 +22181,7 @@
     <row r="277" ht="130" customHeight="1">
       <c r="A277" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (3),CM-6 b</t>
+          <t>CM-6 b,CM-5 (3)</t>
         </is>
       </c>
       <c r="B277" s="2" t="inlineStr">
@@ -22700,7 +22706,7 @@
     <row r="283" ht="130" customHeight="1">
       <c r="A283" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (a),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (a)</t>
         </is>
       </c>
       <c r="B283" s="2" t="inlineStr">
@@ -24139,7 +24145,7 @@
     <row r="302" ht="130" customHeight="1">
       <c r="A302" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (9),AC-2 (4),AU-12 c</t>
+          <t>AC-6 (9),AU-12 c,AC-2 (4)</t>
         </is>
       </c>
       <c r="B302" s="2" t="inlineStr">
@@ -24356,7 +24362,7 @@
     <row r="304" ht="130" customHeight="1">
       <c r="A304" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 (1)</t>
+          <t>AU-5 (1),AU-5 a</t>
         </is>
       </c>
       <c r="B304" s="2" t="inlineStr">
@@ -27868,7 +27874,7 @@
     <row r="351" ht="130" customHeight="1">
       <c r="A351" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),CM-6 b</t>
+          <t>CM-6 b,IA-2 (2)</t>
         </is>
       </c>
       <c r="B351" s="2" t="inlineStr">
@@ -27948,7 +27954,7 @@
     <row r="352" ht="130" customHeight="1">
       <c r="A352" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (1)</t>
+          <t>CM-5 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B352" s="2" t="inlineStr">
@@ -28021,7 +28027,7 @@
     <row r="353" ht="130" customHeight="1">
       <c r="A353" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (1)</t>
+          <t>CM-5 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B353" s="2" t="inlineStr">
@@ -28601,7 +28607,7 @@
     <row r="361" ht="130" customHeight="1">
       <c r="A361" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),CM-6 b</t>
+          <t>CM-6 b,AC-17 (2)</t>
         </is>
       </c>
       <c r="B361" s="2" t="inlineStr">
@@ -30967,7 +30973,7 @@
     <row r="392" ht="130" customHeight="1">
       <c r="A392" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),CM-6 b,CM-7 b,AC-17 (9)</t>
+          <t>AC-17 (9),CM-6 b,AC-17 (1),CM-7 b</t>
         </is>
       </c>
       <c r="B392" s="2" t="inlineStr">
@@ -31045,7 +31051,7 @@
     <row r="393" ht="130" customHeight="1">
       <c r="A393" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),CM-7 b,CM-6 b</t>
+          <t>CM-6 b,AC-17 (1),CM-7 b</t>
         </is>
       </c>
       <c r="B393" s="2" t="inlineStr">
@@ -33544,7 +33550,7 @@
     <row r="422" ht="130" customHeight="1">
       <c r="A422" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B422" s="2" t="inlineStr">
@@ -33619,7 +33625,7 @@
     <row r="423" ht="130" customHeight="1">
       <c r="A423" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B423" s="2" t="inlineStr">
@@ -35361,7 +35367,7 @@
     <row r="445" ht="130" customHeight="1">
       <c r="A445" s="2" t="inlineStr">
         <is>
-          <t>AU-4,CM-6 b</t>
+          <t>CM-6 b,AU-4</t>
         </is>
       </c>
       <c r="B445" s="2" t="inlineStr">
@@ -35661,7 +35667,7 @@
     <row r="449" ht="130" customHeight="1">
       <c r="A449" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B449" s="2" t="inlineStr">
@@ -35738,7 +35744,7 @@
     <row r="450" ht="130" customHeight="1">
       <c r="A450" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B450" s="2" t="inlineStr">
@@ -36120,7 +36126,7 @@
     <row r="455" ht="130" customHeight="1">
       <c r="A455" s="2" t="inlineStr">
         <is>
-          <t>SI-2 (2),CM-6 b</t>
+          <t>CM-6 b,SI-2 (2)</t>
         </is>
       </c>
       <c r="B455" s="2" t="inlineStr">
@@ -36767,7 +36773,7 @@
     <row r="464" ht="130" customHeight="1">
       <c r="A464" s="2" t="inlineStr">
         <is>
-          <t>SI-2 (2),CM-6 b</t>
+          <t>CM-6 b,SI-2 (2)</t>
         </is>
       </c>
       <c r="B464" s="2" t="inlineStr">
@@ -37288,7 +37294,7 @@
     <row r="471" ht="130" customHeight="1">
       <c r="A471" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8</t>
+          <t>SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B471" s="2" t="inlineStr">
@@ -38583,7 +38589,7 @@
     <row r="488" ht="130" customHeight="1">
       <c r="A488" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,IA-3</t>
+          <t>IA-3,CM-7 b</t>
         </is>
       </c>
       <c r="B488" s="2" t="inlineStr">
@@ -39890,7 +39896,7 @@
     <row r="505" ht="130" customHeight="1">
       <c r="A505" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-4 (1)</t>
+          <t>AU-4 (1),AU-4</t>
         </is>
       </c>
       <c r="B505" s="2" t="inlineStr">
@@ -42268,7 +42274,7 @@
     <row r="534" ht="130" customHeight="1">
       <c r="A534" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8</t>
+          <t>SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B534" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@31f9e4c68da837757dd0a221bfc3c7e803f2add6 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -541,7 +541,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -625,7 +625,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -710,7 +710,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -782,7 +782,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -964,7 +964,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-5 b,AU-5 a</t>
+          <t>AU-5 a,AU-5 b</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1446,7 +1446,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AU-7 (1),AU-6 (4),MA-4 (1) (a),CM-6 b,AU-7 a,AU-3 (1),AU-14 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-14 (1),CM-5 (1),MA-4 (1) (a),AU-3,AU-7 (1),AU-6 (4),AU-3 (1),CM-6 b,AU-7 a</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -1531,7 +1531,7 @@
     <row r="14" ht="130" customHeight="1">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -1607,7 +1607,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1761,7 +1761,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -2131,7 +2131,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -2205,7 +2205,7 @@
     <row r="23" ht="130" customHeight="1">
       <c r="A23" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B23" s="2" t="inlineStr">
@@ -3249,7 +3249,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-14 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,AU-14 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3340,7 +3340,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-14 (1)</t>
+          <t>AU-14 (1),AU-4</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3782,7 +3782,7 @@
     <row r="44" ht="130" customHeight="1">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-4 (1)</t>
+          <t>AU-4 (1),AU-3</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
@@ -4161,7 +4161,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-6 (4),CM-6 b</t>
+          <t>CM-6 b,AU-6 (4),AU-4 (1)</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4231,7 +4231,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),CM-6 b</t>
+          <t>CM-6 b,AU-4 (1)</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4311,7 +4311,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-8 (1) (b),AU-8 (1) (a)</t>
+          <t>AU-8 (1) (a),AU-8 (1) (b),AU-8 b</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4552,7 +4552,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12),IA-2 (1)</t>
+          <t>IA-2 (11),IA-2 (1),IA-2 (12)</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4812,7 +4812,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4887,7 +4887,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4962,7 +4962,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -5037,7 +5037,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5112,7 +5112,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5187,7 +5187,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5262,7 +5262,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5337,7 +5337,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5412,7 +5412,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5487,7 +5487,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AU-12 c,AU-7 b,CM-6 b,AU-7 a,AU-8 b,AU-12 a,AU-12 (3)</t>
+          <t>AU-12 a,AU-12 (3),CM-5 (1),AU-12 c,AU-8 b,CM-6 b,AU-7 a,AU-7 b</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5561,7 +5561,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AC-2 (4),AU-12 a</t>
+          <t>AU-12 a,AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5642,7 +5642,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AC-2 (4),AU-12 a</t>
+          <t>AU-12 a,AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5723,7 +5723,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AC-2 (4),AU-12 a</t>
+          <t>AU-12 a,AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5805,7 +5805,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AC-2 (4),AU-12 a</t>
+          <t>AU-12 a,AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5887,7 +5887,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AC-2 (4),AU-12 a</t>
+          <t>AU-12 a,AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5969,7 +5969,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AC-2 (4),AU-12 a</t>
+          <t>AU-12 a,AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -6051,7 +6051,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AC-2 (4),AU-12 a</t>
+          <t>AU-12 a,AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6133,7 +6133,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 a</t>
+          <t>SI-6 a,CM-3 (5)</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6207,7 +6207,7 @@
     <row r="75" ht="130" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
@@ -6290,7 +6290,7 @@
     <row r="76" ht="130" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
@@ -6368,7 +6368,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6459,7 +6459,7 @@
     <row r="78" ht="130" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
@@ -6541,7 +6541,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -7171,7 +7171,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7245,7 +7245,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7319,7 +7319,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7393,7 +7393,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7558,7 +7558,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),AC-17 (2)</t>
+          <t>AC-17 (2),MA-4 (6)</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
@@ -7969,7 +7969,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -8044,7 +8044,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8119,7 +8119,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8194,7 +8194,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8274,7 +8274,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8348,7 +8348,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8422,7 +8422,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8496,7 +8496,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8570,7 +8570,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8644,7 +8644,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8724,7 +8724,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8804,7 +8804,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -8884,7 +8884,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AC-11 (1),AC-11 b</t>
+          <t>AC-11 b,AC-11 (1)</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -9553,7 +9553,7 @@
     <row r="117" ht="130" customHeight="1">
       <c r="A117" s="2" t="inlineStr">
         <is>
-          <t>MA-4 c,SC-13,SC-8,AC-17 (2)</t>
+          <t>SC-13,SC-8,MA-4 c,AC-17 (2)</t>
         </is>
       </c>
       <c r="B117" s="2" t="inlineStr">
@@ -9635,7 +9635,7 @@
     <row r="118" ht="130" customHeight="1">
       <c r="A118" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B118" s="2" t="inlineStr">
@@ -9713,7 +9713,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9791,7 +9791,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -9869,7 +9869,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -9949,7 +9949,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B122" s="2" t="inlineStr">
@@ -10018,7 +10018,7 @@
     <row r="123" ht="130" customHeight="1">
       <c r="A123" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B123" s="2" t="inlineStr">
@@ -10087,7 +10087,7 @@
     <row r="124" ht="130" customHeight="1">
       <c r="A124" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B124" s="2" t="inlineStr">
@@ -10156,7 +10156,7 @@
     <row r="125" ht="130" customHeight="1">
       <c r="A125" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B125" s="2" t="inlineStr">
@@ -10225,7 +10225,7 @@
     <row r="126" ht="130" customHeight="1">
       <c r="A126" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B126" s="2" t="inlineStr">
@@ -11605,7 +11605,7 @@
     <row r="143" ht="130" customHeight="1">
       <c r="A143" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B143" s="2" t="inlineStr">
@@ -11685,7 +11685,7 @@
     <row r="144" ht="130" customHeight="1">
       <c r="A144" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B144" s="2" t="inlineStr">
@@ -11765,7 +11765,7 @@
     <row r="145" ht="130" customHeight="1">
       <c r="A145" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B145" s="2" t="inlineStr">
@@ -11845,7 +11845,7 @@
     <row r="146" ht="130" customHeight="1">
       <c r="A146" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B146" s="2" t="inlineStr">
@@ -12941,7 +12941,7 @@
     <row r="160" ht="130" customHeight="1">
       <c r="A160" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B160" s="2" t="inlineStr">
@@ -13018,7 +13018,7 @@
     <row r="161" ht="130" customHeight="1">
       <c r="A161" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B161" s="2" t="inlineStr">
@@ -13091,7 +13091,7 @@
     <row r="162" ht="130" customHeight="1">
       <c r="A162" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B162" s="2" t="inlineStr">
@@ -13164,7 +13164,7 @@
     <row r="163" ht="130" customHeight="1">
       <c r="A163" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B163" s="2" t="inlineStr">
@@ -13249,7 +13249,7 @@
     <row r="164" ht="130" customHeight="1">
       <c r="A164" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B164" s="2" t="inlineStr">
@@ -13324,7 +13324,7 @@
     <row r="165" ht="130" customHeight="1">
       <c r="A165" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B165" s="2" t="inlineStr">
@@ -13399,7 +13399,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B166" s="2" t="inlineStr">
@@ -13474,7 +13474,7 @@
     <row r="167" ht="130" customHeight="1">
       <c r="A167" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B167" s="2" t="inlineStr">
@@ -13549,7 +13549,7 @@
     <row r="168" ht="130" customHeight="1">
       <c r="A168" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B168" s="2" t="inlineStr">
@@ -13620,7 +13620,7 @@
     <row r="169" ht="130" customHeight="1">
       <c r="A169" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B169" s="2" t="inlineStr">
@@ -13691,7 +13691,7 @@
     <row r="170" ht="130" customHeight="1">
       <c r="A170" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B170" s="2" t="inlineStr">
@@ -13763,7 +13763,7 @@
     <row r="171" ht="130" customHeight="1">
       <c r="A171" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B171" s="2" t="inlineStr">
@@ -13834,7 +13834,7 @@
     <row r="172" ht="130" customHeight="1">
       <c r="A172" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B172" s="2" t="inlineStr">
@@ -13905,7 +13905,7 @@
     <row r="173" ht="130" customHeight="1">
       <c r="A173" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B173" s="2" t="inlineStr">
@@ -13977,7 +13977,7 @@
     <row r="174" ht="130" customHeight="1">
       <c r="A174" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B174" s="2" t="inlineStr">
@@ -14052,7 +14052,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B175" s="2" t="inlineStr">
@@ -14123,7 +14123,7 @@
     <row r="176" ht="130" customHeight="1">
       <c r="A176" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B176" s="2" t="inlineStr">
@@ -14194,7 +14194,7 @@
     <row r="177" ht="130" customHeight="1">
       <c r="A177" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B177" s="2" t="inlineStr">
@@ -14266,7 +14266,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B178" s="2" t="inlineStr">
@@ -14341,7 +14341,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B179" s="2" t="inlineStr">
@@ -14423,7 +14423,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B180" s="2" t="inlineStr">
@@ -14505,7 +14505,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">
@@ -14587,7 +14587,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B182" s="2" t="inlineStr">
@@ -14669,7 +14669,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B183" s="2" t="inlineStr">
@@ -14751,7 +14751,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B184" s="2" t="inlineStr">
@@ -14833,7 +14833,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B185" s="2" t="inlineStr">
@@ -14915,7 +14915,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B186" s="2" t="inlineStr">
@@ -14997,7 +14997,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B187" s="2" t="inlineStr">
@@ -15079,7 +15079,7 @@
     <row r="188" ht="130" customHeight="1">
       <c r="A188" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B188" s="2" t="inlineStr">
@@ -15157,7 +15157,7 @@
     <row r="189" ht="130" customHeight="1">
       <c r="A189" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B189" s="2" t="inlineStr">
@@ -15236,7 +15236,7 @@
     <row r="190" ht="130" customHeight="1">
       <c r="A190" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B190" s="2" t="inlineStr">
@@ -15318,7 +15318,7 @@
     <row r="191" ht="130" customHeight="1">
       <c r="A191" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B191" s="2" t="inlineStr">
@@ -15400,7 +15400,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B192" s="2" t="inlineStr">
@@ -15482,7 +15482,7 @@
     <row r="193" ht="130" customHeight="1">
       <c r="A193" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B193" s="2" t="inlineStr">
@@ -15564,7 +15564,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B194" s="2" t="inlineStr">
@@ -15646,7 +15646,7 @@
     <row r="195" ht="130" customHeight="1">
       <c r="A195" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B195" s="2" t="inlineStr">
@@ -15728,7 +15728,7 @@
     <row r="196" ht="130" customHeight="1">
       <c r="A196" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B196" s="2" t="inlineStr">
@@ -15803,7 +15803,7 @@
     <row r="197" ht="130" customHeight="1">
       <c r="A197" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AC-2 (4),AU-12 a</t>
+          <t>AU-12 a,AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B197" s="2" t="inlineStr">
@@ -15876,7 +15876,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AC-2 (4)</t>
+          <t>AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B198" s="2" t="inlineStr">
@@ -15953,7 +15953,7 @@
     <row r="199" ht="130" customHeight="1">
       <c r="A199" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (4),IA-2 (2),IA-2 (1)</t>
+          <t>IA-2 (4),IA-2 (1),IA-2 (3),IA-2 (2)</t>
         </is>
       </c>
       <c r="B199" s="2" t="inlineStr">
@@ -16040,7 +16040,7 @@
     <row r="200" ht="130" customHeight="1">
       <c r="A200" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (4),IA-2 (2),IA-2,IA-2 (5)</t>
+          <t>IA-2 (2),IA-2 (3),IA-2,IA-2 (4),IA-2 (5)</t>
         </is>
       </c>
       <c r="B200" s="2" t="inlineStr">
@@ -16129,7 +16129,7 @@
     <row r="201" ht="130" customHeight="1">
       <c r="A201" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (4),IA-2 (2),IA-2,IA-2 (5)</t>
+          <t>IA-2 (2),IA-2 (3),IA-2,IA-2 (4),IA-2 (5)</t>
         </is>
       </c>
       <c r="B201" s="2" t="inlineStr">
@@ -16815,7 +16815,7 @@
     <row r="210" ht="130" customHeight="1">
       <c r="A210" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8,SC-8 (1)</t>
+          <t>SC-8,SC-8 (2),SC-8 (1)</t>
         </is>
       </c>
       <c r="B210" s="2" t="inlineStr">
@@ -16892,7 +16892,7 @@
     <row r="211" ht="130" customHeight="1">
       <c r="A211" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8,SC-8 (1)</t>
+          <t>SC-8,SC-8 (2),SC-8 (1)</t>
         </is>
       </c>
       <c r="B211" s="2" t="inlineStr">
@@ -16978,7 +16978,7 @@
     <row r="212" ht="130" customHeight="1">
       <c r="A212" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),SC-8 (1),SC-8</t>
+          <t>SC-8,SC-8 (1),AC-18 (1)</t>
         </is>
       </c>
       <c r="B212" s="2" t="inlineStr">
@@ -17746,7 +17746,7 @@
     <row r="222" ht="130" customHeight="1">
       <c r="A222" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-7 a,CM-6 b</t>
+          <t>CM-7 a,CM-6 b,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B222" s="2" t="inlineStr">
@@ -17906,7 +17906,7 @@
     <row r="224" ht="130" customHeight="1">
       <c r="A224" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-12 a</t>
+          <t>AU-12 a,CM-6 b</t>
         </is>
       </c>
       <c r="B224" s="2" t="inlineStr">
@@ -17992,7 +17992,7 @@
     <row r="225" ht="130" customHeight="1">
       <c r="A225" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-5 (2),SC-5</t>
+          <t>CM-6 b,SC-5,SC-5 (2)</t>
         </is>
       </c>
       <c r="B225" s="2" t="inlineStr">
@@ -18362,7 +18362,7 @@
     <row r="229" ht="130" customHeight="1">
       <c r="A229" s="2" t="inlineStr">
         <is>
-          <t>IA-8,AU-3 (1),IA-2</t>
+          <t>IA-2,IA-8,AU-3 (1)</t>
         </is>
       </c>
       <c r="B229" s="2" t="inlineStr">
@@ -19336,7 +19336,7 @@
     <row r="241" ht="130" customHeight="1">
       <c r="A241" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-16,SC-2</t>
+          <t>CM-6 b,SC-2,SI-16</t>
         </is>
       </c>
       <c r="B241" s="2" t="inlineStr">
@@ -20194,7 +20194,7 @@
     <row r="252" ht="130" customHeight="1">
       <c r="A252" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (b),IA-5 (1) (a)</t>
+          <t>CM-6 b,IA-5 (1) (a),IA-5 (1) (b)</t>
         </is>
       </c>
       <c r="B252" s="2" t="inlineStr">
@@ -20762,7 +20762,7 @@
     <row r="259" ht="130" customHeight="1">
       <c r="A259" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-4</t>
+          <t>SC-4,CM-6 b</t>
         </is>
       </c>
       <c r="B259" s="2" t="inlineStr">
@@ -20843,7 +20843,7 @@
     <row r="260" ht="130" customHeight="1">
       <c r="A260" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SC-4</t>
+          <t>SC-4,SC-2</t>
         </is>
       </c>
       <c r="B260" s="2" t="inlineStr">
@@ -20931,7 +20931,7 @@
     <row r="261" ht="130" customHeight="1">
       <c r="A261" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SC-4</t>
+          <t>SC-4,SC-2</t>
         </is>
       </c>
       <c r="B261" s="2" t="inlineStr">
@@ -21514,7 +21514,7 @@
     <row r="268" ht="130" customHeight="1">
       <c r="A268" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (8),CM-5 (1),AU-7 b,AU-7 a,AU-8 b,AC-6 (9),AU-12 (3)</t>
+          <t>AC-6 (8),AC-6 (9),AU-12 (3),CM-5 (1),AU-8 b,AU-7 a,AU-7 b</t>
         </is>
       </c>
       <c r="B268" s="2" t="inlineStr">
@@ -24145,7 +24145,7 @@
     <row r="302" ht="130" customHeight="1">
       <c r="A302" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (9),AU-12 c,AC-2 (4)</t>
+          <t>AC-2 (4),AC-6 (9),AU-12 c</t>
         </is>
       </c>
       <c r="B302" s="2" t="inlineStr">
@@ -27724,7 +27724,7 @@
     <row r="349" ht="130" customHeight="1">
       <c r="A349" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B349" s="2" t="inlineStr">
@@ -27954,7 +27954,7 @@
     <row r="352" ht="130" customHeight="1">
       <c r="A352" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),CM-6 b</t>
+          <t>CM-6 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B352" s="2" t="inlineStr">
@@ -28027,7 +28027,7 @@
     <row r="353" ht="130" customHeight="1">
       <c r="A353" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),CM-6 b</t>
+          <t>CM-6 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B353" s="2" t="inlineStr">
@@ -30335,7 +30335,7 @@
     <row r="384" ht="130" customHeight="1">
       <c r="A384" s="2" t="inlineStr">
         <is>
-          <t>AU-3,CM-6 b</t>
+          <t>CM-6 b,AU-3</t>
         </is>
       </c>
       <c r="B384" s="2" t="inlineStr">
@@ -30973,7 +30973,7 @@
     <row r="392" ht="130" customHeight="1">
       <c r="A392" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (9),CM-6 b,AC-17 (1),CM-7 b</t>
+          <t>AC-17 (1),CM-6 b,AC-17 (9),CM-7 b</t>
         </is>
       </c>
       <c r="B392" s="2" t="inlineStr">
@@ -31051,7 +31051,7 @@
     <row r="393" ht="130" customHeight="1">
       <c r="A393" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-17 (1),CM-7 b</t>
+          <t>AC-17 (1),CM-6 b,CM-7 b</t>
         </is>
       </c>
       <c r="B393" s="2" t="inlineStr">
@@ -33550,7 +33550,7 @@
     <row r="422" ht="130" customHeight="1">
       <c r="A422" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B422" s="2" t="inlineStr">
@@ -33625,7 +33625,7 @@
     <row r="423" ht="130" customHeight="1">
       <c r="A423" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B423" s="2" t="inlineStr">
@@ -35667,7 +35667,7 @@
     <row r="449" ht="130" customHeight="1">
       <c r="A449" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B449" s="2" t="inlineStr">
@@ -35744,7 +35744,7 @@
     <row r="450" ht="130" customHeight="1">
       <c r="A450" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B450" s="2" t="inlineStr">
@@ -37064,7 +37064,7 @@
     <row r="468" ht="130" customHeight="1">
       <c r="A468" s="2" t="inlineStr">
         <is>
-          <t>MA-4 e,AC-12,MA-4 (7),SC-10</t>
+          <t>MA-4 e,MA-4 (7),SC-10,AC-12</t>
         </is>
       </c>
       <c r="B468" s="2" t="inlineStr">
@@ -37139,7 +37139,7 @@
     <row r="469" ht="130" customHeight="1">
       <c r="A469" s="2" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B469" s="2" t="inlineStr">
@@ -37218,7 +37218,7 @@
     <row r="470" ht="130" customHeight="1">
       <c r="A470" s="2" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B470" s="2" t="inlineStr">
@@ -40135,7 +40135,7 @@
     <row r="508" ht="130" customHeight="1">
       <c r="A508" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B508" s="2" t="inlineStr">
@@ -40237,7 +40237,7 @@
     <row r="509" ht="130" customHeight="1">
       <c r="A509" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B509" s="2" t="inlineStr">
@@ -40347,7 +40347,7 @@
     <row r="510" ht="130" customHeight="1">
       <c r="A510" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B510" s="2" t="inlineStr">
@@ -40458,7 +40458,7 @@
     <row r="511" ht="130" customHeight="1">
       <c r="A511" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B511" s="2" t="inlineStr">
@@ -41161,7 +41161,7 @@
     <row r="520" ht="130" customHeight="1">
       <c r="A520" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8</t>
+          <t>SC-8,SC-8 (2)</t>
         </is>
       </c>
       <c r="B520" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@aa9f957e595eeb29c9a6d6e1278249a62b482118 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -541,7 +541,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -625,7 +625,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -710,7 +710,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -782,7 +782,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -964,7 +964,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 b</t>
+          <t>AU-5 b,AU-5 a</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1446,7 +1446,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-14 (1),CM-5 (1),MA-4 (1) (a),AU-3,AU-7 (1),AU-6 (4),AU-3 (1),CM-6 b,AU-7 a</t>
+          <t>CM-6 b,AU-7 a,AU-14 (1),AU-6 (4),AU-3 (1),AU-3,AU-7 (1),AU-12 a,MA-4 (1) (a),CM-5 (1)</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -1531,7 +1531,7 @@
     <row r="14" ht="130" customHeight="1">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -1607,7 +1607,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1761,7 +1761,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -2131,7 +2131,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -2205,7 +2205,7 @@
     <row r="23" ht="130" customHeight="1">
       <c r="A23" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B23" s="2" t="inlineStr">
@@ -3249,7 +3249,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-14 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-14 (1),AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3340,7 +3340,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),AU-4</t>
+          <t>AU-4,AU-14 (1)</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -4466,7 +4466,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4552,7 +4552,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (1),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11),IA-2 (1)</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4636,7 +4636,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 d,SI-6 b</t>
+          <t>SI-6 d,SI-6 b,CM-3 (5)</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4728,7 +4728,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 d</t>
+          <t>SI-6 d,CM-3 (5)</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4812,7 +4812,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4887,7 +4887,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4962,7 +4962,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -5037,7 +5037,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5112,7 +5112,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5187,7 +5187,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5262,7 +5262,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5337,7 +5337,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5412,7 +5412,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5487,7 +5487,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-12 (3),CM-5 (1),AU-12 c,AU-8 b,CM-6 b,AU-7 a,AU-7 b</t>
+          <t>CM-6 b,AU-8 b,AU-7 a,AU-7 b,AU-12 a,AU-12 c,CM-5 (1),AU-12 (3)</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5561,7 +5561,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AC-2 (4),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5642,7 +5642,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AC-2 (4),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5723,7 +5723,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AC-2 (4),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5805,7 +5805,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AC-2 (4),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5887,7 +5887,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AC-2 (4),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5969,7 +5969,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AC-2 (4),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -6051,7 +6051,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AC-2 (4),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6207,7 +6207,7 @@
     <row r="75" ht="130" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
@@ -6290,7 +6290,7 @@
     <row r="76" ht="130" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
@@ -6368,7 +6368,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6459,7 +6459,7 @@
     <row r="78" ht="130" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
@@ -6541,7 +6541,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -7171,7 +7171,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7245,7 +7245,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7319,7 +7319,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7393,7 +7393,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7473,7 +7473,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7558,7 +7558,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),MA-4 (6)</t>
+          <t>MA-4 (6),AC-17 (2)</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
@@ -7634,7 +7634,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
@@ -7969,7 +7969,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -8044,7 +8044,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8119,7 +8119,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8194,7 +8194,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8274,7 +8274,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8348,7 +8348,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8422,7 +8422,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8496,7 +8496,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8570,7 +8570,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8644,7 +8644,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8724,7 +8724,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8804,7 +8804,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -8884,7 +8884,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 (1)</t>
+          <t>AC-11 (1),AC-11 b</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -9055,7 +9055,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-6 (10)</t>
+          <t>AC-6 (10),AC-11 b</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9553,7 +9553,7 @@
     <row r="117" ht="130" customHeight="1">
       <c r="A117" s="2" t="inlineStr">
         <is>
-          <t>SC-13,SC-8,MA-4 c,AC-17 (2)</t>
+          <t>SC-8,MA-4 c,SC-13,AC-17 (2)</t>
         </is>
       </c>
       <c r="B117" s="2" t="inlineStr">
@@ -9713,7 +9713,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9869,7 +9869,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -10225,7 +10225,7 @@
     <row r="126" ht="130" customHeight="1">
       <c r="A126" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B126" s="2" t="inlineStr">
@@ -10305,7 +10305,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>SC-28 (1),SC-28</t>
+          <t>SC-28,SC-28 (1)</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -11685,7 +11685,7 @@
     <row r="144" ht="130" customHeight="1">
       <c r="A144" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B144" s="2" t="inlineStr">
@@ -11765,7 +11765,7 @@
     <row r="145" ht="130" customHeight="1">
       <c r="A145" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B145" s="2" t="inlineStr">
@@ -11845,7 +11845,7 @@
     <row r="146" ht="130" customHeight="1">
       <c r="A146" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B146" s="2" t="inlineStr">
@@ -12157,7 +12157,7 @@
     <row r="150" ht="130" customHeight="1">
       <c r="A150" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),IA-7</t>
+          <t>IA-7,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B150" s="2" t="inlineStr">
@@ -12544,7 +12544,7 @@
     <row r="155" ht="130" customHeight="1">
       <c r="A155" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B155" s="2" t="inlineStr">
@@ -12620,7 +12620,7 @@
     <row r="156" ht="130" customHeight="1">
       <c r="A156" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B156" s="2" t="inlineStr">
@@ -12705,7 +12705,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B157" s="2" t="inlineStr">
@@ -12862,7 +12862,7 @@
     <row r="159" ht="130" customHeight="1">
       <c r="A159" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,IA-7</t>
+          <t>IA-7,CM-7 a</t>
         </is>
       </c>
       <c r="B159" s="2" t="inlineStr">
@@ -12941,7 +12941,7 @@
     <row r="160" ht="130" customHeight="1">
       <c r="A160" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B160" s="2" t="inlineStr">
@@ -13018,7 +13018,7 @@
     <row r="161" ht="130" customHeight="1">
       <c r="A161" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B161" s="2" t="inlineStr">
@@ -13091,7 +13091,7 @@
     <row r="162" ht="130" customHeight="1">
       <c r="A162" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B162" s="2" t="inlineStr">
@@ -13164,7 +13164,7 @@
     <row r="163" ht="130" customHeight="1">
       <c r="A163" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B163" s="2" t="inlineStr">
@@ -13249,7 +13249,7 @@
     <row r="164" ht="130" customHeight="1">
       <c r="A164" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B164" s="2" t="inlineStr">
@@ -13324,7 +13324,7 @@
     <row r="165" ht="130" customHeight="1">
       <c r="A165" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B165" s="2" t="inlineStr">
@@ -13399,7 +13399,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B166" s="2" t="inlineStr">
@@ -13474,7 +13474,7 @@
     <row r="167" ht="130" customHeight="1">
       <c r="A167" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B167" s="2" t="inlineStr">
@@ -13977,7 +13977,7 @@
     <row r="174" ht="130" customHeight="1">
       <c r="A174" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B174" s="2" t="inlineStr">
@@ -14266,7 +14266,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B178" s="2" t="inlineStr">
@@ -14341,7 +14341,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B179" s="2" t="inlineStr">
@@ -14423,7 +14423,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B180" s="2" t="inlineStr">
@@ -14505,7 +14505,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">
@@ -14587,7 +14587,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B182" s="2" t="inlineStr">
@@ -14669,7 +14669,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B183" s="2" t="inlineStr">
@@ -14751,7 +14751,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B184" s="2" t="inlineStr">
@@ -14833,7 +14833,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B185" s="2" t="inlineStr">
@@ -14915,7 +14915,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B186" s="2" t="inlineStr">
@@ -14997,7 +14997,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B187" s="2" t="inlineStr">
@@ -15079,7 +15079,7 @@
     <row r="188" ht="130" customHeight="1">
       <c r="A188" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B188" s="2" t="inlineStr">
@@ -15157,7 +15157,7 @@
     <row r="189" ht="130" customHeight="1">
       <c r="A189" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B189" s="2" t="inlineStr">
@@ -15236,7 +15236,7 @@
     <row r="190" ht="130" customHeight="1">
       <c r="A190" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B190" s="2" t="inlineStr">
@@ -15318,7 +15318,7 @@
     <row r="191" ht="130" customHeight="1">
       <c r="A191" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B191" s="2" t="inlineStr">
@@ -15400,7 +15400,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B192" s="2" t="inlineStr">
@@ -15482,7 +15482,7 @@
     <row r="193" ht="130" customHeight="1">
       <c r="A193" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B193" s="2" t="inlineStr">
@@ -15564,7 +15564,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B194" s="2" t="inlineStr">
@@ -15646,7 +15646,7 @@
     <row r="195" ht="130" customHeight="1">
       <c r="A195" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B195" s="2" t="inlineStr">
@@ -15728,7 +15728,7 @@
     <row r="196" ht="130" customHeight="1">
       <c r="A196" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B196" s="2" t="inlineStr">
@@ -15803,7 +15803,7 @@
     <row r="197" ht="130" customHeight="1">
       <c r="A197" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AC-2 (4),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B197" s="2" t="inlineStr">
@@ -15876,7 +15876,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,AC-2 (4),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B198" s="2" t="inlineStr">
@@ -15953,7 +15953,7 @@
     <row r="199" ht="130" customHeight="1">
       <c r="A199" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2 (1),IA-2 (3),IA-2 (2)</t>
+          <t>IA-2 (2),IA-2 (3),IA-2 (4),IA-2 (1)</t>
         </is>
       </c>
       <c r="B199" s="2" t="inlineStr">
@@ -16040,7 +16040,7 @@
     <row r="200" ht="130" customHeight="1">
       <c r="A200" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (3),IA-2,IA-2 (4),IA-2 (5)</t>
+          <t>IA-2 (2),IA-2,IA-2 (4),IA-2 (5),IA-2 (3)</t>
         </is>
       </c>
       <c r="B200" s="2" t="inlineStr">
@@ -16129,7 +16129,7 @@
     <row r="201" ht="130" customHeight="1">
       <c r="A201" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (3),IA-2,IA-2 (4),IA-2 (5)</t>
+          <t>IA-2 (2),IA-2,IA-2 (4),IA-2 (5),IA-2 (3)</t>
         </is>
       </c>
       <c r="B201" s="2" t="inlineStr">
@@ -16815,7 +16815,7 @@
     <row r="210" ht="130" customHeight="1">
       <c r="A210" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (2),SC-8 (1)</t>
+          <t>SC-8 (2),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B210" s="2" t="inlineStr">
@@ -16892,7 +16892,7 @@
     <row r="211" ht="130" customHeight="1">
       <c r="A211" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (2),SC-8 (1)</t>
+          <t>SC-8 (2),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B211" s="2" t="inlineStr">
@@ -16978,7 +16978,7 @@
     <row r="212" ht="130" customHeight="1">
       <c r="A212" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (1),AC-18 (1)</t>
+          <t>AC-18 (1),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B212" s="2" t="inlineStr">
@@ -17138,7 +17138,7 @@
     <row r="214" ht="130" customHeight="1">
       <c r="A214" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,SC-10</t>
+          <t>SC-10,AC-11 a</t>
         </is>
       </c>
       <c r="B214" s="2" t="inlineStr">
@@ -17992,7 +17992,7 @@
     <row r="225" ht="130" customHeight="1">
       <c r="A225" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-5,SC-5 (2)</t>
+          <t>SC-5 (2),CM-6 b,SC-5</t>
         </is>
       </c>
       <c r="B225" s="2" t="inlineStr">
@@ -19336,7 +19336,7 @@
     <row r="241" ht="130" customHeight="1">
       <c r="A241" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-2,SI-16</t>
+          <t>CM-6 b,SI-16,SC-2</t>
         </is>
       </c>
       <c r="B241" s="2" t="inlineStr">
@@ -19658,7 +19658,7 @@
     <row r="245" ht="130" customHeight="1">
       <c r="A245" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,AC-18 (1)</t>
+          <t>AC-18 (1),CM-7 a</t>
         </is>
       </c>
       <c r="B245" s="2" t="inlineStr">
@@ -20194,7 +20194,7 @@
     <row r="252" ht="130" customHeight="1">
       <c r="A252" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (a),IA-5 (1) (b)</t>
+          <t>IA-5 (1) (b),CM-6 b,IA-5 (1) (a)</t>
         </is>
       </c>
       <c r="B252" s="2" t="inlineStr">
@@ -21107,7 +21107,7 @@
     <row r="263" ht="130" customHeight="1">
       <c r="A263" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B263" s="2" t="inlineStr">
@@ -21432,7 +21432,7 @@
     <row r="267" ht="130" customHeight="1">
       <c r="A267" s="2" t="inlineStr">
         <is>
-          <t>SC-3,SI-6 a</t>
+          <t>SI-6 a,SC-3</t>
         </is>
       </c>
       <c r="B267" s="2" t="inlineStr">
@@ -21514,7 +21514,7 @@
     <row r="268" ht="130" customHeight="1">
       <c r="A268" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (8),AC-6 (9),AU-12 (3),CM-5 (1),AU-8 b,AU-7 a,AU-7 b</t>
+          <t>AU-8 b,AU-7 a,AU-7 b,AC-6 (8),AC-6 (9),CM-5 (1),AU-12 (3)</t>
         </is>
       </c>
       <c r="B268" s="2" t="inlineStr">
@@ -22181,7 +22181,7 @@
     <row r="277" ht="130" customHeight="1">
       <c r="A277" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (3)</t>
+          <t>CM-5 (3),CM-6 b</t>
         </is>
       </c>
       <c r="B277" s="2" t="inlineStr">
@@ -24145,7 +24145,7 @@
     <row r="302" ht="130" customHeight="1">
       <c r="A302" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AC-6 (9),AU-12 c</t>
+          <t>AC-6 (9),AU-12 c,AC-2 (4)</t>
         </is>
       </c>
       <c r="B302" s="2" t="inlineStr">
@@ -24362,7 +24362,7 @@
     <row r="304" ht="130" customHeight="1">
       <c r="A304" s="2" t="inlineStr">
         <is>
-          <t>AU-5 (1),AU-5 a</t>
+          <t>AU-5 a,AU-5 (1)</t>
         </is>
       </c>
       <c r="B304" s="2" t="inlineStr">
@@ -27874,7 +27874,7 @@
     <row r="351" ht="130" customHeight="1">
       <c r="A351" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (2)</t>
+          <t>IA-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B351" s="2" t="inlineStr">
@@ -30579,7 +30579,7 @@
     <row r="387" ht="130" customHeight="1">
       <c r="A387" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B387" s="2" t="inlineStr">
@@ -30973,7 +30973,7 @@
     <row r="392" ht="130" customHeight="1">
       <c r="A392" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),CM-6 b,AC-17 (9),CM-7 b</t>
+          <t>AC-17 (1),AC-17 (9),CM-6 b,CM-7 b</t>
         </is>
       </c>
       <c r="B392" s="2" t="inlineStr">
@@ -33550,7 +33550,7 @@
     <row r="422" ht="130" customHeight="1">
       <c r="A422" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B422" s="2" t="inlineStr">
@@ -33625,7 +33625,7 @@
     <row r="423" ht="130" customHeight="1">
       <c r="A423" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B423" s="2" t="inlineStr">
@@ -34312,7 +34312,7 @@
     <row r="432" ht="130" customHeight="1">
       <c r="A432" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B432" s="2" t="inlineStr">
@@ -34915,7 +34915,7 @@
     <row r="439" ht="130" customHeight="1">
       <c r="A439" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B439" s="2" t="inlineStr">
@@ -35367,7 +35367,7 @@
     <row r="445" ht="130" customHeight="1">
       <c r="A445" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-4</t>
+          <t>AU-4,CM-6 b</t>
         </is>
       </c>
       <c r="B445" s="2" t="inlineStr">
@@ -35667,7 +35667,7 @@
     <row r="449" ht="130" customHeight="1">
       <c r="A449" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B449" s="2" t="inlineStr">
@@ -35744,7 +35744,7 @@
     <row r="450" ht="130" customHeight="1">
       <c r="A450" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B450" s="2" t="inlineStr">
@@ -37064,7 +37064,7 @@
     <row r="468" ht="130" customHeight="1">
       <c r="A468" s="2" t="inlineStr">
         <is>
-          <t>MA-4 e,MA-4 (7),SC-10,AC-12</t>
+          <t>SC-10,MA-4 e,MA-4 (7),AC-12</t>
         </is>
       </c>
       <c r="B468" s="2" t="inlineStr">
@@ -39896,7 +39896,7 @@
     <row r="505" ht="130" customHeight="1">
       <c r="A505" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-4</t>
+          <t>AU-4,AU-4 (1)</t>
         </is>
       </c>
       <c r="B505" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@8fb9a0a5b8ee416bcd428a3815ee2a735cfdd069 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -541,7 +541,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -625,7 +625,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -710,7 +710,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -782,7 +782,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -964,7 +964,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-5 b,AU-5 a</t>
+          <t>AU-5 a,AU-5 b</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1446,7 +1446,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-7 a,AU-14 (1),AU-6 (4),AU-3 (1),AU-3,AU-7 (1),AU-12 a,MA-4 (1) (a),CM-5 (1)</t>
+          <t>AU-7 (1),AU-14 (1),AU-3 (1),CM-5 (1),AU-3,AU-12 a,AU-6 (4),CM-6 b,MA-4 (1) (a),AU-7 a</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -3249,7 +3249,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-14 (1),AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3782,7 +3782,7 @@
     <row r="44" ht="130" customHeight="1">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-3</t>
+          <t>AU-3,AU-4 (1)</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
@@ -4161,7 +4161,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-6 (4),AU-4 (1)</t>
+          <t>CM-6 b,AU-4 (1),AU-6 (4)</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4311,7 +4311,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (a),AU-8 (1) (b),AU-8 b</t>
+          <t>AU-8 (1) (b),AU-8 b,AU-8 (1) (a)</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4466,7 +4466,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4552,7 +4552,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11),IA-2 (1)</t>
+          <t>IA-2 (11),IA-2 (1),IA-2 (12)</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4636,7 +4636,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>SI-6 d,SI-6 b,CM-3 (5)</t>
+          <t>SI-6 b,CM-3 (5),SI-6 d</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4728,7 +4728,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>SI-6 d,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 d</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4812,7 +4812,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4887,7 +4887,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4962,7 +4962,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -5037,7 +5037,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5112,7 +5112,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5187,7 +5187,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5262,7 +5262,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5337,7 +5337,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5412,7 +5412,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5487,7 +5487,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-8 b,AU-7 a,AU-7 b,AU-12 a,AU-12 c,CM-5 (1),AU-12 (3)</t>
+          <t>AU-8 b,CM-5 (1),CM-6 b,AU-12 a,AU-12 c,AU-12 (3),AU-7 a,AU-7 b</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5561,7 +5561,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,AC-2 (4),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AC-2 (4),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5642,7 +5642,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,AC-2 (4),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AC-2 (4),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5723,7 +5723,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,AC-2 (4),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AC-2 (4),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5805,7 +5805,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,AC-2 (4),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AC-2 (4),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5887,7 +5887,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,AC-2 (4),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AC-2 (4),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5969,7 +5969,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,AC-2 (4),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AC-2 (4),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -6051,7 +6051,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,AC-2 (4),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AC-2 (4),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -7171,7 +7171,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7245,7 +7245,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7319,7 +7319,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7393,7 +7393,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7473,7 +7473,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7634,7 +7634,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
@@ -7969,7 +7969,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -8044,7 +8044,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8119,7 +8119,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8194,7 +8194,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8274,7 +8274,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8348,7 +8348,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8422,7 +8422,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8496,7 +8496,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8570,7 +8570,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8644,7 +8644,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8724,7 +8724,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8804,7 +8804,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -8884,7 +8884,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AC-11 (1),AC-11 b</t>
+          <t>AC-11 b,AC-11 (1)</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -9055,7 +9055,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),AC-11 b</t>
+          <t>AC-11 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9134,7 +9134,7 @@
     <row r="112" ht="130" customHeight="1">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
@@ -9213,7 +9213,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9297,7 +9297,7 @@
     <row r="114" ht="130" customHeight="1">
       <c r="A114" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B114" s="2" t="inlineStr">
@@ -9553,7 +9553,7 @@
     <row r="117" ht="130" customHeight="1">
       <c r="A117" s="2" t="inlineStr">
         <is>
-          <t>SC-8,MA-4 c,SC-13,AC-17 (2)</t>
+          <t>SC-13,SC-8,AC-17 (2),MA-4 c</t>
         </is>
       </c>
       <c r="B117" s="2" t="inlineStr">
@@ -9635,7 +9635,7 @@
     <row r="118" ht="130" customHeight="1">
       <c r="A118" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B118" s="2" t="inlineStr">
@@ -9713,7 +9713,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9791,7 +9791,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -9869,7 +9869,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -9949,7 +9949,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B122" s="2" t="inlineStr">
@@ -10018,7 +10018,7 @@
     <row r="123" ht="130" customHeight="1">
       <c r="A123" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B123" s="2" t="inlineStr">
@@ -10087,7 +10087,7 @@
     <row r="124" ht="130" customHeight="1">
       <c r="A124" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B124" s="2" t="inlineStr">
@@ -10156,7 +10156,7 @@
     <row r="125" ht="130" customHeight="1">
       <c r="A125" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B125" s="2" t="inlineStr">
@@ -10225,7 +10225,7 @@
     <row r="126" ht="130" customHeight="1">
       <c r="A126" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B126" s="2" t="inlineStr">
@@ -10305,7 +10305,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>SC-28,SC-28 (1)</t>
+          <t>SC-28 (1),SC-28</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -11605,7 +11605,7 @@
     <row r="143" ht="130" customHeight="1">
       <c r="A143" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B143" s="2" t="inlineStr">
@@ -11685,7 +11685,7 @@
     <row r="144" ht="130" customHeight="1">
       <c r="A144" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B144" s="2" t="inlineStr">
@@ -11765,7 +11765,7 @@
     <row r="145" ht="130" customHeight="1">
       <c r="A145" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B145" s="2" t="inlineStr">
@@ -11845,7 +11845,7 @@
     <row r="146" ht="130" customHeight="1">
       <c r="A146" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B146" s="2" t="inlineStr">
@@ -12157,7 +12157,7 @@
     <row r="150" ht="130" customHeight="1">
       <c r="A150" s="2" t="inlineStr">
         <is>
-          <t>IA-7,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),IA-7</t>
         </is>
       </c>
       <c r="B150" s="2" t="inlineStr">
@@ -12544,7 +12544,7 @@
     <row r="155" ht="130" customHeight="1">
       <c r="A155" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B155" s="2" t="inlineStr">
@@ -12620,7 +12620,7 @@
     <row r="156" ht="130" customHeight="1">
       <c r="A156" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B156" s="2" t="inlineStr">
@@ -12705,7 +12705,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B157" s="2" t="inlineStr">
@@ -12941,7 +12941,7 @@
     <row r="160" ht="130" customHeight="1">
       <c r="A160" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B160" s="2" t="inlineStr">
@@ -13018,7 +13018,7 @@
     <row r="161" ht="130" customHeight="1">
       <c r="A161" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B161" s="2" t="inlineStr">
@@ -13091,7 +13091,7 @@
     <row r="162" ht="130" customHeight="1">
       <c r="A162" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B162" s="2" t="inlineStr">
@@ -13164,7 +13164,7 @@
     <row r="163" ht="130" customHeight="1">
       <c r="A163" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B163" s="2" t="inlineStr">
@@ -13249,7 +13249,7 @@
     <row r="164" ht="130" customHeight="1">
       <c r="A164" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B164" s="2" t="inlineStr">
@@ -13324,7 +13324,7 @@
     <row r="165" ht="130" customHeight="1">
       <c r="A165" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B165" s="2" t="inlineStr">
@@ -13399,7 +13399,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B166" s="2" t="inlineStr">
@@ -13474,7 +13474,7 @@
     <row r="167" ht="130" customHeight="1">
       <c r="A167" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B167" s="2" t="inlineStr">
@@ -13549,7 +13549,7 @@
     <row r="168" ht="130" customHeight="1">
       <c r="A168" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B168" s="2" t="inlineStr">
@@ -13620,7 +13620,7 @@
     <row r="169" ht="130" customHeight="1">
       <c r="A169" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B169" s="2" t="inlineStr">
@@ -13691,7 +13691,7 @@
     <row r="170" ht="130" customHeight="1">
       <c r="A170" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B170" s="2" t="inlineStr">
@@ -13763,7 +13763,7 @@
     <row r="171" ht="130" customHeight="1">
       <c r="A171" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B171" s="2" t="inlineStr">
@@ -13834,7 +13834,7 @@
     <row r="172" ht="130" customHeight="1">
       <c r="A172" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B172" s="2" t="inlineStr">
@@ -13905,7 +13905,7 @@
     <row r="173" ht="130" customHeight="1">
       <c r="A173" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B173" s="2" t="inlineStr">
@@ -13977,7 +13977,7 @@
     <row r="174" ht="130" customHeight="1">
       <c r="A174" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B174" s="2" t="inlineStr">
@@ -14052,7 +14052,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B175" s="2" t="inlineStr">
@@ -14123,7 +14123,7 @@
     <row r="176" ht="130" customHeight="1">
       <c r="A176" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B176" s="2" t="inlineStr">
@@ -14194,7 +14194,7 @@
     <row r="177" ht="130" customHeight="1">
       <c r="A177" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B177" s="2" t="inlineStr">
@@ -14266,7 +14266,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B178" s="2" t="inlineStr">
@@ -14341,7 +14341,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B179" s="2" t="inlineStr">
@@ -14423,7 +14423,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B180" s="2" t="inlineStr">
@@ -14505,7 +14505,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">
@@ -14587,7 +14587,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3</t>
+          <t>AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B182" s="2" t="inlineStr">
@@ -14669,7 +14669,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B183" s="2" t="inlineStr">
@@ -14751,7 +14751,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B184" s="2" t="inlineStr">
@@ -14833,7 +14833,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B185" s="2" t="inlineStr">
@@ -14915,7 +14915,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B186" s="2" t="inlineStr">
@@ -14997,7 +14997,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B187" s="2" t="inlineStr">
@@ -15079,7 +15079,7 @@
     <row r="188" ht="130" customHeight="1">
       <c r="A188" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B188" s="2" t="inlineStr">
@@ -15157,7 +15157,7 @@
     <row r="189" ht="130" customHeight="1">
       <c r="A189" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B189" s="2" t="inlineStr">
@@ -15236,7 +15236,7 @@
     <row r="190" ht="130" customHeight="1">
       <c r="A190" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B190" s="2" t="inlineStr">
@@ -15318,7 +15318,7 @@
     <row r="191" ht="130" customHeight="1">
       <c r="A191" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B191" s="2" t="inlineStr">
@@ -15400,7 +15400,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-12 c,AU-3</t>
+          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B192" s="2" t="inlineStr">
@@ -15482,7 +15482,7 @@
     <row r="193" ht="130" customHeight="1">
       <c r="A193" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B193" s="2" t="inlineStr">
@@ -15564,7 +15564,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B194" s="2" t="inlineStr">
@@ -15646,7 +15646,7 @@
     <row r="195" ht="130" customHeight="1">
       <c r="A195" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B195" s="2" t="inlineStr">
@@ -15728,7 +15728,7 @@
     <row r="196" ht="130" customHeight="1">
       <c r="A196" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B196" s="2" t="inlineStr">
@@ -15803,7 +15803,7 @@
     <row r="197" ht="130" customHeight="1">
       <c r="A197" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 a,AC-2 (4),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AU-12 a,AC-2 (4),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B197" s="2" t="inlineStr">
@@ -15876,7 +15876,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AC-2 (4),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-3,AC-2 (4),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B198" s="2" t="inlineStr">
@@ -15953,7 +15953,7 @@
     <row r="199" ht="130" customHeight="1">
       <c r="A199" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (3),IA-2 (4),IA-2 (1)</t>
+          <t>IA-2 (4),IA-2 (3),IA-2 (1),IA-2 (2)</t>
         </is>
       </c>
       <c r="B199" s="2" t="inlineStr">
@@ -16040,7 +16040,7 @@
     <row r="200" ht="130" customHeight="1">
       <c r="A200" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2,IA-2 (4),IA-2 (5),IA-2 (3)</t>
+          <t>IA-2 (4),IA-2,IA-2 (3),IA-2 (2),IA-2 (5)</t>
         </is>
       </c>
       <c r="B200" s="2" t="inlineStr">
@@ -16129,7 +16129,7 @@
     <row r="201" ht="130" customHeight="1">
       <c r="A201" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2,IA-2 (4),IA-2 (5),IA-2 (3)</t>
+          <t>IA-2 (4),IA-2,IA-2 (3),IA-2 (2),IA-2 (5)</t>
         </is>
       </c>
       <c r="B201" s="2" t="inlineStr">
@@ -16373,7 +16373,7 @@
     <row r="204" ht="130" customHeight="1">
       <c r="A204" s="2" t="inlineStr">
         <is>
-          <t>AC-3 (4),IA-11</t>
+          <t>IA-11,AC-3 (4)</t>
         </is>
       </c>
       <c r="B204" s="2" t="inlineStr">
@@ -16978,7 +16978,7 @@
     <row r="212" ht="130" customHeight="1">
       <c r="A212" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),SC-8,SC-8 (1)</t>
+          <t>SC-8,SC-8 (1),AC-18 (1)</t>
         </is>
       </c>
       <c r="B212" s="2" t="inlineStr">
@@ -17138,7 +17138,7 @@
     <row r="214" ht="130" customHeight="1">
       <c r="A214" s="2" t="inlineStr">
         <is>
-          <t>SC-10,AC-11 a</t>
+          <t>AC-11 a,SC-10</t>
         </is>
       </c>
       <c r="B214" s="2" t="inlineStr">
@@ -17746,7 +17746,7 @@
     <row r="222" ht="130" customHeight="1">
       <c r="A222" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b,IA-5 (1) (c)</t>
+          <t>CM-6 b,IA-5 (1) (c),CM-7 a</t>
         </is>
       </c>
       <c r="B222" s="2" t="inlineStr">
@@ -17906,7 +17906,7 @@
     <row r="224" ht="130" customHeight="1">
       <c r="A224" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,CM-6 b</t>
+          <t>CM-6 b,AU-12 a</t>
         </is>
       </c>
       <c r="B224" s="2" t="inlineStr">
@@ -17992,7 +17992,7 @@
     <row r="225" ht="130" customHeight="1">
       <c r="A225" s="2" t="inlineStr">
         <is>
-          <t>SC-5 (2),CM-6 b,SC-5</t>
+          <t>CM-6 b,SC-5,SC-5 (2)</t>
         </is>
       </c>
       <c r="B225" s="2" t="inlineStr">
@@ -18172,7 +18172,7 @@
     <row r="227" ht="130" customHeight="1">
       <c r="A227" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,SI-16</t>
+          <t>SI-16,CM-7 a</t>
         </is>
       </c>
       <c r="B227" s="2" t="inlineStr">
@@ -18264,7 +18264,7 @@
     <row r="228" ht="130" customHeight="1">
       <c r="A228" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-16</t>
+          <t>SI-16,CM-6 b</t>
         </is>
       </c>
       <c r="B228" s="2" t="inlineStr">
@@ -18362,7 +18362,7 @@
     <row r="229" ht="130" customHeight="1">
       <c r="A229" s="2" t="inlineStr">
         <is>
-          <t>IA-2,IA-8,AU-3 (1)</t>
+          <t>AU-3 (1),IA-8,IA-2</t>
         </is>
       </c>
       <c r="B229" s="2" t="inlineStr">
@@ -19336,7 +19336,7 @@
     <row r="241" ht="130" customHeight="1">
       <c r="A241" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-16,SC-2</t>
+          <t>SI-16,SC-2,CM-6 b</t>
         </is>
       </c>
       <c r="B241" s="2" t="inlineStr">
@@ -19496,7 +19496,7 @@
     <row r="243" ht="130" customHeight="1">
       <c r="A243" s="2" t="inlineStr">
         <is>
-          <t>SC-3,SI-16</t>
+          <t>SI-16,SC-3</t>
         </is>
       </c>
       <c r="B243" s="2" t="inlineStr">
@@ -20194,7 +20194,7 @@
     <row r="252" ht="130" customHeight="1">
       <c r="A252" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (b),CM-6 b,IA-5 (1) (a)</t>
+          <t>CM-6 b,IA-5 (1) (a),IA-5 (1) (b)</t>
         </is>
       </c>
       <c r="B252" s="2" t="inlineStr">
@@ -20762,7 +20762,7 @@
     <row r="259" ht="130" customHeight="1">
       <c r="A259" s="2" t="inlineStr">
         <is>
-          <t>SC-4,CM-6 b</t>
+          <t>CM-6 b,SC-4</t>
         </is>
       </c>
       <c r="B259" s="2" t="inlineStr">
@@ -20843,7 +20843,7 @@
     <row r="260" ht="130" customHeight="1">
       <c r="A260" s="2" t="inlineStr">
         <is>
-          <t>SC-4,SC-2</t>
+          <t>SC-2,SC-4</t>
         </is>
       </c>
       <c r="B260" s="2" t="inlineStr">
@@ -20931,7 +20931,7 @@
     <row r="261" ht="130" customHeight="1">
       <c r="A261" s="2" t="inlineStr">
         <is>
-          <t>SC-4,SC-2</t>
+          <t>SC-2,SC-4</t>
         </is>
       </c>
       <c r="B261" s="2" t="inlineStr">
@@ -21107,7 +21107,7 @@
     <row r="263" ht="130" customHeight="1">
       <c r="A263" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B263" s="2" t="inlineStr">
@@ -21514,7 +21514,7 @@
     <row r="268" ht="130" customHeight="1">
       <c r="A268" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-7 a,AU-7 b,AC-6 (8),AC-6 (9),CM-5 (1),AU-12 (3)</t>
+          <t>AU-8 b,CM-5 (1),AC-6 (8),AC-6 (9),AU-12 (3),AU-7 a,AU-7 b</t>
         </is>
       </c>
       <c r="B268" s="2" t="inlineStr">
@@ -22108,7 +22108,7 @@
     <row r="276" ht="130" customHeight="1">
       <c r="A276" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-12 c</t>
+          <t>AU-12 c,AU-9</t>
         </is>
       </c>
       <c r="B276" s="2" t="inlineStr">
@@ -22181,7 +22181,7 @@
     <row r="277" ht="130" customHeight="1">
       <c r="A277" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (3),CM-6 b</t>
+          <t>CM-6 b,CM-5 (3)</t>
         </is>
       </c>
       <c r="B277" s="2" t="inlineStr">
@@ -22860,7 +22860,7 @@
     <row r="285" ht="130" customHeight="1">
       <c r="A285" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B285" s="2" t="inlineStr">
@@ -23844,7 +23844,7 @@
     <row r="298" ht="130" customHeight="1">
       <c r="A298" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B298" s="2" t="inlineStr">
@@ -23915,7 +23915,7 @@
     <row r="299" ht="130" customHeight="1">
       <c r="A299" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B299" s="2" t="inlineStr">
@@ -23987,7 +23987,7 @@
     <row r="300" ht="130" customHeight="1">
       <c r="A300" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B300" s="2" t="inlineStr">
@@ -24145,7 +24145,7 @@
     <row r="302" ht="130" customHeight="1">
       <c r="A302" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (9),AU-12 c,AC-2 (4)</t>
+          <t>AU-12 c,AC-6 (9),AC-2 (4)</t>
         </is>
       </c>
       <c r="B302" s="2" t="inlineStr">
@@ -27874,7 +27874,7 @@
     <row r="351" ht="130" customHeight="1">
       <c r="A351" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),CM-6 b</t>
+          <t>CM-6 b,IA-2 (2)</t>
         </is>
       </c>
       <c r="B351" s="2" t="inlineStr">
@@ -30335,7 +30335,7 @@
     <row r="384" ht="130" customHeight="1">
       <c r="A384" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-3</t>
+          <t>AU-3,CM-6 b</t>
         </is>
       </c>
       <c r="B384" s="2" t="inlineStr">
@@ -30973,7 +30973,7 @@
     <row r="392" ht="130" customHeight="1">
       <c r="A392" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),AC-17 (9),CM-6 b,CM-7 b</t>
+          <t>CM-6 b,AC-17 (1),AC-17 (9),CM-7 b</t>
         </is>
       </c>
       <c r="B392" s="2" t="inlineStr">
@@ -31051,7 +31051,7 @@
     <row r="393" ht="130" customHeight="1">
       <c r="A393" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),CM-6 b,CM-7 b</t>
+          <t>CM-6 b,AC-17 (1),CM-7 b</t>
         </is>
       </c>
       <c r="B393" s="2" t="inlineStr">
@@ -33550,7 +33550,7 @@
     <row r="422" ht="130" customHeight="1">
       <c r="A422" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B422" s="2" t="inlineStr">
@@ -33625,7 +33625,7 @@
     <row r="423" ht="130" customHeight="1">
       <c r="A423" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B423" s="2" t="inlineStr">
@@ -35367,7 +35367,7 @@
     <row r="445" ht="130" customHeight="1">
       <c r="A445" s="2" t="inlineStr">
         <is>
-          <t>AU-4,CM-6 b</t>
+          <t>CM-6 b,AU-4</t>
         </is>
       </c>
       <c r="B445" s="2" t="inlineStr">
@@ -35667,7 +35667,7 @@
     <row r="449" ht="130" customHeight="1">
       <c r="A449" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B449" s="2" t="inlineStr">
@@ -35744,7 +35744,7 @@
     <row r="450" ht="130" customHeight="1">
       <c r="A450" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B450" s="2" t="inlineStr">
@@ -37064,7 +37064,7 @@
     <row r="468" ht="130" customHeight="1">
       <c r="A468" s="2" t="inlineStr">
         <is>
-          <t>SC-10,MA-4 e,MA-4 (7),AC-12</t>
+          <t>MA-4 (7),AC-12,MA-4 e,SC-10</t>
         </is>
       </c>
       <c r="B468" s="2" t="inlineStr">
@@ -37139,7 +37139,7 @@
     <row r="469" ht="130" customHeight="1">
       <c r="A469" s="2" t="inlineStr">
         <is>
-          <t>SC-10,AC-12</t>
+          <t>AC-12,SC-10</t>
         </is>
       </c>
       <c r="B469" s="2" t="inlineStr">
@@ -37218,7 +37218,7 @@
     <row r="470" ht="130" customHeight="1">
       <c r="A470" s="2" t="inlineStr">
         <is>
-          <t>SC-10,AC-12</t>
+          <t>AC-12,SC-10</t>
         </is>
       </c>
       <c r="B470" s="2" t="inlineStr">
@@ -41161,7 +41161,7 @@
     <row r="520" ht="130" customHeight="1">
       <c r="A520" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (2)</t>
+          <t>SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B520" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@9519ca6e7ee941d4205dc44fa0d6139f25cb712c 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -550,7 +550,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -634,7 +634,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -719,7 +719,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -791,7 +791,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -973,7 +973,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 b</t>
+          <t>AU-5 b,AU-5 a</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -1455,7 +1455,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),CM-6 b,CM-5 (1),AU-14 (1),AU-7 (1),MA-4 (1) (a),AU-3,AU-6 (4),AU-7 a</t>
+          <t>AU-12 a,AU-3,AU-6 (4),CM-5 (1),MA-4 (1) (a),AU-7 (1),AU-7 a,CM-6 b,AU-3 (1),AU-14 (1)</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -3258,7 +3258,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AU-14 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c,AU-14 (1)</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3349,7 +3349,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-14 (1)</t>
+          <t>AU-14 (1),AU-4</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3832,7 +3832,7 @@
     <row r="44" ht="130" customHeight="1">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-6 (4),CM-6 b</t>
+          <t>AU-6 (4),AU-4 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
@@ -3993,7 +3993,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-8 (1) (b),AU-8 (1) (a)</t>
+          <t>AU-8 b,AU-8 (1) (a),AU-8 (1) (b)</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -4234,7 +4234,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11),IA-2 (1)</t>
+          <t>IA-2 (1),IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4410,7 +4410,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>SI-6 d,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 d</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -4494,7 +4494,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -4569,7 +4569,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -4644,7 +4644,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -4719,7 +4719,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -4794,7 +4794,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -4869,7 +4869,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -4944,7 +4944,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -5019,7 +5019,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -5094,7 +5094,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -5169,7 +5169,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-7 b,AU-12 c,CM-6 b,AU-8 b,AU-12 (3),CM-5 (1),AU-7 a</t>
+          <t>AU-12 a,CM-5 (1),AU-7 b,AU-12 (3),AU-8 b,AU-7 a,CM-6 b,AU-12 c</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5243,7 +5243,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AC-2 (4),AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5324,7 +5324,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AC-2 (4),AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5405,7 +5405,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AC-2 (4),AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5487,7 +5487,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AC-2 (4),AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5569,7 +5569,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AC-2 (4),AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5651,7 +5651,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AC-2 (4),AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5733,7 +5733,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AC-2 (4),AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5815,7 +5815,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>SI-6 a,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 a</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5889,7 +5889,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5972,7 +5972,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -6050,7 +6050,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -6141,7 +6141,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6223,7 +6223,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6853,7 +6853,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -6927,7 +6927,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -7001,7 +7001,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -7075,7 +7075,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -7651,7 +7651,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -7726,7 +7726,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -7801,7 +7801,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -7876,7 +7876,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -7956,7 +7956,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -8038,7 +8038,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -8120,7 +8120,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8202,7 +8202,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8284,7 +8284,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8366,7 +8366,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -8446,7 +8446,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -8526,7 +8526,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -8777,7 +8777,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-6 (10)</t>
+          <t>AC-6 (10),AC-11 b</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8856,7 +8856,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8935,7 +8935,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -9022,7 +9022,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -9109,7 +9109,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -9354,7 +9354,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>SC-13,SC-8,AC-17 (2),MA-4 c</t>
+          <t>SC-8,AC-17 (2),MA-4 c,SC-13</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9436,7 +9436,7 @@
     <row r="114" ht="130" customHeight="1">
       <c r="A114" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B114" s="2" t="inlineStr">
@@ -9514,7 +9514,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9592,7 +9592,7 @@
     <row r="116" ht="130" customHeight="1">
       <c r="A116" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B116" s="2" t="inlineStr">
@@ -9670,7 +9670,7 @@
     <row r="117" ht="130" customHeight="1">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -9750,7 +9750,7 @@
     <row r="118" ht="130" customHeight="1">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
@@ -9819,7 +9819,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
@@ -9888,7 +9888,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
@@ -9957,7 +9957,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
@@ -10026,7 +10026,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -10873,7 +10873,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10954,7 +10954,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -11040,7 +11040,7 @@
     <row r="135" ht="130" customHeight="1">
       <c r="A135" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B135" s="2" t="inlineStr">
@@ -11406,7 +11406,7 @@
     <row r="139" ht="130" customHeight="1">
       <c r="A139" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B139" s="3" t="inlineStr">
@@ -11486,7 +11486,7 @@
     <row r="140" ht="130" customHeight="1">
       <c r="A140" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B140" s="3" t="inlineStr">
@@ -11566,7 +11566,7 @@
     <row r="141" ht="130" customHeight="1">
       <c r="A141" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B141" s="3" t="inlineStr">
@@ -11646,7 +11646,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B142" s="3" t="inlineStr">
@@ -11958,7 +11958,7 @@
     <row r="146" ht="130" customHeight="1">
       <c r="A146" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),IA-7</t>
+          <t>IA-7,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B146" s="2" t="inlineStr">
@@ -12747,7 +12747,7 @@
     <row r="156" ht="130" customHeight="1">
       <c r="A156" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-7 a</t>
+          <t>CM-7 a,IA-7</t>
         </is>
       </c>
       <c r="B156" s="2" t="inlineStr">
@@ -12826,7 +12826,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B157" s="3" t="inlineStr">
@@ -12903,7 +12903,7 @@
     <row r="158" ht="130" customHeight="1">
       <c r="A158" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B158" s="3" t="inlineStr">
@@ -12976,7 +12976,7 @@
     <row r="159" ht="130" customHeight="1">
       <c r="A159" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 a,AU-12 c</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B159" s="3" t="inlineStr">
@@ -13049,7 +13049,7 @@
     <row r="160" ht="130" customHeight="1">
       <c r="A160" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B160" s="3" t="inlineStr">
@@ -13134,7 +13134,7 @@
     <row r="161" ht="130" customHeight="1">
       <c r="A161" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B161" s="3" t="inlineStr">
@@ -13209,7 +13209,7 @@
     <row r="162" ht="130" customHeight="1">
       <c r="A162" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B162" s="3" t="inlineStr">
@@ -13284,7 +13284,7 @@
     <row r="163" ht="130" customHeight="1">
       <c r="A163" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B163" s="3" t="inlineStr">
@@ -13359,7 +13359,7 @@
     <row r="164" ht="130" customHeight="1">
       <c r="A164" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B164" s="3" t="inlineStr">
@@ -13434,7 +13434,7 @@
     <row r="165" ht="130" customHeight="1">
       <c r="A165" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B165" s="3" t="inlineStr">
@@ -13505,7 +13505,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B166" s="3" t="inlineStr">
@@ -13576,7 +13576,7 @@
     <row r="167" ht="130" customHeight="1">
       <c r="A167" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B167" s="3" t="inlineStr">
@@ -13648,7 +13648,7 @@
     <row r="168" ht="130" customHeight="1">
       <c r="A168" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B168" s="3" t="inlineStr">
@@ -13719,7 +13719,7 @@
     <row r="169" ht="130" customHeight="1">
       <c r="A169" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B169" s="3" t="inlineStr">
@@ -13790,7 +13790,7 @@
     <row r="170" ht="130" customHeight="1">
       <c r="A170" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B170" s="3" t="inlineStr">
@@ -13862,7 +13862,7 @@
     <row r="171" ht="130" customHeight="1">
       <c r="A171" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B171" s="3" t="inlineStr">
@@ -13937,7 +13937,7 @@
     <row r="172" ht="130" customHeight="1">
       <c r="A172" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B172" s="3" t="inlineStr">
@@ -14008,7 +14008,7 @@
     <row r="173" ht="130" customHeight="1">
       <c r="A173" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B173" s="3" t="inlineStr">
@@ -14079,7 +14079,7 @@
     <row r="174" ht="130" customHeight="1">
       <c r="A174" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B174" s="3" t="inlineStr">
@@ -14151,7 +14151,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B175" s="3" t="inlineStr">
@@ -14226,7 +14226,7 @@
     <row r="176" ht="130" customHeight="1">
       <c r="A176" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B176" s="3" t="inlineStr">
@@ -14308,7 +14308,7 @@
     <row r="177" ht="130" customHeight="1">
       <c r="A177" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B177" s="3" t="inlineStr">
@@ -14390,7 +14390,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B178" s="3" t="inlineStr">
@@ -14472,7 +14472,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B179" s="3" t="inlineStr">
@@ -14554,7 +14554,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B180" s="3" t="inlineStr">
@@ -14636,7 +14636,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B181" s="3" t="inlineStr">
@@ -14718,7 +14718,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B182" s="3" t="inlineStr">
@@ -14800,7 +14800,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B183" s="3" t="inlineStr">
@@ -14882,7 +14882,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B184" s="3" t="inlineStr">
@@ -14964,7 +14964,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B185" s="3" t="inlineStr">
@@ -15042,7 +15042,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B186" s="3" t="inlineStr">
@@ -15121,7 +15121,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B187" s="3" t="inlineStr">
@@ -15203,7 +15203,7 @@
     <row r="188" ht="130" customHeight="1">
       <c r="A188" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B188" s="3" t="inlineStr">
@@ -15285,7 +15285,7 @@
     <row r="189" ht="130" customHeight="1">
       <c r="A189" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B189" s="3" t="inlineStr">
@@ -15367,7 +15367,7 @@
     <row r="190" ht="130" customHeight="1">
       <c r="A190" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B190" s="3" t="inlineStr">
@@ -15449,7 +15449,7 @@
     <row r="191" ht="130" customHeight="1">
       <c r="A191" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B191" s="3" t="inlineStr">
@@ -15531,7 +15531,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B192" s="3" t="inlineStr">
@@ -15613,7 +15613,7 @@
     <row r="193" ht="130" customHeight="1">
       <c r="A193" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B193" s="3" t="inlineStr">
@@ -15688,7 +15688,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-3</t>
+          <t>AU-12 a,AC-2 (4),AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B194" s="3" t="inlineStr">
@@ -15761,7 +15761,7 @@
     <row r="195" ht="130" customHeight="1">
       <c r="A195" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,AC-2 (4),MA-4 (1) (a),AU-3</t>
+          <t>AC-2 (4),AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B195" s="3" t="inlineStr">
@@ -15838,7 +15838,7 @@
     <row r="196" ht="130" customHeight="1">
       <c r="A196" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2 (3),IA-2 (1),IA-2 (2)</t>
+          <t>IA-2 (1),IA-2 (2),IA-2 (4),IA-2 (3)</t>
         </is>
       </c>
       <c r="B196" s="2" t="inlineStr">
@@ -15925,7 +15925,7 @@
     <row r="197" ht="130" customHeight="1">
       <c r="A197" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),IA-2 (2),IA-2 (4),IA-2,IA-2 (3)</t>
+          <t>IA-2 (5),IA-2 (4),IA-2 (2),IA-2,IA-2 (3)</t>
         </is>
       </c>
       <c r="B197" s="2" t="inlineStr">
@@ -16014,7 +16014,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),IA-2 (2),IA-2 (4),IA-2,IA-2 (3)</t>
+          <t>IA-2 (5),IA-2 (4),IA-2 (2),IA-2,IA-2 (3)</t>
         </is>
       </c>
       <c r="B198" s="2" t="inlineStr">
@@ -16638,7 +16638,7 @@
     <row r="206" ht="130" customHeight="1">
       <c r="A206" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (2),SC-8 (1)</t>
+          <t>SC-8,SC-8 (1),SC-8 (2)</t>
         </is>
       </c>
       <c r="B206" s="2" t="inlineStr">
@@ -16715,7 +16715,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (2),SC-8 (1)</t>
+          <t>SC-8,SC-8 (1),SC-8 (2)</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -16801,7 +16801,7 @@
     <row r="208" ht="130" customHeight="1">
       <c r="A208" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-18 (1),SC-8 (1)</t>
+          <t>SC-8,SC-8 (1),AC-18 (1)</t>
         </is>
       </c>
       <c r="B208" s="2" t="inlineStr">
@@ -17229,7 +17229,7 @@
     <row r="213" ht="130" customHeight="1">
       <c r="A213" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-7 a,CM-6 b</t>
+          <t>CM-7 a,CM-6 b,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B213" s="2" t="inlineStr">
@@ -17475,7 +17475,7 @@
     <row r="216" ht="130" customHeight="1">
       <c r="A216" s="2" t="inlineStr">
         <is>
-          <t>SC-5 (2),SC-5,CM-6 b</t>
+          <t>SC-5,SC-5 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B216" s="2" t="inlineStr">
@@ -18824,7 +18824,7 @@
     <row r="232" ht="130" customHeight="1">
       <c r="A232" s="2" t="inlineStr">
         <is>
-          <t>SI-16,SC-2,CM-6 b</t>
+          <t>SI-16,CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B232" s="2" t="inlineStr">
@@ -19008,7 +19008,7 @@
     <row r="234" ht="130" customHeight="1">
       <c r="A234" s="2" t="inlineStr">
         <is>
-          <t>SI-16,SC-3</t>
+          <t>SC-3,SI-16</t>
         </is>
       </c>
       <c r="B234" s="2" t="inlineStr">
@@ -19732,7 +19732,7 @@
     <row r="243" ht="130" customHeight="1">
       <c r="A243" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (b),IA-5 (1) (a),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (a),IA-5 (1) (b)</t>
         </is>
       </c>
       <c r="B243" s="2" t="inlineStr">
@@ -20556,7 +20556,7 @@
     <row r="253" ht="130" customHeight="1">
       <c r="A253" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (1)</t>
+          <t>IA-2 (1),IA-2 (11)</t>
         </is>
       </c>
       <c r="B253" s="2" t="inlineStr">
@@ -21052,7 +21052,7 @@
     <row r="259" ht="130" customHeight="1">
       <c r="A259" s="3" t="inlineStr">
         <is>
-          <t>AC-6 (9),AC-6 (8)</t>
+          <t>AC-6 (8),AC-6 (9)</t>
         </is>
       </c>
       <c r="B259" s="3" t="inlineStr">
@@ -21646,7 +21646,7 @@
     <row r="267" ht="130" customHeight="1">
       <c r="A267" s="3" t="inlineStr">
         <is>
-          <t>AU-9,AU-12 c</t>
+          <t>AU-12 c,AU-9</t>
         </is>
       </c>
       <c r="B267" s="3" t="inlineStr">
@@ -22552,7 +22552,7 @@
     <row r="278" ht="130" customHeight="1">
       <c r="A278" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-7 a</t>
+          <t>CM-7 a,CM-7 b</t>
         </is>
       </c>
       <c r="B278" s="2" t="inlineStr">
@@ -22632,7 +22632,7 @@
     <row r="279" ht="130" customHeight="1">
       <c r="A279" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-7 a</t>
+          <t>CM-7 a,CM-7 b</t>
         </is>
       </c>
       <c r="B279" s="2" t="inlineStr">
@@ -23701,7 +23701,7 @@
     <row r="293" ht="130" customHeight="1">
       <c r="A293" s="3" t="inlineStr">
         <is>
-          <t>AC-6 (9),AC-2 (4),AU-12 c</t>
+          <t>AU-12 c,AC-2 (4),AC-6 (9)</t>
         </is>
       </c>
       <c r="B293" s="3" t="inlineStr">
@@ -27280,7 +27280,7 @@
     <row r="340" ht="130" customHeight="1">
       <c r="A340" s="3" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B340" s="3" t="inlineStr">
@@ -27430,7 +27430,7 @@
     <row r="342" ht="130" customHeight="1">
       <c r="A342" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (2)</t>
+          <t>IA-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B342" s="2" t="inlineStr">
@@ -28227,7 +28227,7 @@
 following command:
  $ sudo grep RekeyLimit /etc/ssh/sshd_config /etc/ssh/sshd_config.d/* 
 If configured properly, output should be
- RekeyLimit 512M 512M 
+ RekeyLimit 512M 1h 
 If it is commented out or is not set, then this is a finding.</t>
         </is>
       </c>
@@ -29899,7 +29899,7 @@
     <row r="375" ht="130" customHeight="1">
       <c r="A375" s="3" t="inlineStr">
         <is>
-          <t>AU-3,CM-6 b</t>
+          <t>CM-6 b,AU-3</t>
         </is>
       </c>
       <c r="B375" s="3" t="inlineStr">
@@ -30537,7 +30537,7 @@
     <row r="383" ht="130" customHeight="1">
       <c r="A383" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (1),CM-6 b,AC-17 (9)</t>
+          <t>AC-17 (1),AC-17 (9),CM-7 b,CM-6 b</t>
         </is>
       </c>
       <c r="B383" s="2" t="inlineStr">
@@ -30615,7 +30615,7 @@
     <row r="384" ht="130" customHeight="1">
       <c r="A384" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (1),CM-6 b</t>
+          <t>AC-17 (1),CM-7 b,CM-6 b</t>
         </is>
       </c>
       <c r="B384" s="2" t="inlineStr">
@@ -34070,7 +34070,7 @@
     <row r="425" ht="130" customHeight="1">
       <c r="A425" s="3" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b</t>
+          <t>CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B425" s="3" t="inlineStr">
@@ -34157,7 +34157,7 @@
     <row r="426" ht="130" customHeight="1">
       <c r="A426" s="3" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b</t>
+          <t>CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B426" s="3" t="inlineStr">
@@ -35733,7 +35733,7 @@
     <row r="446" ht="130" customHeight="1">
       <c r="A446" s="3" t="inlineStr">
         <is>
-          <t>SI-2 (2),CM-6 b</t>
+          <t>CM-6 b,SI-2 (2)</t>
         </is>
       </c>
       <c r="B446" s="3" t="inlineStr">
@@ -36380,7 +36380,7 @@
     <row r="455" ht="130" customHeight="1">
       <c r="A455" s="3" t="inlineStr">
         <is>
-          <t>SI-2 (2),CM-6 b</t>
+          <t>CM-6 b,SI-2 (2)</t>
         </is>
       </c>
       <c r="B455" s="3" t="inlineStr">
@@ -36671,7 +36671,7 @@
     <row r="459" ht="130" customHeight="1">
       <c r="A459" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (7),MA-4 e,AC-12,SC-10</t>
+          <t>SC-10,AC-12,MA-4 e,MA-4 (7)</t>
         </is>
       </c>
       <c r="B459" s="3" t="inlineStr">
@@ -36901,7 +36901,7 @@
     <row r="462" ht="130" customHeight="1">
       <c r="A462" s="3" t="inlineStr">
         <is>
-          <t>AC-11 a,SC-10</t>
+          <t>SC-10,AC-11 a</t>
         </is>
       </c>
       <c r="B462" s="3" t="inlineStr">
@@ -36978,7 +36978,7 @@
     <row r="463" ht="130" customHeight="1">
       <c r="A463" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2),SC-8 (1)</t>
+          <t>SC-8,SC-8 (1),AC-17 (2)</t>
         </is>
       </c>
       <c r="B463" s="2" t="inlineStr">
@@ -37036,7 +37036,7 @@
 sudo grep RekeyLimit /etc/ssh/ssh_config.d/*.conf  If configured
 properly, output should be  /etc/ssh/ssh_config.d/02-rekey-limit.conf:
 RekeyLimit 512M
-512M  Check also the
+1h  Check also the
 main configuration file with the following command:  $ sudo grep
 RekeyLimit /etc/ssh/ssh_config  The command should not return any
 output.
@@ -37047,7 +37047,7 @@
       <c r="M463" s="2" t="inlineStr">
         <is>
           <t>Configure Red Hat Enterprise Linux 9 to force a frequent session key renegotiation for SSH connections to the server by adding or modifying the following line in the "/etc/ssh/sshd_config" file:
-RekeyLimit 512M 512M
+RekeyLimit 512M 1h
 Restart the SSH daemon for the settings to take effect.
 $ sudo systemctl restart sshd.service</t>
         </is>
@@ -38280,7 +38280,7 @@
     <row r="480" ht="130" customHeight="1">
       <c r="A480" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,IA-3</t>
+          <t>IA-3,CM-7 b</t>
         </is>
       </c>
       <c r="B480" s="2" t="inlineStr">
@@ -38599,7 +38599,7 @@
     <row r="484" ht="130" customHeight="1">
       <c r="A484" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (1)</t>
+          <t>AC-17 (1),CM-7 b</t>
         </is>
       </c>
       <c r="B484" s="2" t="inlineStr">
@@ -38823,9 +38823,9 @@
           <t>Check that the operating system prohibits the reuse of a password for
 a minimum of "5" generations with the following command:
  # grep pam_pwhistory.so /etc/pam.d/password-auth
-password 5 pam_pwhistory.so remember=5 use_authtok 
+password requisite pam_pwhistory.so remember=5 use_authtok 
 If the command does not return a result, or the returned line is commented
-out, has a second column value different from "5", does not contain
+out, has a second column value different from "requisite", does not contain
 "remember" value, or the value is less than
 "5", this is a finding.
 If the value of remember is not set equal to or greater than 5, then this is a finding.</t>
@@ -38898,9 +38898,9 @@
           <t>Check that the operating system prohibits the reuse of a password for
 a minimum of "5" generations with the following command:
  # grep pam_pwhistory.so /etc/pam.d/system-auth
-password 5 pam_pwhistory.so remember=5 use_authtok 
+password requisite pam_pwhistory.so remember=5 use_authtok 
 If the command does not return a result, or the returned line is commented
-out, has a second column value different from "5", does not contain
+out, has a second column value different from "requisite", does not contain
 "remember" value, or the value is less than
 "5", this is a finding.
 If the value of remember is not set equal to or greater than 5, then this is a finding.</t>
@@ -39973,7 +39973,7 @@
     <row r="501" ht="130" customHeight="1">
       <c r="A501" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B501" s="2" t="inlineStr">
@@ -40075,7 +40075,7 @@
     <row r="502" ht="130" customHeight="1">
       <c r="A502" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B502" s="2" t="inlineStr">
@@ -40185,7 +40185,7 @@
     <row r="503" ht="130" customHeight="1">
       <c r="A503" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B503" s="2" t="inlineStr">
@@ -40296,7 +40296,7 @@
     <row r="504" ht="130" customHeight="1">
       <c r="A504" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B504" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@5cfde35fad5b8d5913c9e8f5ea541d68e0c91845 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -973,7 +973,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>AU-5 b,AU-5 a</t>
+          <t>AU-5 a,AU-5 b</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -1455,7 +1455,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AU-6 (4),CM-5 (1),MA-4 (1) (a),AU-7 (1),AU-7 a,CM-6 b,AU-3 (1),AU-14 (1)</t>
+          <t>CM-5 (1),AU-3 (1),AU-14 (1),AU-12 a,AU-7 a,AU-6 (4),AU-7 (1),AU-3,CM-6 b,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -1770,7 +1770,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -2140,7 +2140,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -2214,7 +2214,7 @@
     <row r="23" ht="130" customHeight="1">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -3258,7 +3258,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c,AU-14 (1)</t>
+          <t>AU-12 a,AU-3 (1),AU-14 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3832,7 +3832,7 @@
     <row r="44" ht="130" customHeight="1">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>AU-6 (4),AU-4 (1),CM-6 b</t>
+          <t>AU-4 (1),AU-6 (4),CM-6 b</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
@@ -3993,7 +3993,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-8 (1) (a),AU-8 (1) (b)</t>
+          <t>AU-8 (1) (b),AU-8 (1) (a),AU-8 b</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -4148,7 +4148,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4234,7 +4234,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (1),IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4318,7 +4318,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>SI-6 d,CM-3 (5),SI-6 b</t>
+          <t>CM-3 (5),SI-6 d,SI-6 b</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4494,7 +4494,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -4569,7 +4569,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -4644,7 +4644,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -4719,7 +4719,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -4794,7 +4794,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -4869,7 +4869,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -4944,7 +4944,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -5019,7 +5019,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -5094,7 +5094,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -5169,7 +5169,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,CM-5 (1),AU-7 b,AU-12 (3),AU-8 b,AU-7 a,CM-6 b,AU-12 c</t>
+          <t>CM-5 (1),AU-12 a,AU-7 a,AU-12 (3),AU-7 b,AU-8 b,CM-6 b,AU-12 c</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5243,7 +5243,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AC-2 (4),AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AC-2 (4),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5324,7 +5324,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AC-2 (4),AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AC-2 (4),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5405,7 +5405,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AC-2 (4),AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AC-2 (4),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5487,7 +5487,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AC-2 (4),AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AC-2 (4),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5569,7 +5569,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AC-2 (4),AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AC-2 (4),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5651,7 +5651,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AC-2 (4),AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AC-2 (4),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5733,7 +5733,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AC-2 (4),AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AC-2 (4),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5889,7 +5889,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5972,7 +5972,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -6050,7 +6050,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -6141,7 +6141,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6223,7 +6223,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6853,7 +6853,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -6927,7 +6927,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -7001,7 +7001,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -7075,7 +7075,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -7240,7 +7240,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>AC-17 (2),MA-4 (6)</t>
+          <t>MA-4 (6),AC-17 (2)</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -7499,7 +7499,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>AU-9 (3),AU-9</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -7575,7 +7575,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>AU-9 (3),AU-9</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -7651,7 +7651,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -7726,7 +7726,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -7801,7 +7801,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -7876,7 +7876,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -7956,7 +7956,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -8038,7 +8038,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -8120,7 +8120,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8202,7 +8202,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8284,7 +8284,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8366,7 +8366,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -8446,7 +8446,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -8526,7 +8526,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -9354,7 +9354,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2),MA-4 c,SC-13</t>
+          <t>SC-13,MA-4 c,SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9436,7 +9436,7 @@
     <row r="114" ht="130" customHeight="1">
       <c r="A114" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B114" s="2" t="inlineStr">
@@ -9514,7 +9514,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9592,7 +9592,7 @@
     <row r="116" ht="130" customHeight="1">
       <c r="A116" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B116" s="2" t="inlineStr">
@@ -9670,7 +9670,7 @@
     <row r="117" ht="130" customHeight="1">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -9750,7 +9750,7 @@
     <row r="118" ht="130" customHeight="1">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
@@ -9819,7 +9819,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
@@ -9888,7 +9888,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
@@ -9957,7 +9957,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
@@ -10026,7 +10026,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -10106,7 +10106,7 @@
     <row r="123" ht="130" customHeight="1">
       <c r="A123" s="2" t="inlineStr">
         <is>
-          <t>SC-28,SC-28 (1)</t>
+          <t>SC-28 (1),SC-28</t>
         </is>
       </c>
       <c r="B123" s="2" t="inlineStr">
@@ -11133,7 +11133,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>AC-3 (4),AC-6 (10)</t>
+          <t>AC-6 (10),AC-3 (4)</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -11230,7 +11230,7 @@
     <row r="137" ht="130" customHeight="1">
       <c r="A137" s="2" t="inlineStr">
         <is>
-          <t>AC-3 (4),AC-6 (10)</t>
+          <t>AC-6 (10),AC-3 (4)</t>
         </is>
       </c>
       <c r="B137" s="2" t="inlineStr">
@@ -11406,7 +11406,7 @@
     <row r="139" ht="130" customHeight="1">
       <c r="A139" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B139" s="3" t="inlineStr">
@@ -11486,7 +11486,7 @@
     <row r="140" ht="130" customHeight="1">
       <c r="A140" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B140" s="3" t="inlineStr">
@@ -11566,7 +11566,7 @@
     <row r="141" ht="130" customHeight="1">
       <c r="A141" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B141" s="3" t="inlineStr">
@@ -11646,7 +11646,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B142" s="3" t="inlineStr">
@@ -12429,7 +12429,7 @@
     <row r="152" ht="130" customHeight="1">
       <c r="A152" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B152" s="2" t="inlineStr">
@@ -12505,7 +12505,7 @@
     <row r="153" ht="130" customHeight="1">
       <c r="A153" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B153" s="2" t="inlineStr">
@@ -12590,7 +12590,7 @@
     <row r="154" ht="130" customHeight="1">
       <c r="A154" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B154" s="2" t="inlineStr">
@@ -12826,7 +12826,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B157" s="3" t="inlineStr">
@@ -12903,7 +12903,7 @@
     <row r="158" ht="130" customHeight="1">
       <c r="A158" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B158" s="3" t="inlineStr">
@@ -12976,7 +12976,7 @@
     <row r="159" ht="130" customHeight="1">
       <c r="A159" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B159" s="3" t="inlineStr">
@@ -13049,7 +13049,7 @@
     <row r="160" ht="130" customHeight="1">
       <c r="A160" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B160" s="3" t="inlineStr">
@@ -13134,7 +13134,7 @@
     <row r="161" ht="130" customHeight="1">
       <c r="A161" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B161" s="3" t="inlineStr">
@@ -13209,7 +13209,7 @@
     <row r="162" ht="130" customHeight="1">
       <c r="A162" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B162" s="3" t="inlineStr">
@@ -13284,7 +13284,7 @@
     <row r="163" ht="130" customHeight="1">
       <c r="A163" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B163" s="3" t="inlineStr">
@@ -13359,7 +13359,7 @@
     <row r="164" ht="130" customHeight="1">
       <c r="A164" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B164" s="3" t="inlineStr">
@@ -13434,7 +13434,7 @@
     <row r="165" ht="130" customHeight="1">
       <c r="A165" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B165" s="3" t="inlineStr">
@@ -13505,7 +13505,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B166" s="3" t="inlineStr">
@@ -13576,7 +13576,7 @@
     <row r="167" ht="130" customHeight="1">
       <c r="A167" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B167" s="3" t="inlineStr">
@@ -13648,7 +13648,7 @@
     <row r="168" ht="130" customHeight="1">
       <c r="A168" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B168" s="3" t="inlineStr">
@@ -13719,7 +13719,7 @@
     <row r="169" ht="130" customHeight="1">
       <c r="A169" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B169" s="3" t="inlineStr">
@@ -13790,7 +13790,7 @@
     <row r="170" ht="130" customHeight="1">
       <c r="A170" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B170" s="3" t="inlineStr">
@@ -13862,7 +13862,7 @@
     <row r="171" ht="130" customHeight="1">
       <c r="A171" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B171" s="3" t="inlineStr">
@@ -13937,7 +13937,7 @@
     <row r="172" ht="130" customHeight="1">
       <c r="A172" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B172" s="3" t="inlineStr">
@@ -14008,7 +14008,7 @@
     <row r="173" ht="130" customHeight="1">
       <c r="A173" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B173" s="3" t="inlineStr">
@@ -14079,7 +14079,7 @@
     <row r="174" ht="130" customHeight="1">
       <c r="A174" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B174" s="3" t="inlineStr">
@@ -14151,7 +14151,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B175" s="3" t="inlineStr">
@@ -14226,7 +14226,7 @@
     <row r="176" ht="130" customHeight="1">
       <c r="A176" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B176" s="3" t="inlineStr">
@@ -14308,7 +14308,7 @@
     <row r="177" ht="130" customHeight="1">
       <c r="A177" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B177" s="3" t="inlineStr">
@@ -14390,7 +14390,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B178" s="3" t="inlineStr">
@@ -14472,7 +14472,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B179" s="3" t="inlineStr">
@@ -14554,7 +14554,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B180" s="3" t="inlineStr">
@@ -14636,7 +14636,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B181" s="3" t="inlineStr">
@@ -14718,7 +14718,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B182" s="3" t="inlineStr">
@@ -14800,7 +14800,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B183" s="3" t="inlineStr">
@@ -14882,7 +14882,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B184" s="3" t="inlineStr">
@@ -14964,7 +14964,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B185" s="3" t="inlineStr">
@@ -15042,7 +15042,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B186" s="3" t="inlineStr">
@@ -15121,7 +15121,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B187" s="3" t="inlineStr">
@@ -15203,7 +15203,7 @@
     <row r="188" ht="130" customHeight="1">
       <c r="A188" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B188" s="3" t="inlineStr">
@@ -15285,7 +15285,7 @@
     <row r="189" ht="130" customHeight="1">
       <c r="A189" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B189" s="3" t="inlineStr">
@@ -15367,7 +15367,7 @@
     <row r="190" ht="130" customHeight="1">
       <c r="A190" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B190" s="3" t="inlineStr">
@@ -15449,7 +15449,7 @@
     <row r="191" ht="130" customHeight="1">
       <c r="A191" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B191" s="3" t="inlineStr">
@@ -15531,7 +15531,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B192" s="3" t="inlineStr">
@@ -15613,7 +15613,7 @@
     <row r="193" ht="130" customHeight="1">
       <c r="A193" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B193" s="3" t="inlineStr">
@@ -15688,7 +15688,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AC-2 (4),AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3 (1),AC-2 (4),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B194" s="3" t="inlineStr">
@@ -15761,7 +15761,7 @@
     <row r="195" ht="130" customHeight="1">
       <c r="A195" s="3" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-3 (1),AC-2 (4),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B195" s="3" t="inlineStr">
@@ -15838,7 +15838,7 @@
     <row r="196" ht="130" customHeight="1">
       <c r="A196" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (2),IA-2 (4),IA-2 (3)</t>
+          <t>IA-2 (1),IA-2 (3),IA-2 (4),IA-2 (2)</t>
         </is>
       </c>
       <c r="B196" s="2" t="inlineStr">
@@ -15925,7 +15925,7 @@
     <row r="197" ht="130" customHeight="1">
       <c r="A197" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),IA-2 (4),IA-2 (2),IA-2,IA-2 (3)</t>
+          <t>IA-2 (4),IA-2,IA-2 (5),IA-2 (3),IA-2 (2)</t>
         </is>
       </c>
       <c r="B197" s="2" t="inlineStr">
@@ -16014,7 +16014,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),IA-2 (4),IA-2 (2),IA-2,IA-2 (3)</t>
+          <t>IA-2 (4),IA-2,IA-2 (5),IA-2 (3),IA-2 (2)</t>
         </is>
       </c>
       <c r="B198" s="2" t="inlineStr">
@@ -16638,7 +16638,7 @@
     <row r="206" ht="130" customHeight="1">
       <c r="A206" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (1),SC-8 (2)</t>
+          <t>SC-8 (2),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B206" s="2" t="inlineStr">
@@ -16715,7 +16715,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (1),SC-8 (2)</t>
+          <t>SC-8 (2),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -17229,7 +17229,7 @@
     <row r="213" ht="130" customHeight="1">
       <c r="A213" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b,IA-5 (1) (c)</t>
+          <t>CM-6 b,CM-7 a,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B213" s="2" t="inlineStr">
@@ -17389,7 +17389,7 @@
     <row r="215" ht="130" customHeight="1">
       <c r="A215" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,CM-6 b</t>
+          <t>CM-6 b,AU-12 a</t>
         </is>
       </c>
       <c r="B215" s="3" t="inlineStr">
@@ -17475,7 +17475,7 @@
     <row r="216" ht="130" customHeight="1">
       <c r="A216" s="2" t="inlineStr">
         <is>
-          <t>SC-5,SC-5 (2),CM-6 b</t>
+          <t>CM-6 b,SC-5,SC-5 (2)</t>
         </is>
       </c>
       <c r="B216" s="2" t="inlineStr">
@@ -17747,7 +17747,7 @@
     <row r="219" ht="130" customHeight="1">
       <c r="A219" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-6 b</t>
+          <t>CM-6 b,SI-16</t>
         </is>
       </c>
       <c r="B219" s="2" t="inlineStr">
@@ -18824,7 +18824,7 @@
     <row r="232" ht="130" customHeight="1">
       <c r="A232" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-6 b,SC-2</t>
+          <t>SI-16,SC-2,CM-6 b</t>
         </is>
       </c>
       <c r="B232" s="2" t="inlineStr">
@@ -19732,7 +19732,7 @@
     <row r="243" ht="130" customHeight="1">
       <c r="A243" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (a),IA-5 (1) (b)</t>
+          <t>CM-6 b,IA-5 (1) (b),IA-5 (1) (a)</t>
         </is>
       </c>
       <c r="B243" s="2" t="inlineStr">
@@ -20300,7 +20300,7 @@
     <row r="250" ht="130" customHeight="1">
       <c r="A250" s="2" t="inlineStr">
         <is>
-          <t>SC-4,CM-6 b</t>
+          <t>CM-6 b,SC-4</t>
         </is>
       </c>
       <c r="B250" s="2" t="inlineStr">
@@ -20381,7 +20381,7 @@
     <row r="251" ht="130" customHeight="1">
       <c r="A251" s="3" t="inlineStr">
         <is>
-          <t>SC-4,SC-2</t>
+          <t>SC-2,SC-4</t>
         </is>
       </c>
       <c r="B251" s="3" t="inlineStr">
@@ -20469,7 +20469,7 @@
     <row r="252" ht="130" customHeight="1">
       <c r="A252" s="3" t="inlineStr">
         <is>
-          <t>SC-4,SC-2</t>
+          <t>SC-2,SC-4</t>
         </is>
       </c>
       <c r="B252" s="3" t="inlineStr">
@@ -20645,7 +20645,7 @@
     <row r="254" ht="130" customHeight="1">
       <c r="A254" s="3" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B254" s="3" t="inlineStr">
@@ -20970,7 +20970,7 @@
     <row r="258" ht="130" customHeight="1">
       <c r="A258" s="2" t="inlineStr">
         <is>
-          <t>SC-3,SI-6 a</t>
+          <t>SI-6 a,SC-3</t>
         </is>
       </c>
       <c r="B258" s="2" t="inlineStr">
@@ -21052,7 +21052,7 @@
     <row r="259" ht="130" customHeight="1">
       <c r="A259" s="3" t="inlineStr">
         <is>
-          <t>AC-6 (8),AC-6 (9)</t>
+          <t>AC-6 (9),AC-6 (8)</t>
         </is>
       </c>
       <c r="B259" s="3" t="inlineStr">
@@ -21132,7 +21132,7 @@
     <row r="260" ht="130" customHeight="1">
       <c r="A260" s="3" t="inlineStr">
         <is>
-          <t>IA-2 (5),CM-6 b</t>
+          <t>CM-6 b,IA-2 (5)</t>
         </is>
       </c>
       <c r="B260" s="3" t="inlineStr">
@@ -21719,7 +21719,7 @@
     <row r="268" ht="130" customHeight="1">
       <c r="A268" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (3),CM-6 b</t>
+          <t>CM-6 b,CM-5 (3)</t>
         </is>
       </c>
       <c r="B268" s="2" t="inlineStr">
@@ -22404,7 +22404,7 @@
     <row r="276" ht="130" customHeight="1">
       <c r="A276" s="3" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B276" s="3" t="inlineStr">
@@ -23400,7 +23400,7 @@
     <row r="289" ht="130" customHeight="1">
       <c r="A289" s="3" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B289" s="3" t="inlineStr">
@@ -23471,7 +23471,7 @@
     <row r="290" ht="130" customHeight="1">
       <c r="A290" s="3" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B290" s="3" t="inlineStr">
@@ -23543,7 +23543,7 @@
     <row r="291" ht="130" customHeight="1">
       <c r="A291" s="3" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B291" s="3" t="inlineStr">
@@ -23701,7 +23701,7 @@
     <row r="293" ht="130" customHeight="1">
       <c r="A293" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-2 (4),AC-6 (9)</t>
+          <t>AC-6 (9),AU-12 c,AC-2 (4)</t>
         </is>
       </c>
       <c r="B293" s="3" t="inlineStr">
@@ -27430,7 +27430,7 @@
     <row r="342" ht="130" customHeight="1">
       <c r="A342" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),CM-6 b</t>
+          <t>CM-6 b,IA-2 (2)</t>
         </is>
       </c>
       <c r="B342" s="2" t="inlineStr">
@@ -27511,7 +27511,7 @@
     <row r="343" ht="130" customHeight="1">
       <c r="A343" s="3" t="inlineStr">
         <is>
-          <t>CM-5 (1),CM-6 b</t>
+          <t>CM-6 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B343" s="3" t="inlineStr">
@@ -27585,7 +27585,7 @@
     <row r="344" ht="130" customHeight="1">
       <c r="A344" s="3" t="inlineStr">
         <is>
-          <t>CM-5 (1),CM-6 b</t>
+          <t>CM-6 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B344" s="3" t="inlineStr">
@@ -28168,60 +28168,60 @@
       <c r="Q351" s="3" t="n"/>
     </row>
     <row r="352" ht="130" customHeight="1">
-      <c r="A352" s="3" t="inlineStr">
-        <is>
-          <t>AC-17 (2),CM-6 b</t>
-        </is>
-      </c>
-      <c r="B352" s="3" t="inlineStr">
+      <c r="A352" s="2" t="inlineStr">
+        <is>
+          <t>CM-6 b,AC-17 (2)</t>
+        </is>
+      </c>
+      <c r="B352" s="2" t="inlineStr">
         <is>
           <t>CCI-000068</t>
         </is>
       </c>
-      <c r="C352" s="3" t="inlineStr">
+      <c r="C352" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000480-GPOS-00227,SRG-OS-000033-GPOS-00014</t>
         </is>
       </c>
-      <c r="D352" s="3" t="inlineStr">
+      <c r="D352" s="2" t="inlineStr">
         <is>
           <t>CCE-90815-2</t>
         </is>
       </c>
-      <c r="E352" s="3" t="inlineStr">
+      <c r="E352" s="2" t="inlineStr">
         <is>
           <t>The operating system must be configured in accordance with the security configuration settings based on DoD security configuration or implementation guidance, including STIGs, NSA configuration guides, CTOs, and DTMs.</t>
         </is>
       </c>
-      <c r="F352" s="3" t="inlineStr">
+      <c r="F352" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 must be configured in accordance with the security configuration settings based on DoD security configuration or implementation guidance, including STIGs, NSA configuration guides, CTOs, and DTMs.</t>
         </is>
       </c>
-      <c r="G352" s="3" t="inlineStr">
+      <c r="G352" s="2" t="inlineStr">
         <is>
           <t>Configuring the operating system to implement organization-wide security implementation guides and security checklists ensures compliance with federal standards and establishes a common security baseline across DoD that reflects the most restrictive security posture consistent with operational requirements.
 Configuration settings are the set of parameters that can be changed in hardware, software, or firmware components of the system that affect the security posture and/or functionality of the system. Security-related parameters are those parameters impacting the security state of the system, including the parameters required to satisfy other security control requirements. Security-related parameters include, for example: registry settings; account, file, directory permission settings; and settings for functions, ports, protocols, services, and remote connections.</t>
         </is>
       </c>
-      <c r="H352" s="3" t="inlineStr">
+      <c r="H352" s="2" t="inlineStr">
         <is>
           <t>By decreasing the limit based on the amount of data and enabling
 time-based limit, effects of potential attacks against
 encryption keys are limited.</t>
         </is>
       </c>
-      <c r="I352" s="3" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J352" s="3" t="inlineStr">
+      <c r="I352" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J352" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system is configured in accordance with the security configuration settings based on DoD security configuration or implementation guidance, including STIGs, NSA configuration guides, CTOs, and DTMs. If it is not, this is a finding.</t>
         </is>
       </c>
-      <c r="K352" s="3" t="inlineStr">
+      <c r="K352" s="2" t="inlineStr">
         <is>
           <t>To check if RekeyLimit is set correctly, run the
 following command:
@@ -28231,16 +28231,24 @@
 If it is commented out or is not set, then this is a finding.</t>
         </is>
       </c>
-      <c r="L352" s="3" t="n"/>
-      <c r="M352" s="3" t="inlineStr"/>
-      <c r="N352" s="3" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O352" s="3" t="n"/>
-      <c r="P352" s="3" t="n"/>
-      <c r="Q352" s="3" t="n"/>
+      <c r="L352" s="2" t="n"/>
+      <c r="M352" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Configure Red Hat Enterprise Linux 9 to force a frequent session key renegotiation for SSH connections to the server by adding or modifying the following line in the "/etc/ssh/sshd_config.d/00-complianceascode-hardening.conf" file:
+RekeyLimit 512M 1h
+Restart the SSH daemon for the settings to take effect.
+$ sudo systemctl restart sshd.service</t>
+        </is>
+      </c>
+      <c r="N352" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O352" s="2" t="n"/>
+      <c r="P352" s="2" t="n"/>
+      <c r="Q352" s="2" t="n"/>
     </row>
     <row r="353" ht="130" customHeight="1">
       <c r="A353" s="3" t="inlineStr">
@@ -30143,7 +30151,7 @@
     <row r="378" ht="130" customHeight="1">
       <c r="A378" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B378" s="2" t="inlineStr">
@@ -30537,7 +30545,7 @@
     <row r="383" ht="130" customHeight="1">
       <c r="A383" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),AC-17 (9),CM-7 b,CM-6 b</t>
+          <t>CM-6 b,AC-17 (1),AC-17 (9),CM-7 b</t>
         </is>
       </c>
       <c r="B383" s="2" t="inlineStr">
@@ -30615,7 +30623,7 @@
     <row r="384" ht="130" customHeight="1">
       <c r="A384" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),CM-7 b,CM-6 b</t>
+          <t>CM-6 b,AC-17 (1),CM-7 b</t>
         </is>
       </c>
       <c r="B384" s="2" t="inlineStr">
@@ -33114,7 +33122,7 @@
     <row r="413" ht="130" customHeight="1">
       <c r="A413" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B413" s="2" t="inlineStr">
@@ -33196,7 +33204,7 @@
     <row r="414" ht="130" customHeight="1">
       <c r="A414" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B414" s="2" t="inlineStr">
@@ -33889,7 +33897,7 @@
     <row r="423" ht="130" customHeight="1">
       <c r="A423" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B423" s="2" t="inlineStr">
@@ -34492,7 +34500,7 @@
     <row r="430" ht="130" customHeight="1">
       <c r="A430" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B430" s="2" t="inlineStr">
@@ -34944,7 +34952,7 @@
     <row r="436" ht="130" customHeight="1">
       <c r="A436" s="2" t="inlineStr">
         <is>
-          <t>AU-4,CM-6 b</t>
+          <t>CM-6 b,AU-4</t>
         </is>
       </c>
       <c r="B436" s="2" t="inlineStr">
@@ -35248,7 +35256,7 @@
     <row r="440" ht="130" customHeight="1">
       <c r="A440" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B440" s="2" t="inlineStr">
@@ -35338,7 +35346,7 @@
     <row r="441" ht="130" customHeight="1">
       <c r="A441" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B441" s="2" t="inlineStr">
@@ -36671,7 +36679,7 @@
     <row r="459" ht="130" customHeight="1">
       <c r="A459" s="3" t="inlineStr">
         <is>
-          <t>SC-10,AC-12,MA-4 e,MA-4 (7)</t>
+          <t>MA-4 e,MA-4 (7),AC-12,SC-10</t>
         </is>
       </c>
       <c r="B459" s="3" t="inlineStr">
@@ -36746,7 +36754,7 @@
     <row r="460" ht="130" customHeight="1">
       <c r="A460" s="3" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B460" s="3" t="inlineStr">
@@ -36825,7 +36833,7 @@
     <row r="461" ht="130" customHeight="1">
       <c r="A461" s="3" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B461" s="3" t="inlineStr">
@@ -37032,14 +37040,14 @@
       </c>
       <c r="K463" s="2" t="inlineStr">
         <is>
-          <t>To check if RekeyLimit is set correctly, run the following command:  $
-sudo grep RekeyLimit /etc/ssh/ssh_config.d/*.conf  If configured
-properly, output should be  /etc/ssh/ssh_config.d/02-rekey-limit.conf:
-RekeyLimit 512M
-1h  Check also the
-main configuration file with the following command:  $ sudo grep
-RekeyLimit /etc/ssh/ssh_config  The command should not return any
-output.
+          <t>To check if RekeyLimit is set correctly, run the following command:
+ $ sudo grep RekeyLimit /etc/ssh/ssh_config.d/*.conf 
+If configured properly, output should be
+ /etc/ssh/ssh_config.d/02-rekey-limit.conf:
+RekeyLimit 1G 1h 
+Check also the main configuration file with the following command:
+ $ sudo grep RekeyLimit /etc/ssh/ssh_config 
+The command should not return any output.
 If it is commented out or is not set, then this is a finding.</t>
         </is>
       </c>
@@ -37047,7 +37055,7 @@
       <c r="M463" s="2" t="inlineStr">
         <is>
           <t>Configure Red Hat Enterprise Linux 9 to force a frequent session key renegotiation for SSH connections to the server by adding or modifying the following line in the "/etc/ssh/sshd_config" file:
-RekeyLimit 512M 1h
+RekeyLimit 1G 1h
 Restart the SSH daemon for the settings to take effect.
 $ sudo systemctl restart sshd.service</t>
         </is>
@@ -37062,61 +37070,61 @@
       <c r="Q463" s="2" t="n"/>
     </row>
     <row r="464" ht="130" customHeight="1">
-      <c r="A464" s="3" t="inlineStr">
+      <c r="A464" s="2" t="inlineStr">
         <is>
           <t>AC-17 (2)</t>
         </is>
       </c>
-      <c r="B464" s="3" t="inlineStr">
+      <c r="B464" s="2" t="inlineStr">
         <is>
           <t>CCI-000068</t>
         </is>
       </c>
-      <c r="C464" s="3" t="inlineStr">
+      <c r="C464" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000033-GPOS-00014</t>
         </is>
       </c>
-      <c r="D464" s="3" t="inlineStr">
+      <c r="D464" s="2" t="inlineStr">
         <is>
           <t>CCE-83446-5</t>
         </is>
       </c>
-      <c r="E464" s="3" t="inlineStr">
+      <c r="E464" s="2" t="inlineStr">
         <is>
           <t>The operating system must implement DoD-approved encryption to protect the confidentiality of remote access sessions.</t>
         </is>
       </c>
-      <c r="F464" s="3" t="inlineStr">
+      <c r="F464" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 must implement DoD-approved encryption to protect the confidentiality of remote access sessions.</t>
         </is>
       </c>
-      <c r="G464" s="3" t="inlineStr">
+      <c r="G464" s="2" t="inlineStr">
         <is>
           <t>Without confidentiality protection mechanisms, unauthorized individuals may gain access to sensitive information via a remote access session.
 Remote access is access to DoD nonpublic information systems by an authorized user (or an information system) communicating through an external, non-organization-controlled network. Remote access methods include, for example, dial-up, broadband, and wireless.
 Encryption provides a means to secure the remote connection to prevent unauthorized access to the data traversing the remote access connection (e.g., RDP), thereby providing a degree of confidentiality. The encryption strength of a mechanism is selected based on the security categorization of the information.</t>
         </is>
       </c>
-      <c r="H464" s="3" t="inlineStr">
+      <c r="H464" s="2" t="inlineStr">
         <is>
           <t>Overriding the system crypto policy makes the behavior of the Libreswan
 service violate expectations, and makes system configuration more
 fragmented.</t>
         </is>
       </c>
-      <c r="I464" s="3" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J464" s="3" t="inlineStr">
+      <c r="I464" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J464" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system implements DoD-approved encryption to protect the confidentiality of remote access sessions. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K464" s="3" t="inlineStr">
+      <c r="K464" s="2" t="inlineStr">
         <is>
           <t>To verify that Libreswan uses the system crypto policy, run the following command:
  $ grep include /etc/ipsec.conf 
@@ -37125,16 +37133,22 @@
 If Libreswan is installed and "/etc/ipsec.conf" does not contain "include /etc/crypto-policies/back-ends/libreswan.config", then this is a finding.</t>
         </is>
       </c>
-      <c r="L464" s="3" t="n"/>
-      <c r="M464" s="3" t="inlineStr"/>
-      <c r="N464" s="3" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O464" s="3" t="n"/>
-      <c r="P464" s="3" t="n"/>
-      <c r="Q464" s="3" t="n"/>
+      <c r="L464" s="2" t="n"/>
+      <c r="M464" s="2" t="inlineStr">
+        <is>
+          <t>Configure Libreswan to use the system cryptographic policy.
+Add the following line to "/etc/ipsec.conf":
+include /etc/crypto-policies/back-ends/libreswan.config</t>
+        </is>
+      </c>
+      <c r="N464" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O464" s="2" t="n"/>
+      <c r="P464" s="2" t="n"/>
+      <c r="Q464" s="2" t="n"/>
     </row>
     <row r="465" ht="130" customHeight="1">
       <c r="A465" s="2" t="inlineStr">
@@ -39973,7 +39987,7 @@
     <row r="501" ht="130" customHeight="1">
       <c r="A501" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B501" s="2" t="inlineStr">
@@ -40075,7 +40089,7 @@
     <row r="502" ht="130" customHeight="1">
       <c r="A502" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B502" s="2" t="inlineStr">
@@ -40185,7 +40199,7 @@
     <row r="503" ht="130" customHeight="1">
       <c r="A503" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B503" s="2" t="inlineStr">
@@ -40296,7 +40310,7 @@
     <row r="504" ht="130" customHeight="1">
       <c r="A504" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B504" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@ca85e07343cdaabad7c15469b017d72bac3bfa7c 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -973,7 +973,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>AU-5 b,AU-5 a</t>
+          <t>AU-5 a,AU-5 b</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -1455,7 +1455,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),AU-3,CM-6 b,AU-3 (1),CM-5 (1),MA-4 (1) (a),AU-12 a,AU-6 (4),AU-7 a,AU-7 (1)</t>
+          <t>AU-7 a,AU-12 a,AU-3,MA-4 (1) (a),AU-6 (4),AU-7 (1),AU-3 (1),CM-5 (1),CM-6 b,AU-14 (1)</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -1540,7 +1540,7 @@
     <row r="14" ht="130" customHeight="1">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -1616,7 +1616,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1770,7 +1770,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -2140,7 +2140,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -2214,7 +2214,7 @@
     <row r="23" ht="130" customHeight="1">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -3258,7 +3258,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c,AU-14 (1)</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3349,7 +3349,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),AU-4</t>
+          <t>AU-4,AU-14 (1)</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3438,7 +3438,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-4 (1)</t>
+          <t>AU-4 (1),AU-3</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3832,7 +3832,7 @@
     <row r="44" ht="130" customHeight="1">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),CM-6 b,AU-6 (4)</t>
+          <t>AU-6 (4),AU-4 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
@@ -3908,7 +3908,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),CM-6 b</t>
+          <t>CM-6 b,AU-4 (1)</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3993,7 +3993,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (a),AU-8 (1) (b),AU-8 b</t>
+          <t>AU-8 b,AU-8 (1) (b),AU-8 (1) (a)</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -4148,7 +4148,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4234,7 +4234,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11),IA-2 (1)</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4494,7 +4494,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -4569,7 +4569,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -4644,7 +4644,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -4719,7 +4719,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -4794,7 +4794,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -4869,7 +4869,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -4944,7 +4944,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -5019,7 +5019,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -5094,7 +5094,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -5169,7 +5169,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-12 (3),CM-6 b,CM-5 (1),AU-12 c,AU-12 a,AU-8 b,AU-7 b,AU-7 a</t>
+          <t>AU-7 a,AU-7 b,AU-12 (3),AU-12 a,CM-6 b,CM-5 (1),AU-12 c,AU-8 b</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5243,7 +5243,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-12 c</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5324,7 +5324,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-12 c</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5405,7 +5405,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-12 c</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5487,7 +5487,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-12 c</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5569,7 +5569,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-12 c</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5651,7 +5651,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-12 c</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5733,7 +5733,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-12 c</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5889,7 +5889,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5972,7 +5972,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -6050,7 +6050,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -6141,7 +6141,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6223,7 +6223,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6853,7 +6853,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -6927,7 +6927,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -7001,7 +7001,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -7075,7 +7075,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -7155,7 +7155,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -7240,7 +7240,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>AC-17 (2),MA-4 (6)</t>
+          <t>MA-4 (6),AC-17 (2)</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -7316,7 +7316,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -7499,7 +7499,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>AU-9 (3),AU-9</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -7575,7 +7575,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>AU-9 (3),AU-9</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -7651,7 +7651,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -7726,7 +7726,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -7801,7 +7801,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -7876,7 +7876,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -7956,7 +7956,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -8038,7 +8038,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -8120,7 +8120,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8202,7 +8202,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8284,7 +8284,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8366,7 +8366,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -8446,7 +8446,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -8526,7 +8526,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -8606,7 +8606,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AC-11 (1),AC-11 b</t>
+          <t>AC-11 b,AC-11 (1)</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -9354,7 +9354,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-13,SC-8,MA-4 c</t>
+          <t>SC-13,SC-8,AC-17 (2),MA-4 c</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9436,7 +9436,7 @@
     <row r="114" ht="130" customHeight="1">
       <c r="A114" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B114" s="2" t="inlineStr">
@@ -9514,7 +9514,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9592,7 +9592,7 @@
     <row r="116" ht="130" customHeight="1">
       <c r="A116" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B116" s="2" t="inlineStr">
@@ -9670,7 +9670,7 @@
     <row r="117" ht="130" customHeight="1">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -9750,7 +9750,7 @@
     <row r="118" ht="130" customHeight="1">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
@@ -9819,7 +9819,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
@@ -9888,7 +9888,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
@@ -9957,7 +9957,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
@@ -10026,7 +10026,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -10106,7 +10106,7 @@
     <row r="123" ht="130" customHeight="1">
       <c r="A123" s="2" t="inlineStr">
         <is>
-          <t>SC-28,SC-28 (1)</t>
+          <t>SC-28 (1),SC-28</t>
         </is>
       </c>
       <c r="B123" s="2" t="inlineStr">
@@ -11110,7 +11110,7 @@
 If the service is masked the command will return the following outputs:
  LoadState=masked 
  UnitFileState=masked 
-If , then this is a finding.</t>
+If the "debug-shell" is loaded and not masked, then this is a finding.</t>
         </is>
       </c>
       <c r="L135" s="2" t="n"/>
@@ -11406,7 +11406,7 @@
     <row r="139" ht="130" customHeight="1">
       <c r="A139" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B139" s="3" t="inlineStr">
@@ -11486,7 +11486,7 @@
     <row r="140" ht="130" customHeight="1">
       <c r="A140" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B140" s="3" t="inlineStr">
@@ -11566,7 +11566,7 @@
     <row r="141" ht="130" customHeight="1">
       <c r="A141" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B141" s="3" t="inlineStr">
@@ -11646,7 +11646,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B142" s="3" t="inlineStr">
@@ -11958,7 +11958,7 @@
     <row r="146" ht="130" customHeight="1">
       <c r="A146" s="2" t="inlineStr">
         <is>
-          <t>IA-7,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),IA-7</t>
         </is>
       </c>
       <c r="B146" s="2" t="inlineStr">
@@ -12826,7 +12826,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B157" s="3" t="inlineStr">
@@ -12903,7 +12903,7 @@
     <row r="158" ht="130" customHeight="1">
       <c r="A158" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B158" s="3" t="inlineStr">
@@ -12976,7 +12976,7 @@
     <row r="159" ht="130" customHeight="1">
       <c r="A159" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B159" s="3" t="inlineStr">
@@ -13049,7 +13049,7 @@
     <row r="160" ht="130" customHeight="1">
       <c r="A160" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B160" s="3" t="inlineStr">
@@ -13134,7 +13134,7 @@
     <row r="161" ht="130" customHeight="1">
       <c r="A161" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B161" s="3" t="inlineStr">
@@ -13209,7 +13209,7 @@
     <row r="162" ht="130" customHeight="1">
       <c r="A162" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B162" s="3" t="inlineStr">
@@ -13284,7 +13284,7 @@
     <row r="163" ht="130" customHeight="1">
       <c r="A163" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B163" s="3" t="inlineStr">
@@ -13359,7 +13359,7 @@
     <row r="164" ht="130" customHeight="1">
       <c r="A164" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B164" s="3" t="inlineStr">
@@ -13434,7 +13434,7 @@
     <row r="165" ht="130" customHeight="1">
       <c r="A165" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B165" s="3" t="inlineStr">
@@ -13505,7 +13505,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B166" s="3" t="inlineStr">
@@ -13576,7 +13576,7 @@
     <row r="167" ht="130" customHeight="1">
       <c r="A167" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B167" s="3" t="inlineStr">
@@ -13648,7 +13648,7 @@
     <row r="168" ht="130" customHeight="1">
       <c r="A168" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B168" s="3" t="inlineStr">
@@ -13719,7 +13719,7 @@
     <row r="169" ht="130" customHeight="1">
       <c r="A169" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B169" s="3" t="inlineStr">
@@ -13790,7 +13790,7 @@
     <row r="170" ht="130" customHeight="1">
       <c r="A170" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B170" s="3" t="inlineStr">
@@ -13862,7 +13862,7 @@
     <row r="171" ht="130" customHeight="1">
       <c r="A171" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B171" s="3" t="inlineStr">
@@ -13937,7 +13937,7 @@
     <row r="172" ht="130" customHeight="1">
       <c r="A172" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B172" s="3" t="inlineStr">
@@ -14008,7 +14008,7 @@
     <row r="173" ht="130" customHeight="1">
       <c r="A173" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B173" s="3" t="inlineStr">
@@ -14079,7 +14079,7 @@
     <row r="174" ht="130" customHeight="1">
       <c r="A174" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B174" s="3" t="inlineStr">
@@ -14151,7 +14151,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B175" s="3" t="inlineStr">
@@ -14226,7 +14226,7 @@
     <row r="176" ht="130" customHeight="1">
       <c r="A176" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B176" s="3" t="inlineStr">
@@ -14308,7 +14308,7 @@
     <row r="177" ht="130" customHeight="1">
       <c r="A177" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B177" s="3" t="inlineStr">
@@ -14390,7 +14390,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B178" s="3" t="inlineStr">
@@ -14472,7 +14472,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B179" s="3" t="inlineStr">
@@ -14554,7 +14554,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B180" s="3" t="inlineStr">
@@ -14636,7 +14636,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B181" s="3" t="inlineStr">
@@ -14718,7 +14718,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B182" s="3" t="inlineStr">
@@ -14800,7 +14800,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B183" s="3" t="inlineStr">
@@ -14882,7 +14882,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B184" s="3" t="inlineStr">
@@ -14964,7 +14964,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B185" s="3" t="inlineStr">
@@ -15042,7 +15042,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B186" s="3" t="inlineStr">
@@ -15121,7 +15121,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B187" s="3" t="inlineStr">
@@ -15203,7 +15203,7 @@
     <row r="188" ht="130" customHeight="1">
       <c r="A188" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B188" s="3" t="inlineStr">
@@ -15285,7 +15285,7 @@
     <row r="189" ht="130" customHeight="1">
       <c r="A189" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B189" s="3" t="inlineStr">
@@ -15367,7 +15367,7 @@
     <row r="190" ht="130" customHeight="1">
       <c r="A190" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B190" s="3" t="inlineStr">
@@ -15449,7 +15449,7 @@
     <row r="191" ht="130" customHeight="1">
       <c r="A191" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B191" s="3" t="inlineStr">
@@ -15531,7 +15531,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B192" s="3" t="inlineStr">
@@ -15613,7 +15613,7 @@
     <row r="193" ht="130" customHeight="1">
       <c r="A193" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B193" s="3" t="inlineStr">
@@ -15688,7 +15688,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-3 (1),AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-12 c</t>
         </is>
       </c>
       <c r="B194" s="3" t="inlineStr">
@@ -15761,7 +15761,7 @@
     <row r="195" ht="130" customHeight="1">
       <c r="A195" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-12 c</t>
         </is>
       </c>
       <c r="B195" s="3" t="inlineStr">
@@ -15838,7 +15838,7 @@
     <row r="196" ht="130" customHeight="1">
       <c r="A196" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (2),IA-2 (3),IA-2 (4)</t>
+          <t>IA-2 (2),IA-2 (4),IA-2 (3),IA-2 (1)</t>
         </is>
       </c>
       <c r="B196" s="2" t="inlineStr">
@@ -15925,7 +15925,7 @@
     <row r="197" ht="130" customHeight="1">
       <c r="A197" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2 (5),IA-2 (2),IA-2,IA-2 (3)</t>
+          <t>IA-2 (3),IA-2 (5),IA-2 (2),IA-2 (4),IA-2</t>
         </is>
       </c>
       <c r="B197" s="2" t="inlineStr">
@@ -16014,7 +16014,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2 (5),IA-2 (2),IA-2,IA-2 (3)</t>
+          <t>IA-2 (3),IA-2 (5),IA-2 (2),IA-2 (4),IA-2</t>
         </is>
       </c>
       <c r="B198" s="2" t="inlineStr">
@@ -16258,7 +16258,7 @@
     <row r="201" ht="130" customHeight="1">
       <c r="A201" s="2" t="inlineStr">
         <is>
-          <t>AC-3 (4),IA-11</t>
+          <t>IA-11,AC-3 (4)</t>
         </is>
       </c>
       <c r="B201" s="2" t="inlineStr">
@@ -16638,7 +16638,7 @@
     <row r="206" ht="130" customHeight="1">
       <c r="A206" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (1),SC-8 (2)</t>
+          <t>SC-8 (1),SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B206" s="2" t="inlineStr">
@@ -16715,7 +16715,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (1),SC-8 (2)</t>
+          <t>SC-8 (1),SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -16801,7 +16801,7 @@
     <row r="208" ht="130" customHeight="1">
       <c r="A208" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-18 (1),SC-8 (1)</t>
+          <t>SC-8 (1),AC-18 (1),SC-8</t>
         </is>
       </c>
       <c r="B208" s="2" t="inlineStr">
@@ -17229,7 +17229,7 @@
     <row r="213" ht="130" customHeight="1">
       <c r="A213" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b,IA-5 (1) (c)</t>
+          <t>CM-7 a,IA-5 (1) (c),CM-6 b</t>
         </is>
       </c>
       <c r="B213" s="2" t="inlineStr">
@@ -17475,7 +17475,7 @@
     <row r="216" ht="130" customHeight="1">
       <c r="A216" s="2" t="inlineStr">
         <is>
-          <t>SC-5,CM-6 b,SC-5 (2)</t>
+          <t>CM-6 b,SC-5 (2),SC-5</t>
         </is>
       </c>
       <c r="B216" s="2" t="inlineStr">
@@ -17845,7 +17845,7 @@
     <row r="220" ht="130" customHeight="1">
       <c r="A220" s="2" t="inlineStr">
         <is>
-          <t>IA-8,IA-2,AU-3 (1)</t>
+          <t>AU-3 (1),IA-8,IA-2</t>
         </is>
       </c>
       <c r="B220" s="2" t="inlineStr">
@@ -18824,7 +18824,7 @@
     <row r="232" ht="130" customHeight="1">
       <c r="A232" s="2" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b,SI-16</t>
+          <t>CM-6 b,SI-16,SC-2</t>
         </is>
       </c>
       <c r="B232" s="2" t="inlineStr">
@@ -19008,7 +19008,7 @@
     <row r="234" ht="130" customHeight="1">
       <c r="A234" s="2" t="inlineStr">
         <is>
-          <t>SC-3,SI-16</t>
+          <t>SI-16,SC-3</t>
         </is>
       </c>
       <c r="B234" s="2" t="inlineStr">
@@ -19170,7 +19170,7 @@
     <row r="236" ht="130" customHeight="1">
       <c r="A236" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),CM-7 a</t>
+          <t>CM-7 a,AC-18 (1)</t>
         </is>
       </c>
       <c r="B236" s="2" t="inlineStr">
@@ -20300,7 +20300,7 @@
     <row r="250" ht="130" customHeight="1">
       <c r="A250" s="2" t="inlineStr">
         <is>
-          <t>SC-4,CM-6 b</t>
+          <t>CM-6 b,SC-4</t>
         </is>
       </c>
       <c r="B250" s="2" t="inlineStr">
@@ -20381,7 +20381,7 @@
     <row r="251" ht="130" customHeight="1">
       <c r="A251" s="3" t="inlineStr">
         <is>
-          <t>SC-2,SC-4</t>
+          <t>SC-4,SC-2</t>
         </is>
       </c>
       <c r="B251" s="3" t="inlineStr">
@@ -20469,7 +20469,7 @@
     <row r="252" ht="130" customHeight="1">
       <c r="A252" s="3" t="inlineStr">
         <is>
-          <t>SC-2,SC-4</t>
+          <t>SC-4,SC-2</t>
         </is>
       </c>
       <c r="B252" s="3" t="inlineStr">
@@ -20556,7 +20556,7 @@
     <row r="253" ht="130" customHeight="1">
       <c r="A253" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (1)</t>
         </is>
       </c>
       <c r="B253" s="2" t="inlineStr">
@@ -20645,7 +20645,7 @@
     <row r="254" ht="130" customHeight="1">
       <c r="A254" s="3" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B254" s="3" t="inlineStr">
@@ -20970,7 +20970,7 @@
     <row r="258" ht="130" customHeight="1">
       <c r="A258" s="2" t="inlineStr">
         <is>
-          <t>SC-3,SI-6 a</t>
+          <t>SI-6 a,SC-3</t>
         </is>
       </c>
       <c r="B258" s="2" t="inlineStr">
@@ -21052,7 +21052,7 @@
     <row r="259" ht="130" customHeight="1">
       <c r="A259" s="3" t="inlineStr">
         <is>
-          <t>AC-6 (8),AC-6 (9)</t>
+          <t>AC-6 (9),AC-6 (8)</t>
         </is>
       </c>
       <c r="B259" s="3" t="inlineStr">
@@ -21132,7 +21132,7 @@
     <row r="260" ht="130" customHeight="1">
       <c r="A260" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (5)</t>
+          <t>IA-2 (5),CM-6 b</t>
         </is>
       </c>
       <c r="B260" s="3" t="inlineStr">
@@ -21598,7 +21598,7 @@
     <row r="266" ht="130" customHeight="1">
       <c r="A266" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-9</t>
+          <t>AU-9,AU-12 c</t>
         </is>
       </c>
       <c r="B266" s="2" t="inlineStr">
@@ -22366,7 +22366,7 @@
     <row r="275" ht="130" customHeight="1">
       <c r="A275" s="3" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B275" s="3" t="inlineStr">
@@ -22514,7 +22514,7 @@
     <row r="277" ht="130" customHeight="1">
       <c r="A277" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-7 a</t>
+          <t>CM-7 a,CM-7 b</t>
         </is>
       </c>
       <c r="B277" s="2" t="inlineStr">
@@ -22594,7 +22594,7 @@
     <row r="278" ht="130" customHeight="1">
       <c r="A278" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-7 a</t>
+          <t>CM-7 a,CM-7 b</t>
         </is>
       </c>
       <c r="B278" s="2" t="inlineStr">
@@ -23663,7 +23663,7 @@
     <row r="292" ht="130" customHeight="1">
       <c r="A292" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-2 (4),AC-6 (9)</t>
+          <t>AC-6 (9),AC-2 (4),AU-12 c</t>
         </is>
       </c>
       <c r="B292" s="3" t="inlineStr">
@@ -23880,7 +23880,7 @@
     <row r="294" ht="130" customHeight="1">
       <c r="A294" s="3" t="inlineStr">
         <is>
-          <t>AU-5 (1),AU-5 a</t>
+          <t>AU-5 a,AU-5 (1)</t>
         </is>
       </c>
       <c r="B294" s="3" t="inlineStr">
@@ -24382,7 +24382,7 @@
 If the service is masked the command will return the following outputs:
  LoadState=masked 
  UnitFileState=masked 
-If , then this is a finding.</t>
+If the "kdump" is loaded and not masked, then this is a finding.</t>
         </is>
       </c>
       <c r="L300" s="3" t="n"/>
@@ -27392,7 +27392,7 @@
     <row r="341" ht="130" customHeight="1">
       <c r="A341" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),CM-6 b</t>
+          <t>CM-6 b,IA-2 (2)</t>
         </is>
       </c>
       <c r="B341" s="2" t="inlineStr">
@@ -27473,7 +27473,7 @@
     <row r="342" ht="130" customHeight="1">
       <c r="A342" s="3" t="inlineStr">
         <is>
-          <t>CM-5 (1),CM-6 b</t>
+          <t>CM-6 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B342" s="3" t="inlineStr">
@@ -27547,7 +27547,7 @@
     <row r="343" ht="130" customHeight="1">
       <c r="A343" s="3" t="inlineStr">
         <is>
-          <t>CM-5 (1),CM-6 b</t>
+          <t>CM-6 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B343" s="3" t="inlineStr">
@@ -28132,7 +28132,7 @@
     <row r="351" ht="130" customHeight="1">
       <c r="A351" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),CM-6 b</t>
+          <t>CM-6 b,AC-17 (2)</t>
         </is>
       </c>
       <c r="B351" s="2" t="inlineStr">
@@ -29869,7 +29869,7 @@
     <row r="374" ht="130" customHeight="1">
       <c r="A374" s="3" t="inlineStr">
         <is>
-          <t>AU-3,CM-6 b</t>
+          <t>CM-6 b,AU-3</t>
         </is>
       </c>
       <c r="B374" s="3" t="inlineStr">
@@ -30113,7 +30113,7 @@
     <row r="377" ht="130" customHeight="1">
       <c r="A377" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B377" s="2" t="inlineStr">
@@ -30507,7 +30507,7 @@
     <row r="382" ht="130" customHeight="1">
       <c r="A382" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (9),CM-7 b,CM-6 b,AC-17 (1)</t>
+          <t>CM-6 b,CM-7 b,AC-17 (9),AC-17 (1)</t>
         </is>
       </c>
       <c r="B382" s="2" t="inlineStr">
@@ -30585,7 +30585,7 @@
     <row r="383" ht="130" customHeight="1">
       <c r="A383" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-6 b,AC-17 (1)</t>
+          <t>CM-6 b,CM-7 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B383" s="2" t="inlineStr">
@@ -33237,7 +33237,7 @@
 If the service is masked the command will return the following outputs:
  LoadState=masked 
  UnitFileState=masked 
-If the autofs service is not disabled, then this is a finding.</t>
+If the "autofs" is loaded and not masked, then this is a finding.</t>
         </is>
       </c>
       <c r="L413" s="2" t="n"/>
@@ -33859,7 +33859,7 @@
     <row r="422" ht="130" customHeight="1">
       <c r="A422" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B422" s="2" t="inlineStr">
@@ -34040,7 +34040,7 @@
     <row r="424" ht="130" customHeight="1">
       <c r="A424" s="3" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b</t>
+          <t>CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B424" s="3" t="inlineStr">
@@ -34127,7 +34127,7 @@
     <row r="425" ht="130" customHeight="1">
       <c r="A425" s="3" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b</t>
+          <t>CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B425" s="3" t="inlineStr">
@@ -34462,7 +34462,7 @@
     <row r="429" ht="130" customHeight="1">
       <c r="A429" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B429" s="2" t="inlineStr">
@@ -34914,7 +34914,7 @@
     <row r="435" ht="130" customHeight="1">
       <c r="A435" s="2" t="inlineStr">
         <is>
-          <t>AU-4,CM-6 b</t>
+          <t>CM-6 b,AU-4</t>
         </is>
       </c>
       <c r="B435" s="2" t="inlineStr">
@@ -36641,7 +36641,7 @@
     <row r="458" ht="130" customHeight="1">
       <c r="A458" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (7),MA-4 e,AC-12,SC-10</t>
+          <t>AC-12,MA-4 (7),SC-10,MA-4 e</t>
         </is>
       </c>
       <c r="B458" s="3" t="inlineStr">
@@ -36666,7 +36666,7 @@
       </c>
       <c r="F458" s="3" t="inlineStr">
         <is>
-          <t>Red Hat Enterprise Linux 9 must terminate all network connections associated with a communications session at the end of the session, or as follows: for in-band management sessions (privileged sessions), the session must be terminated after 10 minutes of inacti</t>
+          <t>Red Hat Enterprise Linux 9 must terminate all network connections associated with a communications session at the end of the session, or as follows: for in-band management sessions (privileged sessions), the session must be terminated after 10 minutes of inactivity; and for user sessions (non-privileged session), the session must be terminated after 15 minutes of inactivity, except to fulfill documented and validated mission requirements.</t>
         </is>
       </c>
       <c r="G458" s="3" t="inlineStr">
@@ -36716,7 +36716,7 @@
     <row r="459" ht="130" customHeight="1">
       <c r="A459" s="3" t="inlineStr">
         <is>
-          <t>SC-10,AC-12</t>
+          <t>AC-12,SC-10</t>
         </is>
       </c>
       <c r="B459" s="3" t="inlineStr">
@@ -36741,7 +36741,7 @@
       </c>
       <c r="F459" s="3" t="inlineStr">
         <is>
-          <t>Red Hat Enterprise Linux 9 must terminate all network connections associated with a communications session at the end of the session, or as follows: for in-band management sessions (privileged sessions), the session must be terminated after 10 minutes of inacti</t>
+          <t>Red Hat Enterprise Linux 9 must terminate all network connections associated with a communications session at the end of the session, or as follows: for in-band management sessions (privileged sessions), the session must be terminated after 10 minutes of inactivity; and for user sessions (non-privileged session), the session must be terminated after 15 minutes of inactivity, except to fulfill documented and validated mission requirements.</t>
         </is>
       </c>
       <c r="G459" s="3" t="inlineStr">
@@ -36795,7 +36795,7 @@
     <row r="460" ht="130" customHeight="1">
       <c r="A460" s="3" t="inlineStr">
         <is>
-          <t>SC-10,AC-12</t>
+          <t>AC-12,SC-10</t>
         </is>
       </c>
       <c r="B460" s="3" t="inlineStr">
@@ -36820,7 +36820,7 @@
       </c>
       <c r="F460" s="3" t="inlineStr">
         <is>
-          <t>Red Hat Enterprise Linux 9 must terminate all network connections associated with a communications session at the end of the session, or as follows: for in-band management sessions (privileged sessions), the session must be terminated after 10 minutes of inacti</t>
+          <t>Red Hat Enterprise Linux 9 must terminate all network connections associated with a communications session at the end of the session, or as follows: for in-band management sessions (privileged sessions), the session must be terminated after 10 minutes of inactivity; and for user sessions (non-privileged session), the session must be terminated after 15 minutes of inactivity, except to fulfill documented and validated mission requirements.</t>
         </is>
       </c>
       <c r="G460" s="3" t="inlineStr">
@@ -36896,7 +36896,7 @@
       </c>
       <c r="F461" s="3" t="inlineStr">
         <is>
-          <t>Red Hat Enterprise Linux 9 must terminate all network connections associated with a communications session at the end of the session, or as follows: for in-band management sessions (privileged sessions), the session must be terminated after 10 minutes of inacti</t>
+          <t>Red Hat Enterprise Linux 9 must terminate all network connections associated with a communications session at the end of the session, or as follows: for in-band management sessions (privileged sessions), the session must be terminated after 10 minutes of inactivity; and for user sessions (non-privileged session), the session must be terminated after 15 minutes of inactivity, except to fulfill documented and validated mission requirements.</t>
         </is>
       </c>
       <c r="G461" s="3" t="inlineStr">
@@ -36948,7 +36948,7 @@
     <row r="462" ht="130" customHeight="1">
       <c r="A462" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2),SC-8 (1)</t>
+          <t>SC-8 (1),SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B462" s="2" t="inlineStr">
@@ -39698,7 +39698,7 @@
     <row r="497" ht="130" customHeight="1">
       <c r="A497" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-4</t>
+          <t>AU-4,AU-4 (1)</t>
         </is>
       </c>
       <c r="B497" s="2" t="inlineStr">
@@ -39949,7 +39949,7 @@
     <row r="500" ht="130" customHeight="1">
       <c r="A500" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B500" s="2" t="inlineStr">
@@ -40051,7 +40051,7 @@
     <row r="501" ht="130" customHeight="1">
       <c r="A501" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B501" s="2" t="inlineStr">
@@ -40161,7 +40161,7 @@
     <row r="502" ht="130" customHeight="1">
       <c r="A502" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B502" s="2" t="inlineStr">
@@ -40272,7 +40272,7 @@
     <row r="503" ht="130" customHeight="1">
       <c r="A503" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B503" s="2" t="inlineStr">
@@ -41418,7 +41418,7 @@
     <row r="518" ht="130" customHeight="1">
       <c r="A518" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (2)</t>
+          <t>SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B518" s="2" t="inlineStr">
@@ -42608,7 +42608,7 @@
     <row r="533" ht="130" customHeight="1">
       <c r="A533" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8</t>
+          <t>SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B533" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@ded1f3dc2ba182fcb2ca38f1d779d4b2f02f3952 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -973,7 +973,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 b</t>
+          <t>AU-5 b,AU-5 a</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -1455,7 +1455,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>AU-7 a,AU-12 a,AU-3,MA-4 (1) (a),AU-6 (4),AU-7 (1),AU-3 (1),CM-5 (1),CM-6 b,AU-14 (1)</t>
+          <t>AU-12 a,AU-3,CM-5 (1),MA-4 (1) (a),CM-6 b,AU-6 (4),AU-7 (1),AU-14 (1),AU-7 a,AU-3 (1)</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -1770,7 +1770,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -2140,7 +2140,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -2214,7 +2214,7 @@
     <row r="23" ht="130" customHeight="1">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -3258,7 +3258,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c,AU-14 (1)</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-14 (1),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3349,7 +3349,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-14 (1)</t>
+          <t>AU-14 (1),AU-4</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3438,7 +3438,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-3</t>
+          <t>AU-3,AU-4 (1)</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3832,7 +3832,7 @@
     <row r="44" ht="130" customHeight="1">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>AU-6 (4),AU-4 (1),CM-6 b</t>
+          <t>AU-6 (4),CM-6 b,AU-4 (1)</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
@@ -4148,7 +4148,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4234,7 +4234,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11),IA-2 (1)</t>
+          <t>IA-2 (11),IA-2 (1),IA-2 (12)</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4318,7 +4318,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 b,SI-6 d</t>
+          <t>SI-6 d,SI-6 b,CM-3 (5)</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4410,7 +4410,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 d</t>
+          <t>SI-6 d,CM-3 (5)</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -4494,7 +4494,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -4569,7 +4569,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -4644,7 +4644,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -4719,7 +4719,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -4794,7 +4794,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -4869,7 +4869,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -4944,7 +4944,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -5019,7 +5019,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -5094,7 +5094,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -5169,7 +5169,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-7 a,AU-7 b,AU-12 (3),AU-12 a,CM-6 b,CM-5 (1),AU-12 c,AU-8 b</t>
+          <t>AU-12 a,CM-5 (1),CM-6 b,AU-8 b,AU-7 a,AU-7 b,AU-12 c,AU-12 (3)</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5243,7 +5243,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5324,7 +5324,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5405,7 +5405,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5487,7 +5487,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5569,7 +5569,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5651,7 +5651,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5733,7 +5733,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5815,7 +5815,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 a</t>
+          <t>SI-6 a,CM-3 (5)</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -6853,7 +6853,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -6927,7 +6927,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -7001,7 +7001,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -7075,7 +7075,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -7155,7 +7155,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -7240,7 +7240,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (6),AC-17 (2)</t>
+          <t>AC-17 (2),MA-4 (6)</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -7316,7 +7316,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -7651,7 +7651,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -7726,7 +7726,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -7801,7 +7801,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -7876,7 +7876,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -7956,7 +7956,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -8038,7 +8038,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -8120,7 +8120,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8202,7 +8202,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8284,7 +8284,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8366,7 +8366,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -8446,7 +8446,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -8526,7 +8526,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -8606,7 +8606,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 (1)</t>
+          <t>AC-11 (1),AC-11 b</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -9354,7 +9354,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>SC-13,SC-8,AC-17 (2),MA-4 c</t>
+          <t>AC-17 (2),SC-8,SC-13,MA-4 c</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9436,7 +9436,7 @@
     <row r="114" ht="130" customHeight="1">
       <c r="A114" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B114" s="2" t="inlineStr">
@@ -9514,7 +9514,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9592,7 +9592,7 @@
     <row r="116" ht="130" customHeight="1">
       <c r="A116" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B116" s="2" t="inlineStr">
@@ -9670,7 +9670,7 @@
     <row r="117" ht="130" customHeight="1">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -10026,7 +10026,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -10106,7 +10106,7 @@
     <row r="123" ht="130" customHeight="1">
       <c r="A123" s="2" t="inlineStr">
         <is>
-          <t>SC-28 (1),SC-28</t>
+          <t>SC-28,SC-28 (1)</t>
         </is>
       </c>
       <c r="B123" s="2" t="inlineStr">
@@ -10873,7 +10873,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10954,7 +10954,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -11040,7 +11040,7 @@
     <row r="135" ht="130" customHeight="1">
       <c r="A135" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B135" s="2" t="inlineStr">
@@ -11133,7 +11133,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>AC-3 (4),AC-6 (10)</t>
+          <t>AC-6 (10),AC-3 (4)</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -11230,7 +11230,7 @@
     <row r="137" ht="130" customHeight="1">
       <c r="A137" s="2" t="inlineStr">
         <is>
-          <t>AC-3 (4),AC-6 (10)</t>
+          <t>AC-6 (10),AC-3 (4)</t>
         </is>
       </c>
       <c r="B137" s="2" t="inlineStr">
@@ -11406,7 +11406,7 @@
     <row r="139" ht="130" customHeight="1">
       <c r="A139" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B139" s="3" t="inlineStr">
@@ -11486,7 +11486,7 @@
     <row r="140" ht="130" customHeight="1">
       <c r="A140" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B140" s="3" t="inlineStr">
@@ -11566,7 +11566,7 @@
     <row r="141" ht="130" customHeight="1">
       <c r="A141" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B141" s="3" t="inlineStr">
@@ -11646,7 +11646,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B142" s="3" t="inlineStr">
@@ -11958,7 +11958,7 @@
     <row r="146" ht="130" customHeight="1">
       <c r="A146" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),IA-7</t>
+          <t>IA-7,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B146" s="2" t="inlineStr">
@@ -12429,7 +12429,7 @@
     <row r="152" ht="130" customHeight="1">
       <c r="A152" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B152" s="2" t="inlineStr">
@@ -12505,7 +12505,7 @@
     <row r="153" ht="130" customHeight="1">
       <c r="A153" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B153" s="2" t="inlineStr">
@@ -12590,7 +12590,7 @@
     <row r="154" ht="130" customHeight="1">
       <c r="A154" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B154" s="2" t="inlineStr">
@@ -12826,7 +12826,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B157" s="3" t="inlineStr">
@@ -12903,7 +12903,7 @@
     <row r="158" ht="130" customHeight="1">
       <c r="A158" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B158" s="3" t="inlineStr">
@@ -12976,7 +12976,7 @@
     <row r="159" ht="130" customHeight="1">
       <c r="A159" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B159" s="3" t="inlineStr">
@@ -13049,7 +13049,7 @@
     <row r="160" ht="130" customHeight="1">
       <c r="A160" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B160" s="3" t="inlineStr">
@@ -13134,7 +13134,7 @@
     <row r="161" ht="130" customHeight="1">
       <c r="A161" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B161" s="3" t="inlineStr">
@@ -13209,7 +13209,7 @@
     <row r="162" ht="130" customHeight="1">
       <c r="A162" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B162" s="3" t="inlineStr">
@@ -13284,7 +13284,7 @@
     <row r="163" ht="130" customHeight="1">
       <c r="A163" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B163" s="3" t="inlineStr">
@@ -13359,7 +13359,7 @@
     <row r="164" ht="130" customHeight="1">
       <c r="A164" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B164" s="3" t="inlineStr">
@@ -13862,7 +13862,7 @@
     <row r="171" ht="130" customHeight="1">
       <c r="A171" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B171" s="3" t="inlineStr">
@@ -14151,7 +14151,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B175" s="3" t="inlineStr">
@@ -14226,7 +14226,7 @@
     <row r="176" ht="130" customHeight="1">
       <c r="A176" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B176" s="3" t="inlineStr">
@@ -14308,7 +14308,7 @@
     <row r="177" ht="130" customHeight="1">
       <c r="A177" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B177" s="3" t="inlineStr">
@@ -14390,7 +14390,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B178" s="3" t="inlineStr">
@@ -14472,7 +14472,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B179" s="3" t="inlineStr">
@@ -14554,7 +14554,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B180" s="3" t="inlineStr">
@@ -14636,7 +14636,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B181" s="3" t="inlineStr">
@@ -14718,7 +14718,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B182" s="3" t="inlineStr">
@@ -14800,7 +14800,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B183" s="3" t="inlineStr">
@@ -14882,7 +14882,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B184" s="3" t="inlineStr">
@@ -14964,7 +14964,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B185" s="3" t="inlineStr">
@@ -15042,7 +15042,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B186" s="3" t="inlineStr">
@@ -15121,7 +15121,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B187" s="3" t="inlineStr">
@@ -15203,7 +15203,7 @@
     <row r="188" ht="130" customHeight="1">
       <c r="A188" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B188" s="3" t="inlineStr">
@@ -15285,7 +15285,7 @@
     <row r="189" ht="130" customHeight="1">
       <c r="A189" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B189" s="3" t="inlineStr">
@@ -15367,7 +15367,7 @@
     <row r="190" ht="130" customHeight="1">
       <c r="A190" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B190" s="3" t="inlineStr">
@@ -15449,7 +15449,7 @@
     <row r="191" ht="130" customHeight="1">
       <c r="A191" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B191" s="3" t="inlineStr">
@@ -15531,7 +15531,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B192" s="3" t="inlineStr">
@@ -15613,7 +15613,7 @@
     <row r="193" ht="130" customHeight="1">
       <c r="A193" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B193" s="3" t="inlineStr">
@@ -15688,7 +15688,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B194" s="3" t="inlineStr">
@@ -15761,7 +15761,7 @@
     <row r="195" ht="130" customHeight="1">
       <c r="A195" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-12 c</t>
+          <t>AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B195" s="3" t="inlineStr">
@@ -15838,7 +15838,7 @@
     <row r="196" ht="130" customHeight="1">
       <c r="A196" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (4),IA-2 (3),IA-2 (1)</t>
+          <t>IA-2 (1),IA-2 (2),IA-2 (4),IA-2 (3)</t>
         </is>
       </c>
       <c r="B196" s="2" t="inlineStr">
@@ -15925,7 +15925,7 @@
     <row r="197" ht="130" customHeight="1">
       <c r="A197" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (5),IA-2 (2),IA-2 (4),IA-2</t>
+          <t>IA-2 (4),IA-2 (5),IA-2 (2),IA-2 (3),IA-2</t>
         </is>
       </c>
       <c r="B197" s="2" t="inlineStr">
@@ -16014,7 +16014,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (5),IA-2 (2),IA-2 (4),IA-2</t>
+          <t>IA-2 (4),IA-2 (5),IA-2 (2),IA-2 (3),IA-2</t>
         </is>
       </c>
       <c r="B198" s="2" t="inlineStr">
@@ -16638,7 +16638,7 @@
     <row r="206" ht="130" customHeight="1">
       <c r="A206" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8 (2),SC-8</t>
+          <t>SC-8 (2),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B206" s="2" t="inlineStr">
@@ -16715,7 +16715,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8 (2),SC-8</t>
+          <t>SC-8 (2),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -16801,7 +16801,7 @@
     <row r="208" ht="130" customHeight="1">
       <c r="A208" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),AC-18 (1),SC-8</t>
+          <t>AC-18 (1),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B208" s="2" t="inlineStr">
@@ -17389,7 +17389,7 @@
     <row r="215" ht="130" customHeight="1">
       <c r="A215" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-12 a</t>
+          <t>AU-12 a,CM-6 b</t>
         </is>
       </c>
       <c r="B215" s="3" t="inlineStr">
@@ -17475,7 +17475,7 @@
     <row r="216" ht="130" customHeight="1">
       <c r="A216" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-5 (2),SC-5</t>
+          <t>SC-5 (2),SC-5,CM-6 b</t>
         </is>
       </c>
       <c r="B216" s="2" t="inlineStr">
@@ -17747,7 +17747,7 @@
     <row r="219" ht="130" customHeight="1">
       <c r="A219" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-16</t>
+          <t>SI-16,CM-6 b</t>
         </is>
       </c>
       <c r="B219" s="2" t="inlineStr">
@@ -17845,7 +17845,7 @@
     <row r="220" ht="130" customHeight="1">
       <c r="A220" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),IA-8,IA-2</t>
+          <t>IA-8,AU-3 (1),IA-2</t>
         </is>
       </c>
       <c r="B220" s="2" t="inlineStr">
@@ -18824,7 +18824,7 @@
     <row r="232" ht="130" customHeight="1">
       <c r="A232" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-16,SC-2</t>
+          <t>SI-16,SC-2,CM-6 b</t>
         </is>
       </c>
       <c r="B232" s="2" t="inlineStr">
@@ -19008,7 +19008,7 @@
     <row r="234" ht="130" customHeight="1">
       <c r="A234" s="2" t="inlineStr">
         <is>
-          <t>SI-16,SC-3</t>
+          <t>SC-3,SI-16</t>
         </is>
       </c>
       <c r="B234" s="2" t="inlineStr">
@@ -19732,7 +19732,7 @@
     <row r="243" ht="130" customHeight="1">
       <c r="A243" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (a),IA-5 (1) (b)</t>
+          <t>CM-6 b,IA-5 (1) (b),IA-5 (1) (a)</t>
         </is>
       </c>
       <c r="B243" s="2" t="inlineStr">
@@ -20381,7 +20381,7 @@
     <row r="251" ht="130" customHeight="1">
       <c r="A251" s="3" t="inlineStr">
         <is>
-          <t>SC-4,SC-2</t>
+          <t>SC-2,SC-4</t>
         </is>
       </c>
       <c r="B251" s="3" t="inlineStr">
@@ -20469,7 +20469,7 @@
     <row r="252" ht="130" customHeight="1">
       <c r="A252" s="3" t="inlineStr">
         <is>
-          <t>SC-4,SC-2</t>
+          <t>SC-2,SC-4</t>
         </is>
       </c>
       <c r="B252" s="3" t="inlineStr">
@@ -20645,7 +20645,7 @@
     <row r="254" ht="130" customHeight="1">
       <c r="A254" s="3" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B254" s="3" t="inlineStr">
@@ -20970,7 +20970,7 @@
     <row r="258" ht="130" customHeight="1">
       <c r="A258" s="2" t="inlineStr">
         <is>
-          <t>SI-6 a,SC-3</t>
+          <t>SC-3,SI-6 a</t>
         </is>
       </c>
       <c r="B258" s="2" t="inlineStr">
@@ -22366,7 +22366,7 @@
     <row r="275" ht="130" customHeight="1">
       <c r="A275" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B275" s="3" t="inlineStr">
@@ -23880,7 +23880,7 @@
     <row r="294" ht="130" customHeight="1">
       <c r="A294" s="3" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 (1)</t>
+          <t>AU-5 (1),AU-5 a</t>
         </is>
       </c>
       <c r="B294" s="3" t="inlineStr">
@@ -27242,7 +27242,7 @@
     <row r="339" ht="130" customHeight="1">
       <c r="A339" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),CM-6 b</t>
         </is>
       </c>
       <c r="B339" s="3" t="inlineStr">
@@ -27392,7 +27392,7 @@
     <row r="341" ht="130" customHeight="1">
       <c r="A341" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (2)</t>
+          <t>IA-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B341" s="2" t="inlineStr">
@@ -27473,7 +27473,7 @@
     <row r="342" ht="130" customHeight="1">
       <c r="A342" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (1)</t>
+          <t>CM-5 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B342" s="3" t="inlineStr">
@@ -27547,7 +27547,7 @@
     <row r="343" ht="130" customHeight="1">
       <c r="A343" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (1)</t>
+          <t>CM-5 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B343" s="3" t="inlineStr">
@@ -28132,7 +28132,7 @@
     <row r="351" ht="130" customHeight="1">
       <c r="A351" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-17 (2)</t>
+          <t>AC-17 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B351" s="2" t="inlineStr">
@@ -29869,7 +29869,7 @@
     <row r="374" ht="130" customHeight="1">
       <c r="A374" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-3</t>
+          <t>AU-3,CM-6 b</t>
         </is>
       </c>
       <c r="B374" s="3" t="inlineStr">
@@ -30113,7 +30113,7 @@
     <row r="377" ht="130" customHeight="1">
       <c r="A377" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B377" s="2" t="inlineStr">
@@ -30507,7 +30507,7 @@
     <row r="382" ht="130" customHeight="1">
       <c r="A382" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 b,AC-17 (9),AC-17 (1)</t>
+          <t>AC-17 (9),CM-7 b,AC-17 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B382" s="2" t="inlineStr">
@@ -30585,7 +30585,7 @@
     <row r="383" ht="130" customHeight="1">
       <c r="A383" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 b,AC-17 (1)</t>
+          <t>CM-7 b,AC-17 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B383" s="2" t="inlineStr">
@@ -33859,7 +33859,7 @@
     <row r="422" ht="130" customHeight="1">
       <c r="A422" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B422" s="2" t="inlineStr">
@@ -34040,7 +34040,7 @@
     <row r="424" ht="130" customHeight="1">
       <c r="A424" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-2</t>
+          <t>SC-2,CM-6 b</t>
         </is>
       </c>
       <c r="B424" s="3" t="inlineStr">
@@ -34127,7 +34127,7 @@
     <row r="425" ht="130" customHeight="1">
       <c r="A425" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-2</t>
+          <t>SC-2,CM-6 b</t>
         </is>
       </c>
       <c r="B425" s="3" t="inlineStr">
@@ -34462,7 +34462,7 @@
     <row r="429" ht="130" customHeight="1">
       <c r="A429" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B429" s="2" t="inlineStr">
@@ -35703,7 +35703,7 @@
     <row r="445" ht="130" customHeight="1">
       <c r="A445" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-2 (2)</t>
+          <t>SI-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B445" s="3" t="inlineStr">
@@ -36350,7 +36350,7 @@
     <row r="454" ht="130" customHeight="1">
       <c r="A454" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-2 (2)</t>
+          <t>SI-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B454" s="3" t="inlineStr">
@@ -36641,7 +36641,7 @@
     <row r="458" ht="130" customHeight="1">
       <c r="A458" s="3" t="inlineStr">
         <is>
-          <t>AC-12,MA-4 (7),SC-10,MA-4 e</t>
+          <t>MA-4 (7),SC-10,MA-4 e,AC-12</t>
         </is>
       </c>
       <c r="B458" s="3" t="inlineStr">
@@ -36871,7 +36871,7 @@
     <row r="461" ht="130" customHeight="1">
       <c r="A461" s="3" t="inlineStr">
         <is>
-          <t>SC-10,AC-11 a</t>
+          <t>AC-11 a,SC-10</t>
         </is>
       </c>
       <c r="B461" s="3" t="inlineStr">
@@ -36948,7 +36948,7 @@
     <row r="462" ht="130" customHeight="1">
       <c r="A462" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8,AC-17 (2)</t>
+          <t>AC-17 (2),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B462" s="2" t="inlineStr">
@@ -38256,7 +38256,7 @@
     <row r="479" ht="130" customHeight="1">
       <c r="A479" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-7 b</t>
+          <t>CM-7 b,IA-3</t>
         </is>
       </c>
       <c r="B479" s="2" t="inlineStr">
@@ -39698,7 +39698,7 @@
     <row r="497" ht="130" customHeight="1">
       <c r="A497" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-4 (1)</t>
+          <t>AU-4 (1),AU-4</t>
         </is>
       </c>
       <c r="B497" s="2" t="inlineStr">
@@ -42608,7 +42608,7 @@
     <row r="533" ht="130" customHeight="1">
       <c r="A533" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2)</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B533" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@83a7e566fd8b8b2645b149f7ff0bde98f7d09f58 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -550,7 +550,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -634,7 +634,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -719,7 +719,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -791,7 +791,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -973,7 +973,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>AU-5 b,AU-5 a</t>
+          <t>AU-5 a,AU-5 b</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -1455,7 +1455,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,CM-5 (1),MA-4 (1) (a),CM-6 b,AU-6 (4),AU-7 (1),AU-14 (1),AU-7 a,AU-3 (1)</t>
+          <t>AU-3,CM-6 b,AU-6 (4),AU-3 (1),CM-5 (1),AU-7 (1),AU-7 a,AU-12 a,MA-4 (1) (a),AU-14 (1)</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -1540,7 +1540,7 @@
     <row r="14" ht="130" customHeight="1">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -1616,7 +1616,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -3258,7 +3258,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-14 (1),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a),AU-14 (1)</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3349,7 +3349,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),AU-4</t>
+          <t>AU-4,AU-14 (1)</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3832,7 +3832,7 @@
     <row r="44" ht="130" customHeight="1">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>AU-6 (4),CM-6 b,AU-4 (1)</t>
+          <t>AU-6 (4),AU-4 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
@@ -3908,7 +3908,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-4 (1)</t>
+          <t>AU-4 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3993,7 +3993,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-8 (1) (b),AU-8 (1) (a)</t>
+          <t>AU-8 b,AU-8 (1) (a),AU-8 (1) (b)</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -4318,7 +4318,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>SI-6 d,SI-6 b,CM-3 (5)</t>
+          <t>SI-6 b,CM-3 (5),SI-6 d</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4410,7 +4410,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>SI-6 d,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 d</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -4494,7 +4494,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -4569,7 +4569,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -4644,7 +4644,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -4719,7 +4719,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -4794,7 +4794,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -4869,7 +4869,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -4944,7 +4944,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -5019,7 +5019,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -5094,7 +5094,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -5169,7 +5169,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,CM-5 (1),CM-6 b,AU-8 b,AU-7 a,AU-7 b,AU-12 c,AU-12 (3)</t>
+          <t>CM-6 b,AU-12 c,AU-12 (3),AU-7 b,CM-5 (1),AU-7 a,AU-12 a,AU-8 b</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5243,7 +5243,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AC-2 (4),AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5324,7 +5324,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AC-2 (4),AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5405,7 +5405,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AC-2 (4),AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5487,7 +5487,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AC-2 (4),AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5569,7 +5569,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AC-2 (4),AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5651,7 +5651,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AC-2 (4),AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5733,7 +5733,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AC-2 (4),AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5815,7 +5815,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>SI-6 a,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 a</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5889,7 +5889,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5972,7 +5972,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -6050,7 +6050,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -6141,7 +6141,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6223,7 +6223,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6853,7 +6853,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -6927,7 +6927,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -7001,7 +7001,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -7075,7 +7075,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -7155,7 +7155,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -7240,7 +7240,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>AC-17 (2),MA-4 (6)</t>
+          <t>MA-4 (6),AC-17 (2)</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -7316,7 +7316,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -7651,7 +7651,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -7726,7 +7726,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -7801,7 +7801,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -7876,7 +7876,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -7956,7 +7956,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -8038,7 +8038,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -8120,7 +8120,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8202,7 +8202,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8284,7 +8284,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8366,7 +8366,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -8446,7 +8446,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -8526,7 +8526,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -8606,7 +8606,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AC-11 (1),AC-11 b</t>
+          <t>AC-11 b,AC-11 (1)</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -9354,7 +9354,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8,SC-13,MA-4 c</t>
+          <t>AC-17 (2),SC-13,SC-8,MA-4 c</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9436,7 +9436,7 @@
     <row r="114" ht="130" customHeight="1">
       <c r="A114" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B114" s="2" t="inlineStr">
@@ -9514,7 +9514,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9592,7 +9592,7 @@
     <row r="116" ht="130" customHeight="1">
       <c r="A116" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B116" s="2" t="inlineStr">
@@ -9670,7 +9670,7 @@
     <row r="117" ht="130" customHeight="1">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -9750,7 +9750,7 @@
     <row r="118" ht="130" customHeight="1">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
@@ -9819,7 +9819,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
@@ -9888,7 +9888,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
@@ -9957,7 +9957,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
@@ -10026,7 +10026,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -10873,7 +10873,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10954,7 +10954,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -11040,7 +11040,7 @@
     <row r="135" ht="130" customHeight="1">
       <c r="A135" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B135" s="2" t="inlineStr">
@@ -11406,7 +11406,7 @@
     <row r="139" ht="130" customHeight="1">
       <c r="A139" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B139" s="3" t="inlineStr">
@@ -11486,7 +11486,7 @@
     <row r="140" ht="130" customHeight="1">
       <c r="A140" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B140" s="3" t="inlineStr">
@@ -11566,7 +11566,7 @@
     <row r="141" ht="130" customHeight="1">
       <c r="A141" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B141" s="3" t="inlineStr">
@@ -11646,7 +11646,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B142" s="3" t="inlineStr">
@@ -12268,7 +12268,7 @@
     <row r="150" ht="130" customHeight="1">
       <c r="A150" s="2" t="inlineStr">
         <is>
-          <t>AC-11 (1),AC-11 a</t>
+          <t>AC-11 a,AC-11 (1)</t>
         </is>
       </c>
       <c r="B150" s="2" t="inlineStr">
@@ -12747,7 +12747,7 @@
     <row r="156" ht="130" customHeight="1">
       <c r="A156" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,IA-7</t>
+          <t>IA-7,CM-7 a</t>
         </is>
       </c>
       <c r="B156" s="2" t="inlineStr">
@@ -12826,7 +12826,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B157" s="3" t="inlineStr">
@@ -12903,7 +12903,7 @@
     <row r="158" ht="130" customHeight="1">
       <c r="A158" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B158" s="3" t="inlineStr">
@@ -12976,7 +12976,7 @@
     <row r="159" ht="130" customHeight="1">
       <c r="A159" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B159" s="3" t="inlineStr">
@@ -13049,7 +13049,7 @@
     <row r="160" ht="130" customHeight="1">
       <c r="A160" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B160" s="3" t="inlineStr">
@@ -13134,7 +13134,7 @@
     <row r="161" ht="130" customHeight="1">
       <c r="A161" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B161" s="3" t="inlineStr">
@@ -13209,7 +13209,7 @@
     <row r="162" ht="130" customHeight="1">
       <c r="A162" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B162" s="3" t="inlineStr">
@@ -13284,7 +13284,7 @@
     <row r="163" ht="130" customHeight="1">
       <c r="A163" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B163" s="3" t="inlineStr">
@@ -13359,7 +13359,7 @@
     <row r="164" ht="130" customHeight="1">
       <c r="A164" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B164" s="3" t="inlineStr">
@@ -13434,7 +13434,7 @@
     <row r="165" ht="130" customHeight="1">
       <c r="A165" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B165" s="3" t="inlineStr">
@@ -13505,7 +13505,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B166" s="3" t="inlineStr">
@@ -13576,7 +13576,7 @@
     <row r="167" ht="130" customHeight="1">
       <c r="A167" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B167" s="3" t="inlineStr">
@@ -13648,7 +13648,7 @@
     <row r="168" ht="130" customHeight="1">
       <c r="A168" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B168" s="3" t="inlineStr">
@@ -13719,7 +13719,7 @@
     <row r="169" ht="130" customHeight="1">
       <c r="A169" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B169" s="3" t="inlineStr">
@@ -13790,7 +13790,7 @@
     <row r="170" ht="130" customHeight="1">
       <c r="A170" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B170" s="3" t="inlineStr">
@@ -13862,7 +13862,7 @@
     <row r="171" ht="130" customHeight="1">
       <c r="A171" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B171" s="3" t="inlineStr">
@@ -13937,7 +13937,7 @@
     <row r="172" ht="130" customHeight="1">
       <c r="A172" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B172" s="3" t="inlineStr">
@@ -14008,7 +14008,7 @@
     <row r="173" ht="130" customHeight="1">
       <c r="A173" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B173" s="3" t="inlineStr">
@@ -14079,7 +14079,7 @@
     <row r="174" ht="130" customHeight="1">
       <c r="A174" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B174" s="3" t="inlineStr">
@@ -14151,7 +14151,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B175" s="3" t="inlineStr">
@@ -14226,7 +14226,7 @@
     <row r="176" ht="130" customHeight="1">
       <c r="A176" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B176" s="3" t="inlineStr">
@@ -14308,7 +14308,7 @@
     <row r="177" ht="130" customHeight="1">
       <c r="A177" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B177" s="3" t="inlineStr">
@@ -14390,7 +14390,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B178" s="3" t="inlineStr">
@@ -14472,7 +14472,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3,AU-3 (1)</t>
         </is>
       </c>
       <c r="B179" s="3" t="inlineStr">
@@ -14554,7 +14554,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B180" s="3" t="inlineStr">
@@ -14636,7 +14636,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B181" s="3" t="inlineStr">
@@ -14718,7 +14718,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B182" s="3" t="inlineStr">
@@ -14800,7 +14800,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B183" s="3" t="inlineStr">
@@ -14882,7 +14882,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B184" s="3" t="inlineStr">
@@ -15042,7 +15042,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B186" s="3" t="inlineStr">
@@ -15121,7 +15121,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B187" s="3" t="inlineStr">
@@ -15203,7 +15203,7 @@
     <row r="188" ht="130" customHeight="1">
       <c r="A188" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B188" s="3" t="inlineStr">
@@ -15285,7 +15285,7 @@
     <row r="189" ht="130" customHeight="1">
       <c r="A189" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B189" s="3" t="inlineStr">
@@ -15367,7 +15367,7 @@
     <row r="190" ht="130" customHeight="1">
       <c r="A190" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B190" s="3" t="inlineStr">
@@ -15449,7 +15449,7 @@
     <row r="191" ht="130" customHeight="1">
       <c r="A191" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B191" s="3" t="inlineStr">
@@ -15531,7 +15531,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B192" s="3" t="inlineStr">
@@ -15613,7 +15613,7 @@
     <row r="193" ht="130" customHeight="1">
       <c r="A193" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B193" s="3" t="inlineStr">
@@ -15688,7 +15688,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AC-2 (4),AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B194" s="3" t="inlineStr">
@@ -15761,7 +15761,7 @@
     <row r="195" ht="130" customHeight="1">
       <c r="A195" s="3" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AC-2 (4),AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AC-2 (4),AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B195" s="3" t="inlineStr">
@@ -15838,7 +15838,7 @@
     <row r="196" ht="130" customHeight="1">
       <c r="A196" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (2),IA-2 (4),IA-2 (3)</t>
+          <t>IA-2 (3),IA-2 (1),IA-2 (4),IA-2 (2)</t>
         </is>
       </c>
       <c r="B196" s="2" t="inlineStr">
@@ -15925,7 +15925,7 @@
     <row r="197" ht="130" customHeight="1">
       <c r="A197" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2 (5),IA-2 (2),IA-2 (3),IA-2</t>
+          <t>IA-2 (5),IA-2 (2),IA-2 (3),IA-2,IA-2 (4)</t>
         </is>
       </c>
       <c r="B197" s="2" t="inlineStr">
@@ -16014,7 +16014,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2 (5),IA-2 (2),IA-2 (3),IA-2</t>
+          <t>IA-2 (5),IA-2 (2),IA-2 (3),IA-2,IA-2 (4)</t>
         </is>
       </c>
       <c r="B198" s="2" t="inlineStr">
@@ -16638,7 +16638,7 @@
     <row r="206" ht="130" customHeight="1">
       <c r="A206" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8,SC-8 (1)</t>
+          <t>SC-8 (1),SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B206" s="2" t="inlineStr">
@@ -16715,7 +16715,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8,SC-8 (1)</t>
+          <t>SC-8 (1),SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -16801,7 +16801,7 @@
     <row r="208" ht="130" customHeight="1">
       <c r="A208" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),SC-8,SC-8 (1)</t>
+          <t>SC-8,AC-18 (1),SC-8 (1)</t>
         </is>
       </c>
       <c r="B208" s="2" t="inlineStr">
@@ -16887,7 +16887,7 @@
     <row r="209" ht="130" customHeight="1">
       <c r="A209" s="2" t="inlineStr">
         <is>
-          <t>AC-11 (1),AC-11 a</t>
+          <t>AC-11 a,AC-11 (1)</t>
         </is>
       </c>
       <c r="B209" s="2" t="inlineStr">
@@ -16976,7 +16976,7 @@
     <row r="210" ht="130" customHeight="1">
       <c r="A210" s="2" t="inlineStr">
         <is>
-          <t>AC-11 (1),AC-11 a</t>
+          <t>AC-11 a,AC-11 (1)</t>
         </is>
       </c>
       <c r="B210" s="2" t="inlineStr">
@@ -17229,7 +17229,7 @@
     <row r="213" ht="130" customHeight="1">
       <c r="A213" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,IA-5 (1) (c),CM-6 b</t>
+          <t>IA-5 (1) (c),CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B213" s="2" t="inlineStr">
@@ -17389,7 +17389,7 @@
     <row r="215" ht="130" customHeight="1">
       <c r="A215" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,CM-6 b</t>
+          <t>CM-6 b,AU-12 a</t>
         </is>
       </c>
       <c r="B215" s="3" t="inlineStr">
@@ -17475,7 +17475,7 @@
     <row r="216" ht="130" customHeight="1">
       <c r="A216" s="2" t="inlineStr">
         <is>
-          <t>SC-5 (2),SC-5,CM-6 b</t>
+          <t>SC-5,CM-6 b,SC-5 (2)</t>
         </is>
       </c>
       <c r="B216" s="2" t="inlineStr">
@@ -17655,7 +17655,7 @@
     <row r="218" ht="130" customHeight="1">
       <c r="A218" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,SI-16</t>
+          <t>SI-16,CM-7 a</t>
         </is>
       </c>
       <c r="B218" s="2" t="inlineStr">
@@ -17845,7 +17845,7 @@
     <row r="220" ht="130" customHeight="1">
       <c r="A220" s="2" t="inlineStr">
         <is>
-          <t>IA-8,AU-3 (1),IA-2</t>
+          <t>IA-2,IA-8,AU-3 (1)</t>
         </is>
       </c>
       <c r="B220" s="2" t="inlineStr">
@@ -18824,7 +18824,7 @@
     <row r="232" ht="130" customHeight="1">
       <c r="A232" s="2" t="inlineStr">
         <is>
-          <t>SI-16,SC-2,CM-6 b</t>
+          <t>SC-2,SI-16,CM-6 b</t>
         </is>
       </c>
       <c r="B232" s="2" t="inlineStr">
@@ -19008,7 +19008,7 @@
     <row r="234" ht="130" customHeight="1">
       <c r="A234" s="2" t="inlineStr">
         <is>
-          <t>SC-3,SI-16</t>
+          <t>SI-16,SC-3</t>
         </is>
       </c>
       <c r="B234" s="2" t="inlineStr">
@@ -19170,7 +19170,7 @@
     <row r="236" ht="130" customHeight="1">
       <c r="A236" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,AC-18 (1)</t>
+          <t>AC-18 (1),CM-7 a</t>
         </is>
       </c>
       <c r="B236" s="2" t="inlineStr">
@@ -19732,7 +19732,7 @@
     <row r="243" ht="130" customHeight="1">
       <c r="A243" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (b),IA-5 (1) (a)</t>
+          <t>IA-5 (1) (b),IA-5 (1) (a),CM-6 b</t>
         </is>
       </c>
       <c r="B243" s="2" t="inlineStr">
@@ -20970,7 +20970,7 @@
     <row r="258" ht="130" customHeight="1">
       <c r="A258" s="2" t="inlineStr">
         <is>
-          <t>SC-3,SI-6 a</t>
+          <t>SI-6 a,SC-3</t>
         </is>
       </c>
       <c r="B258" s="2" t="inlineStr">
@@ -21052,7 +21052,7 @@
     <row r="259" ht="130" customHeight="1">
       <c r="A259" s="3" t="inlineStr">
         <is>
-          <t>AC-6 (9),AC-6 (8)</t>
+          <t>AC-6 (8),AC-6 (9)</t>
         </is>
       </c>
       <c r="B259" s="3" t="inlineStr">
@@ -22286,45 +22286,45 @@
       <c r="Q273" s="2" t="n"/>
     </row>
     <row r="274" ht="130" customHeight="1">
-      <c r="A274" s="3" t="inlineStr">
+      <c r="A274" s="2" t="inlineStr">
         <is>
           <t>IA-5 (1) (a)</t>
         </is>
       </c>
-      <c r="B274" s="3" t="inlineStr">
+      <c r="B274" s="2" t="inlineStr">
         <is>
           <t>CCI-000192</t>
         </is>
       </c>
-      <c r="C274" s="3" t="inlineStr">
+      <c r="C274" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000069-GPOS-00037</t>
         </is>
       </c>
-      <c r="D274" s="3" t="inlineStr">
+      <c r="D274" s="2" t="inlineStr">
         <is>
           <t>CCE-83568-6</t>
         </is>
       </c>
-      <c r="E274" s="3" t="inlineStr">
+      <c r="E274" s="2" t="inlineStr">
         <is>
           <t>The operating system must enforce password complexity by requiring that at least one upper-case character be used.</t>
         </is>
       </c>
-      <c r="F274" s="3" t="inlineStr">
+      <c r="F274" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 must enforce password complexity by requiring that at least one upper-case character be used.</t>
         </is>
       </c>
-      <c r="G274" s="3" t="inlineStr">
+      <c r="G274" s="2" t="inlineStr">
         <is>
           <t>Use of a complex password helps to increase the time and resources required to compromise the password. Password complexity, or strength, is a measure of the effectiveness of a password in resisting attempts at guessing and brute-force attacks.
 Password complexity is one factor of several that determines how long it takes to crack a password. The more complex the password, the greater the number of possible combinations that need to be tested before the password is compromised.</t>
         </is>
       </c>
-      <c r="H274" s="3" t="inlineStr">
-        <is>
-          <t>Use of a complex password helps to increase the time and resources reuiqred to compromise the password.
+      <c r="H274" s="2" t="inlineStr">
+        <is>
+          <t>Use of a complex password helps to increase the time and resources required to compromise the password.
 Password complexity, or strength, is a measure of the effectiveness of a password in resisting attempts
 at guessing and brute-force attacks.
 Password complexity is one factor of several that determines how long it takes to crack a password. The more
@@ -22332,41 +22332,46 @@
 the password is compromised.</t>
         </is>
       </c>
-      <c r="I274" s="3" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J274" s="3" t="inlineStr">
+      <c r="I274" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J274" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system enforces password complexity by requiring that at least one upper-case character be used. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K274" s="3" t="inlineStr">
+      <c r="K274" s="2" t="inlineStr">
         <is>
           <t>To check how many uppercase characters are required in a password, run the following command:
  $ grep ucredit /etc/security/pwquality.conf 
 The "ucredit" parameter (as a negative number) will indicate how many uppercase characters are required.
-The DoD and FISMA require at least one uppercase character in a password.
 This would appear as "ucredit = -1".
-If ucredit is not found or not set less than or equal to the required value, then this is a finding.</t>
-        </is>
-      </c>
-      <c r="L274" s="3" t="n"/>
-      <c r="M274" s="3" t="inlineStr"/>
-      <c r="N274" s="3" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O274" s="3" t="n"/>
-      <c r="P274" s="3" t="n"/>
-      <c r="Q274" s="3" t="n"/>
+If ucredit is not found or not set to the required value, then this is a finding.</t>
+        </is>
+      </c>
+      <c r="L274" s="2" t="n"/>
+      <c r="M274" s="2" t="inlineStr">
+        <is>
+          <t>Configure Red Hat Enterprise Linux 9 to enforce password complexity by requiring that at least one upper-case character be used by setting the "ucredit" option.
+Add the following line to /etc/security/pwquality.conf (or modify the line to have the required value):
+ucredit = -1</t>
+        </is>
+      </c>
+      <c r="N274" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O274" s="2" t="n"/>
+      <c r="P274" s="2" t="n"/>
+      <c r="Q274" s="2" t="n"/>
     </row>
     <row r="275" ht="130" customHeight="1">
       <c r="A275" s="3" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B275" s="3" t="inlineStr">
@@ -22514,7 +22519,7 @@
     <row r="277" ht="130" customHeight="1">
       <c r="A277" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-7 b</t>
+          <t>CM-7 b,CM-7 a</t>
         </is>
       </c>
       <c r="B277" s="2" t="inlineStr">
@@ -22594,7 +22599,7 @@
     <row r="278" ht="130" customHeight="1">
       <c r="A278" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-7 b</t>
+          <t>CM-7 b,CM-7 a</t>
         </is>
       </c>
       <c r="B278" s="2" t="inlineStr">
@@ -23362,7 +23367,7 @@
     <row r="288" ht="130" customHeight="1">
       <c r="A288" s="3" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B288" s="3" t="inlineStr">
@@ -23433,7 +23438,7 @@
     <row r="289" ht="130" customHeight="1">
       <c r="A289" s="3" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B289" s="3" t="inlineStr">
@@ -23505,7 +23510,7 @@
     <row r="290" ht="130" customHeight="1">
       <c r="A290" s="3" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B290" s="3" t="inlineStr">
@@ -23663,7 +23668,7 @@
     <row r="292" ht="130" customHeight="1">
       <c r="A292" s="3" t="inlineStr">
         <is>
-          <t>AC-6 (9),AC-2 (4),AU-12 c</t>
+          <t>AU-12 c,AC-6 (9),AC-2 (4)</t>
         </is>
       </c>
       <c r="B292" s="3" t="inlineStr">
@@ -23880,7 +23885,7 @@
     <row r="294" ht="130" customHeight="1">
       <c r="A294" s="3" t="inlineStr">
         <is>
-          <t>AU-5 (1),AU-5 a</t>
+          <t>AU-5 a,AU-5 (1)</t>
         </is>
       </c>
       <c r="B294" s="3" t="inlineStr">
@@ -27392,7 +27397,7 @@
     <row r="341" ht="130" customHeight="1">
       <c r="A341" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),CM-6 b</t>
+          <t>CM-6 b,IA-2 (2)</t>
         </is>
       </c>
       <c r="B341" s="2" t="inlineStr">
@@ -30113,7 +30118,7 @@
     <row r="377" ht="130" customHeight="1">
       <c r="A377" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B377" s="2" t="inlineStr">
@@ -30507,7 +30512,7 @@
     <row r="382" ht="130" customHeight="1">
       <c r="A382" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (9),CM-7 b,AC-17 (1),CM-6 b</t>
+          <t>CM-7 b,AC-17 (1),CM-6 b,AC-17 (9)</t>
         </is>
       </c>
       <c r="B382" s="2" t="inlineStr">
@@ -33859,7 +33864,7 @@
     <row r="422" ht="130" customHeight="1">
       <c r="A422" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B422" s="2" t="inlineStr">
@@ -34462,7 +34467,7 @@
     <row r="429" ht="130" customHeight="1">
       <c r="A429" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B429" s="2" t="inlineStr">
@@ -34914,7 +34919,7 @@
     <row r="435" ht="130" customHeight="1">
       <c r="A435" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-4</t>
+          <t>AU-4,CM-6 b</t>
         </is>
       </c>
       <c r="B435" s="2" t="inlineStr">
@@ -36641,7 +36646,7 @@
     <row r="458" ht="130" customHeight="1">
       <c r="A458" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (7),SC-10,MA-4 e,AC-12</t>
+          <t>AC-12,SC-10,MA-4 (7),MA-4 e</t>
         </is>
       </c>
       <c r="B458" s="3" t="inlineStr">
@@ -36948,7 +36953,7 @@
     <row r="462" ht="130" customHeight="1">
       <c r="A462" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8,SC-8 (1)</t>
+          <t>AC-17 (2),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B462" s="2" t="inlineStr">
@@ -39698,7 +39703,7 @@
     <row r="497" ht="130" customHeight="1">
       <c r="A497" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-4</t>
+          <t>AU-4,AU-4 (1)</t>
         </is>
       </c>
       <c r="B497" s="2" t="inlineStr">
@@ -39949,7 +39954,7 @@
     <row r="500" ht="130" customHeight="1">
       <c r="A500" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B500" s="2" t="inlineStr">
@@ -40051,7 +40056,7 @@
     <row r="501" ht="130" customHeight="1">
       <c r="A501" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B501" s="2" t="inlineStr">
@@ -40161,7 +40166,7 @@
     <row r="502" ht="130" customHeight="1">
       <c r="A502" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B502" s="2" t="inlineStr">
@@ -40272,7 +40277,7 @@
     <row r="503" ht="130" customHeight="1">
       <c r="A503" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B503" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@4f9aa1cf31a502b93f04bce47b9a64b9d19f040a 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -1455,7 +1455,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>AU-3,CM-6 b,AU-6 (4),AU-3 (1),CM-5 (1),AU-7 (1),AU-7 a,AU-12 a,MA-4 (1) (a),AU-14 (1)</t>
+          <t>AU-3,CM-5 (1),AU-12 a,AU-7 a,CM-6 b,AU-7 (1),AU-6 (4),AU-14 (1),AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -3258,7 +3258,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a),AU-14 (1)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-14 (1),AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3349,7 +3349,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-14 (1)</t>
+          <t>AU-14 (1),AU-4</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3832,7 +3832,7 @@
     <row r="44" ht="130" customHeight="1">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>AU-6 (4),AU-4 (1),CM-6 b</t>
+          <t>CM-6 b,AU-4 (1),AU-6 (4)</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
@@ -3908,7 +3908,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),CM-6 b</t>
+          <t>CM-6 b,AU-4 (1)</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3993,7 +3993,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-8 (1) (a),AU-8 (1) (b)</t>
+          <t>AU-8 (1) (b),AU-8 (1) (a),AU-8 b</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -4148,7 +4148,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4234,7 +4234,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (1),IA-2 (12)</t>
+          <t>IA-2 (1),IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4318,7 +4318,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>SI-6 b,CM-3 (5),SI-6 d</t>
+          <t>SI-6 d,CM-3 (5),SI-6 b</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4410,7 +4410,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 d</t>
+          <t>SI-6 d,CM-3 (5)</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -4494,7 +4494,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -4569,7 +4569,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -4644,7 +4644,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -4719,7 +4719,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -4794,7 +4794,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -4869,7 +4869,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -4944,7 +4944,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -5019,7 +5019,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -5094,7 +5094,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -5169,7 +5169,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-12 c,AU-12 (3),AU-7 b,CM-5 (1),AU-7 a,AU-12 a,AU-8 b</t>
+          <t>CM-5 (1),AU-12 a,AU-7 a,CM-6 b,AU-12 (3),AU-12 c,AU-8 b,AU-7 b</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5243,7 +5243,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5324,7 +5324,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5405,7 +5405,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5487,7 +5487,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5569,7 +5569,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5651,7 +5651,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5733,7 +5733,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5889,7 +5889,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5972,7 +5972,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -6050,7 +6050,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -6141,7 +6141,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6223,7 +6223,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6853,7 +6853,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -6927,7 +6927,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -7001,7 +7001,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -7075,7 +7075,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -7155,7 +7155,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -7240,7 +7240,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (6),AC-17 (2)</t>
+          <t>AC-17 (2),MA-4 (6)</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -7316,7 +7316,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -7651,7 +7651,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -7726,7 +7726,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -7801,7 +7801,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -7876,7 +7876,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -7956,7 +7956,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -8038,7 +8038,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -8120,7 +8120,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8202,7 +8202,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8284,7 +8284,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8366,7 +8366,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -8446,7 +8446,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -8526,7 +8526,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -9354,7 +9354,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-13,SC-8,MA-4 c</t>
+          <t>SC-8,AC-17 (2),SC-13,MA-4 c</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9514,7 +9514,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9670,7 +9670,7 @@
     <row r="117" ht="130" customHeight="1">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -10026,7 +10026,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -11133,7 +11133,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),AC-3 (4)</t>
+          <t>AC-3 (4),AC-6 (10)</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -11230,7 +11230,7 @@
     <row r="137" ht="130" customHeight="1">
       <c r="A137" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),AC-3 (4)</t>
+          <t>AC-3 (4),AC-6 (10)</t>
         </is>
       </c>
       <c r="B137" s="2" t="inlineStr">
@@ -11486,7 +11486,7 @@
     <row r="140" ht="130" customHeight="1">
       <c r="A140" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B140" s="3" t="inlineStr">
@@ -11566,7 +11566,7 @@
     <row r="141" ht="130" customHeight="1">
       <c r="A141" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B141" s="3" t="inlineStr">
@@ -11646,7 +11646,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B142" s="3" t="inlineStr">
@@ -12429,7 +12429,7 @@
     <row r="152" ht="130" customHeight="1">
       <c r="A152" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B152" s="2" t="inlineStr">
@@ -12505,7 +12505,7 @@
     <row r="153" ht="130" customHeight="1">
       <c r="A153" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B153" s="2" t="inlineStr">
@@ -12590,7 +12590,7 @@
     <row r="154" ht="130" customHeight="1">
       <c r="A154" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B154" s="2" t="inlineStr">
@@ -12826,7 +12826,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B157" s="3" t="inlineStr">
@@ -12903,7 +12903,7 @@
     <row r="158" ht="130" customHeight="1">
       <c r="A158" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B158" s="3" t="inlineStr">
@@ -12976,7 +12976,7 @@
     <row r="159" ht="130" customHeight="1">
       <c r="A159" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B159" s="3" t="inlineStr">
@@ -13049,7 +13049,7 @@
     <row r="160" ht="130" customHeight="1">
       <c r="A160" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B160" s="3" t="inlineStr">
@@ -13134,7 +13134,7 @@
     <row r="161" ht="130" customHeight="1">
       <c r="A161" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B161" s="3" t="inlineStr">
@@ -13209,7 +13209,7 @@
     <row r="162" ht="130" customHeight="1">
       <c r="A162" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B162" s="3" t="inlineStr">
@@ -13284,7 +13284,7 @@
     <row r="163" ht="130" customHeight="1">
       <c r="A163" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B163" s="3" t="inlineStr">
@@ -13359,7 +13359,7 @@
     <row r="164" ht="130" customHeight="1">
       <c r="A164" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B164" s="3" t="inlineStr">
@@ -13862,7 +13862,7 @@
     <row r="171" ht="130" customHeight="1">
       <c r="A171" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B171" s="3" t="inlineStr">
@@ -14151,7 +14151,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B175" s="3" t="inlineStr">
@@ -14226,7 +14226,7 @@
     <row r="176" ht="130" customHeight="1">
       <c r="A176" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B176" s="3" t="inlineStr">
@@ -14308,7 +14308,7 @@
     <row r="177" ht="130" customHeight="1">
       <c r="A177" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B177" s="3" t="inlineStr">
@@ -14390,7 +14390,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B178" s="3" t="inlineStr">
@@ -14472,7 +14472,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-3 (1)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B179" s="3" t="inlineStr">
@@ -14554,7 +14554,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B180" s="3" t="inlineStr">
@@ -14636,7 +14636,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B181" s="3" t="inlineStr">
@@ -14718,7 +14718,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B182" s="3" t="inlineStr">
@@ -14800,7 +14800,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B183" s="3" t="inlineStr">
@@ -14882,7 +14882,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B184" s="3" t="inlineStr">
@@ -14964,7 +14964,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B185" s="3" t="inlineStr">
@@ -15042,7 +15042,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B186" s="3" t="inlineStr">
@@ -15121,7 +15121,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B187" s="3" t="inlineStr">
@@ -15203,7 +15203,7 @@
     <row r="188" ht="130" customHeight="1">
       <c r="A188" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B188" s="3" t="inlineStr">
@@ -15285,7 +15285,7 @@
     <row r="189" ht="130" customHeight="1">
       <c r="A189" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3,AU-12 c,AU-3 (1)</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B189" s="3" t="inlineStr">
@@ -15367,7 +15367,7 @@
     <row r="190" ht="130" customHeight="1">
       <c r="A190" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B190" s="3" t="inlineStr">
@@ -15449,7 +15449,7 @@
     <row r="191" ht="130" customHeight="1">
       <c r="A191" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B191" s="3" t="inlineStr">
@@ -15531,7 +15531,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B192" s="3" t="inlineStr">
@@ -15613,7 +15613,7 @@
     <row r="193" ht="130" customHeight="1">
       <c r="A193" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B193" s="3" t="inlineStr">
@@ -15688,7 +15688,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-12 c,AU-3 (1),AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B194" s="3" t="inlineStr">
@@ -15761,7 +15761,7 @@
     <row r="195" ht="130" customHeight="1">
       <c r="A195" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 c,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B195" s="3" t="inlineStr">
@@ -15838,7 +15838,7 @@
     <row r="196" ht="130" customHeight="1">
       <c r="A196" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (1),IA-2 (4),IA-2 (2)</t>
+          <t>IA-2 (1),IA-2 (2),IA-2 (4),IA-2 (3)</t>
         </is>
       </c>
       <c r="B196" s="2" t="inlineStr">
@@ -15925,7 +15925,7 @@
     <row r="197" ht="130" customHeight="1">
       <c r="A197" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),IA-2 (2),IA-2 (3),IA-2,IA-2 (4)</t>
+          <t>IA-2 (5),IA-2 (3),IA-2 (2),IA-2,IA-2 (4)</t>
         </is>
       </c>
       <c r="B197" s="2" t="inlineStr">
@@ -16014,7 +16014,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),IA-2 (2),IA-2 (3),IA-2,IA-2 (4)</t>
+          <t>IA-2 (5),IA-2 (3),IA-2 (2),IA-2,IA-2 (4)</t>
         </is>
       </c>
       <c r="B198" s="2" t="inlineStr">
@@ -16258,7 +16258,7 @@
     <row r="201" ht="130" customHeight="1">
       <c r="A201" s="2" t="inlineStr">
         <is>
-          <t>IA-11,AC-3 (4)</t>
+          <t>AC-3 (4),IA-11</t>
         </is>
       </c>
       <c r="B201" s="2" t="inlineStr">
@@ -16638,7 +16638,7 @@
     <row r="206" ht="130" customHeight="1">
       <c r="A206" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8 (2),SC-8</t>
+          <t>SC-8,SC-8 (2),SC-8 (1)</t>
         </is>
       </c>
       <c r="B206" s="2" t="inlineStr">
@@ -16715,7 +16715,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8 (2),SC-8</t>
+          <t>SC-8,SC-8 (2),SC-8 (1)</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -16801,7 +16801,7 @@
     <row r="208" ht="130" customHeight="1">
       <c r="A208" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-18 (1),SC-8 (1)</t>
+          <t>AC-18 (1),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B208" s="2" t="inlineStr">
@@ -17229,7 +17229,7 @@
     <row r="213" ht="130" customHeight="1">
       <c r="A213" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-7 a,CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (c),CM-7 a</t>
         </is>
       </c>
       <c r="B213" s="2" t="inlineStr">
@@ -17389,7 +17389,7 @@
     <row r="215" ht="130" customHeight="1">
       <c r="A215" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-12 a</t>
+          <t>AU-12 a,CM-6 b</t>
         </is>
       </c>
       <c r="B215" s="3" t="inlineStr">
@@ -17475,7 +17475,7 @@
     <row r="216" ht="130" customHeight="1">
       <c r="A216" s="2" t="inlineStr">
         <is>
-          <t>SC-5,CM-6 b,SC-5 (2)</t>
+          <t>SC-5 (2),SC-5,CM-6 b</t>
         </is>
       </c>
       <c r="B216" s="2" t="inlineStr">
@@ -17845,7 +17845,7 @@
     <row r="220" ht="130" customHeight="1">
       <c r="A220" s="2" t="inlineStr">
         <is>
-          <t>IA-2,IA-8,AU-3 (1)</t>
+          <t>IA-8,IA-2,AU-3 (1)</t>
         </is>
       </c>
       <c r="B220" s="2" t="inlineStr">
@@ -18824,7 +18824,7 @@
     <row r="232" ht="130" customHeight="1">
       <c r="A232" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SI-16,CM-6 b</t>
+          <t>SI-16,CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B232" s="2" t="inlineStr">
@@ -19732,7 +19732,7 @@
     <row r="243" ht="130" customHeight="1">
       <c r="A243" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (b),IA-5 (1) (a),CM-6 b</t>
+          <t>IA-5 (1) (a),CM-6 b,IA-5 (1) (b)</t>
         </is>
       </c>
       <c r="B243" s="2" t="inlineStr">
@@ -20381,7 +20381,7 @@
     <row r="251" ht="130" customHeight="1">
       <c r="A251" s="3" t="inlineStr">
         <is>
-          <t>SC-2,SC-4</t>
+          <t>SC-4,SC-2</t>
         </is>
       </c>
       <c r="B251" s="3" t="inlineStr">
@@ -20469,7 +20469,7 @@
     <row r="252" ht="130" customHeight="1">
       <c r="A252" s="3" t="inlineStr">
         <is>
-          <t>SC-2,SC-4</t>
+          <t>SC-4,SC-2</t>
         </is>
       </c>
       <c r="B252" s="3" t="inlineStr">
@@ -20556,7 +20556,7 @@
     <row r="253" ht="130" customHeight="1">
       <c r="A253" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (1)</t>
+          <t>IA-2 (1),IA-2 (11)</t>
         </is>
       </c>
       <c r="B253" s="2" t="inlineStr">
@@ -20645,7 +20645,7 @@
     <row r="254" ht="130" customHeight="1">
       <c r="A254" s="3" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B254" s="3" t="inlineStr">
@@ -21052,7 +21052,7 @@
     <row r="259" ht="130" customHeight="1">
       <c r="A259" s="3" t="inlineStr">
         <is>
-          <t>AC-6 (8),AC-6 (9)</t>
+          <t>AC-6 (9),AC-6 (8)</t>
         </is>
       </c>
       <c r="B259" s="3" t="inlineStr">
@@ -21132,7 +21132,7 @@
     <row r="260" ht="130" customHeight="1">
       <c r="A260" s="3" t="inlineStr">
         <is>
-          <t>IA-2 (5),CM-6 b</t>
+          <t>CM-6 b,IA-2 (5)</t>
         </is>
       </c>
       <c r="B260" s="3" t="inlineStr">
@@ -21598,7 +21598,7 @@
     <row r="266" ht="130" customHeight="1">
       <c r="A266" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-12 c</t>
+          <t>AU-12 c,AU-9</t>
         </is>
       </c>
       <c r="B266" s="2" t="inlineStr">
@@ -21681,7 +21681,7 @@
     <row r="267" ht="130" customHeight="1">
       <c r="A267" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (3)</t>
+          <t>CM-5 (3),CM-6 b</t>
         </is>
       </c>
       <c r="B267" s="2" t="inlineStr">
@@ -23668,7 +23668,7 @@
     <row r="292" ht="130" customHeight="1">
       <c r="A292" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-6 (9),AC-2 (4)</t>
+          <t>AC-2 (4),AC-6 (9),AU-12 c</t>
         </is>
       </c>
       <c r="B292" s="3" t="inlineStr">
@@ -27247,7 +27247,7 @@
     <row r="339" ht="130" customHeight="1">
       <c r="A339" s="3" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B339" s="3" t="inlineStr">
@@ -27397,7 +27397,7 @@
     <row r="341" ht="130" customHeight="1">
       <c r="A341" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (2)</t>
+          <t>IA-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B341" s="2" t="inlineStr">
@@ -30512,7 +30512,7 @@
     <row r="382" ht="130" customHeight="1">
       <c r="A382" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (1),CM-6 b,AC-17 (9)</t>
+          <t>AC-17 (1),AC-17 (9),CM-7 b,CM-6 b</t>
         </is>
       </c>
       <c r="B382" s="2" t="inlineStr">
@@ -30590,7 +30590,7 @@
     <row r="383" ht="130" customHeight="1">
       <c r="A383" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (1),CM-6 b</t>
+          <t>AC-17 (1),CM-7 b,CM-6 b</t>
         </is>
       </c>
       <c r="B383" s="2" t="inlineStr">
@@ -34045,7 +34045,7 @@
     <row r="424" ht="130" customHeight="1">
       <c r="A424" s="3" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b</t>
+          <t>CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B424" s="3" t="inlineStr">
@@ -34132,7 +34132,7 @@
     <row r="425" ht="130" customHeight="1">
       <c r="A425" s="3" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b</t>
+          <t>CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B425" s="3" t="inlineStr">
@@ -34919,7 +34919,7 @@
     <row r="435" ht="130" customHeight="1">
       <c r="A435" s="2" t="inlineStr">
         <is>
-          <t>AU-4,CM-6 b</t>
+          <t>CM-6 b,AU-4</t>
         </is>
       </c>
       <c r="B435" s="2" t="inlineStr">
@@ -35708,7 +35708,7 @@
     <row r="445" ht="130" customHeight="1">
       <c r="A445" s="3" t="inlineStr">
         <is>
-          <t>SI-2 (2),CM-6 b</t>
+          <t>CM-6 b,SI-2 (2)</t>
         </is>
       </c>
       <c r="B445" s="3" t="inlineStr">
@@ -36355,7 +36355,7 @@
     <row r="454" ht="130" customHeight="1">
       <c r="A454" s="3" t="inlineStr">
         <is>
-          <t>SI-2 (2),CM-6 b</t>
+          <t>CM-6 b,SI-2 (2)</t>
         </is>
       </c>
       <c r="B454" s="3" t="inlineStr">
@@ -36646,7 +36646,7 @@
     <row r="458" ht="130" customHeight="1">
       <c r="A458" s="3" t="inlineStr">
         <is>
-          <t>AC-12,SC-10,MA-4 (7),MA-4 e</t>
+          <t>SC-10,MA-4 e,MA-4 (7),AC-12</t>
         </is>
       </c>
       <c r="B458" s="3" t="inlineStr">
@@ -36721,7 +36721,7 @@
     <row r="459" ht="130" customHeight="1">
       <c r="A459" s="3" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B459" s="3" t="inlineStr">
@@ -36800,7 +36800,7 @@
     <row r="460" ht="130" customHeight="1">
       <c r="A460" s="3" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B460" s="3" t="inlineStr">
@@ -36876,7 +36876,7 @@
     <row r="461" ht="130" customHeight="1">
       <c r="A461" s="3" t="inlineStr">
         <is>
-          <t>AC-11 a,SC-10</t>
+          <t>SC-10,AC-11 a</t>
         </is>
       </c>
       <c r="B461" s="3" t="inlineStr">
@@ -36953,7 +36953,7 @@
     <row r="462" ht="130" customHeight="1">
       <c r="A462" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8 (1),SC-8</t>
+          <t>SC-8,AC-17 (2),SC-8 (1)</t>
         </is>
       </c>
       <c r="B462" s="2" t="inlineStr">
@@ -37751,7 +37751,7 @@
       </c>
       <c r="F472" s="3" t="inlineStr">
         <is>
-          <t>Red Hat Enterprise Linux 9 must display the Standard Mandatory DoD Notice and Consent Banner until users acknowledge the usage conditions and take explicit actions to log on for further access.</t>
+          <t>Red Hat Enterprise Linux 9 must display the Standard Mandatory DoD Notice and Consent Banner until users acknowledge the usage conditions and take explicit actions to log on for further access via CLI and Graphical access.</t>
         </is>
       </c>
       <c r="G472" s="3" t="inlineStr">
@@ -37788,7 +37788,7 @@
       <c r="P472" s="3" t="n"/>
       <c r="Q472" s="3" t="inlineStr">
         <is>
-          <t>Red Hat Enterprise Linux 9 does not have configuration options to meet this requirement.</t>
+          <t>Red Hat Enterprise Linux 9 does not natively support a method of presenting an interactive acknowledgement of the login banner.</t>
         </is>
       </c>
     </row>
@@ -38261,7 +38261,7 @@
     <row r="479" ht="130" customHeight="1">
       <c r="A479" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,IA-3</t>
+          <t>IA-3,CM-7 b</t>
         </is>
       </c>
       <c r="B479" s="2" t="inlineStr">
@@ -38580,7 +38580,7 @@
     <row r="483" ht="130" customHeight="1">
       <c r="A483" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (1)</t>
+          <t>AC-17 (1),CM-7 b</t>
         </is>
       </c>
       <c r="B483" s="2" t="inlineStr">
@@ -39703,7 +39703,7 @@
     <row r="497" ht="130" customHeight="1">
       <c r="A497" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-4 (1)</t>
+          <t>AU-4 (1),AU-4</t>
         </is>
       </c>
       <c r="B497" s="2" t="inlineStr">
@@ -41423,7 +41423,7 @@
     <row r="518" ht="130" customHeight="1">
       <c r="A518" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8</t>
+          <t>SC-8,SC-8 (2)</t>
         </is>
       </c>
       <c r="B518" s="2" t="inlineStr">
@@ -42613,7 +42613,7 @@
     <row r="533" ht="130" customHeight="1">
       <c r="A533" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8</t>
+          <t>SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B533" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@2c4c03eb40c43ef361248d732c303f7e51147fca 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -550,7 +550,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -634,7 +634,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -719,7 +719,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -791,7 +791,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -1455,7 +1455,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>AU-3,CM-5 (1),AU-12 a,AU-7 a,CM-6 b,AU-7 (1),AU-6 (4),AU-14 (1),AU-3 (1),MA-4 (1) (a)</t>
+          <t>CM-5 (1),AU-14 (1),AU-7 a,AU-3,AU-12 a,AU-7 (1),AU-6 (4),CM-6 b,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -3258,7 +3258,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-14 (1),AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-14 (1),AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3349,7 +3349,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),AU-4</t>
+          <t>AU-4,AU-14 (1)</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3908,7 +3908,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-4 (1)</t>
+          <t>AU-4 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3993,7 +3993,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (b),AU-8 (1) (a),AU-8 b</t>
+          <t>AU-8 (1) (b),AU-8 b,AU-8 (1) (a)</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -4234,7 +4234,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12),IA-2 (1)</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4318,7 +4318,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>SI-6 d,CM-3 (5),SI-6 b</t>
+          <t>SI-6 b,SI-6 d,CM-3 (5)</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4494,7 +4494,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -4569,7 +4569,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -4644,7 +4644,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -4719,7 +4719,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -4794,7 +4794,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -4869,7 +4869,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -4944,7 +4944,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -5019,7 +5019,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -5094,7 +5094,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -5169,7 +5169,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AU-12 a,AU-7 a,CM-6 b,AU-12 (3),AU-12 c,AU-8 b,AU-7 b</t>
+          <t>CM-5 (1),AU-12 c,AU-8 b,AU-7 a,AU-12 (3),AU-12 a,AU-7 b,CM-6 b</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5243,7 +5243,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5324,7 +5324,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5405,7 +5405,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5487,7 +5487,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5569,7 +5569,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5651,7 +5651,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5733,7 +5733,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5815,7 +5815,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 a</t>
+          <t>SI-6 a,CM-3 (5)</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -6853,7 +6853,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -6927,7 +6927,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -7001,7 +7001,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -7075,7 +7075,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -7155,7 +7155,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -7240,7 +7240,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>AC-17 (2),MA-4 (6)</t>
+          <t>MA-4 (6),AC-17 (2)</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -7316,7 +7316,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -7499,7 +7499,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>AU-9,AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -7575,7 +7575,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>AU-9,AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -7651,7 +7651,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -7726,7 +7726,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -7801,7 +7801,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -7876,7 +7876,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -7956,7 +7956,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -8038,7 +8038,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -8120,7 +8120,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8202,7 +8202,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8284,7 +8284,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8366,7 +8366,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -8446,7 +8446,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -8526,7 +8526,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -9354,7 +9354,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2),SC-13,MA-4 c</t>
+          <t>MA-4 c,SC-13,AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9514,7 +9514,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9670,7 +9670,7 @@
     <row r="117" ht="130" customHeight="1">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -10026,7 +10026,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -10873,7 +10873,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10954,7 +10954,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -11040,7 +11040,7 @@
     <row r="135" ht="130" customHeight="1">
       <c r="A135" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B135" s="2" t="inlineStr">
@@ -11486,7 +11486,7 @@
     <row r="140" ht="130" customHeight="1">
       <c r="A140" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B140" s="3" t="inlineStr">
@@ -11566,7 +11566,7 @@
     <row r="141" ht="130" customHeight="1">
       <c r="A141" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B141" s="3" t="inlineStr">
@@ -11646,7 +11646,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B142" s="3" t="inlineStr">
@@ -12429,7 +12429,7 @@
     <row r="152" ht="130" customHeight="1">
       <c r="A152" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B152" s="2" t="inlineStr">
@@ -12505,7 +12505,7 @@
     <row r="153" ht="130" customHeight="1">
       <c r="A153" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B153" s="2" t="inlineStr">
@@ -12590,7 +12590,7 @@
     <row r="154" ht="130" customHeight="1">
       <c r="A154" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B154" s="2" t="inlineStr">
@@ -12826,7 +12826,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B157" s="3" t="inlineStr">
@@ -12903,7 +12903,7 @@
     <row r="158" ht="130" customHeight="1">
       <c r="A158" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-12 c,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B158" s="3" t="inlineStr">
@@ -12976,7 +12976,7 @@
     <row r="159" ht="130" customHeight="1">
       <c r="A159" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 a,AU-12 c,AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B159" s="3" t="inlineStr">
@@ -13049,7 +13049,7 @@
     <row r="160" ht="130" customHeight="1">
       <c r="A160" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B160" s="3" t="inlineStr">
@@ -13134,7 +13134,7 @@
     <row r="161" ht="130" customHeight="1">
       <c r="A161" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B161" s="3" t="inlineStr">
@@ -13209,7 +13209,7 @@
     <row r="162" ht="130" customHeight="1">
       <c r="A162" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B162" s="3" t="inlineStr">
@@ -13284,7 +13284,7 @@
     <row r="163" ht="130" customHeight="1">
       <c r="A163" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B163" s="3" t="inlineStr">
@@ -13359,7 +13359,7 @@
     <row r="164" ht="130" customHeight="1">
       <c r="A164" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B164" s="3" t="inlineStr">
@@ -13862,7 +13862,7 @@
     <row r="171" ht="130" customHeight="1">
       <c r="A171" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B171" s="3" t="inlineStr">
@@ -14151,7 +14151,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B175" s="3" t="inlineStr">
@@ -14226,7 +14226,7 @@
     <row r="176" ht="130" customHeight="1">
       <c r="A176" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B176" s="3" t="inlineStr">
@@ -14308,7 +14308,7 @@
     <row r="177" ht="130" customHeight="1">
       <c r="A177" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B177" s="3" t="inlineStr">
@@ -14390,7 +14390,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B178" s="3" t="inlineStr">
@@ -14472,7 +14472,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B179" s="3" t="inlineStr">
@@ -14554,7 +14554,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B180" s="3" t="inlineStr">
@@ -14636,7 +14636,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B181" s="3" t="inlineStr">
@@ -14718,7 +14718,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B182" s="3" t="inlineStr">
@@ -14800,7 +14800,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B183" s="3" t="inlineStr">
@@ -14882,7 +14882,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B184" s="3" t="inlineStr">
@@ -14964,7 +14964,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B185" s="3" t="inlineStr">
@@ -15042,7 +15042,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B186" s="3" t="inlineStr">
@@ -15121,7 +15121,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B187" s="3" t="inlineStr">
@@ -15203,7 +15203,7 @@
     <row r="188" ht="130" customHeight="1">
       <c r="A188" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B188" s="3" t="inlineStr">
@@ -15285,7 +15285,7 @@
     <row r="189" ht="130" customHeight="1">
       <c r="A189" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B189" s="3" t="inlineStr">
@@ -15367,7 +15367,7 @@
     <row r="190" ht="130" customHeight="1">
       <c r="A190" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B190" s="3" t="inlineStr">
@@ -15449,7 +15449,7 @@
     <row r="191" ht="130" customHeight="1">
       <c r="A191" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B191" s="3" t="inlineStr">
@@ -15531,7 +15531,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B192" s="3" t="inlineStr">
@@ -15613,7 +15613,7 @@
     <row r="193" ht="130" customHeight="1">
       <c r="A193" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B193" s="3" t="inlineStr">
@@ -15688,7 +15688,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AU-12 a,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B194" s="3" t="inlineStr">
@@ -15761,7 +15761,7 @@
     <row r="195" ht="130" customHeight="1">
       <c r="A195" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B195" s="3" t="inlineStr">
@@ -15838,7 +15838,7 @@
     <row r="196" ht="130" customHeight="1">
       <c r="A196" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (2),IA-2 (4),IA-2 (3)</t>
+          <t>IA-2 (2),IA-2 (4),IA-2 (3),IA-2 (1)</t>
         </is>
       </c>
       <c r="B196" s="2" t="inlineStr">
@@ -15925,7 +15925,7 @@
     <row r="197" ht="130" customHeight="1">
       <c r="A197" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),IA-2 (3),IA-2 (2),IA-2,IA-2 (4)</t>
+          <t>IA-2 (4),IA-2 (2),IA-2 (5),IA-2,IA-2 (3)</t>
         </is>
       </c>
       <c r="B197" s="2" t="inlineStr">
@@ -16014,7 +16014,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),IA-2 (3),IA-2 (2),IA-2,IA-2 (4)</t>
+          <t>IA-2 (4),IA-2 (2),IA-2 (5),IA-2,IA-2 (3)</t>
         </is>
       </c>
       <c r="B198" s="2" t="inlineStr">
@@ -16258,7 +16258,7 @@
     <row r="201" ht="130" customHeight="1">
       <c r="A201" s="2" t="inlineStr">
         <is>
-          <t>AC-3 (4),IA-11</t>
+          <t>IA-11,AC-3 (4)</t>
         </is>
       </c>
       <c r="B201" s="2" t="inlineStr">
@@ -16638,7 +16638,7 @@
     <row r="206" ht="130" customHeight="1">
       <c r="A206" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (2),SC-8 (1)</t>
+          <t>SC-8 (2),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B206" s="2" t="inlineStr">
@@ -16715,7 +16715,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (2),SC-8 (1)</t>
+          <t>SC-8 (2),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -16801,7 +16801,7 @@
     <row r="208" ht="130" customHeight="1">
       <c r="A208" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),SC-8,SC-8 (1)</t>
+          <t>SC-8,AC-18 (1),SC-8 (1)</t>
         </is>
       </c>
       <c r="B208" s="2" t="inlineStr">
@@ -17229,7 +17229,7 @@
     <row r="213" ht="130" customHeight="1">
       <c r="A213" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (c),CM-7 a</t>
+          <t>CM-7 a,IA-5 (1) (c),CM-6 b</t>
         </is>
       </c>
       <c r="B213" s="2" t="inlineStr">
@@ -18824,7 +18824,7 @@
     <row r="232" ht="130" customHeight="1">
       <c r="A232" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-6 b,SC-2</t>
+          <t>SI-16,SC-2,CM-6 b</t>
         </is>
       </c>
       <c r="B232" s="2" t="inlineStr">
@@ -19732,7 +19732,7 @@
     <row r="243" ht="130" customHeight="1">
       <c r="A243" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (a),CM-6 b,IA-5 (1) (b)</t>
+          <t>IA-5 (1) (b),IA-5 (1) (a),CM-6 b</t>
         </is>
       </c>
       <c r="B243" s="2" t="inlineStr">
@@ -20300,7 +20300,7 @@
     <row r="250" ht="130" customHeight="1">
       <c r="A250" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-4</t>
+          <t>SC-4,CM-6 b</t>
         </is>
       </c>
       <c r="B250" s="2" t="inlineStr">
@@ -22371,7 +22371,7 @@
     <row r="275" ht="130" customHeight="1">
       <c r="A275" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B275" s="3" t="inlineStr">
@@ -23367,7 +23367,7 @@
     <row r="288" ht="130" customHeight="1">
       <c r="A288" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B288" s="3" t="inlineStr">
@@ -23438,7 +23438,7 @@
     <row r="289" ht="130" customHeight="1">
       <c r="A289" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B289" s="3" t="inlineStr">
@@ -23510,7 +23510,7 @@
     <row r="290" ht="130" customHeight="1">
       <c r="A290" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B290" s="3" t="inlineStr">
@@ -23668,7 +23668,7 @@
     <row r="292" ht="130" customHeight="1">
       <c r="A292" s="3" t="inlineStr">
         <is>
-          <t>AC-2 (4),AC-6 (9),AU-12 c</t>
+          <t>AU-12 c,AC-2 (4),AC-6 (9)</t>
         </is>
       </c>
       <c r="B292" s="3" t="inlineStr">
@@ -27247,7 +27247,7 @@
     <row r="339" ht="130" customHeight="1">
       <c r="A339" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),CM-6 b</t>
         </is>
       </c>
       <c r="B339" s="3" t="inlineStr">
@@ -30118,7 +30118,7 @@
     <row r="377" ht="130" customHeight="1">
       <c r="A377" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B377" s="2" t="inlineStr">
@@ -30512,7 +30512,7 @@
     <row r="382" ht="130" customHeight="1">
       <c r="A382" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),AC-17 (9),CM-7 b,CM-6 b</t>
+          <t>CM-7 b,AC-17 (1),AC-17 (9),CM-6 b</t>
         </is>
       </c>
       <c r="B382" s="2" t="inlineStr">
@@ -30590,7 +30590,7 @@
     <row r="383" ht="130" customHeight="1">
       <c r="A383" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),CM-7 b,CM-6 b</t>
+          <t>CM-7 b,AC-17 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B383" s="2" t="inlineStr">
@@ -33864,7 +33864,7 @@
     <row r="422" ht="130" customHeight="1">
       <c r="A422" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B422" s="2" t="inlineStr">
@@ -34045,7 +34045,7 @@
     <row r="424" ht="130" customHeight="1">
       <c r="A424" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-2</t>
+          <t>SC-2,CM-6 b</t>
         </is>
       </c>
       <c r="B424" s="3" t="inlineStr">
@@ -34132,7 +34132,7 @@
     <row r="425" ht="130" customHeight="1">
       <c r="A425" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-2</t>
+          <t>SC-2,CM-6 b</t>
         </is>
       </c>
       <c r="B425" s="3" t="inlineStr">
@@ -34467,7 +34467,7 @@
     <row r="429" ht="130" customHeight="1">
       <c r="A429" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B429" s="2" t="inlineStr">
@@ -34919,7 +34919,7 @@
     <row r="435" ht="130" customHeight="1">
       <c r="A435" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-4</t>
+          <t>AU-4,CM-6 b</t>
         </is>
       </c>
       <c r="B435" s="2" t="inlineStr">
@@ -35708,7 +35708,7 @@
     <row r="445" ht="130" customHeight="1">
       <c r="A445" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-2 (2)</t>
+          <t>SI-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B445" s="3" t="inlineStr">
@@ -36355,7 +36355,7 @@
     <row r="454" ht="130" customHeight="1">
       <c r="A454" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-2 (2)</t>
+          <t>SI-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B454" s="3" t="inlineStr">
@@ -36646,7 +36646,7 @@
     <row r="458" ht="130" customHeight="1">
       <c r="A458" s="3" t="inlineStr">
         <is>
-          <t>SC-10,MA-4 e,MA-4 (7),AC-12</t>
+          <t>MA-4 e,MA-4 (7),AC-12,SC-10</t>
         </is>
       </c>
       <c r="B458" s="3" t="inlineStr">
@@ -36721,7 +36721,7 @@
     <row r="459" ht="130" customHeight="1">
       <c r="A459" s="3" t="inlineStr">
         <is>
-          <t>SC-10,AC-12</t>
+          <t>AC-12,SC-10</t>
         </is>
       </c>
       <c r="B459" s="3" t="inlineStr">
@@ -36800,7 +36800,7 @@
     <row r="460" ht="130" customHeight="1">
       <c r="A460" s="3" t="inlineStr">
         <is>
-          <t>SC-10,AC-12</t>
+          <t>AC-12,SC-10</t>
         </is>
       </c>
       <c r="B460" s="3" t="inlineStr">
@@ -36876,7 +36876,7 @@
     <row r="461" ht="130" customHeight="1">
       <c r="A461" s="3" t="inlineStr">
         <is>
-          <t>SC-10,AC-11 a</t>
+          <t>AC-11 a,SC-10</t>
         </is>
       </c>
       <c r="B461" s="3" t="inlineStr">
@@ -36953,7 +36953,7 @@
     <row r="462" ht="130" customHeight="1">
       <c r="A462" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2),SC-8 (1)</t>
+          <t>AC-17 (2),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B462" s="2" t="inlineStr">
@@ -38580,7 +38580,7 @@
     <row r="483" ht="130" customHeight="1">
       <c r="A483" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),CM-7 b</t>
+          <t>CM-7 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B483" s="2" t="inlineStr">
@@ -39703,7 +39703,7 @@
     <row r="497" ht="130" customHeight="1">
       <c r="A497" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-4</t>
+          <t>AU-4,AU-4 (1)</t>
         </is>
       </c>
       <c r="B497" s="2" t="inlineStr">
@@ -39954,7 +39954,7 @@
     <row r="500" ht="130" customHeight="1">
       <c r="A500" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B500" s="2" t="inlineStr">
@@ -40056,7 +40056,7 @@
     <row r="501" ht="130" customHeight="1">
       <c r="A501" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B501" s="2" t="inlineStr">
@@ -40166,7 +40166,7 @@
     <row r="502" ht="130" customHeight="1">
       <c r="A502" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B502" s="2" t="inlineStr">
@@ -40277,7 +40277,7 @@
     <row r="503" ht="130" customHeight="1">
       <c r="A503" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B503" s="2" t="inlineStr">
@@ -41423,7 +41423,7 @@
     <row r="518" ht="130" customHeight="1">
       <c r="A518" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (2)</t>
+          <t>SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B518" s="2" t="inlineStr">
@@ -42613,7 +42613,7 @@
     <row r="533" ht="130" customHeight="1">
       <c r="A533" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2)</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B533" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@b77bb44f19b2f79987727ad201de6ba526ba5d66 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -550,7 +550,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -634,7 +634,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -719,7 +719,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -791,7 +791,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -973,7 +973,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 b</t>
+          <t>AU-5 b,AU-5 a</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -1455,7 +1455,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AU-14 (1),AU-7 a,AU-3,AU-12 a,AU-7 (1),AU-6 (4),CM-6 b,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-6 (4),AU-7 (1),AU-14 (1),AU-3,CM-5 (1),MA-4 (1) (a),AU-7 a,AU-12 a,CM-6 b</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -3258,7 +3258,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-14 (1),AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-14 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3438,7 +3438,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-4 (1)</t>
+          <t>AU-4 (1),AU-3</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3832,7 +3832,7 @@
     <row r="44" ht="130" customHeight="1">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-4 (1),AU-6 (4)</t>
+          <t>AU-6 (4),AU-4 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
@@ -4234,7 +4234,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12),IA-2 (1)</t>
+          <t>IA-2 (12),IA-2 (1),IA-2 (11)</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4318,7 +4318,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>SI-6 b,SI-6 d,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 b,SI-6 d</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4410,7 +4410,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>SI-6 d,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 d</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -4494,7 +4494,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -4569,7 +4569,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -4644,7 +4644,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -4719,7 +4719,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -4794,7 +4794,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -4869,7 +4869,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -4944,7 +4944,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -5019,7 +5019,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -5094,7 +5094,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -5169,7 +5169,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AU-12 c,AU-8 b,AU-7 a,AU-12 (3),AU-12 a,AU-7 b,CM-6 b</t>
+          <t>AU-7 b,AU-8 b,CM-5 (1),AU-12 c,AU-7 a,AU-12 (3),AU-12 a,CM-6 b</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5243,7 +5243,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AC-2 (4)</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5324,7 +5324,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AC-2 (4)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5405,7 +5405,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AC-2 (4)</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5487,7 +5487,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AC-2 (4)</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5569,7 +5569,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AC-2 (4)</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5651,7 +5651,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AC-2 (4)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5733,7 +5733,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AC-2 (4)</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -6853,7 +6853,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -6927,7 +6927,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -7001,7 +7001,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -7075,7 +7075,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -7499,7 +7499,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>AU-9 (3),AU-9</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -7575,7 +7575,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>AU-9 (3),AU-9</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -7651,7 +7651,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -7726,7 +7726,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -7801,7 +7801,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -7876,7 +7876,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -7956,7 +7956,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -8038,7 +8038,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -8120,7 +8120,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8202,7 +8202,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8284,7 +8284,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8366,7 +8366,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -8446,7 +8446,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -8526,7 +8526,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -8856,7 +8856,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8935,7 +8935,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -9022,7 +9022,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -9109,7 +9109,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -9354,7 +9354,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>MA-4 c,SC-13,AC-17 (2),SC-8</t>
+          <t>SC-8,MA-4 c,SC-13,AC-17 (2)</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9514,7 +9514,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9670,7 +9670,7 @@
     <row r="117" ht="130" customHeight="1">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -10026,7 +10026,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -11486,7 +11486,7 @@
     <row r="140" ht="130" customHeight="1">
       <c r="A140" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B140" s="3" t="inlineStr">
@@ -11566,7 +11566,7 @@
     <row r="141" ht="130" customHeight="1">
       <c r="A141" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B141" s="3" t="inlineStr">
@@ -11646,7 +11646,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B142" s="3" t="inlineStr">
@@ -12747,7 +12747,7 @@
     <row r="156" ht="130" customHeight="1">
       <c r="A156" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-7 a</t>
+          <t>CM-7 a,IA-7</t>
         </is>
       </c>
       <c r="B156" s="2" t="inlineStr">
@@ -12826,7 +12826,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B157" s="3" t="inlineStr">
@@ -12903,7 +12903,7 @@
     <row r="158" ht="130" customHeight="1">
       <c r="A158" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B158" s="3" t="inlineStr">
@@ -12976,7 +12976,7 @@
     <row r="159" ht="130" customHeight="1">
       <c r="A159" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-12 c,AU-3,MA-4 (1) (a)</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
         </is>
       </c>
       <c r="B159" s="3" t="inlineStr">
@@ -13049,7 +13049,7 @@
     <row r="160" ht="130" customHeight="1">
       <c r="A160" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B160" s="3" t="inlineStr">
@@ -13134,7 +13134,7 @@
     <row r="161" ht="130" customHeight="1">
       <c r="A161" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B161" s="3" t="inlineStr">
@@ -13209,7 +13209,7 @@
     <row r="162" ht="130" customHeight="1">
       <c r="A162" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B162" s="3" t="inlineStr">
@@ -13284,7 +13284,7 @@
     <row r="163" ht="130" customHeight="1">
       <c r="A163" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B163" s="3" t="inlineStr">
@@ -13359,7 +13359,7 @@
     <row r="164" ht="130" customHeight="1">
       <c r="A164" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B164" s="3" t="inlineStr">
@@ -13862,7 +13862,7 @@
     <row r="171" ht="130" customHeight="1">
       <c r="A171" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B171" s="3" t="inlineStr">
@@ -14151,7 +14151,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B175" s="3" t="inlineStr">
@@ -14226,7 +14226,7 @@
     <row r="176" ht="130" customHeight="1">
       <c r="A176" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B176" s="3" t="inlineStr">
@@ -14308,7 +14308,7 @@
     <row r="177" ht="130" customHeight="1">
       <c r="A177" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B177" s="3" t="inlineStr">
@@ -14390,7 +14390,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B178" s="3" t="inlineStr">
@@ -14472,7 +14472,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B179" s="3" t="inlineStr">
@@ -14554,7 +14554,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B180" s="3" t="inlineStr">
@@ -14636,7 +14636,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B181" s="3" t="inlineStr">
@@ -14718,7 +14718,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B182" s="3" t="inlineStr">
@@ -14800,7 +14800,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B183" s="3" t="inlineStr">
@@ -14882,7 +14882,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B184" s="3" t="inlineStr">
@@ -14964,7 +14964,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B185" s="3" t="inlineStr">
@@ -15042,7 +15042,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B186" s="3" t="inlineStr">
@@ -15121,7 +15121,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B187" s="3" t="inlineStr">
@@ -15203,7 +15203,7 @@
     <row r="188" ht="130" customHeight="1">
       <c r="A188" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B188" s="3" t="inlineStr">
@@ -15285,7 +15285,7 @@
     <row r="189" ht="130" customHeight="1">
       <c r="A189" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B189" s="3" t="inlineStr">
@@ -15367,7 +15367,7 @@
     <row r="190" ht="130" customHeight="1">
       <c r="A190" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B190" s="3" t="inlineStr">
@@ -15449,7 +15449,7 @@
     <row r="191" ht="130" customHeight="1">
       <c r="A191" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B191" s="3" t="inlineStr">
@@ -15531,7 +15531,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B192" s="3" t="inlineStr">
@@ -15613,7 +15613,7 @@
     <row r="193" ht="130" customHeight="1">
       <c r="A193" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B193" s="3" t="inlineStr">
@@ -15688,7 +15688,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-12 a,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AC-2 (4)</t>
         </is>
       </c>
       <c r="B194" s="3" t="inlineStr">
@@ -15761,7 +15761,7 @@
     <row r="195" ht="130" customHeight="1">
       <c r="A195" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AC-2 (4)</t>
         </is>
       </c>
       <c r="B195" s="3" t="inlineStr">
@@ -15838,7 +15838,7 @@
     <row r="196" ht="130" customHeight="1">
       <c r="A196" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (4),IA-2 (3),IA-2 (1)</t>
+          <t>IA-2 (3),IA-2 (2),IA-2 (1),IA-2 (4)</t>
         </is>
       </c>
       <c r="B196" s="2" t="inlineStr">
@@ -15925,7 +15925,7 @@
     <row r="197" ht="130" customHeight="1">
       <c r="A197" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2 (2),IA-2 (5),IA-2,IA-2 (3)</t>
+          <t>IA-2,IA-2 (5),IA-2 (3),IA-2 (2),IA-2 (4)</t>
         </is>
       </c>
       <c r="B197" s="2" t="inlineStr">
@@ -16014,7 +16014,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2 (2),IA-2 (5),IA-2,IA-2 (3)</t>
+          <t>IA-2,IA-2 (5),IA-2 (3),IA-2 (2),IA-2 (4)</t>
         </is>
       </c>
       <c r="B198" s="2" t="inlineStr">
@@ -16258,7 +16258,7 @@
     <row r="201" ht="130" customHeight="1">
       <c r="A201" s="2" t="inlineStr">
         <is>
-          <t>IA-11,AC-3 (4)</t>
+          <t>AC-3 (4),IA-11</t>
         </is>
       </c>
       <c r="B201" s="2" t="inlineStr">
@@ -16638,7 +16638,7 @@
     <row r="206" ht="130" customHeight="1">
       <c r="A206" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8,SC-8 (1)</t>
+          <t>SC-8,SC-8 (1),SC-8 (2)</t>
         </is>
       </c>
       <c r="B206" s="2" t="inlineStr">
@@ -16715,7 +16715,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8,SC-8 (1)</t>
+          <t>SC-8,SC-8 (1),SC-8 (2)</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -16801,7 +16801,7 @@
     <row r="208" ht="130" customHeight="1">
       <c r="A208" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-18 (1),SC-8 (1)</t>
+          <t>SC-8,SC-8 (1),AC-18 (1)</t>
         </is>
       </c>
       <c r="B208" s="2" t="inlineStr">
@@ -17655,7 +17655,7 @@
     <row r="218" ht="130" customHeight="1">
       <c r="A218" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-7 a</t>
+          <t>CM-7 a,SI-16</t>
         </is>
       </c>
       <c r="B218" s="2" t="inlineStr">
@@ -17845,7 +17845,7 @@
     <row r="220" ht="130" customHeight="1">
       <c r="A220" s="2" t="inlineStr">
         <is>
-          <t>IA-8,IA-2,AU-3 (1)</t>
+          <t>AU-3 (1),IA-8,IA-2</t>
         </is>
       </c>
       <c r="B220" s="2" t="inlineStr">
@@ -19008,7 +19008,7 @@
     <row r="234" ht="130" customHeight="1">
       <c r="A234" s="2" t="inlineStr">
         <is>
-          <t>SI-16,SC-3</t>
+          <t>SC-3,SI-16</t>
         </is>
       </c>
       <c r="B234" s="2" t="inlineStr">
@@ -19170,7 +19170,7 @@
     <row r="236" ht="130" customHeight="1">
       <c r="A236" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),CM-7 a</t>
+          <t>CM-7 a,AC-18 (1)</t>
         </is>
       </c>
       <c r="B236" s="2" t="inlineStr">
@@ -19732,7 +19732,7 @@
     <row r="243" ht="130" customHeight="1">
       <c r="A243" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (b),IA-5 (1) (a),CM-6 b</t>
+          <t>IA-5 (1) (a),IA-5 (1) (b),CM-6 b</t>
         </is>
       </c>
       <c r="B243" s="2" t="inlineStr">
@@ -20556,7 +20556,7 @@
     <row r="253" ht="130" customHeight="1">
       <c r="A253" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (1)</t>
         </is>
       </c>
       <c r="B253" s="2" t="inlineStr">
@@ -20643,37 +20643,37 @@
       <c r="Q253" s="2" t="n"/>
     </row>
     <row r="254" ht="130" customHeight="1">
-      <c r="A254" s="3" t="inlineStr">
+      <c r="A254" s="2" t="inlineStr">
         <is>
           <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
-      <c r="B254" s="3" t="inlineStr">
+      <c r="B254" s="2" t="inlineStr">
         <is>
           <t>CCI-001954,CCI-001953</t>
         </is>
       </c>
-      <c r="C254" s="3" t="inlineStr">
+      <c r="C254" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000375-GPOS-00160,SRG-OS-000376-GPOS-00161</t>
         </is>
       </c>
-      <c r="D254" s="3" t="inlineStr">
+      <c r="D254" s="2" t="inlineStr">
         <is>
           <t>CCE-83595-9</t>
         </is>
       </c>
-      <c r="E254" s="3" t="inlineStr">
+      <c r="E254" s="2" t="inlineStr">
         <is>
           <t>The operating system must implement multifactor authentication for remote access to privileged accounts in such a way that one of the factors is provided by a device separate from the system gaining access.</t>
         </is>
       </c>
-      <c r="F254" s="3" t="inlineStr">
+      <c r="F254" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 must implement multifactor authentication for remote access to privileged accounts in such a way that one of the factors is provided by a device separate from the system gaining access.</t>
         </is>
       </c>
-      <c r="G254" s="3" t="inlineStr">
+      <c r="G254" s="2" t="inlineStr">
         <is>
           <t>Using an authentication device, such as a CAC or token that is separate from the information system, ensures that even if the information system is compromised, that compromise will not affect credentials stored on the authentication device.
 Multifactor solutions that require devices separate from information systems gaining access include, for example, hardware tokens providing time-based or challenge-response authenticators and smart cards such as the U.S. Government Personal Identity Verification card and the DoD Common Access Card.
@@ -20683,7 +20683,7 @@
 Requires further clarification from NIST.</t>
         </is>
       </c>
-      <c r="H254" s="3" t="inlineStr">
+      <c r="H254" s="2" t="inlineStr">
         <is>
           <t>Using an authentication device, such as a CAC or token that is separate from
 the information system, ensures that even if the information system is
@@ -20696,32 +20696,38 @@
 Access Card.</t>
         </is>
       </c>
-      <c r="I254" s="3" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J254" s="3" t="inlineStr">
+      <c r="I254" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J254" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system implements multifactor authentication for remote access to privileged accounts in such a way that one of the factors is provided by a device separate from the system gaining access. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K254" s="3" t="inlineStr">
+      <c r="K254" s="2" t="inlineStr">
         <is>
           <t>Run the following command to determine if the  opensc  package is installed:  $ rpm -q opensc 
 If the package is not installed, then this is a finding.</t>
         </is>
       </c>
-      <c r="L254" s="3" t="n"/>
-      <c r="M254" s="3" t="inlineStr"/>
-      <c r="N254" s="3" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O254" s="3" t="n"/>
-      <c r="P254" s="3" t="n"/>
-      <c r="Q254" s="3" t="n"/>
+      <c r="L254" s="2" t="n"/>
+      <c r="M254" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+The  opensc  package can be installed with the following command:
+$ sudo dnf install opensc </t>
+        </is>
+      </c>
+      <c r="N254" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O254" s="2" t="n"/>
+      <c r="P254" s="2" t="n"/>
+      <c r="Q254" s="2" t="n"/>
     </row>
     <row r="255" ht="130" customHeight="1">
       <c r="A255" s="3" t="inlineStr">
@@ -20970,7 +20976,7 @@
     <row r="258" ht="130" customHeight="1">
       <c r="A258" s="2" t="inlineStr">
         <is>
-          <t>SI-6 a,SC-3</t>
+          <t>SC-3,SI-6 a</t>
         </is>
       </c>
       <c r="B258" s="2" t="inlineStr">
@@ -21052,7 +21058,7 @@
     <row r="259" ht="130" customHeight="1">
       <c r="A259" s="3" t="inlineStr">
         <is>
-          <t>AC-6 (9),AC-6 (8)</t>
+          <t>AC-6 (8),AC-6 (9)</t>
         </is>
       </c>
       <c r="B259" s="3" t="inlineStr">
@@ -21598,7 +21604,7 @@
     <row r="266" ht="130" customHeight="1">
       <c r="A266" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-9</t>
+          <t>AU-9,AU-12 c</t>
         </is>
       </c>
       <c r="B266" s="2" t="inlineStr">
@@ -23668,7 +23674,7 @@
     <row r="292" ht="130" customHeight="1">
       <c r="A292" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-2 (4),AC-6 (9)</t>
+          <t>AC-6 (9),AU-12 c,AC-2 (4)</t>
         </is>
       </c>
       <c r="B292" s="3" t="inlineStr">
@@ -29874,7 +29880,7 @@
     <row r="374" ht="130" customHeight="1">
       <c r="A374" s="3" t="inlineStr">
         <is>
-          <t>AU-3,CM-6 b</t>
+          <t>CM-6 b,AU-3</t>
         </is>
       </c>
       <c r="B374" s="3" t="inlineStr">
@@ -36646,7 +36652,7 @@
     <row r="458" ht="130" customHeight="1">
       <c r="A458" s="3" t="inlineStr">
         <is>
-          <t>MA-4 e,MA-4 (7),AC-12,SC-10</t>
+          <t>AC-12,MA-4 e,MA-4 (7),SC-10</t>
         </is>
       </c>
       <c r="B458" s="3" t="inlineStr">
@@ -36953,7 +36959,7 @@
     <row r="462" ht="130" customHeight="1">
       <c r="A462" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8,SC-8 (1)</t>
+          <t>SC-8,AC-17 (2),SC-8 (1)</t>
         </is>
       </c>
       <c r="B462" s="2" t="inlineStr">
@@ -38261,7 +38267,7 @@
     <row r="479" ht="130" customHeight="1">
       <c r="A479" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-7 b</t>
+          <t>CM-7 b,IA-3</t>
         </is>
       </c>
       <c r="B479" s="2" t="inlineStr">
@@ -39954,7 +39960,7 @@
     <row r="500" ht="130" customHeight="1">
       <c r="A500" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B500" s="2" t="inlineStr">
@@ -40056,7 +40062,7 @@
     <row r="501" ht="130" customHeight="1">
       <c r="A501" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B501" s="2" t="inlineStr">
@@ -40166,7 +40172,7 @@
     <row r="502" ht="130" customHeight="1">
       <c r="A502" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B502" s="2" t="inlineStr">
@@ -40277,7 +40283,7 @@
     <row r="503" ht="130" customHeight="1">
       <c r="A503" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B503" s="2" t="inlineStr">
@@ -41423,7 +41429,7 @@
     <row r="518" ht="130" customHeight="1">
       <c r="A518" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8</t>
+          <t>SC-8,SC-8 (2)</t>
         </is>
       </c>
       <c r="B518" s="2" t="inlineStr">
@@ -42613,7 +42619,7 @@
     <row r="533" ht="130" customHeight="1">
       <c r="A533" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8</t>
+          <t>SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B533" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@4b009c21cbfbdfbec66fbb92c15a4dfab376966f 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -550,7 +550,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -634,7 +634,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -719,7 +719,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -791,7 +791,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -1455,7 +1455,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-6 (4),AU-7 (1),AU-14 (1),AU-3,CM-5 (1),MA-4 (1) (a),AU-7 a,AU-12 a,CM-6 b</t>
+          <t>AU-3,AU-7 (1),AU-3 (1),AU-7 a,AU-14 (1),AU-12 a,AU-6 (4),CM-6 b,MA-4 (1) (a),CM-5 (1)</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -3258,7 +3258,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-14 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-14 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3438,7 +3438,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-3</t>
+          <t>AU-3,AU-4 (1)</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3503,7 +3503,7 @@
       <c r="M39" s="2" t="inlineStr">
         <is>
           <t>Edit the file "/etc/audit/auditd.conf" and add or edit the following line:
-name_format=hostname</t>
+name_format = hostname</t>
         </is>
       </c>
       <c r="N39" s="2" t="inlineStr">
@@ -3832,7 +3832,7 @@
     <row r="44" ht="130" customHeight="1">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>AU-6 (4),AU-4 (1),CM-6 b</t>
+          <t>AU-4 (1),AU-6 (4),CM-6 b</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
@@ -3993,7 +3993,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (b),AU-8 b,AU-8 (1) (a)</t>
+          <t>AU-8 (1) (a),AU-8 b,AU-8 (1) (b)</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -4148,7 +4148,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4234,7 +4234,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (1),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (1),IA-2 (12)</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4318,7 +4318,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 b,SI-6 d</t>
+          <t>SI-6 d,CM-3 (5),SI-6 b</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4410,7 +4410,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 d</t>
+          <t>SI-6 d,CM-3 (5)</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -4494,7 +4494,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -4569,7 +4569,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -4644,7 +4644,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -4719,7 +4719,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -4794,7 +4794,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -4869,7 +4869,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -4944,7 +4944,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -5019,7 +5019,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -5094,7 +5094,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -5169,7 +5169,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-7 b,AU-8 b,CM-5 (1),AU-12 c,AU-7 a,AU-12 (3),AU-12 a,CM-6 b</t>
+          <t>AU-7 a,AU-12 (3),AU-7 b,AU-12 a,CM-6 b,AU-12 c,AU-8 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5243,7 +5243,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AC-2 (4)</t>
+          <t>AU-3,AU-3 (1),AC-2 (4),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5324,7 +5324,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AC-2 (4)</t>
+          <t>AU-3,AU-3 (1),AC-2 (4),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5405,7 +5405,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AC-2 (4)</t>
+          <t>AU-3,AU-3 (1),AC-2 (4),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5487,7 +5487,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AC-2 (4)</t>
+          <t>AU-3,AU-3 (1),AC-2 (4),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5569,7 +5569,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AC-2 (4)</t>
+          <t>AU-3,AU-3 (1),AC-2 (4),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5651,7 +5651,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AC-2 (4)</t>
+          <t>AU-3,AU-3 (1),AC-2 (4),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5733,7 +5733,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AC-2 (4)</t>
+          <t>AU-3,AU-3 (1),AC-2 (4),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5815,7 +5815,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>SI-6 a,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 a</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -6853,7 +6853,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -6927,7 +6927,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -7001,7 +7001,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -7075,7 +7075,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -7240,7 +7240,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (6),AC-17 (2)</t>
+          <t>AC-17 (2),MA-4 (6)</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -7651,7 +7651,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -7726,7 +7726,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -7801,7 +7801,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -7876,7 +7876,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -7956,7 +7956,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -8038,7 +8038,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -8120,7 +8120,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8202,7 +8202,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8284,7 +8284,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8366,7 +8366,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -8446,7 +8446,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -8526,7 +8526,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -8856,7 +8856,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8935,7 +8935,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -9022,7 +9022,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -9109,7 +9109,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -9354,7 +9354,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>SC-8,MA-4 c,SC-13,AC-17 (2)</t>
+          <t>AC-17 (2),MA-4 c,SC-8,SC-13</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9514,7 +9514,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9670,7 +9670,7 @@
     <row r="117" ht="130" customHeight="1">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -10026,7 +10026,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -10106,7 +10106,7 @@
     <row r="123" ht="130" customHeight="1">
       <c r="A123" s="2" t="inlineStr">
         <is>
-          <t>SC-28,SC-28 (1)</t>
+          <t>SC-28 (1),SC-28</t>
         </is>
       </c>
       <c r="B123" s="2" t="inlineStr">
@@ -11486,7 +11486,7 @@
     <row r="140" ht="130" customHeight="1">
       <c r="A140" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B140" s="3" t="inlineStr">
@@ -11566,7 +11566,7 @@
     <row r="141" ht="130" customHeight="1">
       <c r="A141" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B141" s="3" t="inlineStr">
@@ -11646,7 +11646,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B142" s="3" t="inlineStr">
@@ -11958,7 +11958,7 @@
     <row r="146" ht="130" customHeight="1">
       <c r="A146" s="2" t="inlineStr">
         <is>
-          <t>IA-7,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),IA-7</t>
         </is>
       </c>
       <c r="B146" s="2" t="inlineStr">
@@ -12268,7 +12268,7 @@
     <row r="150" ht="130" customHeight="1">
       <c r="A150" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 (1)</t>
+          <t>AC-11 (1),AC-11 a</t>
         </is>
       </c>
       <c r="B150" s="2" t="inlineStr">
@@ -12747,7 +12747,7 @@
     <row r="156" ht="130" customHeight="1">
       <c r="A156" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,IA-7</t>
+          <t>IA-7,CM-7 a</t>
         </is>
       </c>
       <c r="B156" s="2" t="inlineStr">
@@ -12826,7 +12826,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B157" s="3" t="inlineStr">
@@ -12903,7 +12903,7 @@
     <row r="158" ht="130" customHeight="1">
       <c r="A158" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B158" s="3" t="inlineStr">
@@ -12976,7 +12976,7 @@
     <row r="159" ht="130" customHeight="1">
       <c r="A159" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-12 a,AU-3</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B159" s="3" t="inlineStr">
@@ -13049,7 +13049,7 @@
     <row r="160" ht="130" customHeight="1">
       <c r="A160" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B160" s="3" t="inlineStr">
@@ -13134,7 +13134,7 @@
     <row r="161" ht="130" customHeight="1">
       <c r="A161" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B161" s="3" t="inlineStr">
@@ -13209,7 +13209,7 @@
     <row r="162" ht="130" customHeight="1">
       <c r="A162" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B162" s="3" t="inlineStr">
@@ -13284,7 +13284,7 @@
     <row r="163" ht="130" customHeight="1">
       <c r="A163" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B163" s="3" t="inlineStr">
@@ -13359,7 +13359,7 @@
     <row r="164" ht="130" customHeight="1">
       <c r="A164" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B164" s="3" t="inlineStr">
@@ -13862,7 +13862,7 @@
     <row r="171" ht="130" customHeight="1">
       <c r="A171" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B171" s="3" t="inlineStr">
@@ -14151,7 +14151,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B175" s="3" t="inlineStr">
@@ -14226,7 +14226,7 @@
     <row r="176" ht="130" customHeight="1">
       <c r="A176" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B176" s="3" t="inlineStr">
@@ -14308,7 +14308,7 @@
     <row r="177" ht="130" customHeight="1">
       <c r="A177" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B177" s="3" t="inlineStr">
@@ -14390,7 +14390,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B178" s="3" t="inlineStr">
@@ -14472,7 +14472,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B179" s="3" t="inlineStr">
@@ -14554,7 +14554,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B180" s="3" t="inlineStr">
@@ -14636,7 +14636,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B181" s="3" t="inlineStr">
@@ -14718,7 +14718,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B182" s="3" t="inlineStr">
@@ -14800,7 +14800,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B183" s="3" t="inlineStr">
@@ -14882,7 +14882,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B184" s="3" t="inlineStr">
@@ -14964,7 +14964,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B185" s="3" t="inlineStr">
@@ -15042,7 +15042,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B186" s="3" t="inlineStr">
@@ -15121,7 +15121,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B187" s="3" t="inlineStr">
@@ -15203,7 +15203,7 @@
     <row r="188" ht="130" customHeight="1">
       <c r="A188" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B188" s="3" t="inlineStr">
@@ -15285,7 +15285,7 @@
     <row r="189" ht="130" customHeight="1">
       <c r="A189" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a),AU-3</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B189" s="3" t="inlineStr">
@@ -15367,7 +15367,7 @@
     <row r="190" ht="130" customHeight="1">
       <c r="A190" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B190" s="3" t="inlineStr">
@@ -15449,7 +15449,7 @@
     <row r="191" ht="130" customHeight="1">
       <c r="A191" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B191" s="3" t="inlineStr">
@@ -15531,7 +15531,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B192" s="3" t="inlineStr">
@@ -15613,7 +15613,7 @@
     <row r="193" ht="130" customHeight="1">
       <c r="A193" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B193" s="3" t="inlineStr">
@@ -15688,7 +15688,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a,AC-2 (4)</t>
+          <t>AU-3,AU-3 (1),AC-2 (4),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B194" s="3" t="inlineStr">
@@ -15761,7 +15761,7 @@
     <row r="195" ht="130" customHeight="1">
       <c r="A195" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c,AC-2 (4)</t>
+          <t>AU-3,AU-3 (1),AC-2 (4),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B195" s="3" t="inlineStr">
@@ -15925,7 +15925,7 @@
     <row r="197" ht="130" customHeight="1">
       <c r="A197" s="2" t="inlineStr">
         <is>
-          <t>IA-2,IA-2 (5),IA-2 (3),IA-2 (2),IA-2 (4)</t>
+          <t>IA-2 (4),IA-2,IA-2 (2),IA-2 (3),IA-2 (5)</t>
         </is>
       </c>
       <c r="B197" s="2" t="inlineStr">
@@ -16014,7 +16014,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="2" t="inlineStr">
         <is>
-          <t>IA-2,IA-2 (5),IA-2 (3),IA-2 (2),IA-2 (4)</t>
+          <t>IA-2 (4),IA-2,IA-2 (2),IA-2 (3),IA-2 (5)</t>
         </is>
       </c>
       <c r="B198" s="2" t="inlineStr">
@@ -16638,7 +16638,7 @@
     <row r="206" ht="130" customHeight="1">
       <c r="A206" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (1),SC-8 (2)</t>
+          <t>SC-8 (2),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B206" s="2" t="inlineStr">
@@ -16715,7 +16715,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (1),SC-8 (2)</t>
+          <t>SC-8 (2),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -16801,7 +16801,7 @@
     <row r="208" ht="130" customHeight="1">
       <c r="A208" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (1),AC-18 (1)</t>
+          <t>SC-8 (1),AC-18 (1),SC-8</t>
         </is>
       </c>
       <c r="B208" s="2" t="inlineStr">
@@ -16887,7 +16887,7 @@
     <row r="209" ht="130" customHeight="1">
       <c r="A209" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 (1)</t>
+          <t>AC-11 (1),AC-11 a</t>
         </is>
       </c>
       <c r="B209" s="2" t="inlineStr">
@@ -16976,7 +16976,7 @@
     <row r="210" ht="130" customHeight="1">
       <c r="A210" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 (1)</t>
+          <t>AC-11 (1),AC-11 a</t>
         </is>
       </c>
       <c r="B210" s="2" t="inlineStr">
@@ -17229,7 +17229,7 @@
     <row r="213" ht="130" customHeight="1">
       <c r="A213" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,IA-5 (1) (c),CM-6 b</t>
+          <t>IA-5 (1) (c),CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B213" s="2" t="inlineStr">
@@ -17387,37 +17387,37 @@
       <c r="Q214" s="3" t="n"/>
     </row>
     <row r="215" ht="130" customHeight="1">
-      <c r="A215" s="3" t="inlineStr">
+      <c r="A215" s="2" t="inlineStr">
         <is>
           <t>AU-12 a,CM-6 b</t>
         </is>
       </c>
-      <c r="B215" s="3" t="inlineStr">
+      <c r="B215" s="2" t="inlineStr">
         <is>
           <t>CCI-000366</t>
         </is>
       </c>
-      <c r="C215" s="3" t="inlineStr">
+      <c r="C215" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000062-GPOS-00031,SRG-OS-000480-GPOS-00227</t>
         </is>
       </c>
-      <c r="D215" s="3" t="inlineStr">
+      <c r="D215" s="2" t="inlineStr">
         <is>
           <t>CCE-83682-5</t>
         </is>
       </c>
-      <c r="E215" s="3" t="inlineStr">
+      <c r="E215" s="2" t="inlineStr">
         <is>
           <t>The operating system must provide audit record generation capability for DoD-defined auditable events for all operating system components.</t>
         </is>
       </c>
-      <c r="F215" s="3" t="inlineStr">
+      <c r="F215" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 must provide audit record generation capability for DoD-defined auditable events for all operating system components.</t>
         </is>
       </c>
-      <c r="G215" s="3" t="inlineStr">
+      <c r="G215" s="2" t="inlineStr">
         <is>
           <t>Without the capability to generate audit records, it would be difficult to establish, correlate, and investigate the events relating to an incident or identify those responsible for one.
 Audit records can be generated from various components within the information system (e.g., module or policy filter).
@@ -17429,18 +17429,18 @@
 4) All kernel module load, unload, and restart actions.</t>
         </is>
       </c>
-      <c r="H215" s="3" t="inlineStr">
+      <c r="H215" s="2" t="inlineStr">
         <is>
           <t>If option "local_events" isn't set to "yes" only events from
 network will be aggregated.</t>
         </is>
       </c>
-      <c r="I215" s="3" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J215" s="3" t="inlineStr">
+      <c r="I215" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J215" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system provides audit record generation capability for DoD-defined auditable events for all operating system components. 
 DoD has defined the list of events for which the operating system will provide an audit record generation capability as the following: 
@@ -17451,7 +17451,7 @@
 If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K215" s="3" t="inlineStr">
+      <c r="K215" s="2" t="inlineStr">
         <is>
           <t>To verify that Audit Daemon is configured to include local events, run the
 following command:
@@ -17461,16 +17461,21 @@
 If local_events isn't set to yes, then this is a finding.</t>
         </is>
       </c>
-      <c r="L215" s="3" t="n"/>
-      <c r="M215" s="3" t="inlineStr"/>
-      <c r="N215" s="3" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O215" s="3" t="n"/>
-      <c r="P215" s="3" t="n"/>
-      <c r="Q215" s="3" t="n"/>
+      <c r="L215" s="2" t="n"/>
+      <c r="M215" s="2" t="inlineStr">
+        <is>
+          <t>Edit the file "/etc/audit/auditd.conf" and add or edit the following line:
+local_events = yes</t>
+        </is>
+      </c>
+      <c r="N215" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O215" s="2" t="n"/>
+      <c r="P215" s="2" t="n"/>
+      <c r="Q215" s="2" t="n"/>
     </row>
     <row r="216" ht="130" customHeight="1">
       <c r="A216" s="2" t="inlineStr">
@@ -17845,7 +17850,7 @@
     <row r="220" ht="130" customHeight="1">
       <c r="A220" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),IA-8,IA-2</t>
+          <t>IA-2,AU-3 (1),IA-8</t>
         </is>
       </c>
       <c r="B220" s="2" t="inlineStr">
@@ -18824,7 +18829,7 @@
     <row r="232" ht="130" customHeight="1">
       <c r="A232" s="2" t="inlineStr">
         <is>
-          <t>SI-16,SC-2,CM-6 b</t>
+          <t>SC-2,SI-16,CM-6 b</t>
         </is>
       </c>
       <c r="B232" s="2" t="inlineStr">
@@ -19170,7 +19175,7 @@
     <row r="236" ht="130" customHeight="1">
       <c r="A236" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,AC-18 (1)</t>
+          <t>AC-18 (1),CM-7 a</t>
         </is>
       </c>
       <c r="B236" s="2" t="inlineStr">
@@ -19252,61 +19257,61 @@
       <c r="Q236" s="2" t="n"/>
     </row>
     <row r="237" ht="130" customHeight="1">
-      <c r="A237" s="3" t="inlineStr">
+      <c r="A237" s="2" t="inlineStr">
         <is>
           <t>AU-6 (4)</t>
         </is>
       </c>
-      <c r="B237" s="3" t="inlineStr">
+      <c r="B237" s="2" t="inlineStr">
         <is>
           <t>CCI-000154</t>
         </is>
       </c>
-      <c r="C237" s="3" t="inlineStr">
+      <c r="C237" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000051-GPOS-00024</t>
         </is>
       </c>
-      <c r="D237" s="3" t="inlineStr">
+      <c r="D237" s="2" t="inlineStr">
         <is>
           <t>CCE-83704-7</t>
         </is>
       </c>
-      <c r="E237" s="3" t="inlineStr">
+      <c r="E237" s="2" t="inlineStr">
         <is>
           <t>The operating system must provide the capability to centrally review and analyze audit records from multiple components within the system.</t>
         </is>
       </c>
-      <c r="F237" s="3" t="inlineStr">
+      <c r="F237" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 must provide the capability to centrally review and analyze audit records from multiple components within the system.</t>
         </is>
       </c>
-      <c r="G237" s="3" t="inlineStr">
+      <c r="G237" s="2" t="inlineStr">
         <is>
           <t>Successful incident response and auditing relies on timely, accurate system information and analysis in order to allow the organization to identify and respond to potential incidents in a proficient manner. If the operating system does not provide the ability to centrally review the operating system logs, forensic analysis is negatively impacted.
 Segregation of logging data to multiple disparate computer systems is counterproductive and makes log analysis and log event alarming difficult to implement and manage, particularly when the system has multiple logging components writing to different locations or systems.
 To support the centralized capability, the operating system must be able to provide the information in a format that can be extracted and used, allowing the application performing the centralization of the log records to meet this requirement.</t>
         </is>
       </c>
-      <c r="H237" s="3" t="inlineStr">
+      <c r="H237" s="2" t="inlineStr">
         <is>
           <t>If option "freq" isn't set to "50", the flush to disk
 may happen after higher number of records, increasing the danger
 of audit loss.</t>
         </is>
       </c>
-      <c r="I237" s="3" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J237" s="3" t="inlineStr">
+      <c r="I237" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J237" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system provides the capability to centrally review and analyze audit records from multiple components within the system. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K237" s="3" t="inlineStr">
+      <c r="K237" s="2" t="inlineStr">
         <is>
           <t>To verify that Audit Daemon is configured to flush to disk after
 every 50 records, run the following command:
@@ -19316,16 +19321,21 @@
 If freq isn't set to 50, then this is a finding.</t>
         </is>
       </c>
-      <c r="L237" s="3" t="n"/>
-      <c r="M237" s="3" t="inlineStr"/>
-      <c r="N237" s="3" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O237" s="3" t="n"/>
-      <c r="P237" s="3" t="n"/>
-      <c r="Q237" s="3" t="n"/>
+      <c r="L237" s="2" t="n"/>
+      <c r="M237" s="2" t="inlineStr">
+        <is>
+          <t>Edit the file "/etc/audit/auditd.conf" and add or edit the following line:
+freq = 50</t>
+        </is>
+      </c>
+      <c r="N237" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O237" s="2" t="n"/>
+      <c r="P237" s="2" t="n"/>
+      <c r="Q237" s="2" t="n"/>
     </row>
     <row r="238" ht="130" customHeight="1">
       <c r="A238" s="2" t="inlineStr">
@@ -19732,7 +19742,7 @@
     <row r="243" ht="130" customHeight="1">
       <c r="A243" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (a),IA-5 (1) (b),CM-6 b</t>
+          <t>IA-5 (1) (b),IA-5 (1) (a),CM-6 b</t>
         </is>
       </c>
       <c r="B243" s="2" t="inlineStr">
@@ -20381,7 +20391,7 @@
     <row r="251" ht="130" customHeight="1">
       <c r="A251" s="3" t="inlineStr">
         <is>
-          <t>SC-4,SC-2</t>
+          <t>SC-2,SC-4</t>
         </is>
       </c>
       <c r="B251" s="3" t="inlineStr">
@@ -20469,7 +20479,7 @@
     <row r="252" ht="130" customHeight="1">
       <c r="A252" s="3" t="inlineStr">
         <is>
-          <t>SC-4,SC-2</t>
+          <t>SC-2,SC-4</t>
         </is>
       </c>
       <c r="B252" s="3" t="inlineStr">
@@ -20645,7 +20655,7 @@
     <row r="254" ht="130" customHeight="1">
       <c r="A254" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B254" s="2" t="inlineStr">
@@ -21058,7 +21068,7 @@
     <row r="259" ht="130" customHeight="1">
       <c r="A259" s="3" t="inlineStr">
         <is>
-          <t>AC-6 (8),AC-6 (9)</t>
+          <t>AC-6 (9),AC-6 (8)</t>
         </is>
       </c>
       <c r="B259" s="3" t="inlineStr">
@@ -21138,7 +21148,7 @@
     <row r="260" ht="130" customHeight="1">
       <c r="A260" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (5)</t>
+          <t>IA-2 (5),CM-6 b</t>
         </is>
       </c>
       <c r="B260" s="3" t="inlineStr">
@@ -22525,7 +22535,7 @@
     <row r="277" ht="130" customHeight="1">
       <c r="A277" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-7 a</t>
+          <t>CM-7 a,CM-7 b</t>
         </is>
       </c>
       <c r="B277" s="2" t="inlineStr">
@@ -22605,7 +22615,7 @@
     <row r="278" ht="130" customHeight="1">
       <c r="A278" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,CM-7 a</t>
+          <t>CM-7 a,CM-7 b</t>
         </is>
       </c>
       <c r="B278" s="2" t="inlineStr">
@@ -23674,7 +23684,7 @@
     <row r="292" ht="130" customHeight="1">
       <c r="A292" s="3" t="inlineStr">
         <is>
-          <t>AC-6 (9),AU-12 c,AC-2 (4)</t>
+          <t>AU-12 c,AC-6 (9),AC-2 (4)</t>
         </is>
       </c>
       <c r="B292" s="3" t="inlineStr">
@@ -23891,7 +23901,7 @@
     <row r="294" ht="130" customHeight="1">
       <c r="A294" s="3" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 (1)</t>
+          <t>AU-5 (1),AU-5 a</t>
         </is>
       </c>
       <c r="B294" s="3" t="inlineStr">
@@ -29878,59 +29888,59 @@
       <c r="Q373" s="3" t="n"/>
     </row>
     <row r="374" ht="130" customHeight="1">
-      <c r="A374" s="3" t="inlineStr">
-        <is>
-          <t>CM-6 b,AU-3</t>
-        </is>
-      </c>
-      <c r="B374" s="3" t="inlineStr">
+      <c r="A374" s="2" t="inlineStr">
+        <is>
+          <t>AU-3,CM-6 b</t>
+        </is>
+      </c>
+      <c r="B374" s="2" t="inlineStr">
         <is>
           <t>CCI-000366</t>
         </is>
       </c>
-      <c r="C374" s="3" t="inlineStr">
+      <c r="C374" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000255-GPOS-00096,SRG-OS-000480-GPOS-00227</t>
         </is>
       </c>
-      <c r="D374" s="3" t="inlineStr">
+      <c r="D374" s="2" t="inlineStr">
         <is>
           <t>CCE-83696-5</t>
         </is>
       </c>
-      <c r="E374" s="3" t="inlineStr">
+      <c r="E374" s="2" t="inlineStr">
         <is>
           <t>The operating system must be configured in accordance with the security configuration settings based on DoD security configuration or implementation guidance, including STIGs, NSA configuration guides, CTOs, and DTMs.</t>
         </is>
       </c>
-      <c r="F374" s="3" t="inlineStr">
+      <c r="F374" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 must be configured in accordance with the security configuration settings based on DoD security configuration or implementation guidance, including STIGs, NSA configuration guides, CTOs, and DTMs.</t>
         </is>
       </c>
-      <c r="G374" s="3" t="inlineStr">
+      <c r="G374" s="2" t="inlineStr">
         <is>
           <t>Configuring the operating system to implement organization-wide security implementation guides and security checklists ensures compliance with federal standards and establishes a common security baseline across DoD that reflects the most restrictive security posture consistent with operational requirements.
 Configuration settings are the set of parameters that can be changed in hardware, software, or firmware components of the system that affect the security posture and/or functionality of the system. Security-related parameters are those parameters impacting the security state of the system, including the parameters required to satisfy other security control requirements. Security-related parameters include, for example: registry settings; account, file, directory permission settings; and settings for functions, ports, protocols, services, and remote connections.</t>
         </is>
       </c>
-      <c r="H374" s="3" t="inlineStr">
+      <c r="H374" s="2" t="inlineStr">
         <is>
           <t>If option "log_format" isn't set to "ENRICHED", the
 audit records will be stored in a format exactly as the kernel sends them.</t>
         </is>
       </c>
-      <c r="I374" s="3" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J374" s="3" t="inlineStr">
+      <c r="I374" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J374" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system is configured in accordance with the security configuration settings based on DoD security configuration or implementation guidance, including STIGs, NSA configuration guides, CTOs, and DTMs. If it is not, this is a finding.</t>
         </is>
       </c>
-      <c r="K374" s="3" t="inlineStr">
+      <c r="K374" s="2" t="inlineStr">
         <is>
           <t>To verify that Audit Daemon is configured to resolve all uid, gid, syscall,
 architecture, and socket address information before writing the event to disk,
@@ -29941,71 +29951,76 @@
 If log_format isn't set to ENRICHED, then this is a finding.</t>
         </is>
       </c>
-      <c r="L374" s="3" t="n"/>
-      <c r="M374" s="3" t="inlineStr"/>
-      <c r="N374" s="3" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O374" s="3" t="n"/>
-      <c r="P374" s="3" t="n"/>
-      <c r="Q374" s="3" t="n"/>
+      <c r="L374" s="2" t="n"/>
+      <c r="M374" s="2" t="inlineStr">
+        <is>
+          <t>Edit the file "/etc/audit/auditd.conf" and add or edit the following line:
+log_format = ENRICHED</t>
+        </is>
+      </c>
+      <c r="N374" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O374" s="2" t="n"/>
+      <c r="P374" s="2" t="n"/>
+      <c r="Q374" s="2" t="n"/>
     </row>
     <row r="375" ht="130" customHeight="1">
-      <c r="A375" s="3" t="inlineStr">
+      <c r="A375" s="2" t="inlineStr">
         <is>
           <t>CM-6 b</t>
         </is>
       </c>
-      <c r="B375" s="3" t="inlineStr">
+      <c r="B375" s="2" t="inlineStr">
         <is>
           <t>CCI-000366</t>
         </is>
       </c>
-      <c r="C375" s="3" t="inlineStr">
+      <c r="C375" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000480-GPOS-00227</t>
         </is>
       </c>
-      <c r="D375" s="3" t="inlineStr">
+      <c r="D375" s="2" t="inlineStr">
         <is>
           <t>CCE-83705-4</t>
         </is>
       </c>
-      <c r="E375" s="3" t="inlineStr">
+      <c r="E375" s="2" t="inlineStr">
         <is>
           <t>The operating system must be configured in accordance with the security configuration settings based on DoD security configuration or implementation guidance, including STIGs, NSA configuration guides, CTOs, and DTMs.</t>
         </is>
       </c>
-      <c r="F375" s="3" t="inlineStr">
+      <c r="F375" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 must be configured in accordance with the security configuration settings based on DoD security configuration or implementation guidance, including STIGs, NSA configuration guides, CTOs, and DTMs.</t>
         </is>
       </c>
-      <c r="G375" s="3" t="inlineStr">
+      <c r="G375" s="2" t="inlineStr">
         <is>
           <t>Configuring the operating system to implement organization-wide security implementation guides and security checklists ensures compliance with federal standards and establishes a common security baseline across DoD that reflects the most restrictive security posture consistent with operational requirements.
 Configuration settings are the set of parameters that can be changed in hardware, software, or firmware components of the system that affect the security posture and/or functionality of the system. Security-related parameters are those parameters impacting the security state of the system, including the parameters required to satisfy other security control requirements. Security-related parameters include, for example: registry settings; account, file, directory permission settings; and settings for functions, ports, protocols, services, and remote connections.</t>
         </is>
       </c>
-      <c r="H375" s="3" t="inlineStr">
+      <c r="H375" s="2" t="inlineStr">
         <is>
           <t>If "write_logs" isn't set to "yes", the Audit logs will
 not be written to the disk.</t>
         </is>
       </c>
-      <c r="I375" s="3" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J375" s="3" t="inlineStr">
+      <c r="I375" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J375" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system is configured in accordance with the security configuration settings based on DoD security configuration or implementation guidance, including STIGs, NSA configuration guides, CTOs, and DTMs. If it is not, this is a finding.</t>
         </is>
       </c>
-      <c r="K375" s="3" t="inlineStr">
+      <c r="K375" s="2" t="inlineStr">
         <is>
           <t>To verify that Audit Daemon is configured to write logs to the disk, run the
 following command:
@@ -30015,16 +30030,21 @@
 If write_logs isn't set to yes, then this is a finding.</t>
         </is>
       </c>
-      <c r="L375" s="3" t="n"/>
-      <c r="M375" s="3" t="inlineStr"/>
-      <c r="N375" s="3" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O375" s="3" t="n"/>
-      <c r="P375" s="3" t="n"/>
-      <c r="Q375" s="3" t="n"/>
+      <c r="L375" s="2" t="n"/>
+      <c r="M375" s="2" t="inlineStr">
+        <is>
+          <t>Edit the file "/etc/audit/auditd.conf" and add or edit the following line:
+write_logs = yes</t>
+        </is>
+      </c>
+      <c r="N375" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O375" s="2" t="n"/>
+      <c r="P375" s="2" t="n"/>
+      <c r="Q375" s="2" t="n"/>
     </row>
     <row r="376" ht="130" customHeight="1">
       <c r="A376" s="3" t="inlineStr">
@@ -30518,7 +30538,7 @@
     <row r="382" ht="130" customHeight="1">
       <c r="A382" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (1),AC-17 (9),CM-6 b</t>
+          <t>AC-17 (9),AC-17 (1),CM-6 b,CM-7 b</t>
         </is>
       </c>
       <c r="B382" s="2" t="inlineStr">
@@ -30596,7 +30616,7 @@
     <row r="383" ht="130" customHeight="1">
       <c r="A383" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (1),CM-6 b</t>
+          <t>CM-6 b,AC-17 (1),CM-7 b</t>
         </is>
       </c>
       <c r="B383" s="2" t="inlineStr">
@@ -35714,7 +35734,7 @@
     <row r="445" ht="130" customHeight="1">
       <c r="A445" s="3" t="inlineStr">
         <is>
-          <t>SI-2 (2),CM-6 b</t>
+          <t>CM-6 b,SI-2 (2)</t>
         </is>
       </c>
       <c r="B445" s="3" t="inlineStr">
@@ -36652,7 +36672,7 @@
     <row r="458" ht="130" customHeight="1">
       <c r="A458" s="3" t="inlineStr">
         <is>
-          <t>AC-12,MA-4 e,MA-4 (7),SC-10</t>
+          <t>AC-12,SC-10,MA-4 e,MA-4 (7)</t>
         </is>
       </c>
       <c r="B458" s="3" t="inlineStr">
@@ -36727,7 +36747,7 @@
     <row r="459" ht="130" customHeight="1">
       <c r="A459" s="3" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B459" s="3" t="inlineStr">
@@ -36806,7 +36826,7 @@
     <row r="460" ht="130" customHeight="1">
       <c r="A460" s="3" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B460" s="3" t="inlineStr">
@@ -36882,7 +36902,7 @@
     <row r="461" ht="130" customHeight="1">
       <c r="A461" s="3" t="inlineStr">
         <is>
-          <t>AC-11 a,SC-10</t>
+          <t>SC-10,AC-11 a</t>
         </is>
       </c>
       <c r="B461" s="3" t="inlineStr">
@@ -36959,7 +36979,7 @@
     <row r="462" ht="130" customHeight="1">
       <c r="A462" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2),SC-8 (1)</t>
+          <t>AC-17 (2),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B462" s="2" t="inlineStr">
@@ -38267,7 +38287,7 @@
     <row r="479" ht="130" customHeight="1">
       <c r="A479" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,IA-3</t>
+          <t>IA-3,CM-7 b</t>
         </is>
       </c>
       <c r="B479" s="2" t="inlineStr">
@@ -38586,7 +38606,7 @@
     <row r="483" ht="130" customHeight="1">
       <c r="A483" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,AC-17 (1)</t>
+          <t>AC-17 (1),CM-7 b</t>
         </is>
       </c>
       <c r="B483" s="2" t="inlineStr">
@@ -41429,7 +41449,7 @@
     <row r="518" ht="130" customHeight="1">
       <c r="A518" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (2)</t>
+          <t>SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B518" s="2" t="inlineStr">
@@ -42619,7 +42639,7 @@
     <row r="533" ht="130" customHeight="1">
       <c r="A533" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2)</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B533" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@39ce2e7b991cdaf0c524c66df3ce2acecdb1bb22 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -550,7 +550,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -634,7 +634,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -719,7 +719,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -791,7 +791,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -971,37 +971,37 @@
       <c r="Q6" s="2" t="n"/>
     </row>
     <row r="7" ht="130" customHeight="1">
-      <c r="A7" s="3" t="inlineStr">
-        <is>
-          <t>AU-5 b,AU-5 a</t>
-        </is>
-      </c>
-      <c r="B7" s="3" t="inlineStr">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>AU-5 a,AU-5 b</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
         <is>
           <t>CCI-000139,CCI-000140</t>
         </is>
       </c>
-      <c r="C7" s="3" t="inlineStr">
+      <c r="C7" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000046-GPOS-00022,SRG-OS-000047-GPOS-00023</t>
         </is>
       </c>
-      <c r="D7" s="3" t="inlineStr">
+      <c r="D7" s="2" t="inlineStr">
         <is>
           <t>CCE-83709-6</t>
         </is>
       </c>
-      <c r="E7" s="3" t="inlineStr">
+      <c r="E7" s="2" t="inlineStr">
         <is>
           <t>The operating system must shut down by default upon audit failure (unless availability is an overriding concern).</t>
         </is>
       </c>
-      <c r="F7" s="3" t="inlineStr">
+      <c r="F7" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 must shut down by default upon audit failure (unless availability is an overriding concern).</t>
         </is>
       </c>
-      <c r="G7" s="3" t="inlineStr">
+      <c r="G7" s="2" t="inlineStr">
         <is>
           <t>It is critical that when the operating system is at risk of failing to process audit logs as required, it takes action to mitigate the failure. Audit processing failures include: software/hardware errors; failures in the audit capturing mechanisms; and audit storage capacity being reached or exceeded. Responses to audit failure depend upon the nature of the failure mode.
 When availability is an overriding concern, other approved actions in response to an audit failure are as follows: 
@@ -1009,7 +1009,7 @@
 2) If audit records are sent to a centralized collection server and communication with this server is lost or the server fails, the operating system must queue audit records locally until communication is restored or until the audit records are retrieved manually. Upon restoration of the connection to the centralized collection server, action should be taken to synchronize the local audit data with the collection server.</t>
         </is>
       </c>
-      <c r="H7" s="3" t="inlineStr">
+      <c r="H7" s="2" t="inlineStr">
         <is>
           <t>It is critical for the appropriate personnel to be aware if a system
 is at risk of failing to process audit logs as required. Without this
@@ -1020,17 +1020,17 @@
 exceeded.</t>
         </is>
       </c>
-      <c r="I7" s="3" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J7" s="3" t="inlineStr">
+      <c r="I7" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J7" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system shuts down by default upon audit failure (unless availability is an overriding concern). If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K7" s="3" t="inlineStr">
+      <c r="K7" s="2" t="inlineStr">
         <is>
           <t>To verify that the system will shutdown when "auditd" fails,
 run the following command:
@@ -1040,16 +1040,28 @@
 If the system is not configured to shutdown on auditd failures, then this is a finding.</t>
         </is>
       </c>
-      <c r="L7" s="3" t="n"/>
-      <c r="M7" s="3" t="inlineStr"/>
-      <c r="N7" s="3" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O7" s="3" t="n"/>
-      <c r="P7" s="3" t="n"/>
-      <c r="Q7" s="3" t="n"/>
+      <c r="L7" s="2" t="n"/>
+      <c r="M7" s="2" t="inlineStr">
+        <is>
+          <t>Configure Red Hat Enterprise Linux 9 to shutdown when auditing failures occur.
+If the auditd daemon is configured to use the augenrules program to read
+audit rules during daemon startup (the default), add the following line to
+the bottom of "/etc/audit/rules.d/immutable.rules":
+-f 2
+If the auditd daemon is configured to use the auditctl utility to read
+audit rules during daemon startup, add the following line to the
+bottom of the /etc/audit/audit.rules file:
+-f 2</t>
+        </is>
+      </c>
+      <c r="N7" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O7" s="2" t="n"/>
+      <c r="P7" s="2" t="n"/>
+      <c r="Q7" s="2" t="n"/>
     </row>
     <row r="8" ht="130" customHeight="1">
       <c r="A8" s="3" t="inlineStr">
@@ -1455,7 +1467,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-7 (1),AU-3 (1),AU-7 a,AU-14 (1),AU-12 a,AU-6 (4),CM-6 b,MA-4 (1) (a),CM-5 (1)</t>
+          <t>CM-6 b,CM-5 (1),AU-6 (4),AU-7 (1),AU-7 a,AU-3 (1),AU-12 a,MA-4 (1) (a),AU-14 (1),AU-3</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -1540,7 +1552,7 @@
     <row r="14" ht="130" customHeight="1">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -1616,7 +1628,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1770,7 +1782,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -2140,7 +2152,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -2214,7 +2226,7 @@
     <row r="23" ht="130" customHeight="1">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -3258,7 +3270,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-14 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-14 (1),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3349,7 +3361,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-14 (1)</t>
+          <t>AU-14 (1),AU-4</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3438,7 +3450,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-4 (1)</t>
+          <t>AU-4 (1),AU-3</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3832,7 +3844,7 @@
     <row r="44" ht="130" customHeight="1">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-6 (4),CM-6 b</t>
+          <t>AU-6 (4),CM-6 b,AU-4 (1)</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
@@ -3908,7 +3920,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),CM-6 b</t>
+          <t>CM-6 b,AU-4 (1)</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3993,7 +4005,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (a),AU-8 b,AU-8 (1) (b)</t>
+          <t>AU-8 b,AU-8 (1) (b),AU-8 (1) (a)</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -4148,7 +4160,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4234,7 +4246,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (1),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (1),IA-2 (11)</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4318,7 +4330,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>SI-6 d,CM-3 (5),SI-6 b</t>
+          <t>CM-3 (5),SI-6 d,SI-6 b</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4410,7 +4422,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>SI-6 d,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 d</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -4494,7 +4506,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -4569,7 +4581,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -4644,7 +4656,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -4719,7 +4731,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -4794,7 +4806,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -4869,7 +4881,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -4944,7 +4956,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -5019,7 +5031,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -5094,7 +5106,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -5169,7 +5181,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-7 a,AU-12 (3),AU-7 b,AU-12 a,CM-6 b,AU-12 c,AU-8 b,CM-5 (1)</t>
+          <t>CM-6 b,CM-5 (1),AU-12 (3),AU-7 a,AU-12 a,AU-8 b,AU-7 b,AU-12 c</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5243,7 +5255,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AC-2 (4),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AC-2 (4),AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5324,7 +5336,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AC-2 (4),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AC-2 (4),AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5405,7 +5417,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AC-2 (4),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AC-2 (4),AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5487,7 +5499,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AC-2 (4),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AC-2 (4),AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5569,7 +5581,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AC-2 (4),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AC-2 (4),AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5651,7 +5663,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AC-2 (4),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AC-2 (4),AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5733,7 +5745,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AC-2 (4),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AC-2 (4),AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5889,7 +5901,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5972,7 +5984,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -6050,7 +6062,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -6141,7 +6153,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6223,7 +6235,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6853,7 +6865,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -6927,7 +6939,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -7001,7 +7013,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -7075,7 +7087,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -7155,7 +7167,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -7240,7 +7252,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>AC-17 (2),MA-4 (6)</t>
+          <t>MA-4 (6),AC-17 (2)</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -7316,7 +7328,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -7651,7 +7663,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -7726,7 +7738,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -7801,7 +7813,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -7876,7 +7888,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -7956,7 +7968,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -8038,7 +8050,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -8120,7 +8132,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8202,7 +8214,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8284,7 +8296,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8366,7 +8378,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -8446,7 +8458,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -8526,7 +8538,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -9354,7 +9366,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),MA-4 c,SC-8,SC-13</t>
+          <t>SC-13,SC-8,MA-4 c,AC-17 (2)</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9514,7 +9526,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9670,7 +9682,7 @@
     <row r="117" ht="130" customHeight="1">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -10026,7 +10038,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -10106,7 +10118,7 @@
     <row r="123" ht="130" customHeight="1">
       <c r="A123" s="2" t="inlineStr">
         <is>
-          <t>SC-28 (1),SC-28</t>
+          <t>SC-28,SC-28 (1)</t>
         </is>
       </c>
       <c r="B123" s="2" t="inlineStr">
@@ -10873,7 +10885,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10954,7 +10966,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -11040,7 +11052,7 @@
     <row r="135" ht="130" customHeight="1">
       <c r="A135" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B135" s="2" t="inlineStr">
@@ -11486,7 +11498,7 @@
     <row r="140" ht="130" customHeight="1">
       <c r="A140" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B140" s="3" t="inlineStr">
@@ -11566,7 +11578,7 @@
     <row r="141" ht="130" customHeight="1">
       <c r="A141" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B141" s="3" t="inlineStr">
@@ -11646,7 +11658,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B142" s="3" t="inlineStr">
@@ -12429,7 +12441,7 @@
     <row r="152" ht="130" customHeight="1">
       <c r="A152" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B152" s="2" t="inlineStr">
@@ -12505,7 +12517,7 @@
     <row r="153" ht="130" customHeight="1">
       <c r="A153" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B153" s="2" t="inlineStr">
@@ -12590,7 +12602,7 @@
     <row r="154" ht="130" customHeight="1">
       <c r="A154" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B154" s="2" t="inlineStr">
@@ -12747,7 +12759,7 @@
     <row r="156" ht="130" customHeight="1">
       <c r="A156" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-7 a</t>
+          <t>CM-7 a,IA-7</t>
         </is>
       </c>
       <c r="B156" s="2" t="inlineStr">
@@ -12826,7 +12838,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B157" s="3" t="inlineStr">
@@ -13049,7 +13061,7 @@
     <row r="160" ht="130" customHeight="1">
       <c r="A160" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B160" s="3" t="inlineStr">
@@ -13134,7 +13146,7 @@
     <row r="161" ht="130" customHeight="1">
       <c r="A161" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B161" s="3" t="inlineStr">
@@ -13209,7 +13221,7 @@
     <row r="162" ht="130" customHeight="1">
       <c r="A162" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B162" s="3" t="inlineStr">
@@ -13284,7 +13296,7 @@
     <row r="163" ht="130" customHeight="1">
       <c r="A163" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B163" s="3" t="inlineStr">
@@ -13359,7 +13371,7 @@
     <row r="164" ht="130" customHeight="1">
       <c r="A164" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B164" s="3" t="inlineStr">
@@ -13862,7 +13874,7 @@
     <row r="171" ht="130" customHeight="1">
       <c r="A171" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B171" s="3" t="inlineStr">
@@ -14151,7 +14163,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B175" s="3" t="inlineStr">
@@ -14226,7 +14238,7 @@
     <row r="176" ht="130" customHeight="1">
       <c r="A176" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B176" s="3" t="inlineStr">
@@ -14308,7 +14320,7 @@
     <row r="177" ht="130" customHeight="1">
       <c r="A177" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B177" s="3" t="inlineStr">
@@ -14390,7 +14402,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B178" s="3" t="inlineStr">
@@ -14472,7 +14484,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B179" s="3" t="inlineStr">
@@ -14554,7 +14566,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B180" s="3" t="inlineStr">
@@ -14636,7 +14648,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B181" s="3" t="inlineStr">
@@ -14718,7 +14730,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B182" s="3" t="inlineStr">
@@ -14800,7 +14812,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B183" s="3" t="inlineStr">
@@ -14882,7 +14894,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B184" s="3" t="inlineStr">
@@ -14964,7 +14976,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B185" s="3" t="inlineStr">
@@ -15042,7 +15054,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B186" s="3" t="inlineStr">
@@ -15121,7 +15133,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B187" s="3" t="inlineStr">
@@ -15203,7 +15215,7 @@
     <row r="188" ht="130" customHeight="1">
       <c r="A188" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B188" s="3" t="inlineStr">
@@ -15285,7 +15297,7 @@
     <row r="189" ht="130" customHeight="1">
       <c r="A189" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B189" s="3" t="inlineStr">
@@ -15367,7 +15379,7 @@
     <row r="190" ht="130" customHeight="1">
       <c r="A190" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B190" s="3" t="inlineStr">
@@ -15449,7 +15461,7 @@
     <row r="191" ht="130" customHeight="1">
       <c r="A191" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B191" s="3" t="inlineStr">
@@ -15531,7 +15543,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B192" s="3" t="inlineStr">
@@ -15613,7 +15625,7 @@
     <row r="193" ht="130" customHeight="1">
       <c r="A193" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B193" s="3" t="inlineStr">
@@ -15688,7 +15700,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AC-2 (4),AU-12 a,AU-12 c,MA-4 (1) (a)</t>
+          <t>AC-2 (4),AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B194" s="3" t="inlineStr">
@@ -15761,7 +15773,7 @@
     <row r="195" ht="130" customHeight="1">
       <c r="A195" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-3 (1),AC-2 (4),AU-12 c,MA-4 (1) (a)</t>
+          <t>AC-2 (4),AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c</t>
         </is>
       </c>
       <c r="B195" s="3" t="inlineStr">
@@ -15838,7 +15850,7 @@
     <row r="196" ht="130" customHeight="1">
       <c r="A196" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (2),IA-2 (1),IA-2 (4)</t>
+          <t>IA-2 (3),IA-2 (4),IA-2 (1),IA-2 (2)</t>
         </is>
       </c>
       <c r="B196" s="2" t="inlineStr">
@@ -15925,7 +15937,7 @@
     <row r="197" ht="130" customHeight="1">
       <c r="A197" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2,IA-2 (2),IA-2 (3),IA-2 (5)</t>
+          <t>IA-2 (3),IA-2 (5),IA-2 (4),IA-2 (2),IA-2</t>
         </is>
       </c>
       <c r="B197" s="2" t="inlineStr">
@@ -16014,7 +16026,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2,IA-2 (2),IA-2 (3),IA-2 (5)</t>
+          <t>IA-2 (3),IA-2 (5),IA-2 (4),IA-2 (2),IA-2</t>
         </is>
       </c>
       <c r="B198" s="2" t="inlineStr">
@@ -16258,7 +16270,7 @@
     <row r="201" ht="130" customHeight="1">
       <c r="A201" s="2" t="inlineStr">
         <is>
-          <t>AC-3 (4),IA-11</t>
+          <t>IA-11,AC-3 (4)</t>
         </is>
       </c>
       <c r="B201" s="2" t="inlineStr">
@@ -16638,7 +16650,7 @@
     <row r="206" ht="130" customHeight="1">
       <c r="A206" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8 (1),SC-8</t>
+          <t>SC-8 (1),SC-8,SC-8 (2)</t>
         </is>
       </c>
       <c r="B206" s="2" t="inlineStr">
@@ -16715,7 +16727,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8 (1),SC-8</t>
+          <t>SC-8 (1),SC-8,SC-8 (2)</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -16801,7 +16813,7 @@
     <row r="208" ht="130" customHeight="1">
       <c r="A208" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),AC-18 (1),SC-8</t>
+          <t>SC-8 (1),SC-8,AC-18 (1)</t>
         </is>
       </c>
       <c r="B208" s="2" t="inlineStr">
@@ -17229,7 +17241,7 @@
     <row r="213" ht="130" customHeight="1">
       <c r="A213" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-7 a,CM-6 b</t>
+          <t>CM-7 a,IA-5 (1) (c),CM-6 b</t>
         </is>
       </c>
       <c r="B213" s="2" t="inlineStr">
@@ -17389,7 +17401,7 @@
     <row r="215" ht="130" customHeight="1">
       <c r="A215" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,CM-6 b</t>
+          <t>CM-6 b,AU-12 a</t>
         </is>
       </c>
       <c r="B215" s="2" t="inlineStr">
@@ -17480,7 +17492,7 @@
     <row r="216" ht="130" customHeight="1">
       <c r="A216" s="2" t="inlineStr">
         <is>
-          <t>SC-5 (2),SC-5,CM-6 b</t>
+          <t>CM-6 b,SC-5 (2),SC-5</t>
         </is>
       </c>
       <c r="B216" s="2" t="inlineStr">
@@ -17752,7 +17764,7 @@
     <row r="219" ht="130" customHeight="1">
       <c r="A219" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-6 b</t>
+          <t>CM-6 b,SI-16</t>
         </is>
       </c>
       <c r="B219" s="2" t="inlineStr">
@@ -17850,7 +17862,7 @@
     <row r="220" ht="130" customHeight="1">
       <c r="A220" s="2" t="inlineStr">
         <is>
-          <t>IA-2,AU-3 (1),IA-8</t>
+          <t>AU-3 (1),IA-2,IA-8</t>
         </is>
       </c>
       <c r="B220" s="2" t="inlineStr">
@@ -18829,7 +18841,7 @@
     <row r="232" ht="130" customHeight="1">
       <c r="A232" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SI-16,CM-6 b</t>
+          <t>SC-2,CM-6 b,SI-16</t>
         </is>
       </c>
       <c r="B232" s="2" t="inlineStr">
@@ -19175,7 +19187,7 @@
     <row r="236" ht="130" customHeight="1">
       <c r="A236" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),CM-7 a</t>
+          <t>CM-7 a,AC-18 (1)</t>
         </is>
       </c>
       <c r="B236" s="2" t="inlineStr">
@@ -19742,7 +19754,7 @@
     <row r="243" ht="130" customHeight="1">
       <c r="A243" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (b),IA-5 (1) (a),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (a),IA-5 (1) (b)</t>
         </is>
       </c>
       <c r="B243" s="2" t="inlineStr">
@@ -20310,7 +20322,7 @@
     <row r="250" ht="130" customHeight="1">
       <c r="A250" s="2" t="inlineStr">
         <is>
-          <t>SC-4,CM-6 b</t>
+          <t>CM-6 b,SC-4</t>
         </is>
       </c>
       <c r="B250" s="2" t="inlineStr">
@@ -20566,7 +20578,7 @@
     <row r="253" ht="130" customHeight="1">
       <c r="A253" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (1)</t>
+          <t>IA-2 (1),IA-2 (11)</t>
         </is>
       </c>
       <c r="B253" s="2" t="inlineStr">
@@ -20655,7 +20667,7 @@
     <row r="254" ht="130" customHeight="1">
       <c r="A254" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B254" s="2" t="inlineStr">
@@ -20986,7 +20998,7 @@
     <row r="258" ht="130" customHeight="1">
       <c r="A258" s="2" t="inlineStr">
         <is>
-          <t>SC-3,SI-6 a</t>
+          <t>SI-6 a,SC-3</t>
         </is>
       </c>
       <c r="B258" s="2" t="inlineStr">
@@ -21697,7 +21709,7 @@
     <row r="267" ht="130" customHeight="1">
       <c r="A267" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (3),CM-6 b</t>
+          <t>CM-6 b,CM-5 (3)</t>
         </is>
       </c>
       <c r="B267" s="2" t="inlineStr">
@@ -22387,7 +22399,7 @@
     <row r="275" ht="130" customHeight="1">
       <c r="A275" s="3" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B275" s="3" t="inlineStr">
@@ -23823,136 +23835,144 @@
       <c r="Q292" s="3" t="n"/>
     </row>
     <row r="293" ht="130" customHeight="1">
-      <c r="A293" s="3" t="inlineStr">
+      <c r="A293" s="2" t="inlineStr">
         <is>
           <t>AU-5 a</t>
         </is>
       </c>
-      <c r="B293" s="3" t="inlineStr">
+      <c r="B293" s="2" t="inlineStr">
         <is>
           <t>CCI-000139,CCI-000366</t>
         </is>
       </c>
-      <c r="C293" s="3" t="inlineStr">
+      <c r="C293" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000046-GPOS-00022</t>
         </is>
       </c>
-      <c r="D293" s="3" t="inlineStr">
+      <c r="D293" s="2" t="inlineStr">
         <is>
           <t>CCE-90826-9</t>
         </is>
       </c>
-      <c r="E293" s="3" t="inlineStr">
+      <c r="E293" s="2" t="inlineStr">
         <is>
           <t>The operating system must alert the ISSO and SA (at a minimum) in the event of an audit processing failure.</t>
         </is>
       </c>
-      <c r="F293" s="3" t="inlineStr">
+      <c r="F293" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 must alert the ISSO and SA (at a minimum) in the event of an audit processing failure.</t>
         </is>
       </c>
-      <c r="G293" s="3" t="inlineStr">
+      <c r="G293" s="2" t="inlineStr">
         <is>
           <t>It is critical for the appropriate personnel to be aware if a system is at risk of failing to process audit logs as required. Without this notification, the security personnel may be unaware of an impending failure of the audit capability, and system operation may be adversely affected.
 Audit processing failures include software/hardware errors, failures in the audit capturing mechanisms, and audit storage capacity being reached or exceeded.
 This requirement applies to each audit data storage repository (i.e., distinct information system component where audit records are stored), the centralized audit storage capacity of organizations (i.e., all audit data storage repositories combined), or both.</t>
         </is>
       </c>
-      <c r="H293" s="3" t="inlineStr">
+      <c r="H293" s="2" t="inlineStr">
         <is>
           <t>A number of system services utilize email messages sent to the root user to
 notify system administrators of active or impending issues.  These messages must
 be forwarded to at least one monitored email address.</t>
         </is>
       </c>
-      <c r="I293" s="3" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J293" s="3" t="inlineStr">
+      <c r="I293" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J293" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system alerts the ISSO and SA (at a minimum) in the event of an audit processing failure. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K293" s="3" t="inlineStr">
+      <c r="K293" s="2" t="inlineStr">
         <is>
           <t>Find the list of alias maps used by the Postfix mail server:
  $ sudo postconf alias_maps 
 Query the Postfix alias maps for an alias for the  root  user:
  $ sudo postmap -q root hash:/etc/aliases 
 The output should return an alias.
-If it is not, then this is a finding.</t>
-        </is>
-      </c>
-      <c r="L293" s="3" t="n"/>
-      <c r="M293" s="3" t="inlineStr"/>
-      <c r="N293" s="3" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O293" s="3" t="n"/>
-      <c r="P293" s="3" t="n"/>
-      <c r="Q293" s="3" t="n"/>
+If the alias is not set, then this is a finding.</t>
+        </is>
+      </c>
+      <c r="L293" s="2" t="n"/>
+      <c r="M293" s="2" t="inlineStr">
+        <is>
+          <t>Configure a valid email address as an alias for the root account.
+Append the following line to "/etc/aliases":
+root: system.administrator@mail.mil
+Then, run the following command:
+$ sudo newaliases</t>
+        </is>
+      </c>
+      <c r="N293" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O293" s="2" t="n"/>
+      <c r="P293" s="2" t="n"/>
+      <c r="Q293" s="2" t="n"/>
     </row>
     <row r="294" ht="130" customHeight="1">
-      <c r="A294" s="3" t="inlineStr">
-        <is>
-          <t>AU-5 (1),AU-5 a</t>
-        </is>
-      </c>
-      <c r="B294" s="3" t="inlineStr">
+      <c r="A294" s="2" t="inlineStr">
+        <is>
+          <t>AU-5 a,AU-5 (1)</t>
+        </is>
+      </c>
+      <c r="B294" s="2" t="inlineStr">
         <is>
           <t>CCI-000139,CCI-001855</t>
         </is>
       </c>
-      <c r="C294" s="3" t="inlineStr">
+      <c r="C294" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000046-GPOS-00022,SRG-OS-000343-GPOS-00134</t>
         </is>
       </c>
-      <c r="D294" s="3" t="inlineStr">
+      <c r="D294" s="2" t="inlineStr">
         <is>
           <t>CCE-83698-1</t>
         </is>
       </c>
-      <c r="E294" s="3" t="inlineStr">
+      <c r="E294" s="2" t="inlineStr">
         <is>
           <t>The operating system must alert the ISSO and SA (at a minimum) in the event of an audit processing failure.</t>
         </is>
       </c>
-      <c r="F294" s="3" t="inlineStr">
+      <c r="F294" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 must alert the ISSO and SA (at a minimum) in the event of an audit processing failure.</t>
         </is>
       </c>
-      <c r="G294" s="3" t="inlineStr">
+      <c r="G294" s="2" t="inlineStr">
         <is>
           <t>It is critical for the appropriate personnel to be aware if a system is at risk of failing to process audit logs as required. Without this notification, the security personnel may be unaware of an impending failure of the audit capability, and system operation may be adversely affected.
 Audit processing failures include software/hardware errors, failures in the audit capturing mechanisms, and audit storage capacity being reached or exceeded.
 This requirement applies to each audit data storage repository (i.e., distinct information system component where audit records are stored), the centralized audit storage capacity of organizations (i.e., all audit data storage repositories combined), or both.</t>
         </is>
       </c>
-      <c r="H294" s="3" t="inlineStr">
+      <c r="H294" s="2" t="inlineStr">
         <is>
           <t>Email sent to the root account is typically aliased to the
 administrators of the system, who can take appropriate action.</t>
         </is>
       </c>
-      <c r="I294" s="3" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J294" s="3" t="inlineStr">
+      <c r="I294" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J294" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system alerts the ISSO and SA (at a minimum) in the event of an audit processing failure. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K294" s="3" t="inlineStr">
+      <c r="K294" s="2" t="inlineStr">
         <is>
           <t>Inspect "/etc/audit/auditd.conf" and locate the following line to
 determine if the system is configured to send email to an
@@ -23961,16 +23981,22 @@
 If auditd is not configured to send emails per identified actions, then this is a finding.</t>
         </is>
       </c>
-      <c r="L294" s="3" t="n"/>
-      <c r="M294" s="3" t="inlineStr"/>
-      <c r="N294" s="3" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O294" s="3" t="n"/>
-      <c r="P294" s="3" t="n"/>
-      <c r="Q294" s="3" t="n"/>
+      <c r="L294" s="2" t="n"/>
+      <c r="M294" s="2" t="inlineStr">
+        <is>
+          <t>Configure "auditd" service to notify the SA and ISSO in the event of an audit processing failure.
+Edit the following line in "/etc/audit/auditd.conf" to ensure that administrators are notified via email for those situations:
+action_mail_acct = root</t>
+        </is>
+      </c>
+      <c r="N294" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O294" s="2" t="n"/>
+      <c r="P294" s="2" t="n"/>
+      <c r="Q294" s="2" t="n"/>
     </row>
     <row r="295" ht="130" customHeight="1">
       <c r="A295" s="3" t="inlineStr">
@@ -27263,7 +27289,7 @@
     <row r="339" ht="130" customHeight="1">
       <c r="A339" s="3" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B339" s="3" t="inlineStr">
@@ -27413,7 +27439,7 @@
     <row r="341" ht="130" customHeight="1">
       <c r="A341" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),CM-6 b</t>
+          <t>CM-6 b,IA-2 (2)</t>
         </is>
       </c>
       <c r="B341" s="2" t="inlineStr">
@@ -27494,7 +27520,7 @@
     <row r="342" ht="130" customHeight="1">
       <c r="A342" s="3" t="inlineStr">
         <is>
-          <t>CM-5 (1),CM-6 b</t>
+          <t>CM-6 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B342" s="3" t="inlineStr">
@@ -27568,7 +27594,7 @@
     <row r="343" ht="130" customHeight="1">
       <c r="A343" s="3" t="inlineStr">
         <is>
-          <t>CM-5 (1),CM-6 b</t>
+          <t>CM-6 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B343" s="3" t="inlineStr">
@@ -28153,7 +28179,7 @@
     <row r="351" ht="130" customHeight="1">
       <c r="A351" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),CM-6 b</t>
+          <t>CM-6 b,AC-17 (2)</t>
         </is>
       </c>
       <c r="B351" s="2" t="inlineStr">
@@ -29890,7 +29916,7 @@
     <row r="374" ht="130" customHeight="1">
       <c r="A374" s="2" t="inlineStr">
         <is>
-          <t>AU-3,CM-6 b</t>
+          <t>CM-6 b,AU-3</t>
         </is>
       </c>
       <c r="B374" s="2" t="inlineStr">
@@ -30144,7 +30170,7 @@
     <row r="377" ht="130" customHeight="1">
       <c r="A377" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B377" s="2" t="inlineStr">
@@ -30538,7 +30564,7 @@
     <row r="382" ht="130" customHeight="1">
       <c r="A382" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (9),AC-17 (1),CM-6 b,CM-7 b</t>
+          <t>AC-17 (1),AC-17 (9),CM-7 b,CM-6 b</t>
         </is>
       </c>
       <c r="B382" s="2" t="inlineStr">
@@ -30616,7 +30642,7 @@
     <row r="383" ht="130" customHeight="1">
       <c r="A383" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-17 (1),CM-7 b</t>
+          <t>AC-17 (1),CM-7 b,CM-6 b</t>
         </is>
       </c>
       <c r="B383" s="2" t="inlineStr">
@@ -33115,7 +33141,7 @@
     <row r="412" ht="130" customHeight="1">
       <c r="A412" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B412" s="2" t="inlineStr">
@@ -33197,7 +33223,7 @@
     <row r="413" ht="130" customHeight="1">
       <c r="A413" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B413" s="2" t="inlineStr">
@@ -33890,7 +33916,7 @@
     <row r="422" ht="130" customHeight="1">
       <c r="A422" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B422" s="2" t="inlineStr">
@@ -34493,7 +34519,7 @@
     <row r="429" ht="130" customHeight="1">
       <c r="A429" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B429" s="2" t="inlineStr">
@@ -34945,7 +34971,7 @@
     <row r="435" ht="130" customHeight="1">
       <c r="A435" s="2" t="inlineStr">
         <is>
-          <t>AU-4,CM-6 b</t>
+          <t>CM-6 b,AU-4</t>
         </is>
       </c>
       <c r="B435" s="2" t="inlineStr">
@@ -35249,7 +35275,7 @@
     <row r="439" ht="130" customHeight="1">
       <c r="A439" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B439" s="2" t="inlineStr">
@@ -35339,7 +35365,7 @@
     <row r="440" ht="130" customHeight="1">
       <c r="A440" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B440" s="2" t="inlineStr">
@@ -36381,7 +36407,7 @@
     <row r="454" ht="130" customHeight="1">
       <c r="A454" s="3" t="inlineStr">
         <is>
-          <t>SI-2 (2),CM-6 b</t>
+          <t>CM-6 b,SI-2 (2)</t>
         </is>
       </c>
       <c r="B454" s="3" t="inlineStr">
@@ -36672,7 +36698,7 @@
     <row r="458" ht="130" customHeight="1">
       <c r="A458" s="3" t="inlineStr">
         <is>
-          <t>AC-12,SC-10,MA-4 e,MA-4 (7)</t>
+          <t>MA-4 e,SC-10,MA-4 (7),AC-12</t>
         </is>
       </c>
       <c r="B458" s="3" t="inlineStr">
@@ -36979,7 +37005,7 @@
     <row r="462" ht="130" customHeight="1">
       <c r="A462" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8 (1),SC-8</t>
+          <t>SC-8 (1),SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B462" s="2" t="inlineStr">
@@ -38287,7 +38313,7 @@
     <row r="479" ht="130" customHeight="1">
       <c r="A479" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-7 b</t>
+          <t>CM-7 b,IA-3</t>
         </is>
       </c>
       <c r="B479" s="2" t="inlineStr">
@@ -39729,7 +39755,7 @@
     <row r="497" ht="130" customHeight="1">
       <c r="A497" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-4 (1)</t>
+          <t>AU-4 (1),AU-4</t>
         </is>
       </c>
       <c r="B497" s="2" t="inlineStr">
@@ -39980,7 +40006,7 @@
     <row r="500" ht="130" customHeight="1">
       <c r="A500" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B500" s="2" t="inlineStr">
@@ -40082,7 +40108,7 @@
     <row r="501" ht="130" customHeight="1">
       <c r="A501" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B501" s="2" t="inlineStr">
@@ -40192,7 +40218,7 @@
     <row r="502" ht="130" customHeight="1">
       <c r="A502" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B502" s="2" t="inlineStr">
@@ -40303,7 +40329,7 @@
     <row r="503" ht="130" customHeight="1">
       <c r="A503" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
+          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
         </is>
       </c>
       <c r="B503" s="2" t="inlineStr">
@@ -41449,7 +41475,7 @@
     <row r="518" ht="130" customHeight="1">
       <c r="A518" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8</t>
+          <t>SC-8,SC-8 (2)</t>
         </is>
       </c>
       <c r="B518" s="2" t="inlineStr">
@@ -42639,7 +42665,7 @@
     <row r="533" ht="130" customHeight="1">
       <c r="A533" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),SC-8</t>
+          <t>SC-8,AC-17 (2)</t>
         </is>
       </c>
       <c r="B533" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@36b4f501a63d0d344733b36a91e7d63839ce31f4 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -550,7 +550,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -634,7 +634,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -719,7 +719,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -791,7 +791,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -973,7 +973,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 b</t>
+          <t>AU-5 b,AU-5 a</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1439,11 +1439,11 @@
       </c>
       <c r="K12" s="2" t="inlineStr">
         <is>
-          <t>For every temporary and emergency account, run the following command
+          <t>For every temporary account, run the following command
 to obtain its account aging and expiration information:
  $ sudo chage -l  USER  
 Verify each of these accounts has an expiration date set as documented.
-If any temporary or emergency accounts have no expiration date set or do not expire within a documented time frame, then this is a finding.</t>
+If any temporary accounts have no expiration date set or do not expire within a documented time frame, then this is a finding.</t>
         </is>
       </c>
       <c r="L12" s="2" t="n"/>
@@ -1467,7 +1467,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (1),AU-6 (4),AU-7 (1),AU-7 a,AU-3 (1),AU-12 a,MA-4 (1) (a),AU-14 (1),AU-3</t>
+          <t>AU-14 (1),AU-12 a,AU-7 (1),AU-6 (4),AU-3,CM-5 (1),AU-3 (1),MA-4 (1) (a),AU-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -1782,7 +1782,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -2152,7 +2152,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -2226,7 +2226,7 @@
     <row r="23" ht="130" customHeight="1">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -3270,7 +3270,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-14 (1),AU-3,AU-12 c</t>
+          <t>AU-14 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3844,7 +3844,7 @@
     <row r="44" ht="130" customHeight="1">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>AU-6 (4),CM-6 b,AU-4 (1)</t>
+          <t>AU-4 (1),AU-6 (4),CM-6 b</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
@@ -3920,7 +3920,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-4 (1)</t>
+          <t>AU-4 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -4005,7 +4005,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-8 (1) (b),AU-8 (1) (a)</t>
+          <t>AU-8 (1) (a),AU-8 (1) (b),AU-8 b</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -4160,7 +4160,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4246,7 +4246,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (1),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12),IA-2 (1)</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4330,7 +4330,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 d,SI-6 b</t>
+          <t>SI-6 d,CM-3 (5),SI-6 b</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4422,7 +4422,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 d</t>
+          <t>SI-6 d,CM-3 (5)</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -4506,7 +4506,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -4581,7 +4581,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -4656,7 +4656,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -4731,7 +4731,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -4806,7 +4806,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -4881,7 +4881,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -4956,7 +4956,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -5031,7 +5031,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -5106,7 +5106,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -5181,7 +5181,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (1),AU-12 (3),AU-7 a,AU-12 a,AU-8 b,AU-7 b,AU-12 c</t>
+          <t>AU-12 a,AU-8 b,AU-12 (3),CM-5 (1),AU-7 b,AU-7 a,AU-12 c,CM-6 b</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5255,7 +5255,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,AC-2 (4),MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5336,7 +5336,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,AC-2 (4),MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5417,7 +5417,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,AC-2 (4),MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5499,7 +5499,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,AC-2 (4),MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5581,7 +5581,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,AC-2 (4),MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5663,7 +5663,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,AC-2 (4),MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5745,7 +5745,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,AC-2 (4),MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5827,7 +5827,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5),SI-6 a</t>
+          <t>SI-6 a,CM-3 (5)</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -6865,7 +6865,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -6939,7 +6939,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -7013,7 +7013,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -7087,7 +7087,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -7252,7 +7252,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (6),AC-17 (2)</t>
+          <t>AC-17 (2),MA-4 (6)</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -7511,7 +7511,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>AU-9,AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -7587,7 +7587,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>AU-9,AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -7663,7 +7663,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -7738,7 +7738,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -7813,7 +7813,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -7888,7 +7888,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -7968,7 +7968,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -8050,7 +8050,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -8132,7 +8132,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8214,7 +8214,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8296,7 +8296,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8378,7 +8378,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -8458,7 +8458,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -8538,7 +8538,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -8618,7 +8618,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 (1)</t>
+          <t>AC-11 (1),AC-11 b</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8789,7 +8789,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-6 (10)</t>
+          <t>AC-6 (10),AC-11 b</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8868,7 +8868,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8947,7 +8947,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -9034,7 +9034,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -9121,7 +9121,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -9366,7 +9366,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>SC-13,SC-8,MA-4 c,AC-17 (2)</t>
+          <t>SC-13,AC-17 (2),SC-8,MA-4 c</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9526,7 +9526,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9682,7 +9682,7 @@
     <row r="117" ht="130" customHeight="1">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -10038,7 +10038,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -10118,7 +10118,7 @@
     <row r="123" ht="130" customHeight="1">
       <c r="A123" s="2" t="inlineStr">
         <is>
-          <t>SC-28,SC-28 (1)</t>
+          <t>SC-28 (1),SC-28</t>
         </is>
       </c>
       <c r="B123" s="2" t="inlineStr">
@@ -10235,7 +10235,14 @@
 Techniques used to address this include protocols using nonces (e.g., numbers generated for a specific one-time use) or challenges (e.g., TLS, WS_Security). Additional techniques include time-synchronous or challenge-response one-time authenticators.</t>
         </is>
       </c>
-      <c r="H124" s="2" t="inlineStr"/>
+      <c r="H124" s="2" t="inlineStr">
+        <is>
+          <t>A replay attack may enable an unauthorized user to gain access to Red Hat Enterprise Linux 9. Authentication sessions between the authenticator and Red Hat Enterprise Linux 9 validating the user credentials must not be vulnerable to a replay attack.
+An authentication process resists replay attacks if it is impractical to achieve a successful authentication by recording and replaying a previous authentication message.
+A privileged account is any information system account with authorizations of a privileged user.
+Techniques used to address this include protocols using nonces (e.g., numbers generated for a specific one-time use) or challenges (e.g., TLS, WS_Security). Additional techniques include time-synchronous or challenge-response one-time authenticators.</t>
+        </is>
+      </c>
       <c r="I124" s="2" t="inlineStr">
         <is>
           <t>Applicable - Inherently Met</t>
@@ -10885,7 +10892,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10966,7 +10973,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -11052,7 +11059,7 @@
     <row r="135" ht="130" customHeight="1">
       <c r="A135" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B135" s="2" t="inlineStr">
@@ -11145,7 +11152,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>AC-3 (4),AC-6 (10)</t>
+          <t>AC-6 (10),AC-3 (4)</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -11242,7 +11249,7 @@
     <row r="137" ht="130" customHeight="1">
       <c r="A137" s="2" t="inlineStr">
         <is>
-          <t>AC-3 (4),AC-6 (10)</t>
+          <t>AC-6 (10),AC-3 (4)</t>
         </is>
       </c>
       <c r="B137" s="2" t="inlineStr">
@@ -11498,7 +11505,7 @@
     <row r="140" ht="130" customHeight="1">
       <c r="A140" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B140" s="3" t="inlineStr">
@@ -11578,7 +11585,7 @@
     <row r="141" ht="130" customHeight="1">
       <c r="A141" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B141" s="3" t="inlineStr">
@@ -11658,7 +11665,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B142" s="3" t="inlineStr">
@@ -12280,7 +12287,7 @@
     <row r="150" ht="130" customHeight="1">
       <c r="A150" s="2" t="inlineStr">
         <is>
-          <t>AC-11 (1),AC-11 a</t>
+          <t>AC-11 a,AC-11 (1)</t>
         </is>
       </c>
       <c r="B150" s="2" t="inlineStr">
@@ -12441,7 +12448,7 @@
     <row r="152" ht="130" customHeight="1">
       <c r="A152" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B152" s="2" t="inlineStr">
@@ -12517,7 +12524,7 @@
     <row r="153" ht="130" customHeight="1">
       <c r="A153" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B153" s="2" t="inlineStr">
@@ -12602,7 +12609,7 @@
     <row r="154" ht="130" customHeight="1">
       <c r="A154" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-7</t>
+          <t>IA-7,CM-6 b</t>
         </is>
       </c>
       <c r="B154" s="2" t="inlineStr">
@@ -12759,7 +12766,7 @@
     <row r="156" ht="130" customHeight="1">
       <c r="A156" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,IA-7</t>
+          <t>IA-7,CM-7 a</t>
         </is>
       </c>
       <c r="B156" s="2" t="inlineStr">
@@ -12838,7 +12845,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B157" s="3" t="inlineStr">
@@ -12915,7 +12922,7 @@
     <row r="158" ht="130" customHeight="1">
       <c r="A158" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B158" s="3" t="inlineStr">
@@ -12988,7 +12995,7 @@
     <row r="159" ht="130" customHeight="1">
       <c r="A159" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
+          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3</t>
         </is>
       </c>
       <c r="B159" s="3" t="inlineStr">
@@ -13061,7 +13068,7 @@
     <row r="160" ht="130" customHeight="1">
       <c r="A160" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B160" s="3" t="inlineStr">
@@ -13146,7 +13153,7 @@
     <row r="161" ht="130" customHeight="1">
       <c r="A161" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B161" s="3" t="inlineStr">
@@ -13221,7 +13228,7 @@
     <row r="162" ht="130" customHeight="1">
       <c r="A162" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B162" s="3" t="inlineStr">
@@ -13296,7 +13303,7 @@
     <row r="163" ht="130" customHeight="1">
       <c r="A163" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B163" s="3" t="inlineStr">
@@ -13371,7 +13378,7 @@
     <row r="164" ht="130" customHeight="1">
       <c r="A164" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B164" s="3" t="inlineStr">
@@ -13874,7 +13881,7 @@
     <row r="171" ht="130" customHeight="1">
       <c r="A171" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B171" s="3" t="inlineStr">
@@ -14163,7 +14170,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B175" s="3" t="inlineStr">
@@ -14238,7 +14245,7 @@
     <row r="176" ht="130" customHeight="1">
       <c r="A176" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B176" s="3" t="inlineStr">
@@ -14320,7 +14327,7 @@
     <row r="177" ht="130" customHeight="1">
       <c r="A177" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B177" s="3" t="inlineStr">
@@ -14402,7 +14409,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B178" s="3" t="inlineStr">
@@ -14484,7 +14491,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B179" s="3" t="inlineStr">
@@ -14566,7 +14573,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B180" s="3" t="inlineStr">
@@ -14648,7 +14655,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B181" s="3" t="inlineStr">
@@ -14730,7 +14737,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B182" s="3" t="inlineStr">
@@ -14812,7 +14819,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B183" s="3" t="inlineStr">
@@ -14894,7 +14901,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B184" s="3" t="inlineStr">
@@ -14976,7 +14983,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B185" s="3" t="inlineStr">
@@ -15054,7 +15061,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B186" s="3" t="inlineStr">
@@ -15133,7 +15140,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B187" s="3" t="inlineStr">
@@ -15215,7 +15222,7 @@
     <row r="188" ht="130" customHeight="1">
       <c r="A188" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B188" s="3" t="inlineStr">
@@ -15297,7 +15304,7 @@
     <row r="189" ht="130" customHeight="1">
       <c r="A189" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3</t>
         </is>
       </c>
       <c r="B189" s="3" t="inlineStr">
@@ -15379,7 +15386,7 @@
     <row r="190" ht="130" customHeight="1">
       <c r="A190" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B190" s="3" t="inlineStr">
@@ -15461,7 +15468,7 @@
     <row r="191" ht="130" customHeight="1">
       <c r="A191" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B191" s="3" t="inlineStr">
@@ -15543,7 +15550,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B192" s="3" t="inlineStr">
@@ -15625,7 +15632,7 @@
     <row r="193" ht="130" customHeight="1">
       <c r="A193" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B193" s="3" t="inlineStr">
@@ -15700,7 +15707,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="3" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),AU-12 a,MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-12 a,AU-3,AC-2 (4),MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B194" s="3" t="inlineStr">
@@ -15773,7 +15780,7 @@
     <row r="195" ht="130" customHeight="1">
       <c r="A195" s="3" t="inlineStr">
         <is>
-          <t>AC-2 (4),AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-3,AC-2 (4),MA-4 (1) (a),AU-3 (1),AU-12 c</t>
         </is>
       </c>
       <c r="B195" s="3" t="inlineStr">
@@ -15850,7 +15857,7 @@
     <row r="196" ht="130" customHeight="1">
       <c r="A196" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (4),IA-2 (1),IA-2 (2)</t>
+          <t>IA-2 (2),IA-2 (4),IA-2 (3),IA-2 (1)</t>
         </is>
       </c>
       <c r="B196" s="2" t="inlineStr">
@@ -15937,7 +15944,7 @@
     <row r="197" ht="130" customHeight="1">
       <c r="A197" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (5),IA-2 (4),IA-2 (2),IA-2</t>
+          <t>IA-2 (3),IA-2,IA-2 (4),IA-2 (2),IA-2 (5)</t>
         </is>
       </c>
       <c r="B197" s="2" t="inlineStr">
@@ -16026,7 +16033,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (5),IA-2 (4),IA-2 (2),IA-2</t>
+          <t>IA-2 (3),IA-2,IA-2 (4),IA-2 (2),IA-2 (5)</t>
         </is>
       </c>
       <c r="B198" s="2" t="inlineStr">
@@ -16270,7 +16277,7 @@
     <row r="201" ht="130" customHeight="1">
       <c r="A201" s="2" t="inlineStr">
         <is>
-          <t>IA-11,AC-3 (4)</t>
+          <t>AC-3 (4),IA-11</t>
         </is>
       </c>
       <c r="B201" s="2" t="inlineStr">
@@ -16650,7 +16657,7 @@
     <row r="206" ht="130" customHeight="1">
       <c r="A206" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8,SC-8 (2)</t>
+          <t>SC-8 (2),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B206" s="2" t="inlineStr">
@@ -16727,7 +16734,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8,SC-8 (2)</t>
+          <t>SC-8 (2),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -16813,7 +16820,7 @@
     <row r="208" ht="130" customHeight="1">
       <c r="A208" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8,AC-18 (1)</t>
+          <t>SC-8,SC-8 (1),AC-18 (1)</t>
         </is>
       </c>
       <c r="B208" s="2" t="inlineStr">
@@ -16899,7 +16906,7 @@
     <row r="209" ht="130" customHeight="1">
       <c r="A209" s="2" t="inlineStr">
         <is>
-          <t>AC-11 (1),AC-11 a</t>
+          <t>AC-11 a,AC-11 (1)</t>
         </is>
       </c>
       <c r="B209" s="2" t="inlineStr">
@@ -16988,7 +16995,7 @@
     <row r="210" ht="130" customHeight="1">
       <c r="A210" s="2" t="inlineStr">
         <is>
-          <t>AC-11 (1),AC-11 a</t>
+          <t>AC-11 a,AC-11 (1)</t>
         </is>
       </c>
       <c r="B210" s="2" t="inlineStr">
@@ -17241,7 +17248,7 @@
     <row r="213" ht="130" customHeight="1">
       <c r="A213" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,IA-5 (1) (c),CM-6 b</t>
+          <t>IA-5 (1) (c),CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B213" s="2" t="inlineStr">
@@ -17401,7 +17408,7 @@
     <row r="215" ht="130" customHeight="1">
       <c r="A215" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-12 a</t>
+          <t>AU-12 a,CM-6 b</t>
         </is>
       </c>
       <c r="B215" s="2" t="inlineStr">
@@ -17492,7 +17499,7 @@
     <row r="216" ht="130" customHeight="1">
       <c r="A216" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-5 (2),SC-5</t>
+          <t>SC-5 (2),SC-5,CM-6 b</t>
         </is>
       </c>
       <c r="B216" s="2" t="inlineStr">
@@ -17672,7 +17679,7 @@
     <row r="218" ht="130" customHeight="1">
       <c r="A218" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,SI-16</t>
+          <t>SI-16,CM-7 a</t>
         </is>
       </c>
       <c r="B218" s="2" t="inlineStr">
@@ -17764,7 +17771,7 @@
     <row r="219" ht="130" customHeight="1">
       <c r="A219" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-16</t>
+          <t>SI-16,CM-6 b</t>
         </is>
       </c>
       <c r="B219" s="2" t="inlineStr">
@@ -17862,7 +17869,7 @@
     <row r="220" ht="130" customHeight="1">
       <c r="A220" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),IA-2,IA-8</t>
+          <t>IA-2,IA-8,AU-3 (1)</t>
         </is>
       </c>
       <c r="B220" s="2" t="inlineStr">
@@ -18841,7 +18848,7 @@
     <row r="232" ht="130" customHeight="1">
       <c r="A232" s="2" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b,SI-16</t>
+          <t>SC-2,SI-16,CM-6 b</t>
         </is>
       </c>
       <c r="B232" s="2" t="inlineStr">
@@ -19025,7 +19032,7 @@
     <row r="234" ht="130" customHeight="1">
       <c r="A234" s="2" t="inlineStr">
         <is>
-          <t>SC-3,SI-16</t>
+          <t>SI-16,SC-3</t>
         </is>
       </c>
       <c r="B234" s="2" t="inlineStr">
@@ -19187,7 +19194,7 @@
     <row r="236" ht="130" customHeight="1">
       <c r="A236" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,AC-18 (1)</t>
+          <t>AC-18 (1),CM-7 a</t>
         </is>
       </c>
       <c r="B236" s="2" t="inlineStr">
@@ -19754,7 +19761,7 @@
     <row r="243" ht="130" customHeight="1">
       <c r="A243" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (a),IA-5 (1) (b)</t>
+          <t>IA-5 (1) (b),IA-5 (1) (a),CM-6 b</t>
         </is>
       </c>
       <c r="B243" s="2" t="inlineStr">
@@ -20322,7 +20329,7 @@
     <row r="250" ht="130" customHeight="1">
       <c r="A250" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-4</t>
+          <t>SC-4,CM-6 b</t>
         </is>
       </c>
       <c r="B250" s="2" t="inlineStr">
@@ -20578,7 +20585,7 @@
     <row r="253" ht="130" customHeight="1">
       <c r="A253" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (1)</t>
         </is>
       </c>
       <c r="B253" s="2" t="inlineStr">
@@ -20667,7 +20674,7 @@
     <row r="254" ht="130" customHeight="1">
       <c r="A254" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B254" s="2" t="inlineStr">
@@ -21080,7 +21087,7 @@
     <row r="259" ht="130" customHeight="1">
       <c r="A259" s="3" t="inlineStr">
         <is>
-          <t>AC-6 (9),AC-6 (8)</t>
+          <t>AC-6 (8),AC-6 (9)</t>
         </is>
       </c>
       <c r="B259" s="3" t="inlineStr">
@@ -21626,7 +21633,7 @@
     <row r="266" ht="130" customHeight="1">
       <c r="A266" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-12 c</t>
+          <t>AU-12 c,AU-9</t>
         </is>
       </c>
       <c r="B266" s="2" t="inlineStr">
@@ -21709,7 +21716,7 @@
     <row r="267" ht="130" customHeight="1">
       <c r="A267" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (3)</t>
+          <t>CM-5 (3),CM-6 b</t>
         </is>
       </c>
       <c r="B267" s="2" t="inlineStr">
@@ -22399,7 +22406,7 @@
     <row r="275" ht="130" customHeight="1">
       <c r="A275" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 a</t>
+          <t>CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B275" s="3" t="inlineStr">
@@ -23921,7 +23928,7 @@
     <row r="294" ht="130" customHeight="1">
       <c r="A294" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 (1)</t>
+          <t>AU-5 (1),AU-5 a</t>
         </is>
       </c>
       <c r="B294" s="2" t="inlineStr">
@@ -27289,7 +27296,7 @@
     <row r="339" ht="130" customHeight="1">
       <c r="A339" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (c)</t>
+          <t>IA-5 (1) (c),CM-6 b</t>
         </is>
       </c>
       <c r="B339" s="3" t="inlineStr">
@@ -27439,7 +27446,7 @@
     <row r="341" ht="130" customHeight="1">
       <c r="A341" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (2)</t>
+          <t>IA-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B341" s="2" t="inlineStr">
@@ -28179,7 +28186,7 @@
     <row r="351" ht="130" customHeight="1">
       <c r="A351" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-17 (2)</t>
+          <t>AC-17 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B351" s="2" t="inlineStr">
@@ -29916,7 +29923,7 @@
     <row r="374" ht="130" customHeight="1">
       <c r="A374" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-3</t>
+          <t>AU-3,CM-6 b</t>
         </is>
       </c>
       <c r="B374" s="2" t="inlineStr">
@@ -30170,7 +30177,7 @@
     <row r="377" ht="130" customHeight="1">
       <c r="A377" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B377" s="2" t="inlineStr">
@@ -33141,7 +33148,7 @@
     <row r="412" ht="130" customHeight="1">
       <c r="A412" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B412" s="2" t="inlineStr">
@@ -33223,7 +33230,7 @@
     <row r="413" ht="130" customHeight="1">
       <c r="A413" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B413" s="2" t="inlineStr">
@@ -33916,7 +33923,7 @@
     <row r="422" ht="130" customHeight="1">
       <c r="A422" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B422" s="2" t="inlineStr">
@@ -34519,7 +34526,7 @@
     <row r="429" ht="130" customHeight="1">
       <c r="A429" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B429" s="2" t="inlineStr">
@@ -34971,7 +34978,7 @@
     <row r="435" ht="130" customHeight="1">
       <c r="A435" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-4</t>
+          <t>AU-4,CM-6 b</t>
         </is>
       </c>
       <c r="B435" s="2" t="inlineStr">
@@ -35275,7 +35282,7 @@
     <row r="439" ht="130" customHeight="1">
       <c r="A439" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B439" s="2" t="inlineStr">
@@ -35365,7 +35372,7 @@
     <row r="440" ht="130" customHeight="1">
       <c r="A440" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B440" s="2" t="inlineStr">
@@ -35760,7 +35767,7 @@
     <row r="445" ht="130" customHeight="1">
       <c r="A445" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-2 (2)</t>
+          <t>SI-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B445" s="3" t="inlineStr">
@@ -36407,7 +36414,7 @@
     <row r="454" ht="130" customHeight="1">
       <c r="A454" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-2 (2)</t>
+          <t>SI-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B454" s="3" t="inlineStr">
@@ -36698,7 +36705,7 @@
     <row r="458" ht="130" customHeight="1">
       <c r="A458" s="3" t="inlineStr">
         <is>
-          <t>MA-4 e,SC-10,MA-4 (7),AC-12</t>
+          <t>SC-10,AC-12,MA-4 (7),MA-4 e</t>
         </is>
       </c>
       <c r="B458" s="3" t="inlineStr">
@@ -37005,7 +37012,7 @@
     <row r="462" ht="130" customHeight="1">
       <c r="A462" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8,AC-17 (2)</t>
+          <t>SC-8 (1),AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B462" s="2" t="inlineStr">
@@ -38313,7 +38320,7 @@
     <row r="479" ht="130" customHeight="1">
       <c r="A479" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,IA-3</t>
+          <t>IA-3,CM-7 b</t>
         </is>
       </c>
       <c r="B479" s="2" t="inlineStr">
@@ -41475,7 +41482,7 @@
     <row r="518" ht="130" customHeight="1">
       <c r="A518" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (2)</t>
+          <t>SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B518" s="2" t="inlineStr">
@@ -42665,7 +42672,7 @@
     <row r="533" ht="130" customHeight="1">
       <c r="A533" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2)</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B533" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@2217dbfaed772205b6bc8fbde79be820cd422e3a 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -550,7 +550,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -634,7 +634,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -719,7 +719,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -791,7 +791,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -973,7 +973,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-5 b,AU-5 a</t>
+          <t>AU-5 a,AU-5 b</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1467,7 +1467,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),AU-12 a,AU-7 (1),AU-6 (4),AU-3,CM-5 (1),AU-3 (1),MA-4 (1) (a),AU-7 a,CM-6 b</t>
+          <t>AU-7 a,CM-5 (1),MA-4 (1) (a),AU-7 (1),CM-6 b,AU-6 (4),AU-3 (1),AU-3,AU-14 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -1552,7 +1552,7 @@
     <row r="14" ht="130" customHeight="1">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -3270,7 +3270,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-14 (1),AU-12 a</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3361,7 +3361,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AU-14 (1),AU-4</t>
+          <t>AU-4,AU-14 (1)</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3450,7 +3450,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-3</t>
+          <t>AU-3,AU-4 (1)</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3844,7 +3844,7 @@
     <row r="44" ht="130" customHeight="1">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-6 (4),CM-6 b</t>
+          <t>CM-6 b,AU-6 (4),AU-4 (1)</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
@@ -3920,7 +3920,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),CM-6 b</t>
+          <t>CM-6 b,AU-4 (1)</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -4005,7 +4005,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (a),AU-8 (1) (b),AU-8 b</t>
+          <t>AU-8 (1) (a),AU-8 b,AU-8 (1) (b)</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -4246,7 +4246,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12),IA-2 (1)</t>
+          <t>IA-2 (1),IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4506,7 +4506,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -4581,7 +4581,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -4656,7 +4656,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -4731,7 +4731,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -4806,7 +4806,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -4881,7 +4881,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -4956,7 +4956,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -5031,7 +5031,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -5106,7 +5106,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -5181,7 +5181,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-8 b,AU-12 (3),CM-5 (1),AU-7 b,AU-7 a,AU-12 c,CM-6 b</t>
+          <t>AU-7 a,CM-5 (1),AU-12 c,CM-6 b,AU-7 b,AU-8 b,AU-12 (3),AU-12 a</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5255,7 +5255,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AC-2 (4),MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a,AC-2 (4)</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5336,7 +5336,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AC-2 (4),MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a,AC-2 (4)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5417,7 +5417,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AC-2 (4),MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a,AC-2 (4)</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5499,7 +5499,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AC-2 (4),MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a,AC-2 (4)</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5581,7 +5581,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AC-2 (4),MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a,AC-2 (4)</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5663,7 +5663,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AC-2 (4),MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a,AC-2 (4)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5745,7 +5745,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AC-2 (4),MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a,AC-2 (4)</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -6865,7 +6865,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -6939,7 +6939,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -7013,7 +7013,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -7087,7 +7087,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -7663,7 +7663,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -7738,7 +7738,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -7813,7 +7813,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -7888,7 +7888,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -7968,7 +7968,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -8050,7 +8050,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -8132,7 +8132,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8214,7 +8214,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8296,7 +8296,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8378,7 +8378,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -8458,7 +8458,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -8538,7 +8538,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -8618,7 +8618,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AC-11 (1),AC-11 b</t>
+          <t>AC-11 b,AC-11 (1)</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8789,7 +8789,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),AC-11 b</t>
+          <t>AC-11 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -9526,7 +9526,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9682,7 +9682,7 @@
     <row r="117" ht="130" customHeight="1">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -10038,7 +10038,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -10892,7 +10892,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10973,7 +10973,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -11059,7 +11059,7 @@
     <row r="135" ht="130" customHeight="1">
       <c r="A135" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B135" s="2" t="inlineStr">
@@ -11152,7 +11152,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),AC-3 (4)</t>
+          <t>AC-3 (4),AC-6 (10)</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -11249,7 +11249,7 @@
     <row r="137" ht="130" customHeight="1">
       <c r="A137" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),AC-3 (4)</t>
+          <t>AC-3 (4),AC-6 (10)</t>
         </is>
       </c>
       <c r="B137" s="2" t="inlineStr">
@@ -11505,7 +11505,7 @@
     <row r="140" ht="130" customHeight="1">
       <c r="A140" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B140" s="3" t="inlineStr">
@@ -11585,7 +11585,7 @@
     <row r="141" ht="130" customHeight="1">
       <c r="A141" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B141" s="3" t="inlineStr">
@@ -11665,7 +11665,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B142" s="3" t="inlineStr">
@@ -12448,7 +12448,7 @@
     <row r="152" ht="130" customHeight="1">
       <c r="A152" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B152" s="2" t="inlineStr">
@@ -12524,7 +12524,7 @@
     <row r="153" ht="130" customHeight="1">
       <c r="A153" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B153" s="2" t="inlineStr">
@@ -12609,7 +12609,7 @@
     <row r="154" ht="130" customHeight="1">
       <c r="A154" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B154" s="2" t="inlineStr">
@@ -12766,7 +12766,7 @@
     <row r="156" ht="130" customHeight="1">
       <c r="A156" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-7 a</t>
+          <t>CM-7 a,IA-7</t>
         </is>
       </c>
       <c r="B156" s="2" t="inlineStr">
@@ -12845,7 +12845,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B157" s="3" t="inlineStr">
@@ -12922,7 +12922,7 @@
     <row r="158" ht="130" customHeight="1">
       <c r="A158" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B158" s="3" t="inlineStr">
@@ -12995,7 +12995,7 @@
     <row r="159" ht="130" customHeight="1">
       <c r="A159" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3</t>
+          <t>AU-12 c,AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B159" s="3" t="inlineStr">
@@ -13068,7 +13068,7 @@
     <row r="160" ht="130" customHeight="1">
       <c r="A160" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B160" s="3" t="inlineStr">
@@ -13153,7 +13153,7 @@
     <row r="161" ht="130" customHeight="1">
       <c r="A161" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B161" s="3" t="inlineStr">
@@ -13228,7 +13228,7 @@
     <row r="162" ht="130" customHeight="1">
       <c r="A162" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B162" s="3" t="inlineStr">
@@ -13303,7 +13303,7 @@
     <row r="163" ht="130" customHeight="1">
       <c r="A163" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B163" s="3" t="inlineStr">
@@ -13378,7 +13378,7 @@
     <row r="164" ht="130" customHeight="1">
       <c r="A164" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B164" s="3" t="inlineStr">
@@ -13881,7 +13881,7 @@
     <row r="171" ht="130" customHeight="1">
       <c r="A171" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B171" s="3" t="inlineStr">
@@ -14170,7 +14170,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B175" s="3" t="inlineStr">
@@ -14245,7 +14245,7 @@
     <row r="176" ht="130" customHeight="1">
       <c r="A176" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B176" s="3" t="inlineStr">
@@ -14327,7 +14327,7 @@
     <row r="177" ht="130" customHeight="1">
       <c r="A177" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B177" s="3" t="inlineStr">
@@ -14409,7 +14409,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B178" s="3" t="inlineStr">
@@ -14491,7 +14491,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B179" s="3" t="inlineStr">
@@ -14573,7 +14573,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B180" s="3" t="inlineStr">
@@ -14655,7 +14655,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B181" s="3" t="inlineStr">
@@ -14737,7 +14737,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B182" s="3" t="inlineStr">
@@ -14819,7 +14819,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B183" s="3" t="inlineStr">
@@ -14901,7 +14901,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B184" s="3" t="inlineStr">
@@ -14983,7 +14983,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B185" s="3" t="inlineStr">
@@ -15061,7 +15061,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B186" s="3" t="inlineStr">
@@ -15140,7 +15140,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B187" s="3" t="inlineStr">
@@ -15222,7 +15222,7 @@
     <row r="188" ht="130" customHeight="1">
       <c r="A188" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B188" s="3" t="inlineStr">
@@ -15304,7 +15304,7 @@
     <row r="189" ht="130" customHeight="1">
       <c r="A189" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B189" s="3" t="inlineStr">
@@ -15386,7 +15386,7 @@
     <row r="190" ht="130" customHeight="1">
       <c r="A190" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B190" s="3" t="inlineStr">
@@ -15468,7 +15468,7 @@
     <row r="191" ht="130" customHeight="1">
       <c r="A191" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B191" s="3" t="inlineStr">
@@ -15550,7 +15550,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B192" s="3" t="inlineStr">
@@ -15632,7 +15632,7 @@
     <row r="193" ht="130" customHeight="1">
       <c r="A193" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
         </is>
       </c>
       <c r="B193" s="3" t="inlineStr">
@@ -15707,7 +15707,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="3" t="inlineStr">
         <is>
-          <t>AU-12 a,AU-3,AC-2 (4),MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a,AC-2 (4)</t>
         </is>
       </c>
       <c r="B194" s="3" t="inlineStr">
@@ -15780,7 +15780,7 @@
     <row r="195" ht="130" customHeight="1">
       <c r="A195" s="3" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AC-2 (4)</t>
         </is>
       </c>
       <c r="B195" s="3" t="inlineStr">
@@ -15857,7 +15857,7 @@
     <row r="196" ht="130" customHeight="1">
       <c r="A196" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (4),IA-2 (3),IA-2 (1)</t>
+          <t>IA-2 (3),IA-2 (2),IA-2 (1),IA-2 (4)</t>
         </is>
       </c>
       <c r="B196" s="2" t="inlineStr">
@@ -15944,7 +15944,7 @@
     <row r="197" ht="130" customHeight="1">
       <c r="A197" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2,IA-2 (4),IA-2 (2),IA-2 (5)</t>
+          <t>IA-2 (5),IA-2,IA-2 (3),IA-2 (4),IA-2 (2)</t>
         </is>
       </c>
       <c r="B197" s="2" t="inlineStr">
@@ -16033,7 +16033,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2,IA-2 (4),IA-2 (2),IA-2 (5)</t>
+          <t>IA-2 (5),IA-2,IA-2 (3),IA-2 (4),IA-2 (2)</t>
         </is>
       </c>
       <c r="B198" s="2" t="inlineStr">
@@ -16657,7 +16657,7 @@
     <row r="206" ht="130" customHeight="1">
       <c r="A206" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8 (1),SC-8</t>
+          <t>SC-8 (2),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B206" s="2" t="inlineStr">
@@ -16734,7 +16734,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8 (1),SC-8</t>
+          <t>SC-8 (2),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -16820,7 +16820,7 @@
     <row r="208" ht="130" customHeight="1">
       <c r="A208" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (1),AC-18 (1)</t>
+          <t>SC-8 (1),SC-8,AC-18 (1)</t>
         </is>
       </c>
       <c r="B208" s="2" t="inlineStr">
@@ -17408,7 +17408,7 @@
     <row r="215" ht="130" customHeight="1">
       <c r="A215" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,CM-6 b</t>
+          <t>CM-6 b,AU-12 a</t>
         </is>
       </c>
       <c r="B215" s="2" t="inlineStr">
@@ -17499,7 +17499,7 @@
     <row r="216" ht="130" customHeight="1">
       <c r="A216" s="2" t="inlineStr">
         <is>
-          <t>SC-5 (2),SC-5,CM-6 b</t>
+          <t>SC-5,CM-6 b,SC-5 (2)</t>
         </is>
       </c>
       <c r="B216" s="2" t="inlineStr">
@@ -17869,7 +17869,7 @@
     <row r="220" ht="130" customHeight="1">
       <c r="A220" s="2" t="inlineStr">
         <is>
-          <t>IA-2,IA-8,AU-3 (1)</t>
+          <t>AU-3 (1),IA-8,IA-2</t>
         </is>
       </c>
       <c r="B220" s="2" t="inlineStr">
@@ -18104,43 +18104,43 @@
       <c r="Q222" s="2" t="n"/>
     </row>
     <row r="223" ht="130" customHeight="1">
-      <c r="A223" s="3" t="inlineStr">
+      <c r="A223" s="2" t="inlineStr">
         <is>
           <t>CM-5 (6)</t>
         </is>
       </c>
-      <c r="B223" s="3" t="inlineStr">
+      <c r="B223" s="2" t="inlineStr">
         <is>
           <t>CCI-001499</t>
         </is>
       </c>
-      <c r="C223" s="3" t="inlineStr">
+      <c r="C223" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000259-GPOS-00100</t>
         </is>
       </c>
-      <c r="D223" s="3" t="inlineStr">
+      <c r="D223" s="2" t="inlineStr">
         <is>
           <t>CCE-89858-5</t>
         </is>
       </c>
-      <c r="E223" s="3" t="inlineStr">
+      <c r="E223" s="2" t="inlineStr">
         <is>
           <t>The operating system must limit privileges to change software resident within software libraries.</t>
         </is>
       </c>
-      <c r="F223" s="3" t="inlineStr">
+      <c r="F223" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 must limit privileges to change software resident within software libraries.</t>
         </is>
       </c>
-      <c r="G223" s="3" t="inlineStr">
+      <c r="G223" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> If the operating system were to allow any user to make changes to software libraries, then those changes might be implemented without undergoing the appropriate testing and approvals that are part of a robust change management process.
 This requirement applies to operating systems with software libraries that are accessible and configurable, as in the case of interpreted languages. Software libraries also include privileged programs which execute with escalated privileges. Only qualified and authorized individuals shall be allowed to obtain access to information system components for purposes of initiating changes, including upgrades and modifications.</t>
         </is>
       </c>
-      <c r="H223" s="3" t="inlineStr">
+      <c r="H223" s="2" t="inlineStr">
         <is>
           <t>Files from shared library directories are loaded into the address
 space of processes (including privileged ones) or of the kernel itself at
@@ -18148,78 +18148,79 @@
 the integrity of the system.</t>
         </is>
       </c>
-      <c r="I223" s="3" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J223" s="3" t="inlineStr">
+      <c r="I223" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J223" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system limits privileges to change software resident within software libraries. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K223" s="3" t="inlineStr">
-        <is>
-          <t>Shared libraries are stored in the following directories:
- /lib
-/lib64
-/usr/lib
-/usr/lib64 
-For each of these directories, run the following command to find files not
-owned by root:
- $ sudo find -L  $DIR  ! -user root -type d -exec chgrp root {} \; 
-If any of these directories are not group-owned by root, then this is a finding.</t>
-        </is>
-      </c>
-      <c r="L223" s="3" t="n"/>
-      <c r="M223" s="3" t="inlineStr"/>
-      <c r="N223" s="3" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O223" s="3" t="n"/>
-      <c r="P223" s="3" t="n"/>
-      <c r="Q223" s="3" t="n"/>
+      <c r="K223" s="2" t="inlineStr">
+        <is>
+          <t>Verify the system-wide shared library directories are group-owned by "root" with the following command:
+$ sudo find /lib /lib64 /usr/lib /usr/lib64 ! -group root -type d -exec stat -c "%n %G" '{}' \;
+If any system-wide shared library directory is returned and is not group-owned by a required system account, this is a finding.
+If any system-wide shared library directory is returned and is not group-owned by a required system account, then this is a finding.</t>
+        </is>
+      </c>
+      <c r="L223" s="2" t="n"/>
+      <c r="M223" s="2" t="inlineStr">
+        <is>
+          <t>Configure the system-wide shared library directories (/lib, /lib64, /usr/lib and /usr/lib64) to be protected from unauthorized access.
+Run the following command, replacing "[DIRECTORY]" with any library directory not group-owned by "root".
+$ sudo chgrp root [DIRECTORY]</t>
+        </is>
+      </c>
+      <c r="N223" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O223" s="2" t="n"/>
+      <c r="P223" s="2" t="n"/>
+      <c r="Q223" s="2" t="n"/>
     </row>
     <row r="224" ht="130" customHeight="1">
-      <c r="A224" s="3" t="inlineStr">
+      <c r="A224" s="2" t="inlineStr">
         <is>
           <t>CM-5 (6)</t>
         </is>
       </c>
-      <c r="B224" s="3" t="inlineStr">
+      <c r="B224" s="2" t="inlineStr">
         <is>
           <t>CCI-001499</t>
         </is>
       </c>
-      <c r="C224" s="3" t="inlineStr">
+      <c r="C224" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000259-GPOS-00100</t>
         </is>
       </c>
-      <c r="D224" s="3" t="inlineStr">
+      <c r="D224" s="2" t="inlineStr">
         <is>
           <t>CCE-89022-8</t>
         </is>
       </c>
-      <c r="E224" s="3" t="inlineStr">
+      <c r="E224" s="2" t="inlineStr">
         <is>
           <t>The operating system must limit privileges to change software resident within software libraries.</t>
         </is>
       </c>
-      <c r="F224" s="3" t="inlineStr">
+      <c r="F224" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 must limit privileges to change software resident within software libraries.</t>
         </is>
       </c>
-      <c r="G224" s="3" t="inlineStr">
+      <c r="G224" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> If the operating system were to allow any user to make changes to software libraries, then those changes might be implemented without undergoing the appropriate testing and approvals that are part of a robust change management process.
 This requirement applies to operating systems with software libraries that are accessible and configurable, as in the case of interpreted languages. Software libraries also include privileged programs which execute with escalated privileges. Only qualified and authorized individuals shall be allowed to obtain access to information system components for purposes of initiating changes, including upgrades and modifications.</t>
         </is>
       </c>
-      <c r="H224" s="3" t="inlineStr">
+      <c r="H224" s="2" t="inlineStr">
         <is>
           <t>Files from shared library directories are loaded into the address
 space of processes (including privileged ones) or of the kernel itself at
@@ -18227,78 +18228,78 @@
 the integrity of the system.</t>
         </is>
       </c>
-      <c r="I224" s="3" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J224" s="3" t="inlineStr">
+      <c r="I224" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J224" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system limits privileges to change software resident within software libraries. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K224" s="3" t="inlineStr">
-        <is>
-          <t>Shared libraries are stored in the following directories:
- /lib
-/lib64
-/usr/lib
-/usr/lib64 
-For each of these directories, run the following command to find files not
-owned by root:
- $ sudo find -L  $DIR  ! -user root -type d -exec chown root {} \; 
-If any of these directories are not owned by root, then this is a finding.</t>
-        </is>
-      </c>
-      <c r="L224" s="3" t="n"/>
-      <c r="M224" s="3" t="inlineStr"/>
-      <c r="N224" s="3" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O224" s="3" t="n"/>
-      <c r="P224" s="3" t="n"/>
-      <c r="Q224" s="3" t="n"/>
+      <c r="K224" s="2" t="inlineStr">
+        <is>
+          <t>Verify the system-wide shared library directories are owned by "root" with the following command:
+$ sudo find /lib /lib64 /usr/lib /usr/lib64 ! -user root -type d -exec stat -c "%n %U" '{}' \;
+If any system-wide shared library directory is not owned by root, then this is a finding.</t>
+        </is>
+      </c>
+      <c r="L224" s="2" t="n"/>
+      <c r="M224" s="2" t="inlineStr">
+        <is>
+          <t>Configure the system-wide shared library directories within (/lib, /lib64, /usr/lib and /usr/lib64) to be protected from unauthorized access.
+Run the following command, replacing "[DIRECTORY]" with any library directory not owned by "root".
+$ sudo chown root [DIRECTORY]</t>
+        </is>
+      </c>
+      <c r="N224" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O224" s="2" t="n"/>
+      <c r="P224" s="2" t="n"/>
+      <c r="Q224" s="2" t="n"/>
     </row>
     <row r="225" ht="130" customHeight="1">
-      <c r="A225" s="3" t="inlineStr">
+      <c r="A225" s="2" t="inlineStr">
         <is>
           <t>CM-5 (6)</t>
         </is>
       </c>
-      <c r="B225" s="3" t="inlineStr">
+      <c r="B225" s="2" t="inlineStr">
         <is>
           <t>CCI-001499</t>
         </is>
       </c>
-      <c r="C225" s="3" t="inlineStr">
+      <c r="C225" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000259-GPOS-00100</t>
         </is>
       </c>
-      <c r="D225" s="3" t="inlineStr">
+      <c r="D225" s="2" t="inlineStr">
         <is>
           <t>CCE-89442-8</t>
         </is>
       </c>
-      <c r="E225" s="3" t="inlineStr">
+      <c r="E225" s="2" t="inlineStr">
         <is>
           <t>The operating system must limit privileges to change software resident within software libraries.</t>
         </is>
       </c>
-      <c r="F225" s="3" t="inlineStr">
+      <c r="F225" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 must limit privileges to change software resident within software libraries.</t>
         </is>
       </c>
-      <c r="G225" s="3" t="inlineStr">
+      <c r="G225" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> If the operating system were to allow any user to make changes to software libraries, then those changes might be implemented without undergoing the appropriate testing and approvals that are part of a robust change management process.
 This requirement applies to operating systems with software libraries that are accessible and configurable, as in the case of interpreted languages. Software libraries also include privileged programs which execute with escalated privileges. Only qualified and authorized individuals shall be allowed to obtain access to information system components for purposes of initiating changes, including upgrades and modifications.</t>
         </is>
       </c>
-      <c r="H225" s="3" t="inlineStr">
+      <c r="H225" s="2" t="inlineStr">
         <is>
           <t>If the operating system allows any user to make changes to software
 libraries, then those changes might be implemented without undergoing the
@@ -18312,398 +18313,389 @@
 of initiating changes, including upgrades and modifications.</t>
         </is>
       </c>
-      <c r="I225" s="3" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J225" s="3" t="inlineStr">
+      <c r="I225" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J225" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system limits privileges to change software resident within software libraries. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K225" s="3" t="inlineStr">
-        <is>
-          <t>System commands are stored in the following directories:
- /bin
-/sbin
-/usr/bin
-/usr/sbin
-/usr/local/bin
-/usr/local/sbin 
-For each of these directories, run the following command to find files not
-owned by root group:
- $ sudo find -L  $DIR  ! -group root -type f \; 
-If any of these files are not owned by root group, then this is a finding.</t>
-        </is>
-      </c>
-      <c r="L225" s="3" t="n"/>
-      <c r="M225" s="3" t="inlineStr"/>
-      <c r="N225" s="3" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O225" s="3" t="n"/>
-      <c r="P225" s="3" t="n"/>
-      <c r="Q225" s="3" t="n"/>
+      <c r="K225" s="2" t="inlineStr">
+        <is>
+          <t>Verify the system commands contained in the following directories are group-owned by "root", or a required system account, with the following command:
+$ sudo find -L /bin /sbin /usr/bin /usr/sbin /usr/local/bin /usr/local/sbin ! -group root -exec ls -l {} \;
+If any system commands are returned and is not group-owned by a required system account, then this is a finding.</t>
+        </is>
+      </c>
+      <c r="L225" s="2" t="n"/>
+      <c r="M225" s="2" t="inlineStr">
+        <is>
+          <t>Configure the system commands to be protected from unauthorized access.
+Run the following command, replacing "[FILE]" with any system command file not group-owned by "root" or a required system account.
+$ sudo chgrp root [FILE]</t>
+        </is>
+      </c>
+      <c r="N225" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O225" s="2" t="n"/>
+      <c r="P225" s="2" t="n"/>
+      <c r="Q225" s="2" t="n"/>
     </row>
     <row r="226" ht="130" customHeight="1">
-      <c r="A226" s="3" t="inlineStr">
+      <c r="A226" s="2" t="inlineStr">
         <is>
           <t>CM-5 (6)</t>
         </is>
       </c>
-      <c r="B226" s="3" t="inlineStr">
+      <c r="B226" s="2" t="inlineStr">
         <is>
           <t>CCI-001499</t>
         </is>
       </c>
-      <c r="C226" s="3" t="inlineStr">
+      <c r="C226" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000259-GPOS-00100</t>
         </is>
       </c>
-      <c r="D226" s="3" t="inlineStr">
+      <c r="D226" s="2" t="inlineStr">
         <is>
           <t>CCE-83908-4</t>
         </is>
       </c>
-      <c r="E226" s="3" t="inlineStr">
+      <c r="E226" s="2" t="inlineStr">
         <is>
           <t>The operating system must limit privileges to change software resident within software libraries.</t>
         </is>
       </c>
-      <c r="F226" s="3" t="inlineStr">
+      <c r="F226" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 must limit privileges to change software resident within software libraries.</t>
         </is>
       </c>
-      <c r="G226" s="3" t="inlineStr">
+      <c r="G226" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> If the operating system were to allow any user to make changes to software libraries, then those changes might be implemented without undergoing the appropriate testing and approvals that are part of a robust change management process.
 This requirement applies to operating systems with software libraries that are accessible and configurable, as in the case of interpreted languages. Software libraries also include privileged programs which execute with escalated privileges. Only qualified and authorized individuals shall be allowed to obtain access to information system components for purposes of initiating changes, including upgrades and modifications.</t>
         </is>
       </c>
-      <c r="H226" s="3" t="inlineStr">
+      <c r="H226" s="2" t="inlineStr">
         <is>
           <t>System binaries are executed by privileged users as well as system services,
 and restrictive permissions are necessary to ensure that their
 execution of these programs cannot be co-opted.</t>
         </is>
       </c>
-      <c r="I226" s="3" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J226" s="3" t="inlineStr">
+      <c r="I226" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J226" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system limits privileges to change software resident within software libraries. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K226" s="3" t="inlineStr">
-        <is>
-          <t>System executables are stored in the following directories by default:
- /bin
-/sbin
-/usr/bin
-/usr/libexec
-/usr/local/bin
-/usr/local/sbin
-/usr/sbin 
-To find system executables that are not owned by "root",
-run the following command for each directory  DIR  which contains system executables:
- $ sudo find  DIR/  \! -user root 
-If any system executables are found to not be owned by root, then this is a finding.</t>
-        </is>
-      </c>
-      <c r="L226" s="3" t="n"/>
-      <c r="M226" s="3" t="inlineStr"/>
-      <c r="N226" s="3" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O226" s="3" t="n"/>
-      <c r="P226" s="3" t="n"/>
-      <c r="Q226" s="3" t="n"/>
+      <c r="K226" s="2" t="inlineStr">
+        <is>
+          <t>Verify the system commands contained in the following directories are owned by "root" with the following command:
+$ sudo find -L /bin /sbin /usr/bin /usr/sbin /usr/libexec /usr/local/bin /usr/local/sbin ! -user root -exec ls -l {} \;
+If any system commands are found to not be owned by root, then this is a finding.</t>
+        </is>
+      </c>
+      <c r="L226" s="2" t="n"/>
+      <c r="M226" s="2" t="inlineStr">
+        <is>
+          <t>Configure the system commands to be protected from unauthorized access.
+Run the following command, replacing "[FILE]" with any system command file not owned by "root".
+$ sudo chown root [FILE]</t>
+        </is>
+      </c>
+      <c r="N226" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O226" s="2" t="n"/>
+      <c r="P226" s="2" t="n"/>
+      <c r="Q226" s="2" t="n"/>
     </row>
     <row r="227" ht="130" customHeight="1">
-      <c r="A227" s="3" t="inlineStr">
+      <c r="A227" s="2" t="inlineStr">
         <is>
           <t>CM-5 (6)</t>
         </is>
       </c>
-      <c r="B227" s="3" t="inlineStr">
+      <c r="B227" s="2" t="inlineStr">
         <is>
           <t>CCI-001499</t>
         </is>
       </c>
-      <c r="C227" s="3" t="inlineStr">
+      <c r="C227" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000259-GPOS-00100</t>
         </is>
       </c>
-      <c r="D227" s="3" t="inlineStr">
+      <c r="D227" s="2" t="inlineStr">
         <is>
           <t>CCE-83907-6</t>
         </is>
       </c>
-      <c r="E227" s="3" t="inlineStr">
+      <c r="E227" s="2" t="inlineStr">
         <is>
           <t>The operating system must limit privileges to change software resident within software libraries.</t>
         </is>
       </c>
-      <c r="F227" s="3" t="inlineStr">
+      <c r="F227" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 must limit privileges to change software resident within software libraries.</t>
         </is>
       </c>
-      <c r="G227" s="3" t="inlineStr">
+      <c r="G227" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> If the operating system were to allow any user to make changes to software libraries, then those changes might be implemented without undergoing the appropriate testing and approvals that are part of a robust change management process.
 This requirement applies to operating systems with software libraries that are accessible and configurable, as in the case of interpreted languages. Software libraries also include privileged programs which execute with escalated privileges. Only qualified and authorized individuals shall be allowed to obtain access to information system components for purposes of initiating changes, including upgrades and modifications.</t>
         </is>
       </c>
-      <c r="H227" s="3" t="inlineStr">
+      <c r="H227" s="2" t="inlineStr">
         <is>
           <t>Files from shared library directories are loaded into the address
 space of processes (including privileged ones) or of the kernel itself at
 runtime. Proper ownership is necessary to protect the integrity of the system.</t>
         </is>
       </c>
-      <c r="I227" s="3" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J227" s="3" t="inlineStr">
+      <c r="I227" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J227" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system limits privileges to change software resident within software libraries. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K227" s="3" t="inlineStr">
-        <is>
-          <t>Shared libraries are stored in the following directories:
- /lib
-/lib64
-/usr/lib
-/usr/lib64 
-For each of these directories, run the following command to find files not
-owned by root:
- $ sudo find -L  $DIR  ! -user root -exec chown root {} \; 
-If any of these files are not owned by root, then this is a finding.</t>
-        </is>
-      </c>
-      <c r="L227" s="3" t="n"/>
-      <c r="M227" s="3" t="inlineStr"/>
-      <c r="N227" s="3" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O227" s="3" t="n"/>
-      <c r="P227" s="3" t="n"/>
-      <c r="Q227" s="3" t="n"/>
+      <c r="K227" s="2" t="inlineStr">
+        <is>
+          <t>Verify the system-wide shared library files are owned by "root" with the following command:
+$ sudo find -L /lib /lib64 /usr/lib /usr/lib64 ! -user root -exec ls -l {} \;
+If any system wide shared library file is not owned by root, then this is a finding.</t>
+        </is>
+      </c>
+      <c r="L227" s="2" t="n"/>
+      <c r="M227" s="2" t="inlineStr">
+        <is>
+          <t>Configure the system-wide shared library files (/lib, /lib64, /usr/lib and /usr/lib64) to be protected from unauthorized access.
+Run the following command, replacing "[FILE]" with any library file not owned by "root".
+$ sudo chown root [FILE]</t>
+        </is>
+      </c>
+      <c r="N227" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O227" s="2" t="n"/>
+      <c r="P227" s="2" t="n"/>
+      <c r="Q227" s="2" t="n"/>
     </row>
     <row r="228" ht="130" customHeight="1">
-      <c r="A228" s="3" t="inlineStr">
+      <c r="A228" s="2" t="inlineStr">
         <is>
           <t>CM-5 (6)</t>
         </is>
       </c>
-      <c r="B228" s="3" t="inlineStr">
+      <c r="B228" s="2" t="inlineStr">
         <is>
           <t>CCI-001499</t>
         </is>
       </c>
-      <c r="C228" s="3" t="inlineStr">
+      <c r="C228" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000259-GPOS-00100</t>
         </is>
       </c>
-      <c r="D228" s="3" t="inlineStr">
+      <c r="D228" s="2" t="inlineStr">
         <is>
           <t>CCE-83911-8</t>
         </is>
       </c>
-      <c r="E228" s="3" t="inlineStr">
+      <c r="E228" s="2" t="inlineStr">
         <is>
           <t>The operating system must limit privileges to change software resident within software libraries.</t>
         </is>
       </c>
-      <c r="F228" s="3" t="inlineStr">
+      <c r="F228" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 must limit privileges to change software resident within software libraries.</t>
         </is>
       </c>
-      <c r="G228" s="3" t="inlineStr">
+      <c r="G228" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> If the operating system were to allow any user to make changes to software libraries, then those changes might be implemented without undergoing the appropriate testing and approvals that are part of a robust change management process.
 This requirement applies to operating systems with software libraries that are accessible and configurable, as in the case of interpreted languages. Software libraries also include privileged programs which execute with escalated privileges. Only qualified and authorized individuals shall be allowed to obtain access to information system components for purposes of initiating changes, including upgrades and modifications.</t>
         </is>
       </c>
-      <c r="H228" s="3" t="inlineStr">
+      <c r="H228" s="2" t="inlineStr">
         <is>
           <t>System binaries are executed by privileged users, as well as system services,
 and restrictive permissions are necessary to ensure execution of these programs
 cannot be co-opted.</t>
         </is>
       </c>
-      <c r="I228" s="3" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J228" s="3" t="inlineStr">
+      <c r="I228" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J228" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system limits privileges to change software resident within software libraries. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K228" s="3" t="inlineStr">
-        <is>
-          <t>System executables are stored in the following directories by default:
- /bin
-/sbin
-/usr/bin
-/usr/libexec
-/usr/local/bin
-/usr/local/sbin
-/usr/sbin 
-To find system executables that are group-writable or world-writable,
-run the following command for each directory  DIR  which contains system executables:
- $ sudo find -L  DIR  -perm /022 -type f 
-If any system executables are found to be group or world writable, then this is a finding.</t>
-        </is>
-      </c>
-      <c r="L228" s="3" t="n"/>
-      <c r="M228" s="3" t="inlineStr"/>
-      <c r="N228" s="3" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O228" s="3" t="n"/>
-      <c r="P228" s="3" t="n"/>
-      <c r="Q228" s="3" t="n"/>
+      <c r="K228" s="2" t="inlineStr">
+        <is>
+          <t>Verify the system commands contained in the following directories have mode "755" or less permissive with the following command:
+$ sudo find -L /bin /sbin /usr/bin /usr/sbin /usr/libexec /usr/local/bin /usr/local/sbin -perm /022 -exec ls -l {} \;
+If any system commands are found to be group-writable or world-writable, then this is a finding.</t>
+        </is>
+      </c>
+      <c r="L228" s="2" t="n"/>
+      <c r="M228" s="2" t="inlineStr">
+        <is>
+          <t>Configure the system commands to be protected from unauthorized access.
+Run the following command, replacing "[FILE]" with any system command with a mode more permissive than "755".
+$ sudo chmod 755 [FILE]</t>
+        </is>
+      </c>
+      <c r="N228" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O228" s="2" t="n"/>
+      <c r="P228" s="2" t="n"/>
+      <c r="Q228" s="2" t="n"/>
     </row>
     <row r="229" ht="130" customHeight="1">
-      <c r="A229" s="3" t="inlineStr">
+      <c r="A229" s="2" t="inlineStr">
         <is>
           <t>CM-5 (6)</t>
         </is>
       </c>
-      <c r="B229" s="3" t="inlineStr">
+      <c r="B229" s="2" t="inlineStr">
         <is>
           <t>CCI-001499</t>
         </is>
       </c>
-      <c r="C229" s="3" t="inlineStr">
+      <c r="C229" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000259-GPOS-00100</t>
         </is>
       </c>
-      <c r="D229" s="3" t="inlineStr">
+      <c r="D229" s="2" t="inlineStr">
         <is>
           <t>CCE-83909-2</t>
         </is>
       </c>
-      <c r="E229" s="3" t="inlineStr">
+      <c r="E229" s="2" t="inlineStr">
         <is>
           <t>The operating system must limit privileges to change software resident within software libraries.</t>
         </is>
       </c>
-      <c r="F229" s="3" t="inlineStr">
+      <c r="F229" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 must limit privileges to change software resident within software libraries.</t>
         </is>
       </c>
-      <c r="G229" s="3" t="inlineStr">
+      <c r="G229" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> If the operating system were to allow any user to make changes to software libraries, then those changes might be implemented without undergoing the appropriate testing and approvals that are part of a robust change management process.
 This requirement applies to operating systems with software libraries that are accessible and configurable, as in the case of interpreted languages. Software libraries also include privileged programs which execute with escalated privileges. Only qualified and authorized individuals shall be allowed to obtain access to information system components for purposes of initiating changes, including upgrades and modifications.</t>
         </is>
       </c>
-      <c r="H229" s="3" t="inlineStr">
+      <c r="H229" s="2" t="inlineStr">
         <is>
           <t>Files from shared library directories are loaded into the address
 space of processes (including privileged ones) or of the kernel itself at
 runtime. Restrictive permissions are necessary to protect the integrity of the system.</t>
         </is>
       </c>
-      <c r="I229" s="3" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J229" s="3" t="inlineStr">
+      <c r="I229" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J229" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system limits privileges to change software resident within software libraries. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K229" s="3" t="inlineStr">
-        <is>
-          <t>Shared libraries are stored in the following directories:
- /lib
-/lib64
-/usr/lib
-/usr/lib64
-To find shared libraries that are group-writable or world-writable,
-run the following command for each directory  DIR  which contains shared libraries:
- $ sudo find -L  DIR  -perm /022 -type f 
-If any of these files are group-writable or world-writable, then this is a finding.</t>
-        </is>
-      </c>
-      <c r="L229" s="3" t="n"/>
-      <c r="M229" s="3" t="inlineStr"/>
-      <c r="N229" s="3" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O229" s="3" t="n"/>
-      <c r="P229" s="3" t="n"/>
-      <c r="Q229" s="3" t="n"/>
+      <c r="K229" s="2" t="inlineStr">
+        <is>
+          <t>Verify the system-wide shared library files contained in the following directories have mode "755" or less permissive with the following command:
+$ sudo find -L /lib /lib64 /usr/lib /usr/lib64 -perm /022 -type f -exec ls -l {} \;
+If any system-wide shared library file is found to be group-writable or world-writable, then this is a finding.</t>
+        </is>
+      </c>
+      <c r="L229" s="2" t="n"/>
+      <c r="M229" s="2" t="inlineStr">
+        <is>
+          <t>Configure the library files to be protected from unauthorized access. Run the following command, replacing "[FILE]" with any library file with a mode more permissive than 755.
+$ sudo chmod 755 [FILE]</t>
+        </is>
+      </c>
+      <c r="N229" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O229" s="2" t="n"/>
+      <c r="P229" s="2" t="n"/>
+      <c r="Q229" s="2" t="n"/>
     </row>
     <row r="230" ht="130" customHeight="1">
-      <c r="A230" s="3" t="inlineStr">
+      <c r="A230" s="2" t="inlineStr">
         <is>
           <t>CM-5 (6)</t>
         </is>
       </c>
-      <c r="B230" s="3" t="inlineStr">
+      <c r="B230" s="2" t="inlineStr">
         <is>
           <t>CCI-001499</t>
         </is>
       </c>
-      <c r="C230" s="3" t="inlineStr">
+      <c r="C230" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000259-GPOS-00100</t>
         </is>
       </c>
-      <c r="D230" s="3" t="inlineStr">
+      <c r="D230" s="2" t="inlineStr">
         <is>
           <t>CCE-87108-7</t>
         </is>
       </c>
-      <c r="E230" s="3" t="inlineStr">
+      <c r="E230" s="2" t="inlineStr">
         <is>
           <t>The operating system must limit privileges to change software resident within software libraries.</t>
         </is>
       </c>
-      <c r="F230" s="3" t="inlineStr">
+      <c r="F230" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 must limit privileges to change software resident within software libraries.</t>
         </is>
       </c>
-      <c r="G230" s="3" t="inlineStr">
+      <c r="G230" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> If the operating system were to allow any user to make changes to software libraries, then those changes might be implemented without undergoing the appropriate testing and approvals that are part of a robust change management process.
 This requirement applies to operating systems with software libraries that are accessible and configurable, as in the case of interpreted languages. Software libraries also include privileged programs which execute with escalated privileges. Only qualified and authorized individuals shall be allowed to obtain access to information system components for purposes of initiating changes, including upgrades and modifications.</t>
         </is>
       </c>
-      <c r="H230" s="3" t="inlineStr">
+      <c r="H230" s="2" t="inlineStr">
         <is>
           <t>If the operating system were to allow any user to make changes to software libraries,
 then those changes might be implemented without undergoing the appropriate testing and
@@ -18715,39 +18707,39 @@
 for purposes of initiating changes, including upgrades and modifications.</t>
         </is>
       </c>
-      <c r="I230" s="3" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J230" s="3" t="inlineStr">
+      <c r="I230" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J230" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system limits privileges to change software resident within software libraries. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K230" s="3" t="inlineStr">
-        <is>
-          <t>System-wide library files are stored in the following directories:
- /lib
-/lib64
-/usr/lib
-/usr/lib64
-To find if system-wide library files stored in these directories are not group-owned by
-root run the following command for each directory  DIR :
- $ sudo find -L  DIR  ! -group root -type f  
-If system wide library files are not group-owned by root, then this is a finding.</t>
-        </is>
-      </c>
-      <c r="L230" s="3" t="n"/>
-      <c r="M230" s="3" t="inlineStr"/>
-      <c r="N230" s="3" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O230" s="3" t="n"/>
-      <c r="P230" s="3" t="n"/>
-      <c r="Q230" s="3" t="n"/>
+      <c r="K230" s="2" t="inlineStr">
+        <is>
+          <t>Verify the system-wide shared library files are group-owned by "root" with the following command:
+$ sudo find -L /lib /lib64 /usr/lib /usr/lib64 ! -group root -exec ls -l {} \;
+If any system wide shared library file is returned and is not group-owned by a required system account, then this is a finding.</t>
+        </is>
+      </c>
+      <c r="L230" s="2" t="n"/>
+      <c r="M230" s="2" t="inlineStr">
+        <is>
+          <t>Configure the system-wide shared library files (/lib, /lib64, /usr/lib and /usr/lib64) to be protected from unauthorized access.
+Run the following command, replacing "[FILE]" with any library file not group-owned by "root".
+$ sudo chgrp root [FILE]</t>
+        </is>
+      </c>
+      <c r="N230" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O230" s="2" t="n"/>
+      <c r="P230" s="2" t="n"/>
+      <c r="Q230" s="2" t="n"/>
     </row>
     <row r="231" ht="130" customHeight="1">
       <c r="A231" s="2" t="inlineStr">
@@ -18848,7 +18840,7 @@
     <row r="232" ht="130" customHeight="1">
       <c r="A232" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SI-16,CM-6 b</t>
+          <t>SI-16,CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B232" s="2" t="inlineStr">
@@ -19194,7 +19186,7 @@
     <row r="236" ht="130" customHeight="1">
       <c r="A236" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),CM-7 a</t>
+          <t>CM-7 a,AC-18 (1)</t>
         </is>
       </c>
       <c r="B236" s="2" t="inlineStr">
@@ -19761,7 +19753,7 @@
     <row r="243" ht="130" customHeight="1">
       <c r="A243" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (b),IA-5 (1) (a),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (a),IA-5 (1) (b)</t>
         </is>
       </c>
       <c r="B243" s="2" t="inlineStr">
@@ -20329,7 +20321,7 @@
     <row r="250" ht="130" customHeight="1">
       <c r="A250" s="2" t="inlineStr">
         <is>
-          <t>SC-4,CM-6 b</t>
+          <t>CM-6 b,SC-4</t>
         </is>
       </c>
       <c r="B250" s="2" t="inlineStr">
@@ -20410,7 +20402,7 @@
     <row r="251" ht="130" customHeight="1">
       <c r="A251" s="3" t="inlineStr">
         <is>
-          <t>SC-2,SC-4</t>
+          <t>SC-4,SC-2</t>
         </is>
       </c>
       <c r="B251" s="3" t="inlineStr">
@@ -20498,7 +20490,7 @@
     <row r="252" ht="130" customHeight="1">
       <c r="A252" s="3" t="inlineStr">
         <is>
-          <t>SC-2,SC-4</t>
+          <t>SC-4,SC-2</t>
         </is>
       </c>
       <c r="B252" s="3" t="inlineStr">
@@ -20585,7 +20577,7 @@
     <row r="253" ht="130" customHeight="1">
       <c r="A253" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (1)</t>
+          <t>IA-2 (1),IA-2 (11)</t>
         </is>
       </c>
       <c r="B253" s="2" t="inlineStr">
@@ -21087,7 +21079,7 @@
     <row r="259" ht="130" customHeight="1">
       <c r="A259" s="3" t="inlineStr">
         <is>
-          <t>AC-6 (8),AC-6 (9)</t>
+          <t>AC-6 (9),AC-6 (8)</t>
         </is>
       </c>
       <c r="B259" s="3" t="inlineStr">
@@ -21633,7 +21625,7 @@
     <row r="266" ht="130" customHeight="1">
       <c r="A266" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-9</t>
+          <t>AU-9,AU-12 c</t>
         </is>
       </c>
       <c r="B266" s="2" t="inlineStr">
@@ -21716,7 +21708,7 @@
     <row r="267" ht="130" customHeight="1">
       <c r="A267" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (3),CM-6 b</t>
+          <t>CM-6 b,CM-5 (3)</t>
         </is>
       </c>
       <c r="B267" s="2" t="inlineStr">
@@ -22406,7 +22398,7 @@
     <row r="275" ht="130" customHeight="1">
       <c r="A275" s="3" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B275" s="3" t="inlineStr">
@@ -23402,7 +23394,7 @@
     <row r="288" ht="130" customHeight="1">
       <c r="A288" s="3" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B288" s="3" t="inlineStr">
@@ -23473,7 +23465,7 @@
     <row r="289" ht="130" customHeight="1">
       <c r="A289" s="3" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B289" s="3" t="inlineStr">
@@ -23545,7 +23537,7 @@
     <row r="290" ht="130" customHeight="1">
       <c r="A290" s="3" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-6 b</t>
+          <t>CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B290" s="3" t="inlineStr">
@@ -23703,7 +23695,7 @@
     <row r="292" ht="130" customHeight="1">
       <c r="A292" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AC-6 (9),AC-2 (4)</t>
+          <t>AC-2 (4),AU-12 c,AC-6 (9)</t>
         </is>
       </c>
       <c r="B292" s="3" t="inlineStr">
@@ -27446,7 +27438,7 @@
     <row r="341" ht="130" customHeight="1">
       <c r="A341" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),CM-6 b</t>
+          <t>CM-6 b,IA-2 (2)</t>
         </is>
       </c>
       <c r="B341" s="2" t="inlineStr">
@@ -27527,7 +27519,7 @@
     <row r="342" ht="130" customHeight="1">
       <c r="A342" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (1)</t>
+          <t>CM-5 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B342" s="3" t="inlineStr">
@@ -27601,7 +27593,7 @@
     <row r="343" ht="130" customHeight="1">
       <c r="A343" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (1)</t>
+          <t>CM-5 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B343" s="3" t="inlineStr">
@@ -29923,7 +29915,7 @@
     <row r="374" ht="130" customHeight="1">
       <c r="A374" s="2" t="inlineStr">
         <is>
-          <t>AU-3,CM-6 b</t>
+          <t>CM-6 b,AU-3</t>
         </is>
       </c>
       <c r="B374" s="2" t="inlineStr">
@@ -30177,7 +30169,7 @@
     <row r="377" ht="130" customHeight="1">
       <c r="A377" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B377" s="2" t="inlineStr">
@@ -30571,7 +30563,7 @@
     <row r="382" ht="130" customHeight="1">
       <c r="A382" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),AC-17 (9),CM-7 b,CM-6 b</t>
+          <t>CM-6 b,CM-7 b,AC-17 (1),AC-17 (9)</t>
         </is>
       </c>
       <c r="B382" s="2" t="inlineStr">
@@ -30649,7 +30641,7 @@
     <row r="383" ht="130" customHeight="1">
       <c r="A383" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),CM-7 b,CM-6 b</t>
+          <t>CM-6 b,CM-7 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B383" s="2" t="inlineStr">
@@ -33148,7 +33140,7 @@
     <row r="412" ht="130" customHeight="1">
       <c r="A412" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B412" s="2" t="inlineStr">
@@ -33230,7 +33222,7 @@
     <row r="413" ht="130" customHeight="1">
       <c r="A413" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B413" s="2" t="inlineStr">
@@ -33923,7 +33915,7 @@
     <row r="422" ht="130" customHeight="1">
       <c r="A422" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B422" s="2" t="inlineStr">
@@ -34104,7 +34096,7 @@
     <row r="424" ht="130" customHeight="1">
       <c r="A424" s="3" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b</t>
+          <t>CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B424" s="3" t="inlineStr">
@@ -34191,7 +34183,7 @@
     <row r="425" ht="130" customHeight="1">
       <c r="A425" s="3" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b</t>
+          <t>CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B425" s="3" t="inlineStr">
@@ -34526,7 +34518,7 @@
     <row r="429" ht="130" customHeight="1">
       <c r="A429" s="2" t="inlineStr">
         <is>
-          <t>SC-3,CM-6 b</t>
+          <t>CM-6 b,SC-3</t>
         </is>
       </c>
       <c r="B429" s="2" t="inlineStr">
@@ -35282,7 +35274,7 @@
     <row r="439" ht="130" customHeight="1">
       <c r="A439" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B439" s="2" t="inlineStr">
@@ -35372,7 +35364,7 @@
     <row r="440" ht="130" customHeight="1">
       <c r="A440" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B440" s="2" t="inlineStr">
@@ -35767,7 +35759,7 @@
     <row r="445" ht="130" customHeight="1">
       <c r="A445" s="3" t="inlineStr">
         <is>
-          <t>SI-2 (2),CM-6 b</t>
+          <t>CM-6 b,SI-2 (2)</t>
         </is>
       </c>
       <c r="B445" s="3" t="inlineStr">
@@ -36414,7 +36406,7 @@
     <row r="454" ht="130" customHeight="1">
       <c r="A454" s="3" t="inlineStr">
         <is>
-          <t>SI-2 (2),CM-6 b</t>
+          <t>CM-6 b,SI-2 (2)</t>
         </is>
       </c>
       <c r="B454" s="3" t="inlineStr">
@@ -36705,7 +36697,7 @@
     <row r="458" ht="130" customHeight="1">
       <c r="A458" s="3" t="inlineStr">
         <is>
-          <t>SC-10,AC-12,MA-4 (7),MA-4 e</t>
+          <t>AC-12,MA-4 e,SC-10,MA-4 (7)</t>
         </is>
       </c>
       <c r="B458" s="3" t="inlineStr">
@@ -36780,7 +36772,7 @@
     <row r="459" ht="130" customHeight="1">
       <c r="A459" s="3" t="inlineStr">
         <is>
-          <t>SC-10,AC-12</t>
+          <t>AC-12,SC-10</t>
         </is>
       </c>
       <c r="B459" s="3" t="inlineStr">
@@ -36859,7 +36851,7 @@
     <row r="460" ht="130" customHeight="1">
       <c r="A460" s="3" t="inlineStr">
         <is>
-          <t>SC-10,AC-12</t>
+          <t>AC-12,SC-10</t>
         </is>
       </c>
       <c r="B460" s="3" t="inlineStr">
@@ -36935,7 +36927,7 @@
     <row r="461" ht="130" customHeight="1">
       <c r="A461" s="3" t="inlineStr">
         <is>
-          <t>SC-10,AC-11 a</t>
+          <t>AC-11 a,SC-10</t>
         </is>
       </c>
       <c r="B461" s="3" t="inlineStr">
@@ -37012,7 +37004,7 @@
     <row r="462" ht="130" customHeight="1">
       <c r="A462" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),AC-17 (2),SC-8</t>
+          <t>AC-17 (2),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B462" s="2" t="inlineStr">
@@ -38320,7 +38312,7 @@
     <row r="479" ht="130" customHeight="1">
       <c r="A479" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-7 b</t>
+          <t>CM-7 b,IA-3</t>
         </is>
       </c>
       <c r="B479" s="2" t="inlineStr">
@@ -38639,7 +38631,7 @@
     <row r="483" ht="130" customHeight="1">
       <c r="A483" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),CM-7 b</t>
+          <t>CM-7 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B483" s="2" t="inlineStr">
@@ -39762,7 +39754,7 @@
     <row r="497" ht="130" customHeight="1">
       <c r="A497" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-4</t>
+          <t>AU-4,AU-4 (1)</t>
         </is>
       </c>
       <c r="B497" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@bad89e3d0540c4b9faf6af019279b7c9fefd0721 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -973,7 +973,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 b</t>
+          <t>AU-5 b,AU-5 a</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1467,7 +1467,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>AU-7 a,CM-5 (1),MA-4 (1) (a),AU-7 (1),CM-6 b,AU-6 (4),AU-3 (1),AU-3,AU-14 (1),AU-12 a</t>
+          <t>CM-6 b,AU-6 (4),CM-5 (1),AU-7 (1),AU-3,AU-7 a,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-14 (1)</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -1552,7 +1552,7 @@
     <row r="14" ht="130" customHeight="1">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1782,7 +1782,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -2152,7 +2152,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -2226,7 +2226,7 @@
     <row r="23" ht="130" customHeight="1">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -3270,7 +3270,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-14 (1),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1),AU-14 (1)</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -4246,7 +4246,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (11),IA-2 (12),IA-2 (1)</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4330,7 +4330,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>SI-6 d,CM-3 (5),SI-6 b</t>
+          <t>SI-6 b,CM-3 (5),SI-6 d</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4422,7 +4422,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>SI-6 d,CM-3 (5)</t>
+          <t>CM-3 (5),SI-6 d</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -4506,7 +4506,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -4581,7 +4581,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -4656,7 +4656,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -4731,7 +4731,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -4806,7 +4806,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -4881,7 +4881,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -4956,7 +4956,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -5031,7 +5031,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -5106,7 +5106,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -5181,7 +5181,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-7 a,CM-5 (1),AU-12 c,CM-6 b,AU-7 b,AU-8 b,AU-12 (3),AU-12 a</t>
+          <t>CM-6 b,AU-7 b,CM-5 (1),AU-12 c,AU-12 (3),AU-7 a,AU-8 b,AU-12 a</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5255,7 +5255,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a,AC-2 (4)</t>
+          <t>AC-2 (4),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5336,7 +5336,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a,AC-2 (4)</t>
+          <t>AC-2 (4),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5417,7 +5417,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a,AC-2 (4)</t>
+          <t>AC-2 (4),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5499,7 +5499,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a,AC-2 (4)</t>
+          <t>AC-2 (4),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5581,7 +5581,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a,AC-2 (4)</t>
+          <t>AC-2 (4),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5663,7 +5663,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a,AC-2 (4)</t>
+          <t>AC-2 (4),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5745,7 +5745,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a,AC-2 (4)</t>
+          <t>AC-2 (4),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -6865,7 +6865,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -6939,7 +6939,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -7013,7 +7013,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -7087,7 +7087,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -7663,7 +7663,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -7738,7 +7738,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -7813,7 +7813,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -7888,7 +7888,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -7968,7 +7968,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -8050,7 +8050,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -8132,7 +8132,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8214,7 +8214,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8296,7 +8296,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8378,7 +8378,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -8458,7 +8458,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -8538,7 +8538,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -8868,7 +8868,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8947,7 +8947,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -9034,7 +9034,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -9121,7 +9121,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -9366,7 +9366,7 @@
     <row r="113" ht="130" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
-          <t>SC-13,AC-17 (2),SC-8,MA-4 c</t>
+          <t>AC-17 (2),MA-4 c,SC-13,SC-8</t>
         </is>
       </c>
       <c r="B113" s="2" t="inlineStr">
@@ -9526,7 +9526,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9682,7 +9682,7 @@
     <row r="117" ht="130" customHeight="1">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -10038,7 +10038,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -10118,7 +10118,7 @@
     <row r="123" ht="130" customHeight="1">
       <c r="A123" s="2" t="inlineStr">
         <is>
-          <t>SC-28 (1),SC-28</t>
+          <t>SC-28,SC-28 (1)</t>
         </is>
       </c>
       <c r="B123" s="2" t="inlineStr">
@@ -11505,7 +11505,7 @@
     <row r="140" ht="130" customHeight="1">
       <c r="A140" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B140" s="3" t="inlineStr">
@@ -11585,7 +11585,7 @@
     <row r="141" ht="130" customHeight="1">
       <c r="A141" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B141" s="3" t="inlineStr">
@@ -11665,7 +11665,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B142" s="3" t="inlineStr">
@@ -11977,7 +11977,7 @@
     <row r="146" ht="130" customHeight="1">
       <c r="A146" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),IA-7</t>
+          <t>IA-7,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B146" s="2" t="inlineStr">
@@ -12766,7 +12766,7 @@
     <row r="156" ht="130" customHeight="1">
       <c r="A156" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,IA-7</t>
+          <t>IA-7,CM-7 a</t>
         </is>
       </c>
       <c r="B156" s="2" t="inlineStr">
@@ -12845,7 +12845,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B157" s="3" t="inlineStr">
@@ -12922,7 +12922,7 @@
     <row r="158" ht="130" customHeight="1">
       <c r="A158" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B158" s="3" t="inlineStr">
@@ -12995,7 +12995,7 @@
     <row r="159" ht="130" customHeight="1">
       <c r="A159" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,MA-4 (1) (a),AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B159" s="3" t="inlineStr">
@@ -13068,7 +13068,7 @@
     <row r="160" ht="130" customHeight="1">
       <c r="A160" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B160" s="3" t="inlineStr">
@@ -13153,7 +13153,7 @@
     <row r="161" ht="130" customHeight="1">
       <c r="A161" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B161" s="3" t="inlineStr">
@@ -13228,7 +13228,7 @@
     <row r="162" ht="130" customHeight="1">
       <c r="A162" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B162" s="3" t="inlineStr">
@@ -13303,7 +13303,7 @@
     <row r="163" ht="130" customHeight="1">
       <c r="A163" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B163" s="3" t="inlineStr">
@@ -13378,7 +13378,7 @@
     <row r="164" ht="130" customHeight="1">
       <c r="A164" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B164" s="3" t="inlineStr">
@@ -13881,7 +13881,7 @@
     <row r="171" ht="130" customHeight="1">
       <c r="A171" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B171" s="3" t="inlineStr">
@@ -14170,7 +14170,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B175" s="3" t="inlineStr">
@@ -14245,7 +14245,7 @@
     <row r="176" ht="130" customHeight="1">
       <c r="A176" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B176" s="3" t="inlineStr">
@@ -14327,7 +14327,7 @@
     <row r="177" ht="130" customHeight="1">
       <c r="A177" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B177" s="3" t="inlineStr">
@@ -14409,7 +14409,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B178" s="3" t="inlineStr">
@@ -14491,7 +14491,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B179" s="3" t="inlineStr">
@@ -14573,7 +14573,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B180" s="3" t="inlineStr">
@@ -14655,7 +14655,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B181" s="3" t="inlineStr">
@@ -14737,7 +14737,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B182" s="3" t="inlineStr">
@@ -14819,7 +14819,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B183" s="3" t="inlineStr">
@@ -14901,7 +14901,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B184" s="3" t="inlineStr">
@@ -14983,7 +14983,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B185" s="3" t="inlineStr">
@@ -15061,7 +15061,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B186" s="3" t="inlineStr">
@@ -15140,7 +15140,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B187" s="3" t="inlineStr">
@@ -15222,7 +15222,7 @@
     <row r="188" ht="130" customHeight="1">
       <c r="A188" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B188" s="3" t="inlineStr">
@@ -15304,7 +15304,7 @@
     <row r="189" ht="130" customHeight="1">
       <c r="A189" s="3" t="inlineStr">
         <is>
-          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
+          <t>AU-3,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B189" s="3" t="inlineStr">
@@ -15386,7 +15386,7 @@
     <row r="190" ht="130" customHeight="1">
       <c r="A190" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B190" s="3" t="inlineStr">
@@ -15468,7 +15468,7 @@
     <row r="191" ht="130" customHeight="1">
       <c r="A191" s="3" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a),AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B191" s="3" t="inlineStr">
@@ -15550,7 +15550,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B192" s="3" t="inlineStr">
@@ -15632,7 +15632,7 @@
     <row r="193" ht="130" customHeight="1">
       <c r="A193" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a</t>
+          <t>AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B193" s="3" t="inlineStr">
@@ -15707,7 +15707,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AU-12 a,AC-2 (4)</t>
+          <t>AC-2 (4),AU-3,AU-12 c,AU-12 a,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B194" s="3" t="inlineStr">
@@ -15780,7 +15780,7 @@
     <row r="195" ht="130" customHeight="1">
       <c r="A195" s="3" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3,AC-2 (4)</t>
+          <t>AC-2 (4),AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B195" s="3" t="inlineStr">
@@ -15857,7 +15857,7 @@
     <row r="196" ht="130" customHeight="1">
       <c r="A196" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2 (2),IA-2 (1),IA-2 (4)</t>
+          <t>IA-2 (2),IA-2 (4),IA-2 (3),IA-2 (1)</t>
         </is>
       </c>
       <c r="B196" s="2" t="inlineStr">
@@ -15944,7 +15944,7 @@
     <row r="197" ht="130" customHeight="1">
       <c r="A197" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),IA-2,IA-2 (3),IA-2 (4),IA-2 (2)</t>
+          <t>IA-2 (3),IA-2 (5),IA-2 (2),IA-2 (4),IA-2</t>
         </is>
       </c>
       <c r="B197" s="2" t="inlineStr">
@@ -16033,7 +16033,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),IA-2,IA-2 (3),IA-2 (4),IA-2 (2)</t>
+          <t>IA-2 (3),IA-2 (5),IA-2 (2),IA-2 (4),IA-2</t>
         </is>
       </c>
       <c r="B198" s="2" t="inlineStr">
@@ -16657,7 +16657,7 @@
     <row r="206" ht="130" customHeight="1">
       <c r="A206" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8,SC-8 (1)</t>
+          <t>SC-8,SC-8 (2),SC-8 (1)</t>
         </is>
       </c>
       <c r="B206" s="2" t="inlineStr">
@@ -16734,7 +16734,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8,SC-8 (1)</t>
+          <t>SC-8,SC-8 (2),SC-8 (1)</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -16820,7 +16820,7 @@
     <row r="208" ht="130" customHeight="1">
       <c r="A208" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8,AC-18 (1)</t>
+          <t>AC-18 (1),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B208" s="2" t="inlineStr">
@@ -17248,7 +17248,7 @@
     <row r="213" ht="130" customHeight="1">
       <c r="A213" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-7 a,CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (c),CM-7 a</t>
         </is>
       </c>
       <c r="B213" s="2" t="inlineStr">
@@ -17499,7 +17499,7 @@
     <row r="216" ht="130" customHeight="1">
       <c r="A216" s="2" t="inlineStr">
         <is>
-          <t>SC-5,CM-6 b,SC-5 (2)</t>
+          <t>CM-6 b,SC-5 (2),SC-5</t>
         </is>
       </c>
       <c r="B216" s="2" t="inlineStr">
@@ -17771,7 +17771,7 @@
     <row r="219" ht="130" customHeight="1">
       <c r="A219" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-6 b</t>
+          <t>CM-6 b,SI-16</t>
         </is>
       </c>
       <c r="B219" s="2" t="inlineStr">
@@ -17869,7 +17869,7 @@
     <row r="220" ht="130" customHeight="1">
       <c r="A220" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),IA-8,IA-2</t>
+          <t>IA-8,IA-2,AU-3 (1)</t>
         </is>
       </c>
       <c r="B220" s="2" t="inlineStr">
@@ -18840,7 +18840,7 @@
     <row r="232" ht="130" customHeight="1">
       <c r="A232" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-6 b,SC-2</t>
+          <t>CM-6 b,SI-16,SC-2</t>
         </is>
       </c>
       <c r="B232" s="2" t="inlineStr">
@@ -19186,7 +19186,7 @@
     <row r="236" ht="130" customHeight="1">
       <c r="A236" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,AC-18 (1)</t>
+          <t>AC-18 (1),CM-7 a</t>
         </is>
       </c>
       <c r="B236" s="2" t="inlineStr">
@@ -20577,7 +20577,7 @@
     <row r="253" ht="130" customHeight="1">
       <c r="A253" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (1)</t>
         </is>
       </c>
       <c r="B253" s="2" t="inlineStr">
@@ -21159,7 +21159,7 @@
     <row r="260" ht="130" customHeight="1">
       <c r="A260" s="3" t="inlineStr">
         <is>
-          <t>IA-2 (5),CM-6 b</t>
+          <t>CM-6 b,IA-2 (5)</t>
         </is>
       </c>
       <c r="B260" s="3" t="inlineStr">
@@ -21625,7 +21625,7 @@
     <row r="266" ht="130" customHeight="1">
       <c r="A266" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-12 c</t>
+          <t>AU-12 c,AU-9</t>
         </is>
       </c>
       <c r="B266" s="2" t="inlineStr">
@@ -22546,7 +22546,7 @@
     <row r="277" ht="130" customHeight="1">
       <c r="A277" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-7 b</t>
+          <t>CM-7 b,CM-7 a</t>
         </is>
       </c>
       <c r="B277" s="2" t="inlineStr">
@@ -22626,7 +22626,7 @@
     <row r="278" ht="130" customHeight="1">
       <c r="A278" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a,CM-7 b</t>
+          <t>CM-7 b,CM-7 a</t>
         </is>
       </c>
       <c r="B278" s="2" t="inlineStr">
@@ -27288,7 +27288,7 @@
     <row r="339" ht="130" customHeight="1">
       <c r="A339" s="3" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B339" s="3" t="inlineStr">
@@ -27519,7 +27519,7 @@
     <row r="342" ht="130" customHeight="1">
       <c r="A342" s="3" t="inlineStr">
         <is>
-          <t>CM-5 (1),CM-6 b</t>
+          <t>CM-6 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B342" s="3" t="inlineStr">
@@ -27593,7 +27593,7 @@
     <row r="343" ht="130" customHeight="1">
       <c r="A343" s="3" t="inlineStr">
         <is>
-          <t>CM-5 (1),CM-6 b</t>
+          <t>CM-6 b,CM-5 (1)</t>
         </is>
       </c>
       <c r="B343" s="3" t="inlineStr">
@@ -28178,7 +28178,7 @@
     <row r="351" ht="130" customHeight="1">
       <c r="A351" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),CM-6 b</t>
+          <t>CM-6 b,AC-17 (2)</t>
         </is>
       </c>
       <c r="B351" s="2" t="inlineStr">
@@ -33140,7 +33140,7 @@
     <row r="412" ht="130" customHeight="1">
       <c r="A412" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B412" s="2" t="inlineStr">
@@ -33222,7 +33222,7 @@
     <row r="413" ht="130" customHeight="1">
       <c r="A413" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B413" s="2" t="inlineStr">
@@ -34970,7 +34970,7 @@
     <row r="435" ht="130" customHeight="1">
       <c r="A435" s="2" t="inlineStr">
         <is>
-          <t>AU-4,CM-6 b</t>
+          <t>CM-6 b,AU-4</t>
         </is>
       </c>
       <c r="B435" s="2" t="inlineStr">
@@ -35274,7 +35274,7 @@
     <row r="439" ht="130" customHeight="1">
       <c r="A439" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B439" s="2" t="inlineStr">
@@ -35364,7 +35364,7 @@
     <row r="440" ht="130" customHeight="1">
       <c r="A440" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B440" s="2" t="inlineStr">
@@ -36697,7 +36697,7 @@
     <row r="458" ht="130" customHeight="1">
       <c r="A458" s="3" t="inlineStr">
         <is>
-          <t>AC-12,MA-4 e,SC-10,MA-4 (7)</t>
+          <t>MA-4 e,MA-4 (7),SC-10,AC-12</t>
         </is>
       </c>
       <c r="B458" s="3" t="inlineStr">
@@ -36772,7 +36772,7 @@
     <row r="459" ht="130" customHeight="1">
       <c r="A459" s="3" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B459" s="3" t="inlineStr">
@@ -36851,7 +36851,7 @@
     <row r="460" ht="130" customHeight="1">
       <c r="A460" s="3" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B460" s="3" t="inlineStr">
@@ -38312,7 +38312,7 @@
     <row r="479" ht="130" customHeight="1">
       <c r="A479" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b,IA-3</t>
+          <t>IA-3,CM-7 b</t>
         </is>
       </c>
       <c r="B479" s="2" t="inlineStr">
@@ -41474,7 +41474,7 @@
     <row r="518" ht="130" customHeight="1">
       <c r="A518" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8</t>
+          <t>SC-8,SC-8 (2)</t>
         </is>
       </c>
       <c r="B518" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ rhmdnd/content@3cc1fb136547a4c738ce416193ea9666031333fb 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -550,7 +550,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -634,7 +634,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -719,7 +719,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -791,7 +791,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -973,7 +973,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 b</t>
+          <t>AU-5 b,AU-5 a</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1467,7 +1467,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-14 (1),MA-4 (1) (a),AU-3 (1),AU-7 (1),CM-5 (1),AU-12 a,AU-6 (4),CM-6 b,AU-7 a</t>
+          <t>AU-7 b,AU-3 (1),AU-14 (1),AU-3,MA-4 (1) (a),AU-8 b,CM-5 (1),AU-12 c,AU-12 a,AU-6 (4),AU-7 (1),AU-12 (3),AU-7 a</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -1477,7 +1477,7 @@
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>SRG-OS-000037-GPOS-00015,SRG-OS-000038-GPOS-00016,SRG-OS-000039-GPOS-00017,SRG-OS-000040-GPOS-00018,SRG-OS-000041-GPOS-00019,SRG-OS-000042-GPOS-00021,SRG-OS-000051-GPOS-00024,SRG-OS-000054-GPOS-00025,SRG-OS-000122-GPOS-00063,SRG-OS-000254-GPOS-00095,SRG-OS-000255-GPOS-00096,SRG-OS-000365-GPOS-00152,SRG-OS-000392-GPOS-00172,SRG-OS-000480-GPOS-00227,SRG-OS-000062-GPOS-00031,SRG-OS-000349-GPOS-00137</t>
+          <t>SRG-OS-000062-GPOS-00031,SRG-OS-000037-GPOS-00015,SRG-OS-000038-GPOS-00016,SRG-OS-000039-GPOS-00017,SRG-OS-000040-GPOS-00018,SRG-OS-000041-GPOS-00019,SRG-OS-000042-GPOS-00021,SRG-OS-000051-GPOS-00024,SRG-OS-000054-GPOS-00025,SRG-OS-000122-GPOS-00063,SRG-OS-000254-GPOS-00095,SRG-OS-000255-GPOS-00096,SRG-OS-000337-GPOS-00129,SRG-OS-000348-GPOS-00136,SRG-OS-000349-GPOS-00137,SRG-OS-000350-GPOS-00138,SRG-OS-000351-GPOS-00139,SRG-OS-000352-GPOS-00140,SRG-OS-000353-GPOS-00141,SRG-OS-000354-GPOS-00142,SRG-OS-000358-GPOS-00145,SRG-OS-000365-GPOS-00152,SRG-OS-000392-GPOS-00172,SRG-OS-000475-GPOS-00220</t>
         </is>
       </c>
       <c r="D13" s="2" t="inlineStr">
@@ -1552,7 +1552,7 @@
     <row r="14" ht="130" customHeight="1">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1782,7 +1782,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -2152,7 +2152,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -2226,7 +2226,7 @@
     <row r="23" ht="130" customHeight="1">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-7 (2)</t>
+          <t>CM-7 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -3270,7 +3270,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3,AU-14 (1),MA-4 (1) (a),AU-3 (1),AU-12 a</t>
+          <t>AU-3 (1),AU-14 (1),AU-3,MA-4 (1) (a),AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3343,7 +3343,7 @@
         <is>
           <t xml:space="preserve">To ensure that "audit=1" is added as a kernel command line
 argument to newly installed kernels, add "audit=1" to the
-default Grub2 command line for Linux operating systems.  Modify the line within
+default Grub2 command line for Linux operating systems. Modify the line within
 "/etc/default/grub" as shown below:
  GRUB_CMDLINE_LINUX="... audit=1 ..." 
 Run the following command to update command line for already installed kernels: # grubby --update-kernel=ALL --args="audit=1" </t>
@@ -3361,7 +3361,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-14 (1)</t>
+          <t>AU-14 (1),AU-4</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3432,10 +3432,9 @@
       <c r="L38" s="2" t="n"/>
       <c r="M38" s="2" t="inlineStr">
         <is>
-          <t>Configure Red Hat Enterprise Linux 9 to allocate sufficient audit_backlog_limit to capture processes that start prior to the audit daemon with the following command:
-$ sudo grubby --update-kernel=ALL --args="audit_backlog_limit=8192"
-Add or modify the following line in "/etc/default/grub" to ensure the configuration survives kernel updates:
-GRUB_CMDLINE_LINUX="audit_backlog_limit=8192"</t>
+          <t xml:space="preserve">
+Run the following command:
+$ sudo grubby --update-kernel=ALL --args=audit_backlog_limit=8192</t>
         </is>
       </c>
       <c r="N38" s="2" t="inlineStr">
@@ -3450,58 +3449,131 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-3</t>
+          <t>AU-7 b,AU-3 (1),AU-14 (1),AU-3,MA-4 (1) (a),AU-8 b,CM-5 (1),AU-12 c,AU-12 a,AU-6 (4),AU-7 (1),AU-12 (3),AU-7 a</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
         <is>
+          <t>CCI-000172,CCI-001814,CCI-001875,CCI-001877,CCI-001878,CCI-001879,CCI-001880,CCI-001881,CCI-001882,CCI-001889,CCI-001914,CCI-000169</t>
+        </is>
+      </c>
+      <c r="C39" s="2" t="inlineStr">
+        <is>
+          <t>SRG-OS-000062-GPOS-00031,SRG-OS-000037-GPOS-00015,SRG-OS-000038-GPOS-00016,SRG-OS-000039-GPOS-00017,SRG-OS-000040-GPOS-00018,SRG-OS-000041-GPOS-00019,SRG-OS-000042-GPOS-00021,SRG-OS-000051-GPOS-00024,SRG-OS-000054-GPOS-00025,SRG-OS-000122-GPOS-00063,SRG-OS-000254-GPOS-00095,SRG-OS-000255-GPOS-00096,SRG-OS-000337-GPOS-00129,SRG-OS-000348-GPOS-00136,SRG-OS-000349-GPOS-00137,SRG-OS-000350-GPOS-00138,SRG-OS-000351-GPOS-00139,SRG-OS-000352-GPOS-00140,SRG-OS-000353-GPOS-00141,SRG-OS-000354-GPOS-00142,SRG-OS-000358-GPOS-00145,SRG-OS-000365-GPOS-00152,SRG-OS-000392-GPOS-00172,SRG-OS-000475-GPOS-00220</t>
+        </is>
+      </c>
+      <c r="D39" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83649-4</t>
+        </is>
+      </c>
+      <c r="E39" s="2" t="inlineStr">
+        <is>
+          <t>The operating system must initiate session audits at system start-up.</t>
+        </is>
+      </c>
+      <c r="F39" s="2" t="inlineStr">
+        <is>
+          <t>Red Hat Enterprise Linux 9 Must Initiate Session Audits At System Start-Up.</t>
+        </is>
+      </c>
+      <c r="G39" s="2" t="inlineStr">
+        <is>
+          <t>If auditing is enabled late in the start-up process, the actions of some start-up processes may not be audited. Some audit systems also maintain state information only available if auditing is enabled before a given process is created.</t>
+        </is>
+      </c>
+      <c r="H39" s="2" t="inlineStr">
+        <is>
+          <t>The auditd service is an access monitoring and accounting daemon, watching system calls to audit any access, in comparison with potential local access control policy such as SELinux policy.</t>
+        </is>
+      </c>
+      <c r="I39" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J39" s="2" t="inlineStr">
+        <is>
+          <t>Verify the operating system initiates session audits at system start-up. If it does not, this is a finding.</t>
+        </is>
+      </c>
+      <c r="K39" s="2" t="inlineStr">
+        <is>
+          <t>Run the following command to determine if the  audit  package is installed:  $ rpm -q audit 
+If the audit package is not installed, then this is a finding.</t>
+        </is>
+      </c>
+      <c r="L39" s="2" t="n"/>
+      <c r="M39" s="2" t="inlineStr">
+        <is>
+          <t>Install the audit service (if the audit service is not already installed) with the following command:
+$ sudo dnf install audit</t>
+        </is>
+      </c>
+      <c r="N39" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O39" s="2" t="n"/>
+      <c r="P39" s="2" t="n"/>
+      <c r="Q39" s="2" t="n"/>
+    </row>
+    <row r="40" ht="130" customHeight="1">
+      <c r="A40" s="2" t="inlineStr">
+        <is>
+          <t>AU-3,AU-4 (1)</t>
+        </is>
+      </c>
+      <c r="B40" s="2" t="inlineStr">
+        <is>
           <t>CCI-001851</t>
         </is>
       </c>
-      <c r="C39" s="2" t="inlineStr">
+      <c r="C40" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000039-GPOS-00017,SRG-OS-000342-GPOS-00133,SRG-OS-000479-GPOS-00224</t>
         </is>
       </c>
-      <c r="D39" s="2" t="inlineStr">
+      <c r="D40" s="2" t="inlineStr">
         <is>
           <t>CCE-83686-6</t>
         </is>
       </c>
-      <c r="E39" s="2" t="inlineStr">
+      <c r="E40" s="2" t="inlineStr">
         <is>
           <t>The operating system must, at a minimum, off-load audit data from interconnected systems in real time and off-load audit data from standalone systems weekly.</t>
         </is>
       </c>
-      <c r="F39" s="2" t="inlineStr">
+      <c r="F40" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 Must, At A Minimum, Off-Load Audit Data From Interconnected Systems In Real Time And Off-Load Audit Data From Standalone Systems Weekly.</t>
         </is>
       </c>
-      <c r="G39" s="2" t="inlineStr">
+      <c r="G40" s="2" t="inlineStr">
         <is>
           <t>Information stored in one location is vulnerable to accidental or incidental deletion or alteration.
 Off-loading is a common process in information systems with limited audit storage capacity.</t>
         </is>
       </c>
-      <c r="H39" s="2" t="inlineStr">
+      <c r="H40" s="2" t="inlineStr">
         <is>
           <t>If option "name_format" is left at its default value of
 "none", audit events from different computers may be hard
 to distinguish.</t>
         </is>
       </c>
-      <c r="I39" s="2" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J39" s="2" t="inlineStr">
+      <c r="I40" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J40" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system, at a minimum, off-loads interconnected systems in real time and off-loads standalone systems weekly. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K39" s="2" t="inlineStr">
+      <c r="K40" s="2" t="inlineStr">
         <is>
           <t>To verify that Audit Daemon is configured to record the hostname
 in audit events, run the following command:
@@ -3511,76 +3583,76 @@
 If name_format isn't set to hostname, then this is a finding.</t>
         </is>
       </c>
-      <c r="L39" s="2" t="n"/>
-      <c r="M39" s="2" t="inlineStr">
+      <c r="L40" s="2" t="n"/>
+      <c r="M40" s="2" t="inlineStr">
         <is>
           <t>Edit the file "/etc/audit/auditd.conf" and add or edit the following line:
 name_format = hostname</t>
         </is>
       </c>
-      <c r="N39" s="2" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O39" s="2" t="n"/>
-      <c r="P39" s="2" t="n"/>
-      <c r="Q39" s="2" t="n"/>
-    </row>
-    <row r="40" ht="130" customHeight="1">
-      <c r="A40" s="3" t="inlineStr">
+      <c r="N40" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O40" s="2" t="n"/>
+      <c r="P40" s="2" t="n"/>
+      <c r="Q40" s="2" t="n"/>
+    </row>
+    <row r="41" ht="130" customHeight="1">
+      <c r="A41" s="3" t="inlineStr">
         <is>
           <t>AU-4 (1)</t>
         </is>
       </c>
-      <c r="B40" s="3" t="inlineStr">
+      <c r="B41" s="3" t="inlineStr">
         <is>
           <t>CCI-001851</t>
         </is>
       </c>
-      <c r="C40" s="3" t="inlineStr">
+      <c r="C41" s="3" t="inlineStr">
         <is>
           <t>SRG-OS-000342-GPOS-00133,SRG-OS-000479-GPOS-00224</t>
         </is>
       </c>
-      <c r="D40" s="3" t="inlineStr">
+      <c r="D41" s="3" t="inlineStr">
         <is>
           <t>CCE-87901-5</t>
         </is>
       </c>
-      <c r="E40" s="3" t="inlineStr">
+      <c r="E41" s="3" t="inlineStr">
         <is>
           <t>The operating system must, at a minimum, off-load audit data from interconnected systems in real time and off-load audit data from standalone systems weekly.</t>
         </is>
       </c>
-      <c r="F40" s="3" t="inlineStr">
+      <c r="F41" s="3" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 Must, At A Minimum, Off-Load Audit Data From Interconnected Systems In Real Time And Off-Load Audit Data From Standalone Systems Weekly.</t>
         </is>
       </c>
-      <c r="G40" s="3" t="inlineStr">
+      <c r="G41" s="3" t="inlineStr">
         <is>
           <t>Information stored in one location is vulnerable to accidental or incidental deletion or alteration.
 Off-loading is a common process in information systems with limited audit storage capacity.</t>
         </is>
       </c>
-      <c r="H40" s="3" t="inlineStr">
+      <c r="H41" s="3" t="inlineStr">
         <is>
           <t>The audit system should have an action setup in the event the internal event queue becomes full
 so that no data is lost.</t>
         </is>
       </c>
-      <c r="I40" s="3" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J40" s="3" t="inlineStr">
+      <c r="I41" s="3" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J41" s="3" t="inlineStr">
         <is>
           <t>Verify the operating system, at a minimum, off-loads interconnected systems in real time and off-loads standalone systems weekly. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K40" s="3" t="inlineStr">
+      <c r="K41" s="3" t="inlineStr">
         <is>
           <t>Verify the audit system is configured to take an appropriate action when the internal event queue is full:
  $ sudo grep -i overflow_action /etc/audit/auditd.conf 
@@ -3591,72 +3663,72 @@
 If auditd overflow action is not setup correctly, then this is a finding.</t>
         </is>
       </c>
-      <c r="L40" s="3" t="n"/>
-      <c r="M40" s="3" t="inlineStr"/>
-      <c r="N40" s="3" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O40" s="3" t="n"/>
-      <c r="P40" s="3" t="n"/>
-      <c r="Q40" s="3" t="n"/>
-    </row>
-    <row r="41" ht="130" customHeight="1">
-      <c r="A41" s="2" t="inlineStr">
+      <c r="L41" s="3" t="n"/>
+      <c r="M41" s="3" t="inlineStr"/>
+      <c r="N41" s="3" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O41" s="3" t="n"/>
+      <c r="P41" s="3" t="n"/>
+      <c r="Q41" s="3" t="n"/>
+    </row>
+    <row r="42" ht="130" customHeight="1">
+      <c r="A42" s="2" t="inlineStr">
         <is>
           <t>AU-4 (1)</t>
         </is>
       </c>
-      <c r="B41" s="2" t="inlineStr">
+      <c r="B42" s="2" t="inlineStr">
         <is>
           <t>CCI-001851</t>
         </is>
       </c>
-      <c r="C41" s="2" t="inlineStr">
+      <c r="C42" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000342-GPOS-00133,SRG-OS-000479-GPOS-00224</t>
         </is>
       </c>
-      <c r="D41" s="2" t="inlineStr">
+      <c r="D42" s="2" t="inlineStr">
         <is>
           <t>CCE-86871-1</t>
         </is>
       </c>
-      <c r="E41" s="2" t="inlineStr">
+      <c r="E42" s="2" t="inlineStr">
         <is>
           <t>The operating system must, at a minimum, off-load audit data from interconnected systems in real time and off-load audit data from standalone systems weekly.</t>
         </is>
       </c>
-      <c r="F41" s="2" t="inlineStr">
+      <c r="F42" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 Must, At A Minimum, Off-Load Audit Data From Interconnected Systems In Real Time And Off-Load Audit Data From Standalone Systems Weekly.</t>
         </is>
       </c>
-      <c r="G41" s="2" t="inlineStr">
+      <c r="G42" s="2" t="inlineStr">
         <is>
           <t>Information stored in one location is vulnerable to accidental or incidental deletion or alteration.
 Off-loading is a common process in information systems with limited audit storage capacity.</t>
         </is>
       </c>
-      <c r="H41" s="2" t="inlineStr">
+      <c r="H42" s="2" t="inlineStr">
         <is>
           <t>The audit records generated by Rsyslog contain valuable information regarding system
 configuration, user authentication, and other such information. Audit records should be
 protected from unauthorized access.</t>
         </is>
       </c>
-      <c r="I41" s="2" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J41" s="2" t="inlineStr">
+      <c r="I42" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J42" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system, at a minimum, off-loads interconnected systems in real time and off-loads standalone systems weekly. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K41" s="2" t="inlineStr">
+      <c r="K42" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system authenticates the remote logging server for off-loading audit logs with the following command:
  $ sudo grep -i '$ActionSendStreamDriverAuthMode' /etc/rsyslog.conf /etc/rsyslog.d/*.conf 
@@ -3665,77 +3737,77 @@
 If $ActionSendStreamDriverAuthMode in /etc/rsyslog.conf is not set to x509/name, then this is a finding.</t>
         </is>
       </c>
-      <c r="L41" s="2" t="n"/>
-      <c r="M41" s="2" t="inlineStr">
+      <c r="L42" s="2" t="n"/>
+      <c r="M42" s="2" t="inlineStr">
         <is>
           <t>Configure Red Hat Enterprise Linux 9 to authenticate the remote logging server for off-loading audit logs by setting the following option in "/etc/rsyslog.conf" or "/etc/rsyslog.d/[customfile].conf":
 $ActionSendStreamDriverAuthMode x509/name</t>
         </is>
       </c>
-      <c r="N41" s="2" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O41" s="2" t="n"/>
-      <c r="P41" s="2" t="n"/>
-      <c r="Q41" s="2" t="n"/>
-    </row>
-    <row r="42" ht="130" customHeight="1">
-      <c r="A42" s="2" t="inlineStr">
+      <c r="N42" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O42" s="2" t="n"/>
+      <c r="P42" s="2" t="n"/>
+      <c r="Q42" s="2" t="n"/>
+    </row>
+    <row r="43" ht="130" customHeight="1">
+      <c r="A43" s="2" t="inlineStr">
         <is>
           <t>AU-4 (1)</t>
         </is>
       </c>
-      <c r="B42" s="2" t="inlineStr">
+      <c r="B43" s="2" t="inlineStr">
         <is>
           <t>CCI-001851</t>
         </is>
       </c>
-      <c r="C42" s="2" t="inlineStr">
+      <c r="C43" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000342-GPOS-00133,SRG-OS-000479-GPOS-00224</t>
         </is>
       </c>
-      <c r="D42" s="2" t="inlineStr">
+      <c r="D43" s="2" t="inlineStr">
         <is>
           <t>CCE-90191-8</t>
         </is>
       </c>
-      <c r="E42" s="2" t="inlineStr">
+      <c r="E43" s="2" t="inlineStr">
         <is>
           <t>The operating system must, at a minimum, off-load audit data from interconnected systems in real time and off-load audit data from standalone systems weekly.</t>
         </is>
       </c>
-      <c r="F42" s="2" t="inlineStr">
+      <c r="F43" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 Must, At A Minimum, Off-Load Audit Data From Interconnected Systems In Real Time And Off-Load Audit Data From Standalone Systems Weekly.</t>
         </is>
       </c>
-      <c r="G42" s="2" t="inlineStr">
+      <c r="G43" s="2" t="inlineStr">
         <is>
           <t>Information stored in one location is vulnerable to accidental or incidental deletion or alteration.
 Off-loading is a common process in information systems with limited audit storage capacity.</t>
         </is>
       </c>
-      <c r="H42" s="2" t="inlineStr">
+      <c r="H43" s="2" t="inlineStr">
         <is>
           <t>The audit records generated by Rsyslog contain valuable information regarding system
 configuration, user authentication, and other such information. Audit records should be
 protected from unauthorized access.</t>
         </is>
       </c>
-      <c r="I42" s="2" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J42" s="2" t="inlineStr">
+      <c r="I43" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J43" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system, at a minimum, off-loads interconnected systems in real time and off-loads standalone systems weekly. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K42" s="2" t="inlineStr">
+      <c r="K43" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system encrypts audit records off-loaded onto a different system
 or media from the system being audited with the following commands:
@@ -3745,77 +3817,77 @@
 If rsyslogd ActionSendStreamDriverMode not set to 1, then this is a finding.</t>
         </is>
       </c>
-      <c r="L42" s="2" t="n"/>
-      <c r="M42" s="2" t="inlineStr">
+      <c r="L43" s="2" t="n"/>
+      <c r="M43" s="2" t="inlineStr">
         <is>
           <t>Configure the operating system to encrypt off-loaded audit records by setting the following options in "/etc/rsyslog.conf" or "/etc/rsyslog.d/[customfile].conf":
 $ActionSendStreamDriverMode 1</t>
         </is>
       </c>
-      <c r="N42" s="2" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O42" s="2" t="n"/>
-      <c r="P42" s="2" t="n"/>
-      <c r="Q42" s="2" t="n"/>
-    </row>
-    <row r="43" ht="130" customHeight="1">
-      <c r="A43" s="2" t="inlineStr">
+      <c r="N43" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O43" s="2" t="n"/>
+      <c r="P43" s="2" t="n"/>
+      <c r="Q43" s="2" t="n"/>
+    </row>
+    <row r="44" ht="130" customHeight="1">
+      <c r="A44" s="2" t="inlineStr">
         <is>
           <t>AU-4 (1)</t>
         </is>
       </c>
-      <c r="B43" s="2" t="inlineStr">
+      <c r="B44" s="2" t="inlineStr">
         <is>
           <t>CCI-001851</t>
         </is>
       </c>
-      <c r="C43" s="2" t="inlineStr">
+      <c r="C44" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000342-GPOS-00133,SRG-OS-000479-GPOS-00224</t>
         </is>
       </c>
-      <c r="D43" s="2" t="inlineStr">
+      <c r="D44" s="2" t="inlineStr">
         <is>
           <t>CCE-86782-0</t>
         </is>
       </c>
-      <c r="E43" s="2" t="inlineStr">
+      <c r="E44" s="2" t="inlineStr">
         <is>
           <t>The operating system must, at a minimum, off-load audit data from interconnected systems in real time and off-load audit data from standalone systems weekly.</t>
         </is>
       </c>
-      <c r="F43" s="2" t="inlineStr">
+      <c r="F44" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 Must, At A Minimum, Off-Load Audit Data From Interconnected Systems In Real Time And Off-Load Audit Data From Standalone Systems Weekly.</t>
         </is>
       </c>
-      <c r="G43" s="2" t="inlineStr">
+      <c r="G44" s="2" t="inlineStr">
         <is>
           <t>Information stored in one location is vulnerable to accidental or incidental deletion or alteration.
 Off-loading is a common process in information systems with limited audit storage capacity.</t>
         </is>
       </c>
-      <c r="H43" s="2" t="inlineStr">
+      <c r="H44" s="2" t="inlineStr">
         <is>
           <t>The audit records generated by Rsyslog contain valuable information regarding system
 configuration, user authentication, and other such information. Audit records should be
 protected from unauthorized access.</t>
         </is>
       </c>
-      <c r="I43" s="2" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J43" s="2" t="inlineStr">
+      <c r="I44" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J44" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system, at a minimum, off-loads interconnected systems in real time and off-loads standalone systems weekly. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K43" s="2" t="inlineStr">
+      <c r="K44" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system encrypts audit records off-loaded onto a different system
 or media from the system being audited with the following commands:
@@ -3825,136 +3897,136 @@
 If rsyslogd DefaultNetstreamDriver not set to gtls, then this is a finding.</t>
         </is>
       </c>
-      <c r="L43" s="2" t="n"/>
-      <c r="M43" s="2" t="inlineStr">
+      <c r="L44" s="2" t="n"/>
+      <c r="M44" s="2" t="inlineStr">
         <is>
           <t>Configure the operating system to encrypt off-loaded audit records by setting the following options in "/etc/rsyslog.conf" or "/etc/rsyslog.d/[customfile].conf":
 $DefaultNetstreamDriver gtls</t>
         </is>
       </c>
-      <c r="N43" s="2" t="inlineStr">
-        <is>
-          <t>CAT II</t>
-        </is>
-      </c>
-      <c r="O43" s="2" t="n"/>
-      <c r="P43" s="2" t="n"/>
-      <c r="Q43" s="2" t="n"/>
-    </row>
-    <row r="44" ht="130" customHeight="1">
-      <c r="A44" s="2" t="inlineStr">
-        <is>
-          <t>AU-4 (1),CM-6 b,AU-6 (4)</t>
-        </is>
-      </c>
-      <c r="B44" s="2" t="inlineStr">
+      <c r="N44" s="2" t="inlineStr">
+        <is>
+          <t>CAT II</t>
+        </is>
+      </c>
+      <c r="O44" s="2" t="n"/>
+      <c r="P44" s="2" t="n"/>
+      <c r="Q44" s="2" t="n"/>
+    </row>
+    <row r="45" ht="130" customHeight="1">
+      <c r="A45" s="2" t="inlineStr">
+        <is>
+          <t>AU-6 (4),AU-4 (1),CM-6 b</t>
+        </is>
+      </c>
+      <c r="B45" s="2" t="inlineStr">
         <is>
           <t>CCI-001311,CCI-001312,CCI-000366</t>
         </is>
       </c>
-      <c r="C44" s="2" t="inlineStr">
+      <c r="C45" s="2" t="inlineStr">
         <is>
           <t>SRG-OS-000479-GPOS-00224,SRG-OS-000051-GPOS-00024,SRG-OS-000480-GPOS-00227</t>
         </is>
       </c>
-      <c r="D44" s="2" t="inlineStr">
+      <c r="D45" s="2" t="inlineStr">
         <is>
           <t>CCE-84063-7</t>
         </is>
       </c>
-      <c r="E44" s="2" t="inlineStr">
+      <c r="E45" s="2" t="inlineStr">
         <is>
           <t>The operating system must, at a minimum, off-load audit data from interconnected systems in real time and off-load audit data from standalone systems weekly.</t>
         </is>
       </c>
-      <c r="F44" s="2" t="inlineStr">
+      <c r="F45" s="2" t="inlineStr">
         <is>
           <t>Red Hat Enterprise Linux 9 Must, At A Minimum, Off-Load Audit Data From Interconnected Systems In Real Time And Off-Load Audit Data From Standalone Systems Weekly.</t>
         </is>
       </c>
-      <c r="G44" s="2" t="inlineStr">
+      <c r="G45" s="2" t="inlineStr">
         <is>
           <t>Information stored in one location is vulnerable to accidental or incidental deletion or alteration.
 Off-loading is a common process in information systems with limited audit storage capacity.</t>
         </is>
       </c>
-      <c r="H44" s="2" t="inlineStr">
+      <c r="H45" s="2" t="inlineStr">
         <is>
           <t>The rsyslog package provides the rsyslog daemon, which provides
 system logging services.</t>
         </is>
       </c>
-      <c r="I44" s="2" t="inlineStr">
-        <is>
-          <t>Applicable - Configurable</t>
-        </is>
-      </c>
-      <c r="J44" s="2" t="inlineStr">
+      <c r="I45" s="2" t="inlineStr">
+        <is>
+          <t>Applicable - Configurable</t>
+        </is>
+      </c>
+      <c r="J45" s="2" t="inlineStr">
         <is>
           <t>Verify the operating system, at a minimum, off-loads interconnected systems in real time and off-loads standalone systems weekly. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K44" s="2" t="inlineStr">
+      <c r="K45" s="2" t="inlineStr">
         <is>
           <t>Run the following command to determine if the  rsyslog  package is installed:  $ rpm -q rsyslog 
 If the package is not installed, then this is a finding.</t>
         </is>
       </c>
-      <c r="L44" s="2" t="n"/>
-      <c r="M44" s="2" t="inlineStr">
+      <c r="L45" s="2" t="n"/>
+      <c r="M45" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Configure Red Hat Enterprise Linux 9 to offload audit logs by installi